<commit_message>
Started adding 3d histogram plotting. Bug fixes.
</commit_message>
<xml_diff>
--- a/libinfo.xlsx
+++ b/libinfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tchan\Code\SCMB_Project\RNA-mediated_DSB_repair\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F060A8-6BE7-42B3-913A-7C631FD43BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C3EEDB-24BF-4238-8CE0-429B00C78CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="2" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="136">
   <si>
     <t>yjl217</t>
   </si>
@@ -305,9 +305,6 @@
     <t>file_out</t>
   </si>
   <si>
-    <t>command</t>
-  </si>
-  <si>
     <t>ref_file</t>
   </si>
   <si>
@@ -362,12 +359,6 @@
     <t>dsb_type</t>
   </si>
   <si>
-    <t>format</t>
-  </si>
-  <si>
-    <t>individual</t>
-  </si>
-  <si>
     <t>hguide</t>
   </si>
   <si>
@@ -453,6 +444,9 @@
   </si>
   <si>
     <t>command_main_data_combined</t>
+  </si>
+  <si>
+    <t>command_combine</t>
   </si>
 </sst>
 </file>
@@ -833,27 +827,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -896,7 +890,7 @@
         <v>82</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>83</v>
@@ -905,25 +899,25 @@
         <v>84</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>87</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -937,7 +931,7 @@
         <v>74</v>
       </c>
       <c r="D2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E2" t="s">
         <v>75</v>
@@ -983,7 +977,7 @@
         <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E3" t="s">
         <v>75</v>
@@ -1029,7 +1023,7 @@
         <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E4" t="s">
         <v>75</v>
@@ -1075,7 +1069,7 @@
         <v>74</v>
       </c>
       <c r="D5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E5" t="s">
         <v>75</v>
@@ -1121,7 +1115,7 @@
         <v>74</v>
       </c>
       <c r="D6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E6" t="s">
         <v>76</v>
@@ -1167,7 +1161,7 @@
         <v>74</v>
       </c>
       <c r="D7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E7" t="s">
         <v>76</v>
@@ -1213,7 +1207,7 @@
         <v>74</v>
       </c>
       <c r="D8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E8" t="s">
         <v>76</v>
@@ -1259,7 +1253,7 @@
         <v>74</v>
       </c>
       <c r="D9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E9" t="s">
         <v>76</v>
@@ -1305,7 +1299,7 @@
         <v>74</v>
       </c>
       <c r="D10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E10" t="s">
         <v>77</v>
@@ -1351,7 +1345,7 @@
         <v>74</v>
       </c>
       <c r="D11" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E11" t="s">
         <v>77</v>
@@ -1397,7 +1391,7 @@
         <v>74</v>
       </c>
       <c r="D12" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E12" t="s">
         <v>77</v>
@@ -1443,7 +1437,7 @@
         <v>74</v>
       </c>
       <c r="D13" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E13" t="s">
         <v>77</v>
@@ -1489,7 +1483,7 @@
         <v>74</v>
       </c>
       <c r="D14" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E14" t="s">
         <v>75</v>
@@ -1535,7 +1529,7 @@
         <v>74</v>
       </c>
       <c r="D15" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E15" t="s">
         <v>75</v>
@@ -1581,7 +1575,7 @@
         <v>74</v>
       </c>
       <c r="D16" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E16" t="s">
         <v>75</v>
@@ -1627,7 +1621,7 @@
         <v>74</v>
       </c>
       <c r="D17" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E17" t="s">
         <v>75</v>
@@ -1673,7 +1667,7 @@
         <v>74</v>
       </c>
       <c r="D18" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E18" t="s">
         <v>76</v>
@@ -1719,7 +1713,7 @@
         <v>74</v>
       </c>
       <c r="D19" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E19" t="s">
         <v>76</v>
@@ -1765,7 +1759,7 @@
         <v>74</v>
       </c>
       <c r="D20" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E20" t="s">
         <v>76</v>
@@ -1811,7 +1805,7 @@
         <v>74</v>
       </c>
       <c r="D21" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E21" t="s">
         <v>76</v>
@@ -1857,7 +1851,7 @@
         <v>74</v>
       </c>
       <c r="D22" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E22" t="s">
         <v>77</v>
@@ -1903,7 +1897,7 @@
         <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E23" t="s">
         <v>77</v>
@@ -1949,7 +1943,7 @@
         <v>74</v>
       </c>
       <c r="D24" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E24" t="s">
         <v>77</v>
@@ -1995,7 +1989,7 @@
         <v>74</v>
       </c>
       <c r="D25" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E25" t="s">
         <v>77</v>
@@ -2041,7 +2035,7 @@
         <v>74</v>
       </c>
       <c r="D26" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E26" t="s">
         <v>75</v>
@@ -2087,7 +2081,7 @@
         <v>74</v>
       </c>
       <c r="D27" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E27" t="s">
         <v>75</v>
@@ -2133,7 +2127,7 @@
         <v>74</v>
       </c>
       <c r="D28" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E28" t="s">
         <v>75</v>
@@ -2179,7 +2173,7 @@
         <v>74</v>
       </c>
       <c r="D29" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E29" t="s">
         <v>75</v>
@@ -2225,7 +2219,7 @@
         <v>74</v>
       </c>
       <c r="D30" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E30" t="s">
         <v>76</v>
@@ -2271,7 +2265,7 @@
         <v>74</v>
       </c>
       <c r="D31" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E31" t="s">
         <v>76</v>
@@ -2317,7 +2311,7 @@
         <v>74</v>
       </c>
       <c r="D32" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E32" t="s">
         <v>76</v>
@@ -2363,7 +2357,7 @@
         <v>74</v>
       </c>
       <c r="D33" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E33" t="s">
         <v>76</v>
@@ -2409,7 +2403,7 @@
         <v>74</v>
       </c>
       <c r="D34" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E34" t="s">
         <v>77</v>
@@ -2455,7 +2449,7 @@
         <v>74</v>
       </c>
       <c r="D35" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E35" t="s">
         <v>77</v>
@@ -2501,7 +2495,7 @@
         <v>74</v>
       </c>
       <c r="D36" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E36" t="s">
         <v>77</v>
@@ -2547,7 +2541,7 @@
         <v>74</v>
       </c>
       <c r="D37" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E37" t="s">
         <v>77</v>
@@ -2593,7 +2587,7 @@
         <v>74</v>
       </c>
       <c r="D38" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E38" t="s">
         <v>75</v>
@@ -2639,7 +2633,7 @@
         <v>74</v>
       </c>
       <c r="D39" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E39" t="s">
         <v>75</v>
@@ -2685,7 +2679,7 @@
         <v>74</v>
       </c>
       <c r="D40" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E40" t="s">
         <v>75</v>
@@ -2731,7 +2725,7 @@
         <v>74</v>
       </c>
       <c r="D41" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E41" t="s">
         <v>75</v>
@@ -2777,7 +2771,7 @@
         <v>74</v>
       </c>
       <c r="D42" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E42" t="s">
         <v>76</v>
@@ -2823,7 +2817,7 @@
         <v>74</v>
       </c>
       <c r="D43" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E43" t="s">
         <v>76</v>
@@ -2869,7 +2863,7 @@
         <v>74</v>
       </c>
       <c r="D44" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E44" t="s">
         <v>76</v>
@@ -2915,7 +2909,7 @@
         <v>74</v>
       </c>
       <c r="D45" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E45" t="s">
         <v>76</v>
@@ -2961,7 +2955,7 @@
         <v>74</v>
       </c>
       <c r="D46" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E46" t="s">
         <v>77</v>
@@ -3007,7 +3001,7 @@
         <v>74</v>
       </c>
       <c r="D47" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E47" t="s">
         <v>77</v>
@@ -3053,7 +3047,7 @@
         <v>74</v>
       </c>
       <c r="D48" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E48" t="s">
         <v>77</v>
@@ -3099,7 +3093,7 @@
         <v>74</v>
       </c>
       <c r="D49" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E49" t="s">
         <v>77</v>
@@ -3142,7 +3136,7 @@
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D50" t="s">
         <v>78</v>
@@ -3188,7 +3182,7 @@
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D51" t="s">
         <v>78</v>
@@ -3234,7 +3228,7 @@
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D52" t="s">
         <v>78</v>
@@ -3280,7 +3274,7 @@
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D53" t="s">
         <v>78</v>
@@ -3326,7 +3320,7 @@
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D54" t="s">
         <v>78</v>
@@ -3372,7 +3366,7 @@
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D55" t="s">
         <v>78</v>
@@ -3418,7 +3412,7 @@
         <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D56" t="s">
         <v>78</v>
@@ -3464,7 +3458,7 @@
         <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D57" t="s">
         <v>78</v>
@@ -3510,7 +3504,7 @@
         <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D58" t="s">
         <v>78</v>
@@ -3556,7 +3550,7 @@
         <v>1</v>
       </c>
       <c r="C59" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D59" t="s">
         <v>78</v>
@@ -3602,7 +3596,7 @@
         <v>1</v>
       </c>
       <c r="C60" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D60" t="s">
         <v>78</v>
@@ -3648,7 +3642,7 @@
         <v>1</v>
       </c>
       <c r="C61" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D61" t="s">
         <v>78</v>
@@ -3694,7 +3688,7 @@
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D62" t="s">
         <v>79</v>
@@ -3740,7 +3734,7 @@
         <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D63" t="s">
         <v>79</v>
@@ -3786,7 +3780,7 @@
         <v>1</v>
       </c>
       <c r="C64" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D64" t="s">
         <v>79</v>
@@ -3832,7 +3826,7 @@
         <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D65" t="s">
         <v>79</v>
@@ -3878,7 +3872,7 @@
         <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D66" t="s">
         <v>79</v>
@@ -3924,7 +3918,7 @@
         <v>1</v>
       </c>
       <c r="C67" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D67" t="s">
         <v>79</v>
@@ -3970,7 +3964,7 @@
         <v>1</v>
       </c>
       <c r="C68" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D68" t="s">
         <v>79</v>
@@ -4016,7 +4010,7 @@
         <v>1</v>
       </c>
       <c r="C69" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D69" t="s">
         <v>79</v>
@@ -4062,7 +4056,7 @@
         <v>1</v>
       </c>
       <c r="C70" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D70" t="s">
         <v>79</v>
@@ -4108,7 +4102,7 @@
         <v>1</v>
       </c>
       <c r="C71" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D71" t="s">
         <v>79</v>
@@ -4154,7 +4148,7 @@
         <v>1</v>
       </c>
       <c r="C72" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D72" t="s">
         <v>79</v>
@@ -4200,7 +4194,7 @@
         <v>1</v>
       </c>
       <c r="C73" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D73" t="s">
         <v>79</v>
@@ -4246,7 +4240,7 @@
         <v>14</v>
       </c>
       <c r="C74" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D74" t="s">
         <v>78</v>
@@ -4292,7 +4286,7 @@
         <v>14</v>
       </c>
       <c r="C75" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D75" t="s">
         <v>78</v>
@@ -4338,7 +4332,7 @@
         <v>14</v>
       </c>
       <c r="C76" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D76" t="s">
         <v>78</v>
@@ -4384,7 +4378,7 @@
         <v>14</v>
       </c>
       <c r="C77" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D77" t="s">
         <v>78</v>
@@ -4430,7 +4424,7 @@
         <v>14</v>
       </c>
       <c r="C78" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D78" t="s">
         <v>78</v>
@@ -4476,7 +4470,7 @@
         <v>14</v>
       </c>
       <c r="C79" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D79" t="s">
         <v>78</v>
@@ -4522,7 +4516,7 @@
         <v>14</v>
       </c>
       <c r="C80" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D80" t="s">
         <v>78</v>
@@ -4568,7 +4562,7 @@
         <v>14</v>
       </c>
       <c r="C81" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D81" t="s">
         <v>78</v>
@@ -4614,7 +4608,7 @@
         <v>14</v>
       </c>
       <c r="C82" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D82" t="s">
         <v>78</v>
@@ -4660,7 +4654,7 @@
         <v>14</v>
       </c>
       <c r="C83" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D83" t="s">
         <v>78</v>
@@ -4706,7 +4700,7 @@
         <v>14</v>
       </c>
       <c r="C84" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D84" t="s">
         <v>78</v>
@@ -4752,7 +4746,7 @@
         <v>14</v>
       </c>
       <c r="C85" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D85" t="s">
         <v>78</v>
@@ -4798,7 +4792,7 @@
         <v>14</v>
       </c>
       <c r="C86" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D86" t="s">
         <v>79</v>
@@ -4844,7 +4838,7 @@
         <v>14</v>
       </c>
       <c r="C87" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D87" t="s">
         <v>79</v>
@@ -4890,7 +4884,7 @@
         <v>14</v>
       </c>
       <c r="C88" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D88" t="s">
         <v>79</v>
@@ -4936,7 +4930,7 @@
         <v>14</v>
       </c>
       <c r="C89" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D89" t="s">
         <v>79</v>
@@ -4982,7 +4976,7 @@
         <v>14</v>
       </c>
       <c r="C90" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D90" t="s">
         <v>79</v>
@@ -5028,7 +5022,7 @@
         <v>14</v>
       </c>
       <c r="C91" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D91" t="s">
         <v>79</v>
@@ -5074,7 +5068,7 @@
         <v>14</v>
       </c>
       <c r="C92" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D92" t="s">
         <v>79</v>
@@ -5120,7 +5114,7 @@
         <v>14</v>
       </c>
       <c r="C93" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D93" t="s">
         <v>79</v>
@@ -5166,7 +5160,7 @@
         <v>14</v>
       </c>
       <c r="C94" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D94" t="s">
         <v>79</v>
@@ -5212,7 +5206,7 @@
         <v>14</v>
       </c>
       <c r="C95" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D95" t="s">
         <v>79</v>
@@ -5258,7 +5252,7 @@
         <v>14</v>
       </c>
       <c r="C96" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D96" t="s">
         <v>79</v>
@@ -5304,7 +5298,7 @@
         <v>14</v>
       </c>
       <c r="C97" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D97" t="s">
         <v>79</v>
@@ -5344,19 +5338,19 @@
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B98" t="s">
         <v>1</v>
       </c>
       <c r="C98" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D98" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E98" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F98" t="s">
         <v>85</v>
@@ -5390,19 +5384,19 @@
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B99" t="s">
         <v>1</v>
       </c>
       <c r="C99" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D99" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E99" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F99" t="s">
         <v>85</v>
@@ -5436,19 +5430,19 @@
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B100" t="s">
         <v>1</v>
       </c>
       <c r="C100" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D100" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E100" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F100" t="s">
         <v>85</v>
@@ -5482,19 +5476,19 @@
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B101" t="s">
         <v>1</v>
       </c>
       <c r="C101" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D101" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E101" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F101" t="s">
         <v>85</v>
@@ -5528,19 +5522,19 @@
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B102" t="s">
         <v>1</v>
       </c>
       <c r="C102" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D102" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E102" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F102" t="s">
         <v>85</v>
@@ -5574,19 +5568,19 @@
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B103" t="s">
         <v>1</v>
       </c>
       <c r="C103" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D103" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E103" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F103" t="s">
         <v>85</v>
@@ -5620,19 +5614,19 @@
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B104" t="s">
         <v>1</v>
       </c>
       <c r="C104" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D104" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E104" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F104" t="s">
         <v>85</v>
@@ -5666,19 +5660,19 @@
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B105" t="s">
         <v>1</v>
       </c>
       <c r="C105" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D105" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E105" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F105" t="s">
         <v>85</v>
@@ -5712,19 +5706,19 @@
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B106" t="s">
         <v>1</v>
       </c>
       <c r="C106" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D106" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E106" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F106" t="s">
         <v>86</v>
@@ -5758,19 +5752,19 @@
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B107" t="s">
         <v>1</v>
       </c>
       <c r="C107" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D107" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E107" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F107" t="s">
         <v>86</v>
@@ -5804,19 +5798,19 @@
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B108" t="s">
         <v>1</v>
       </c>
       <c r="C108" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D108" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E108" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F108" t="s">
         <v>86</v>
@@ -5850,19 +5844,19 @@
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B109" t="s">
         <v>1</v>
       </c>
       <c r="C109" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D109" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E109" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F109" t="s">
         <v>86</v>
@@ -5896,19 +5890,19 @@
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B110" t="s">
         <v>1</v>
       </c>
       <c r="C110" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D110" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E110" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F110" t="s">
         <v>86</v>
@@ -5942,19 +5936,19 @@
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B111" t="s">
         <v>1</v>
       </c>
       <c r="C111" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D111" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E111" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F111" t="s">
         <v>86</v>
@@ -5988,19 +5982,19 @@
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B112" t="s">
         <v>1</v>
       </c>
       <c r="C112" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D112" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E112" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F112" t="s">
         <v>86</v>
@@ -6034,19 +6028,19 @@
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B113" t="s">
         <v>1</v>
       </c>
       <c r="C113" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D113" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E113" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F113" t="s">
         <v>86</v>
@@ -6089,7 +6083,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12B0900B-E55F-43FE-AC1A-BE82F1C8E743}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G19" workbookViewId="0">
       <selection activeCell="Q3" sqref="Q3:Q30"/>
     </sheetView>
   </sheetViews>
@@ -6115,13 +6109,13 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>84</v>
@@ -6130,37 +6124,37 @@
         <v>83</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="Q1" s="1" t="s">
-        <v>88</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -6218,8 +6212,8 @@
         <v>sgAB</v>
       </c>
       <c r="H3" t="str">
-        <f ca="1">_xlfn.CONCAT(D3, "_", G3, "_", F3)</f>
-        <v>WT_sgAB_sense</v>
+        <f ca="1">_xlfn.CONCAT(D3, "_", G3, "_", E3, "_", F3)</f>
+        <v>WT_sgAB_R1_sense</v>
       </c>
       <c r="I3" t="str">
         <f ca="1">OFFSET('1'!$I$1, 4 * (A3 - 1)  + ($I$2), 0)</f>
@@ -6255,7 +6249,7 @@
       </c>
       <c r="Q3" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -in ", dirs!$A$2, "/", I3, ".tsv ", dirs!$A$2, "/", K3, ".tsv ", dirs!$A$2, "/", M3, ".tsv ", dirs!$A$2, "/", O3, ".tsv --total_reads ", J3, " ", L3, " ", N3, " ", P3, " -o ", dirs!$A$3, "/", H3, ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl217_WT_sgAB_R1_sense.tsv libraries_2/yjl218_WT_sgAB_R1_sense.tsv libraries_2/yjl219_WT_sgAB_R1_sense.tsv libraries_2/yjl220_WT_sgAB_R1_sense.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgAB_sense.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl217_WT_sgAB_R1_sense.tsv libraries_2/yjl218_WT_sgAB_R1_sense.tsv libraries_2/yjl219_WT_sgAB_R1_sense.tsv libraries_2/yjl220_WT_sgAB_R1_sense.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgAB_R1_sense.tsv --quiet </v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -6287,8 +6281,8 @@
         <v>sgAB</v>
       </c>
       <c r="H4" t="str">
-        <f t="shared" ref="H4:H30" ca="1" si="0">_xlfn.CONCAT(D4, "_", G4, "_", F4)</f>
-        <v>WT_sgAB_branch</v>
+        <f t="shared" ref="H4:H30" ca="1" si="0">_xlfn.CONCAT(D4, "_", G4, "_", E4, "_", F4)</f>
+        <v>WT_sgAB_R1_branch</v>
       </c>
       <c r="I4" t="str">
         <f ca="1">OFFSET('1'!$I$1, 4 * (A4 - 1)  + ($I$2), 0)</f>
@@ -6324,7 +6318,7 @@
       </c>
       <c r="Q4" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -in ", dirs!$A$2, "/", I4, ".tsv ", dirs!$A$2, "/", K4, ".tsv ", dirs!$A$2, "/", M4, ".tsv ", dirs!$A$2, "/", O4, ".tsv --total_reads ", J4, " ", L4, " ", N4, " ", P4, " -o ", dirs!$A$3, "/", H4, ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl221_WT_sgAB_R1_branch.tsv libraries_2/yjl222_WT_sgAB_R1_branch.tsv libraries_2/yjl223_WT_sgAB_R1_branch.tsv libraries_2/yjl224_WT_sgAB_R1_branch.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgAB_branch.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl221_WT_sgAB_R1_branch.tsv libraries_2/yjl222_WT_sgAB_R1_branch.tsv libraries_2/yjl223_WT_sgAB_R1_branch.tsv libraries_2/yjl224_WT_sgAB_R1_branch.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgAB_R1_branch.tsv --quiet </v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -6357,7 +6351,7 @@
       </c>
       <c r="H5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>WT_sgAB_cmv</v>
+        <v>WT_sgAB_R1_cmv</v>
       </c>
       <c r="I5" t="str">
         <f ca="1">OFFSET('1'!$I$1, 4 * (A5 - 1)  + ($I$2), 0)</f>
@@ -6393,7 +6387,7 @@
       </c>
       <c r="Q5" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -in ", dirs!$A$2, "/", I5, ".tsv ", dirs!$A$2, "/", K5, ".tsv ", dirs!$A$2, "/", M5, ".tsv ", dirs!$A$2, "/", O5, ".tsv --total_reads ", J5, " ", L5, " ", N5, " ", P5, " -o ", dirs!$A$3, "/", H5, ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl225_WT_sgAB_R1_cmv.tsv libraries_2/yjl226_WT_sgAB_R1_cmv.tsv libraries_2/yjl227_WT_sgAB_R1_cmv.tsv libraries_2/yjl228_WT_sgAB_R1_cmv.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgAB_cmv.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl225_WT_sgAB_R1_cmv.tsv libraries_2/yjl226_WT_sgAB_R1_cmv.tsv libraries_2/yjl227_WT_sgAB_R1_cmv.tsv libraries_2/yjl228_WT_sgAB_R1_cmv.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgAB_R1_cmv.tsv --quiet </v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -6426,7 +6420,7 @@
       </c>
       <c r="H6" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>KO_sgAB_sense</v>
+        <v>KO_sgAB_R1_sense</v>
       </c>
       <c r="I6" t="str">
         <f ca="1">OFFSET('1'!$I$1, 4 * (A6 - 1)  + ($I$2), 0)</f>
@@ -6462,7 +6456,7 @@
       </c>
       <c r="Q6" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -in ", dirs!$A$2, "/", I6, ".tsv ", dirs!$A$2, "/", K6, ".tsv ", dirs!$A$2, "/", M6, ".tsv ", dirs!$A$2, "/", O6, ".tsv --total_reads ", J6, " ", L6, " ", N6, " ", P6, " -o ", dirs!$A$3, "/", H6, ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl229_KO_sgAB_R1_sense.tsv libraries_2/yjl230_KO_sgAB_R1_sense.tsv libraries_2/yjl231_KO_sgAB_R1_sense.tsv libraries_2/yjl232_KO_sgAB_R1_sense.tsv --total_reads 96 97 98 99 -o libraries_3/KO_sgAB_sense.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl229_KO_sgAB_R1_sense.tsv libraries_2/yjl230_KO_sgAB_R1_sense.tsv libraries_2/yjl231_KO_sgAB_R1_sense.tsv libraries_2/yjl232_KO_sgAB_R1_sense.tsv --total_reads 96 97 98 99 -o libraries_3/KO_sgAB_R1_sense.tsv --quiet </v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -6495,7 +6489,7 @@
       </c>
       <c r="H7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>KO_sgAB_branch</v>
+        <v>KO_sgAB_R1_branch</v>
       </c>
       <c r="I7" t="str">
         <f ca="1">OFFSET('1'!$I$1, 4 * (A7 - 1)  + ($I$2), 0)</f>
@@ -6531,7 +6525,7 @@
       </c>
       <c r="Q7" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -in ", dirs!$A$2, "/", I7, ".tsv ", dirs!$A$2, "/", K7, ".tsv ", dirs!$A$2, "/", M7, ".tsv ", dirs!$A$2, "/", O7, ".tsv --total_reads ", J7, " ", L7, " ", N7, " ", P7, " -o ", dirs!$A$3, "/", H7, ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl233_KO_sgAB_R1_branch.tsv libraries_2/yjl234_KO_sgAB_R1_branch.tsv libraries_2/yjl235_KO_sgAB_R1_branch.tsv libraries_2/yjl236_KO_sgAB_R1_branch.tsv --total_reads 96 97 98 99 -o libraries_3/KO_sgAB_branch.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl233_KO_sgAB_R1_branch.tsv libraries_2/yjl234_KO_sgAB_R1_branch.tsv libraries_2/yjl235_KO_sgAB_R1_branch.tsv libraries_2/yjl236_KO_sgAB_R1_branch.tsv --total_reads 96 97 98 99 -o libraries_3/KO_sgAB_R1_branch.tsv --quiet </v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -6564,7 +6558,7 @@
       </c>
       <c r="H8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>KO_sgAB_cmv</v>
+        <v>KO_sgAB_R1_cmv</v>
       </c>
       <c r="I8" t="str">
         <f ca="1">OFFSET('1'!$I$1, 4 * (A8 - 1)  + ($I$2), 0)</f>
@@ -6600,7 +6594,7 @@
       </c>
       <c r="Q8" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -in ", dirs!$A$2, "/", I8, ".tsv ", dirs!$A$2, "/", K8, ".tsv ", dirs!$A$2, "/", M8, ".tsv ", dirs!$A$2, "/", O8, ".tsv --total_reads ", J8, " ", L8, " ", N8, " ", P8, " -o ", dirs!$A$3, "/", H8, ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl237_KO_sgAB_R1_cmv.tsv libraries_2/yjl238_KO_sgAB_R1_cmv.tsv libraries_2/yjl239_KO_sgAB_R1_cmv.tsv libraries_2/yjl240_KO_sgAB_R1_cmv.tsv --total_reads 96 97 98 99 -o libraries_3/KO_sgAB_cmv.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl237_KO_sgAB_R1_cmv.tsv libraries_2/yjl238_KO_sgAB_R1_cmv.tsv libraries_2/yjl239_KO_sgAB_R1_cmv.tsv libraries_2/yjl240_KO_sgAB_R1_cmv.tsv --total_reads 96 97 98 99 -o libraries_3/KO_sgAB_R1_cmv.tsv --quiet </v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -6633,7 +6627,7 @@
       </c>
       <c r="H9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>WT_sgAB_sense</v>
+        <v>WT_sgAB_R2_sense</v>
       </c>
       <c r="I9" t="str">
         <f ca="1">OFFSET('1'!$I$1, 4 * (A9 - 1)  + ($I$2), 0)</f>
@@ -6669,7 +6663,7 @@
       </c>
       <c r="Q9" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -in ", dirs!$A$2, "/", I9, ".tsv ", dirs!$A$2, "/", K9, ".tsv ", dirs!$A$2, "/", M9, ".tsv ", dirs!$A$2, "/", O9, ".tsv --total_reads ", J9, " ", L9, " ", N9, " ", P9, " -o ", dirs!$A$3, "/", H9, ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl217_WT_sgAB_R2_sense.tsv libraries_2/yjl218_WT_sgAB_R2_sense.tsv libraries_2/yjl219_WT_sgAB_R2_sense.tsv libraries_2/yjl220_WT_sgAB_R2_sense.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgAB_sense.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl217_WT_sgAB_R2_sense.tsv libraries_2/yjl218_WT_sgAB_R2_sense.tsv libraries_2/yjl219_WT_sgAB_R2_sense.tsv libraries_2/yjl220_WT_sgAB_R2_sense.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgAB_R2_sense.tsv --quiet </v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -6702,7 +6696,7 @@
       </c>
       <c r="H10" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>WT_sgAB_branch</v>
+        <v>WT_sgAB_R2_branch</v>
       </c>
       <c r="I10" t="str">
         <f ca="1">OFFSET('1'!$I$1, 4 * (A10 - 1)  + ($I$2), 0)</f>
@@ -6738,7 +6732,7 @@
       </c>
       <c r="Q10" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -in ", dirs!$A$2, "/", I10, ".tsv ", dirs!$A$2, "/", K10, ".tsv ", dirs!$A$2, "/", M10, ".tsv ", dirs!$A$2, "/", O10, ".tsv --total_reads ", J10, " ", L10, " ", N10, " ", P10, " -o ", dirs!$A$3, "/", H10, ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl221_WT_sgAB_R2_branch.tsv libraries_2/yjl222_WT_sgAB_R2_branch.tsv libraries_2/yjl223_WT_sgAB_R2_branch.tsv libraries_2/yjl224_WT_sgAB_R2_branch.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgAB_branch.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl221_WT_sgAB_R2_branch.tsv libraries_2/yjl222_WT_sgAB_R2_branch.tsv libraries_2/yjl223_WT_sgAB_R2_branch.tsv libraries_2/yjl224_WT_sgAB_R2_branch.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgAB_R2_branch.tsv --quiet </v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -6771,7 +6765,7 @@
       </c>
       <c r="H11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>WT_sgAB_cmv</v>
+        <v>WT_sgAB_R2_cmv</v>
       </c>
       <c r="I11" t="str">
         <f ca="1">OFFSET('1'!$I$1, 4 * (A11 - 1)  + ($I$2), 0)</f>
@@ -6807,7 +6801,7 @@
       </c>
       <c r="Q11" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -in ", dirs!$A$2, "/", I11, ".tsv ", dirs!$A$2, "/", K11, ".tsv ", dirs!$A$2, "/", M11, ".tsv ", dirs!$A$2, "/", O11, ".tsv --total_reads ", J11, " ", L11, " ", N11, " ", P11, " -o ", dirs!$A$3, "/", H11, ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl225_WT_sgAB_R2_cmv.tsv libraries_2/yjl226_WT_sgAB_R2_cmv.tsv libraries_2/yjl227_WT_sgAB_R2_cmv.tsv libraries_2/yjl228_WT_sgAB_R2_cmv.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgAB_cmv.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl225_WT_sgAB_R2_cmv.tsv libraries_2/yjl226_WT_sgAB_R2_cmv.tsv libraries_2/yjl227_WT_sgAB_R2_cmv.tsv libraries_2/yjl228_WT_sgAB_R2_cmv.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgAB_R2_cmv.tsv --quiet </v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -6840,7 +6834,7 @@
       </c>
       <c r="H12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>KO_sgAB_sense</v>
+        <v>KO_sgAB_R2_sense</v>
       </c>
       <c r="I12" t="str">
         <f ca="1">OFFSET('1'!$I$1, 4 * (A12 - 1)  + ($I$2), 0)</f>
@@ -6876,7 +6870,7 @@
       </c>
       <c r="Q12" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -in ", dirs!$A$2, "/", I12, ".tsv ", dirs!$A$2, "/", K12, ".tsv ", dirs!$A$2, "/", M12, ".tsv ", dirs!$A$2, "/", O12, ".tsv --total_reads ", J12, " ", L12, " ", N12, " ", P12, " -o ", dirs!$A$3, "/", H12, ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl229_KO_sgAB_R2_sense.tsv libraries_2/yjl230_KO_sgAB_R2_sense.tsv libraries_2/yjl231_KO_sgAB_R2_sense.tsv libraries_2/yjl232_KO_sgAB_R2_sense.tsv --total_reads 96 97 98 99 -o libraries_3/KO_sgAB_sense.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl229_KO_sgAB_R2_sense.tsv libraries_2/yjl230_KO_sgAB_R2_sense.tsv libraries_2/yjl231_KO_sgAB_R2_sense.tsv libraries_2/yjl232_KO_sgAB_R2_sense.tsv --total_reads 96 97 98 99 -o libraries_3/KO_sgAB_R2_sense.tsv --quiet </v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -6909,7 +6903,7 @@
       </c>
       <c r="H13" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>KO_sgAB_branch</v>
+        <v>KO_sgAB_R2_branch</v>
       </c>
       <c r="I13" t="str">
         <f ca="1">OFFSET('1'!$I$1, 4 * (A13 - 1)  + ($I$2), 0)</f>
@@ -6945,7 +6939,7 @@
       </c>
       <c r="Q13" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -in ", dirs!$A$2, "/", I13, ".tsv ", dirs!$A$2, "/", K13, ".tsv ", dirs!$A$2, "/", M13, ".tsv ", dirs!$A$2, "/", O13, ".tsv --total_reads ", J13, " ", L13, " ", N13, " ", P13, " -o ", dirs!$A$3, "/", H13, ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl233_KO_sgAB_R2_branch.tsv libraries_2/yjl234_KO_sgAB_R2_branch.tsv libraries_2/yjl235_KO_sgAB_R2_branch.tsv libraries_2/yjl236_KO_sgAB_R2_branch.tsv --total_reads 96 97 98 99 -o libraries_3/KO_sgAB_branch.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl233_KO_sgAB_R2_branch.tsv libraries_2/yjl234_KO_sgAB_R2_branch.tsv libraries_2/yjl235_KO_sgAB_R2_branch.tsv libraries_2/yjl236_KO_sgAB_R2_branch.tsv --total_reads 96 97 98 99 -o libraries_3/KO_sgAB_R2_branch.tsv --quiet </v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -6978,7 +6972,7 @@
       </c>
       <c r="H14" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>KO_sgAB_cmv</v>
+        <v>KO_sgAB_R2_cmv</v>
       </c>
       <c r="I14" t="str">
         <f ca="1">OFFSET('1'!$I$1, 4 * (A14 - 1)  + ($I$2), 0)</f>
@@ -7014,7 +7008,7 @@
       </c>
       <c r="Q14" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -in ", dirs!$A$2, "/", I14, ".tsv ", dirs!$A$2, "/", K14, ".tsv ", dirs!$A$2, "/", M14, ".tsv ", dirs!$A$2, "/", O14, ".tsv --total_reads ", J14, " ", L14, " ", N14, " ", P14, " -o ", dirs!$A$3, "/", H14, ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl237_KO_sgAB_R2_cmv.tsv libraries_2/yjl238_KO_sgAB_R2_cmv.tsv libraries_2/yjl239_KO_sgAB_R2_cmv.tsv libraries_2/yjl240_KO_sgAB_R2_cmv.tsv --total_reads 96 97 98 99 -o libraries_3/KO_sgAB_cmv.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl237_KO_sgAB_R2_cmv.tsv libraries_2/yjl238_KO_sgAB_R2_cmv.tsv libraries_2/yjl239_KO_sgAB_R2_cmv.tsv libraries_2/yjl240_KO_sgAB_R2_cmv.tsv --total_reads 96 97 98 99 -o libraries_3/KO_sgAB_R2_cmv.tsv --quiet </v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -7047,7 +7041,7 @@
       </c>
       <c r="H15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>WT_sgA_sense</v>
+        <v>WT_sgA_R1_sense</v>
       </c>
       <c r="I15" t="str">
         <f ca="1">OFFSET('1'!$I$1, 4 * (A15 - 1)  + ($I$2), 0)</f>
@@ -7083,7 +7077,7 @@
       </c>
       <c r="Q15" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -in ", dirs!$A$2, "/", I15, ".tsv ", dirs!$A$2, "/", K15, ".tsv ", dirs!$A$2, "/", M15, ".tsv ", dirs!$A$2, "/", O15, ".tsv --total_reads ", J15, " ", L15, " ", N15, " ", P15, " -o ", dirs!$A$3, "/", H15, ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl255_WT_sgA_R1_sense.tsv libraries_2/yjl256_WT_sgA_R1_sense.tsv libraries_2/yjl257_WT_sgA_R1_sense.tsv libraries_2/yjl258_WT_sgA_R1_sense.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgA_sense.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl255_WT_sgA_R1_sense.tsv libraries_2/yjl256_WT_sgA_R1_sense.tsv libraries_2/yjl257_WT_sgA_R1_sense.tsv libraries_2/yjl258_WT_sgA_R1_sense.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgA_R1_sense.tsv --quiet </v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -7116,7 +7110,7 @@
       </c>
       <c r="H16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>WT_sgA_branch</v>
+        <v>WT_sgA_R1_branch</v>
       </c>
       <c r="I16" t="str">
         <f ca="1">OFFSET('1'!$I$1, 4 * (A16 - 1)  + ($I$2), 0)</f>
@@ -7152,7 +7146,7 @@
       </c>
       <c r="Q16" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -in ", dirs!$A$2, "/", I16, ".tsv ", dirs!$A$2, "/", K16, ".tsv ", dirs!$A$2, "/", M16, ".tsv ", dirs!$A$2, "/", O16, ".tsv --total_reads ", J16, " ", L16, " ", N16, " ", P16, " -o ", dirs!$A$3, "/", H16, ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl259_WT_sgA_R1_branch.tsv libraries_2/yjl260_WT_sgA_R1_branch.tsv libraries_2/yjl261_WT_sgA_R1_branch.tsv libraries_2/yjl262_WT_sgA_R1_branch.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgA_branch.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl259_WT_sgA_R1_branch.tsv libraries_2/yjl260_WT_sgA_R1_branch.tsv libraries_2/yjl261_WT_sgA_R1_branch.tsv libraries_2/yjl262_WT_sgA_R1_branch.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgA_R1_branch.tsv --quiet </v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -7185,7 +7179,7 @@
       </c>
       <c r="H17" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>WT_sgA_cmv</v>
+        <v>WT_sgA_R1_cmv</v>
       </c>
       <c r="I17" t="str">
         <f ca="1">OFFSET('1'!$I$1, 4 * (A17 - 1)  + ($I$2), 0)</f>
@@ -7221,7 +7215,7 @@
       </c>
       <c r="Q17" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -in ", dirs!$A$2, "/", I17, ".tsv ", dirs!$A$2, "/", K17, ".tsv ", dirs!$A$2, "/", M17, ".tsv ", dirs!$A$2, "/", O17, ".tsv --total_reads ", J17, " ", L17, " ", N17, " ", P17, " -o ", dirs!$A$3, "/", H17, ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl263_WT_sgA_R1_cmv.tsv libraries_2/yjl264_WT_sgA_R1_cmv.tsv libraries_2/yjl265_WT_sgA_R1_cmv.tsv libraries_2/yjl266_WT_sgA_R1_cmv.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgA_cmv.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl263_WT_sgA_R1_cmv.tsv libraries_2/yjl264_WT_sgA_R1_cmv.tsv libraries_2/yjl265_WT_sgA_R1_cmv.tsv libraries_2/yjl266_WT_sgA_R1_cmv.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgA_R1_cmv.tsv --quiet </v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -7254,7 +7248,7 @@
       </c>
       <c r="H18" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>WT_sgB_sense</v>
+        <v>WT_sgB_R2_sense</v>
       </c>
       <c r="I18" t="str">
         <f ca="1">OFFSET('1'!$I$1, 4 * (A18 - 1)  + ($I$2), 0)</f>
@@ -7290,7 +7284,7 @@
       </c>
       <c r="Q18" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -in ", dirs!$A$2, "/", I18, ".tsv ", dirs!$A$2, "/", K18, ".tsv ", dirs!$A$2, "/", M18, ".tsv ", dirs!$A$2, "/", O18, ".tsv --total_reads ", J18, " ", L18, " ", N18, " ", P18, " -o ", dirs!$A$3, "/", H18, ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl267_WT_sgB_R2_sense.tsv libraries_2/yjl268_WT_sgB_R2_sense.tsv libraries_2/yjl269_WT_sgB_R2_sense.tsv libraries_2/yjl270_WT_sgB_R2_sense.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgB_sense.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl267_WT_sgB_R2_sense.tsv libraries_2/yjl268_WT_sgB_R2_sense.tsv libraries_2/yjl269_WT_sgB_R2_sense.tsv libraries_2/yjl270_WT_sgB_R2_sense.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgB_R2_sense.tsv --quiet </v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -7323,7 +7317,7 @@
       </c>
       <c r="H19" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>WT_sgB_branch</v>
+        <v>WT_sgB_R2_branch</v>
       </c>
       <c r="I19" t="str">
         <f ca="1">OFFSET('1'!$I$1, 4 * (A19 - 1)  + ($I$2), 0)</f>
@@ -7359,7 +7353,7 @@
       </c>
       <c r="Q19" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -in ", dirs!$A$2, "/", I19, ".tsv ", dirs!$A$2, "/", K19, ".tsv ", dirs!$A$2, "/", M19, ".tsv ", dirs!$A$2, "/", O19, ".tsv --total_reads ", J19, " ", L19, " ", N19, " ", P19, " -o ", dirs!$A$3, "/", H19, ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl271_WT_sgB_R2_branch.tsv libraries_2/yjl272_WT_sgB_R2_branch.tsv libraries_2/yjl273_WT_sgB_R2_branch.tsv libraries_2/yjl274_WT_sgB_R2_branch.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgB_branch.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl271_WT_sgB_R2_branch.tsv libraries_2/yjl272_WT_sgB_R2_branch.tsv libraries_2/yjl273_WT_sgB_R2_branch.tsv libraries_2/yjl274_WT_sgB_R2_branch.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgB_R2_branch.tsv --quiet </v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -7392,7 +7386,7 @@
       </c>
       <c r="H20" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>WT_sgB_cmv</v>
+        <v>WT_sgB_R2_cmv</v>
       </c>
       <c r="I20" t="str">
         <f ca="1">OFFSET('1'!$I$1, 4 * (A20 - 1)  + ($I$2), 0)</f>
@@ -7428,7 +7422,7 @@
       </c>
       <c r="Q20" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -in ", dirs!$A$2, "/", I20, ".tsv ", dirs!$A$2, "/", K20, ".tsv ", dirs!$A$2, "/", M20, ".tsv ", dirs!$A$2, "/", O20, ".tsv --total_reads ", J20, " ", L20, " ", N20, " ", P20, " -o ", dirs!$A$3, "/", H20, ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl275_WT_sgB_R2_cmv.tsv libraries_2/yjl276_WT_sgB_R2_cmv.tsv libraries_2/yjl277_WT_sgB_R2_cmv.tsv libraries_2/yjl278_WT_sgB_R2_cmv.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgB_cmv.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl275_WT_sgB_R2_cmv.tsv libraries_2/yjl276_WT_sgB_R2_cmv.tsv libraries_2/yjl277_WT_sgB_R2_cmv.tsv libraries_2/yjl278_WT_sgB_R2_cmv.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgB_R2_cmv.tsv --quiet </v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -7461,7 +7455,7 @@
       </c>
       <c r="H21" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>KO_sgA_sense</v>
+        <v>KO_sgA_R1_sense</v>
       </c>
       <c r="I21" t="str">
         <f ca="1">OFFSET('1'!$I$1, 4 * (A21 - 1)  + ($I$2), 0)</f>
@@ -7497,7 +7491,7 @@
       </c>
       <c r="Q21" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -in ", dirs!$A$2, "/", I21, ".tsv ", dirs!$A$2, "/", K21, ".tsv ", dirs!$A$2, "/", M21, ".tsv ", dirs!$A$2, "/", O21, ".tsv --total_reads ", J21, " ", L21, " ", N21, " ", P21, " -o ", dirs!$A$3, "/", H21, ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl292_KO_sgA_R1_sense.tsv libraries_2/yjl293_KO_sgA_R1_sense.tsv libraries_2/yjl294_KO_sgA_R1_sense.tsv libraries_2/yjl295_KO_sgA_R1_sense.tsv --total_reads 96 97 98 99 -o libraries_3/KO_sgA_sense.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl292_KO_sgA_R1_sense.tsv libraries_2/yjl293_KO_sgA_R1_sense.tsv libraries_2/yjl294_KO_sgA_R1_sense.tsv libraries_2/yjl295_KO_sgA_R1_sense.tsv --total_reads 96 97 98 99 -o libraries_3/KO_sgA_R1_sense.tsv --quiet </v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -7530,7 +7524,7 @@
       </c>
       <c r="H22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>KO_sgA_branch</v>
+        <v>KO_sgA_R1_branch</v>
       </c>
       <c r="I22" t="str">
         <f ca="1">OFFSET('1'!$I$1, 4 * (A22 - 1)  + ($I$2), 0)</f>
@@ -7566,7 +7560,7 @@
       </c>
       <c r="Q22" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -in ", dirs!$A$2, "/", I22, ".tsv ", dirs!$A$2, "/", K22, ".tsv ", dirs!$A$2, "/", M22, ".tsv ", dirs!$A$2, "/", O22, ".tsv --total_reads ", J22, " ", L22, " ", N22, " ", P22, " -o ", dirs!$A$3, "/", H22, ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl296_KO_sgA_R1_branch.tsv libraries_2/yjl297_KO_sgA_R1_branch.tsv libraries_2/yjl298_KO_sgA_R1_branch.tsv libraries_2/yjl299_KO_sgA_R1_branch.tsv --total_reads 96 97 98 99 -o libraries_3/KO_sgA_branch.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl296_KO_sgA_R1_branch.tsv libraries_2/yjl297_KO_sgA_R1_branch.tsv libraries_2/yjl298_KO_sgA_R1_branch.tsv libraries_2/yjl299_KO_sgA_R1_branch.tsv --total_reads 96 97 98 99 -o libraries_3/KO_sgA_R1_branch.tsv --quiet </v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -7599,7 +7593,7 @@
       </c>
       <c r="H23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>KO_sgA_cmv</v>
+        <v>KO_sgA_R1_cmv</v>
       </c>
       <c r="I23" t="str">
         <f ca="1">OFFSET('1'!$I$1, 4 * (A23 - 1)  + ($I$2), 0)</f>
@@ -7635,7 +7629,7 @@
       </c>
       <c r="Q23" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -in ", dirs!$A$2, "/", I23, ".tsv ", dirs!$A$2, "/", K23, ".tsv ", dirs!$A$2, "/", M23, ".tsv ", dirs!$A$2, "/", O23, ".tsv --total_reads ", J23, " ", L23, " ", N23, " ", P23, " -o ", dirs!$A$3, "/", H23, ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl300_KO_sgA_R1_cmv.tsv libraries_2/yjl301_KO_sgA_R1_cmv.tsv libraries_2/yjl302_KO_sgA_R1_cmv.tsv libraries_2/yjl303_KO_sgA_R1_cmv.tsv --total_reads 96 97 98 99 -o libraries_3/KO_sgA_cmv.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl300_KO_sgA_R1_cmv.tsv libraries_2/yjl301_KO_sgA_R1_cmv.tsv libraries_2/yjl302_KO_sgA_R1_cmv.tsv libraries_2/yjl303_KO_sgA_R1_cmv.tsv --total_reads 96 97 98 99 -o libraries_3/KO_sgA_R1_cmv.tsv --quiet </v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -7668,7 +7662,7 @@
       </c>
       <c r="H24" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>KO_sgB_sense</v>
+        <v>KO_sgB_R2_sense</v>
       </c>
       <c r="I24" t="str">
         <f ca="1">OFFSET('1'!$I$1, 4 * (A24 - 1)  + ($I$2), 0)</f>
@@ -7704,7 +7698,7 @@
       </c>
       <c r="Q24" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -in ", dirs!$A$2, "/", I24, ".tsv ", dirs!$A$2, "/", K24, ".tsv ", dirs!$A$2, "/", M24, ".tsv ", dirs!$A$2, "/", O24, ".tsv --total_reads ", J24, " ", L24, " ", N24, " ", P24, " -o ", dirs!$A$3, "/", H24, ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl304_KO_sgB_R2_sense.tsv libraries_2/yjl305_KO_sgB_R2_sense.tsv libraries_2/yjl306_KO_sgB_R2_sense.tsv libraries_2/yjl307_KO_sgB_R2_sense.tsv --total_reads 96 97 98 99 -o libraries_3/KO_sgB_sense.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl304_KO_sgB_R2_sense.tsv libraries_2/yjl305_KO_sgB_R2_sense.tsv libraries_2/yjl306_KO_sgB_R2_sense.tsv libraries_2/yjl307_KO_sgB_R2_sense.tsv --total_reads 96 97 98 99 -o libraries_3/KO_sgB_R2_sense.tsv --quiet </v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -7737,7 +7731,7 @@
       </c>
       <c r="H25" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>KO_sgB_branch</v>
+        <v>KO_sgB_R2_branch</v>
       </c>
       <c r="I25" t="str">
         <f ca="1">OFFSET('1'!$I$1, 4 * (A25 - 1)  + ($I$2), 0)</f>
@@ -7773,7 +7767,7 @@
       </c>
       <c r="Q25" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -in ", dirs!$A$2, "/", I25, ".tsv ", dirs!$A$2, "/", K25, ".tsv ", dirs!$A$2, "/", M25, ".tsv ", dirs!$A$2, "/", O25, ".tsv --total_reads ", J25, " ", L25, " ", N25, " ", P25, " -o ", dirs!$A$3, "/", H25, ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl308_KO_sgB_R2_branch.tsv libraries_2/yjl309_KO_sgB_R2_branch.tsv libraries_2/yjl310_KO_sgB_R2_branch.tsv libraries_2/yjl311_KO_sgB_R2_branch.tsv --total_reads 96 97 98 99 -o libraries_3/KO_sgB_branch.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl308_KO_sgB_R2_branch.tsv libraries_2/yjl309_KO_sgB_R2_branch.tsv libraries_2/yjl310_KO_sgB_R2_branch.tsv libraries_2/yjl311_KO_sgB_R2_branch.tsv --total_reads 96 97 98 99 -o libraries_3/KO_sgB_R2_branch.tsv --quiet </v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -7806,7 +7800,7 @@
       </c>
       <c r="H26" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>KO_sgB_cmv</v>
+        <v>KO_sgB_R2_cmv</v>
       </c>
       <c r="I26" t="str">
         <f ca="1">OFFSET('1'!$I$1, 4 * (A26 - 1)  + ($I$2), 0)</f>
@@ -7842,7 +7836,7 @@
       </c>
       <c r="Q26" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -in ", dirs!$A$2, "/", I26, ".tsv ", dirs!$A$2, "/", K26, ".tsv ", dirs!$A$2, "/", M26, ".tsv ", dirs!$A$2, "/", O26, ".tsv --total_reads ", J26, " ", L26, " ", N26, " ", P26, " -o ", dirs!$A$3, "/", H26, ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl312_KO_sgB_R2_cmv.tsv libraries_2/yjl313_KO_sgB_R2_cmv.tsv libraries_2/yjl314_KO_sgB_R2_cmv.tsv libraries_2/yjl315_KO_sgB_R2_cmv.tsv --total_reads 96 97 98 99 -o libraries_3/KO_sgB_cmv.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl312_KO_sgB_R2_cmv.tsv libraries_2/yjl313_KO_sgB_R2_cmv.tsv libraries_2/yjl314_KO_sgB_R2_cmv.tsv libraries_2/yjl315_KO_sgB_R2_cmv.tsv --total_reads 96 97 98 99 -o libraries_3/KO_sgB_R2_cmv.tsv --quiet </v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -7875,7 +7869,7 @@
       </c>
       <c r="H27" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>WT_sgCD_antisense</v>
+        <v>WT_sgCD_R1_antisense</v>
       </c>
       <c r="I27" t="str">
         <f ca="1">OFFSET('1'!$I$1, 4 * (A27 - 1)  + ($I$2), 0)</f>
@@ -7911,7 +7905,7 @@
       </c>
       <c r="Q27" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -in ", dirs!$A$2, "/", I27, ".tsv ", dirs!$A$2, "/", K27, ".tsv ", dirs!$A$2, "/", M27, ".tsv ", dirs!$A$2, "/", O27, ".tsv --total_reads ", J27, " ", L27, " ", N27, " ", P27, " -o ", dirs!$A$3, "/", H27, ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl89_WT_sgCD_R1_antisense.tsv libraries_2/yjl90_WT_sgCD_R1_antisense.tsv libraries_2/yjl91_WT_sgCD_R1_antisense.tsv libraries_2/yjl92_WT_sgCD_R1_antisense.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgCD_antisense.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl89_WT_sgCD_R1_antisense.tsv libraries_2/yjl90_WT_sgCD_R1_antisense.tsv libraries_2/yjl91_WT_sgCD_R1_antisense.tsv libraries_2/yjl92_WT_sgCD_R1_antisense.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgCD_R1_antisense.tsv --quiet </v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -7944,7 +7938,7 @@
       </c>
       <c r="H28" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>WT_sgCD_splicing</v>
+        <v>WT_sgCD_R1_splicing</v>
       </c>
       <c r="I28" t="str">
         <f ca="1">OFFSET('1'!$I$1, 4 * (A28 - 1)  + ($I$2), 0)</f>
@@ -7980,7 +7974,7 @@
       </c>
       <c r="Q28" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -in ", dirs!$A$2, "/", I28, ".tsv ", dirs!$A$2, "/", K28, ".tsv ", dirs!$A$2, "/", M28, ".tsv ", dirs!$A$2, "/", O28, ".tsv --total_reads ", J28, " ", L28, " ", N28, " ", P28, " -o ", dirs!$A$3, "/", H28, ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl93_WT_sgCD_R1_splicing.tsv libraries_2/yjl94_WT_sgCD_R1_splicing.tsv libraries_2/yjl95_WT_sgCD_R1_splicing.tsv libraries_2/yjl96_WT_sgCD_R1_splicing.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgCD_splicing.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl93_WT_sgCD_R1_splicing.tsv libraries_2/yjl94_WT_sgCD_R1_splicing.tsv libraries_2/yjl95_WT_sgCD_R1_splicing.tsv libraries_2/yjl96_WT_sgCD_R1_splicing.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgCD_R1_splicing.tsv --quiet </v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -8013,7 +8007,7 @@
       </c>
       <c r="H29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>WT_sgCD_antisense</v>
+        <v>WT_sgCD_R2_antisense</v>
       </c>
       <c r="I29" t="str">
         <f ca="1">OFFSET('1'!$I$1, 4 * (A29 - 1)  + ($I$2), 0)</f>
@@ -8049,7 +8043,7 @@
       </c>
       <c r="Q29" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -in ", dirs!$A$2, "/", I29, ".tsv ", dirs!$A$2, "/", K29, ".tsv ", dirs!$A$2, "/", M29, ".tsv ", dirs!$A$2, "/", O29, ".tsv --total_reads ", J29, " ", L29, " ", N29, " ", P29, " -o ", dirs!$A$3, "/", H29, ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl89_WT_sgCD_R2_antisense.tsv libraries_2/yjl90_WT_sgCD_R2_antisense.tsv libraries_2/yjl91_WT_sgCD_R2_antisense.tsv libraries_2/yjl92_WT_sgCD_R2_antisense.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgCD_antisense.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl89_WT_sgCD_R2_antisense.tsv libraries_2/yjl90_WT_sgCD_R2_antisense.tsv libraries_2/yjl91_WT_sgCD_R2_antisense.tsv libraries_2/yjl92_WT_sgCD_R2_antisense.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgCD_R2_antisense.tsv --quiet </v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -8082,7 +8076,7 @@
       </c>
       <c r="H30" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>WT_sgCD_splicing</v>
+        <v>WT_sgCD_R2_splicing</v>
       </c>
       <c r="I30" t="str">
         <f ca="1">OFFSET('1'!$I$1, 4 * (A30 - 1)  + ($I$2), 0)</f>
@@ -8118,7 +8112,7 @@
       </c>
       <c r="Q30" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -in ", dirs!$A$2, "/", I30, ".tsv ", dirs!$A$2, "/", K30, ".tsv ", dirs!$A$2, "/", M30, ".tsv ", dirs!$A$2, "/", O30, ".tsv --total_reads ", J30, " ", L30, " ", N30, " ", P30, " -o ", dirs!$A$3, "/", H30, ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl93_WT_sgCD_R2_splicing.tsv libraries_2/yjl94_WT_sgCD_R2_splicing.tsv libraries_2/yjl95_WT_sgCD_R2_splicing.tsv libraries_2/yjl96_WT_sgCD_R2_splicing.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgCD_splicing.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -in libraries_2/yjl93_WT_sgCD_R2_splicing.tsv libraries_2/yjl94_WT_sgCD_R2_splicing.tsv libraries_2/yjl95_WT_sgCD_R2_splicing.tsv libraries_2/yjl96_WT_sgCD_R2_splicing.tsv --total_reads 96 97 98 99 -o libraries_3/WT_sgCD_R2_splicing.tsv --quiet </v>
       </c>
     </row>
   </sheetData>
@@ -8128,10 +8122,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7FB6E33-93C4-4971-BF44-23A0F65AADA0}">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8139,54 +8133,50 @@
     <col min="1" max="1" width="31.140625" customWidth="1"/>
     <col min="2" max="2" width="31.28515625" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="9" max="10" width="11.85546875" customWidth="1"/>
-    <col min="11" max="11" width="50.7109375" customWidth="1"/>
-    <col min="12" max="12" width="51" customWidth="1"/>
+    <col min="8" max="9" width="11.85546875" customWidth="1"/>
+    <col min="10" max="10" width="50.85546875" customWidth="1"/>
+    <col min="11" max="11" width="51" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="J1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f ca="1">'2'!H3</f>
-        <v>WT_sgAB_sense</v>
+        <v>WT_sgAB_R1_sense</v>
       </c>
       <c r="B2" t="str">
         <f ca="1">'2'!B3</f>
@@ -8200,41 +8190,38 @@
         <f ca="1">IF('2'!G3="2DSB", 2, 1)</f>
         <v>1</v>
       </c>
-      <c r="E2" t="s">
-        <v>108</v>
-      </c>
-      <c r="F2" t="str">
+      <c r="E2" t="str">
         <f ca="1">'2'!E3</f>
         <v>R1</v>
       </c>
+      <c r="F2" t="str">
+        <f ca="1">MID('2'!G3, 3, 100)</f>
+        <v>AB</v>
+      </c>
       <c r="G2" t="str">
-        <f ca="1">'2'!G3</f>
-        <v>sgAB</v>
-      </c>
-      <c r="H2" t="str">
         <f ca="1">'2'!D3</f>
         <v>WT</v>
       </c>
-      <c r="I2" t="str">
+      <c r="H2" t="str">
         <f ca="1">'2'!F3</f>
         <v>sense</v>
       </c>
-      <c r="J2" t="s">
-        <v>113</v>
+      <c r="I2" t="s">
+        <v>110</v>
+      </c>
+      <c r="J2" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A2, ".tsv -o ", dirs!$A$4, "/", A2, " -ref ref_seq/", B2, " -dsb ", C2, " --dsb_type ", D2, " --strand ", E2, " --hguide ", F2, " --cell ", G2, " --treatment ", H2, " --subst_type ", I2)</f>
+        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgAB_R1_sense.tsv -o libraries_4/WT_sgAB_R1_sense -ref ref_seq/2DSB_R1_sense.fa -dsb 67 --dsb_type 1 --strand R1 --hguide AB --cell WT --treatment sense --subst_type without</v>
       </c>
       <c r="K2" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A2, ".tsv -o ", dirs!$A$4, "/", A2, " -ref ref_seq/", B2, " -dsb ", C2, " --dsb_type ", D2, " --format ", E2, " --strand ", F2, " --hguide ", G2, " --cell ", H2, " --treatments ", I2, " --subst_type ", J2)</f>
-        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgAB_sense.tsv -o libraries_4/WT_sgAB_sense -ref ref_seq/2DSB_R1_sense.fa -dsb 67 --dsb_type 1 --format individual --strand R1 --hguide sgAB --cell WT --treatments sense --subst_type without</v>
-      </c>
-      <c r="L2" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A2)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgAB_sense</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgAB_R1_sense</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f ca="1">'2'!H4</f>
-        <v>WT_sgAB_branch</v>
+        <v>WT_sgAB_R1_branch</v>
       </c>
       <c r="B3" t="str">
         <f ca="1">'2'!B4</f>
@@ -8248,41 +8235,38 @@
         <f ca="1">IF('2'!G4="2DSB", 2, 1)</f>
         <v>1</v>
       </c>
-      <c r="E3" t="s">
-        <v>108</v>
-      </c>
-      <c r="F3" t="str">
+      <c r="E3" t="str">
         <f ca="1">'2'!E4</f>
         <v>R1</v>
       </c>
+      <c r="F3" t="str">
+        <f ca="1">MID('2'!G4, 3, 100)</f>
+        <v>AB</v>
+      </c>
       <c r="G3" t="str">
-        <f ca="1">'2'!G4</f>
-        <v>sgAB</v>
-      </c>
-      <c r="H3" t="str">
         <f ca="1">'2'!D4</f>
         <v>WT</v>
       </c>
-      <c r="I3" t="str">
+      <c r="H3" t="str">
         <f ca="1">'2'!F4</f>
         <v>branch</v>
       </c>
-      <c r="J3" t="s">
-        <v>113</v>
+      <c r="I3" t="s">
+        <v>110</v>
+      </c>
+      <c r="J3" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A3, ".tsv -o ", dirs!$A$4, "/", A3, " -ref ref_seq/", B3, " -dsb ", C3, " --dsb_type ", D3, " --strand ", E3, " --hguide ", F3, " --cell ", G3, " --treatment ", H3, " --subst_type ", I3)</f>
+        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgAB_R1_branch.tsv -o libraries_4/WT_sgAB_R1_branch -ref ref_seq/2DSB_R1_branch.fa -dsb 67 --dsb_type 1 --strand R1 --hguide AB --cell WT --treatment branch --subst_type without</v>
       </c>
       <c r="K3" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A3, ".tsv -o ", dirs!$A$4, "/", A3, " -ref ref_seq/", B3, " -dsb ", C3, " --dsb_type ", D3, " --format ", E3, " --strand ", F3, " --hguide ", G3, " --cell ", H3, " --treatments ", I3, " --subst_type ", J3)</f>
-        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgAB_branch.tsv -o libraries_4/WT_sgAB_branch -ref ref_seq/2DSB_R1_branch.fa -dsb 67 --dsb_type 1 --format individual --strand R1 --hguide sgAB --cell WT --treatments branch --subst_type without</v>
-      </c>
-      <c r="L3" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A3)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgAB_branch</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgAB_R1_branch</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f ca="1">'2'!H5</f>
-        <v>WT_sgAB_cmv</v>
+        <v>WT_sgAB_R1_cmv</v>
       </c>
       <c r="B4" t="str">
         <f ca="1">'2'!B5</f>
@@ -8296,41 +8280,38 @@
         <f ca="1">IF('2'!G5="2DSB", 2, 1)</f>
         <v>1</v>
       </c>
-      <c r="E4" t="s">
-        <v>108</v>
-      </c>
-      <c r="F4" t="str">
+      <c r="E4" t="str">
         <f ca="1">'2'!E5</f>
         <v>R1</v>
       </c>
+      <c r="F4" t="str">
+        <f ca="1">MID('2'!G5, 3, 100)</f>
+        <v>AB</v>
+      </c>
       <c r="G4" t="str">
-        <f ca="1">'2'!G5</f>
-        <v>sgAB</v>
-      </c>
-      <c r="H4" t="str">
         <f ca="1">'2'!D5</f>
         <v>WT</v>
       </c>
-      <c r="I4" t="str">
+      <c r="H4" t="str">
         <f ca="1">'2'!F5</f>
         <v>cmv</v>
       </c>
-      <c r="J4" t="s">
-        <v>113</v>
+      <c r="I4" t="s">
+        <v>110</v>
+      </c>
+      <c r="J4" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A4, ".tsv -o ", dirs!$A$4, "/", A4, " -ref ref_seq/", B4, " -dsb ", C4, " --dsb_type ", D4, " --strand ", E4, " --hguide ", F4, " --cell ", G4, " --treatment ", H4, " --subst_type ", I4)</f>
+        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgAB_R1_cmv.tsv -o libraries_4/WT_sgAB_R1_cmv -ref ref_seq/2DSB_R1_cmv.fa -dsb 67 --dsb_type 1 --strand R1 --hguide AB --cell WT --treatment cmv --subst_type without</v>
       </c>
       <c r="K4" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A4, ".tsv -o ", dirs!$A$4, "/", A4, " -ref ref_seq/", B4, " -dsb ", C4, " --dsb_type ", D4, " --format ", E4, " --strand ", F4, " --hguide ", G4, " --cell ", H4, " --treatments ", I4, " --subst_type ", J4)</f>
-        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgAB_cmv.tsv -o libraries_4/WT_sgAB_cmv -ref ref_seq/2DSB_R1_cmv.fa -dsb 67 --dsb_type 1 --format individual --strand R1 --hguide sgAB --cell WT --treatments cmv --subst_type without</v>
-      </c>
-      <c r="L4" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A4)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgAB_cmv</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgAB_R1_cmv</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f ca="1">'2'!H6</f>
-        <v>KO_sgAB_sense</v>
+        <v>KO_sgAB_R1_sense</v>
       </c>
       <c r="B5" t="str">
         <f ca="1">'2'!B6</f>
@@ -8344,41 +8325,38 @@
         <f ca="1">IF('2'!G6="2DSB", 2, 1)</f>
         <v>1</v>
       </c>
-      <c r="E5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F5" t="str">
+      <c r="E5" t="str">
         <f ca="1">'2'!E6</f>
         <v>R1</v>
       </c>
+      <c r="F5" t="str">
+        <f ca="1">MID('2'!G6, 3, 100)</f>
+        <v>AB</v>
+      </c>
       <c r="G5" t="str">
-        <f ca="1">'2'!G6</f>
-        <v>sgAB</v>
-      </c>
-      <c r="H5" t="str">
         <f ca="1">'2'!D6</f>
         <v>KO</v>
       </c>
-      <c r="I5" t="str">
+      <c r="H5" t="str">
         <f ca="1">'2'!F6</f>
         <v>sense</v>
       </c>
-      <c r="J5" t="s">
-        <v>113</v>
+      <c r="I5" t="s">
+        <v>110</v>
+      </c>
+      <c r="J5" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A5, ".tsv -o ", dirs!$A$4, "/", A5, " -ref ref_seq/", B5, " -dsb ", C5, " --dsb_type ", D5, " --strand ", E5, " --hguide ", F5, " --cell ", G5, " --treatment ", H5, " --subst_type ", I5)</f>
+        <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgAB_R1_sense.tsv -o libraries_4/KO_sgAB_R1_sense -ref ref_seq/2DSB_R1_sense.fa -dsb 67 --dsb_type 1 --strand R1 --hguide AB --cell KO --treatment sense --subst_type without</v>
       </c>
       <c r="K5" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A5, ".tsv -o ", dirs!$A$4, "/", A5, " -ref ref_seq/", B5, " -dsb ", C5, " --dsb_type ", D5, " --format ", E5, " --strand ", F5, " --hguide ", G5, " --cell ", H5, " --treatments ", I5, " --subst_type ", J5)</f>
-        <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgAB_sense.tsv -o libraries_4/KO_sgAB_sense -ref ref_seq/2DSB_R1_sense.fa -dsb 67 --dsb_type 1 --format individual --strand R1 --hguide sgAB --cell KO --treatments sense --subst_type without</v>
-      </c>
-      <c r="L5" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A5)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgAB_sense</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgAB_R1_sense</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f ca="1">'2'!H7</f>
-        <v>KO_sgAB_branch</v>
+        <v>KO_sgAB_R1_branch</v>
       </c>
       <c r="B6" t="str">
         <f ca="1">'2'!B7</f>
@@ -8392,41 +8370,38 @@
         <f ca="1">IF('2'!G7="2DSB", 2, 1)</f>
         <v>1</v>
       </c>
-      <c r="E6" t="s">
-        <v>108</v>
-      </c>
-      <c r="F6" t="str">
+      <c r="E6" t="str">
         <f ca="1">'2'!E7</f>
         <v>R1</v>
       </c>
+      <c r="F6" t="str">
+        <f ca="1">MID('2'!G7, 3, 100)</f>
+        <v>AB</v>
+      </c>
       <c r="G6" t="str">
-        <f ca="1">'2'!G7</f>
-        <v>sgAB</v>
-      </c>
-      <c r="H6" t="str">
         <f ca="1">'2'!D7</f>
         <v>KO</v>
       </c>
-      <c r="I6" t="str">
+      <c r="H6" t="str">
         <f ca="1">'2'!F7</f>
         <v>branch</v>
       </c>
-      <c r="J6" t="s">
-        <v>113</v>
+      <c r="I6" t="s">
+        <v>110</v>
+      </c>
+      <c r="J6" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A6, ".tsv -o ", dirs!$A$4, "/", A6, " -ref ref_seq/", B6, " -dsb ", C6, " --dsb_type ", D6, " --strand ", E6, " --hguide ", F6, " --cell ", G6, " --treatment ", H6, " --subst_type ", I6)</f>
+        <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgAB_R1_branch.tsv -o libraries_4/KO_sgAB_R1_branch -ref ref_seq/2DSB_R1_branch.fa -dsb 67 --dsb_type 1 --strand R1 --hguide AB --cell KO --treatment branch --subst_type without</v>
       </c>
       <c r="K6" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A6, ".tsv -o ", dirs!$A$4, "/", A6, " -ref ref_seq/", B6, " -dsb ", C6, " --dsb_type ", D6, " --format ", E6, " --strand ", F6, " --hguide ", G6, " --cell ", H6, " --treatments ", I6, " --subst_type ", J6)</f>
-        <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgAB_branch.tsv -o libraries_4/KO_sgAB_branch -ref ref_seq/2DSB_R1_branch.fa -dsb 67 --dsb_type 1 --format individual --strand R1 --hguide sgAB --cell KO --treatments branch --subst_type without</v>
-      </c>
-      <c r="L6" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A6)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgAB_branch</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgAB_R1_branch</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f ca="1">'2'!H8</f>
-        <v>KO_sgAB_cmv</v>
+        <v>KO_sgAB_R1_cmv</v>
       </c>
       <c r="B7" t="str">
         <f ca="1">'2'!B8</f>
@@ -8440,41 +8415,38 @@
         <f ca="1">IF('2'!G8="2DSB", 2, 1)</f>
         <v>1</v>
       </c>
-      <c r="E7" t="s">
-        <v>108</v>
-      </c>
-      <c r="F7" t="str">
+      <c r="E7" t="str">
         <f ca="1">'2'!E8</f>
         <v>R1</v>
       </c>
+      <c r="F7" t="str">
+        <f ca="1">MID('2'!G8, 3, 100)</f>
+        <v>AB</v>
+      </c>
       <c r="G7" t="str">
-        <f ca="1">'2'!G8</f>
-        <v>sgAB</v>
-      </c>
-      <c r="H7" t="str">
         <f ca="1">'2'!D8</f>
         <v>KO</v>
       </c>
-      <c r="I7" t="str">
+      <c r="H7" t="str">
         <f ca="1">'2'!F8</f>
         <v>cmv</v>
       </c>
-      <c r="J7" t="s">
-        <v>113</v>
+      <c r="I7" t="s">
+        <v>110</v>
+      </c>
+      <c r="J7" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A7, ".tsv -o ", dirs!$A$4, "/", A7, " -ref ref_seq/", B7, " -dsb ", C7, " --dsb_type ", D7, " --strand ", E7, " --hguide ", F7, " --cell ", G7, " --treatment ", H7, " --subst_type ", I7)</f>
+        <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgAB_R1_cmv.tsv -o libraries_4/KO_sgAB_R1_cmv -ref ref_seq/2DSB_R1_cmv.fa -dsb 67 --dsb_type 1 --strand R1 --hguide AB --cell KO --treatment cmv --subst_type without</v>
       </c>
       <c r="K7" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A7, ".tsv -o ", dirs!$A$4, "/", A7, " -ref ref_seq/", B7, " -dsb ", C7, " --dsb_type ", D7, " --format ", E7, " --strand ", F7, " --hguide ", G7, " --cell ", H7, " --treatments ", I7, " --subst_type ", J7)</f>
-        <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgAB_cmv.tsv -o libraries_4/KO_sgAB_cmv -ref ref_seq/2DSB_R1_cmv.fa -dsb 67 --dsb_type 1 --format individual --strand R1 --hguide sgAB --cell KO --treatments cmv --subst_type without</v>
-      </c>
-      <c r="L7" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A7)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgAB_cmv</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgAB_R1_cmv</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f ca="1">'2'!H9</f>
-        <v>WT_sgAB_sense</v>
+        <v>WT_sgAB_R2_sense</v>
       </c>
       <c r="B8" t="str">
         <f ca="1">'2'!B9</f>
@@ -8488,41 +8460,38 @@
         <f ca="1">IF('2'!G9="2DSB", 2, 1)</f>
         <v>1</v>
       </c>
-      <c r="E8" t="s">
-        <v>108</v>
-      </c>
-      <c r="F8" t="str">
+      <c r="E8" t="str">
         <f ca="1">'2'!E9</f>
         <v>R2</v>
       </c>
+      <c r="F8" t="str">
+        <f ca="1">MID('2'!G9, 3, 100)</f>
+        <v>AB</v>
+      </c>
       <c r="G8" t="str">
-        <f ca="1">'2'!G9</f>
-        <v>sgAB</v>
-      </c>
-      <c r="H8" t="str">
         <f ca="1">'2'!D9</f>
         <v>WT</v>
       </c>
-      <c r="I8" t="str">
+      <c r="H8" t="str">
         <f ca="1">'2'!F9</f>
         <v>sense</v>
       </c>
-      <c r="J8" t="s">
-        <v>113</v>
+      <c r="I8" t="s">
+        <v>110</v>
+      </c>
+      <c r="J8" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A8, ".tsv -o ", dirs!$A$4, "/", A8, " -ref ref_seq/", B8, " -dsb ", C8, " --dsb_type ", D8, " --strand ", E8, " --hguide ", F8, " --cell ", G8, " --treatment ", H8, " --subst_type ", I8)</f>
+        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgAB_R2_sense.tsv -o libraries_4/WT_sgAB_R2_sense -ref ref_seq/2DSB_R2_sense.fa -dsb 46 --dsb_type 1 --strand R2 --hguide AB --cell WT --treatment sense --subst_type without</v>
       </c>
       <c r="K8" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A8, ".tsv -o ", dirs!$A$4, "/", A8, " -ref ref_seq/", B8, " -dsb ", C8, " --dsb_type ", D8, " --format ", E8, " --strand ", F8, " --hguide ", G8, " --cell ", H8, " --treatments ", I8, " --subst_type ", J8)</f>
-        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgAB_sense.tsv -o libraries_4/WT_sgAB_sense -ref ref_seq/2DSB_R2_sense.fa -dsb 46 --dsb_type 1 --format individual --strand R2 --hguide sgAB --cell WT --treatments sense --subst_type without</v>
-      </c>
-      <c r="L8" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A8)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgAB_sense</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgAB_R2_sense</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f ca="1">'2'!H10</f>
-        <v>WT_sgAB_branch</v>
+        <v>WT_sgAB_R2_branch</v>
       </c>
       <c r="B9" t="str">
         <f ca="1">'2'!B10</f>
@@ -8536,41 +8505,38 @@
         <f ca="1">IF('2'!G10="2DSB", 2, 1)</f>
         <v>1</v>
       </c>
-      <c r="E9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F9" t="str">
+      <c r="E9" t="str">
         <f ca="1">'2'!E10</f>
         <v>R2</v>
       </c>
+      <c r="F9" t="str">
+        <f ca="1">MID('2'!G10, 3, 100)</f>
+        <v>AB</v>
+      </c>
       <c r="G9" t="str">
-        <f ca="1">'2'!G10</f>
-        <v>sgAB</v>
-      </c>
-      <c r="H9" t="str">
         <f ca="1">'2'!D10</f>
         <v>WT</v>
       </c>
-      <c r="I9" t="str">
+      <c r="H9" t="str">
         <f ca="1">'2'!F10</f>
         <v>branch</v>
       </c>
-      <c r="J9" t="s">
-        <v>113</v>
+      <c r="I9" t="s">
+        <v>110</v>
+      </c>
+      <c r="J9" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A9, ".tsv -o ", dirs!$A$4, "/", A9, " -ref ref_seq/", B9, " -dsb ", C9, " --dsb_type ", D9, " --strand ", E9, " --hguide ", F9, " --cell ", G9, " --treatment ", H9, " --subst_type ", I9)</f>
+        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgAB_R2_branch.tsv -o libraries_4/WT_sgAB_R2_branch -ref ref_seq/2DSB_R2_branch.fa -dsb 46 --dsb_type 1 --strand R2 --hguide AB --cell WT --treatment branch --subst_type without</v>
       </c>
       <c r="K9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A9, ".tsv -o ", dirs!$A$4, "/", A9, " -ref ref_seq/", B9, " -dsb ", C9, " --dsb_type ", D9, " --format ", E9, " --strand ", F9, " --hguide ", G9, " --cell ", H9, " --treatments ", I9, " --subst_type ", J9)</f>
-        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgAB_branch.tsv -o libraries_4/WT_sgAB_branch -ref ref_seq/2DSB_R2_branch.fa -dsb 46 --dsb_type 1 --format individual --strand R2 --hguide sgAB --cell WT --treatments branch --subst_type without</v>
-      </c>
-      <c r="L9" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A9)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgAB_branch</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgAB_R2_branch</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f ca="1">'2'!H11</f>
-        <v>WT_sgAB_cmv</v>
+        <v>WT_sgAB_R2_cmv</v>
       </c>
       <c r="B10" t="str">
         <f ca="1">'2'!B11</f>
@@ -8584,41 +8550,38 @@
         <f ca="1">IF('2'!G11="2DSB", 2, 1)</f>
         <v>1</v>
       </c>
-      <c r="E10" t="s">
-        <v>108</v>
-      </c>
-      <c r="F10" t="str">
+      <c r="E10" t="str">
         <f ca="1">'2'!E11</f>
         <v>R2</v>
       </c>
+      <c r="F10" t="str">
+        <f ca="1">MID('2'!G11, 3, 100)</f>
+        <v>AB</v>
+      </c>
       <c r="G10" t="str">
-        <f ca="1">'2'!G11</f>
-        <v>sgAB</v>
-      </c>
-      <c r="H10" t="str">
         <f ca="1">'2'!D11</f>
         <v>WT</v>
       </c>
-      <c r="I10" t="str">
+      <c r="H10" t="str">
         <f ca="1">'2'!F11</f>
         <v>cmv</v>
       </c>
-      <c r="J10" t="s">
-        <v>113</v>
+      <c r="I10" t="s">
+        <v>110</v>
+      </c>
+      <c r="J10" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A10, ".tsv -o ", dirs!$A$4, "/", A10, " -ref ref_seq/", B10, " -dsb ", C10, " --dsb_type ", D10, " --strand ", E10, " --hguide ", F10, " --cell ", G10, " --treatment ", H10, " --subst_type ", I10)</f>
+        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgAB_R2_cmv.tsv -o libraries_4/WT_sgAB_R2_cmv -ref ref_seq/2DSB_R2_cmv.fa -dsb 46 --dsb_type 1 --strand R2 --hguide AB --cell WT --treatment cmv --subst_type without</v>
       </c>
       <c r="K10" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A10, ".tsv -o ", dirs!$A$4, "/", A10, " -ref ref_seq/", B10, " -dsb ", C10, " --dsb_type ", D10, " --format ", E10, " --strand ", F10, " --hguide ", G10, " --cell ", H10, " --treatments ", I10, " --subst_type ", J10)</f>
-        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgAB_cmv.tsv -o libraries_4/WT_sgAB_cmv -ref ref_seq/2DSB_R2_cmv.fa -dsb 46 --dsb_type 1 --format individual --strand R2 --hguide sgAB --cell WT --treatments cmv --subst_type without</v>
-      </c>
-      <c r="L10" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A10)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgAB_cmv</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgAB_R2_cmv</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f ca="1">'2'!H12</f>
-        <v>KO_sgAB_sense</v>
+        <v>KO_sgAB_R2_sense</v>
       </c>
       <c r="B11" t="str">
         <f ca="1">'2'!B12</f>
@@ -8632,41 +8595,38 @@
         <f ca="1">IF('2'!G12="2DSB", 2, 1)</f>
         <v>1</v>
       </c>
-      <c r="E11" t="s">
-        <v>108</v>
-      </c>
-      <c r="F11" t="str">
+      <c r="E11" t="str">
         <f ca="1">'2'!E12</f>
         <v>R2</v>
       </c>
+      <c r="F11" t="str">
+        <f ca="1">MID('2'!G12, 3, 100)</f>
+        <v>AB</v>
+      </c>
       <c r="G11" t="str">
-        <f ca="1">'2'!G12</f>
-        <v>sgAB</v>
-      </c>
-      <c r="H11" t="str">
         <f ca="1">'2'!D12</f>
         <v>KO</v>
       </c>
-      <c r="I11" t="str">
+      <c r="H11" t="str">
         <f ca="1">'2'!F12</f>
         <v>sense</v>
       </c>
-      <c r="J11" t="s">
-        <v>113</v>
+      <c r="I11" t="s">
+        <v>110</v>
+      </c>
+      <c r="J11" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A11, ".tsv -o ", dirs!$A$4, "/", A11, " -ref ref_seq/", B11, " -dsb ", C11, " --dsb_type ", D11, " --strand ", E11, " --hguide ", F11, " --cell ", G11, " --treatment ", H11, " --subst_type ", I11)</f>
+        <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgAB_R2_sense.tsv -o libraries_4/KO_sgAB_R2_sense -ref ref_seq/2DSB_R2_sense.fa -dsb 46 --dsb_type 1 --strand R2 --hguide AB --cell KO --treatment sense --subst_type without</v>
       </c>
       <c r="K11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A11, ".tsv -o ", dirs!$A$4, "/", A11, " -ref ref_seq/", B11, " -dsb ", C11, " --dsb_type ", D11, " --format ", E11, " --strand ", F11, " --hguide ", G11, " --cell ", H11, " --treatments ", I11, " --subst_type ", J11)</f>
-        <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgAB_sense.tsv -o libraries_4/KO_sgAB_sense -ref ref_seq/2DSB_R2_sense.fa -dsb 46 --dsb_type 1 --format individual --strand R2 --hguide sgAB --cell KO --treatments sense --subst_type without</v>
-      </c>
-      <c r="L11" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A11)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgAB_sense</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgAB_R2_sense</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f ca="1">'2'!H13</f>
-        <v>KO_sgAB_branch</v>
+        <v>KO_sgAB_R2_branch</v>
       </c>
       <c r="B12" t="str">
         <f ca="1">'2'!B13</f>
@@ -8680,41 +8640,38 @@
         <f ca="1">IF('2'!G13="2DSB", 2, 1)</f>
         <v>1</v>
       </c>
-      <c r="E12" t="s">
-        <v>108</v>
-      </c>
-      <c r="F12" t="str">
+      <c r="E12" t="str">
         <f ca="1">'2'!E13</f>
         <v>R2</v>
       </c>
+      <c r="F12" t="str">
+        <f ca="1">MID('2'!G13, 3, 100)</f>
+        <v>AB</v>
+      </c>
       <c r="G12" t="str">
-        <f ca="1">'2'!G13</f>
-        <v>sgAB</v>
-      </c>
-      <c r="H12" t="str">
         <f ca="1">'2'!D13</f>
         <v>KO</v>
       </c>
-      <c r="I12" t="str">
+      <c r="H12" t="str">
         <f ca="1">'2'!F13</f>
         <v>branch</v>
       </c>
-      <c r="J12" t="s">
-        <v>113</v>
+      <c r="I12" t="s">
+        <v>110</v>
+      </c>
+      <c r="J12" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A12, ".tsv -o ", dirs!$A$4, "/", A12, " -ref ref_seq/", B12, " -dsb ", C12, " --dsb_type ", D12, " --strand ", E12, " --hguide ", F12, " --cell ", G12, " --treatment ", H12, " --subst_type ", I12)</f>
+        <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgAB_R2_branch.tsv -o libraries_4/KO_sgAB_R2_branch -ref ref_seq/2DSB_R2_branch.fa -dsb 46 --dsb_type 1 --strand R2 --hguide AB --cell KO --treatment branch --subst_type without</v>
       </c>
       <c r="K12" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A12, ".tsv -o ", dirs!$A$4, "/", A12, " -ref ref_seq/", B12, " -dsb ", C12, " --dsb_type ", D12, " --format ", E12, " --strand ", F12, " --hguide ", G12, " --cell ", H12, " --treatments ", I12, " --subst_type ", J12)</f>
-        <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgAB_branch.tsv -o libraries_4/KO_sgAB_branch -ref ref_seq/2DSB_R2_branch.fa -dsb 46 --dsb_type 1 --format individual --strand R2 --hguide sgAB --cell KO --treatments branch --subst_type without</v>
-      </c>
-      <c r="L12" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A12)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgAB_branch</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgAB_R2_branch</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f ca="1">'2'!H14</f>
-        <v>KO_sgAB_cmv</v>
+        <v>KO_sgAB_R2_cmv</v>
       </c>
       <c r="B13" t="str">
         <f ca="1">'2'!B14</f>
@@ -8728,41 +8685,38 @@
         <f ca="1">IF('2'!G14="2DSB", 2, 1)</f>
         <v>1</v>
       </c>
-      <c r="E13" t="s">
-        <v>108</v>
-      </c>
-      <c r="F13" t="str">
+      <c r="E13" t="str">
         <f ca="1">'2'!E14</f>
         <v>R2</v>
       </c>
+      <c r="F13" t="str">
+        <f ca="1">MID('2'!G14, 3, 100)</f>
+        <v>AB</v>
+      </c>
       <c r="G13" t="str">
-        <f ca="1">'2'!G14</f>
-        <v>sgAB</v>
-      </c>
-      <c r="H13" t="str">
         <f ca="1">'2'!D14</f>
         <v>KO</v>
       </c>
-      <c r="I13" t="str">
+      <c r="H13" t="str">
         <f ca="1">'2'!F14</f>
         <v>cmv</v>
       </c>
-      <c r="J13" t="s">
-        <v>113</v>
+      <c r="I13" t="s">
+        <v>110</v>
+      </c>
+      <c r="J13" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A13, ".tsv -o ", dirs!$A$4, "/", A13, " -ref ref_seq/", B13, " -dsb ", C13, " --dsb_type ", D13, " --strand ", E13, " --hguide ", F13, " --cell ", G13, " --treatment ", H13, " --subst_type ", I13)</f>
+        <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgAB_R2_cmv.tsv -o libraries_4/KO_sgAB_R2_cmv -ref ref_seq/2DSB_R2_cmv.fa -dsb 46 --dsb_type 1 --strand R2 --hguide AB --cell KO --treatment cmv --subst_type without</v>
       </c>
       <c r="K13" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A13, ".tsv -o ", dirs!$A$4, "/", A13, " -ref ref_seq/", B13, " -dsb ", C13, " --dsb_type ", D13, " --format ", E13, " --strand ", F13, " --hguide ", G13, " --cell ", H13, " --treatments ", I13, " --subst_type ", J13)</f>
-        <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgAB_cmv.tsv -o libraries_4/KO_sgAB_cmv -ref ref_seq/2DSB_R2_cmv.fa -dsb 46 --dsb_type 1 --format individual --strand R2 --hguide sgAB --cell KO --treatments cmv --subst_type without</v>
-      </c>
-      <c r="L13" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A13)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgAB_cmv</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgAB_R2_cmv</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f ca="1">'2'!H15</f>
-        <v>WT_sgA_sense</v>
+        <v>WT_sgA_R1_sense</v>
       </c>
       <c r="B14" t="str">
         <f ca="1">'2'!B15</f>
@@ -8776,41 +8730,38 @@
         <f ca="1">IF('2'!G15="2DSB", 2, 1)</f>
         <v>1</v>
       </c>
-      <c r="E14" t="s">
-        <v>108</v>
-      </c>
-      <c r="F14" t="str">
+      <c r="E14" t="str">
         <f ca="1">'2'!E15</f>
         <v>R1</v>
       </c>
+      <c r="F14" t="str">
+        <f ca="1">MID('2'!G15, 3, 100)</f>
+        <v>A</v>
+      </c>
       <c r="G14" t="str">
-        <f ca="1">'2'!G15</f>
-        <v>sgA</v>
-      </c>
-      <c r="H14" t="str">
         <f ca="1">'2'!D15</f>
         <v>WT</v>
       </c>
-      <c r="I14" t="str">
+      <c r="H14" t="str">
         <f ca="1">'2'!F15</f>
         <v>sense</v>
       </c>
-      <c r="J14" t="s">
-        <v>113</v>
+      <c r="I14" t="s">
+        <v>110</v>
+      </c>
+      <c r="J14" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A14, ".tsv -o ", dirs!$A$4, "/", A14, " -ref ref_seq/", B14, " -dsb ", C14, " --dsb_type ", D14, " --strand ", E14, " --hguide ", F14, " --cell ", G14, " --treatment ", H14, " --subst_type ", I14)</f>
+        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgA_R1_sense.tsv -o libraries_4/WT_sgA_R1_sense -ref ref_seq/1DSB_R1_sense.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell WT --treatment sense --subst_type without</v>
       </c>
       <c r="K14" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A14, ".tsv -o ", dirs!$A$4, "/", A14, " -ref ref_seq/", B14, " -dsb ", C14, " --dsb_type ", D14, " --format ", E14, " --strand ", F14, " --hguide ", G14, " --cell ", H14, " --treatments ", I14, " --subst_type ", J14)</f>
-        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgA_sense.tsv -o libraries_4/WT_sgA_sense -ref ref_seq/1DSB_R1_sense.fa -dsb 67 --dsb_type 1 --format individual --strand R1 --hguide sgA --cell WT --treatments sense --subst_type without</v>
-      </c>
-      <c r="L14" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A14)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgA_sense</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgA_R1_sense</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f ca="1">'2'!H16</f>
-        <v>WT_sgA_branch</v>
+        <v>WT_sgA_R1_branch</v>
       </c>
       <c r="B15" t="str">
         <f ca="1">'2'!B16</f>
@@ -8824,41 +8775,38 @@
         <f ca="1">IF('2'!G16="2DSB", 2, 1)</f>
         <v>1</v>
       </c>
-      <c r="E15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F15" t="str">
+      <c r="E15" t="str">
         <f ca="1">'2'!E16</f>
         <v>R1</v>
       </c>
+      <c r="F15" t="str">
+        <f ca="1">MID('2'!G16, 3, 100)</f>
+        <v>A</v>
+      </c>
       <c r="G15" t="str">
-        <f ca="1">'2'!G16</f>
-        <v>sgA</v>
-      </c>
-      <c r="H15" t="str">
         <f ca="1">'2'!D16</f>
         <v>WT</v>
       </c>
-      <c r="I15" t="str">
+      <c r="H15" t="str">
         <f ca="1">'2'!F16</f>
         <v>branch</v>
       </c>
-      <c r="J15" t="s">
-        <v>113</v>
+      <c r="I15" t="s">
+        <v>110</v>
+      </c>
+      <c r="J15" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A15, ".tsv -o ", dirs!$A$4, "/", A15, " -ref ref_seq/", B15, " -dsb ", C15, " --dsb_type ", D15, " --strand ", E15, " --hguide ", F15, " --cell ", G15, " --treatment ", H15, " --subst_type ", I15)</f>
+        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgA_R1_branch.tsv -o libraries_4/WT_sgA_R1_branch -ref ref_seq/1DSB_R1_branch.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell WT --treatment branch --subst_type without</v>
       </c>
       <c r="K15" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A15, ".tsv -o ", dirs!$A$4, "/", A15, " -ref ref_seq/", B15, " -dsb ", C15, " --dsb_type ", D15, " --format ", E15, " --strand ", F15, " --hguide ", G15, " --cell ", H15, " --treatments ", I15, " --subst_type ", J15)</f>
-        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgA_branch.tsv -o libraries_4/WT_sgA_branch -ref ref_seq/1DSB_R1_branch.fa -dsb 67 --dsb_type 1 --format individual --strand R1 --hguide sgA --cell WT --treatments branch --subst_type without</v>
-      </c>
-      <c r="L15" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A15)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgA_branch</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgA_R1_branch</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f ca="1">'2'!H17</f>
-        <v>WT_sgA_cmv</v>
+        <v>WT_sgA_R1_cmv</v>
       </c>
       <c r="B16" t="str">
         <f ca="1">'2'!B17</f>
@@ -8872,41 +8820,38 @@
         <f ca="1">IF('2'!G17="2DSB", 2, 1)</f>
         <v>1</v>
       </c>
-      <c r="E16" t="s">
-        <v>108</v>
-      </c>
-      <c r="F16" t="str">
+      <c r="E16" t="str">
         <f ca="1">'2'!E17</f>
         <v>R1</v>
       </c>
+      <c r="F16" t="str">
+        <f ca="1">MID('2'!G17, 3, 100)</f>
+        <v>A</v>
+      </c>
       <c r="G16" t="str">
-        <f ca="1">'2'!G17</f>
-        <v>sgA</v>
-      </c>
-      <c r="H16" t="str">
         <f ca="1">'2'!D17</f>
         <v>WT</v>
       </c>
-      <c r="I16" t="str">
+      <c r="H16" t="str">
         <f ca="1">'2'!F17</f>
         <v>cmv</v>
       </c>
-      <c r="J16" t="s">
-        <v>113</v>
+      <c r="I16" t="s">
+        <v>110</v>
+      </c>
+      <c r="J16" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A16, ".tsv -o ", dirs!$A$4, "/", A16, " -ref ref_seq/", B16, " -dsb ", C16, " --dsb_type ", D16, " --strand ", E16, " --hguide ", F16, " --cell ", G16, " --treatment ", H16, " --subst_type ", I16)</f>
+        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgA_R1_cmv.tsv -o libraries_4/WT_sgA_R1_cmv -ref ref_seq/1DSB_R1_cmv.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell WT --treatment cmv --subst_type without</v>
       </c>
       <c r="K16" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A16, ".tsv -o ", dirs!$A$4, "/", A16, " -ref ref_seq/", B16, " -dsb ", C16, " --dsb_type ", D16, " --format ", E16, " --strand ", F16, " --hguide ", G16, " --cell ", H16, " --treatments ", I16, " --subst_type ", J16)</f>
-        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgA_cmv.tsv -o libraries_4/WT_sgA_cmv -ref ref_seq/1DSB_R1_cmv.fa -dsb 67 --dsb_type 1 --format individual --strand R1 --hguide sgA --cell WT --treatments cmv --subst_type without</v>
-      </c>
-      <c r="L16" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A16)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgA_cmv</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgA_R1_cmv</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f ca="1">'2'!H18</f>
-        <v>WT_sgB_sense</v>
+        <v>WT_sgB_R2_sense</v>
       </c>
       <c r="B17" t="str">
         <f ca="1">'2'!B18</f>
@@ -8920,41 +8865,38 @@
         <f ca="1">IF('2'!G18="2DSB", 2, 1)</f>
         <v>1</v>
       </c>
-      <c r="E17" t="s">
-        <v>108</v>
-      </c>
-      <c r="F17" t="str">
+      <c r="E17" t="str">
         <f ca="1">'2'!E18</f>
         <v>R2</v>
       </c>
+      <c r="F17" t="str">
+        <f ca="1">MID('2'!G18, 3, 100)</f>
+        <v>B</v>
+      </c>
       <c r="G17" t="str">
-        <f ca="1">'2'!G18</f>
-        <v>sgB</v>
-      </c>
-      <c r="H17" t="str">
         <f ca="1">'2'!D18</f>
         <v>WT</v>
       </c>
-      <c r="I17" t="str">
+      <c r="H17" t="str">
         <f ca="1">'2'!F18</f>
         <v>sense</v>
       </c>
-      <c r="J17" t="s">
-        <v>113</v>
+      <c r="I17" t="s">
+        <v>110</v>
+      </c>
+      <c r="J17" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A17, ".tsv -o ", dirs!$A$4, "/", A17, " -ref ref_seq/", B17, " -dsb ", C17, " --dsb_type ", D17, " --strand ", E17, " --hguide ", F17, " --cell ", G17, " --treatment ", H17, " --subst_type ", I17)</f>
+        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgB_R2_sense.tsv -o libraries_4/WT_sgB_R2_sense -ref ref_seq/1DSB_R2_sense.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell WT --treatment sense --subst_type without</v>
       </c>
       <c r="K17" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A17, ".tsv -o ", dirs!$A$4, "/", A17, " -ref ref_seq/", B17, " -dsb ", C17, " --dsb_type ", D17, " --format ", E17, " --strand ", F17, " --hguide ", G17, " --cell ", H17, " --treatments ", I17, " --subst_type ", J17)</f>
-        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgB_sense.tsv -o libraries_4/WT_sgB_sense -ref ref_seq/1DSB_R2_sense.fa -dsb 46 --dsb_type 1 --format individual --strand R2 --hguide sgB --cell WT --treatments sense --subst_type without</v>
-      </c>
-      <c r="L17" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A17)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgB_sense</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgB_R2_sense</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f ca="1">'2'!H19</f>
-        <v>WT_sgB_branch</v>
+        <v>WT_sgB_R2_branch</v>
       </c>
       <c r="B18" t="str">
         <f ca="1">'2'!B19</f>
@@ -8968,41 +8910,38 @@
         <f ca="1">IF('2'!G19="2DSB", 2, 1)</f>
         <v>1</v>
       </c>
-      <c r="E18" t="s">
-        <v>108</v>
-      </c>
-      <c r="F18" t="str">
+      <c r="E18" t="str">
         <f ca="1">'2'!E19</f>
         <v>R2</v>
       </c>
+      <c r="F18" t="str">
+        <f ca="1">MID('2'!G19, 3, 100)</f>
+        <v>B</v>
+      </c>
       <c r="G18" t="str">
-        <f ca="1">'2'!G19</f>
-        <v>sgB</v>
-      </c>
-      <c r="H18" t="str">
         <f ca="1">'2'!D19</f>
         <v>WT</v>
       </c>
-      <c r="I18" t="str">
+      <c r="H18" t="str">
         <f ca="1">'2'!F19</f>
         <v>branch</v>
       </c>
-      <c r="J18" t="s">
-        <v>113</v>
+      <c r="I18" t="s">
+        <v>110</v>
+      </c>
+      <c r="J18" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A18, ".tsv -o ", dirs!$A$4, "/", A18, " -ref ref_seq/", B18, " -dsb ", C18, " --dsb_type ", D18, " --strand ", E18, " --hguide ", F18, " --cell ", G18, " --treatment ", H18, " --subst_type ", I18)</f>
+        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgB_R2_branch.tsv -o libraries_4/WT_sgB_R2_branch -ref ref_seq/1DSB_R2_branch.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell WT --treatment branch --subst_type without</v>
       </c>
       <c r="K18" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A18, ".tsv -o ", dirs!$A$4, "/", A18, " -ref ref_seq/", B18, " -dsb ", C18, " --dsb_type ", D18, " --format ", E18, " --strand ", F18, " --hguide ", G18, " --cell ", H18, " --treatments ", I18, " --subst_type ", J18)</f>
-        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgB_branch.tsv -o libraries_4/WT_sgB_branch -ref ref_seq/1DSB_R2_branch.fa -dsb 46 --dsb_type 1 --format individual --strand R2 --hguide sgB --cell WT --treatments branch --subst_type without</v>
-      </c>
-      <c r="L18" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A18)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgB_branch</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgB_R2_branch</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f ca="1">'2'!H20</f>
-        <v>WT_sgB_cmv</v>
+        <v>WT_sgB_R2_cmv</v>
       </c>
       <c r="B19" t="str">
         <f ca="1">'2'!B20</f>
@@ -9016,41 +8955,38 @@
         <f ca="1">IF('2'!G20="2DSB", 2, 1)</f>
         <v>1</v>
       </c>
-      <c r="E19" t="s">
-        <v>108</v>
-      </c>
-      <c r="F19" t="str">
+      <c r="E19" t="str">
         <f ca="1">'2'!E20</f>
         <v>R2</v>
       </c>
+      <c r="F19" t="str">
+        <f ca="1">MID('2'!G20, 3, 100)</f>
+        <v>B</v>
+      </c>
       <c r="G19" t="str">
-        <f ca="1">'2'!G20</f>
-        <v>sgB</v>
-      </c>
-      <c r="H19" t="str">
         <f ca="1">'2'!D20</f>
         <v>WT</v>
       </c>
-      <c r="I19" t="str">
+      <c r="H19" t="str">
         <f ca="1">'2'!F20</f>
         <v>cmv</v>
       </c>
-      <c r="J19" t="s">
-        <v>113</v>
+      <c r="I19" t="s">
+        <v>110</v>
+      </c>
+      <c r="J19" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A19, ".tsv -o ", dirs!$A$4, "/", A19, " -ref ref_seq/", B19, " -dsb ", C19, " --dsb_type ", D19, " --strand ", E19, " --hguide ", F19, " --cell ", G19, " --treatment ", H19, " --subst_type ", I19)</f>
+        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgB_R2_cmv.tsv -o libraries_4/WT_sgB_R2_cmv -ref ref_seq/1DSB_R2_cmv.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell WT --treatment cmv --subst_type without</v>
       </c>
       <c r="K19" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A19, ".tsv -o ", dirs!$A$4, "/", A19, " -ref ref_seq/", B19, " -dsb ", C19, " --dsb_type ", D19, " --format ", E19, " --strand ", F19, " --hguide ", G19, " --cell ", H19, " --treatments ", I19, " --subst_type ", J19)</f>
-        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgB_cmv.tsv -o libraries_4/WT_sgB_cmv -ref ref_seq/1DSB_R2_cmv.fa -dsb 46 --dsb_type 1 --format individual --strand R2 --hguide sgB --cell WT --treatments cmv --subst_type without</v>
-      </c>
-      <c r="L19" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A19)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgB_cmv</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgB_R2_cmv</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f ca="1">'2'!H21</f>
-        <v>KO_sgA_sense</v>
+        <v>KO_sgA_R1_sense</v>
       </c>
       <c r="B20" t="str">
         <f ca="1">'2'!B21</f>
@@ -9064,41 +9000,38 @@
         <f ca="1">IF('2'!G21="2DSB", 2, 1)</f>
         <v>1</v>
       </c>
-      <c r="E20" t="s">
-        <v>108</v>
-      </c>
-      <c r="F20" t="str">
+      <c r="E20" t="str">
         <f ca="1">'2'!E21</f>
         <v>R1</v>
       </c>
+      <c r="F20" t="str">
+        <f ca="1">MID('2'!G21, 3, 100)</f>
+        <v>A</v>
+      </c>
       <c r="G20" t="str">
-        <f ca="1">'2'!G21</f>
-        <v>sgA</v>
-      </c>
-      <c r="H20" t="str">
         <f ca="1">'2'!D21</f>
         <v>KO</v>
       </c>
-      <c r="I20" t="str">
+      <c r="H20" t="str">
         <f ca="1">'2'!F21</f>
         <v>sense</v>
       </c>
-      <c r="J20" t="s">
-        <v>113</v>
+      <c r="I20" t="s">
+        <v>110</v>
+      </c>
+      <c r="J20" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A20, ".tsv -o ", dirs!$A$4, "/", A20, " -ref ref_seq/", B20, " -dsb ", C20, " --dsb_type ", D20, " --strand ", E20, " --hguide ", F20, " --cell ", G20, " --treatment ", H20, " --subst_type ", I20)</f>
+        <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgA_R1_sense.tsv -o libraries_4/KO_sgA_R1_sense -ref ref_seq/1DSB_R1_sense.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell KO --treatment sense --subst_type without</v>
       </c>
       <c r="K20" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A20, ".tsv -o ", dirs!$A$4, "/", A20, " -ref ref_seq/", B20, " -dsb ", C20, " --dsb_type ", D20, " --format ", E20, " --strand ", F20, " --hguide ", G20, " --cell ", H20, " --treatments ", I20, " --subst_type ", J20)</f>
-        <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgA_sense.tsv -o libraries_4/KO_sgA_sense -ref ref_seq/1DSB_R1_sense.fa -dsb 67 --dsb_type 1 --format individual --strand R1 --hguide sgA --cell KO --treatments sense --subst_type without</v>
-      </c>
-      <c r="L20" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A20)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgA_sense</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgA_R1_sense</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f ca="1">'2'!H22</f>
-        <v>KO_sgA_branch</v>
+        <v>KO_sgA_R1_branch</v>
       </c>
       <c r="B21" t="str">
         <f ca="1">'2'!B22</f>
@@ -9112,41 +9045,38 @@
         <f ca="1">IF('2'!G22="2DSB", 2, 1)</f>
         <v>1</v>
       </c>
-      <c r="E21" t="s">
-        <v>108</v>
-      </c>
-      <c r="F21" t="str">
+      <c r="E21" t="str">
         <f ca="1">'2'!E22</f>
         <v>R1</v>
       </c>
+      <c r="F21" t="str">
+        <f ca="1">MID('2'!G22, 3, 100)</f>
+        <v>A</v>
+      </c>
       <c r="G21" t="str">
-        <f ca="1">'2'!G22</f>
-        <v>sgA</v>
-      </c>
-      <c r="H21" t="str">
         <f ca="1">'2'!D22</f>
         <v>KO</v>
       </c>
-      <c r="I21" t="str">
+      <c r="H21" t="str">
         <f ca="1">'2'!F22</f>
         <v>branch</v>
       </c>
-      <c r="J21" t="s">
-        <v>113</v>
+      <c r="I21" t="s">
+        <v>110</v>
+      </c>
+      <c r="J21" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A21, ".tsv -o ", dirs!$A$4, "/", A21, " -ref ref_seq/", B21, " -dsb ", C21, " --dsb_type ", D21, " --strand ", E21, " --hguide ", F21, " --cell ", G21, " --treatment ", H21, " --subst_type ", I21)</f>
+        <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgA_R1_branch.tsv -o libraries_4/KO_sgA_R1_branch -ref ref_seq/1DSB_R1_branch.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell KO --treatment branch --subst_type without</v>
       </c>
       <c r="K21" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A21, ".tsv -o ", dirs!$A$4, "/", A21, " -ref ref_seq/", B21, " -dsb ", C21, " --dsb_type ", D21, " --format ", E21, " --strand ", F21, " --hguide ", G21, " --cell ", H21, " --treatments ", I21, " --subst_type ", J21)</f>
-        <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgA_branch.tsv -o libraries_4/KO_sgA_branch -ref ref_seq/1DSB_R1_branch.fa -dsb 67 --dsb_type 1 --format individual --strand R1 --hguide sgA --cell KO --treatments branch --subst_type without</v>
-      </c>
-      <c r="L21" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A21)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgA_branch</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgA_R1_branch</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f ca="1">'2'!H23</f>
-        <v>KO_sgA_cmv</v>
+        <v>KO_sgA_R1_cmv</v>
       </c>
       <c r="B22" t="str">
         <f ca="1">'2'!B23</f>
@@ -9160,41 +9090,38 @@
         <f ca="1">IF('2'!G23="2DSB", 2, 1)</f>
         <v>1</v>
       </c>
-      <c r="E22" t="s">
-        <v>108</v>
-      </c>
-      <c r="F22" t="str">
+      <c r="E22" t="str">
         <f ca="1">'2'!E23</f>
         <v>R1</v>
       </c>
+      <c r="F22" t="str">
+        <f ca="1">MID('2'!G23, 3, 100)</f>
+        <v>A</v>
+      </c>
       <c r="G22" t="str">
-        <f ca="1">'2'!G23</f>
-        <v>sgA</v>
-      </c>
-      <c r="H22" t="str">
         <f ca="1">'2'!D23</f>
         <v>KO</v>
       </c>
-      <c r="I22" t="str">
+      <c r="H22" t="str">
         <f ca="1">'2'!F23</f>
         <v>cmv</v>
       </c>
-      <c r="J22" t="s">
-        <v>113</v>
+      <c r="I22" t="s">
+        <v>110</v>
+      </c>
+      <c r="J22" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A22, ".tsv -o ", dirs!$A$4, "/", A22, " -ref ref_seq/", B22, " -dsb ", C22, " --dsb_type ", D22, " --strand ", E22, " --hguide ", F22, " --cell ", G22, " --treatment ", H22, " --subst_type ", I22)</f>
+        <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgA_R1_cmv.tsv -o libraries_4/KO_sgA_R1_cmv -ref ref_seq/1DSB_R1_cmv.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell KO --treatment cmv --subst_type without</v>
       </c>
       <c r="K22" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A22, ".tsv -o ", dirs!$A$4, "/", A22, " -ref ref_seq/", B22, " -dsb ", C22, " --dsb_type ", D22, " --format ", E22, " --strand ", F22, " --hguide ", G22, " --cell ", H22, " --treatments ", I22, " --subst_type ", J22)</f>
-        <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgA_cmv.tsv -o libraries_4/KO_sgA_cmv -ref ref_seq/1DSB_R1_cmv.fa -dsb 67 --dsb_type 1 --format individual --strand R1 --hguide sgA --cell KO --treatments cmv --subst_type without</v>
-      </c>
-      <c r="L22" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A22)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgA_cmv</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgA_R1_cmv</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f ca="1">'2'!H24</f>
-        <v>KO_sgB_sense</v>
+        <v>KO_sgB_R2_sense</v>
       </c>
       <c r="B23" t="str">
         <f ca="1">'2'!B24</f>
@@ -9208,41 +9135,38 @@
         <f ca="1">IF('2'!G24="2DSB", 2, 1)</f>
         <v>1</v>
       </c>
-      <c r="E23" t="s">
-        <v>108</v>
-      </c>
-      <c r="F23" t="str">
+      <c r="E23" t="str">
         <f ca="1">'2'!E24</f>
         <v>R2</v>
       </c>
+      <c r="F23" t="str">
+        <f ca="1">MID('2'!G24, 3, 100)</f>
+        <v>B</v>
+      </c>
       <c r="G23" t="str">
-        <f ca="1">'2'!G24</f>
-        <v>sgB</v>
-      </c>
-      <c r="H23" t="str">
         <f ca="1">'2'!D24</f>
         <v>KO</v>
       </c>
-      <c r="I23" t="str">
+      <c r="H23" t="str">
         <f ca="1">'2'!F24</f>
         <v>sense</v>
       </c>
-      <c r="J23" t="s">
-        <v>113</v>
+      <c r="I23" t="s">
+        <v>110</v>
+      </c>
+      <c r="J23" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A23, ".tsv -o ", dirs!$A$4, "/", A23, " -ref ref_seq/", B23, " -dsb ", C23, " --dsb_type ", D23, " --strand ", E23, " --hguide ", F23, " --cell ", G23, " --treatment ", H23, " --subst_type ", I23)</f>
+        <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgB_R2_sense.tsv -o libraries_4/KO_sgB_R2_sense -ref ref_seq/1DSB_R2_sense.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell KO --treatment sense --subst_type without</v>
       </c>
       <c r="K23" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A23, ".tsv -o ", dirs!$A$4, "/", A23, " -ref ref_seq/", B23, " -dsb ", C23, " --dsb_type ", D23, " --format ", E23, " --strand ", F23, " --hguide ", G23, " --cell ", H23, " --treatments ", I23, " --subst_type ", J23)</f>
-        <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgB_sense.tsv -o libraries_4/KO_sgB_sense -ref ref_seq/1DSB_R2_sense.fa -dsb 46 --dsb_type 1 --format individual --strand R2 --hguide sgB --cell KO --treatments sense --subst_type without</v>
-      </c>
-      <c r="L23" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A23)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgB_sense</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgB_R2_sense</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f ca="1">'2'!H25</f>
-        <v>KO_sgB_branch</v>
+        <v>KO_sgB_R2_branch</v>
       </c>
       <c r="B24" t="str">
         <f ca="1">'2'!B25</f>
@@ -9256,41 +9180,38 @@
         <f ca="1">IF('2'!G25="2DSB", 2, 1)</f>
         <v>1</v>
       </c>
-      <c r="E24" t="s">
-        <v>108</v>
-      </c>
-      <c r="F24" t="str">
+      <c r="E24" t="str">
         <f ca="1">'2'!E25</f>
         <v>R2</v>
       </c>
+      <c r="F24" t="str">
+        <f ca="1">MID('2'!G25, 3, 100)</f>
+        <v>B</v>
+      </c>
       <c r="G24" t="str">
-        <f ca="1">'2'!G25</f>
-        <v>sgB</v>
-      </c>
-      <c r="H24" t="str">
         <f ca="1">'2'!D25</f>
         <v>KO</v>
       </c>
-      <c r="I24" t="str">
+      <c r="H24" t="str">
         <f ca="1">'2'!F25</f>
         <v>branch</v>
       </c>
-      <c r="J24" t="s">
-        <v>113</v>
+      <c r="I24" t="s">
+        <v>110</v>
+      </c>
+      <c r="J24" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A24, ".tsv -o ", dirs!$A$4, "/", A24, " -ref ref_seq/", B24, " -dsb ", C24, " --dsb_type ", D24, " --strand ", E24, " --hguide ", F24, " --cell ", G24, " --treatment ", H24, " --subst_type ", I24)</f>
+        <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgB_R2_branch.tsv -o libraries_4/KO_sgB_R2_branch -ref ref_seq/1DSB_R2_branch.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell KO --treatment branch --subst_type without</v>
       </c>
       <c r="K24" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A24, ".tsv -o ", dirs!$A$4, "/", A24, " -ref ref_seq/", B24, " -dsb ", C24, " --dsb_type ", D24, " --format ", E24, " --strand ", F24, " --hguide ", G24, " --cell ", H24, " --treatments ", I24, " --subst_type ", J24)</f>
-        <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgB_branch.tsv -o libraries_4/KO_sgB_branch -ref ref_seq/1DSB_R2_branch.fa -dsb 46 --dsb_type 1 --format individual --strand R2 --hguide sgB --cell KO --treatments branch --subst_type without</v>
-      </c>
-      <c r="L24" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A24)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgB_branch</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgB_R2_branch</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f ca="1">'2'!H26</f>
-        <v>KO_sgB_cmv</v>
+        <v>KO_sgB_R2_cmv</v>
       </c>
       <c r="B25" t="str">
         <f ca="1">'2'!B26</f>
@@ -9304,41 +9225,38 @@
         <f ca="1">IF('2'!G26="2DSB", 2, 1)</f>
         <v>1</v>
       </c>
-      <c r="E25" t="s">
-        <v>108</v>
-      </c>
-      <c r="F25" t="str">
+      <c r="E25" t="str">
         <f ca="1">'2'!E26</f>
         <v>R2</v>
       </c>
+      <c r="F25" t="str">
+        <f ca="1">MID('2'!G26, 3, 100)</f>
+        <v>B</v>
+      </c>
       <c r="G25" t="str">
-        <f ca="1">'2'!G26</f>
-        <v>sgB</v>
-      </c>
-      <c r="H25" t="str">
         <f ca="1">'2'!D26</f>
         <v>KO</v>
       </c>
-      <c r="I25" t="str">
+      <c r="H25" t="str">
         <f ca="1">'2'!F26</f>
         <v>cmv</v>
       </c>
-      <c r="J25" t="s">
-        <v>113</v>
+      <c r="I25" t="s">
+        <v>110</v>
+      </c>
+      <c r="J25" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A25, ".tsv -o ", dirs!$A$4, "/", A25, " -ref ref_seq/", B25, " -dsb ", C25, " --dsb_type ", D25, " --strand ", E25, " --hguide ", F25, " --cell ", G25, " --treatment ", H25, " --subst_type ", I25)</f>
+        <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgB_R2_cmv.tsv -o libraries_4/KO_sgB_R2_cmv -ref ref_seq/1DSB_R2_cmv.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell KO --treatment cmv --subst_type without</v>
       </c>
       <c r="K25" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A25, ".tsv -o ", dirs!$A$4, "/", A25, " -ref ref_seq/", B25, " -dsb ", C25, " --dsb_type ", D25, " --format ", E25, " --strand ", F25, " --hguide ", G25, " --cell ", H25, " --treatments ", I25, " --subst_type ", J25)</f>
-        <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgB_cmv.tsv -o libraries_4/KO_sgB_cmv -ref ref_seq/1DSB_R2_cmv.fa -dsb 46 --dsb_type 1 --format individual --strand R2 --hguide sgB --cell KO --treatments cmv --subst_type without</v>
-      </c>
-      <c r="L25" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A25)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgB_cmv</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgB_R2_cmv</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f ca="1">'2'!H27</f>
-        <v>WT_sgCD_antisense</v>
+        <v>WT_sgCD_R1_antisense</v>
       </c>
       <c r="B26" t="str">
         <f ca="1">'2'!B27</f>
@@ -9352,41 +9270,38 @@
         <f ca="1">IF('2'!G27="2DSB", 2, 1)</f>
         <v>1</v>
       </c>
-      <c r="E26" t="s">
-        <v>108</v>
-      </c>
-      <c r="F26" t="str">
+      <c r="E26" t="str">
         <f ca="1">'2'!E27</f>
         <v>R1</v>
       </c>
+      <c r="F26" t="str">
+        <f ca="1">MID('2'!G27, 3, 100)</f>
+        <v>CD</v>
+      </c>
       <c r="G26" t="str">
-        <f ca="1">'2'!G27</f>
-        <v>sgCD</v>
-      </c>
-      <c r="H26" t="str">
         <f ca="1">'2'!D27</f>
         <v>WT</v>
       </c>
-      <c r="I26" t="str">
+      <c r="H26" t="str">
         <f ca="1">'2'!F27</f>
         <v>antisense</v>
       </c>
-      <c r="J26" t="s">
-        <v>113</v>
+      <c r="I26" t="s">
+        <v>110</v>
+      </c>
+      <c r="J26" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A26, ".tsv -o ", dirs!$A$4, "/", A26, " -ref ref_seq/", B26, " -dsb ", C26, " --dsb_type ", D26, " --strand ", E26, " --hguide ", F26, " --cell ", G26, " --treatment ", H26, " --subst_type ", I26)</f>
+        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgCD_R1_antisense.tsv -o libraries_4/WT_sgCD_R1_antisense -ref ref_seq/2DSBanti_R1_antisense.fa -dsb 50 --dsb_type 1 --strand R1 --hguide CD --cell WT --treatment antisense --subst_type without</v>
       </c>
       <c r="K26" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A26, ".tsv -o ", dirs!$A$4, "/", A26, " -ref ref_seq/", B26, " -dsb ", C26, " --dsb_type ", D26, " --format ", E26, " --strand ", F26, " --hguide ", G26, " --cell ", H26, " --treatments ", I26, " --subst_type ", J26)</f>
-        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgCD_antisense.tsv -o libraries_4/WT_sgCD_antisense -ref ref_seq/2DSBanti_R1_antisense.fa -dsb 50 --dsb_type 1 --format individual --strand R1 --hguide sgCD --cell WT --treatments antisense --subst_type without</v>
-      </c>
-      <c r="L26" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A26)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgCD_antisense</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgCD_R1_antisense</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f ca="1">'2'!H28</f>
-        <v>WT_sgCD_splicing</v>
+        <v>WT_sgCD_R1_splicing</v>
       </c>
       <c r="B27" t="str">
         <f ca="1">'2'!B28</f>
@@ -9400,41 +9315,38 @@
         <f ca="1">IF('2'!G28="2DSB", 2, 1)</f>
         <v>1</v>
       </c>
-      <c r="E27" t="s">
-        <v>108</v>
-      </c>
-      <c r="F27" t="str">
+      <c r="E27" t="str">
         <f ca="1">'2'!E28</f>
         <v>R1</v>
       </c>
+      <c r="F27" t="str">
+        <f ca="1">MID('2'!G28, 3, 100)</f>
+        <v>CD</v>
+      </c>
       <c r="G27" t="str">
-        <f ca="1">'2'!G28</f>
-        <v>sgCD</v>
-      </c>
-      <c r="H27" t="str">
         <f ca="1">'2'!D28</f>
         <v>WT</v>
       </c>
-      <c r="I27" t="str">
+      <c r="H27" t="str">
         <f ca="1">'2'!F28</f>
         <v>splicing</v>
       </c>
-      <c r="J27" t="s">
-        <v>113</v>
+      <c r="I27" t="s">
+        <v>110</v>
+      </c>
+      <c r="J27" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A27, ".tsv -o ", dirs!$A$4, "/", A27, " -ref ref_seq/", B27, " -dsb ", C27, " --dsb_type ", D27, " --strand ", E27, " --hguide ", F27, " --cell ", G27, " --treatment ", H27, " --subst_type ", I27)</f>
+        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgCD_R1_splicing.tsv -o libraries_4/WT_sgCD_R1_splicing -ref ref_seq/2DSBanti_R1_splicing.fa -dsb 50 --dsb_type 1 --strand R1 --hguide CD --cell WT --treatment splicing --subst_type without</v>
       </c>
       <c r="K27" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A27, ".tsv -o ", dirs!$A$4, "/", A27, " -ref ref_seq/", B27, " -dsb ", C27, " --dsb_type ", D27, " --format ", E27, " --strand ", F27, " --hguide ", G27, " --cell ", H27, " --treatments ", I27, " --subst_type ", J27)</f>
-        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgCD_splicing.tsv -o libraries_4/WT_sgCD_splicing -ref ref_seq/2DSBanti_R1_splicing.fa -dsb 50 --dsb_type 1 --format individual --strand R1 --hguide sgCD --cell WT --treatments splicing --subst_type without</v>
-      </c>
-      <c r="L27" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A27)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgCD_splicing</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgCD_R1_splicing</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f ca="1">'2'!H29</f>
-        <v>WT_sgCD_antisense</v>
+        <v>WT_sgCD_R2_antisense</v>
       </c>
       <c r="B28" t="str">
         <f ca="1">'2'!B29</f>
@@ -9448,41 +9360,38 @@
         <f ca="1">IF('2'!G29="2DSB", 2, 1)</f>
         <v>1</v>
       </c>
-      <c r="E28" t="s">
-        <v>108</v>
-      </c>
-      <c r="F28" t="str">
+      <c r="E28" t="str">
         <f ca="1">'2'!E29</f>
         <v>R2</v>
       </c>
+      <c r="F28" t="str">
+        <f ca="1">MID('2'!G29, 3, 100)</f>
+        <v>CD</v>
+      </c>
       <c r="G28" t="str">
-        <f ca="1">'2'!G29</f>
-        <v>sgCD</v>
-      </c>
-      <c r="H28" t="str">
         <f ca="1">'2'!D29</f>
         <v>WT</v>
       </c>
-      <c r="I28" t="str">
+      <c r="H28" t="str">
         <f ca="1">'2'!F29</f>
         <v>antisense</v>
       </c>
-      <c r="J28" t="s">
-        <v>113</v>
+      <c r="I28" t="s">
+        <v>110</v>
+      </c>
+      <c r="J28" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A28, ".tsv -o ", dirs!$A$4, "/", A28, " -ref ref_seq/", B28, " -dsb ", C28, " --dsb_type ", D28, " --strand ", E28, " --hguide ", F28, " --cell ", G28, " --treatment ", H28, " --subst_type ", I28)</f>
+        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgCD_R2_antisense.tsv -o libraries_4/WT_sgCD_R2_antisense -ref ref_seq/2DSBanti_R2_antisense.fa -dsb 47 --dsb_type 1 --strand R2 --hguide CD --cell WT --treatment antisense --subst_type without</v>
       </c>
       <c r="K28" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A28, ".tsv -o ", dirs!$A$4, "/", A28, " -ref ref_seq/", B28, " -dsb ", C28, " --dsb_type ", D28, " --format ", E28, " --strand ", F28, " --hguide ", G28, " --cell ", H28, " --treatments ", I28, " --subst_type ", J28)</f>
-        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgCD_antisense.tsv -o libraries_4/WT_sgCD_antisense -ref ref_seq/2DSBanti_R2_antisense.fa -dsb 47 --dsb_type 1 --format individual --strand R2 --hguide sgCD --cell WT --treatments antisense --subst_type without</v>
-      </c>
-      <c r="L28" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A28)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgCD_antisense</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgCD_R2_antisense</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f ca="1">'2'!H30</f>
-        <v>WT_sgCD_splicing</v>
+        <v>WT_sgCD_R2_splicing</v>
       </c>
       <c r="B29" t="str">
         <f ca="1">'2'!B30</f>
@@ -9496,35 +9405,32 @@
         <f ca="1">IF('2'!G30="2DSB", 2, 1)</f>
         <v>1</v>
       </c>
-      <c r="E29" t="s">
-        <v>108</v>
-      </c>
-      <c r="F29" t="str">
+      <c r="E29" t="str">
         <f ca="1">'2'!E30</f>
         <v>R2</v>
       </c>
+      <c r="F29" t="str">
+        <f ca="1">MID('2'!G30, 3, 100)</f>
+        <v>CD</v>
+      </c>
       <c r="G29" t="str">
-        <f ca="1">'2'!G30</f>
-        <v>sgCD</v>
-      </c>
-      <c r="H29" t="str">
         <f ca="1">'2'!D30</f>
         <v>WT</v>
       </c>
-      <c r="I29" t="str">
+      <c r="H29" t="str">
         <f ca="1">'2'!F30</f>
         <v>splicing</v>
       </c>
-      <c r="J29" t="s">
-        <v>113</v>
+      <c r="I29" t="s">
+        <v>110</v>
+      </c>
+      <c r="J29" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A29, ".tsv -o ", dirs!$A$4, "/", A29, " -ref ref_seq/", B29, " -dsb ", C29, " --dsb_type ", D29, " --strand ", E29, " --hguide ", F29, " --cell ", G29, " --treatment ", H29, " --subst_type ", I29)</f>
+        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgCD_R2_splicing.tsv -o libraries_4/WT_sgCD_R2_splicing -ref ref_seq/2DSBanti_R2_splicing.fa -dsb 47 --dsb_type 1 --strand R2 --hguide CD --cell WT --treatment splicing --subst_type without</v>
       </c>
       <c r="K29" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-in ", dirs!$A$3, "/", '3'!A29, ".tsv -o ", dirs!$A$4, "/", A29, " -ref ref_seq/", B29, " -dsb ", C29, " --dsb_type ", D29, " --format ", E29, " --strand ", F29, " --hguide ", G29, " --cell ", H29, " --treatments ", I29, " --subst_type ", J29)</f>
-        <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgCD_splicing.tsv -o libraries_4/WT_sgCD_splicing -ref ref_seq/2DSBanti_R2_splicing.fa -dsb 47 --dsb_type 1 --format individual --strand R2 --hguide sgCD --cell WT --treatments splicing --subst_type without</v>
-      </c>
-      <c r="L29" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A29)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgCD_splicing</v>
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgCD_R2_splicing</v>
       </c>
     </row>
   </sheetData>
@@ -9552,22 +9458,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -9576,22 +9482,22 @@
       </c>
       <c r="B2" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A2 - 1), 0)</f>
-        <v>WT_sgAB_sense</v>
+        <v>WT_sgAB_R1_sense</v>
       </c>
       <c r="C2" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A2 - 1) + 1, 0)</f>
-        <v>WT_sgAB_branch</v>
+        <v>WT_sgAB_R1_branch</v>
       </c>
       <c r="D2" t="str">
         <f ca="1">_xlfn.CONCAT(B2, "_", "branch")</f>
-        <v>WT_sgAB_sense_branch</v>
+        <v>WT_sgAB_R1_sense_branch</v>
       </c>
       <c r="E2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F2" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B2, " ", dirs!$A$4, "/", C2, " ", " -o ", dirs!$A$4, "/", D2, " --subst_type ", E2)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgAB_sense libraries_4/WT_sgAB_branch  -o libraries_4/WT_sgAB_sense_branch --subst_type without</v>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgAB_R1_sense libraries_4/WT_sgAB_R1_branch  -o libraries_4/WT_sgAB_R1_sense_branch --subst_type without</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -9600,22 +9506,22 @@
       </c>
       <c r="B3" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A3 - 1), 0)</f>
-        <v>WT_sgAB_sense</v>
+        <v>WT_sgAB_R1_sense</v>
       </c>
       <c r="C3" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A3 - 1) + 2, 0)</f>
-        <v>WT_sgAB_cmv</v>
+        <v>WT_sgAB_R1_cmv</v>
       </c>
       <c r="D3" t="str">
         <f ca="1">_xlfn.CONCAT(B2, "_", "cmv")</f>
-        <v>WT_sgAB_sense_cmv</v>
+        <v>WT_sgAB_R1_sense_cmv</v>
       </c>
       <c r="E3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F3" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B3, " ", dirs!$A$4, "/", C3, " ", " -o ", dirs!$A$4, "/", D3, " --subst_type ", E3)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgAB_sense libraries_4/WT_sgAB_cmv  -o libraries_4/WT_sgAB_sense_cmv --subst_type without</v>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgAB_R1_sense libraries_4/WT_sgAB_R1_cmv  -o libraries_4/WT_sgAB_R1_sense_cmv --subst_type without</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -9624,22 +9530,22 @@
       </c>
       <c r="B4" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A4 - 1), 0)</f>
-        <v>KO_sgAB_sense</v>
+        <v>KO_sgAB_R1_sense</v>
       </c>
       <c r="C4" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A4 - 1) + 1, 0)</f>
-        <v>KO_sgAB_branch</v>
+        <v>KO_sgAB_R1_branch</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" ref="D4" ca="1" si="0">_xlfn.CONCAT(B4, "_", "branch")</f>
-        <v>KO_sgAB_sense_branch</v>
+        <v>KO_sgAB_R1_sense_branch</v>
       </c>
       <c r="E4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F4" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B4, " ", dirs!$A$4, "/", C4, " ", " -o ", dirs!$A$4, "/", D4, " --subst_type ", E4)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgAB_sense libraries_4/KO_sgAB_branch  -o libraries_4/KO_sgAB_sense_branch --subst_type without</v>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgAB_R1_sense libraries_4/KO_sgAB_R1_branch  -o libraries_4/KO_sgAB_R1_sense_branch --subst_type without</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -9648,22 +9554,22 @@
       </c>
       <c r="B5" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A5 - 1), 0)</f>
-        <v>KO_sgAB_sense</v>
+        <v>KO_sgAB_R1_sense</v>
       </c>
       <c r="C5" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A5 - 1) + 2, 0)</f>
-        <v>KO_sgAB_cmv</v>
+        <v>KO_sgAB_R1_cmv</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" ref="D5" ca="1" si="1">_xlfn.CONCAT(B4, "_", "cmv")</f>
-        <v>KO_sgAB_sense_cmv</v>
+        <v>KO_sgAB_R1_sense_cmv</v>
       </c>
       <c r="E5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F5" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B5, " ", dirs!$A$4, "/", C5, " ", " -o ", dirs!$A$4, "/", D5, " --subst_type ", E5)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgAB_sense libraries_4/KO_sgAB_cmv  -o libraries_4/KO_sgAB_sense_cmv --subst_type without</v>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgAB_R1_sense libraries_4/KO_sgAB_R1_cmv  -o libraries_4/KO_sgAB_R1_sense_cmv --subst_type without</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -9672,22 +9578,22 @@
       </c>
       <c r="B6" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A6 - 1), 0)</f>
-        <v>WT_sgAB_sense</v>
+        <v>WT_sgAB_R2_sense</v>
       </c>
       <c r="C6" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A6 - 1) + 1, 0)</f>
-        <v>WT_sgAB_branch</v>
+        <v>WT_sgAB_R2_branch</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" ref="D6" ca="1" si="2">_xlfn.CONCAT(B6, "_", "branch")</f>
-        <v>WT_sgAB_sense_branch</v>
+        <v>WT_sgAB_R2_sense_branch</v>
       </c>
       <c r="E6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F6" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B6, " ", dirs!$A$4, "/", C6, " ", " -o ", dirs!$A$4, "/", D6, " --subst_type ", E6)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgAB_sense libraries_4/WT_sgAB_branch  -o libraries_4/WT_sgAB_sense_branch --subst_type without</v>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgAB_R2_sense libraries_4/WT_sgAB_R2_branch  -o libraries_4/WT_sgAB_R2_sense_branch --subst_type without</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -9696,22 +9602,22 @@
       </c>
       <c r="B7" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A7 - 1), 0)</f>
-        <v>WT_sgAB_sense</v>
+        <v>WT_sgAB_R2_sense</v>
       </c>
       <c r="C7" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A7 - 1) + 2, 0)</f>
-        <v>WT_sgAB_cmv</v>
+        <v>WT_sgAB_R2_cmv</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" ref="D7" ca="1" si="3">_xlfn.CONCAT(B6, "_", "cmv")</f>
-        <v>WT_sgAB_sense_cmv</v>
+        <v>WT_sgAB_R2_sense_cmv</v>
       </c>
       <c r="E7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F7" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B7, " ", dirs!$A$4, "/", C7, " ", " -o ", dirs!$A$4, "/", D7, " --subst_type ", E7)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgAB_sense libraries_4/WT_sgAB_cmv  -o libraries_4/WT_sgAB_sense_cmv --subst_type without</v>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgAB_R2_sense libraries_4/WT_sgAB_R2_cmv  -o libraries_4/WT_sgAB_R2_sense_cmv --subst_type without</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -9720,22 +9626,22 @@
       </c>
       <c r="B8" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A8 - 1), 0)</f>
-        <v>KO_sgAB_sense</v>
+        <v>KO_sgAB_R2_sense</v>
       </c>
       <c r="C8" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A8 - 1) + 1, 0)</f>
-        <v>KO_sgAB_branch</v>
+        <v>KO_sgAB_R2_branch</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" ref="D8" ca="1" si="4">_xlfn.CONCAT(B8, "_", "branch")</f>
-        <v>KO_sgAB_sense_branch</v>
+        <v>KO_sgAB_R2_sense_branch</v>
       </c>
       <c r="E8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F8" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B8, " ", dirs!$A$4, "/", C8, " ", " -o ", dirs!$A$4, "/", D8, " --subst_type ", E8)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgAB_sense libraries_4/KO_sgAB_branch  -o libraries_4/KO_sgAB_sense_branch --subst_type without</v>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgAB_R2_sense libraries_4/KO_sgAB_R2_branch  -o libraries_4/KO_sgAB_R2_sense_branch --subst_type without</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -9744,22 +9650,22 @@
       </c>
       <c r="B9" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A9 - 1), 0)</f>
-        <v>KO_sgAB_sense</v>
+        <v>KO_sgAB_R2_sense</v>
       </c>
       <c r="C9" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A9 - 1) + 2, 0)</f>
-        <v>KO_sgAB_cmv</v>
+        <v>KO_sgAB_R2_cmv</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" ref="D9" ca="1" si="5">_xlfn.CONCAT(B8, "_", "cmv")</f>
-        <v>KO_sgAB_sense_cmv</v>
+        <v>KO_sgAB_R2_sense_cmv</v>
       </c>
       <c r="E9" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F9" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B9, " ", dirs!$A$4, "/", C9, " ", " -o ", dirs!$A$4, "/", D9, " --subst_type ", E9)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgAB_sense libraries_4/KO_sgAB_cmv  -o libraries_4/KO_sgAB_sense_cmv --subst_type without</v>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgAB_R2_sense libraries_4/KO_sgAB_R2_cmv  -o libraries_4/KO_sgAB_R2_sense_cmv --subst_type without</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -9768,22 +9674,22 @@
       </c>
       <c r="B10" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A10 - 1), 0)</f>
-        <v>WT_sgA_sense</v>
+        <v>WT_sgA_R1_sense</v>
       </c>
       <c r="C10" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A10 - 1) + 1, 0)</f>
-        <v>WT_sgA_branch</v>
+        <v>WT_sgA_R1_branch</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" ref="D10" ca="1" si="6">_xlfn.CONCAT(B10, "_", "branch")</f>
-        <v>WT_sgA_sense_branch</v>
+        <v>WT_sgA_R1_sense_branch</v>
       </c>
       <c r="E10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F10" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B10, " ", dirs!$A$4, "/", C10, " ", " -o ", dirs!$A$4, "/", D10, " --subst_type ", E10)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgA_sense libraries_4/WT_sgA_branch  -o libraries_4/WT_sgA_sense_branch --subst_type without</v>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgA_R1_sense libraries_4/WT_sgA_R1_branch  -o libraries_4/WT_sgA_R1_sense_branch --subst_type without</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -9792,22 +9698,22 @@
       </c>
       <c r="B11" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A11 - 1), 0)</f>
-        <v>WT_sgA_sense</v>
+        <v>WT_sgA_R1_sense</v>
       </c>
       <c r="C11" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A11 - 1) + 2, 0)</f>
-        <v>WT_sgA_cmv</v>
+        <v>WT_sgA_R1_cmv</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" ref="D11" ca="1" si="7">_xlfn.CONCAT(B10, "_", "cmv")</f>
-        <v>WT_sgA_sense_cmv</v>
+        <v>WT_sgA_R1_sense_cmv</v>
       </c>
       <c r="E11" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F11" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B11, " ", dirs!$A$4, "/", C11, " ", " -o ", dirs!$A$4, "/", D11, " --subst_type ", E11)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgA_sense libraries_4/WT_sgA_cmv  -o libraries_4/WT_sgA_sense_cmv --subst_type without</v>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgA_R1_sense libraries_4/WT_sgA_R1_cmv  -o libraries_4/WT_sgA_R1_sense_cmv --subst_type without</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -9816,22 +9722,22 @@
       </c>
       <c r="B12" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A12 - 1), 0)</f>
-        <v>WT_sgB_sense</v>
+        <v>WT_sgB_R2_sense</v>
       </c>
       <c r="C12" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A12 - 1) + 1, 0)</f>
-        <v>WT_sgB_branch</v>
+        <v>WT_sgB_R2_branch</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" ref="D12" ca="1" si="8">_xlfn.CONCAT(B12, "_", "branch")</f>
-        <v>WT_sgB_sense_branch</v>
+        <v>WT_sgB_R2_sense_branch</v>
       </c>
       <c r="E12" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F12" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B12, " ", dirs!$A$4, "/", C12, " ", " -o ", dirs!$A$4, "/", D12, " --subst_type ", E12)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgB_sense libraries_4/WT_sgB_branch  -o libraries_4/WT_sgB_sense_branch --subst_type without</v>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgB_R2_sense libraries_4/WT_sgB_R2_branch  -o libraries_4/WT_sgB_R2_sense_branch --subst_type without</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -9840,22 +9746,22 @@
       </c>
       <c r="B13" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A13 - 1), 0)</f>
-        <v>WT_sgB_sense</v>
+        <v>WT_sgB_R2_sense</v>
       </c>
       <c r="C13" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A13 - 1) + 2, 0)</f>
-        <v>WT_sgB_cmv</v>
+        <v>WT_sgB_R2_cmv</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" ref="D13" ca="1" si="9">_xlfn.CONCAT(B12, "_", "cmv")</f>
-        <v>WT_sgB_sense_cmv</v>
+        <v>WT_sgB_R2_sense_cmv</v>
       </c>
       <c r="E13" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F13" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B13, " ", dirs!$A$4, "/", C13, " ", " -o ", dirs!$A$4, "/", D13, " --subst_type ", E13)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgB_sense libraries_4/WT_sgB_cmv  -o libraries_4/WT_sgB_sense_cmv --subst_type without</v>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgB_R2_sense libraries_4/WT_sgB_R2_cmv  -o libraries_4/WT_sgB_R2_sense_cmv --subst_type without</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -9864,22 +9770,22 @@
       </c>
       <c r="B14" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A14 - 1), 0)</f>
-        <v>KO_sgA_sense</v>
+        <v>KO_sgA_R1_sense</v>
       </c>
       <c r="C14" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A14 - 1) + 1, 0)</f>
-        <v>KO_sgA_branch</v>
+        <v>KO_sgA_R1_branch</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" ref="D14" ca="1" si="10">_xlfn.CONCAT(B14, "_", "branch")</f>
-        <v>KO_sgA_sense_branch</v>
+        <v>KO_sgA_R1_sense_branch</v>
       </c>
       <c r="E14" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F14" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B14, " ", dirs!$A$4, "/", C14, " ", " -o ", dirs!$A$4, "/", D14, " --subst_type ", E14)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgA_sense libraries_4/KO_sgA_branch  -o libraries_4/KO_sgA_sense_branch --subst_type without</v>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgA_R1_sense libraries_4/KO_sgA_R1_branch  -o libraries_4/KO_sgA_R1_sense_branch --subst_type without</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -9888,22 +9794,22 @@
       </c>
       <c r="B15" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A15 - 1), 0)</f>
-        <v>KO_sgA_sense</v>
+        <v>KO_sgA_R1_sense</v>
       </c>
       <c r="C15" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A15 - 1) + 2, 0)</f>
-        <v>KO_sgA_cmv</v>
+        <v>KO_sgA_R1_cmv</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" ref="D15" ca="1" si="11">_xlfn.CONCAT(B14, "_", "cmv")</f>
-        <v>KO_sgA_sense_cmv</v>
+        <v>KO_sgA_R1_sense_cmv</v>
       </c>
       <c r="E15" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F15" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B15, " ", dirs!$A$4, "/", C15, " ", " -o ", dirs!$A$4, "/", D15, " --subst_type ", E15)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgA_sense libraries_4/KO_sgA_cmv  -o libraries_4/KO_sgA_sense_cmv --subst_type without</v>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgA_R1_sense libraries_4/KO_sgA_R1_cmv  -o libraries_4/KO_sgA_R1_sense_cmv --subst_type without</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -9912,22 +9818,22 @@
       </c>
       <c r="B16" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A16 - 1), 0)</f>
-        <v>KO_sgB_sense</v>
+        <v>KO_sgB_R2_sense</v>
       </c>
       <c r="C16" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A16 - 1) + 1, 0)</f>
-        <v>KO_sgB_branch</v>
+        <v>KO_sgB_R2_branch</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" ref="D16" ca="1" si="12">_xlfn.CONCAT(B16, "_", "branch")</f>
-        <v>KO_sgB_sense_branch</v>
+        <v>KO_sgB_R2_sense_branch</v>
       </c>
       <c r="E16" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F16" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B16, " ", dirs!$A$4, "/", C16, " ", " -o ", dirs!$A$4, "/", D16, " --subst_type ", E16)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgB_sense libraries_4/KO_sgB_branch  -o libraries_4/KO_sgB_sense_branch --subst_type without</v>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgB_R2_sense libraries_4/KO_sgB_R2_branch  -o libraries_4/KO_sgB_R2_sense_branch --subst_type without</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -9936,22 +9842,22 @@
       </c>
       <c r="B17" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A17 - 1), 0)</f>
-        <v>KO_sgB_sense</v>
+        <v>KO_sgB_R2_sense</v>
       </c>
       <c r="C17" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A17 - 1) + 2, 0)</f>
-        <v>KO_sgB_cmv</v>
+        <v>KO_sgB_R2_cmv</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" ref="D17" ca="1" si="13">_xlfn.CONCAT(B16, "_", "cmv")</f>
-        <v>KO_sgB_sense_cmv</v>
+        <v>KO_sgB_R2_sense_cmv</v>
       </c>
       <c r="E17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F17" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B17, " ", dirs!$A$4, "/", C17, " ", " -o ", dirs!$A$4, "/", D17, " --subst_type ", E17)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgB_sense libraries_4/KO_sgB_cmv  -o libraries_4/KO_sgB_sense_cmv --subst_type without</v>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgB_R2_sense libraries_4/KO_sgB_R2_cmv  -o libraries_4/KO_sgB_R2_sense_cmv --subst_type without</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -9960,22 +9866,22 @@
       </c>
       <c r="B18" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A18 - 1), 0)</f>
-        <v>WT_sgCD_antisense</v>
+        <v>WT_sgCD_R1_antisense</v>
       </c>
       <c r="C18" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A18 - 1) + 1, 0)</f>
-        <v>WT_sgCD_splicing</v>
+        <v>WT_sgCD_R1_splicing</v>
       </c>
       <c r="D18" t="str">
         <f ca="1">_xlfn.CONCAT(B17, "_", "splicing")</f>
-        <v>KO_sgB_sense_splicing</v>
+        <v>KO_sgB_R2_sense_splicing</v>
       </c>
       <c r="E18" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F18" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B18, " ", dirs!$A$4, "/", C18, " ", " -o ", dirs!$A$4, "/", D18, " --subst_type ", E18)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgCD_antisense libraries_4/WT_sgCD_splicing  -o libraries_4/KO_sgB_sense_splicing --subst_type without</v>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgCD_R1_antisense libraries_4/WT_sgCD_R1_splicing  -o libraries_4/KO_sgB_R2_sense_splicing --subst_type without</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -9984,22 +9890,22 @@
       </c>
       <c r="B19" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A19 - 1), 0)</f>
-        <v>WT_sgCD_antisense</v>
+        <v>WT_sgCD_R1_antisense</v>
       </c>
       <c r="C19" t="str">
         <f ca="1">OFFSET('3'!$A$2, 3 * (A19 - 1) + 1, 0)</f>
-        <v>WT_sgCD_splicing</v>
+        <v>WT_sgCD_R1_splicing</v>
       </c>
       <c r="D19" t="str">
         <f ca="1">_xlfn.CONCAT(B18, "_", "splicing")</f>
-        <v>WT_sgCD_antisense_splicing</v>
+        <v>WT_sgCD_R1_antisense_splicing</v>
       </c>
       <c r="E19" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F19" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B19, " ", dirs!$A$4, "/", C19, " ", " -o ", dirs!$A$4, "/", D19, " --subst_type ", E19)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgCD_antisense libraries_4/WT_sgCD_splicing  -o libraries_4/WT_sgCD_antisense_splicing --subst_type without</v>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgCD_R1_antisense libraries_4/WT_sgCD_R1_splicing  -o libraries_4/WT_sgCD_R1_antisense_splicing --subst_type without</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3d histogram code first pass done.
</commit_message>
<xml_diff>
--- a/libinfo.xlsx
+++ b/libinfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tchan\Code\SCMB_Project\RNA-mediated_DSB_repair\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8168026-2C8B-4AEA-8343-7EC28A32DF8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B5666E-6F88-4A84-B72D-C4718E6AE17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="2" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="3" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
   </bookViews>
   <sheets>
     <sheet name="dirs" sheetId="3" r:id="rId1"/>
@@ -6083,7 +6083,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12B0900B-E55F-43FE-AC1A-BE82F1C8E743}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G19" workbookViewId="0">
+    <sheetView topLeftCell="G19" workbookViewId="0">
       <selection activeCell="Q3" sqref="Q3:Q30"/>
     </sheetView>
   </sheetViews>
@@ -8124,8 +8124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7FB6E33-93C4-4971-BF44-23A0F65AADA0}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J29"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6:K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8394,8 +8394,8 @@
         <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgAB_R1_branch.tsv -o libraries_4/KO_sgAB_R1_branch -ref ref_seq/2DSB_R1_branch.fa -dsb 67 --dsb_type 1 --strand R1 --hguide AB --cell KO --treatment branch --subst_type without</v>
       </c>
       <c r="K6" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A6)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgAB_R1_branch</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without",  " -dir ", dirs!$A$4, "/", '3'!A6)</f>
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgAB_R1_branch</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -8439,8 +8439,8 @@
         <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgAB_R1_cmv.tsv -o libraries_4/KO_sgAB_R1_cmv -ref ref_seq/2DSB_R1_cmv.fa -dsb 67 --dsb_type 1 --strand R1 --hguide AB --cell KO --treatment cmv --subst_type without</v>
       </c>
       <c r="K7" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A7)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgAB_R1_cmv</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without",  " -dir ", dirs!$A$4, "/", '3'!A7)</f>
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgAB_R1_cmv</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -8484,8 +8484,8 @@
         <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgAB_R2_sense.tsv -o libraries_4/WT_sgAB_R2_sense -ref ref_seq/2DSB_R2_sense.fa -dsb 46 --dsb_type 1 --strand R2 --hguide AB --cell WT --treatment sense --subst_type without</v>
       </c>
       <c r="K8" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A8)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgAB_R2_sense</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without",  " -dir ", dirs!$A$4, "/", '3'!A8)</f>
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgAB_R2_sense</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -8529,8 +8529,8 @@
         <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgAB_R2_branch.tsv -o libraries_4/WT_sgAB_R2_branch -ref ref_seq/2DSB_R2_branch.fa -dsb 46 --dsb_type 1 --strand R2 --hguide AB --cell WT --treatment branch --subst_type without</v>
       </c>
       <c r="K9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A9)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgAB_R2_branch</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without",  " -dir ", dirs!$A$4, "/", '3'!A9)</f>
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgAB_R2_branch</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -8574,8 +8574,8 @@
         <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgAB_R2_cmv.tsv -o libraries_4/WT_sgAB_R2_cmv -ref ref_seq/2DSB_R2_cmv.fa -dsb 46 --dsb_type 1 --strand R2 --hguide AB --cell WT --treatment cmv --subst_type without</v>
       </c>
       <c r="K10" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A10)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgAB_R2_cmv</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without",  " -dir ", dirs!$A$4, "/", '3'!A10)</f>
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgAB_R2_cmv</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -8619,8 +8619,8 @@
         <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgAB_R2_sense.tsv -o libraries_4/KO_sgAB_R2_sense -ref ref_seq/2DSB_R2_sense.fa -dsb 46 --dsb_type 1 --strand R2 --hguide AB --cell KO --treatment sense --subst_type without</v>
       </c>
       <c r="K11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A11)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgAB_R2_sense</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without",  " -dir ", dirs!$A$4, "/", '3'!A11)</f>
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgAB_R2_sense</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -8664,8 +8664,8 @@
         <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgAB_R2_branch.tsv -o libraries_4/KO_sgAB_R2_branch -ref ref_seq/2DSB_R2_branch.fa -dsb 46 --dsb_type 1 --strand R2 --hguide AB --cell KO --treatment branch --subst_type without</v>
       </c>
       <c r="K12" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A12)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgAB_R2_branch</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without",  " -dir ", dirs!$A$4, "/", '3'!A12)</f>
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgAB_R2_branch</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -8709,8 +8709,8 @@
         <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgAB_R2_cmv.tsv -o libraries_4/KO_sgAB_R2_cmv -ref ref_seq/2DSB_R2_cmv.fa -dsb 46 --dsb_type 1 --strand R2 --hguide AB --cell KO --treatment cmv --subst_type without</v>
       </c>
       <c r="K13" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A13)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgAB_R2_cmv</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without",  " -dir ", dirs!$A$4, "/", '3'!A13)</f>
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgAB_R2_cmv</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -8754,8 +8754,8 @@
         <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgA_R1_sense.tsv -o libraries_4/WT_sgA_R1_sense -ref ref_seq/1DSB_R1_sense.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell WT --treatment sense --subst_type without</v>
       </c>
       <c r="K14" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A14)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgA_R1_sense</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without",  " -dir ", dirs!$A$4, "/", '3'!A14)</f>
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgA_R1_sense</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -8799,8 +8799,8 @@
         <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgA_R1_branch.tsv -o libraries_4/WT_sgA_R1_branch -ref ref_seq/1DSB_R1_branch.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell WT --treatment branch --subst_type without</v>
       </c>
       <c r="K15" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A15)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgA_R1_branch</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without",  " -dir ", dirs!$A$4, "/", '3'!A15)</f>
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgA_R1_branch</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -8844,8 +8844,8 @@
         <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgA_R1_cmv.tsv -o libraries_4/WT_sgA_R1_cmv -ref ref_seq/1DSB_R1_cmv.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell WT --treatment cmv --subst_type without</v>
       </c>
       <c r="K16" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A16)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgA_R1_cmv</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without",  " -dir ", dirs!$A$4, "/", '3'!A16)</f>
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgA_R1_cmv</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -8889,8 +8889,8 @@
         <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgB_R2_sense.tsv -o libraries_4/WT_sgB_R2_sense -ref ref_seq/1DSB_R2_sense.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell WT --treatment sense --subst_type without</v>
       </c>
       <c r="K17" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A17)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgB_R2_sense</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without",  " -dir ", dirs!$A$4, "/", '3'!A17)</f>
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgB_R2_sense</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -8934,8 +8934,8 @@
         <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgB_R2_branch.tsv -o libraries_4/WT_sgB_R2_branch -ref ref_seq/1DSB_R2_branch.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell WT --treatment branch --subst_type without</v>
       </c>
       <c r="K18" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A18)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgB_R2_branch</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without",  " -dir ", dirs!$A$4, "/", '3'!A18)</f>
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgB_R2_branch</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -8979,8 +8979,8 @@
         <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgB_R2_cmv.tsv -o libraries_4/WT_sgB_R2_cmv -ref ref_seq/1DSB_R2_cmv.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell WT --treatment cmv --subst_type without</v>
       </c>
       <c r="K19" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A19)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgB_R2_cmv</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without",  " -dir ", dirs!$A$4, "/", '3'!A19)</f>
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgB_R2_cmv</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -9024,8 +9024,8 @@
         <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgA_R1_sense.tsv -o libraries_4/KO_sgA_R1_sense -ref ref_seq/1DSB_R1_sense.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell KO --treatment sense --subst_type without</v>
       </c>
       <c r="K20" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A20)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgA_R1_sense</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without",  " -dir ", dirs!$A$4, "/", '3'!A20)</f>
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgA_R1_sense</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -9069,8 +9069,8 @@
         <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgA_R1_branch.tsv -o libraries_4/KO_sgA_R1_branch -ref ref_seq/1DSB_R1_branch.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell KO --treatment branch --subst_type without</v>
       </c>
       <c r="K21" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A21)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgA_R1_branch</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without",  " -dir ", dirs!$A$4, "/", '3'!A21)</f>
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgA_R1_branch</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -9114,8 +9114,8 @@
         <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgA_R1_cmv.tsv -o libraries_4/KO_sgA_R1_cmv -ref ref_seq/1DSB_R1_cmv.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell KO --treatment cmv --subst_type without</v>
       </c>
       <c r="K22" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A22)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgA_R1_cmv</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without",  " -dir ", dirs!$A$4, "/", '3'!A22)</f>
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgA_R1_cmv</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -9159,8 +9159,8 @@
         <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgB_R2_sense.tsv -o libraries_4/KO_sgB_R2_sense -ref ref_seq/1DSB_R2_sense.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell KO --treatment sense --subst_type without</v>
       </c>
       <c r="K23" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A23)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgB_R2_sense</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without",  " -dir ", dirs!$A$4, "/", '3'!A23)</f>
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgB_R2_sense</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -9204,8 +9204,8 @@
         <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgB_R2_branch.tsv -o libraries_4/KO_sgB_R2_branch -ref ref_seq/1DSB_R2_branch.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell KO --treatment branch --subst_type without</v>
       </c>
       <c r="K24" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A24)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgB_R2_branch</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without",  " -dir ", dirs!$A$4, "/", '3'!A24)</f>
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgB_R2_branch</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -9249,8 +9249,8 @@
         <v>python 2_graph_processing/make_main_data.py -in libraries_3/KO_sgB_R2_cmv.tsv -o libraries_4/KO_sgB_R2_cmv -ref ref_seq/1DSB_R2_cmv.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell KO --treatment cmv --subst_type without</v>
       </c>
       <c r="K25" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A25)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/KO_sgB_R2_cmv</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without",  " -dir ", dirs!$A$4, "/", '3'!A25)</f>
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgB_R2_cmv</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -9294,8 +9294,8 @@
         <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgCD_R1_antisense.tsv -o libraries_4/WT_sgCD_R1_antisense -ref ref_seq/2DSBanti_R1_antisense.fa -dsb 50 --dsb_type 1 --strand R1 --hguide CD --cell WT --treatment antisense --subst_type without</v>
       </c>
       <c r="K26" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A26)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgCD_R1_antisense</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without",  " -dir ", dirs!$A$4, "/", '3'!A26)</f>
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgCD_R1_antisense</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -9339,8 +9339,8 @@
         <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgCD_R1_splicing.tsv -o libraries_4/WT_sgCD_R1_splicing -ref ref_seq/2DSBanti_R1_splicing.fa -dsb 50 --dsb_type 1 --strand R1 --hguide CD --cell WT --treatment splicing --subst_type without</v>
       </c>
       <c r="K27" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A27)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgCD_R1_splicing</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without",  " -dir ", dirs!$A$4, "/", '3'!A27)</f>
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgCD_R1_splicing</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -9384,8 +9384,8 @@
         <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgCD_R2_antisense.tsv -o libraries_4/WT_sgCD_R2_antisense -ref ref_seq/2DSBanti_R2_antisense.fa -dsb 47 --dsb_type 1 --strand R2 --hguide CD --cell WT --treatment antisense --subst_type without</v>
       </c>
       <c r="K28" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A28)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgCD_R2_antisense</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without",  " -dir ", dirs!$A$4, "/", '3'!A28)</f>
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgCD_R2_antisense</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -9429,8 +9429,8 @@
         <v>python 2_graph_processing/make_main_data.py -in libraries_3/WT_sgCD_R2_splicing.tsv -o libraries_4/WT_sgCD_R2_splicing -ref ref_seq/2DSBanti_R2_splicing.fa -dsb 47 --dsb_type 1 --strand R2 --hguide CD --cell WT --treatment splicing --subst_type without</v>
       </c>
       <c r="K29" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without ",  " -dir ", dirs!$A$4, "/", '3'!A29)</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type without  -dir libraries_4/WT_sgCD_R2_splicing</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type without",  " -dir ", dirs!$A$4, "/", '3'!A29)</f>
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgCD_R2_splicing</v>
       </c>
     </row>
   </sheetData>
@@ -9444,7 +9444,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F2" sqref="F2:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9496,8 +9496,8 @@
         <v>110</v>
       </c>
       <c r="F2" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B2, " ", dirs!$A$4, "/", C2, " ", " -o ", dirs!$A$4, "/", D2, " --subst_type ", E2)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgAB_R1_sense libraries_4/WT_sgAB_R1_branch  -o libraries_4/WT_sgAB_R1_sense_branch --subst_type without</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B2, " ", dirs!$A$4, "/", C2, " -o ", dirs!$A$4, "/", D2, " --subst_type ", E2)</f>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgAB_R1_sense libraries_4/WT_sgAB_R1_branch -o libraries_4/WT_sgAB_R1_sense_branch --subst_type without</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -9520,8 +9520,8 @@
         <v>110</v>
       </c>
       <c r="F3" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B3, " ", dirs!$A$4, "/", C3, " ", " -o ", dirs!$A$4, "/", D3, " --subst_type ", E3)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgAB_R1_sense libraries_4/WT_sgAB_R1_cmv  -o libraries_4/WT_sgAB_R1_sense_cmv --subst_type without</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B3, " ", dirs!$A$4, "/", C3, " -o ", dirs!$A$4, "/", D3, " --subst_type ", E3)</f>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgAB_R1_sense libraries_4/WT_sgAB_R1_cmv -o libraries_4/WT_sgAB_R1_sense_cmv --subst_type without</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -9544,8 +9544,8 @@
         <v>110</v>
       </c>
       <c r="F4" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B4, " ", dirs!$A$4, "/", C4, " ", " -o ", dirs!$A$4, "/", D4, " --subst_type ", E4)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgAB_R1_sense libraries_4/KO_sgAB_R1_branch  -o libraries_4/KO_sgAB_R1_sense_branch --subst_type without</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B4, " ", dirs!$A$4, "/", C4, " -o ", dirs!$A$4, "/", D4, " --subst_type ", E4)</f>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgAB_R1_sense libraries_4/KO_sgAB_R1_branch -o libraries_4/KO_sgAB_R1_sense_branch --subst_type without</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -9568,8 +9568,8 @@
         <v>110</v>
       </c>
       <c r="F5" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B5, " ", dirs!$A$4, "/", C5, " ", " -o ", dirs!$A$4, "/", D5, " --subst_type ", E5)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgAB_R1_sense libraries_4/KO_sgAB_R1_cmv  -o libraries_4/KO_sgAB_R1_sense_cmv --subst_type without</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B5, " ", dirs!$A$4, "/", C5, " -o ", dirs!$A$4, "/", D5, " --subst_type ", E5)</f>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgAB_R1_sense libraries_4/KO_sgAB_R1_cmv -o libraries_4/KO_sgAB_R1_sense_cmv --subst_type without</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -9592,8 +9592,8 @@
         <v>110</v>
       </c>
       <c r="F6" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B6, " ", dirs!$A$4, "/", C6, " ", " -o ", dirs!$A$4, "/", D6, " --subst_type ", E6)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgAB_R2_sense libraries_4/WT_sgAB_R2_branch  -o libraries_4/WT_sgAB_R2_sense_branch --subst_type without</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B6, " ", dirs!$A$4, "/", C6, " -o ", dirs!$A$4, "/", D6, " --subst_type ", E6)</f>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgAB_R2_sense libraries_4/WT_sgAB_R2_branch -o libraries_4/WT_sgAB_R2_sense_branch --subst_type without</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -9616,8 +9616,8 @@
         <v>110</v>
       </c>
       <c r="F7" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B7, " ", dirs!$A$4, "/", C7, " ", " -o ", dirs!$A$4, "/", D7, " --subst_type ", E7)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgAB_R2_sense libraries_4/WT_sgAB_R2_cmv  -o libraries_4/WT_sgAB_R2_sense_cmv --subst_type without</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B7, " ", dirs!$A$4, "/", C7, " -o ", dirs!$A$4, "/", D7, " --subst_type ", E7)</f>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgAB_R2_sense libraries_4/WT_sgAB_R2_cmv -o libraries_4/WT_sgAB_R2_sense_cmv --subst_type without</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -9640,8 +9640,8 @@
         <v>110</v>
       </c>
       <c r="F8" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B8, " ", dirs!$A$4, "/", C8, " ", " -o ", dirs!$A$4, "/", D8, " --subst_type ", E8)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgAB_R2_sense libraries_4/KO_sgAB_R2_branch  -o libraries_4/KO_sgAB_R2_sense_branch --subst_type without</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B8, " ", dirs!$A$4, "/", C8, " -o ", dirs!$A$4, "/", D8, " --subst_type ", E8)</f>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgAB_R2_sense libraries_4/KO_sgAB_R2_branch -o libraries_4/KO_sgAB_R2_sense_branch --subst_type without</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -9664,8 +9664,8 @@
         <v>110</v>
       </c>
       <c r="F9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B9, " ", dirs!$A$4, "/", C9, " ", " -o ", dirs!$A$4, "/", D9, " --subst_type ", E9)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgAB_R2_sense libraries_4/KO_sgAB_R2_cmv  -o libraries_4/KO_sgAB_R2_sense_cmv --subst_type without</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B9, " ", dirs!$A$4, "/", C9, " -o ", dirs!$A$4, "/", D9, " --subst_type ", E9)</f>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgAB_R2_sense libraries_4/KO_sgAB_R2_cmv -o libraries_4/KO_sgAB_R2_sense_cmv --subst_type without</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -9688,8 +9688,8 @@
         <v>110</v>
       </c>
       <c r="F10" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B10, " ", dirs!$A$4, "/", C10, " ", " -o ", dirs!$A$4, "/", D10, " --subst_type ", E10)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgA_R1_sense libraries_4/WT_sgA_R1_branch  -o libraries_4/WT_sgA_R1_sense_branch --subst_type without</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B10, " ", dirs!$A$4, "/", C10, " -o ", dirs!$A$4, "/", D10, " --subst_type ", E10)</f>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgA_R1_sense libraries_4/WT_sgA_R1_branch -o libraries_4/WT_sgA_R1_sense_branch --subst_type without</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -9712,8 +9712,8 @@
         <v>110</v>
       </c>
       <c r="F11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B11, " ", dirs!$A$4, "/", C11, " ", " -o ", dirs!$A$4, "/", D11, " --subst_type ", E11)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgA_R1_sense libraries_4/WT_sgA_R1_cmv  -o libraries_4/WT_sgA_R1_sense_cmv --subst_type without</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B11, " ", dirs!$A$4, "/", C11, " -o ", dirs!$A$4, "/", D11, " --subst_type ", E11)</f>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgA_R1_sense libraries_4/WT_sgA_R1_cmv -o libraries_4/WT_sgA_R1_sense_cmv --subst_type without</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -9736,8 +9736,8 @@
         <v>110</v>
       </c>
       <c r="F12" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B12, " ", dirs!$A$4, "/", C12, " ", " -o ", dirs!$A$4, "/", D12, " --subst_type ", E12)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgB_R2_sense libraries_4/WT_sgB_R2_branch  -o libraries_4/WT_sgB_R2_sense_branch --subst_type without</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B12, " ", dirs!$A$4, "/", C12, " -o ", dirs!$A$4, "/", D12, " --subst_type ", E12)</f>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgB_R2_sense libraries_4/WT_sgB_R2_branch -o libraries_4/WT_sgB_R2_sense_branch --subst_type without</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -9760,8 +9760,8 @@
         <v>110</v>
       </c>
       <c r="F13" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B13, " ", dirs!$A$4, "/", C13, " ", " -o ", dirs!$A$4, "/", D13, " --subst_type ", E13)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgB_R2_sense libraries_4/WT_sgB_R2_cmv  -o libraries_4/WT_sgB_R2_sense_cmv --subst_type without</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B13, " ", dirs!$A$4, "/", C13, " -o ", dirs!$A$4, "/", D13, " --subst_type ", E13)</f>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgB_R2_sense libraries_4/WT_sgB_R2_cmv -o libraries_4/WT_sgB_R2_sense_cmv --subst_type without</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -9784,8 +9784,8 @@
         <v>110</v>
       </c>
       <c r="F14" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B14, " ", dirs!$A$4, "/", C14, " ", " -o ", dirs!$A$4, "/", D14, " --subst_type ", E14)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgA_R1_sense libraries_4/KO_sgA_R1_branch  -o libraries_4/KO_sgA_R1_sense_branch --subst_type without</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B14, " ", dirs!$A$4, "/", C14, " -o ", dirs!$A$4, "/", D14, " --subst_type ", E14)</f>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgA_R1_sense libraries_4/KO_sgA_R1_branch -o libraries_4/KO_sgA_R1_sense_branch --subst_type without</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -9808,8 +9808,8 @@
         <v>110</v>
       </c>
       <c r="F15" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B15, " ", dirs!$A$4, "/", C15, " ", " -o ", dirs!$A$4, "/", D15, " --subst_type ", E15)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgA_R1_sense libraries_4/KO_sgA_R1_cmv  -o libraries_4/KO_sgA_R1_sense_cmv --subst_type without</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B15, " ", dirs!$A$4, "/", C15, " -o ", dirs!$A$4, "/", D15, " --subst_type ", E15)</f>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgA_R1_sense libraries_4/KO_sgA_R1_cmv -o libraries_4/KO_sgA_R1_sense_cmv --subst_type without</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -9832,8 +9832,8 @@
         <v>110</v>
       </c>
       <c r="F16" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B16, " ", dirs!$A$4, "/", C16, " ", " -o ", dirs!$A$4, "/", D16, " --subst_type ", E16)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgB_R2_sense libraries_4/KO_sgB_R2_branch  -o libraries_4/KO_sgB_R2_sense_branch --subst_type without</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B16, " ", dirs!$A$4, "/", C16, " -o ", dirs!$A$4, "/", D16, " --subst_type ", E16)</f>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgB_R2_sense libraries_4/KO_sgB_R2_branch -o libraries_4/KO_sgB_R2_sense_branch --subst_type without</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -9856,8 +9856,8 @@
         <v>110</v>
       </c>
       <c r="F17" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B17, " ", dirs!$A$4, "/", C17, " ", " -o ", dirs!$A$4, "/", D17, " --subst_type ", E17)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgB_R2_sense libraries_4/KO_sgB_R2_cmv  -o libraries_4/KO_sgB_R2_sense_cmv --subst_type without</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B17, " ", dirs!$A$4, "/", C17, " -o ", dirs!$A$4, "/", D17, " --subst_type ", E17)</f>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgB_R2_sense libraries_4/KO_sgB_R2_cmv -o libraries_4/KO_sgB_R2_sense_cmv --subst_type without</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -9880,8 +9880,8 @@
         <v>110</v>
       </c>
       <c r="F18" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B18, " ", dirs!$A$4, "/", C18, " ", " -o ", dirs!$A$4, "/", D18, " --subst_type ", E18)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgCD_R1_antisense libraries_4/WT_sgCD_R1_splicing  -o libraries_4/KO_sgB_R2_sense_splicing --subst_type without</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B18, " ", dirs!$A$4, "/", C18, " -o ", dirs!$A$4, "/", D18, " --subst_type ", E18)</f>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgCD_R1_antisense libraries_4/WT_sgCD_R1_splicing -o libraries_4/KO_sgB_R2_sense_splicing --subst_type without</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -9904,8 +9904,8 @@
         <v>110</v>
       </c>
       <c r="F19" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B19, " ", dirs!$A$4, "/", C19, " ", " -o ", dirs!$A$4, "/", D19, " --subst_type ", E19)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgCD_R1_antisense libraries_4/WT_sgCD_R1_splicing  -o libraries_4/WT_sgCD_R1_antisense_splicing --subst_type without</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B19, " ", dirs!$A$4, "/", C19, " -o ", dirs!$A$4, "/", D19, " --subst_type ", E19)</f>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgCD_R1_antisense libraries_4/WT_sgCD_R1_splicing -o libraries_4/WT_sgCD_R1_antisense_splicing --subst_type without</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Begin making command line args for graph script.
</commit_message>
<xml_diff>
--- a/libinfo.xlsx
+++ b/libinfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tchan\Code\SCMB_Project\RNA-mediated_DSB_repair\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B5666E-6F88-4A84-B72D-C4718E6AE17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46FD791-FF59-48E6-8612-E9AD180DFA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="3" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
   </bookViews>
@@ -8124,8 +8124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7FB6E33-93C4-4971-BF44-23A0F65AADA0}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6:K29"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9443,8 +9443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AFDA2BA-58B9-4C12-83E9-7C389A51814A}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F19"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9513,15 +9513,15 @@
         <v>WT_sgAB_R1_cmv</v>
       </c>
       <c r="D3" t="str">
-        <f ca="1">_xlfn.CONCAT(B2, "_", "cmv")</f>
-        <v>WT_sgAB_R1_sense_cmv</v>
+        <f t="shared" ref="D3:D19" ca="1" si="0">_xlfn.CONCAT(B3, "_", "branch")</f>
+        <v>WT_sgAB_R1_sense_branch</v>
       </c>
       <c r="E3" t="s">
         <v>110</v>
       </c>
       <c r="F3" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B3, " ", dirs!$A$4, "/", C3, " -o ", dirs!$A$4, "/", D3, " --subst_type ", E3)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgAB_R1_sense libraries_4/WT_sgAB_R1_cmv -o libraries_4/WT_sgAB_R1_sense_cmv --subst_type without</v>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgAB_R1_sense libraries_4/WT_sgAB_R1_cmv -o libraries_4/WT_sgAB_R1_sense_branch --subst_type without</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -9537,7 +9537,7 @@
         <v>KO_sgAB_R1_branch</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" ref="D4" ca="1" si="0">_xlfn.CONCAT(B4, "_", "branch")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>KO_sgAB_R1_sense_branch</v>
       </c>
       <c r="E4" t="s">
@@ -9561,15 +9561,15 @@
         <v>KO_sgAB_R1_cmv</v>
       </c>
       <c r="D5" t="str">
-        <f t="shared" ref="D5" ca="1" si="1">_xlfn.CONCAT(B4, "_", "cmv")</f>
-        <v>KO_sgAB_R1_sense_cmv</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>KO_sgAB_R1_sense_branch</v>
       </c>
       <c r="E5" t="s">
         <v>110</v>
       </c>
       <c r="F5" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B5, " ", dirs!$A$4, "/", C5, " -o ", dirs!$A$4, "/", D5, " --subst_type ", E5)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgAB_R1_sense libraries_4/KO_sgAB_R1_cmv -o libraries_4/KO_sgAB_R1_sense_cmv --subst_type without</v>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgAB_R1_sense libraries_4/KO_sgAB_R1_cmv -o libraries_4/KO_sgAB_R1_sense_branch --subst_type without</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -9585,7 +9585,7 @@
         <v>WT_sgAB_R2_branch</v>
       </c>
       <c r="D6" t="str">
-        <f t="shared" ref="D6" ca="1" si="2">_xlfn.CONCAT(B6, "_", "branch")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>WT_sgAB_R2_sense_branch</v>
       </c>
       <c r="E6" t="s">
@@ -9609,15 +9609,15 @@
         <v>WT_sgAB_R2_cmv</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" ref="D7" ca="1" si="3">_xlfn.CONCAT(B6, "_", "cmv")</f>
-        <v>WT_sgAB_R2_sense_cmv</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>WT_sgAB_R2_sense_branch</v>
       </c>
       <c r="E7" t="s">
         <v>110</v>
       </c>
       <c r="F7" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B7, " ", dirs!$A$4, "/", C7, " -o ", dirs!$A$4, "/", D7, " --subst_type ", E7)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgAB_R2_sense libraries_4/WT_sgAB_R2_cmv -o libraries_4/WT_sgAB_R2_sense_cmv --subst_type without</v>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgAB_R2_sense libraries_4/WT_sgAB_R2_cmv -o libraries_4/WT_sgAB_R2_sense_branch --subst_type without</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -9633,7 +9633,7 @@
         <v>KO_sgAB_R2_branch</v>
       </c>
       <c r="D8" t="str">
-        <f t="shared" ref="D8" ca="1" si="4">_xlfn.CONCAT(B8, "_", "branch")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>KO_sgAB_R2_sense_branch</v>
       </c>
       <c r="E8" t="s">
@@ -9657,15 +9657,15 @@
         <v>KO_sgAB_R2_cmv</v>
       </c>
       <c r="D9" t="str">
-        <f t="shared" ref="D9" ca="1" si="5">_xlfn.CONCAT(B8, "_", "cmv")</f>
-        <v>KO_sgAB_R2_sense_cmv</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>KO_sgAB_R2_sense_branch</v>
       </c>
       <c r="E9" t="s">
         <v>110</v>
       </c>
       <c r="F9" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B9, " ", dirs!$A$4, "/", C9, " -o ", dirs!$A$4, "/", D9, " --subst_type ", E9)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgAB_R2_sense libraries_4/KO_sgAB_R2_cmv -o libraries_4/KO_sgAB_R2_sense_cmv --subst_type without</v>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgAB_R2_sense libraries_4/KO_sgAB_R2_cmv -o libraries_4/KO_sgAB_R2_sense_branch --subst_type without</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -9681,7 +9681,7 @@
         <v>WT_sgA_R1_branch</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" ref="D10" ca="1" si="6">_xlfn.CONCAT(B10, "_", "branch")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>WT_sgA_R1_sense_branch</v>
       </c>
       <c r="E10" t="s">
@@ -9705,15 +9705,15 @@
         <v>WT_sgA_R1_cmv</v>
       </c>
       <c r="D11" t="str">
-        <f t="shared" ref="D11" ca="1" si="7">_xlfn.CONCAT(B10, "_", "cmv")</f>
-        <v>WT_sgA_R1_sense_cmv</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>WT_sgA_R1_sense_branch</v>
       </c>
       <c r="E11" t="s">
         <v>110</v>
       </c>
       <c r="F11" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B11, " ", dirs!$A$4, "/", C11, " -o ", dirs!$A$4, "/", D11, " --subst_type ", E11)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgA_R1_sense libraries_4/WT_sgA_R1_cmv -o libraries_4/WT_sgA_R1_sense_cmv --subst_type without</v>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgA_R1_sense libraries_4/WT_sgA_R1_cmv -o libraries_4/WT_sgA_R1_sense_branch --subst_type without</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -9729,7 +9729,7 @@
         <v>WT_sgB_R2_branch</v>
       </c>
       <c r="D12" t="str">
-        <f t="shared" ref="D12" ca="1" si="8">_xlfn.CONCAT(B12, "_", "branch")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>WT_sgB_R2_sense_branch</v>
       </c>
       <c r="E12" t="s">
@@ -9753,15 +9753,15 @@
         <v>WT_sgB_R2_cmv</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" ref="D13" ca="1" si="9">_xlfn.CONCAT(B12, "_", "cmv")</f>
-        <v>WT_sgB_R2_sense_cmv</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>WT_sgB_R2_sense_branch</v>
       </c>
       <c r="E13" t="s">
         <v>110</v>
       </c>
       <c r="F13" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B13, " ", dirs!$A$4, "/", C13, " -o ", dirs!$A$4, "/", D13, " --subst_type ", E13)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgB_R2_sense libraries_4/WT_sgB_R2_cmv -o libraries_4/WT_sgB_R2_sense_cmv --subst_type without</v>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgB_R2_sense libraries_4/WT_sgB_R2_cmv -o libraries_4/WT_sgB_R2_sense_branch --subst_type without</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -9777,7 +9777,7 @@
         <v>KO_sgA_R1_branch</v>
       </c>
       <c r="D14" t="str">
-        <f t="shared" ref="D14" ca="1" si="10">_xlfn.CONCAT(B14, "_", "branch")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>KO_sgA_R1_sense_branch</v>
       </c>
       <c r="E14" t="s">
@@ -9801,15 +9801,15 @@
         <v>KO_sgA_R1_cmv</v>
       </c>
       <c r="D15" t="str">
-        <f t="shared" ref="D15" ca="1" si="11">_xlfn.CONCAT(B14, "_", "cmv")</f>
-        <v>KO_sgA_R1_sense_cmv</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>KO_sgA_R1_sense_branch</v>
       </c>
       <c r="E15" t="s">
         <v>110</v>
       </c>
       <c r="F15" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B15, " ", dirs!$A$4, "/", C15, " -o ", dirs!$A$4, "/", D15, " --subst_type ", E15)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgA_R1_sense libraries_4/KO_sgA_R1_cmv -o libraries_4/KO_sgA_R1_sense_cmv --subst_type without</v>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgA_R1_sense libraries_4/KO_sgA_R1_cmv -o libraries_4/KO_sgA_R1_sense_branch --subst_type without</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -9825,7 +9825,7 @@
         <v>KO_sgB_R2_branch</v>
       </c>
       <c r="D16" t="str">
-        <f t="shared" ref="D16" ca="1" si="12">_xlfn.CONCAT(B16, "_", "branch")</f>
+        <f t="shared" ca="1" si="0"/>
         <v>KO_sgB_R2_sense_branch</v>
       </c>
       <c r="E16" t="s">
@@ -9849,15 +9849,15 @@
         <v>KO_sgB_R2_cmv</v>
       </c>
       <c r="D17" t="str">
-        <f t="shared" ref="D17" ca="1" si="13">_xlfn.CONCAT(B16, "_", "cmv")</f>
-        <v>KO_sgB_R2_sense_cmv</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>KO_sgB_R2_sense_branch</v>
       </c>
       <c r="E17" t="s">
         <v>110</v>
       </c>
       <c r="F17" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B17, " ", dirs!$A$4, "/", C17, " -o ", dirs!$A$4, "/", D17, " --subst_type ", E17)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgB_R2_sense libraries_4/KO_sgB_R2_cmv -o libraries_4/KO_sgB_R2_sense_cmv --subst_type without</v>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgB_R2_sense libraries_4/KO_sgB_R2_cmv -o libraries_4/KO_sgB_R2_sense_branch --subst_type without</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -9873,15 +9873,15 @@
         <v>WT_sgCD_R1_splicing</v>
       </c>
       <c r="D18" t="str">
-        <f ca="1">_xlfn.CONCAT(B17, "_", "splicing")</f>
-        <v>KO_sgB_R2_sense_splicing</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>WT_sgCD_R1_antisense_branch</v>
       </c>
       <c r="E18" t="s">
         <v>110</v>
       </c>
       <c r="F18" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B18, " ", dirs!$A$4, "/", C18, " -o ", dirs!$A$4, "/", D18, " --subst_type ", E18)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgCD_R1_antisense libraries_4/WT_sgCD_R1_splicing -o libraries_4/KO_sgB_R2_sense_splicing --subst_type without</v>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgCD_R1_antisense libraries_4/WT_sgCD_R1_splicing -o libraries_4/WT_sgCD_R1_antisense_branch --subst_type without</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -9897,15 +9897,15 @@
         <v>WT_sgCD_R1_splicing</v>
       </c>
       <c r="D19" t="str">
-        <f ca="1">_xlfn.CONCAT(B18, "_", "splicing")</f>
-        <v>WT_sgCD_R1_antisense_splicing</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>WT_sgCD_R1_antisense_branch</v>
       </c>
       <c r="E19" t="s">
         <v>110</v>
       </c>
       <c r="F19" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", dirs!$A$4, "/", B19, " ", dirs!$A$4, "/", C19, " -o ", dirs!$A$4, "/", D19, " --subst_type ", E19)</f>
-        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgCD_R1_antisense libraries_4/WT_sgCD_R1_splicing -o libraries_4/WT_sgCD_R1_antisense_splicing --subst_type without</v>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgCD_R1_antisense libraries_4/WT_sgCD_R1_splicing -o libraries_4/WT_sgCD_R1_antisense_branch --subst_type without</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small fixes. Working on graph plots.
</commit_message>
<xml_diff>
--- a/libinfo.xlsx
+++ b/libinfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tchan\Code\SCMB_Project\RNA-mediated_DSB_repair\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2B7B77-686E-4572-9A8D-09DFE54C5CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A643F8D8-B727-4BDC-A863-1B6E854126FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="6" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="7" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
   </bookViews>
   <sheets>
     <sheet name="globals" sheetId="3" r:id="rId1"/>
@@ -20,9 +20,11 @@
     <sheet name="3_graph" sheetId="4" r:id="rId5"/>
     <sheet name="4_graph_combined" sheetId="5" r:id="rId6"/>
     <sheet name="5_histogram_3d" sheetId="11" r:id="rId7"/>
+    <sheet name="6_plot_graph" sheetId="13" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="dsb">'1_repeats'!$D:$D</definedName>
+    <definedName name="graph">globals!$A$7</definedName>
     <definedName name="histogram_3d">globals!$A$6</definedName>
     <definedName name="libraries_1">globals!$A$1</definedName>
     <definedName name="libraries_2">globals!$A$2</definedName>
@@ -73,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1473" uniqueCount="177">
   <si>
     <t>yjl217</t>
   </si>
@@ -602,6 +604,9 @@
   <si>
     <t>command</t>
   </si>
+  <si>
+    <t>plots/graphs</t>
+  </si>
 </sst>
 </file>
 
@@ -691,7 +696,76 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{FFD19645-61C4-4244-A560-0232B787F38C}"/>
   </cellStyles>
-  <dxfs count="100">
+  <dxfs count="116">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -882,9 +956,6 @@
         </patternFill>
       </fill>
       <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1365,7 +1436,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22A90416-B904-4D3D-A6DB-EFCB9FD1EAED}" name="Table1" displayName="Table1" ref="A1:N173" totalsRowShown="0" headerRowDxfId="99">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22A90416-B904-4D3D-A6DB-EFCB9FD1EAED}" name="Table1" displayName="Table1" ref="A1:N173" totalsRowShown="0" headerRowDxfId="115">
   <autoFilter ref="A1:N173" xr:uid="{22A90416-B904-4D3D-A6DB-EFCB9FD1EAED}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{5C1CDEE9-AAC7-4E12-B88F-1314CF422335}" name="library"/>
@@ -1375,25 +1446,25 @@
     <tableColumn id="5" xr3:uid="{81A143FE-8E74-4182-8124-E697DD5A7C62}" name="hguide"/>
     <tableColumn id="6" xr3:uid="{4A316E6A-69F3-4B78-9C01-4675AEB656FA}" name="treatment"/>
     <tableColumn id="7" xr3:uid="{25B8E763-346D-4756-8B58-D3C8CB103545}" name="strand"/>
-    <tableColumn id="8" xr3:uid="{4B708639-BB19-4DC1-A57D-214FA0EFB1EA}" name="dsb_pos" dataDxfId="98">
+    <tableColumn id="8" xr3:uid="{4B708639-BB19-4DC1-A57D-214FA0EFB1EA}" name="dsb_pos" dataDxfId="114">
       <calculatedColumnFormula array="1">IF(D2="2DSB", IF(G2="R1", 67, 46), IF(D2="1DSB", IF(G2="R1", 67, 46), IF(D2="2DSBanti", IF(G2="R1", 50, 47), NA))) + IF(Table1[[#This Row],[control]]="30bpDown", 30, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{CCF6021C-1B60-4954-A92E-3F2848564215}" name="file_in" dataDxfId="97">
+    <tableColumn id="9" xr3:uid="{CCF6021C-1B60-4954-A92E-3F2848564215}" name="file_in" dataDxfId="113">
       <calculatedColumnFormula>IF(OR(Table1[[#This Row],[control]]="none", Table1[[#This Row],[control]]="30bpDown"), _xlfn.CONCAT(Table1[[#This Row],[library]], IF(Table1[[#This Row],[dsb]] = "2DSBanti", "_anti", ""), "_",Table1[[#This Row],[strand]],"_", IF(LEFT(Table1[[#This Row],[dsb]], 1)="2","2DSBs", Table1[[#This Row],[hguide]]), ".sam"), _xlfn.CONCAT(Table1[[#This Row],[library]], "_NHEJ_", IF(Table1[[#This Row],[hguide]]="sgA", "hg39", IF(Table1[[#This Row],[hguide]]="sgB", "hg42", "2DSB")), "_", Table1[[#This Row],[strand]], ".sam"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{58220462-2A11-4DAD-A247-C0871AFCFDB4}" name="file_out" dataDxfId="96">
+    <tableColumn id="10" xr3:uid="{58220462-2A11-4DAD-A247-C0871AFCFDB4}" name="file_out" dataDxfId="112">
       <calculatedColumnFormula>_xlfn.CONCAT(Table1[[#This Row],[library]], "_", Table1[[#This Row],[cell_line]], "_", Table1[[#This Row],[hguide]], "_", Table1[[#This Row],[strand]], "_", Table1[[#This Row],[treatment]], IF(Table1[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", Table1[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{775EE7A9-3C78-4568-BF98-500DE451177C}" name="ref_file" dataDxfId="95">
+    <tableColumn id="11" xr3:uid="{775EE7A9-3C78-4568-BF98-500DE451177C}" name="ref_file" dataDxfId="111">
       <calculatedColumnFormula>_xlfn.CONCAT(Table1[[#This Row],[dsb]],"_", Table1[[#This Row],[strand]],"_", Table1[[#This Row],[treatment]], ".fa")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="12" xr3:uid="{5B945FB6-D054-40C4-AAEF-BB50B19F8936}" name="total_reads">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],[library]], Table9[#All], 2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{66485B06-471E-47D3-BA91-FC751F58FA5A}" name="min_length" dataDxfId="94">
+    <tableColumn id="13" xr3:uid="{66485B06-471E-47D3-BA91-FC751F58FA5A}" name="min_length" dataDxfId="110">
       <calculatedColumnFormula>IF(LEFT(Table1[[#This Row],[dsb]], 1) = "2", 50, 130)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{DF3C46EA-690D-4E6A-99CF-BBC2B2F74AFF}" name="command_filter_nhej" dataDxfId="25">
+    <tableColumn id="14" xr3:uid="{DF3C46EA-690D-4E6A-99CF-BBC2B2F74AFF}" name="command_filter_nhej" dataDxfId="42">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", Table1[[#This Row],[file_in]], " -ref ref_seq/", Table1[[#This Row],[ref_file]], " -o ", libraries_2, "/", Table1[[#This Row],[file_out]], ".tsv", " --min_length ", Table1[[#This Row],[min_length]], " -dsb ", Table1[[#This Row],[dsb_pos]], " --quiet")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1402,44 +1473,44 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}" name="Table513" displayName="Table513" ref="A1:M41" totalsRowShown="0" headerRowDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}" name="Table513" displayName="Table513" ref="A1:M41" totalsRowShown="0" headerRowDxfId="57">
   <autoFilter ref="A1:M41" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
   <tableColumns count="13">
-    <tableColumn id="25" xr3:uid="{43F57146-0E56-46F3-A0E3-717A41010F4A}" name="index" dataDxfId="40"/>
-    <tableColumn id="1" xr3:uid="{B0B3F6B0-7577-49AC-B865-1E873B4DC53C}" name="dir" dataDxfId="39">
+    <tableColumn id="25" xr3:uid="{43F57146-0E56-46F3-A0E3-717A41010F4A}" name="index" dataDxfId="56"/>
+    <tableColumn id="1" xr3:uid="{B0B3F6B0-7577-49AC-B865-1E873B4DC53C}" name="dir" dataDxfId="55">
       <calculatedColumnFormula>'2_combined'!J3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{D04F356F-9288-416D-ACDA-6BFE128B70D7}" name="control" dataDxfId="38">
+    <tableColumn id="13" xr3:uid="{D04F356F-9288-416D-ACDA-6BFE128B70D7}" name="control" dataDxfId="54">
       <calculatedColumnFormula>'2_combined'!C3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{9C168B22-F534-40D4-947C-918239C33FD9}" name="ref" dataDxfId="37">
+    <tableColumn id="2" xr3:uid="{9C168B22-F534-40D4-947C-918239C33FD9}" name="ref" dataDxfId="53">
       <calculatedColumnFormula>'2_combined'!B3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{6F64477B-0C66-4251-9156-22307A6D70A0}" name="dsb_pos" dataDxfId="36">
+    <tableColumn id="3" xr3:uid="{6F64477B-0C66-4251-9156-22307A6D70A0}" name="dsb_pos" dataDxfId="52">
       <calculatedColumnFormula>'2_combined'!E3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{D037F4F2-543F-4D7D-AB36-0B253FD61B0D}" name="dsb_type" dataDxfId="35">
+    <tableColumn id="4" xr3:uid="{D037F4F2-543F-4D7D-AB36-0B253FD61B0D}" name="dsb_type" dataDxfId="51">
       <calculatedColumnFormula>'2_combined'!D3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{407AC5E6-13CB-409A-8E78-64B8CC121882}" name="dsb_type_command" dataDxfId="34">
+    <tableColumn id="12" xr3:uid="{407AC5E6-13CB-409A-8E78-64B8CC121882}" name="dsb_type_command" dataDxfId="50">
       <calculatedColumnFormula array="1">IF(Table513[[#This Row],[dsb_type]]="2DSB", "2", IF(Table513[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table513[[#This Row],[dsb_type]]="1DSB", "1", NA)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{1A24C844-2A10-4394-818F-0C25A569B414}" name="strand" dataDxfId="33">
+    <tableColumn id="5" xr3:uid="{1A24C844-2A10-4394-818F-0C25A569B414}" name="strand" dataDxfId="49">
       <calculatedColumnFormula>'2_combined'!G3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{4F0A02F9-5555-489E-BA41-E3CBF81D1114}" name="hguide" dataDxfId="32">
+    <tableColumn id="6" xr3:uid="{4F0A02F9-5555-489E-BA41-E3CBF81D1114}" name="hguide" dataDxfId="48">
       <calculatedColumnFormula>MID('2_combined'!I3, 3, 100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FAE741F2-7C1B-41F2-8875-9F7A2EF40A54}" name="cell" dataDxfId="31">
+    <tableColumn id="7" xr3:uid="{FAE741F2-7C1B-41F2-8875-9F7A2EF40A54}" name="cell" dataDxfId="47">
       <calculatedColumnFormula>'2_combined'!F3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{FE3ED128-2534-43D1-9244-11AB1FB57650}" name="treatment" dataDxfId="30">
+    <tableColumn id="8" xr3:uid="{FE3ED128-2534-43D1-9244-11AB1FB57650}" name="treatment" dataDxfId="46">
       <calculatedColumnFormula>'2_combined'!H3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{65ACBC9C-0EC8-4074-B310-05F4B70BFAD5}" name="subst_type" dataDxfId="18">
+    <tableColumn id="9" xr3:uid="{65ACBC9C-0EC8-4074-B310-05F4B70BFAD5}" name="subst_type" dataDxfId="35">
       <calculatedColumnFormula>"with"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{F80F6FB9-4F35-4819-8285-D77131C6EFCE}" name="command" dataDxfId="19">
+    <tableColumn id="10" xr3:uid="{F80F6FB9-4F35-4819-8285-D77131C6EFCE}" name="command" dataDxfId="36">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/",Table513[[#This Row],[dir]], " -o ", histogram_3d, "/")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1448,14 +1519,14 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{D74A5276-1A50-4DA1-9131-9669404C8622}" name="Table1014" displayName="Table1014" ref="A43:N55" totalsRowShown="0">
-  <autoFilter ref="A43:N55" xr:uid="{D74A5276-1A50-4DA1-9131-9669404C8622}"/>
-  <tableColumns count="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{D74A5276-1A50-4DA1-9131-9669404C8622}" name="Table1014" displayName="Table1014" ref="A43:M55" totalsRowShown="0">
+  <autoFilter ref="A43:M55" xr:uid="{D74A5276-1A50-4DA1-9131-9669404C8622}"/>
+  <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{8AC09A63-4226-4C75-8801-68CF93C0F078}" name="index"/>
     <tableColumn id="2" xr3:uid="{77584C42-D70C-48A4-979A-F4DEA0B31542}" name="dir">
       <calculatedColumnFormula>'2_combined'!J45</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{483E3D73-4059-4B65-84EC-5DC4E7008F35}" name="control" dataDxfId="29">
+    <tableColumn id="3" xr3:uid="{483E3D73-4059-4B65-84EC-5DC4E7008F35}" name="control" dataDxfId="45">
       <calculatedColumnFormula>SUBSTITUTE('2_combined'!C45, "dsb", "DSB")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{5859A8DB-4C52-4451-BBB6-C6BEBF497540}" name="ref">
@@ -1482,14 +1553,103 @@
     <tableColumn id="11" xr3:uid="{0F1B5F9E-B10D-4258-9052-90BCDC89F0B0}" name="treatment">
       <calculatedColumnFormula>'2_combined'!H45</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A2723EF6-80E8-4D8D-A6DC-7556C1996222}" name="subst_type" dataDxfId="17">
+    <tableColumn id="12" xr3:uid="{A2723EF6-80E8-4D8D-A6DC-7556C1996222}" name="subst_type" dataDxfId="34">
       <calculatedColumnFormula>"with"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{02531CCA-6CDE-42BA-80E3-31C0F97A3546}" name="command_main_data" dataDxfId="16">
+    <tableColumn id="13" xr3:uid="{02531CCA-6CDE-42BA-80E3-31C0F97A3546}" name="command" dataDxfId="33">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/",Table1014[[#This Row],[dir]], " -o ", histogram_3d, "/")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{044D252B-8D18-4E92-82F7-0C8FAA410CB0}" name="command_graph_data" dataDxfId="28">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", Table1014[[#This Row],[subst_type]], " -dir ", globals!$A$4, "/", Table1014[[#This Row],[dir]])</calculatedColumnFormula>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{86CE8E4A-18BF-427A-81F0-F9655767A016}" name="Table51315" displayName="Table51315" ref="A1:M41" totalsRowShown="0" headerRowDxfId="16">
+  <autoFilter ref="A1:M41" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
+  <tableColumns count="13">
+    <tableColumn id="25" xr3:uid="{C323C376-24D3-4404-9E0F-6E9361862271}" name="index" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="14">
+      <calculatedColumnFormula>'2_combined'!J3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="13">
+      <calculatedColumnFormula>'2_combined'!C3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="12">
+      <calculatedColumnFormula>'2_combined'!B3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="11">
+      <calculatedColumnFormula>'2_combined'!E3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="10">
+      <calculatedColumnFormula>'2_combined'!D3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="9">
+      <calculatedColumnFormula array="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="8">
+      <calculatedColumnFormula>'2_combined'!G3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="7">
+      <calculatedColumnFormula>MID('2_combined'!I3, 3, 100)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="6">
+      <calculatedColumnFormula>'2_combined'!F3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="5">
+      <calculatedColumnFormula>'2_combined'!H3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="4">
+      <calculatedColumnFormula>"with"</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="1">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{B47D9508-D874-40FC-B6F6-C106B48F6A94}" name="Table101416" displayName="Table101416" ref="A43:M55" totalsRowShown="0">
+  <autoFilter ref="A43:M55" xr:uid="{D74A5276-1A50-4DA1-9131-9669404C8622}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{488C5146-A746-4F74-BCC8-806E4DC740CE}" name="index"/>
+    <tableColumn id="2" xr3:uid="{C2A88DF4-2444-4C4C-A089-6CF9ADE79BD8}" name="dir">
+      <calculatedColumnFormula>'2_combined'!J45</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{7698ACE3-2351-400D-B00F-5A70184F8A33}" name="control" dataDxfId="3">
+      <calculatedColumnFormula>SUBSTITUTE('2_combined'!C45, "dsb", "DSB")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{5E82B04C-FF09-492C-8A23-7E43B5990149}" name="ref">
+      <calculatedColumnFormula>'2_combined'!B45</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{F4D36A0E-549B-4F3A-BCA9-75E151448998}" name="dsb_pos">
+      <calculatedColumnFormula>'2_combined'!E45</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{AEBBBB88-8CE2-409D-AE19-9C23263250A9}" name="dsb_type">
+      <calculatedColumnFormula>'2_combined'!D45</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{3E71E7D2-0FA5-4FD5-BDC3-2955A091A9E6}" name="dsb_type_command">
+      <calculatedColumnFormula array="1">IF(Table101416[[#This Row],[dsb_type]]="2DSB", "2", IF(Table101416[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table101416[[#This Row],[dsb_type]]="1DSB", "1", NA)))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{EBD35881-E696-4202-9149-75A4EFFFAAD6}" name="strand">
+      <calculatedColumnFormula>'2_combined'!G45</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{123CA279-0CB6-41C1-9CD8-20D375B9B66D}" name="hguide">
+      <calculatedColumnFormula>MID('2_combined'!I45, 3, 100)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{3DCE3F3A-187D-411E-93FC-8C6C3EE9CAA2}" name="cell">
+      <calculatedColumnFormula>'2_combined'!F45</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{9E585D29-AB3E-4D04-8C1D-24F78339C9A3}" name="treatment">
+      <calculatedColumnFormula>'2_combined'!H45</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="12" xr3:uid="{928286B8-23FB-4375-B52B-617DD59D6098}" name="subst_type" dataDxfId="2">
+      <calculatedColumnFormula>"with"</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="13" xr3:uid="{0917AB98-1545-4642-9BE8-618AAA1E404A}" name="command" dataDxfId="0">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table101416[[#This Row],[dir]], " -o ", graph, "/")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1508,62 +1668,62 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}" name="Table3" displayName="Table3" ref="A2:S42" totalsRowShown="0" headerRowDxfId="93">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}" name="Table3" displayName="Table3" ref="A2:S42" totalsRowShown="0" headerRowDxfId="109">
   <autoFilter ref="A2:S42" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{C373869E-A92E-4B06-B8E5-C5A873420ED4}" name="index" dataDxfId="92"/>
-    <tableColumn id="2" xr3:uid="{A28AAC50-FA09-494A-B052-8489F07A5A70}" name="ref" dataDxfId="91">
+    <tableColumn id="1" xr3:uid="{C373869E-A92E-4B06-B8E5-C5A873420ED4}" name="index" dataDxfId="108"/>
+    <tableColumn id="2" xr3:uid="{A28AAC50-FA09-494A-B052-8489F07A5A70}" name="ref" dataDxfId="107">
       <calculatedColumnFormula>OFFSET('1_repeats'!$K$2, 4 * (Table3[[#This Row],[index]] - 1), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{07D57089-9737-4983-8884-C4ACCDCFF6CB}" name="control" dataDxfId="90">
+    <tableColumn id="18" xr3:uid="{07D57089-9737-4983-8884-C4ACCDCFF6CB}" name="control" dataDxfId="106">
       <calculatedColumnFormula>OFFSET('1_repeats'!$C$2, 4 * (Table3[[#This Row],[index]] - 1), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{C6423FEA-272F-48D3-BC6A-909FCA937DA9}" name="dsb" dataDxfId="89">
+    <tableColumn id="19" xr3:uid="{C6423FEA-272F-48D3-BC6A-909FCA937DA9}" name="dsb" dataDxfId="105">
       <calculatedColumnFormula>OFFSET('1_repeats'!$D$2, 4 * (Table3[[#This Row],[index]] - 1), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B8F61088-5FFA-4860-BF4E-1BFB301A31D9}" name="dsb_pos" dataDxfId="88">
+    <tableColumn id="3" xr3:uid="{B8F61088-5FFA-4860-BF4E-1BFB301A31D9}" name="dsb_pos" dataDxfId="104">
       <calculatedColumnFormula>OFFSET('1_repeats'!$H$2, 4 * (Table3[[#This Row],[index]] - 1), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{524D5B3D-BB20-420D-B7E9-93A7F77CA728}" name="cell" dataDxfId="87">
+    <tableColumn id="4" xr3:uid="{524D5B3D-BB20-420D-B7E9-93A7F77CA728}" name="cell" dataDxfId="103">
       <calculatedColumnFormula>OFFSET('1_repeats'!$B$2, 4 * (Table3[[#This Row],[index]] - 1), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{CC918D20-5D79-4223-9717-2CA0EFFA213F}" name="strand" dataDxfId="86">
+    <tableColumn id="5" xr3:uid="{CC918D20-5D79-4223-9717-2CA0EFFA213F}" name="strand" dataDxfId="102">
       <calculatedColumnFormula>OFFSET('1_repeats'!$G$2, 4 * (Table3[[#This Row],[index]] - 1), 0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{B2851465-D533-4787-80C4-E844BB2ABB8C}" name="treatment">
       <calculatedColumnFormula>OFFSET('1_repeats'!$F$2, 4 * (A3 - 1), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{849BE448-7739-4815-A2C5-5843F62D83D7}" name="hguide" dataDxfId="85">
+    <tableColumn id="7" xr3:uid="{849BE448-7739-4815-A2C5-5843F62D83D7}" name="hguide" dataDxfId="101">
       <calculatedColumnFormula>OFFSET('1_repeats'!$E$2, 4 * (Table3[[#This Row],[index]]- 1), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{343716D9-C3A9-4F90-A58A-42B1B9C79EBF}" name="output_dir" dataDxfId="63">
+    <tableColumn id="8" xr3:uid="{343716D9-C3A9-4F90-A58A-42B1B9C79EBF}" name="output_dir" dataDxfId="79">
       <calculatedColumnFormula>_xlfn.CONCAT(Table3[[#This Row],[cell]], "_", Table3[[#This Row],[hguide]], "_", Table3[[#This Row],[strand]], "_", Table3[[#This Row],[treatment]], IF(Table3[[#This Row],[control]]&lt;&gt;"none",_xlfn.CONCAT("_", Table3[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D29558AA-D418-4CDD-81AE-A987E7BC501D}" name="input_1" dataDxfId="84">
+    <tableColumn id="9" xr3:uid="{D29558AA-D418-4CDD-81AE-A987E7BC501D}" name="input_1" dataDxfId="100">
       <calculatedColumnFormula>OFFSET('1_repeats'!$J$1, 4 * (Table3[[#This Row],[index]] - 1)  + ($K$1), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{E2ABF5A3-B032-47F7-9141-9F269EFD9D49}" name="total_reads_1" dataDxfId="83">
+    <tableColumn id="10" xr3:uid="{E2ABF5A3-B032-47F7-9141-9F269EFD9D49}" name="total_reads_1" dataDxfId="99">
       <calculatedColumnFormula array="1">OFFSET('1_repeats'!$L$1, 4 * (Table3[[#This Row],[index]] - 1)  + INDIRECT(ADDRESS(1, COLUMN())), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{6B1B21F6-1584-4712-844D-99F3DBE8B3D9}" name="input_2" dataDxfId="82">
+    <tableColumn id="11" xr3:uid="{6B1B21F6-1584-4712-844D-99F3DBE8B3D9}" name="input_2" dataDxfId="98">
       <calculatedColumnFormula>OFFSET('1_repeats'!$J$1, 4 * (Table3[[#This Row],[index]] - 1)  + ($M$1), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{C7B1BE14-3BD6-413B-8575-DE9712F9761A}" name="total_reads_2" dataDxfId="81">
+    <tableColumn id="12" xr3:uid="{C7B1BE14-3BD6-413B-8575-DE9712F9761A}" name="total_reads_2" dataDxfId="97">
       <calculatedColumnFormula array="1">OFFSET('1_repeats'!$L$1, 4 * (Table3[[#This Row],[index]] - 1)  + INDIRECT(ADDRESS(1, COLUMN())), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{6BE840C3-79BA-41DC-90D3-918C6C412936}" name="input_3" dataDxfId="80">
+    <tableColumn id="13" xr3:uid="{6BE840C3-79BA-41DC-90D3-918C6C412936}" name="input_3" dataDxfId="96">
       <calculatedColumnFormula>OFFSET('1_repeats'!$J$1, 4 * (Table3[[#This Row],[index]] - 1)  + ($O$1), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{6A8CE344-45B9-42E3-95D8-8EB6A485D968}" name="total_reads_3" dataDxfId="79">
+    <tableColumn id="14" xr3:uid="{6A8CE344-45B9-42E3-95D8-8EB6A485D968}" name="total_reads_3" dataDxfId="95">
       <calculatedColumnFormula array="1">OFFSET('1_repeats'!$L$1, 4 * (Table3[[#This Row],[index]] - 1)  + INDIRECT(ADDRESS(1, COLUMN())), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{17F598DE-E755-49D6-AFC6-70309C0348FD}" name="input_4" dataDxfId="78">
+    <tableColumn id="15" xr3:uid="{17F598DE-E755-49D6-AFC6-70309C0348FD}" name="input_4" dataDxfId="94">
       <calculatedColumnFormula>OFFSET('1_repeats'!$J$1, 4 * (Table3[[#This Row],[index]] - 1)  + ($Q$1), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{AC170216-9CAE-43B8-A8E2-8FE1529F6D55}" name="total_reads_4" dataDxfId="77">
+    <tableColumn id="16" xr3:uid="{AC170216-9CAE-43B8-A8E2-8FE1529F6D55}" name="total_reads_4" dataDxfId="93">
       <calculatedColumnFormula array="1">OFFSET('1_repeats'!$L$1, 4 * (Table3[[#This Row],[index]] - 1)  + INDIRECT(ADDRESS(1, COLUMN())), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{A285A0DD-6F6D-404D-AE2A-0D1FC3DDB459}" name="command_combine" dataDxfId="15">
+    <tableColumn id="17" xr3:uid="{A285A0DD-6F6D-404D-AE2A-0D1FC3DDB459}" name="command_combine" dataDxfId="32">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -in ", libraries_2, "/", Table3[[#This Row],[input_1]], ".tsv ", libraries_2, "/", Table3[[#This Row],[input_2]], ".tsv ", libraries_2, "/", Table3[[#This Row],[input_3]], ".tsv ", libraries_2, "/", Table3[[#This Row],[input_4]], ".tsv --total_reads ", Table3[[#This Row],[total_reads_1]], " ", Table3[[#This Row],[total_reads_2]], " ", Table3[[#This Row],[total_reads_3]], " ", Table3[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", Table3[[#This Row],[output_dir]], ".tsv", " --quiet ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1575,7 +1735,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{7D969AC7-2D2F-45B0-BA99-D174130B0A52}" name="Table11" displayName="Table11" ref="A44:M56" totalsRowShown="0">
   <autoFilter ref="A44:M56" xr:uid="{7D969AC7-2D2F-45B0-BA99-D174130B0A52}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{D612E3DF-AA8E-4EE0-9306-7903B4821992}" name="index" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{D612E3DF-AA8E-4EE0-9306-7903B4821992}" name="index" dataDxfId="65"/>
     <tableColumn id="2" xr3:uid="{B00239B6-16E0-4472-B8C9-F25D625D21DD}" name="ref">
       <calculatedColumnFormula>'1_repeats'!K162</calculatedColumnFormula>
     </tableColumn>
@@ -1609,7 +1769,7 @@
     <tableColumn id="12" xr3:uid="{BB84920E-3487-4670-93ED-5671EACD3061}" name="total_reads">
       <calculatedColumnFormula>'1_repeats'!L162</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{0CE6DAF6-0C4C-4EC5-8FE5-9B3840A02412}" name="command_combine" dataDxfId="24">
+    <tableColumn id="13" xr3:uid="{0CE6DAF6-0C4C-4EC5-8FE5-9B3840A02412}" name="command_combine" dataDxfId="41">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", Table11[[#This Row],[input]], ".tsv ", " --total_reads ", Table11[[#This Row],[total_reads]], " -o ", libraries_3, "/", Table11[[#This Row],[output_dir]], ".tsv", " --quiet ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1618,47 +1778,47 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}" name="Table5" displayName="Table5" ref="A1:N41" totalsRowShown="0" headerRowDxfId="76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}" name="Table5" displayName="Table5" ref="A1:N41" totalsRowShown="0" headerRowDxfId="92">
   <autoFilter ref="A1:N41" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}"/>
   <tableColumns count="14">
-    <tableColumn id="25" xr3:uid="{93D2F09B-24D5-4FE1-BF34-C037E361889F}" name="index" dataDxfId="75"/>
-    <tableColumn id="1" xr3:uid="{2F28DC66-449D-4F81-AA63-8F24B25F33D1}" name="dir" dataDxfId="74">
+    <tableColumn id="25" xr3:uid="{93D2F09B-24D5-4FE1-BF34-C037E361889F}" name="index" dataDxfId="91"/>
+    <tableColumn id="1" xr3:uid="{2F28DC66-449D-4F81-AA63-8F24B25F33D1}" name="dir" dataDxfId="90">
       <calculatedColumnFormula>'2_combined'!J3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{3DF6F698-1F9A-4B05-A310-657CCFCE9F66}" name="control" dataDxfId="64">
+    <tableColumn id="13" xr3:uid="{3DF6F698-1F9A-4B05-A310-657CCFCE9F66}" name="control" dataDxfId="80">
       <calculatedColumnFormula>'2_combined'!C3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{362C2395-52F7-4A62-B7BA-2DD97ED5E6FB}" name="ref" dataDxfId="73">
+    <tableColumn id="2" xr3:uid="{362C2395-52F7-4A62-B7BA-2DD97ED5E6FB}" name="ref" dataDxfId="89">
       <calculatedColumnFormula>'2_combined'!B3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5F0895D9-2EF2-4524-8BC7-15A33FE68636}" name="dsb_pos" dataDxfId="72">
+    <tableColumn id="3" xr3:uid="{5F0895D9-2EF2-4524-8BC7-15A33FE68636}" name="dsb_pos" dataDxfId="88">
       <calculatedColumnFormula>'2_combined'!E3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C6D28829-46E6-4D97-8EA4-0AD12EF6CF10}" name="dsb_type" dataDxfId="71">
+    <tableColumn id="4" xr3:uid="{C6D28829-46E6-4D97-8EA4-0AD12EF6CF10}" name="dsb_type" dataDxfId="87">
       <calculatedColumnFormula>'2_combined'!D3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{E8B2E211-C273-4602-86F0-60EA4259B7A4}" name="dsb_type_command" dataDxfId="70">
+    <tableColumn id="12" xr3:uid="{E8B2E211-C273-4602-86F0-60EA4259B7A4}" name="dsb_type_command" dataDxfId="86">
       <calculatedColumnFormula array="1">IF(Table5[[#This Row],[dsb_type]]="2DSB", "2", IF(Table5[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table5[[#This Row],[dsb_type]]="1DSB", "1", NA)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{15578E86-B7BE-4D8E-8FD4-E6C9C4F35C9C}" name="strand" dataDxfId="69">
+    <tableColumn id="5" xr3:uid="{15578E86-B7BE-4D8E-8FD4-E6C9C4F35C9C}" name="strand" dataDxfId="85">
       <calculatedColumnFormula>'2_combined'!G3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3366AC40-6578-4797-B607-19265E7DBF5C}" name="hguide" dataDxfId="68">
+    <tableColumn id="6" xr3:uid="{3366AC40-6578-4797-B607-19265E7DBF5C}" name="hguide" dataDxfId="84">
       <calculatedColumnFormula>MID('2_combined'!I3, 3, 100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{554F4E79-98DE-474B-A5C8-D4B536772E95}" name="cell" dataDxfId="67">
+    <tableColumn id="7" xr3:uid="{554F4E79-98DE-474B-A5C8-D4B536772E95}" name="cell" dataDxfId="83">
       <calculatedColumnFormula>'2_combined'!F3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{32FC5061-DD85-4234-9ED8-FEAF6D9E3BC0}" name="treatment" dataDxfId="66">
+    <tableColumn id="8" xr3:uid="{32FC5061-DD85-4234-9ED8-FEAF6D9E3BC0}" name="treatment" dataDxfId="82">
       <calculatedColumnFormula>'2_combined'!H3</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{DB6998A3-1431-4DDD-8DA0-525B805BF436}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{367B0912-E7A8-4430-962D-4F79EE14E5EA}" name="command_main_data" dataDxfId="14">
+    <tableColumn id="10" xr3:uid="{367B0912-E7A8-4430-962D-4F79EE14E5EA}" name="command_main_data" dataDxfId="31">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",Table5[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", Table5[[#This Row],[dir]], " -ref ref_seq/", Table5[[#This Row],[ref]], " -dsb ", Table5[[#This Row],[dsb_pos]], " --dsb_type ",Table5[[#This Row],[dsb_type_command]], " --strand ", Table5[[#This Row],[strand]], " --hguide ", Table5[[#This Row],[hguide]], " --cell ", Table5[[#This Row],[cell]], " --treatment ", Table5[[#This Row],[treatment]], " --subst_type ", Table5[[#This Row],[subst_type]], " --control ", Table5[[#This Row],[control]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{4A65279E-321E-4E3E-8383-26D448C2012F}" name="command_graph_data" dataDxfId="23">
+    <tableColumn id="11" xr3:uid="{4A65279E-321E-4E3E-8383-26D448C2012F}" name="command_graph_data" dataDxfId="40">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", Table5[[#This Row],[subst_type]], " -dir ", libraries_4, "/", Table5[[#This Row],[dir]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1674,7 +1834,7 @@
     <tableColumn id="2" xr3:uid="{5B7F1A2A-EC69-4E5A-BEF9-DA0BB1F6D84F}" name="dir">
       <calculatedColumnFormula>'2_combined'!J45</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5911EF6D-9D4A-4737-925D-230D175C0AD0}" name="control" dataDxfId="44">
+    <tableColumn id="3" xr3:uid="{5911EF6D-9D4A-4737-925D-230D175C0AD0}" name="control" dataDxfId="60">
       <calculatedColumnFormula>SUBSTITUTE('2_combined'!C45, "dsb", "DSB")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{8DB9ADE6-D3E8-4451-9780-7AC62CFAAC8A}" name="ref">
@@ -1701,13 +1861,13 @@
     <tableColumn id="11" xr3:uid="{08EAD756-AA31-4DE2-B500-71FE3AA9EA6F}" name="treatment">
       <calculatedColumnFormula>'2_combined'!H45</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{79869E15-3FDE-43F8-AD44-2CB6888FCFF5}" name="subst_type" dataDxfId="27">
+    <tableColumn id="12" xr3:uid="{79869E15-3FDE-43F8-AD44-2CB6888FCFF5}" name="subst_type" dataDxfId="44">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{F52A28AD-B89A-419E-8DBE-A81D738193B6}" name="command_main_data" dataDxfId="13">
+    <tableColumn id="13" xr3:uid="{F52A28AD-B89A-419E-8DBE-A81D738193B6}" name="command_main_data" dataDxfId="30">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",Table10[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", Table10[[#This Row],[dir]], " -ref ref_seq/", Table10[[#This Row],[ref]], " -dsb ", Table10[[#This Row],[dsb_pos]], " --dsb_type ",Table10[[#This Row],[dsb_type_command]], " --strand ", Table10[[#This Row],[strand]], " --hguide ", Table10[[#This Row],[hguide]], " --cell ", Table10[[#This Row],[cell]], " --treatment ", Table10[[#This Row],[treatment]], " --subst_type ", Table10[[#This Row],[subst_type]], " --control ", Table10[[#This Row],[control]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{AC6F291F-482F-4B13-86D4-8C748D325E95}" name="command_graph_data" dataDxfId="22">
+    <tableColumn id="14" xr3:uid="{AC6F291F-482F-4B13-86D4-8C748D325E95}" name="command_graph_data" dataDxfId="39">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", Table10[[#This Row],[subst_type]], " -dir ", libraries_4, "/", Table10[[#This Row],[dir]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1716,38 +1876,38 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}" name="Table6" displayName="Table6" ref="A1:K17" totalsRowShown="0" headerRowDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}" name="Table6" displayName="Table6" ref="A1:K17" totalsRowShown="0" headerRowDxfId="81">
   <autoFilter ref="A1:K17" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B7EC223D-BA24-48F1-9EE3-DC56DEFDE4C2}" name="index" dataDxfId="61"/>
-    <tableColumn id="7" xr3:uid="{D9F1ADDA-18A2-4F81-862D-6B0F786079FF}" name="control" dataDxfId="59">
+    <tableColumn id="1" xr3:uid="{B7EC223D-BA24-48F1-9EE3-DC56DEFDE4C2}" name="index" dataDxfId="77"/>
+    <tableColumn id="7" xr3:uid="{D9F1ADDA-18A2-4F81-862D-6B0F786079FF}" name="control" dataDxfId="75">
       <calculatedColumnFormula>OFFSET('3_graph'!$C$3, 3 * QUOTIENT(Table6[[#This Row],[index]] - 1, 2), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{0EA5A81F-6EA1-4256-9717-03273165F7BF}" name="treatment_1" dataDxfId="58">
+    <tableColumn id="8" xr3:uid="{0EA5A81F-6EA1-4256-9717-03273165F7BF}" name="treatment_1" dataDxfId="74">
       <calculatedColumnFormula>OFFSET('3_graph'!$K$2, 3 * QUOTIENT(Table6[[#This Row],[index]] - 1, 2), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5F6D005A-96D8-4801-93E2-101BAE551BA8}" name="dir_1" dataDxfId="60">
+    <tableColumn id="2" xr3:uid="{5F6D005A-96D8-4801-93E2-101BAE551BA8}" name="dir_1" dataDxfId="76">
       <calculatedColumnFormula>OFFSET('3_graph'!$B$2, 3 * QUOTIENT(Table6[[#This Row],[index]] - 1, 2), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C21D1AF7-7ABE-4181-AA2A-42227869A8DD}" name="treatment_2" dataDxfId="57">
+    <tableColumn id="9" xr3:uid="{C21D1AF7-7ABE-4181-AA2A-42227869A8DD}" name="treatment_2" dataDxfId="73">
       <calculatedColumnFormula>OFFSET('3_graph'!$K$2, 3 * QUOTIENT(Table6[[#This Row],[index]] - 1, 2) + 1 + MOD(Table6[[#This Row],[index]] - 1, 2), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{D66426AC-E0B2-4B07-A4D4-5A74AA033E80}" name="dir_2" dataDxfId="62">
+    <tableColumn id="3" xr3:uid="{D66426AC-E0B2-4B07-A4D4-5A74AA033E80}" name="dir_2" dataDxfId="78">
       <calculatedColumnFormula>OFFSET('3_graph'!$B$2, 3 * QUOTIENT(Table6[[#This Row],[index]] - 1, 2) + 1 + MOD(Table6[[#This Row],[index]] - 1, 2), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{0C8146A0-DC77-4DC4-82FF-74F4C74CF33E}" name="treatments_out" dataDxfId="46">
+    <tableColumn id="10" xr3:uid="{0C8146A0-DC77-4DC4-82FF-74F4C74CF33E}" name="treatments_out" dataDxfId="62">
       <calculatedColumnFormula>_xlfn.CONCAT(Table6[[#This Row],[treatment_1]], "_", Table6[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{519A6397-7A3C-4009-B8B9-A71C0B3A591B}" name="dir_out" dataDxfId="45">
+    <tableColumn id="4" xr3:uid="{519A6397-7A3C-4009-B8B9-A71C0B3A591B}" name="dir_out" dataDxfId="61">
       <calculatedColumnFormula>SUBSTITUTE(Table6[[#This Row],[dir_1]], Table6[[#This Row],[treatment_1]], Table6[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E1629355-7D02-4819-98A1-EEB3B5FADE18}" name="subst_type" dataDxfId="26">
+    <tableColumn id="5" xr3:uid="{E1629355-7D02-4819-98A1-EEB3B5FADE18}" name="subst_type" dataDxfId="43">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{BC9117A0-CB6F-4D3C-A0E4-BF8395854D9A}" name="command_main_data_combined" dataDxfId="21">
+    <tableColumn id="6" xr3:uid="{BC9117A0-CB6F-4D3C-A0E4-BF8395854D9A}" name="command_main_data_combined" dataDxfId="38">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", Table6[[#This Row],[dir_1]], " ", libraries_4, "/", Table6[[#This Row],[dir_2]], " -o ", libraries_4, "/", Table6[[#This Row],[dir_out]], " --subst_type ", Table6[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{D384013E-9937-4DD8-A36A-43325757359B}" name="command_graph_data" dataDxfId="43">
+    <tableColumn id="11" xr3:uid="{D384013E-9937-4DD8-A36A-43325757359B}" name="command_graph_data" dataDxfId="59">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", Table6[[#This Row],[subst_type]], " -dir ", globals!$A$4, "/", Table6[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1756,38 +1916,38 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}" name="Table68" displayName="Table68" ref="A19:K21" totalsRowShown="0" headerRowDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}" name="Table68" displayName="Table68" ref="A19:K21" totalsRowShown="0" headerRowDxfId="72">
   <autoFilter ref="A19:K21" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{7F5A3A15-751D-407C-A035-61B2605E693F}" name="index" dataDxfId="55"/>
-    <tableColumn id="7" xr3:uid="{45863AB0-FD32-49FE-B4BF-F8EE865F7604}" name="control" dataDxfId="54">
+    <tableColumn id="1" xr3:uid="{7F5A3A15-751D-407C-A035-61B2605E693F}" name="index" dataDxfId="71"/>
+    <tableColumn id="7" xr3:uid="{45863AB0-FD32-49FE-B4BF-F8EE865F7604}" name="control" dataDxfId="70">
       <calculatedColumnFormula>OFFSET('3_graph'!$C$26, 2 * (Table68[[#This Row],[index]] - 1), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{CD16648D-267E-410B-A366-3E12367C037C}" name="treatment_1" dataDxfId="53">
+    <tableColumn id="8" xr3:uid="{CD16648D-267E-410B-A366-3E12367C037C}" name="treatment_1" dataDxfId="69">
       <calculatedColumnFormula>OFFSET('3_graph'!$K$26, 2 * (Table68[[#This Row],[index]] - 1), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{10C9F90E-86FD-4BFE-939E-298FD6F69F12}" name="dir_1" dataDxfId="52">
+    <tableColumn id="2" xr3:uid="{10C9F90E-86FD-4BFE-939E-298FD6F69F12}" name="dir_1" dataDxfId="68">
       <calculatedColumnFormula>OFFSET('3_graph'!$B$26, 2 * (Table68[[#This Row],[index]] - 1), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{7AB3E4AB-F43B-4FDE-96D7-FBBB4A8B83BE}" name="treatment_2" dataDxfId="51">
+    <tableColumn id="9" xr3:uid="{7AB3E4AB-F43B-4FDE-96D7-FBBB4A8B83BE}" name="treatment_2" dataDxfId="67">
       <calculatedColumnFormula>OFFSET('3_graph'!$K$26, 2 * (Table68[[#This Row],[index]] - 1) + 1, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BF948A3E-9649-41BF-A7E7-57BFDE810FE9}" name="dir_2" dataDxfId="50">
+    <tableColumn id="3" xr3:uid="{BF948A3E-9649-41BF-A7E7-57BFDE810FE9}" name="dir_2" dataDxfId="66">
       <calculatedColumnFormula>OFFSET('3_graph'!$B$26, 2 * (Table68[[#This Row],[index]] - 1) + 1, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{378119E5-F021-4785-A653-4D632F029AA6}" name="treatments_out" dataDxfId="47">
+    <tableColumn id="10" xr3:uid="{378119E5-F021-4785-A653-4D632F029AA6}" name="treatments_out" dataDxfId="63">
       <calculatedColumnFormula>_xlfn.CONCAT(Table68[[#This Row],[treatment_1]], "_", Table68[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AE1A14DC-D0C9-4818-B8CC-09A571E73BC2}" name="dir_out" dataDxfId="48">
+    <tableColumn id="4" xr3:uid="{AE1A14DC-D0C9-4818-B8CC-09A571E73BC2}" name="dir_out" dataDxfId="64">
       <calculatedColumnFormula>SUBSTITUTE(Table68[[#This Row],[dir_1]], Table68[[#This Row],[treatment_1]], Table68[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{F29DAC4E-FEC5-4C1D-AAC1-7CE19E401F25}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{DC4E99F4-97AB-4553-A5FB-D20D3D487947}" name="command_main_data_combined" dataDxfId="20">
+    <tableColumn id="6" xr3:uid="{DC4E99F4-97AB-4553-A5FB-D20D3D487947}" name="command_main_data_combined" dataDxfId="37">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", Table68[[#This Row],[dir_1]], " ", libraries_4, "/", Table68[[#This Row],[dir_2]], " -o ", libraries_4, "/", Table68[[#This Row],[dir_out]], " --subst_type ", Table68[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{E19D3001-2E76-4CC2-BF33-D0465C77D538}" name="command_graph_data" dataDxfId="42">
+    <tableColumn id="11" xr3:uid="{E19D3001-2E76-4CC2-BF33-D0465C77D538}" name="command_graph_data" dataDxfId="58">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", Table68[[#This Row],[subst_type]], " -dir ", globals!$A$4, "/", Table68[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1796,38 +1956,38 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{DF721F9E-54DB-422A-8466-77EDBF2287AF}" name="Table69" displayName="Table69" ref="A24:K32" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{DF721F9E-54DB-422A-8466-77EDBF2287AF}" name="Table69" displayName="Table69" ref="A24:K32" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="A24:K32" xr:uid="{DF721F9E-54DB-422A-8466-77EDBF2287AF}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{4B2D38BB-C594-4CFF-A307-A134FF1DBF8B}" name="index" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{CC939230-FB0E-416F-B345-7A4DD4839870}" name="control" dataDxfId="11">
+    <tableColumn id="1" xr3:uid="{4B2D38BB-C594-4CFF-A307-A134FF1DBF8B}" name="index" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{CC939230-FB0E-416F-B345-7A4DD4839870}" name="control" dataDxfId="28">
       <calculatedColumnFormula>OFFSET('3_graph'!$C$30, 3 * QUOTIENT(Table69[[#This Row],[index]] - 1, 2), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{AF3BF10E-758C-4395-83F8-5F1B20B1ABB6}" name="treatment_1" dataDxfId="10">
+    <tableColumn id="8" xr3:uid="{AF3BF10E-758C-4395-83F8-5F1B20B1ABB6}" name="treatment_1" dataDxfId="27">
       <calculatedColumnFormula>OFFSET('3_graph'!$K$30, 3 * QUOTIENT(Table69[[#This Row],[index]] - 1, 2), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{0E2E8B48-A535-4A36-B8D0-3BC864F39FE8}" name="dir_1" dataDxfId="9">
+    <tableColumn id="2" xr3:uid="{0E2E8B48-A535-4A36-B8D0-3BC864F39FE8}" name="dir_1" dataDxfId="26">
       <calculatedColumnFormula>OFFSET('3_graph'!$B$30, 3 * QUOTIENT(Table69[[#This Row],[index]] - 1, 2), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{10535B63-D8B1-4531-B393-DEE364AD65FC}" name="treatment_2" dataDxfId="8">
+    <tableColumn id="9" xr3:uid="{10535B63-D8B1-4531-B393-DEE364AD65FC}" name="treatment_2" dataDxfId="25">
       <calculatedColumnFormula>OFFSET('3_graph'!$K$30, 3 * QUOTIENT(Table69[[#This Row],[index]] - 1, 2) + 1 + MOD(Table69[[#This Row],[index]] - 1, 2), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{38434F18-6E6B-4445-9468-F1AC68C767A1}" name="dir_2" dataDxfId="7">
+    <tableColumn id="3" xr3:uid="{38434F18-6E6B-4445-9468-F1AC68C767A1}" name="dir_2" dataDxfId="24">
       <calculatedColumnFormula>OFFSET('3_graph'!$B$30, 3 * QUOTIENT(Table69[[#This Row],[index]] - 1, 2) + 1 + MOD(Table69[[#This Row],[index]] - 1, 2), 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{D8505D76-DFE0-404D-80FB-E23FCF6C4138}" name="treatments_out" dataDxfId="6">
+    <tableColumn id="10" xr3:uid="{D8505D76-DFE0-404D-80FB-E23FCF6C4138}" name="treatments_out" dataDxfId="23">
       <calculatedColumnFormula>_xlfn.CONCAT(Table69[[#This Row],[treatment_1]], "_", Table69[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{40A7ED64-C4FB-4223-B672-132B923E0A05}" name="dir_out" dataDxfId="5">
+    <tableColumn id="4" xr3:uid="{40A7ED64-C4FB-4223-B672-132B923E0A05}" name="dir_out" dataDxfId="22">
       <calculatedColumnFormula>SUBSTITUTE(Table69[[#This Row],[dir_1]], Table69[[#This Row],[treatment_1]], Table69[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{8212981C-68FE-482E-8379-C30BF6F1B4E7}" name="subst_type" dataDxfId="4">
+    <tableColumn id="5" xr3:uid="{8212981C-68FE-482E-8379-C30BF6F1B4E7}" name="subst_type" dataDxfId="21">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{A4B6DFAC-3439-4952-AA76-E967563DEB87}" name="command_main_data_combined" dataDxfId="3">
+    <tableColumn id="6" xr3:uid="{A4B6DFAC-3439-4952-AA76-E967563DEB87}" name="command_main_data_combined" dataDxfId="20">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", Table69[[#This Row],[dir_1]], " ", libraries_4, "/", Table69[[#This Row],[dir_2]], " -o ", libraries_4, "/", Table69[[#This Row],[dir_out]], " --subst_type ", Table69[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{C0DE1F11-E7E3-403F-A689-174A1F923BFE}" name="command_graph_data" dataDxfId="2">
+    <tableColumn id="11" xr3:uid="{C0DE1F11-E7E3-403F-A689-174A1F923BFE}" name="command_graph_data" dataDxfId="19">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", Table69[[#This Row],[subst_type]], " -dir ", globals!$A$4, "/", Table69[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2132,10 +2292,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86129707-88BE-44BB-B759-1CA0FE147BD8}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2175,6 +2335,11 @@
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -20137,10 +20302,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FCC207B-A9CD-4866-A17E-A3EE763F139F}">
-  <dimension ref="A1:N55"/>
+  <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D35" workbookViewId="0">
-      <selection activeCell="M44" sqref="M44:M55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21842,7 +22007,7 @@
         <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_cmv_30bpDown -o plots/histogram_3d/</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -21895,7 +22060,7 @@
         <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_sense_30bpDown -o plots/histogram_3d/</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -21948,7 +22113,7 @@
         <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_branch_30bpDown -o plots/histogram_3d/</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -22001,7 +22166,7 @@
         <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_cmv_30bpDown -o plots/histogram_3d/</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -22054,7 +22219,7 @@
         <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_sense_30bpDown -o plots/histogram_3d/</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -22107,7 +22272,7 @@
         <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_branch_30bpDown -o plots/histogram_3d/</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -22160,7 +22325,7 @@
         <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_cmv_30bpDown -o plots/histogram_3d/</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -22213,7 +22378,7 @@
         <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_sense_30bpDown -o plots/histogram_3d/</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -22266,7 +22431,7 @@
         <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_branch_30bpDown -o plots/histogram_3d/</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -22319,7 +22484,7 @@
         <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_cmv_30bpDown -o plots/histogram_3d/</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>116</v>
       </c>
@@ -22357,13 +22522,10 @@
         <v>109</v>
       </c>
       <c r="M43" t="s">
-        <v>111</v>
-      </c>
-      <c r="N43" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1</v>
       </c>
@@ -22415,12 +22577,8 @@
         <f>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/",Table1014[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
         <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_sense_nodsb -o plots/histogram_3d/</v>
       </c>
-      <c r="N44" t="str">
-        <f>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", Table1014[[#This Row],[subst_type]], " -dir ", globals!$A$4, "/", Table1014[[#This Row],[dir]])</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type with -dir libraries_4/WT_sgA_R1_sense_nodsb</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2</v>
       </c>
@@ -22472,12 +22630,8 @@
         <f>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/",Table1014[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
         <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_branch_nodsb -o plots/histogram_3d/</v>
       </c>
-      <c r="N45" t="str">
-        <f>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", Table1014[[#This Row],[subst_type]], " -dir ", globals!$A$4, "/", Table1014[[#This Row],[dir]])</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type with -dir libraries_4/WT_sgA_R1_branch_nodsb</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>3</v>
       </c>
@@ -22529,12 +22683,8 @@
         <f>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/",Table1014[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
         <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_cmv_nodsb -o plots/histogram_3d/</v>
       </c>
-      <c r="N46" t="str">
-        <f>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", Table1014[[#This Row],[subst_type]], " -dir ", globals!$A$4, "/", Table1014[[#This Row],[dir]])</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type with -dir libraries_4/WT_sgA_R1_cmv_nodsb</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>4</v>
       </c>
@@ -22586,12 +22736,8 @@
         <f>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/",Table1014[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
         <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_sense_nodsb -o plots/histogram_3d/</v>
       </c>
-      <c r="N47" t="str">
-        <f>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", Table1014[[#This Row],[subst_type]], " -dir ", globals!$A$4, "/", Table1014[[#This Row],[dir]])</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type with -dir libraries_4/KO_sgA_R1_sense_nodsb</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>5</v>
       </c>
@@ -22643,12 +22789,8 @@
         <f>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/",Table1014[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
         <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_branch_nodsb -o plots/histogram_3d/</v>
       </c>
-      <c r="N48" t="str">
-        <f>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", Table1014[[#This Row],[subst_type]], " -dir ", globals!$A$4, "/", Table1014[[#This Row],[dir]])</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type with -dir libraries_4/KO_sgA_R1_branch_nodsb</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>6</v>
       </c>
@@ -22700,12 +22842,8 @@
         <f>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/",Table1014[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
         <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_cmv_nodsb -o plots/histogram_3d/</v>
       </c>
-      <c r="N49" t="str">
-        <f>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", Table1014[[#This Row],[subst_type]], " -dir ", globals!$A$4, "/", Table1014[[#This Row],[dir]])</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type with -dir libraries_4/KO_sgA_R1_cmv_nodsb</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>7</v>
       </c>
@@ -22757,12 +22895,8 @@
         <f>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/",Table1014[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
         <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_sense_nodsb -o plots/histogram_3d/</v>
       </c>
-      <c r="N50" t="str">
-        <f>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", Table1014[[#This Row],[subst_type]], " -dir ", globals!$A$4, "/", Table1014[[#This Row],[dir]])</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type with -dir libraries_4/WT_sgB_R2_sense_nodsb</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>8</v>
       </c>
@@ -22814,12 +22948,8 @@
         <f>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/",Table1014[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
         <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_branch_nodsb -o plots/histogram_3d/</v>
       </c>
-      <c r="N51" t="str">
-        <f>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", Table1014[[#This Row],[subst_type]], " -dir ", globals!$A$4, "/", Table1014[[#This Row],[dir]])</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type with -dir libraries_4/WT_sgB_R2_branch_nodsb</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>9</v>
       </c>
@@ -22871,12 +23001,8 @@
         <f>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/",Table1014[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
         <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_cmv_nodsb -o plots/histogram_3d/</v>
       </c>
-      <c r="N52" t="str">
-        <f>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", Table1014[[#This Row],[subst_type]], " -dir ", globals!$A$4, "/", Table1014[[#This Row],[dir]])</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type with -dir libraries_4/WT_sgB_R2_cmv_nodsb</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>10</v>
       </c>
@@ -22928,12 +23054,8 @@
         <f>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/",Table1014[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
         <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_sense_nodsb -o plots/histogram_3d/</v>
       </c>
-      <c r="N53" t="str">
-        <f>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", Table1014[[#This Row],[subst_type]], " -dir ", globals!$A$4, "/", Table1014[[#This Row],[dir]])</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type with -dir libraries_4/KO_sgB_R2_sense_nodsb</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>11</v>
       </c>
@@ -22985,12 +23107,8 @@
         <f>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/",Table1014[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
         <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_branch_nodsb -o plots/histogram_3d/</v>
       </c>
-      <c r="N54" t="str">
-        <f>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", Table1014[[#This Row],[subst_type]], " -dir ", globals!$A$4, "/", Table1014[[#This Row],[dir]])</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type with -dir libraries_4/KO_sgB_R2_branch_nodsb</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>12</v>
       </c>
@@ -23042,9 +23160,2875 @@
         <f>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/",Table1014[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
         <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_cmv_nodsb -o plots/histogram_3d/</v>
       </c>
-      <c r="N55" t="str">
-        <f>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", Table1014[[#This Row],[subst_type]], " -dir ", globals!$A$4, "/", Table1014[[#This Row],[dir]])</f>
-        <v>python 2_graph_processing/make_graph_data.py --subst_type with -dir libraries_4/KO_sgB_R2_cmv_nodsb</v>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1375107-D76A-4386-B771-6693BBF75061}">
+  <dimension ref="A1:M55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M45" sqref="M45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="31.28515625" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="8" max="9" width="9.28515625" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="51" customWidth="1"/>
+    <col min="14" max="14" width="22.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <f ca="1">'2_combined'!J3</f>
+        <v>WT_sgAB_R1_sense</v>
+      </c>
+      <c r="C2" t="str">
+        <f ca="1">'2_combined'!C3</f>
+        <v>none</v>
+      </c>
+      <c r="D2" t="str">
+        <f ca="1">'2_combined'!B3</f>
+        <v>2DSB_R1_sense.fa</v>
+      </c>
+      <c r="E2">
+        <f ca="1">'2_combined'!E3</f>
+        <v>67</v>
+      </c>
+      <c r="F2" t="str">
+        <f ca="1">'2_combined'!D3</f>
+        <v>2DSB</v>
+      </c>
+      <c r="G2" t="str" cm="1">
+        <f t="array" aca="1" ref="G2" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>2</v>
+      </c>
+      <c r="H2" t="str">
+        <f ca="1">'2_combined'!G3</f>
+        <v>R1</v>
+      </c>
+      <c r="I2" t="str">
+        <f ca="1">MID('2_combined'!I3, 3, 100)</f>
+        <v>AB</v>
+      </c>
+      <c r="J2" t="str">
+        <f ca="1">'2_combined'!F3</f>
+        <v>WT</v>
+      </c>
+      <c r="K2" t="str">
+        <f ca="1">'2_combined'!H3</f>
+        <v>sense</v>
+      </c>
+      <c r="L2" t="str">
+        <f t="shared" ref="L2:L41" si="0">"with"</f>
+        <v>with</v>
+      </c>
+      <c r="M2" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <f ca="1">'2_combined'!J4</f>
+        <v>WT_sgAB_R1_branch</v>
+      </c>
+      <c r="C3" t="str">
+        <f ca="1">'2_combined'!C4</f>
+        <v>none</v>
+      </c>
+      <c r="D3" t="str">
+        <f ca="1">'2_combined'!B4</f>
+        <v>2DSB_R1_branch.fa</v>
+      </c>
+      <c r="E3">
+        <f ca="1">'2_combined'!E4</f>
+        <v>67</v>
+      </c>
+      <c r="F3" t="str">
+        <f ca="1">'2_combined'!D4</f>
+        <v>2DSB</v>
+      </c>
+      <c r="G3" t="str" cm="1">
+        <f t="array" aca="1" ref="G3" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>2</v>
+      </c>
+      <c r="H3" t="str">
+        <f ca="1">'2_combined'!G4</f>
+        <v>R1</v>
+      </c>
+      <c r="I3" t="str">
+        <f ca="1">MID('2_combined'!I4, 3, 100)</f>
+        <v>AB</v>
+      </c>
+      <c r="J3" t="str">
+        <f ca="1">'2_combined'!F4</f>
+        <v>WT</v>
+      </c>
+      <c r="K3" t="str">
+        <f ca="1">'2_combined'!H4</f>
+        <v>branch</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M3" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_branch -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <f ca="1">'2_combined'!J5</f>
+        <v>WT_sgAB_R1_cmv</v>
+      </c>
+      <c r="C4" t="str">
+        <f ca="1">'2_combined'!C5</f>
+        <v>none</v>
+      </c>
+      <c r="D4" t="str">
+        <f ca="1">'2_combined'!B5</f>
+        <v>2DSB_R1_cmv.fa</v>
+      </c>
+      <c r="E4">
+        <f ca="1">'2_combined'!E5</f>
+        <v>67</v>
+      </c>
+      <c r="F4" t="str">
+        <f ca="1">'2_combined'!D5</f>
+        <v>2DSB</v>
+      </c>
+      <c r="G4" t="str" cm="1">
+        <f t="array" aca="1" ref="G4" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>2</v>
+      </c>
+      <c r="H4" t="str">
+        <f ca="1">'2_combined'!G5</f>
+        <v>R1</v>
+      </c>
+      <c r="I4" t="str">
+        <f ca="1">MID('2_combined'!I5, 3, 100)</f>
+        <v>AB</v>
+      </c>
+      <c r="J4" t="str">
+        <f ca="1">'2_combined'!F5</f>
+        <v>WT</v>
+      </c>
+      <c r="K4" t="str">
+        <f ca="1">'2_combined'!H5</f>
+        <v>cmv</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M4" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_cmv -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <f ca="1">'2_combined'!J6</f>
+        <v>KO_sgAB_R1_sense</v>
+      </c>
+      <c r="C5" t="str">
+        <f ca="1">'2_combined'!C6</f>
+        <v>none</v>
+      </c>
+      <c r="D5" t="str">
+        <f ca="1">'2_combined'!B6</f>
+        <v>2DSB_R1_sense.fa</v>
+      </c>
+      <c r="E5">
+        <f ca="1">'2_combined'!E6</f>
+        <v>67</v>
+      </c>
+      <c r="F5" t="str">
+        <f ca="1">'2_combined'!D6</f>
+        <v>2DSB</v>
+      </c>
+      <c r="G5" t="str" cm="1">
+        <f t="array" aca="1" ref="G5" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>2</v>
+      </c>
+      <c r="H5" t="str">
+        <f ca="1">'2_combined'!G6</f>
+        <v>R1</v>
+      </c>
+      <c r="I5" t="str">
+        <f ca="1">MID('2_combined'!I6, 3, 100)</f>
+        <v>AB</v>
+      </c>
+      <c r="J5" t="str">
+        <f ca="1">'2_combined'!F6</f>
+        <v>KO</v>
+      </c>
+      <c r="K5" t="str">
+        <f ca="1">'2_combined'!H6</f>
+        <v>sense</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M5" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <f ca="1">'2_combined'!J7</f>
+        <v>KO_sgAB_R1_branch</v>
+      </c>
+      <c r="C6" t="str">
+        <f ca="1">'2_combined'!C7</f>
+        <v>none</v>
+      </c>
+      <c r="D6" t="str">
+        <f ca="1">'2_combined'!B7</f>
+        <v>2DSB_R1_branch.fa</v>
+      </c>
+      <c r="E6">
+        <f ca="1">'2_combined'!E7</f>
+        <v>67</v>
+      </c>
+      <c r="F6" t="str">
+        <f ca="1">'2_combined'!D7</f>
+        <v>2DSB</v>
+      </c>
+      <c r="G6" t="str" cm="1">
+        <f t="array" aca="1" ref="G6" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>2</v>
+      </c>
+      <c r="H6" t="str">
+        <f ca="1">'2_combined'!G7</f>
+        <v>R1</v>
+      </c>
+      <c r="I6" t="str">
+        <f ca="1">MID('2_combined'!I7, 3, 100)</f>
+        <v>AB</v>
+      </c>
+      <c r="J6" t="str">
+        <f ca="1">'2_combined'!F7</f>
+        <v>KO</v>
+      </c>
+      <c r="K6" t="str">
+        <f ca="1">'2_combined'!H7</f>
+        <v>branch</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M6" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_branch -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <f ca="1">'2_combined'!J8</f>
+        <v>KO_sgAB_R1_cmv</v>
+      </c>
+      <c r="C7" t="str">
+        <f ca="1">'2_combined'!C8</f>
+        <v>none</v>
+      </c>
+      <c r="D7" t="str">
+        <f ca="1">'2_combined'!B8</f>
+        <v>2DSB_R1_cmv.fa</v>
+      </c>
+      <c r="E7">
+        <f ca="1">'2_combined'!E8</f>
+        <v>67</v>
+      </c>
+      <c r="F7" t="str">
+        <f ca="1">'2_combined'!D8</f>
+        <v>2DSB</v>
+      </c>
+      <c r="G7" t="str" cm="1">
+        <f t="array" aca="1" ref="G7" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>2</v>
+      </c>
+      <c r="H7" t="str">
+        <f ca="1">'2_combined'!G8</f>
+        <v>R1</v>
+      </c>
+      <c r="I7" t="str">
+        <f ca="1">MID('2_combined'!I8, 3, 100)</f>
+        <v>AB</v>
+      </c>
+      <c r="J7" t="str">
+        <f ca="1">'2_combined'!F8</f>
+        <v>KO</v>
+      </c>
+      <c r="K7" t="str">
+        <f ca="1">'2_combined'!H8</f>
+        <v>cmv</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M7" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_cmv -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" t="str">
+        <f ca="1">'2_combined'!J9</f>
+        <v>WT_sgAB_R2_sense</v>
+      </c>
+      <c r="C8" t="str">
+        <f ca="1">'2_combined'!C9</f>
+        <v>none</v>
+      </c>
+      <c r="D8" t="str">
+        <f ca="1">'2_combined'!B9</f>
+        <v>2DSB_R2_sense.fa</v>
+      </c>
+      <c r="E8">
+        <f ca="1">'2_combined'!E9</f>
+        <v>46</v>
+      </c>
+      <c r="F8" t="str">
+        <f ca="1">'2_combined'!D9</f>
+        <v>2DSB</v>
+      </c>
+      <c r="G8" t="str" cm="1">
+        <f t="array" aca="1" ref="G8" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>2</v>
+      </c>
+      <c r="H8" t="str">
+        <f ca="1">'2_combined'!G9</f>
+        <v>R2</v>
+      </c>
+      <c r="I8" t="str">
+        <f ca="1">MID('2_combined'!I9, 3, 100)</f>
+        <v>AB</v>
+      </c>
+      <c r="J8" t="str">
+        <f ca="1">'2_combined'!F9</f>
+        <v>WT</v>
+      </c>
+      <c r="K8" t="str">
+        <f ca="1">'2_combined'!H9</f>
+        <v>sense</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M8" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" t="str">
+        <f ca="1">'2_combined'!J10</f>
+        <v>WT_sgAB_R2_branch</v>
+      </c>
+      <c r="C9" t="str">
+        <f ca="1">'2_combined'!C10</f>
+        <v>none</v>
+      </c>
+      <c r="D9" t="str">
+        <f ca="1">'2_combined'!B10</f>
+        <v>2DSB_R2_branch.fa</v>
+      </c>
+      <c r="E9">
+        <f ca="1">'2_combined'!E10</f>
+        <v>46</v>
+      </c>
+      <c r="F9" t="str">
+        <f ca="1">'2_combined'!D10</f>
+        <v>2DSB</v>
+      </c>
+      <c r="G9" t="str" cm="1">
+        <f t="array" aca="1" ref="G9" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>2</v>
+      </c>
+      <c r="H9" t="str">
+        <f ca="1">'2_combined'!G10</f>
+        <v>R2</v>
+      </c>
+      <c r="I9" t="str">
+        <f ca="1">MID('2_combined'!I10, 3, 100)</f>
+        <v>AB</v>
+      </c>
+      <c r="J9" t="str">
+        <f ca="1">'2_combined'!F10</f>
+        <v>WT</v>
+      </c>
+      <c r="K9" t="str">
+        <f ca="1">'2_combined'!H10</f>
+        <v>branch</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M9" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_branch -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" t="str">
+        <f ca="1">'2_combined'!J11</f>
+        <v>WT_sgAB_R2_cmv</v>
+      </c>
+      <c r="C10" t="str">
+        <f ca="1">'2_combined'!C11</f>
+        <v>none</v>
+      </c>
+      <c r="D10" t="str">
+        <f ca="1">'2_combined'!B11</f>
+        <v>2DSB_R2_cmv.fa</v>
+      </c>
+      <c r="E10">
+        <f ca="1">'2_combined'!E11</f>
+        <v>46</v>
+      </c>
+      <c r="F10" t="str">
+        <f ca="1">'2_combined'!D11</f>
+        <v>2DSB</v>
+      </c>
+      <c r="G10" t="str" cm="1">
+        <f t="array" aca="1" ref="G10" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>2</v>
+      </c>
+      <c r="H10" t="str">
+        <f ca="1">'2_combined'!G11</f>
+        <v>R2</v>
+      </c>
+      <c r="I10" t="str">
+        <f ca="1">MID('2_combined'!I11, 3, 100)</f>
+        <v>AB</v>
+      </c>
+      <c r="J10" t="str">
+        <f ca="1">'2_combined'!F11</f>
+        <v>WT</v>
+      </c>
+      <c r="K10" t="str">
+        <f ca="1">'2_combined'!H11</f>
+        <v>cmv</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M10" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_cmv -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" t="str">
+        <f ca="1">'2_combined'!J12</f>
+        <v>KO_sgAB_R2_sense</v>
+      </c>
+      <c r="C11" t="str">
+        <f ca="1">'2_combined'!C12</f>
+        <v>none</v>
+      </c>
+      <c r="D11" t="str">
+        <f ca="1">'2_combined'!B12</f>
+        <v>2DSB_R2_sense.fa</v>
+      </c>
+      <c r="E11">
+        <f ca="1">'2_combined'!E12</f>
+        <v>46</v>
+      </c>
+      <c r="F11" t="str">
+        <f ca="1">'2_combined'!D12</f>
+        <v>2DSB</v>
+      </c>
+      <c r="G11" t="str" cm="1">
+        <f t="array" aca="1" ref="G11" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>2</v>
+      </c>
+      <c r="H11" t="str">
+        <f ca="1">'2_combined'!G12</f>
+        <v>R2</v>
+      </c>
+      <c r="I11" t="str">
+        <f ca="1">MID('2_combined'!I12, 3, 100)</f>
+        <v>AB</v>
+      </c>
+      <c r="J11" t="str">
+        <f ca="1">'2_combined'!F12</f>
+        <v>KO</v>
+      </c>
+      <c r="K11" t="str">
+        <f ca="1">'2_combined'!H12</f>
+        <v>sense</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M11" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" t="str">
+        <f ca="1">'2_combined'!J13</f>
+        <v>KO_sgAB_R2_branch</v>
+      </c>
+      <c r="C12" t="str">
+        <f ca="1">'2_combined'!C13</f>
+        <v>none</v>
+      </c>
+      <c r="D12" t="str">
+        <f ca="1">'2_combined'!B13</f>
+        <v>2DSB_R2_branch.fa</v>
+      </c>
+      <c r="E12">
+        <f ca="1">'2_combined'!E13</f>
+        <v>46</v>
+      </c>
+      <c r="F12" t="str">
+        <f ca="1">'2_combined'!D13</f>
+        <v>2DSB</v>
+      </c>
+      <c r="G12" t="str" cm="1">
+        <f t="array" aca="1" ref="G12" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>2</v>
+      </c>
+      <c r="H12" t="str">
+        <f ca="1">'2_combined'!G13</f>
+        <v>R2</v>
+      </c>
+      <c r="I12" t="str">
+        <f ca="1">MID('2_combined'!I13, 3, 100)</f>
+        <v>AB</v>
+      </c>
+      <c r="J12" t="str">
+        <f ca="1">'2_combined'!F13</f>
+        <v>KO</v>
+      </c>
+      <c r="K12" t="str">
+        <f ca="1">'2_combined'!H13</f>
+        <v>branch</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M12" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_branch -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" t="str">
+        <f ca="1">'2_combined'!J14</f>
+        <v>KO_sgAB_R2_cmv</v>
+      </c>
+      <c r="C13" t="str">
+        <f ca="1">'2_combined'!C14</f>
+        <v>none</v>
+      </c>
+      <c r="D13" t="str">
+        <f ca="1">'2_combined'!B14</f>
+        <v>2DSB_R2_cmv.fa</v>
+      </c>
+      <c r="E13">
+        <f ca="1">'2_combined'!E14</f>
+        <v>46</v>
+      </c>
+      <c r="F13" t="str">
+        <f ca="1">'2_combined'!D14</f>
+        <v>2DSB</v>
+      </c>
+      <c r="G13" t="str" cm="1">
+        <f t="array" aca="1" ref="G13" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>2</v>
+      </c>
+      <c r="H13" t="str">
+        <f ca="1">'2_combined'!G14</f>
+        <v>R2</v>
+      </c>
+      <c r="I13" t="str">
+        <f ca="1">MID('2_combined'!I14, 3, 100)</f>
+        <v>AB</v>
+      </c>
+      <c r="J13" t="str">
+        <f ca="1">'2_combined'!F14</f>
+        <v>KO</v>
+      </c>
+      <c r="K13" t="str">
+        <f ca="1">'2_combined'!H14</f>
+        <v>cmv</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M13" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_cmv -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" t="str">
+        <f ca="1">'2_combined'!J15</f>
+        <v>WT_sgA_R1_sense</v>
+      </c>
+      <c r="C14" t="str">
+        <f ca="1">'2_combined'!C15</f>
+        <v>none</v>
+      </c>
+      <c r="D14" t="str">
+        <f ca="1">'2_combined'!B15</f>
+        <v>1DSB_R1_sense.fa</v>
+      </c>
+      <c r="E14">
+        <f ca="1">'2_combined'!E15</f>
+        <v>67</v>
+      </c>
+      <c r="F14" t="str">
+        <f ca="1">'2_combined'!D15</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G14" t="str" cm="1">
+        <f t="array" aca="1" ref="G14" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H14" t="str">
+        <f ca="1">'2_combined'!G15</f>
+        <v>R1</v>
+      </c>
+      <c r="I14" t="str">
+        <f ca="1">MID('2_combined'!I15, 3, 100)</f>
+        <v>A</v>
+      </c>
+      <c r="J14" t="str">
+        <f ca="1">'2_combined'!F15</f>
+        <v>WT</v>
+      </c>
+      <c r="K14" t="str">
+        <f ca="1">'2_combined'!H15</f>
+        <v>sense</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M14" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" t="str">
+        <f ca="1">'2_combined'!J16</f>
+        <v>WT_sgA_R1_branch</v>
+      </c>
+      <c r="C15" t="str">
+        <f ca="1">'2_combined'!C16</f>
+        <v>none</v>
+      </c>
+      <c r="D15" t="str">
+        <f ca="1">'2_combined'!B16</f>
+        <v>1DSB_R1_branch.fa</v>
+      </c>
+      <c r="E15">
+        <f ca="1">'2_combined'!E16</f>
+        <v>67</v>
+      </c>
+      <c r="F15" t="str">
+        <f ca="1">'2_combined'!D16</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G15" t="str" cm="1">
+        <f t="array" aca="1" ref="G15" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H15" t="str">
+        <f ca="1">'2_combined'!G16</f>
+        <v>R1</v>
+      </c>
+      <c r="I15" t="str">
+        <f ca="1">MID('2_combined'!I16, 3, 100)</f>
+        <v>A</v>
+      </c>
+      <c r="J15" t="str">
+        <f ca="1">'2_combined'!F16</f>
+        <v>WT</v>
+      </c>
+      <c r="K15" t="str">
+        <f ca="1">'2_combined'!H16</f>
+        <v>branch</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M15" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" t="str">
+        <f ca="1">'2_combined'!J17</f>
+        <v>WT_sgA_R1_cmv</v>
+      </c>
+      <c r="C16" t="str">
+        <f ca="1">'2_combined'!C17</f>
+        <v>none</v>
+      </c>
+      <c r="D16" t="str">
+        <f ca="1">'2_combined'!B17</f>
+        <v>1DSB_R1_cmv.fa</v>
+      </c>
+      <c r="E16">
+        <f ca="1">'2_combined'!E17</f>
+        <v>67</v>
+      </c>
+      <c r="F16" t="str">
+        <f ca="1">'2_combined'!D17</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G16" t="str" cm="1">
+        <f t="array" aca="1" ref="G16" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H16" t="str">
+        <f ca="1">'2_combined'!G17</f>
+        <v>R1</v>
+      </c>
+      <c r="I16" t="str">
+        <f ca="1">MID('2_combined'!I17, 3, 100)</f>
+        <v>A</v>
+      </c>
+      <c r="J16" t="str">
+        <f ca="1">'2_combined'!F17</f>
+        <v>WT</v>
+      </c>
+      <c r="K16" t="str">
+        <f ca="1">'2_combined'!H17</f>
+        <v>cmv</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M16" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17" t="str">
+        <f ca="1">'2_combined'!J18</f>
+        <v>WT_sgB_R2_sense</v>
+      </c>
+      <c r="C17" t="str">
+        <f ca="1">'2_combined'!C18</f>
+        <v>none</v>
+      </c>
+      <c r="D17" t="str">
+        <f ca="1">'2_combined'!B18</f>
+        <v>1DSB_R2_sense.fa</v>
+      </c>
+      <c r="E17">
+        <f ca="1">'2_combined'!E18</f>
+        <v>46</v>
+      </c>
+      <c r="F17" t="str">
+        <f ca="1">'2_combined'!D18</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G17" t="str" cm="1">
+        <f t="array" aca="1" ref="G17" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H17" t="str">
+        <f ca="1">'2_combined'!G18</f>
+        <v>R2</v>
+      </c>
+      <c r="I17" t="str">
+        <f ca="1">MID('2_combined'!I18, 3, 100)</f>
+        <v>B</v>
+      </c>
+      <c r="J17" t="str">
+        <f ca="1">'2_combined'!F18</f>
+        <v>WT</v>
+      </c>
+      <c r="K17" t="str">
+        <f ca="1">'2_combined'!H18</f>
+        <v>sense</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M17" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
+      <c r="B18" t="str">
+        <f ca="1">'2_combined'!J19</f>
+        <v>WT_sgB_R2_branch</v>
+      </c>
+      <c r="C18" t="str">
+        <f ca="1">'2_combined'!C19</f>
+        <v>none</v>
+      </c>
+      <c r="D18" t="str">
+        <f ca="1">'2_combined'!B19</f>
+        <v>1DSB_R2_branch.fa</v>
+      </c>
+      <c r="E18">
+        <f ca="1">'2_combined'!E19</f>
+        <v>46</v>
+      </c>
+      <c r="F18" t="str">
+        <f ca="1">'2_combined'!D19</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G18" t="str" cm="1">
+        <f t="array" aca="1" ref="G18" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H18" t="str">
+        <f ca="1">'2_combined'!G19</f>
+        <v>R2</v>
+      </c>
+      <c r="I18" t="str">
+        <f ca="1">MID('2_combined'!I19, 3, 100)</f>
+        <v>B</v>
+      </c>
+      <c r="J18" t="str">
+        <f ca="1">'2_combined'!F19</f>
+        <v>WT</v>
+      </c>
+      <c r="K18" t="str">
+        <f ca="1">'2_combined'!H19</f>
+        <v>branch</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M18" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>18</v>
+      </c>
+      <c r="B19" t="str">
+        <f ca="1">'2_combined'!J20</f>
+        <v>WT_sgB_R2_cmv</v>
+      </c>
+      <c r="C19" t="str">
+        <f ca="1">'2_combined'!C20</f>
+        <v>none</v>
+      </c>
+      <c r="D19" t="str">
+        <f ca="1">'2_combined'!B20</f>
+        <v>1DSB_R2_cmv.fa</v>
+      </c>
+      <c r="E19">
+        <f ca="1">'2_combined'!E20</f>
+        <v>46</v>
+      </c>
+      <c r="F19" t="str">
+        <f ca="1">'2_combined'!D20</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G19" t="str" cm="1">
+        <f t="array" aca="1" ref="G19" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H19" t="str">
+        <f ca="1">'2_combined'!G20</f>
+        <v>R2</v>
+      </c>
+      <c r="I19" t="str">
+        <f ca="1">MID('2_combined'!I20, 3, 100)</f>
+        <v>B</v>
+      </c>
+      <c r="J19" t="str">
+        <f ca="1">'2_combined'!F20</f>
+        <v>WT</v>
+      </c>
+      <c r="K19" t="str">
+        <f ca="1">'2_combined'!H20</f>
+        <v>cmv</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M19" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
+      <c r="B20" t="str">
+        <f ca="1">'2_combined'!J21</f>
+        <v>KO_sgA_R1_sense</v>
+      </c>
+      <c r="C20" t="str">
+        <f ca="1">'2_combined'!C21</f>
+        <v>none</v>
+      </c>
+      <c r="D20" t="str">
+        <f ca="1">'2_combined'!B21</f>
+        <v>1DSB_R1_sense.fa</v>
+      </c>
+      <c r="E20">
+        <f ca="1">'2_combined'!E21</f>
+        <v>67</v>
+      </c>
+      <c r="F20" t="str">
+        <f ca="1">'2_combined'!D21</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G20" t="str" cm="1">
+        <f t="array" aca="1" ref="G20" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H20" t="str">
+        <f ca="1">'2_combined'!G21</f>
+        <v>R1</v>
+      </c>
+      <c r="I20" t="str">
+        <f ca="1">MID('2_combined'!I21, 3, 100)</f>
+        <v>A</v>
+      </c>
+      <c r="J20" t="str">
+        <f ca="1">'2_combined'!F21</f>
+        <v>KO</v>
+      </c>
+      <c r="K20" t="str">
+        <f ca="1">'2_combined'!H21</f>
+        <v>sense</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M20" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
+      <c r="B21" t="str">
+        <f ca="1">'2_combined'!J22</f>
+        <v>KO_sgA_R1_branch</v>
+      </c>
+      <c r="C21" t="str">
+        <f ca="1">'2_combined'!C22</f>
+        <v>none</v>
+      </c>
+      <c r="D21" t="str">
+        <f ca="1">'2_combined'!B22</f>
+        <v>1DSB_R1_branch.fa</v>
+      </c>
+      <c r="E21">
+        <f ca="1">'2_combined'!E22</f>
+        <v>67</v>
+      </c>
+      <c r="F21" t="str">
+        <f ca="1">'2_combined'!D22</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G21" t="str" cm="1">
+        <f t="array" aca="1" ref="G21" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H21" t="str">
+        <f ca="1">'2_combined'!G22</f>
+        <v>R1</v>
+      </c>
+      <c r="I21" t="str">
+        <f ca="1">MID('2_combined'!I22, 3, 100)</f>
+        <v>A</v>
+      </c>
+      <c r="J21" t="str">
+        <f ca="1">'2_combined'!F22</f>
+        <v>KO</v>
+      </c>
+      <c r="K21" t="str">
+        <f ca="1">'2_combined'!H22</f>
+        <v>branch</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M21" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>21</v>
+      </c>
+      <c r="B22" t="str">
+        <f ca="1">'2_combined'!J23</f>
+        <v>KO_sgA_R1_cmv</v>
+      </c>
+      <c r="C22" t="str">
+        <f ca="1">'2_combined'!C23</f>
+        <v>none</v>
+      </c>
+      <c r="D22" t="str">
+        <f ca="1">'2_combined'!B23</f>
+        <v>1DSB_R1_cmv.fa</v>
+      </c>
+      <c r="E22">
+        <f ca="1">'2_combined'!E23</f>
+        <v>67</v>
+      </c>
+      <c r="F22" t="str">
+        <f ca="1">'2_combined'!D23</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G22" t="str" cm="1">
+        <f t="array" aca="1" ref="G22" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H22" t="str">
+        <f ca="1">'2_combined'!G23</f>
+        <v>R1</v>
+      </c>
+      <c r="I22" t="str">
+        <f ca="1">MID('2_combined'!I23, 3, 100)</f>
+        <v>A</v>
+      </c>
+      <c r="J22" t="str">
+        <f ca="1">'2_combined'!F23</f>
+        <v>KO</v>
+      </c>
+      <c r="K22" t="str">
+        <f ca="1">'2_combined'!H23</f>
+        <v>cmv</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M22" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>22</v>
+      </c>
+      <c r="B23" t="str">
+        <f ca="1">'2_combined'!J24</f>
+        <v>KO_sgB_R2_sense</v>
+      </c>
+      <c r="C23" t="str">
+        <f ca="1">'2_combined'!C24</f>
+        <v>none</v>
+      </c>
+      <c r="D23" t="str">
+        <f ca="1">'2_combined'!B24</f>
+        <v>1DSB_R2_sense.fa</v>
+      </c>
+      <c r="E23">
+        <f ca="1">'2_combined'!E24</f>
+        <v>46</v>
+      </c>
+      <c r="F23" t="str">
+        <f ca="1">'2_combined'!D24</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G23" t="str" cm="1">
+        <f t="array" aca="1" ref="G23" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H23" t="str">
+        <f ca="1">'2_combined'!G24</f>
+        <v>R2</v>
+      </c>
+      <c r="I23" t="str">
+        <f ca="1">MID('2_combined'!I24, 3, 100)</f>
+        <v>B</v>
+      </c>
+      <c r="J23" t="str">
+        <f ca="1">'2_combined'!F24</f>
+        <v>KO</v>
+      </c>
+      <c r="K23" t="str">
+        <f ca="1">'2_combined'!H24</f>
+        <v>sense</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M23" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>23</v>
+      </c>
+      <c r="B24" t="str">
+        <f ca="1">'2_combined'!J25</f>
+        <v>KO_sgB_R2_branch</v>
+      </c>
+      <c r="C24" t="str">
+        <f ca="1">'2_combined'!C25</f>
+        <v>none</v>
+      </c>
+      <c r="D24" t="str">
+        <f ca="1">'2_combined'!B25</f>
+        <v>1DSB_R2_branch.fa</v>
+      </c>
+      <c r="E24">
+        <f ca="1">'2_combined'!E25</f>
+        <v>46</v>
+      </c>
+      <c r="F24" t="str">
+        <f ca="1">'2_combined'!D25</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G24" t="str" cm="1">
+        <f t="array" aca="1" ref="G24" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H24" t="str">
+        <f ca="1">'2_combined'!G25</f>
+        <v>R2</v>
+      </c>
+      <c r="I24" t="str">
+        <f ca="1">MID('2_combined'!I25, 3, 100)</f>
+        <v>B</v>
+      </c>
+      <c r="J24" t="str">
+        <f ca="1">'2_combined'!F25</f>
+        <v>KO</v>
+      </c>
+      <c r="K24" t="str">
+        <f ca="1">'2_combined'!H25</f>
+        <v>branch</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M24" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>24</v>
+      </c>
+      <c r="B25" t="str">
+        <f ca="1">'2_combined'!J26</f>
+        <v>KO_sgB_R2_cmv</v>
+      </c>
+      <c r="C25" t="str">
+        <f ca="1">'2_combined'!C26</f>
+        <v>none</v>
+      </c>
+      <c r="D25" t="str">
+        <f ca="1">'2_combined'!B26</f>
+        <v>1DSB_R2_cmv.fa</v>
+      </c>
+      <c r="E25">
+        <f ca="1">'2_combined'!E26</f>
+        <v>46</v>
+      </c>
+      <c r="F25" t="str">
+        <f ca="1">'2_combined'!D26</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G25" t="str" cm="1">
+        <f t="array" aca="1" ref="G25" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H25" t="str">
+        <f ca="1">'2_combined'!G26</f>
+        <v>R2</v>
+      </c>
+      <c r="I25" t="str">
+        <f ca="1">MID('2_combined'!I26, 3, 100)</f>
+        <v>B</v>
+      </c>
+      <c r="J25" t="str">
+        <f ca="1">'2_combined'!F26</f>
+        <v>KO</v>
+      </c>
+      <c r="K25" t="str">
+        <f ca="1">'2_combined'!H26</f>
+        <v>cmv</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M25" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>25</v>
+      </c>
+      <c r="B26" t="str">
+        <f ca="1">'2_combined'!J27</f>
+        <v>WT_sgCD_R1_antisense</v>
+      </c>
+      <c r="C26" t="str">
+        <f ca="1">'2_combined'!C27</f>
+        <v>none</v>
+      </c>
+      <c r="D26" t="str">
+        <f ca="1">'2_combined'!B27</f>
+        <v>2DSBanti_R1_antisense.fa</v>
+      </c>
+      <c r="E26">
+        <f ca="1">'2_combined'!E27</f>
+        <v>50</v>
+      </c>
+      <c r="F26" t="str">
+        <f ca="1">'2_combined'!D27</f>
+        <v>2DSBanti</v>
+      </c>
+      <c r="G26" t="str" cm="1">
+        <f t="array" aca="1" ref="G26" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>2a</v>
+      </c>
+      <c r="H26" t="str">
+        <f ca="1">'2_combined'!G27</f>
+        <v>R1</v>
+      </c>
+      <c r="I26" t="str">
+        <f ca="1">MID('2_combined'!I27, 3, 100)</f>
+        <v>CD</v>
+      </c>
+      <c r="J26" t="str">
+        <f ca="1">'2_combined'!F27</f>
+        <v>WT</v>
+      </c>
+      <c r="K26" t="str">
+        <f ca="1">'2_combined'!H27</f>
+        <v>antisense</v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M26" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>26</v>
+      </c>
+      <c r="B27" t="str">
+        <f ca="1">'2_combined'!J28</f>
+        <v>WT_sgCD_R1_splicing</v>
+      </c>
+      <c r="C27" t="str">
+        <f ca="1">'2_combined'!C28</f>
+        <v>none</v>
+      </c>
+      <c r="D27" t="str">
+        <f ca="1">'2_combined'!B28</f>
+        <v>2DSBanti_R1_splicing.fa</v>
+      </c>
+      <c r="E27">
+        <f ca="1">'2_combined'!E28</f>
+        <v>50</v>
+      </c>
+      <c r="F27" t="str">
+        <f ca="1">'2_combined'!D28</f>
+        <v>2DSBanti</v>
+      </c>
+      <c r="G27" t="str" cm="1">
+        <f t="array" aca="1" ref="G27" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>2a</v>
+      </c>
+      <c r="H27" t="str">
+        <f ca="1">'2_combined'!G28</f>
+        <v>R1</v>
+      </c>
+      <c r="I27" t="str">
+        <f ca="1">MID('2_combined'!I28, 3, 100)</f>
+        <v>CD</v>
+      </c>
+      <c r="J27" t="str">
+        <f ca="1">'2_combined'!F28</f>
+        <v>WT</v>
+      </c>
+      <c r="K27" t="str">
+        <f ca="1">'2_combined'!H28</f>
+        <v>splicing</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M27" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_splicing -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>27</v>
+      </c>
+      <c r="B28" t="str">
+        <f ca="1">'2_combined'!J29</f>
+        <v>WT_sgCD_R2_antisense</v>
+      </c>
+      <c r="C28" t="str">
+        <f ca="1">'2_combined'!C29</f>
+        <v>none</v>
+      </c>
+      <c r="D28" t="str">
+        <f ca="1">'2_combined'!B29</f>
+        <v>2DSBanti_R2_antisense.fa</v>
+      </c>
+      <c r="E28">
+        <f ca="1">'2_combined'!E29</f>
+        <v>47</v>
+      </c>
+      <c r="F28" t="str">
+        <f ca="1">'2_combined'!D29</f>
+        <v>2DSBanti</v>
+      </c>
+      <c r="G28" t="str" cm="1">
+        <f t="array" aca="1" ref="G28" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>2a</v>
+      </c>
+      <c r="H28" t="str">
+        <f ca="1">'2_combined'!G29</f>
+        <v>R2</v>
+      </c>
+      <c r="I28" t="str">
+        <f ca="1">MID('2_combined'!I29, 3, 100)</f>
+        <v>CD</v>
+      </c>
+      <c r="J28" t="str">
+        <f ca="1">'2_combined'!F29</f>
+        <v>WT</v>
+      </c>
+      <c r="K28" t="str">
+        <f ca="1">'2_combined'!H29</f>
+        <v>antisense</v>
+      </c>
+      <c r="L28" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M28" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>28</v>
+      </c>
+      <c r="B29" t="str">
+        <f ca="1">'2_combined'!J30</f>
+        <v>WT_sgCD_R2_splicing</v>
+      </c>
+      <c r="C29" t="str">
+        <f ca="1">'2_combined'!C30</f>
+        <v>none</v>
+      </c>
+      <c r="D29" t="str">
+        <f ca="1">'2_combined'!B30</f>
+        <v>2DSBanti_R2_splicing.fa</v>
+      </c>
+      <c r="E29">
+        <f ca="1">'2_combined'!E30</f>
+        <v>47</v>
+      </c>
+      <c r="F29" t="str">
+        <f ca="1">'2_combined'!D30</f>
+        <v>2DSBanti</v>
+      </c>
+      <c r="G29" t="str" cm="1">
+        <f t="array" aca="1" ref="G29" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>2a</v>
+      </c>
+      <c r="H29" t="str">
+        <f ca="1">'2_combined'!G30</f>
+        <v>R2</v>
+      </c>
+      <c r="I29" t="str">
+        <f ca="1">MID('2_combined'!I30, 3, 100)</f>
+        <v>CD</v>
+      </c>
+      <c r="J29" t="str">
+        <f ca="1">'2_combined'!F30</f>
+        <v>WT</v>
+      </c>
+      <c r="K29" t="str">
+        <f ca="1">'2_combined'!H30</f>
+        <v>splicing</v>
+      </c>
+      <c r="L29" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M29" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_splicing -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>29</v>
+      </c>
+      <c r="B30" t="str">
+        <f ca="1">'2_combined'!J31</f>
+        <v>WT_sgA_R1_sense_30bpDown</v>
+      </c>
+      <c r="C30" t="str">
+        <f ca="1">'2_combined'!C31</f>
+        <v>30bpDown</v>
+      </c>
+      <c r="D30" t="str">
+        <f ca="1">'2_combined'!B31</f>
+        <v>1DSB_R1_sense.fa</v>
+      </c>
+      <c r="E30">
+        <f ca="1">'2_combined'!E31</f>
+        <v>97</v>
+      </c>
+      <c r="F30" t="str">
+        <f ca="1">'2_combined'!D31</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G30" t="str" cm="1">
+        <f t="array" aca="1" ref="G30" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H30" t="str">
+        <f ca="1">'2_combined'!G31</f>
+        <v>R1</v>
+      </c>
+      <c r="I30" t="str">
+        <f ca="1">MID('2_combined'!I31, 3, 100)</f>
+        <v>A</v>
+      </c>
+      <c r="J30" t="str">
+        <f ca="1">'2_combined'!F31</f>
+        <v>WT</v>
+      </c>
+      <c r="K30" t="str">
+        <f ca="1">'2_combined'!H31</f>
+        <v>sense</v>
+      </c>
+      <c r="L30" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M30" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_30bpDown -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>30</v>
+      </c>
+      <c r="B31" t="str">
+        <f ca="1">'2_combined'!J32</f>
+        <v>WT_sgA_R1_branch_30bpDown</v>
+      </c>
+      <c r="C31" t="str">
+        <f ca="1">'2_combined'!C32</f>
+        <v>30bpDown</v>
+      </c>
+      <c r="D31" t="str">
+        <f ca="1">'2_combined'!B32</f>
+        <v>1DSB_R1_branch.fa</v>
+      </c>
+      <c r="E31">
+        <f ca="1">'2_combined'!E32</f>
+        <v>97</v>
+      </c>
+      <c r="F31" t="str">
+        <f ca="1">'2_combined'!D32</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G31" t="str" cm="1">
+        <f t="array" aca="1" ref="G31" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H31" t="str">
+        <f ca="1">'2_combined'!G32</f>
+        <v>R1</v>
+      </c>
+      <c r="I31" t="str">
+        <f ca="1">MID('2_combined'!I32, 3, 100)</f>
+        <v>A</v>
+      </c>
+      <c r="J31" t="str">
+        <f ca="1">'2_combined'!F32</f>
+        <v>WT</v>
+      </c>
+      <c r="K31" t="str">
+        <f ca="1">'2_combined'!H32</f>
+        <v>branch</v>
+      </c>
+      <c r="L31" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M31" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch_30bpDown -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>31</v>
+      </c>
+      <c r="B32" t="str">
+        <f ca="1">'2_combined'!J33</f>
+        <v>WT_sgA_R1_cmv_30bpDown</v>
+      </c>
+      <c r="C32" t="str">
+        <f ca="1">'2_combined'!C33</f>
+        <v>30bpDown</v>
+      </c>
+      <c r="D32" t="str">
+        <f ca="1">'2_combined'!B33</f>
+        <v>1DSB_R1_cmv.fa</v>
+      </c>
+      <c r="E32">
+        <f ca="1">'2_combined'!E33</f>
+        <v>97</v>
+      </c>
+      <c r="F32" t="str">
+        <f ca="1">'2_combined'!D33</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G32" t="str" cm="1">
+        <f t="array" aca="1" ref="G32" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H32" t="str">
+        <f ca="1">'2_combined'!G33</f>
+        <v>R1</v>
+      </c>
+      <c r="I32" t="str">
+        <f ca="1">MID('2_combined'!I33, 3, 100)</f>
+        <v>A</v>
+      </c>
+      <c r="J32" t="str">
+        <f ca="1">'2_combined'!F33</f>
+        <v>WT</v>
+      </c>
+      <c r="K32" t="str">
+        <f ca="1">'2_combined'!H33</f>
+        <v>cmv</v>
+      </c>
+      <c r="L32" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M32" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv_30bpDown -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>32</v>
+      </c>
+      <c r="B33" t="str">
+        <f ca="1">'2_combined'!J34</f>
+        <v>WT_sgB_R2_sense_30bpDown</v>
+      </c>
+      <c r="C33" t="str">
+        <f ca="1">'2_combined'!C34</f>
+        <v>30bpDown</v>
+      </c>
+      <c r="D33" t="str">
+        <f ca="1">'2_combined'!B34</f>
+        <v>1DSB_R2_sense.fa</v>
+      </c>
+      <c r="E33">
+        <f ca="1">'2_combined'!E34</f>
+        <v>76</v>
+      </c>
+      <c r="F33" t="str">
+        <f ca="1">'2_combined'!D34</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G33" t="str" cm="1">
+        <f t="array" aca="1" ref="G33" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H33" t="str">
+        <f ca="1">'2_combined'!G34</f>
+        <v>R2</v>
+      </c>
+      <c r="I33" t="str">
+        <f ca="1">MID('2_combined'!I34, 3, 100)</f>
+        <v>B</v>
+      </c>
+      <c r="J33" t="str">
+        <f ca="1">'2_combined'!F34</f>
+        <v>WT</v>
+      </c>
+      <c r="K33" t="str">
+        <f ca="1">'2_combined'!H34</f>
+        <v>sense</v>
+      </c>
+      <c r="L33" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M33" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_30bpDown -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>33</v>
+      </c>
+      <c r="B34" t="str">
+        <f ca="1">'2_combined'!J35</f>
+        <v>WT_sgB_R2_branch_30bpDown</v>
+      </c>
+      <c r="C34" t="str">
+        <f ca="1">'2_combined'!C35</f>
+        <v>30bpDown</v>
+      </c>
+      <c r="D34" t="str">
+        <f ca="1">'2_combined'!B35</f>
+        <v>1DSB_R2_branch.fa</v>
+      </c>
+      <c r="E34">
+        <f ca="1">'2_combined'!E35</f>
+        <v>76</v>
+      </c>
+      <c r="F34" t="str">
+        <f ca="1">'2_combined'!D35</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G34" t="str" cm="1">
+        <f t="array" aca="1" ref="G34" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H34" t="str">
+        <f ca="1">'2_combined'!G35</f>
+        <v>R2</v>
+      </c>
+      <c r="I34" t="str">
+        <f ca="1">MID('2_combined'!I35, 3, 100)</f>
+        <v>B</v>
+      </c>
+      <c r="J34" t="str">
+        <f ca="1">'2_combined'!F35</f>
+        <v>WT</v>
+      </c>
+      <c r="K34" t="str">
+        <f ca="1">'2_combined'!H35</f>
+        <v>branch</v>
+      </c>
+      <c r="L34" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M34" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch_30bpDown -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>34</v>
+      </c>
+      <c r="B35" t="str">
+        <f ca="1">'2_combined'!J36</f>
+        <v>WT_sgB_R2_cmv_30bpDown</v>
+      </c>
+      <c r="C35" t="str">
+        <f ca="1">'2_combined'!C36</f>
+        <v>30bpDown</v>
+      </c>
+      <c r="D35" t="str">
+        <f ca="1">'2_combined'!B36</f>
+        <v>1DSB_R2_cmv.fa</v>
+      </c>
+      <c r="E35">
+        <f ca="1">'2_combined'!E36</f>
+        <v>76</v>
+      </c>
+      <c r="F35" t="str">
+        <f ca="1">'2_combined'!D36</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G35" t="str" cm="1">
+        <f t="array" aca="1" ref="G35" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H35" t="str">
+        <f ca="1">'2_combined'!G36</f>
+        <v>R2</v>
+      </c>
+      <c r="I35" t="str">
+        <f ca="1">MID('2_combined'!I36, 3, 100)</f>
+        <v>B</v>
+      </c>
+      <c r="J35" t="str">
+        <f ca="1">'2_combined'!F36</f>
+        <v>WT</v>
+      </c>
+      <c r="K35" t="str">
+        <f ca="1">'2_combined'!H36</f>
+        <v>cmv</v>
+      </c>
+      <c r="L35" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M35" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv_30bpDown -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>35</v>
+      </c>
+      <c r="B36" t="str">
+        <f ca="1">'2_combined'!J37</f>
+        <v>KO_sgA_R1_sense_30bpDown</v>
+      </c>
+      <c r="C36" t="str">
+        <f ca="1">'2_combined'!C37</f>
+        <v>30bpDown</v>
+      </c>
+      <c r="D36" t="str">
+        <f ca="1">'2_combined'!B37</f>
+        <v>1DSB_R1_sense.fa</v>
+      </c>
+      <c r="E36">
+        <f ca="1">'2_combined'!E37</f>
+        <v>97</v>
+      </c>
+      <c r="F36" t="str">
+        <f ca="1">'2_combined'!D37</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G36" t="str" cm="1">
+        <f t="array" aca="1" ref="G36" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H36" t="str">
+        <f ca="1">'2_combined'!G37</f>
+        <v>R1</v>
+      </c>
+      <c r="I36" t="str">
+        <f ca="1">MID('2_combined'!I37, 3, 100)</f>
+        <v>A</v>
+      </c>
+      <c r="J36" t="str">
+        <f ca="1">'2_combined'!F37</f>
+        <v>KO</v>
+      </c>
+      <c r="K36" t="str">
+        <f ca="1">'2_combined'!H37</f>
+        <v>sense</v>
+      </c>
+      <c r="L36" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M36" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_30bpDown -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>36</v>
+      </c>
+      <c r="B37" t="str">
+        <f ca="1">'2_combined'!J38</f>
+        <v>KO_sgA_R1_branch_30bpDown</v>
+      </c>
+      <c r="C37" t="str">
+        <f ca="1">'2_combined'!C38</f>
+        <v>30bpDown</v>
+      </c>
+      <c r="D37" t="str">
+        <f ca="1">'2_combined'!B38</f>
+        <v>1DSB_R1_branch.fa</v>
+      </c>
+      <c r="E37">
+        <f ca="1">'2_combined'!E38</f>
+        <v>97</v>
+      </c>
+      <c r="F37" t="str">
+        <f ca="1">'2_combined'!D38</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G37" t="str" cm="1">
+        <f t="array" aca="1" ref="G37" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H37" t="str">
+        <f ca="1">'2_combined'!G38</f>
+        <v>R1</v>
+      </c>
+      <c r="I37" t="str">
+        <f ca="1">MID('2_combined'!I38, 3, 100)</f>
+        <v>A</v>
+      </c>
+      <c r="J37" t="str">
+        <f ca="1">'2_combined'!F38</f>
+        <v>KO</v>
+      </c>
+      <c r="K37" t="str">
+        <f ca="1">'2_combined'!H38</f>
+        <v>branch</v>
+      </c>
+      <c r="L37" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M37" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch_30bpDown -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>37</v>
+      </c>
+      <c r="B38" t="str">
+        <f ca="1">'2_combined'!J39</f>
+        <v>KO_sgA_R1_cmv_30bpDown</v>
+      </c>
+      <c r="C38" t="str">
+        <f ca="1">'2_combined'!C39</f>
+        <v>30bpDown</v>
+      </c>
+      <c r="D38" t="str">
+        <f ca="1">'2_combined'!B39</f>
+        <v>1DSB_R1_cmv.fa</v>
+      </c>
+      <c r="E38">
+        <f ca="1">'2_combined'!E39</f>
+        <v>97</v>
+      </c>
+      <c r="F38" t="str">
+        <f ca="1">'2_combined'!D39</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G38" t="str" cm="1">
+        <f t="array" aca="1" ref="G38" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H38" t="str">
+        <f ca="1">'2_combined'!G39</f>
+        <v>R1</v>
+      </c>
+      <c r="I38" t="str">
+        <f ca="1">MID('2_combined'!I39, 3, 100)</f>
+        <v>A</v>
+      </c>
+      <c r="J38" t="str">
+        <f ca="1">'2_combined'!F39</f>
+        <v>KO</v>
+      </c>
+      <c r="K38" t="str">
+        <f ca="1">'2_combined'!H39</f>
+        <v>cmv</v>
+      </c>
+      <c r="L38" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M38" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv_30bpDown -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>38</v>
+      </c>
+      <c r="B39" t="str">
+        <f ca="1">'2_combined'!J40</f>
+        <v>KO_sgB_R2_sense_30bpDown</v>
+      </c>
+      <c r="C39" t="str">
+        <f ca="1">'2_combined'!C40</f>
+        <v>30bpDown</v>
+      </c>
+      <c r="D39" t="str">
+        <f ca="1">'2_combined'!B40</f>
+        <v>1DSB_R2_sense.fa</v>
+      </c>
+      <c r="E39">
+        <f ca="1">'2_combined'!E40</f>
+        <v>76</v>
+      </c>
+      <c r="F39" t="str">
+        <f ca="1">'2_combined'!D40</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G39" t="str" cm="1">
+        <f t="array" aca="1" ref="G39" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H39" t="str">
+        <f ca="1">'2_combined'!G40</f>
+        <v>R2</v>
+      </c>
+      <c r="I39" t="str">
+        <f ca="1">MID('2_combined'!I40, 3, 100)</f>
+        <v>B</v>
+      </c>
+      <c r="J39" t="str">
+        <f ca="1">'2_combined'!F40</f>
+        <v>KO</v>
+      </c>
+      <c r="K39" t="str">
+        <f ca="1">'2_combined'!H40</f>
+        <v>sense</v>
+      </c>
+      <c r="L39" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M39" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_30bpDown -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>39</v>
+      </c>
+      <c r="B40" t="str">
+        <f ca="1">'2_combined'!J41</f>
+        <v>KO_sgB_R2_branch_30bpDown</v>
+      </c>
+      <c r="C40" t="str">
+        <f ca="1">'2_combined'!C41</f>
+        <v>30bpDown</v>
+      </c>
+      <c r="D40" t="str">
+        <f ca="1">'2_combined'!B41</f>
+        <v>1DSB_R2_branch.fa</v>
+      </c>
+      <c r="E40">
+        <f ca="1">'2_combined'!E41</f>
+        <v>76</v>
+      </c>
+      <c r="F40" t="str">
+        <f ca="1">'2_combined'!D41</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G40" t="str" cm="1">
+        <f t="array" aca="1" ref="G40" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H40" t="str">
+        <f ca="1">'2_combined'!G41</f>
+        <v>R2</v>
+      </c>
+      <c r="I40" t="str">
+        <f ca="1">MID('2_combined'!I41, 3, 100)</f>
+        <v>B</v>
+      </c>
+      <c r="J40" t="str">
+        <f ca="1">'2_combined'!F41</f>
+        <v>KO</v>
+      </c>
+      <c r="K40" t="str">
+        <f ca="1">'2_combined'!H41</f>
+        <v>branch</v>
+      </c>
+      <c r="L40" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M40" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch_30bpDown -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>40</v>
+      </c>
+      <c r="B41" t="str">
+        <f ca="1">'2_combined'!J42</f>
+        <v>KO_sgB_R2_cmv_30bpDown</v>
+      </c>
+      <c r="C41" t="str">
+        <f ca="1">'2_combined'!C42</f>
+        <v>30bpDown</v>
+      </c>
+      <c r="D41" t="str">
+        <f ca="1">'2_combined'!B42</f>
+        <v>1DSB_R2_cmv.fa</v>
+      </c>
+      <c r="E41">
+        <f ca="1">'2_combined'!E42</f>
+        <v>76</v>
+      </c>
+      <c r="F41" t="str">
+        <f ca="1">'2_combined'!D42</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G41" t="str" cm="1">
+        <f t="array" aca="1" ref="G41" ca="1">IF(Table51315[[#This Row],[dsb_type]]="2DSB", "2", IF(Table51315[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table51315[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H41" t="str">
+        <f ca="1">'2_combined'!G42</f>
+        <v>R2</v>
+      </c>
+      <c r="I41" t="str">
+        <f ca="1">MID('2_combined'!I42, 3, 100)</f>
+        <v>B</v>
+      </c>
+      <c r="J41" t="str">
+        <f ca="1">'2_combined'!F42</f>
+        <v>KO</v>
+      </c>
+      <c r="K41" t="str">
+        <f ca="1">'2_combined'!H42</f>
+        <v>cmv</v>
+      </c>
+      <c r="L41" t="str">
+        <f t="shared" si="0"/>
+        <v>with</v>
+      </c>
+      <c r="M41" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table51315[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv_30bpDown -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>116</v>
+      </c>
+      <c r="B43" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" t="s">
+        <v>139</v>
+      </c>
+      <c r="D43" t="s">
+        <v>89</v>
+      </c>
+      <c r="E43" t="s">
+        <v>104</v>
+      </c>
+      <c r="F43" t="s">
+        <v>105</v>
+      </c>
+      <c r="G43" t="s">
+        <v>148</v>
+      </c>
+      <c r="H43" t="s">
+        <v>84</v>
+      </c>
+      <c r="I43" t="s">
+        <v>106</v>
+      </c>
+      <c r="J43" t="s">
+        <v>107</v>
+      </c>
+      <c r="K43" t="s">
+        <v>83</v>
+      </c>
+      <c r="L43" t="s">
+        <v>109</v>
+      </c>
+      <c r="M43" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44" t="str">
+        <f>'2_combined'!J45</f>
+        <v>WT_sgA_R1_sense_nodsb</v>
+      </c>
+      <c r="C44" t="str">
+        <f>SUBSTITUTE('2_combined'!C45, "dsb", "DSB")</f>
+        <v>noDSB</v>
+      </c>
+      <c r="D44" t="str">
+        <f>'2_combined'!B45</f>
+        <v>1DSB_R1_sense.fa</v>
+      </c>
+      <c r="E44">
+        <f>'2_combined'!E45</f>
+        <v>67</v>
+      </c>
+      <c r="F44" t="str">
+        <f>'2_combined'!D45</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G44" t="str" cm="1">
+        <f t="array" ref="G44">IF(Table101416[[#This Row],[dsb_type]]="2DSB", "2", IF(Table101416[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table101416[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H44" t="str">
+        <f>'2_combined'!G45</f>
+        <v>R1</v>
+      </c>
+      <c r="I44" t="str">
+        <f>MID('2_combined'!I45, 3, 100)</f>
+        <v>A</v>
+      </c>
+      <c r="J44" t="str">
+        <f>'2_combined'!F45</f>
+        <v>WT</v>
+      </c>
+      <c r="K44" t="str">
+        <f>'2_combined'!H45</f>
+        <v>sense</v>
+      </c>
+      <c r="L44" t="str">
+        <f t="shared" ref="L44:L55" si="1">"with"</f>
+        <v>with</v>
+      </c>
+      <c r="M44" t="str">
+        <f>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table101416[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_nodsb -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>2</v>
+      </c>
+      <c r="B45" t="str">
+        <f>'2_combined'!J46</f>
+        <v>WT_sgA_R1_branch_nodsb</v>
+      </c>
+      <c r="C45" t="str">
+        <f>SUBSTITUTE('2_combined'!C46, "dsb", "DSB")</f>
+        <v>noDSB</v>
+      </c>
+      <c r="D45" t="str">
+        <f>'2_combined'!B46</f>
+        <v>1DSB_R1_branch.fa</v>
+      </c>
+      <c r="E45">
+        <f>'2_combined'!E46</f>
+        <v>67</v>
+      </c>
+      <c r="F45" t="str">
+        <f>'2_combined'!D46</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G45" t="str" cm="1">
+        <f t="array" ref="G45">IF(Table101416[[#This Row],[dsb_type]]="2DSB", "2", IF(Table101416[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table101416[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H45" t="str">
+        <f>'2_combined'!G46</f>
+        <v>R1</v>
+      </c>
+      <c r="I45" t="str">
+        <f>MID('2_combined'!I46, 3, 100)</f>
+        <v>A</v>
+      </c>
+      <c r="J45" t="str">
+        <f>'2_combined'!F46</f>
+        <v>WT</v>
+      </c>
+      <c r="K45" t="str">
+        <f>'2_combined'!H46</f>
+        <v>branch</v>
+      </c>
+      <c r="L45" t="str">
+        <f t="shared" si="1"/>
+        <v>with</v>
+      </c>
+      <c r="M45" t="str">
+        <f>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table101416[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch_nodsb -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>3</v>
+      </c>
+      <c r="B46" t="str">
+        <f>'2_combined'!J47</f>
+        <v>WT_sgA_R1_cmv_nodsb</v>
+      </c>
+      <c r="C46" t="str">
+        <f>SUBSTITUTE('2_combined'!C47, "dsb", "DSB")</f>
+        <v>noDSB</v>
+      </c>
+      <c r="D46" t="str">
+        <f>'2_combined'!B47</f>
+        <v>1DSB_R1_cmv.fa</v>
+      </c>
+      <c r="E46">
+        <f>'2_combined'!E47</f>
+        <v>67</v>
+      </c>
+      <c r="F46" t="str">
+        <f>'2_combined'!D47</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G46" t="str" cm="1">
+        <f t="array" ref="G46">IF(Table101416[[#This Row],[dsb_type]]="2DSB", "2", IF(Table101416[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table101416[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H46" t="str">
+        <f>'2_combined'!G47</f>
+        <v>R1</v>
+      </c>
+      <c r="I46" t="str">
+        <f>MID('2_combined'!I47, 3, 100)</f>
+        <v>A</v>
+      </c>
+      <c r="J46" t="str">
+        <f>'2_combined'!F47</f>
+        <v>WT</v>
+      </c>
+      <c r="K46" t="str">
+        <f>'2_combined'!H47</f>
+        <v>cmv</v>
+      </c>
+      <c r="L46" t="str">
+        <f t="shared" si="1"/>
+        <v>with</v>
+      </c>
+      <c r="M46" t="str">
+        <f>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table101416[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv_nodsb -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>4</v>
+      </c>
+      <c r="B47" t="str">
+        <f>'2_combined'!J48</f>
+        <v>KO_sgA_R1_sense_nodsb</v>
+      </c>
+      <c r="C47" t="str">
+        <f>SUBSTITUTE('2_combined'!C48, "dsb", "DSB")</f>
+        <v>noDSB</v>
+      </c>
+      <c r="D47" t="str">
+        <f>'2_combined'!B48</f>
+        <v>1DSB_R1_sense.fa</v>
+      </c>
+      <c r="E47">
+        <f>'2_combined'!E48</f>
+        <v>67</v>
+      </c>
+      <c r="F47" t="str">
+        <f>'2_combined'!D48</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G47" t="str" cm="1">
+        <f t="array" ref="G47">IF(Table101416[[#This Row],[dsb_type]]="2DSB", "2", IF(Table101416[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table101416[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H47" t="str">
+        <f>'2_combined'!G48</f>
+        <v>R1</v>
+      </c>
+      <c r="I47" t="str">
+        <f>MID('2_combined'!I48, 3, 100)</f>
+        <v>A</v>
+      </c>
+      <c r="J47" t="str">
+        <f>'2_combined'!F48</f>
+        <v>KO</v>
+      </c>
+      <c r="K47" t="str">
+        <f>'2_combined'!H48</f>
+        <v>sense</v>
+      </c>
+      <c r="L47" t="str">
+        <f t="shared" si="1"/>
+        <v>with</v>
+      </c>
+      <c r="M47" t="str">
+        <f>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table101416[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_nodsb -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>5</v>
+      </c>
+      <c r="B48" t="str">
+        <f>'2_combined'!J49</f>
+        <v>KO_sgA_R1_branch_nodsb</v>
+      </c>
+      <c r="C48" t="str">
+        <f>SUBSTITUTE('2_combined'!C49, "dsb", "DSB")</f>
+        <v>noDSB</v>
+      </c>
+      <c r="D48" t="str">
+        <f>'2_combined'!B49</f>
+        <v>1DSB_R1_branch.fa</v>
+      </c>
+      <c r="E48">
+        <f>'2_combined'!E49</f>
+        <v>67</v>
+      </c>
+      <c r="F48" t="str">
+        <f>'2_combined'!D49</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G48" t="str" cm="1">
+        <f t="array" ref="G48">IF(Table101416[[#This Row],[dsb_type]]="2DSB", "2", IF(Table101416[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table101416[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H48" t="str">
+        <f>'2_combined'!G49</f>
+        <v>R1</v>
+      </c>
+      <c r="I48" t="str">
+        <f>MID('2_combined'!I49, 3, 100)</f>
+        <v>A</v>
+      </c>
+      <c r="J48" t="str">
+        <f>'2_combined'!F49</f>
+        <v>KO</v>
+      </c>
+      <c r="K48" t="str">
+        <f>'2_combined'!H49</f>
+        <v>branch</v>
+      </c>
+      <c r="L48" t="str">
+        <f t="shared" si="1"/>
+        <v>with</v>
+      </c>
+      <c r="M48" t="str">
+        <f>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table101416[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch_nodsb -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>6</v>
+      </c>
+      <c r="B49" t="str">
+        <f>'2_combined'!J50</f>
+        <v>KO_sgA_R1_cmv_nodsb</v>
+      </c>
+      <c r="C49" t="str">
+        <f>SUBSTITUTE('2_combined'!C50, "dsb", "DSB")</f>
+        <v>noDSB</v>
+      </c>
+      <c r="D49" t="str">
+        <f>'2_combined'!B50</f>
+        <v>1DSB_R1_cmv.fa</v>
+      </c>
+      <c r="E49">
+        <f>'2_combined'!E50</f>
+        <v>67</v>
+      </c>
+      <c r="F49" t="str">
+        <f>'2_combined'!D50</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G49" t="str" cm="1">
+        <f t="array" ref="G49">IF(Table101416[[#This Row],[dsb_type]]="2DSB", "2", IF(Table101416[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table101416[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H49" t="str">
+        <f>'2_combined'!G50</f>
+        <v>R1</v>
+      </c>
+      <c r="I49" t="str">
+        <f>MID('2_combined'!I50, 3, 100)</f>
+        <v>A</v>
+      </c>
+      <c r="J49" t="str">
+        <f>'2_combined'!F50</f>
+        <v>KO</v>
+      </c>
+      <c r="K49" t="str">
+        <f>'2_combined'!H50</f>
+        <v>cmv</v>
+      </c>
+      <c r="L49" t="str">
+        <f t="shared" si="1"/>
+        <v>with</v>
+      </c>
+      <c r="M49" t="str">
+        <f>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table101416[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv_nodsb -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>7</v>
+      </c>
+      <c r="B50" t="str">
+        <f>'2_combined'!J51</f>
+        <v>WT_sgB_R2_sense_nodsb</v>
+      </c>
+      <c r="C50" t="str">
+        <f>SUBSTITUTE('2_combined'!C51, "dsb", "DSB")</f>
+        <v>noDSB</v>
+      </c>
+      <c r="D50" t="str">
+        <f>'2_combined'!B51</f>
+        <v>1DSB_R2_sense.fa</v>
+      </c>
+      <c r="E50">
+        <f>'2_combined'!E51</f>
+        <v>46</v>
+      </c>
+      <c r="F50" t="str">
+        <f>'2_combined'!D51</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G50" t="str" cm="1">
+        <f t="array" ref="G50">IF(Table101416[[#This Row],[dsb_type]]="2DSB", "2", IF(Table101416[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table101416[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H50" t="str">
+        <f>'2_combined'!G51</f>
+        <v>R2</v>
+      </c>
+      <c r="I50" t="str">
+        <f>MID('2_combined'!I51, 3, 100)</f>
+        <v>B</v>
+      </c>
+      <c r="J50" t="str">
+        <f>'2_combined'!F51</f>
+        <v>WT</v>
+      </c>
+      <c r="K50" t="str">
+        <f>'2_combined'!H51</f>
+        <v>sense</v>
+      </c>
+      <c r="L50" t="str">
+        <f t="shared" si="1"/>
+        <v>with</v>
+      </c>
+      <c r="M50" t="str">
+        <f>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table101416[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_nodsb -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>8</v>
+      </c>
+      <c r="B51" t="str">
+        <f>'2_combined'!J52</f>
+        <v>WT_sgB_R2_branch_nodsb</v>
+      </c>
+      <c r="C51" t="str">
+        <f>SUBSTITUTE('2_combined'!C52, "dsb", "DSB")</f>
+        <v>noDSB</v>
+      </c>
+      <c r="D51" t="str">
+        <f>'2_combined'!B52</f>
+        <v>1DSB_R2_branch.fa</v>
+      </c>
+      <c r="E51">
+        <f>'2_combined'!E52</f>
+        <v>46</v>
+      </c>
+      <c r="F51" t="str">
+        <f>'2_combined'!D52</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G51" t="str" cm="1">
+        <f t="array" ref="G51">IF(Table101416[[#This Row],[dsb_type]]="2DSB", "2", IF(Table101416[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table101416[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H51" t="str">
+        <f>'2_combined'!G52</f>
+        <v>R2</v>
+      </c>
+      <c r="I51" t="str">
+        <f>MID('2_combined'!I52, 3, 100)</f>
+        <v>B</v>
+      </c>
+      <c r="J51" t="str">
+        <f>'2_combined'!F52</f>
+        <v>WT</v>
+      </c>
+      <c r="K51" t="str">
+        <f>'2_combined'!H52</f>
+        <v>branch</v>
+      </c>
+      <c r="L51" t="str">
+        <f t="shared" si="1"/>
+        <v>with</v>
+      </c>
+      <c r="M51" t="str">
+        <f>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table101416[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch_nodsb -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>9</v>
+      </c>
+      <c r="B52" t="str">
+        <f>'2_combined'!J53</f>
+        <v>WT_sgB_R2_cmv_nodsb</v>
+      </c>
+      <c r="C52" t="str">
+        <f>SUBSTITUTE('2_combined'!C53, "dsb", "DSB")</f>
+        <v>noDSB</v>
+      </c>
+      <c r="D52" t="str">
+        <f>'2_combined'!B53</f>
+        <v>1DSB_R2_cmv.fa</v>
+      </c>
+      <c r="E52">
+        <f>'2_combined'!E53</f>
+        <v>46</v>
+      </c>
+      <c r="F52" t="str">
+        <f>'2_combined'!D53</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G52" t="str" cm="1">
+        <f t="array" ref="G52">IF(Table101416[[#This Row],[dsb_type]]="2DSB", "2", IF(Table101416[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table101416[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H52" t="str">
+        <f>'2_combined'!G53</f>
+        <v>R2</v>
+      </c>
+      <c r="I52" t="str">
+        <f>MID('2_combined'!I53, 3, 100)</f>
+        <v>B</v>
+      </c>
+      <c r="J52" t="str">
+        <f>'2_combined'!F53</f>
+        <v>WT</v>
+      </c>
+      <c r="K52" t="str">
+        <f>'2_combined'!H53</f>
+        <v>cmv</v>
+      </c>
+      <c r="L52" t="str">
+        <f t="shared" si="1"/>
+        <v>with</v>
+      </c>
+      <c r="M52" t="str">
+        <f>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table101416[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv_nodsb -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>10</v>
+      </c>
+      <c r="B53" t="str">
+        <f>'2_combined'!J54</f>
+        <v>KO_sgB_R2_sense_nodsb</v>
+      </c>
+      <c r="C53" t="str">
+        <f>SUBSTITUTE('2_combined'!C54, "dsb", "DSB")</f>
+        <v>noDSB</v>
+      </c>
+      <c r="D53" t="str">
+        <f>'2_combined'!B54</f>
+        <v>1DSB_R2_sense.fa</v>
+      </c>
+      <c r="E53">
+        <f>'2_combined'!E54</f>
+        <v>46</v>
+      </c>
+      <c r="F53" t="str">
+        <f>'2_combined'!D54</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G53" t="str" cm="1">
+        <f t="array" ref="G53">IF(Table101416[[#This Row],[dsb_type]]="2DSB", "2", IF(Table101416[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table101416[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H53" t="str">
+        <f>'2_combined'!G54</f>
+        <v>R2</v>
+      </c>
+      <c r="I53" t="str">
+        <f>MID('2_combined'!I54, 3, 100)</f>
+        <v>B</v>
+      </c>
+      <c r="J53" t="str">
+        <f>'2_combined'!F54</f>
+        <v>KO</v>
+      </c>
+      <c r="K53" t="str">
+        <f>'2_combined'!H54</f>
+        <v>sense</v>
+      </c>
+      <c r="L53" t="str">
+        <f t="shared" si="1"/>
+        <v>with</v>
+      </c>
+      <c r="M53" t="str">
+        <f>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table101416[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_nodsb -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>11</v>
+      </c>
+      <c r="B54" t="str">
+        <f>'2_combined'!J55</f>
+        <v>KO_sgB_R2_branch_nodsb</v>
+      </c>
+      <c r="C54" t="str">
+        <f>SUBSTITUTE('2_combined'!C55, "dsb", "DSB")</f>
+        <v>noDSB</v>
+      </c>
+      <c r="D54" t="str">
+        <f>'2_combined'!B55</f>
+        <v>1DSB_R2_branch.fa</v>
+      </c>
+      <c r="E54">
+        <f>'2_combined'!E55</f>
+        <v>46</v>
+      </c>
+      <c r="F54" t="str">
+        <f>'2_combined'!D55</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G54" t="str" cm="1">
+        <f t="array" ref="G54">IF(Table101416[[#This Row],[dsb_type]]="2DSB", "2", IF(Table101416[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table101416[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H54" t="str">
+        <f>'2_combined'!G55</f>
+        <v>R2</v>
+      </c>
+      <c r="I54" t="str">
+        <f>MID('2_combined'!I55, 3, 100)</f>
+        <v>B</v>
+      </c>
+      <c r="J54" t="str">
+        <f>'2_combined'!F55</f>
+        <v>KO</v>
+      </c>
+      <c r="K54" t="str">
+        <f>'2_combined'!H55</f>
+        <v>branch</v>
+      </c>
+      <c r="L54" t="str">
+        <f t="shared" si="1"/>
+        <v>with</v>
+      </c>
+      <c r="M54" t="str">
+        <f>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table101416[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch_nodsb -o plots/graphs/</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>12</v>
+      </c>
+      <c r="B55" t="str">
+        <f>'2_combined'!J56</f>
+        <v>KO_sgB_R2_cmv_nodsb</v>
+      </c>
+      <c r="C55" t="str">
+        <f>SUBSTITUTE('2_combined'!C56, "dsb", "DSB")</f>
+        <v>noDSB</v>
+      </c>
+      <c r="D55" t="str">
+        <f>'2_combined'!B56</f>
+        <v>1DSB_R2_cmv.fa</v>
+      </c>
+      <c r="E55">
+        <f>'2_combined'!E56</f>
+        <v>46</v>
+      </c>
+      <c r="F55" t="str">
+        <f>'2_combined'!D56</f>
+        <v>1DSB</v>
+      </c>
+      <c r="G55" t="str" cm="1">
+        <f t="array" ref="G55">IF(Table101416[[#This Row],[dsb_type]]="2DSB", "2", IF(Table101416[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(Table101416[[#This Row],[dsb_type]]="1DSB", "1", NA)))</f>
+        <v>1</v>
+      </c>
+      <c r="H55" t="str">
+        <f>'2_combined'!G56</f>
+        <v>R2</v>
+      </c>
+      <c r="I55" t="str">
+        <f>MID('2_combined'!I56, 3, 100)</f>
+        <v>B</v>
+      </c>
+      <c r="J55" t="str">
+        <f>'2_combined'!F56</f>
+        <v>KO</v>
+      </c>
+      <c r="K55" t="str">
+        <f>'2_combined'!H56</f>
+        <v>cmv</v>
+      </c>
+      <c r="L55" t="str">
+        <f t="shared" si="1"/>
+        <v>with</v>
+      </c>
+      <c r="M55" t="str">
+        <f>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/",Table101416[[#This Row],[dir]], " -o ", graph, "/")</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv_nodsb -o plots/graphs/</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create PPTX from command line working.
</commit_message>
<xml_diff>
--- a/libinfo.xlsx
+++ b/libinfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tchan\Code\SCMB_Project\RNA-mediated_DSB_repair\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7846DFB1-D5A3-414F-A90D-1DBAC17AB621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769DA42C-BE18-4C6A-B1CA-3C699C36E2BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="4" activeTab="9" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="4" activeTab="8" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
   </bookViews>
   <sheets>
     <sheet name="globals" sheetId="3" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -758,6 +758,126 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -765,6 +885,104 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -804,15 +1022,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -829,6 +1038,68 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -952,42 +1223,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1004,72 +1239,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </right>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -1173,364 +1342,6 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -1651,21 +1462,41 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -1705,6 +1536,27 @@
       </font>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1724,6 +1576,79 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -1731,8 +1656,101 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1798,6 +1816,15 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
       </font>
@@ -1834,84 +1861,25 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1920,25 +1888,42 @@
       <font>
         <b/>
       </font>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2001,6 +1986,18 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -2017,6 +2014,9 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2035,7 +2035,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{70502F2F-AE2C-4D63-ADF7-F65702652EBF}" name="table_1_2" displayName="table_1_2" ref="A1:D108" totalsRowShown="0">
   <autoFilter ref="A1:D108" xr:uid="{70502F2F-AE2C-4D63-ADF7-F65702652EBF}"/>
   <tableColumns count="4">
-    <tableColumn id="2" xr3:uid="{BB99DCDA-08D4-474A-ABC3-5229CEAF80CF}" name="id" dataDxfId="162">
+    <tableColumn id="2" xr3:uid="{BB99DCDA-08D4-474A-ABC3-5229CEAF80CF}" name="id" dataDxfId="201">
       <calculatedColumnFormula>INT(MID(table_1_2[[#This Row],[library]], 4, 10))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{5F63B290-093A-48A3-9AFC-EB2FE27DE630}" name="library"/>
@@ -2047,44 +2047,44 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}" name="table_5_1" displayName="table_5_1" ref="A1:M41" totalsRowShown="0" headerRowDxfId="177">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}" name="table_5_1" displayName="table_5_1" ref="A1:M41" totalsRowShown="0" headerRowDxfId="98">
   <autoFilter ref="A1:M41" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
   <tableColumns count="13">
-    <tableColumn id="25" xr3:uid="{43F57146-0E56-46F3-A0E3-717A41010F4A}" name="index" dataDxfId="176"/>
-    <tableColumn id="1" xr3:uid="{B0B3F6B0-7577-49AC-B865-1E873B4DC53C}" name="dir" dataDxfId="99">
+    <tableColumn id="25" xr3:uid="{43F57146-0E56-46F3-A0E3-717A41010F4A}" name="index" dataDxfId="97"/>
+    <tableColumn id="1" xr3:uid="{B0B3F6B0-7577-49AC-B865-1E873B4DC53C}" name="dir" dataDxfId="96">
       <calculatedColumnFormula>table_3_1[[#This Row],[dir]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{D04F356F-9288-416D-ACDA-6BFE128B70D7}" name="control" dataDxfId="98">
+    <tableColumn id="13" xr3:uid="{D04F356F-9288-416D-ACDA-6BFE128B70D7}" name="control" dataDxfId="95">
       <calculatedColumnFormula>table_3_1[[#This Row],[control]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{9C168B22-F534-40D4-947C-918239C33FD9}" name="ref" dataDxfId="97">
+    <tableColumn id="2" xr3:uid="{9C168B22-F534-40D4-947C-918239C33FD9}" name="ref" dataDxfId="94">
       <calculatedColumnFormula>table_3_1[[#This Row],[ref]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{6F64477B-0C66-4251-9156-22307A6D70A0}" name="dsb_pos" dataDxfId="96">
+    <tableColumn id="3" xr3:uid="{6F64477B-0C66-4251-9156-22307A6D70A0}" name="dsb_pos" dataDxfId="93">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_pos]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{D037F4F2-543F-4D7D-AB36-0B253FD61B0D}" name="dsb_type" dataDxfId="95">
+    <tableColumn id="4" xr3:uid="{D037F4F2-543F-4D7D-AB36-0B253FD61B0D}" name="dsb_type" dataDxfId="92">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_type]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{407AC5E6-13CB-409A-8E78-64B8CC121882}" name="dsb_type_command" dataDxfId="94">
+    <tableColumn id="12" xr3:uid="{407AC5E6-13CB-409A-8E78-64B8CC121882}" name="dsb_type_command" dataDxfId="91">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_type_command]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{1A24C844-2A10-4394-818F-0C25A569B414}" name="strand" dataDxfId="93">
+    <tableColumn id="5" xr3:uid="{1A24C844-2A10-4394-818F-0C25A569B414}" name="strand" dataDxfId="90">
       <calculatedColumnFormula>table_3_1[[#This Row],[strand]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{4F0A02F9-5555-489E-BA41-E3CBF81D1114}" name="hguide" dataDxfId="92">
+    <tableColumn id="6" xr3:uid="{4F0A02F9-5555-489E-BA41-E3CBF81D1114}" name="hguide" dataDxfId="89">
       <calculatedColumnFormula>table_3_1[[#This Row],[hguide]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FAE741F2-7C1B-41F2-8875-9F7A2EF40A54}" name="cell" dataDxfId="91">
+    <tableColumn id="7" xr3:uid="{FAE741F2-7C1B-41F2-8875-9F7A2EF40A54}" name="cell" dataDxfId="88">
       <calculatedColumnFormula>table_3_1[[#This Row],[cell]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{FE3ED128-2534-43D1-9244-11AB1FB57650}" name="treatment" dataDxfId="90">
+    <tableColumn id="8" xr3:uid="{FE3ED128-2534-43D1-9244-11AB1FB57650}" name="treatment" dataDxfId="87">
       <calculatedColumnFormula>table_3_1[[#This Row],[treatment]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{65ACBC9C-0EC8-4074-B310-05F4B70BFAD5}" name="subst_type" dataDxfId="169">
+    <tableColumn id="9" xr3:uid="{65ACBC9C-0EC8-4074-B310-05F4B70BFAD5}" name="subst_type" dataDxfId="86">
       <calculatedColumnFormula>"with"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{F80F6FB9-4F35-4819-8285-D77131C6EFCE}" name="command" dataDxfId="78">
+    <tableColumn id="10" xr3:uid="{F80F6FB9-4F35-4819-8285-D77131C6EFCE}" name="command" dataDxfId="85">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2097,40 +2097,40 @@
   <autoFilter ref="A43:M55" xr:uid="{D74A5276-1A50-4DA1-9131-9669404C8622}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{8AC09A63-4226-4C75-8801-68CF93C0F078}" name="index"/>
-    <tableColumn id="2" xr3:uid="{77584C42-D70C-48A4-979A-F4DEA0B31542}" name="dir" dataDxfId="89">
+    <tableColumn id="2" xr3:uid="{77584C42-D70C-48A4-979A-F4DEA0B31542}" name="dir" dataDxfId="84">
       <calculatedColumnFormula>table_3_2[[#This Row],[dir]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{483E3D73-4059-4B65-84EC-5DC4E7008F35}" name="control" dataDxfId="88">
+    <tableColumn id="3" xr3:uid="{483E3D73-4059-4B65-84EC-5DC4E7008F35}" name="control" dataDxfId="83">
       <calculatedColumnFormula>table_3_2[[#This Row],[control]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5859A8DB-4C52-4451-BBB6-C6BEBF497540}" name="ref" dataDxfId="87">
+    <tableColumn id="4" xr3:uid="{5859A8DB-4C52-4451-BBB6-C6BEBF497540}" name="ref" dataDxfId="82">
       <calculatedColumnFormula>table_3_2[[#This Row],[ref]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{06FC4099-C18C-436C-B1E6-9739B71C7F22}" name="dsb_pos" dataDxfId="86">
+    <tableColumn id="5" xr3:uid="{06FC4099-C18C-436C-B1E6-9739B71C7F22}" name="dsb_pos" dataDxfId="81">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_pos]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8F043A8E-C5E7-4596-AE13-3E495C6DB33E}" name="dsb_type" dataDxfId="85">
+    <tableColumn id="6" xr3:uid="{8F043A8E-C5E7-4596-AE13-3E495C6DB33E}" name="dsb_type" dataDxfId="80">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_type]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E2DB136E-6FA9-4095-8B91-F094974333AF}" name="dsb_type_command" dataDxfId="84">
+    <tableColumn id="7" xr3:uid="{E2DB136E-6FA9-4095-8B91-F094974333AF}" name="dsb_type_command" dataDxfId="79">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_type_command]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{55CDC54E-3E43-4365-B1C9-5359F747A157}" name="strand" dataDxfId="83">
+    <tableColumn id="8" xr3:uid="{55CDC54E-3E43-4365-B1C9-5359F747A157}" name="strand" dataDxfId="78">
       <calculatedColumnFormula>table_3_2[[#This Row],[strand]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{056BD8A0-CC40-4C61-9F22-EE7382045F66}" name="hguide" dataDxfId="82">
+    <tableColumn id="9" xr3:uid="{056BD8A0-CC40-4C61-9F22-EE7382045F66}" name="hguide" dataDxfId="77">
       <calculatedColumnFormula>table_3_2[[#This Row],[hguide]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{489E156D-888A-4DDC-BB23-A4721D588249}" name="cell" dataDxfId="81">
+    <tableColumn id="10" xr3:uid="{489E156D-888A-4DDC-BB23-A4721D588249}" name="cell" dataDxfId="76">
       <calculatedColumnFormula>table_3_2[[#This Row],[cell]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{0F1B5F9E-B10D-4258-9052-90BCDC89F0B0}" name="treatment" dataDxfId="80">
+    <tableColumn id="11" xr3:uid="{0F1B5F9E-B10D-4258-9052-90BCDC89F0B0}" name="treatment" dataDxfId="75">
       <calculatedColumnFormula>table_3_2[[#This Row],[treatment]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A2723EF6-80E8-4D8D-A6DC-7556C1996222}" name="subst_type" dataDxfId="168">
+    <tableColumn id="12" xr3:uid="{A2723EF6-80E8-4D8D-A6DC-7556C1996222}" name="subst_type" dataDxfId="74">
       <calculatedColumnFormula>"with"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{02531CCA-6CDE-42BA-80E3-31C0F97A3546}" name="command" dataDxfId="79">
+    <tableColumn id="13" xr3:uid="{02531CCA-6CDE-42BA-80E3-31C0F97A3546}" name="command" dataDxfId="73">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2139,65 +2139,65 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E39D37F2-5006-44FB-A873-CCC98F8BA522}" name="table_6_1" displayName="table_6_1" ref="A1:T7" totalsRowShown="0" headerRowDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E39D37F2-5006-44FB-A873-CCC98F8BA522}" name="table_6_1" displayName="table_6_1" ref="A1:T7" totalsRowShown="0" headerRowDxfId="72">
   <autoFilter ref="A1:T7" xr:uid="{E39D37F2-5006-44FB-A873-CCC98F8BA522}"/>
   <tableColumns count="20">
-    <tableColumn id="25" xr3:uid="{CD5CCC3B-8B5B-4C20-98D1-63A7E1FB075B}" name="index" dataDxfId="46"/>
-    <tableColumn id="18" xr3:uid="{A6E432BE-5846-48EE-948A-BE81A4E2B6F5}" name="dir_1" dataDxfId="17">
+    <tableColumn id="25" xr3:uid="{CD5CCC3B-8B5B-4C20-98D1-63A7E1FB075B}" name="index" dataDxfId="71"/>
+    <tableColumn id="18" xr3:uid="{A6E432BE-5846-48EE-948A-BE81A4E2B6F5}" name="dir_1" dataDxfId="70">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_1]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{A826EC7B-673B-4DCB-8792-35762AD6C5ED}" name="dir_2" dataDxfId="45">
+    <tableColumn id="17" xr3:uid="{A826EC7B-673B-4DCB-8792-35762AD6C5ED}" name="dir_2" dataDxfId="69">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_2]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{F6910118-048E-4746-9072-727F3B1847FE}" name="dir_3" dataDxfId="44">
+    <tableColumn id="16" xr3:uid="{F6910118-048E-4746-9072-727F3B1847FE}" name="dir_3" dataDxfId="68">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_3]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{0BBECB52-3A0A-4374-9C43-DA21C4CA365C}" name="dir_4" dataDxfId="43">
+    <tableColumn id="15" xr3:uid="{0BBECB52-3A0A-4374-9C43-DA21C4CA365C}" name="dir_4" dataDxfId="67">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_4]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{6E2A95BE-29B1-4454-9E5B-BED35BBC5239}" name="dir_5" dataDxfId="42">
+    <tableColumn id="14" xr3:uid="{6E2A95BE-29B1-4454-9E5B-BED35BBC5239}" name="dir_5" dataDxfId="66">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_5]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{4BDBAB17-9D30-4F82-92E5-FBABD10C580E}" name="dir_6" dataDxfId="41">
+    <tableColumn id="1" xr3:uid="{4BDBAB17-9D30-4F82-92E5-FBABD10C580E}" name="dir_6" dataDxfId="65">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_6]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{8377C5E1-81CB-41A4-9754-5BDCCCB5D946}" name="dir_7" dataDxfId="15">
+    <tableColumn id="21" xr3:uid="{8377C5E1-81CB-41A4-9754-5BDCCCB5D946}" name="dir_7" dataDxfId="64">
       <calculatedColumnFormula array="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_7]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{0BBDCF08-0538-454A-A8A3-33839702EB7D}" name="dir_8" dataDxfId="22">
+    <tableColumn id="23" xr3:uid="{0BBDCF08-0538-454A-A8A3-33839702EB7D}" name="dir_8" dataDxfId="63">
       <calculatedColumnFormula array="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_8]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{362AFBD7-D8FE-484B-A796-99C68A4873AF}" name="dir_9" dataDxfId="21">
+    <tableColumn id="24" xr3:uid="{362AFBD7-D8FE-484B-A796-99C68A4873AF}" name="dir_9" dataDxfId="62">
       <calculatedColumnFormula array="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_9]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{F8401415-A0F2-4302-B6F1-2F4769D22B7D}" name="dir_10" dataDxfId="20">
+    <tableColumn id="26" xr3:uid="{F8401415-A0F2-4302-B6F1-2F4769D22B7D}" name="dir_10" dataDxfId="61">
       <calculatedColumnFormula array="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_10]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{EB5FA985-8547-4A83-8A97-6BDBC99AFC75}" name="dir_11" dataDxfId="19">
+    <tableColumn id="27" xr3:uid="{EB5FA985-8547-4A83-8A97-6BDBC99AFC75}" name="dir_11" dataDxfId="60">
       <calculatedColumnFormula array="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_11]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{531860AE-4501-4DFE-ABC6-8AEC03CA2891}" name="dir_12" dataDxfId="18">
+    <tableColumn id="28" xr3:uid="{531860AE-4501-4DFE-ABC6-8AEC03CA2891}" name="dir_12" dataDxfId="59">
       <calculatedColumnFormula array="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_12]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{991CDA96-8100-4EC0-BA2D-509D87E3B77E}" name="control" dataDxfId="28">
+    <tableColumn id="13" xr3:uid="{991CDA96-8100-4EC0-BA2D-509D87E3B77E}" name="control" dataDxfId="58">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 6 * (table_6_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AB636280-F214-4141-A265-B2AC639CF4A7}" name="dsb_type" dataDxfId="27">
+    <tableColumn id="4" xr3:uid="{AB636280-F214-4141-A265-B2AC639CF4A7}" name="dsb_type" dataDxfId="57">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], 6 * (table_6_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{56C39C59-71CD-4F29-9AA2-7C1BE588DDCF}" name="strand" dataDxfId="26">
+    <tableColumn id="5" xr3:uid="{56C39C59-71CD-4F29-9AA2-7C1BE588DDCF}" name="strand" dataDxfId="56">
       <calculatedColumnFormula>OFFSET(table_3_1[strand], 6 * (table_6_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{77B8B06C-E91A-4366-BAAD-4D98914358E6}" name="hguide" dataDxfId="25">
+    <tableColumn id="6" xr3:uid="{77B8B06C-E91A-4366-BAAD-4D98914358E6}" name="hguide" dataDxfId="55">
       <calculatedColumnFormula>OFFSET(table_3_1[hguide], 6 * (table_6_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{64A9E7E6-7F9F-4F61-9A23-E4157ABDCFAC}" name="subst_type" dataDxfId="24">
+    <tableColumn id="9" xr3:uid="{64A9E7E6-7F9F-4F61-9A23-E4157ABDCFAC}" name="subst_type" dataDxfId="54">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{B53E652A-5D37-4D63-8F38-4B8DBDB37226}" name="dir_out" dataDxfId="23">
+    <tableColumn id="19" xr3:uid="{B53E652A-5D37-4D63-8F38-4B8DBDB37226}" name="dir_out" dataDxfId="53">
       <calculatedColumnFormula>_xlfn.CONCAT(table_6_1[[#This Row],[dsb_type]], "_", table_6_1[[#This Row],[strand]], IF(table_6_1[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_1[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{9C3C4C97-49A2-40B9-BCC3-5739C07213CD}" name="command" dataDxfId="16">
+    <tableColumn id="10" xr3:uid="{9C3C4C97-49A2-40B9-BCC3-5739C07213CD}" name="command" dataDxfId="52">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", _xlfn.TEXTJOIN(" ", TRUE, table_6_1[[#This Row],[dir_1]:[dir_12]]), " -o ", layouts, "/", table_6_1[[#This Row],[dir_out]], " --subst_type ", table_6_1[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2206,35 +2206,35 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{5FFA4758-C47A-4F1C-9890-69E7F39BE130}" name="table_6_2" displayName="table_6_2" ref="A10:J12" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="39" tableBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{5FFA4758-C47A-4F1C-9890-69E7F39BE130}" name="table_6_2" displayName="table_6_2" ref="A10:J12" totalsRowShown="0" headerRowDxfId="51" headerRowBorderDxfId="50" tableBorderDxfId="49">
   <autoFilter ref="A10:J12" xr:uid="{5FFA4758-C47A-4F1C-9890-69E7F39BE130}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{40A0667B-C93C-4531-B41F-A65EDE89F51E}" name="index"/>
-    <tableColumn id="2" xr3:uid="{A54C9A1D-E384-4C87-B6DD-98A7ADBAD240}" name="dir_1" dataDxfId="36">
+    <tableColumn id="2" xr3:uid="{A54C9A1D-E384-4C87-B6DD-98A7ADBAD240}" name="dir_1" dataDxfId="48">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset - 1 + COLUMN() - 2 + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{7CACC7DC-6834-41E4-A17F-74F62473FF4D}" name="dir_2" dataDxfId="38">
+    <tableColumn id="3" xr3:uid="{7CACC7DC-6834-41E4-A17F-74F62473FF4D}" name="dir_2" dataDxfId="47">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset - 1 + COLUMN() - 2 + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{BEB4CA3E-14C3-4D70-BAFF-DBFFE398E04E}" name="control" dataDxfId="31">
+    <tableColumn id="4" xr3:uid="{BEB4CA3E-14C3-4D70-BAFF-DBFFE398E04E}" name="control" dataDxfId="46">
       <calculatedColumnFormula>OFFSET(table_3_1[control], var_6_anti_offset - 1 + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{08F18E8F-5127-4F55-95E0-05877340A45E}" name="dsb_type" dataDxfId="32">
+    <tableColumn id="5" xr3:uid="{08F18E8F-5127-4F55-95E0-05877340A45E}" name="dsb_type" dataDxfId="45">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], var_6_anti_offset - 1 + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B0010190-2798-4D5F-A1DA-8D1F1A867502}" name="strand" dataDxfId="33">
+    <tableColumn id="6" xr3:uid="{B0010190-2798-4D5F-A1DA-8D1F1A867502}" name="strand" dataDxfId="44">
       <calculatedColumnFormula array="1">OFFSET(table_3_1[strand], var_6_anti_offset - 1 + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{689C42CC-8508-4116-808A-19A0641C3F05}" name="hguide" dataDxfId="30">
+    <tableColumn id="7" xr3:uid="{689C42CC-8508-4116-808A-19A0641C3F05}" name="hguide" dataDxfId="43">
       <calculatedColumnFormula>OFFSET(table_3_1[hguide], var_6_anti_offset - 1 + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{48005280-1CD9-4496-941A-723AEDDD9036}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{5F8C6AF1-A602-4306-A909-592B4268C611}" name="dir_out" dataDxfId="35">
+    <tableColumn id="9" xr3:uid="{5F8C6AF1-A602-4306-A909-592B4268C611}" name="dir_out" dataDxfId="42">
       <calculatedColumnFormula>_xlfn.CONCAT(table_6_2[[#This Row],[dsb_type]], "_", table_6_2[[#This Row],[strand]], IF(table_6_2[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_2[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{3AEE0650-E928-4CB1-8CCF-22F967A16636}" name="command" dataDxfId="34">
+    <tableColumn id="10" xr3:uid="{3AEE0650-E928-4CB1-8CCF-22F967A16636}" name="command" dataDxfId="41">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", _xlfn.TEXTJOIN(" ", TRUE, table_6_2[[#This Row],[dir_1]:[dir_2]]), " -o ", layouts, "/", table_6_2[[#This Row],[dir_out]], " --subst_type ", table_6_2[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2243,47 +2243,47 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{86CE8E4A-18BF-427A-81F0-F9655767A016}" name="table_7_1" displayName="table_7_1" ref="A1:N41" totalsRowShown="0" headerRowDxfId="166">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{86CE8E4A-18BF-427A-81F0-F9655767A016}" name="table_7_1" displayName="table_7_1" ref="A1:N41" totalsRowShown="0" headerRowDxfId="40">
   <autoFilter ref="A1:N41" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
   <tableColumns count="14">
-    <tableColumn id="25" xr3:uid="{C323C376-24D3-4404-9E0F-6E9361862271}" name="index" dataDxfId="165"/>
-    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="77">
+    <tableColumn id="25" xr3:uid="{C323C376-24D3-4404-9E0F-6E9361862271}" name="index" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="38">
       <calculatedColumnFormula>table_3_1[[#This Row],[dir]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="76">
+    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="37">
       <calculatedColumnFormula>table_3_1[[#This Row],[control]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="75">
+    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="36">
       <calculatedColumnFormula>table_3_1[[#This Row],[ref]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="74">
+    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="35">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_pos]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="73">
+    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="34">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_type]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="72">
+    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="33">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_type_command]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="71">
+    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="32">
       <calculatedColumnFormula>table_3_1[[#This Row],[strand]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="70">
+    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="31">
       <calculatedColumnFormula>table_3_1[[#This Row],[hguide]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="69">
+    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="30">
       <calculatedColumnFormula>table_3_1[[#This Row],[cell]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="68">
+    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="29">
       <calculatedColumnFormula>table_3_1[[#This Row],[treatment]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="164">
+    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="28">
       <calculatedColumnFormula>"with"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="29">
+    <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="27">
       <calculatedColumnFormula>IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[dir_out],QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[dir_out], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="13">
+    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="26">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", " --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2295,41 +2295,41 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{B47D9508-D874-40FC-B6F6-C106B48F6A94}" name="table_7_2" displayName="table_7_2" ref="A43:N55" totalsRowShown="0">
   <autoFilter ref="A43:N55" xr:uid="{D74A5276-1A50-4DA1-9131-9669404C8622}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{488C5146-A746-4F74-BCC8-806E4DC740CE}" name="index" dataDxfId="160"/>
-    <tableColumn id="2" xr3:uid="{C2A88DF4-2444-4C4C-A089-6CF9ADE79BD8}" name="dir" dataDxfId="67">
+    <tableColumn id="1" xr3:uid="{488C5146-A746-4F74-BCC8-806E4DC740CE}" name="index" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{C2A88DF4-2444-4C4C-A089-6CF9ADE79BD8}" name="dir" dataDxfId="24">
       <calculatedColumnFormula>table_3_2[[#This Row],[dir]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{7698ACE3-2351-400D-B00F-5A70184F8A33}" name="control" dataDxfId="66">
+    <tableColumn id="3" xr3:uid="{7698ACE3-2351-400D-B00F-5A70184F8A33}" name="control" dataDxfId="23">
       <calculatedColumnFormula>table_3_2[[#This Row],[control]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5E82B04C-FF09-492C-8A23-7E43B5990149}" name="ref" dataDxfId="65">
+    <tableColumn id="4" xr3:uid="{5E82B04C-FF09-492C-8A23-7E43B5990149}" name="ref" dataDxfId="22">
       <calculatedColumnFormula>table_3_2[[#This Row],[ref]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{F4D36A0E-549B-4F3A-BCA9-75E151448998}" name="dsb_pos" dataDxfId="64">
+    <tableColumn id="5" xr3:uid="{F4D36A0E-549B-4F3A-BCA9-75E151448998}" name="dsb_pos" dataDxfId="21">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_pos]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{AEBBBB88-8CE2-409D-AE19-9C23263250A9}" name="dsb_type" dataDxfId="63">
+    <tableColumn id="6" xr3:uid="{AEBBBB88-8CE2-409D-AE19-9C23263250A9}" name="dsb_type" dataDxfId="20">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_type]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3E71E7D2-0FA5-4FD5-BDC3-2955A091A9E6}" name="dsb_type_command" dataDxfId="62">
+    <tableColumn id="7" xr3:uid="{3E71E7D2-0FA5-4FD5-BDC3-2955A091A9E6}" name="dsb_type_command" dataDxfId="19">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_type_command]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{EBD35881-E696-4202-9149-75A4EFFFAAD6}" name="strand" dataDxfId="61">
+    <tableColumn id="8" xr3:uid="{EBD35881-E696-4202-9149-75A4EFFFAAD6}" name="strand" dataDxfId="18">
       <calculatedColumnFormula>table_3_2[[#This Row],[strand]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{123CA279-0CB6-41C1-9CD8-20D375B9B66D}" name="hguide" dataDxfId="60">
+    <tableColumn id="9" xr3:uid="{123CA279-0CB6-41C1-9CD8-20D375B9B66D}" name="hguide" dataDxfId="17">
       <calculatedColumnFormula>table_3_2[[#This Row],[hguide]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{3DCE3F3A-187D-411E-93FC-8C6C3EE9CAA2}" name="cell" dataDxfId="59">
+    <tableColumn id="10" xr3:uid="{3DCE3F3A-187D-411E-93FC-8C6C3EE9CAA2}" name="cell" dataDxfId="16">
       <calculatedColumnFormula>table_3_2[[#This Row],[cell]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{9E585D29-AB3E-4D04-8C1D-24F78339C9A3}" name="treatment" dataDxfId="58">
+    <tableColumn id="11" xr3:uid="{9E585D29-AB3E-4D04-8C1D-24F78339C9A3}" name="treatment" dataDxfId="15">
       <calculatedColumnFormula>table_3_2[[#This Row],[treatment]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{928286B8-23FB-4375-B52B-617DD59D6098}" name="subst_type" dataDxfId="163">
+    <tableColumn id="12" xr3:uid="{928286B8-23FB-4375-B52B-617DD59D6098}" name="subst_type" dataDxfId="14">
       <calculatedColumnFormula>"with"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{E18D2025-56E8-4128-9201-9E0BF8A67AC0}" name="common_layout_dir" dataDxfId="14">
+    <tableColumn id="15" xr3:uid="{E18D2025-56E8-4128-9201-9E0BF8A67AC0}" name="common_layout_dir" dataDxfId="13">
       <calculatedColumnFormula>OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_2[[#This Row],[index]] - 1, 6) + 2, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="13" xr3:uid="{0917AB98-1545-4642-9BE8-618AAA1E404A}" name="command" dataDxfId="12">
@@ -2341,14 +2341,14 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{B76EEC45-4FC3-44D5-9B2E-9183DF724F60}" name="table_7_3" displayName="table_7_3" ref="A1:C17" totalsRowShown="0" headerRowDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{B76EEC45-4FC3-44D5-9B2E-9183DF724F60}" name="table_7_3" displayName="table_7_3" ref="A1:C17" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="A1:C17" xr:uid="{B76EEC45-4FC3-44D5-9B2E-9183DF724F60}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{FAFADB73-BF3B-401A-8C48-9FCB5D3C4CB6}" name="index" dataDxfId="56"/>
-    <tableColumn id="4" xr3:uid="{8541A14E-3250-4B9C-B315-969FC11BE60A}" name="dir" dataDxfId="51">
+    <tableColumn id="1" xr3:uid="{FAFADB73-BF3B-401A-8C48-9FCB5D3C4CB6}" name="index" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{8541A14E-3250-4B9C-B315-969FC11BE60A}" name="dir" dataDxfId="9">
       <calculatedColumnFormula>table_4_1[[#This Row],[dir_out]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{EAD6D5EC-B61E-4A98-B4FD-4932757CFEA3}" name="command" dataDxfId="5">
+    <tableColumn id="6" xr3:uid="{EAD6D5EC-B61E-4A98-B4FD-4932757CFEA3}" name="command" dataDxfId="8">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, " --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2357,11 +2357,11 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{8B4E853A-A4F1-4022-B857-226C57559A5F}" name="table_7_4" displayName="table_7_4" ref="A19:C21" totalsRowShown="0" headerRowDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{8B4E853A-A4F1-4022-B857-226C57559A5F}" name="table_7_4" displayName="table_7_4" ref="A19:C21" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A19:C21" xr:uid="{8B4E853A-A4F1-4022-B857-226C57559A5F}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{1ECF32A2-E353-4754-B4C5-11C46AACF6C0}" name="index" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{181C59FC-364D-4421-8E54-98DFF4CA7C05}" name="dir" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{1ECF32A2-E353-4754-B4C5-11C46AACF6C0}" name="index" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{181C59FC-364D-4421-8E54-98DFF4CA7C05}" name="dir" dataDxfId="5">
       <calculatedColumnFormula>OFFSET(table_4_2[[dir_out]:[dir_out]], table_7_4[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{6D8CC942-572B-44F2-BCA6-4D31A25A4067}" name="command" dataDxfId="4">
@@ -2373,14 +2373,14 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{58F5EC27-BD76-45AE-8D38-F4E705EF79E9}" name="table_7_5" displayName="table_7_5" ref="A24:C32" totalsRowShown="0" headerRowDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{58F5EC27-BD76-45AE-8D38-F4E705EF79E9}" name="table_7_5" displayName="table_7_5" ref="A24:C32" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A24:C32" xr:uid="{58F5EC27-BD76-45AE-8D38-F4E705EF79E9}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{AAC1476C-44CE-49FD-8254-50BAEAA6929C}" name="index" dataDxfId="52"/>
-    <tableColumn id="4" xr3:uid="{1222E48F-ED5C-48AA-BA39-1443B841BC9F}" name="dir" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{AAC1476C-44CE-49FD-8254-50BAEAA6929C}" name="index" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{1222E48F-ED5C-48AA-BA39-1443B841BC9F}" name="dir" dataDxfId="1">
       <calculatedColumnFormula>OFFSET(table_4_3[[dir_out]:[dir_out]], table_7_5[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{89B7E589-2097-43FC-B96B-19D2EF777E97}" name="command_main_data_combined" dataDxfId="3">
+    <tableColumn id="6" xr3:uid="{89B7E589-2097-43FC-B96B-19D2EF777E97}" name="command_main_data_combined" dataDxfId="0">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, " --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2389,10 +2389,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22A90416-B904-4D3D-A6DB-EFCB9FD1EAED}" name="table_1" displayName="table_1" ref="A1:O173" totalsRowShown="0" headerRowDxfId="201">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22A90416-B904-4D3D-A6DB-EFCB9FD1EAED}" name="table_1" displayName="table_1" ref="A1:O173" totalsRowShown="0" headerRowDxfId="200">
   <autoFilter ref="A1:O173" xr:uid="{22A90416-B904-4D3D-A6DB-EFCB9FD1EAED}"/>
   <tableColumns count="15">
-    <tableColumn id="15" xr3:uid="{A06DA701-31D6-44A5-8655-82CAD7E3082B}" name="index" dataDxfId="115"/>
+    <tableColumn id="15" xr3:uid="{A06DA701-31D6-44A5-8655-82CAD7E3082B}" name="index" dataDxfId="199"/>
     <tableColumn id="1" xr3:uid="{5C1CDEE9-AAC7-4E12-B88F-1314CF422335}" name="library"/>
     <tableColumn id="2" xr3:uid="{D4B174CF-F774-4DA7-B75D-573BC94EE10F}" name="cell"/>
     <tableColumn id="3" xr3:uid="{83898EC9-96DA-46D4-B0B8-F68C7607DCF2}" name="control"/>
@@ -2400,25 +2400,25 @@
     <tableColumn id="5" xr3:uid="{81A143FE-8E74-4182-8124-E697DD5A7C62}" name="hguide"/>
     <tableColumn id="6" xr3:uid="{4A316E6A-69F3-4B78-9C01-4675AEB656FA}" name="treatment"/>
     <tableColumn id="7" xr3:uid="{25B8E763-346D-4756-8B58-D3C8CB103545}" name="strand"/>
-    <tableColumn id="8" xr3:uid="{4B708639-BB19-4DC1-A57D-214FA0EFB1EA}" name="dsb_pos" dataDxfId="200">
+    <tableColumn id="8" xr3:uid="{4B708639-BB19-4DC1-A57D-214FA0EFB1EA}" name="dsb_pos" dataDxfId="198">
       <calculatedColumnFormula array="1">IF(E2="2DSB", IF(H2="R1", 67, 46), IF(E2="1DSB", IF(H2="R1", 67, 46), IF(E2="2DSBanti", IF(H2="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{CCF6021C-1B60-4954-A92E-3F2848564215}" name="file_in" dataDxfId="199">
+    <tableColumn id="9" xr3:uid="{CCF6021C-1B60-4954-A92E-3F2848564215}" name="file_in" dataDxfId="197">
       <calculatedColumnFormula>IF(OR(table_1[[#This Row],[control]]="none", table_1[[#This Row],[control]]="30bpDown"), _xlfn.CONCAT(table_1[[#This Row],[library]], IF(table_1[[#This Row],[dsb_type]] = "2DSBanti", "_anti", ""), "_",table_1[[#This Row],[strand]],"_", IF(LEFT(table_1[[#This Row],[dsb_type]], 1)="2","2DSBs", table_1[[#This Row],[hguide]]), ".sam"), _xlfn.CONCAT(table_1[[#This Row],[library]], "_NHEJ_", IF(table_1[[#This Row],[hguide]]="sgA", "hg39", IF(table_1[[#This Row],[hguide]]="sgB", "hg42", "2DSB")), "_", table_1[[#This Row],[strand]], ".sam"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{58220462-2A11-4DAD-A247-C0871AFCFDB4}" name="file_out" dataDxfId="198">
+    <tableColumn id="10" xr3:uid="{58220462-2A11-4DAD-A247-C0871AFCFDB4}" name="file_out" dataDxfId="196">
       <calculatedColumnFormula>_xlfn.CONCAT(table_1[[#This Row],[library]], "_", table_1[[#This Row],[cell]], "_", table_1[[#This Row],[hguide]], "_", table_1[[#This Row],[strand]], "_", table_1[[#This Row],[treatment]], IF(table_1[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_1[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{775EE7A9-3C78-4568-BF98-500DE451177C}" name="ref" dataDxfId="197">
+    <tableColumn id="11" xr3:uid="{775EE7A9-3C78-4568-BF98-500DE451177C}" name="ref" dataDxfId="195">
       <calculatedColumnFormula>_xlfn.CONCAT(table_1[[#This Row],[dsb_type]],"_", table_1[[#This Row],[strand]],"_", table_1[[#This Row],[treatment]], ".fa")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{5B945FB6-D054-40C4-AAEF-BB50B19F8936}" name="total_reads" dataDxfId="161">
+    <tableColumn id="12" xr3:uid="{5B945FB6-D054-40C4-AAEF-BB50B19F8936}" name="total_reads" dataDxfId="194">
       <calculatedColumnFormula>VLOOKUP(INT(MID(table_1[[#This Row],[library]], 4, 10)), table_1_2[#All], IF(table_1[[#This Row],[strand]]="R1", 3, 4))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{66485B06-471E-47D3-BA91-FC751F58FA5A}" name="min_length" dataDxfId="196">
+    <tableColumn id="13" xr3:uid="{66485B06-471E-47D3-BA91-FC751F58FA5A}" name="min_length" dataDxfId="193">
       <calculatedColumnFormula>IF(LEFT(table_1[[#This Row],[dsb_type]], 1) = "2", 50, 130)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{DF3C46EA-690D-4E6A-99CF-BBC2B2F74AFF}" name="command_filter_nhej" dataDxfId="174">
+    <tableColumn id="14" xr3:uid="{DF3C46EA-690D-4E6A-99CF-BBC2B2F74AFF}" name="command_filter_nhej" dataDxfId="192">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", table_1[[#This Row],[file_in]], " -ref ref_seq/", table_1[[#This Row],[ref]], " -o ", libraries_2, "/", table_1[[#This Row],[file_out]], ".tsv", " --min_length ", table_1[[#This Row],[min_length]], " -dsb ", table_1[[#This Row],[dsb_pos]], " --quiet")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2427,38 +2427,38 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}" name="table_2_1" displayName="table_2_1" ref="A1:S41" totalsRowShown="0" headerRowDxfId="195">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}" name="table_2_1" displayName="table_2_1" ref="A1:S41" totalsRowShown="0" headerRowDxfId="191">
   <autoFilter ref="A1:S41" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{C373869E-A92E-4B06-B8E5-C5A873420ED4}" name="index" dataDxfId="194"/>
-    <tableColumn id="2" xr3:uid="{A28AAC50-FA09-494A-B052-8489F07A5A70}" name="ref" dataDxfId="126">
+    <tableColumn id="1" xr3:uid="{C373869E-A92E-4B06-B8E5-C5A873420ED4}" name="index" dataDxfId="190"/>
+    <tableColumn id="2" xr3:uid="{A28AAC50-FA09-494A-B052-8489F07A5A70}" name="ref" dataDxfId="189">
       <calculatedColumnFormula>OFFSET(table_1[ref], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{07D57089-9737-4983-8884-C4ACCDCFF6CB}" name="control" dataDxfId="125">
+    <tableColumn id="18" xr3:uid="{07D57089-9737-4983-8884-C4ACCDCFF6CB}" name="control" dataDxfId="188">
       <calculatedColumnFormula>OFFSET(table_1[control], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{C6423FEA-272F-48D3-BC6A-909FCA937DA9}" name="dsb_type" dataDxfId="124">
+    <tableColumn id="19" xr3:uid="{C6423FEA-272F-48D3-BC6A-909FCA937DA9}" name="dsb_type" dataDxfId="187">
       <calculatedColumnFormula>OFFSET(table_1[dsb_type], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B8F61088-5FFA-4860-BF4E-1BFB301A31D9}" name="dsb_pos" dataDxfId="123">
+    <tableColumn id="3" xr3:uid="{B8F61088-5FFA-4860-BF4E-1BFB301A31D9}" name="dsb_pos" dataDxfId="186">
       <calculatedColumnFormula>OFFSET(table_1[dsb_pos], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{524D5B3D-BB20-420D-B7E9-93A7F77CA728}" name="cell" dataDxfId="122">
+    <tableColumn id="4" xr3:uid="{524D5B3D-BB20-420D-B7E9-93A7F77CA728}" name="cell" dataDxfId="185">
       <calculatedColumnFormula>OFFSET(table_1[cell], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{CC918D20-5D79-4223-9717-2CA0EFFA213F}" name="strand" dataDxfId="121">
+    <tableColumn id="5" xr3:uid="{CC918D20-5D79-4223-9717-2CA0EFFA213F}" name="strand" dataDxfId="184">
       <calculatedColumnFormula>OFFSET(table_1[strand], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B2851465-D533-4787-80C4-E844BB2ABB8C}" name="treatment" dataDxfId="120">
+    <tableColumn id="6" xr3:uid="{B2851465-D533-4787-80C4-E844BB2ABB8C}" name="treatment" dataDxfId="183">
       <calculatedColumnFormula>OFFSET(table_1[treatment], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{849BE448-7739-4815-A2C5-5843F62D83D7}" name="hguide" dataDxfId="119">
+    <tableColumn id="7" xr3:uid="{849BE448-7739-4815-A2C5-5843F62D83D7}" name="hguide" dataDxfId="182">
       <calculatedColumnFormula>OFFSET(table_1[hguide], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{343716D9-C3A9-4F90-A58A-42B1B9C79EBF}" name="output_dir" dataDxfId="186">
+    <tableColumn id="8" xr3:uid="{343716D9-C3A9-4F90-A58A-42B1B9C79EBF}" name="output_dir" dataDxfId="181">
       <calculatedColumnFormula>_xlfn.CONCAT(table_2_1[[#This Row],[cell]], "_", table_2_1[[#This Row],[hguide]], "_", table_2_1[[#This Row],[strand]], "_", table_2_1[[#This Row],[treatment]], IF(table_2_1[[#This Row],[control]]&lt;&gt;"none",_xlfn.CONCAT("_", table_2_1[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D29558AA-D418-4CDD-81AE-A987E7BC501D}" name="input_1" dataDxfId="118">
+    <tableColumn id="9" xr3:uid="{D29558AA-D418-4CDD-81AE-A987E7BC501D}" name="input_1" dataDxfId="180">
       <calculatedColumnFormula array="1">OFFSET(table_1[[file_out]:[file_out]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 11, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="22" xr3:uid="{3F29C0D1-58A3-430E-AAAA-9F679DCA46D6}" name="input_2">
@@ -2470,19 +2470,19 @@
     <tableColumn id="20" xr3:uid="{28521A62-94B3-4C7C-AF90-F4E2F4163D29}" name="input_4">
       <calculatedColumnFormula array="1">OFFSET(table_1[[file_out]:[file_out]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 11, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{E2ABF5A3-B032-47F7-9141-9F269EFD9D49}" name="total_reads_1" dataDxfId="117">
+    <tableColumn id="10" xr3:uid="{E2ABF5A3-B032-47F7-9141-9F269EFD9D49}" name="total_reads_1" dataDxfId="179">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{C7B1BE14-3BD6-413B-8575-DE9712F9761A}" name="total_reads_2" dataDxfId="193">
+    <tableColumn id="12" xr3:uid="{C7B1BE14-3BD6-413B-8575-DE9712F9761A}" name="total_reads_2" dataDxfId="178">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{6A8CE344-45B9-42E3-95D8-8EB6A485D968}" name="total_reads_3" dataDxfId="192">
+    <tableColumn id="14" xr3:uid="{6A8CE344-45B9-42E3-95D8-8EB6A485D968}" name="total_reads_3" dataDxfId="177">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{AC170216-9CAE-43B8-A8E2-8FE1529F6D55}" name="total_reads_4" dataDxfId="191">
+    <tableColumn id="16" xr3:uid="{AC170216-9CAE-43B8-A8E2-8FE1529F6D55}" name="total_reads_4" dataDxfId="176">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{A285A0DD-6F6D-404D-AE2A-0D1FC3DDB459}" name="command" dataDxfId="116">
+    <tableColumn id="17" xr3:uid="{A285A0DD-6F6D-404D-AE2A-0D1FC3DDB459}" name="command" dataDxfId="175">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2494,41 +2494,41 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{7D969AC7-2D2F-45B0-BA99-D174130B0A52}" name="table_2_2" displayName="table_2_2" ref="A44:M56" totalsRowShown="0">
   <autoFilter ref="A44:M56" xr:uid="{7D969AC7-2D2F-45B0-BA99-D174130B0A52}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{D612E3DF-AA8E-4EE0-9306-7903B4821992}" name="index" dataDxfId="182"/>
-    <tableColumn id="2" xr3:uid="{B00239B6-16E0-4472-B8C9-F25D625D21DD}" name="ref" dataDxfId="114">
+    <tableColumn id="1" xr3:uid="{D612E3DF-AA8E-4EE0-9306-7903B4821992}" name="index" dataDxfId="174"/>
+    <tableColumn id="2" xr3:uid="{B00239B6-16E0-4472-B8C9-F25D625D21DD}" name="ref" dataDxfId="173">
       <calculatedColumnFormula>OFFSET(table_1[ref], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{47FE94A7-C208-4138-B063-127D4AE215A0}" name="control" dataDxfId="113">
+    <tableColumn id="3" xr3:uid="{47FE94A7-C208-4138-B063-127D4AE215A0}" name="control" dataDxfId="172">
       <calculatedColumnFormula>OFFSET(table_1[control], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{43B4F550-AB35-4206-AAAB-820BBA723DEA}" name="dsb_type" dataDxfId="112">
+    <tableColumn id="4" xr3:uid="{43B4F550-AB35-4206-AAAB-820BBA723DEA}" name="dsb_type" dataDxfId="171">
       <calculatedColumnFormula>OFFSET(table_1[dsb_type], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7233C674-8249-48C9-814C-599A94DF6097}" name="dsb_pos" dataDxfId="111">
+    <tableColumn id="5" xr3:uid="{7233C674-8249-48C9-814C-599A94DF6097}" name="dsb_pos" dataDxfId="170">
       <calculatedColumnFormula>OFFSET(table_1[dsb_pos], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8FD419DF-3888-4BC8-ACF7-F31E7AB24754}" name="cell" dataDxfId="110">
+    <tableColumn id="6" xr3:uid="{8FD419DF-3888-4BC8-ACF7-F31E7AB24754}" name="cell" dataDxfId="169">
       <calculatedColumnFormula>OFFSET(table_1[cell], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{612FF909-1004-49E1-BC8F-F65A8C97EEFC}" name="strand" dataDxfId="109">
+    <tableColumn id="7" xr3:uid="{612FF909-1004-49E1-BC8F-F65A8C97EEFC}" name="strand" dataDxfId="168">
       <calculatedColumnFormula>OFFSET(table_1[strand], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C57AB4D7-F308-46D6-8F19-069619F8CF1B}" name="treatment" dataDxfId="108">
+    <tableColumn id="8" xr3:uid="{C57AB4D7-F308-46D6-8F19-069619F8CF1B}" name="treatment" dataDxfId="167">
       <calculatedColumnFormula>OFFSET(table_1[treatment], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{27DAC4C9-BDB2-4621-A4F1-0094D063284E}" name="hguide" dataDxfId="107">
+    <tableColumn id="9" xr3:uid="{27DAC4C9-BDB2-4621-A4F1-0094D063284E}" name="hguide" dataDxfId="166">
       <calculatedColumnFormula>OFFSET(table_1[hguide], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{E0E9E8C1-4E85-4EFB-8220-84140FBAAF8E}" name="output_dir" dataDxfId="106">
+    <tableColumn id="10" xr3:uid="{E0E9E8C1-4E85-4EFB-8220-84140FBAAF8E}" name="output_dir" dataDxfId="165">
       <calculatedColumnFormula>_xlfn.CONCAT(table_2_2[[#This Row],[cell]], "_", table_2_2[[#This Row],[hguide]], "_", table_2_2[[#This Row],[strand]], "_", table_2_2[[#This Row],[treatment]], "_nodsb")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{CAC474F1-3930-4766-B491-65C86C5752E8}" name="input" dataDxfId="105">
+    <tableColumn id="11" xr3:uid="{CAC474F1-3930-4766-B491-65C86C5752E8}" name="input" dataDxfId="164">
       <calculatedColumnFormula>OFFSET(table_1[file_out], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{BB84920E-3487-4670-93ED-5671EACD3061}" name="total_reads" dataDxfId="104">
+    <tableColumn id="12" xr3:uid="{BB84920E-3487-4670-93ED-5671EACD3061}" name="total_reads" dataDxfId="163">
       <calculatedColumnFormula>OFFSET(table_1[total_reads], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{0CE6DAF6-0C4C-4EC5-8FE5-9B3840A02412}" name="command" dataDxfId="173">
+    <tableColumn id="13" xr3:uid="{0CE6DAF6-0C4C-4EC5-8FE5-9B3840A02412}" name="command" dataDxfId="162">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_2[[#This Row],[input]], ".tsv ", " --total_reads ", table_2_2[[#This Row],[total_reads]], " -o ", libraries_3, "/", table_2_2[[#This Row],[output_dir]], ".tsv", " --quiet ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2537,47 +2537,47 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}" name="table_3_1" displayName="table_3_1" ref="A1:N41" totalsRowShown="0" headerRowDxfId="190">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}" name="table_3_1" displayName="table_3_1" ref="A1:N41" totalsRowShown="0" headerRowDxfId="161">
   <autoFilter ref="A1:N41" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}"/>
   <tableColumns count="14">
-    <tableColumn id="25" xr3:uid="{93D2F09B-24D5-4FE1-BF34-C037E361889F}" name="index" dataDxfId="189"/>
-    <tableColumn id="1" xr3:uid="{2F28DC66-449D-4F81-AA63-8F24B25F33D1}" name="dir" dataDxfId="149">
+    <tableColumn id="25" xr3:uid="{93D2F09B-24D5-4FE1-BF34-C037E361889F}" name="index" dataDxfId="160"/>
+    <tableColumn id="1" xr3:uid="{2F28DC66-449D-4F81-AA63-8F24B25F33D1}" name="dir" dataDxfId="159">
       <calculatedColumnFormula>OFFSET(table_2_1[output_dir], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{3DF6F698-1F9A-4B05-A310-657CCFCE9F66}" name="control" dataDxfId="148">
+    <tableColumn id="13" xr3:uid="{3DF6F698-1F9A-4B05-A310-657CCFCE9F66}" name="control" dataDxfId="158">
       <calculatedColumnFormula>OFFSET(table_2_1[control], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{362C2395-52F7-4A62-B7BA-2DD97ED5E6FB}" name="ref" dataDxfId="147">
+    <tableColumn id="2" xr3:uid="{362C2395-52F7-4A62-B7BA-2DD97ED5E6FB}" name="ref" dataDxfId="157">
       <calculatedColumnFormula>OFFSET(table_2_1[ref], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5F0895D9-2EF2-4524-8BC7-15A33FE68636}" name="dsb_pos" dataDxfId="146">
+    <tableColumn id="3" xr3:uid="{5F0895D9-2EF2-4524-8BC7-15A33FE68636}" name="dsb_pos" dataDxfId="156">
       <calculatedColumnFormula>OFFSET(table_2_1[dsb_pos], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C6D28829-46E6-4D97-8EA4-0AD12EF6CF10}" name="dsb_type" dataDxfId="145">
+    <tableColumn id="4" xr3:uid="{C6D28829-46E6-4D97-8EA4-0AD12EF6CF10}" name="dsb_type" dataDxfId="155">
       <calculatedColumnFormula>OFFSET(table_2_1[dsb_type], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{E8B2E211-C273-4602-86F0-60EA4259B7A4}" name="dsb_type_command" dataDxfId="188">
+    <tableColumn id="12" xr3:uid="{E8B2E211-C273-4602-86F0-60EA4259B7A4}" name="dsb_type_command" dataDxfId="154">
       <calculatedColumnFormula array="1">IF(table_3_1[[#This Row],[dsb_type]]="2DSB", "2", IF(table_3_1[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(table_3_1[[#This Row],[dsb_type]]="1DSB", "1", NA)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{15578E86-B7BE-4D8E-8FD4-E6C9C4F35C9C}" name="strand" dataDxfId="144">
+    <tableColumn id="5" xr3:uid="{15578E86-B7BE-4D8E-8FD4-E6C9C4F35C9C}" name="strand" dataDxfId="153">
       <calculatedColumnFormula>OFFSET(table_2_1[strand], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3366AC40-6578-4797-B607-19265E7DBF5C}" name="hguide" dataDxfId="143">
+    <tableColumn id="6" xr3:uid="{3366AC40-6578-4797-B607-19265E7DBF5C}" name="hguide" dataDxfId="152">
       <calculatedColumnFormula>MID(OFFSET(table_2_1[hguide], table_3_1[[#This Row],[index]] - 1, 0, 1, 1), 3, 100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{554F4E79-98DE-474B-A5C8-D4B536772E95}" name="cell" dataDxfId="142">
+    <tableColumn id="7" xr3:uid="{554F4E79-98DE-474B-A5C8-D4B536772E95}" name="cell" dataDxfId="151">
       <calculatedColumnFormula>OFFSET(table_2_1[cell], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{32FC5061-DD85-4234-9ED8-FEAF6D9E3BC0}" name="treatment" dataDxfId="141">
+    <tableColumn id="8" xr3:uid="{32FC5061-DD85-4234-9ED8-FEAF6D9E3BC0}" name="treatment" dataDxfId="150">
       <calculatedColumnFormula>OFFSET(table_2_1[treatment], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{DB6998A3-1431-4DDD-8DA0-525B805BF436}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{367B0912-E7A8-4430-962D-4F79EE14E5EA}" name="command_main_data" dataDxfId="167">
+    <tableColumn id="10" xr3:uid="{367B0912-E7A8-4430-962D-4F79EE14E5EA}" name="command_main_data" dataDxfId="149">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_1[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_1[[#This Row],[dir]], " -ref ref_seq/", table_3_1[[#This Row],[ref]], " -dsb ", table_3_1[[#This Row],[dsb_pos]], " --dsb_type ",table_3_1[[#This Row],[dsb_type_command]], " --strand ", table_3_1[[#This Row],[strand]], " --hguide ", table_3_1[[#This Row],[hguide]], " --cell ", table_3_1[[#This Row],[cell]], " --treatment ", table_3_1[[#This Row],[treatment]], " --subst_type ", table_3_1[[#This Row],[subst_type]], " --control ", table_3_1[[#This Row],[control]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{4A65279E-321E-4E3E-8383-26D448C2012F}" name="command_graph_data" dataDxfId="172">
+    <tableColumn id="11" xr3:uid="{4A65279E-321E-4E3E-8383-26D448C2012F}" name="command_graph_data" dataDxfId="148">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_1[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_1[[#This Row],[dir]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2586,47 +2586,47 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}" name="table_3_2" displayName="table_3_2" ref="A43:N55" totalsRowShown="0" headerRowDxfId="140">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}" name="table_3_2" displayName="table_3_2" ref="A43:N55" totalsRowShown="0" headerRowDxfId="147">
   <autoFilter ref="A43:N55" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}"/>
   <tableColumns count="14">
-    <tableColumn id="25" xr3:uid="{B2894846-EBB9-47DC-8DE1-7F1DA571A0B9}" name="index" dataDxfId="139"/>
-    <tableColumn id="1" xr3:uid="{98269DFC-71F0-4066-B063-59597431C1C3}" name="dir" dataDxfId="135">
+    <tableColumn id="25" xr3:uid="{B2894846-EBB9-47DC-8DE1-7F1DA571A0B9}" name="index" dataDxfId="146"/>
+    <tableColumn id="1" xr3:uid="{98269DFC-71F0-4066-B063-59597431C1C3}" name="dir" dataDxfId="145">
       <calculatedColumnFormula>OFFSET(table_2_2[output_dir], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{EB55B964-D8E2-4E0C-B7CF-07043E026664}" name="control" dataDxfId="134">
+    <tableColumn id="13" xr3:uid="{EB55B964-D8E2-4E0C-B7CF-07043E026664}" name="control" dataDxfId="144">
       <calculatedColumnFormula>OFFSET(table_2_2[control], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{7A83EC55-03CE-4608-92D6-6F1C53B539FE}" name="ref" dataDxfId="133">
+    <tableColumn id="2" xr3:uid="{7A83EC55-03CE-4608-92D6-6F1C53B539FE}" name="ref" dataDxfId="143">
       <calculatedColumnFormula>OFFSET(table_2_2[ref], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{13E984FC-9FD2-479F-AB4C-B74DDF5FD234}" name="dsb_pos" dataDxfId="132">
+    <tableColumn id="3" xr3:uid="{13E984FC-9FD2-479F-AB4C-B74DDF5FD234}" name="dsb_pos" dataDxfId="142">
       <calculatedColumnFormula>OFFSET(table_2_2[dsb_pos], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{EF0F2447-2FA1-4517-A5CE-D8DDAAC8D3F2}" name="dsb_type" dataDxfId="131">
+    <tableColumn id="4" xr3:uid="{EF0F2447-2FA1-4517-A5CE-D8DDAAC8D3F2}" name="dsb_type" dataDxfId="141">
       <calculatedColumnFormula>OFFSET(table_2_2[dsb_type], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A1849AE1-952B-42B5-99EE-20BD2E4C5A6A}" name="dsb_type_command" dataDxfId="138">
+    <tableColumn id="12" xr3:uid="{A1849AE1-952B-42B5-99EE-20BD2E4C5A6A}" name="dsb_type_command" dataDxfId="140">
       <calculatedColumnFormula array="1">IF(table_3_2[[#This Row],[dsb_type]]="2DSB", "2", IF(table_3_2[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(table_3_2[[#This Row],[dsb_type]]="1DSB", "1", NA)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{625E12FC-BF17-4E65-99DB-EDD53FEF055D}" name="strand" dataDxfId="130">
+    <tableColumn id="5" xr3:uid="{625E12FC-BF17-4E65-99DB-EDD53FEF055D}" name="strand" dataDxfId="139">
       <calculatedColumnFormula>OFFSET(table_2_2[strand], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0ABF747E-328F-4A80-85AA-4AF871C860C1}" name="hguide" dataDxfId="129">
+    <tableColumn id="6" xr3:uid="{0ABF747E-328F-4A80-85AA-4AF871C860C1}" name="hguide" dataDxfId="138">
       <calculatedColumnFormula>MID(OFFSET(table_2_2[hguide], table_3_2[[#This Row],[index]] - 1, 0, 1, 1), 3, 100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{29D6C48B-05B8-42C6-88A9-0939BC454FE0}" name="cell" dataDxfId="128">
+    <tableColumn id="7" xr3:uid="{29D6C48B-05B8-42C6-88A9-0939BC454FE0}" name="cell" dataDxfId="137">
       <calculatedColumnFormula>OFFSET(table_2_2[cell], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{BD269EBE-94A9-4B57-B984-C7566AC259DE}" name="treatment" dataDxfId="127">
+    <tableColumn id="8" xr3:uid="{BD269EBE-94A9-4B57-B984-C7566AC259DE}" name="treatment" dataDxfId="136">
       <calculatedColumnFormula>OFFSET(table_2_2[treatment], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{142C480D-E258-4979-A008-3940A3FE78E4}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{19804410-83AB-479E-A819-2D7449105C25}" name="command_main_data" dataDxfId="137">
+    <tableColumn id="10" xr3:uid="{19804410-83AB-479E-A819-2D7449105C25}" name="command_main_data" dataDxfId="135">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_2[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_2[[#This Row],[dir]], " -ref ref_seq/", table_3_2[[#This Row],[ref]], " -dsb ", table_3_2[[#This Row],[dsb_pos]], " --dsb_type ",table_3_2[[#This Row],[dsb_type_command]], " --strand ", table_3_2[[#This Row],[strand]], " --hguide ", table_3_2[[#This Row],[hguide]], " --cell ", table_3_2[[#This Row],[cell]], " --treatment ", table_3_2[[#This Row],[treatment]], " --subst_type ", table_3_2[[#This Row],[subst_type]], " --control ", table_3_2[[#This Row],[control]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{212A69BD-0F88-401C-957F-8B6EC8E55AED}" name="command_graph_data" dataDxfId="136">
+    <tableColumn id="11" xr3:uid="{212A69BD-0F88-401C-957F-8B6EC8E55AED}" name="command_graph_data" dataDxfId="134">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_2[[#This Row],[dir]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2635,38 +2635,38 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}" name="table_4_1" displayName="table_4_1" ref="A1:K17" totalsRowShown="0" headerRowDxfId="187">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}" name="table_4_1" displayName="table_4_1" ref="A1:K17" totalsRowShown="0" headerRowDxfId="133">
   <autoFilter ref="A1:K17" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B7EC223D-BA24-48F1-9EE3-DC56DEFDE4C2}" name="index" dataDxfId="185"/>
-    <tableColumn id="7" xr3:uid="{D9F1ADDA-18A2-4F81-862D-6B0F786079FF}" name="control" dataDxfId="50">
+    <tableColumn id="1" xr3:uid="{B7EC223D-BA24-48F1-9EE3-DC56DEFDE4C2}" name="index" dataDxfId="132"/>
+    <tableColumn id="7" xr3:uid="{D9F1ADDA-18A2-4F81-862D-6B0F786079FF}" name="control" dataDxfId="131">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{0EA5A81F-6EA1-4256-9717-03273165F7BF}" name="treatment_1" dataDxfId="157">
+    <tableColumn id="8" xr3:uid="{0EA5A81F-6EA1-4256-9717-03273165F7BF}" name="treatment_1" dataDxfId="130">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5F6D005A-96D8-4801-93E2-101BAE551BA8}" name="dir_1" dataDxfId="159">
+    <tableColumn id="2" xr3:uid="{5F6D005A-96D8-4801-93E2-101BAE551BA8}" name="dir_1" dataDxfId="129">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C21D1AF7-7ABE-4181-AA2A-42227869A8DD}" name="treatment_2" dataDxfId="150">
+    <tableColumn id="9" xr3:uid="{C21D1AF7-7ABE-4181-AA2A-42227869A8DD}" name="treatment_2" dataDxfId="128">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{D66426AC-E0B2-4B07-A4D4-5A74AA033E80}" name="dir_2" dataDxfId="158">
+    <tableColumn id="3" xr3:uid="{D66426AC-E0B2-4B07-A4D4-5A74AA033E80}" name="dir_2" dataDxfId="127">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{0C8146A0-DC77-4DC4-82FF-74F4C74CF33E}" name="treatments_out" dataDxfId="179">
+    <tableColumn id="10" xr3:uid="{0C8146A0-DC77-4DC4-82FF-74F4C74CF33E}" name="treatments_out" dataDxfId="126">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_1[[#This Row],[treatment_1]], "_", table_4_1[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{519A6397-7A3C-4009-B8B9-A71C0B3A591B}" name="dir_out" dataDxfId="178">
+    <tableColumn id="4" xr3:uid="{519A6397-7A3C-4009-B8B9-A71C0B3A591B}" name="dir_out" dataDxfId="125">
       <calculatedColumnFormula>SUBSTITUTE(table_4_1[[#This Row],[dir_1]], table_4_1[[#This Row],[treatment_1]], table_4_1[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E1629355-7D02-4819-98A1-EEB3B5FADE18}" name="subst_type" dataDxfId="175">
+    <tableColumn id="5" xr3:uid="{E1629355-7D02-4819-98A1-EEB3B5FADE18}" name="subst_type" dataDxfId="124">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{BC9117A0-CB6F-4D3C-A0E4-BF8395854D9A}" name="command_main_data_combined" dataDxfId="171">
+    <tableColumn id="6" xr3:uid="{BC9117A0-CB6F-4D3C-A0E4-BF8395854D9A}" name="command_main_data_combined" dataDxfId="123">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_1[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_1[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_1[[#This Row],[dir_out]], " --subst_type ", table_4_1[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{D384013E-9937-4DD8-A36A-43325757359B}" name="command_graph_data" dataDxfId="0">
+    <tableColumn id="11" xr3:uid="{D384013E-9937-4DD8-A36A-43325757359B}" name="command_graph_data" dataDxfId="122">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_1[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_1[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2675,38 +2675,38 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}" name="table_4_2" displayName="table_4_2" ref="A20:K22" totalsRowShown="0" headerRowDxfId="184">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}" name="table_4_2" displayName="table_4_2" ref="A20:K22" totalsRowShown="0" headerRowDxfId="121">
   <autoFilter ref="A20:K22" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{7F5A3A15-751D-407C-A035-61B2605E693F}" name="index" dataDxfId="183"/>
-    <tableColumn id="7" xr3:uid="{45863AB0-FD32-49FE-B4BF-F8EE865F7604}" name="control" dataDxfId="49">
+    <tableColumn id="1" xr3:uid="{7F5A3A15-751D-407C-A035-61B2605E693F}" name="index" dataDxfId="120"/>
+    <tableColumn id="7" xr3:uid="{45863AB0-FD32-49FE-B4BF-F8EE865F7604}" name="control" dataDxfId="119">
       <calculatedColumnFormula>OFFSET(table_3_1[control], var_4_anti_offset + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{CD16648D-267E-410B-A366-3E12367C037C}" name="treatment_1" dataDxfId="11">
+    <tableColumn id="8" xr3:uid="{CD16648D-267E-410B-A366-3E12367C037C}" name="treatment_1" dataDxfId="118">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{10C9F90E-86FD-4BFE-939E-298FD6F69F12}" name="dir_1" dataDxfId="10">
+    <tableColumn id="2" xr3:uid="{10C9F90E-86FD-4BFE-939E-298FD6F69F12}" name="dir_1" dataDxfId="117">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{7AB3E4AB-F43B-4FDE-96D7-FBBB4A8B83BE}" name="treatment_2" dataDxfId="9">
+    <tableColumn id="9" xr3:uid="{7AB3E4AB-F43B-4FDE-96D7-FBBB4A8B83BE}" name="treatment_2" dataDxfId="116">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1) + 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BF948A3E-9649-41BF-A7E7-57BFDE810FE9}" name="dir_2" dataDxfId="8">
+    <tableColumn id="3" xr3:uid="{BF948A3E-9649-41BF-A7E7-57BFDE810FE9}" name="dir_2" dataDxfId="115">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1) + 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{378119E5-F021-4785-A653-4D632F029AA6}" name="treatments_out" dataDxfId="180">
+    <tableColumn id="10" xr3:uid="{378119E5-F021-4785-A653-4D632F029AA6}" name="treatments_out" dataDxfId="114">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_2[[#This Row],[treatment_1]], "_", table_4_2[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AE1A14DC-D0C9-4818-B8CC-09A571E73BC2}" name="dir_out" dataDxfId="181">
+    <tableColumn id="4" xr3:uid="{AE1A14DC-D0C9-4818-B8CC-09A571E73BC2}" name="dir_out" dataDxfId="113">
       <calculatedColumnFormula>SUBSTITUTE(table_4_2[[#This Row],[dir_1]], table_4_2[[#This Row],[treatment_1]], table_4_2[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{F29DAC4E-FEC5-4C1D-AAC1-7CE19E401F25}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{DC4E99F4-97AB-4553-A5FB-D20D3D487947}" name="command_main_data_combined" dataDxfId="170">
+    <tableColumn id="6" xr3:uid="{DC4E99F4-97AB-4553-A5FB-D20D3D487947}" name="command_main_data_combined" dataDxfId="112">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_2[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_2[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_2[[#This Row],[dir_out]], " --subst_type ", table_4_2[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{E19D3001-2E76-4CC2-BF33-D0465C77D538}" name="command_graph_data" dataDxfId="2">
+    <tableColumn id="11" xr3:uid="{E19D3001-2E76-4CC2-BF33-D0465C77D538}" name="command_graph_data" dataDxfId="111">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_2[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2715,38 +2715,38 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}" name="table_4_3" displayName="table_4_3" ref="A25:K33" totalsRowShown="0" headerRowDxfId="156">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}" name="table_4_3" displayName="table_4_3" ref="A25:K33" totalsRowShown="0" headerRowDxfId="110">
   <autoFilter ref="A25:K33" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{33AF3495-7432-4F03-9832-525A370EADEC}" name="index" dataDxfId="155"/>
-    <tableColumn id="7" xr3:uid="{3D66515C-5022-4D48-A834-4320DA4E73F6}" name="control" dataDxfId="100">
+    <tableColumn id="1" xr3:uid="{33AF3495-7432-4F03-9832-525A370EADEC}" name="index" dataDxfId="109"/>
+    <tableColumn id="7" xr3:uid="{3D66515C-5022-4D48-A834-4320DA4E73F6}" name="control" dataDxfId="108">
       <calculatedColumnFormula>OFFSET(table_3_2[control], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{294B17A9-F0F9-42CA-8342-55C00648E3A5}" name="treatment_1" dataDxfId="103">
+    <tableColumn id="8" xr3:uid="{294B17A9-F0F9-42CA-8342-55C00648E3A5}" name="treatment_1" dataDxfId="107">
       <calculatedColumnFormula>OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E13C38CF-C105-4AB5-8602-7D32E688C737}" name="dir_1" dataDxfId="102">
+    <tableColumn id="2" xr3:uid="{E13C38CF-C105-4AB5-8602-7D32E688C737}" name="dir_1" dataDxfId="106">
       <calculatedColumnFormula>OFFSET(table_3_2[dir], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{15B3CC7F-2A3C-4026-8417-A9DD21E4F004}" name="treatment_2" dataDxfId="48">
+    <tableColumn id="9" xr3:uid="{15B3CC7F-2A3C-4026-8417-A9DD21E4F004}" name="treatment_2" dataDxfId="105">
       <calculatedColumnFormula>OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{FF7D9AD3-1A35-4013-88AE-0C00465033CD}" name="dir_2" dataDxfId="101">
+    <tableColumn id="3" xr3:uid="{FF7D9AD3-1A35-4013-88AE-0C00465033CD}" name="dir_2" dataDxfId="104">
       <calculatedColumnFormula>OFFSET(table_3_2[dir], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{9353B2D3-0D23-4FBB-AFEC-EB68549160F4}" name="treatments_out" dataDxfId="154">
+    <tableColumn id="10" xr3:uid="{9353B2D3-0D23-4FBB-AFEC-EB68549160F4}" name="treatments_out" dataDxfId="103">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_3[[#This Row],[treatment_1]], "_", table_4_3[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{77F1D6F0-DE95-4E63-9E7E-D3CA3CF85F37}" name="dir_out" dataDxfId="153">
+    <tableColumn id="4" xr3:uid="{77F1D6F0-DE95-4E63-9E7E-D3CA3CF85F37}" name="dir_out" dataDxfId="102">
       <calculatedColumnFormula>SUBSTITUTE(table_4_3[[#This Row],[dir_1]], table_4_3[[#This Row],[treatment_1]], table_4_3[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{BBF4F840-178E-461E-8C17-36D699EDE038}" name="subst_type" dataDxfId="152">
+    <tableColumn id="5" xr3:uid="{BBF4F840-178E-461E-8C17-36D699EDE038}" name="subst_type" dataDxfId="101">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9434BF8B-81C5-43DF-BCB7-FA7146BF2FE8}" name="command_main_data_combined" dataDxfId="151">
+    <tableColumn id="6" xr3:uid="{9434BF8B-81C5-43DF-BCB7-FA7146BF2FE8}" name="command_main_data_combined" dataDxfId="100">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_3[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_3[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_3[[#This Row],[dir_out]], " --subst_type ", table_4_3[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{1ABF0B7B-4ECE-42BF-A7D8-EA13E98144EE}" name="command_graph_data" dataDxfId="1">
+    <tableColumn id="11" xr3:uid="{1ABF0B7B-4ECE-42BF-A7D8-EA13E98144EE}" name="command_graph_data" dataDxfId="99">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_3[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_3[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3115,7 +3115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DFB1CC9-23C4-4E30-93CF-6F31CFACE92F}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -18500,7 +18500,7 @@
         <v>sense</v>
       </c>
       <c r="L2" t="str">
-        <f>subst_type</f>
+        <f t="shared" ref="L2:L41" si="0">subst_type</f>
         <v>without</v>
       </c>
       <c r="M2" t="str">
@@ -18557,7 +18557,7 @@
         <v>branch</v>
       </c>
       <c r="L3" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M3" t="str">
@@ -18614,7 +18614,7 @@
         <v>cmv</v>
       </c>
       <c r="L4" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M4" t="str">
@@ -18671,7 +18671,7 @@
         <v>sense</v>
       </c>
       <c r="L5" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M5" t="str">
@@ -18728,7 +18728,7 @@
         <v>branch</v>
       </c>
       <c r="L6" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M6" t="str">
@@ -18785,7 +18785,7 @@
         <v>cmv</v>
       </c>
       <c r="L7" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M7" t="str">
@@ -18842,7 +18842,7 @@
         <v>sense</v>
       </c>
       <c r="L8" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M8" t="str">
@@ -18899,7 +18899,7 @@
         <v>branch</v>
       </c>
       <c r="L9" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M9" t="str">
@@ -18956,7 +18956,7 @@
         <v>cmv</v>
       </c>
       <c r="L10" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M10" t="str">
@@ -19013,7 +19013,7 @@
         <v>sense</v>
       </c>
       <c r="L11" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M11" t="str">
@@ -19070,7 +19070,7 @@
         <v>branch</v>
       </c>
       <c r="L12" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M12" t="str">
@@ -19127,7 +19127,7 @@
         <v>cmv</v>
       </c>
       <c r="L13" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M13" t="str">
@@ -19184,7 +19184,7 @@
         <v>sense</v>
       </c>
       <c r="L14" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M14" t="str">
@@ -19241,7 +19241,7 @@
         <v>branch</v>
       </c>
       <c r="L15" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M15" t="str">
@@ -19298,7 +19298,7 @@
         <v>cmv</v>
       </c>
       <c r="L16" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M16" t="str">
@@ -19355,7 +19355,7 @@
         <v>sense</v>
       </c>
       <c r="L17" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M17" t="str">
@@ -19412,7 +19412,7 @@
         <v>branch</v>
       </c>
       <c r="L18" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M18" t="str">
@@ -19469,7 +19469,7 @@
         <v>cmv</v>
       </c>
       <c r="L19" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M19" t="str">
@@ -19526,7 +19526,7 @@
         <v>sense</v>
       </c>
       <c r="L20" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M20" t="str">
@@ -19583,7 +19583,7 @@
         <v>branch</v>
       </c>
       <c r="L21" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M21" t="str">
@@ -19640,7 +19640,7 @@
         <v>cmv</v>
       </c>
       <c r="L22" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M22" t="str">
@@ -19697,7 +19697,7 @@
         <v>sense</v>
       </c>
       <c r="L23" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M23" t="str">
@@ -19754,7 +19754,7 @@
         <v>branch</v>
       </c>
       <c r="L24" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M24" t="str">
@@ -19811,7 +19811,7 @@
         <v>cmv</v>
       </c>
       <c r="L25" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M25" t="str">
@@ -19868,7 +19868,7 @@
         <v>sense</v>
       </c>
       <c r="L26" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M26" t="str">
@@ -19925,7 +19925,7 @@
         <v>branch</v>
       </c>
       <c r="L27" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M27" t="str">
@@ -19982,7 +19982,7 @@
         <v>cmv</v>
       </c>
       <c r="L28" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M28" t="str">
@@ -20039,7 +20039,7 @@
         <v>sense</v>
       </c>
       <c r="L29" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M29" t="str">
@@ -20096,7 +20096,7 @@
         <v>branch</v>
       </c>
       <c r="L30" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M30" t="str">
@@ -20153,7 +20153,7 @@
         <v>cmv</v>
       </c>
       <c r="L31" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M31" t="str">
@@ -20210,7 +20210,7 @@
         <v>sense</v>
       </c>
       <c r="L32" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M32" t="str">
@@ -20267,7 +20267,7 @@
         <v>branch</v>
       </c>
       <c r="L33" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M33" t="str">
@@ -20324,7 +20324,7 @@
         <v>cmv</v>
       </c>
       <c r="L34" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M34" t="str">
@@ -20381,7 +20381,7 @@
         <v>sense</v>
       </c>
       <c r="L35" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M35" t="str">
@@ -20438,7 +20438,7 @@
         <v>branch</v>
       </c>
       <c r="L36" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M36" t="str">
@@ -20495,7 +20495,7 @@
         <v>cmv</v>
       </c>
       <c r="L37" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M37" t="str">
@@ -20552,7 +20552,7 @@
         <v>antisense</v>
       </c>
       <c r="L38" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M38" t="str">
@@ -20609,7 +20609,7 @@
         <v>splicing</v>
       </c>
       <c r="L39" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M39" t="str">
@@ -20666,7 +20666,7 @@
         <v>antisense</v>
       </c>
       <c r="L40" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M40" t="str">
@@ -20723,7 +20723,7 @@
         <v>splicing</v>
       </c>
       <c r="L41" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="M41" t="str">
@@ -20824,7 +20824,7 @@
         <v>sense</v>
       </c>
       <c r="L44" t="str">
-        <f>subst_type</f>
+        <f t="shared" ref="L44:L55" si="1">subst_type</f>
         <v>without</v>
       </c>
       <c r="M44" t="str">
@@ -20881,7 +20881,7 @@
         <v>branch</v>
       </c>
       <c r="L45" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="1"/>
         <v>without</v>
       </c>
       <c r="M45" t="str">
@@ -20938,7 +20938,7 @@
         <v>cmv</v>
       </c>
       <c r="L46" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="1"/>
         <v>without</v>
       </c>
       <c r="M46" t="str">
@@ -20995,7 +20995,7 @@
         <v>sense</v>
       </c>
       <c r="L47" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="1"/>
         <v>without</v>
       </c>
       <c r="M47" t="str">
@@ -21052,7 +21052,7 @@
         <v>branch</v>
       </c>
       <c r="L48" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="1"/>
         <v>without</v>
       </c>
       <c r="M48" t="str">
@@ -21109,7 +21109,7 @@
         <v>cmv</v>
       </c>
       <c r="L49" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="1"/>
         <v>without</v>
       </c>
       <c r="M49" t="str">
@@ -21166,7 +21166,7 @@
         <v>sense</v>
       </c>
       <c r="L50" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="1"/>
         <v>without</v>
       </c>
       <c r="M50" t="str">
@@ -21223,7 +21223,7 @@
         <v>branch</v>
       </c>
       <c r="L51" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="1"/>
         <v>without</v>
       </c>
       <c r="M51" t="str">
@@ -21280,7 +21280,7 @@
         <v>cmv</v>
       </c>
       <c r="L52" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="1"/>
         <v>without</v>
       </c>
       <c r="M52" t="str">
@@ -21337,7 +21337,7 @@
         <v>sense</v>
       </c>
       <c r="L53" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="1"/>
         <v>without</v>
       </c>
       <c r="M53" t="str">
@@ -21394,7 +21394,7 @@
         <v>branch</v>
       </c>
       <c r="L54" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="1"/>
         <v>without</v>
       </c>
       <c r="M54" t="str">
@@ -21451,7 +21451,7 @@
         <v>cmv</v>
       </c>
       <c r="L55" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="1"/>
         <v>without</v>
       </c>
       <c r="M55" t="str">
@@ -21564,7 +21564,7 @@
         <v>WT_sgAB_R1_sense_branch</v>
       </c>
       <c r="I2" t="str">
-        <f>subst_type</f>
+        <f t="shared" ref="I2:I17" si="0">subst_type</f>
         <v>without</v>
       </c>
       <c r="J2" s="2" t="str">
@@ -21609,7 +21609,7 @@
         <v>WT_sgAB_R1_sense_cmv</v>
       </c>
       <c r="I3" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="J3" s="2" t="str">
@@ -21654,7 +21654,7 @@
         <v>KO_sgAB_R1_sense_branch</v>
       </c>
       <c r="I4" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="J4" t="str">
@@ -21699,7 +21699,7 @@
         <v>KO_sgAB_R1_sense_cmv</v>
       </c>
       <c r="I5" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="J5" t="str">
@@ -21744,7 +21744,7 @@
         <v>WT_sgAB_R2_sense_branch</v>
       </c>
       <c r="I6" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="J6" t="str">
@@ -21789,7 +21789,7 @@
         <v>WT_sgAB_R2_sense_cmv</v>
       </c>
       <c r="I7" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="J7" t="str">
@@ -21834,7 +21834,7 @@
         <v>KO_sgAB_R2_sense_branch</v>
       </c>
       <c r="I8" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="J8" t="str">
@@ -21879,7 +21879,7 @@
         <v>KO_sgAB_R2_sense_cmv</v>
       </c>
       <c r="I9" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="J9" t="str">
@@ -21924,7 +21924,7 @@
         <v>WT_sgA_R1_sense_branch</v>
       </c>
       <c r="I10" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="J10" t="str">
@@ -21969,7 +21969,7 @@
         <v>WT_sgA_R1_sense_cmv</v>
       </c>
       <c r="I11" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="J11" t="str">
@@ -22014,7 +22014,7 @@
         <v>KO_sgA_R1_sense_branch</v>
       </c>
       <c r="I12" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="J12" t="str">
@@ -22059,7 +22059,7 @@
         <v>KO_sgA_R1_sense_cmv</v>
       </c>
       <c r="I13" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="J13" t="str">
@@ -22104,7 +22104,7 @@
         <v>WT_sgB_R2_sense_branch</v>
       </c>
       <c r="I14" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="J14" t="str">
@@ -22149,7 +22149,7 @@
         <v>WT_sgB_R2_sense_cmv</v>
       </c>
       <c r="I15" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="J15" t="str">
@@ -22194,7 +22194,7 @@
         <v>KO_sgB_R2_sense_branch</v>
       </c>
       <c r="I16" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="J16" t="str">
@@ -22239,7 +22239,7 @@
         <v>KO_sgB_R2_sense_cmv</v>
       </c>
       <c r="I17" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="J17" t="str">
@@ -22455,7 +22455,7 @@
         <v>WT_sgA_R1_sense_branch_nodsb</v>
       </c>
       <c r="I26" t="str">
-        <f>subst_type</f>
+        <f t="shared" ref="I26:I33" si="1">subst_type</f>
         <v>without</v>
       </c>
       <c r="J26" s="2" t="str">
@@ -22500,7 +22500,7 @@
         <v>WT_sgA_R1_sense_cmv_nodsb</v>
       </c>
       <c r="I27" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="1"/>
         <v>without</v>
       </c>
       <c r="J27" s="2" t="str">
@@ -22545,7 +22545,7 @@
         <v>KO_sgA_R1_sense_branch_nodsb</v>
       </c>
       <c r="I28" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="1"/>
         <v>without</v>
       </c>
       <c r="J28" t="str">
@@ -22590,7 +22590,7 @@
         <v>KO_sgA_R1_sense_cmv_nodsb</v>
       </c>
       <c r="I29" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="1"/>
         <v>without</v>
       </c>
       <c r="J29" t="str">
@@ -22635,7 +22635,7 @@
         <v>WT_sgB_R2_sense_branch_nodsb</v>
       </c>
       <c r="I30" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="1"/>
         <v>without</v>
       </c>
       <c r="J30" t="str">
@@ -22680,7 +22680,7 @@
         <v>WT_sgB_R2_sense_cmv_nodsb</v>
       </c>
       <c r="I31" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="1"/>
         <v>without</v>
       </c>
       <c r="J31" t="str">
@@ -22725,7 +22725,7 @@
         <v>KO_sgB_R2_sense_branch_nodsb</v>
       </c>
       <c r="I32" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="1"/>
         <v>without</v>
       </c>
       <c r="J32" t="str">
@@ -22770,7 +22770,7 @@
         <v>KO_sgB_R2_sense_cmv_nodsb</v>
       </c>
       <c r="I33" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="1"/>
         <v>without</v>
       </c>
       <c r="J33" t="str">
@@ -25117,7 +25117,7 @@
         <v>branch</v>
       </c>
       <c r="L45" t="str">
-        <f t="shared" ref="L44:L55" si="2">"with"</f>
+        <f t="shared" ref="L45:L55" si="2">"with"</f>
         <v>with</v>
       </c>
       <c r="M45" t="str">
@@ -25818,7 +25818,7 @@
         <v>AB</v>
       </c>
       <c r="R2" t="str">
-        <f>subst_type</f>
+        <f t="shared" ref="R2:R7" si="0">subst_type</f>
         <v>without</v>
       </c>
       <c r="S2" t="str">
@@ -25899,7 +25899,7 @@
         <v>AB</v>
       </c>
       <c r="R3" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="S3" t="str">
@@ -25980,7 +25980,7 @@
         <v>A</v>
       </c>
       <c r="R4" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="S4" t="str">
@@ -26061,7 +26061,7 @@
         <v>B</v>
       </c>
       <c r="R5" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="S5" t="str">
@@ -26142,7 +26142,7 @@
         <v>A</v>
       </c>
       <c r="R6" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="S6" t="str">
@@ -26223,7 +26223,7 @@
         <v>B</v>
       </c>
       <c r="R7" t="str">
-        <f>subst_type</f>
+        <f t="shared" si="0"/>
         <v>without</v>
       </c>
       <c r="S7" t="str">
@@ -26423,8 +26423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1375107-D76A-4386-B771-6693BBF75061}">
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView topLeftCell="F37" workbookViewId="0">
-      <selection activeCell="N44" sqref="N44:N55"/>
+    <sheetView tabSelected="1" topLeftCell="F34" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:N41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
PPTX code for the 3d histograms.
</commit_message>
<xml_diff>
--- a/libinfo.xlsx
+++ b/libinfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tchan\Code\SCMB_Project\RNA-mediated_DSB_repair\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D5FF140-41D8-4339-AC1B-37356F5BDDBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE759840-15A4-4825-B197-92F4FE1CA2F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="5" activeTab="9" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="5" activeTab="8" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
   </bookViews>
   <sheets>
     <sheet name="globals" sheetId="3" r:id="rId1"/>
@@ -40,6 +40,7 @@
     <definedName name="var_6_anti_ofsfset">'6_common_layout'!$A$9</definedName>
     <definedName name="var_7_common_layout">'7_plot_graph'!$B$1</definedName>
     <definedName name="var_7_common_layout_combined">'7_plot_graph_combined'!$B$1</definedName>
+    <definedName name="var_7_ext">'7_plot_graph'!$D$1</definedName>
     <definedName name="var_7_ext_combined">'7_plot_graph_combined'!$D$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -85,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1529" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1531" uniqueCount="189">
   <si>
     <t>yjl217</t>
   </si>
@@ -776,6 +777,18 @@
   <dxfs count="202">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -881,18 +894,6 @@
           <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2378,8 +2379,8 @@
     <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="18">
       <calculatedColumnFormula>IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="17">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="1">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2391,44 +2392,44 @@
   <autoFilter ref="A44:N56" xr:uid="{D74A5276-1A50-4DA1-9131-9669404C8622}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{488C5146-A746-4F74-BCC8-806E4DC740CE}" name="index" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{C2A88DF4-2444-4C4C-A089-6CF9ADE79BD8}" name="dir" dataDxfId="15">
+    <tableColumn id="2" xr3:uid="{C2A88DF4-2444-4C4C-A089-6CF9ADE79BD8}" name="dir" dataDxfId="16">
       <calculatedColumnFormula>OFFSET(table_3_2[[dir]:[dir]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{7698ACE3-2351-400D-B00F-5A70184F8A33}" name="control" dataDxfId="14">
+    <tableColumn id="3" xr3:uid="{7698ACE3-2351-400D-B00F-5A70184F8A33}" name="control" dataDxfId="15">
       <calculatedColumnFormula>OFFSET(table_3_2[[control]:[control]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5E82B04C-FF09-492C-8A23-7E43B5990149}" name="ref" dataDxfId="13">
+    <tableColumn id="4" xr3:uid="{5E82B04C-FF09-492C-8A23-7E43B5990149}" name="ref" dataDxfId="14">
       <calculatedColumnFormula>OFFSET(table_3_2[[ref]:[ref]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{F4D36A0E-549B-4F3A-BCA9-75E151448998}" name="dsb_pos" dataDxfId="12">
+    <tableColumn id="5" xr3:uid="{F4D36A0E-549B-4F3A-BCA9-75E151448998}" name="dsb_pos" dataDxfId="13">
       <calculatedColumnFormula>OFFSET(table_3_2[[dsb_pos]:[dsb_pos]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{AEBBBB88-8CE2-409D-AE19-9C23263250A9}" name="dsb_type" dataDxfId="11">
+    <tableColumn id="6" xr3:uid="{AEBBBB88-8CE2-409D-AE19-9C23263250A9}" name="dsb_type" dataDxfId="12">
       <calculatedColumnFormula>OFFSET(table_3_2[[dsb_type]:[dsb_type]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3E71E7D2-0FA5-4FD5-BDC3-2955A091A9E6}" name="dsb_type_command" dataDxfId="10">
+    <tableColumn id="7" xr3:uid="{3E71E7D2-0FA5-4FD5-BDC3-2955A091A9E6}" name="dsb_type_command" dataDxfId="11">
       <calculatedColumnFormula>OFFSET(table_3_2[[dsb_type_command]:[dsb_type_command]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{EBD35881-E696-4202-9149-75A4EFFFAAD6}" name="strand" dataDxfId="9">
+    <tableColumn id="8" xr3:uid="{EBD35881-E696-4202-9149-75A4EFFFAAD6}" name="strand" dataDxfId="10">
       <calculatedColumnFormula>OFFSET(table_3_2[[strand]:[strand]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{123CA279-0CB6-41C1-9CD8-20D375B9B66D}" name="hguide" dataDxfId="8">
+    <tableColumn id="9" xr3:uid="{123CA279-0CB6-41C1-9CD8-20D375B9B66D}" name="hguide" dataDxfId="9">
       <calculatedColumnFormula>OFFSET(table_3_2[[hguide]:[hguide]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{3DCE3F3A-187D-411E-93FC-8C6C3EE9CAA2}" name="cell" dataDxfId="7">
+    <tableColumn id="10" xr3:uid="{3DCE3F3A-187D-411E-93FC-8C6C3EE9CAA2}" name="cell" dataDxfId="8">
       <calculatedColumnFormula>OFFSET(table_3_2[[cell]:[cell]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{9E585D29-AB3E-4D04-8C1D-24F78339C9A3}" name="treatment" dataDxfId="6">
+    <tableColumn id="11" xr3:uid="{9E585D29-AB3E-4D04-8C1D-24F78339C9A3}" name="treatment" dataDxfId="7">
       <calculatedColumnFormula>OFFSET(table_3_2[[treatment]:[treatment]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{928286B8-23FB-4375-B52B-617DD59D6098}" name="subst_type" dataDxfId="5">
+    <tableColumn id="12" xr3:uid="{928286B8-23FB-4375-B52B-617DD59D6098}" name="subst_type" dataDxfId="6">
       <calculatedColumnFormula>"without"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{E18D2025-56E8-4128-9201-9E0BF8A67AC0}" name="common_layout_dir" dataDxfId="4">
+    <tableColumn id="15" xr3:uid="{E18D2025-56E8-4128-9201-9E0BF8A67AC0}" name="common_layout_dir" dataDxfId="5">
       <calculatedColumnFormula>OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_2[[#This Row],[index]] - 1, 6) + 2, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{0917AB98-1545-4642-9BE8-618AAA1E404A}" name="command" dataDxfId="3">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""))</calculatedColumnFormula>
+    <tableColumn id="13" xr3:uid="{0917AB98-1545-4642-9BE8-618AAA1E404A}" name="command" dataDxfId="0">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2440,10 +2441,10 @@
   <autoFilter ref="A3:C19" xr:uid="{B76EEC45-4FC3-44D5-9B2E-9183DF724F60}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{FAFADB73-BF3B-401A-8C48-9FCB5D3C4CB6}" name="index" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{8541A14E-3250-4B9C-B315-969FC11BE60A}" name="dir" dataDxfId="16">
+    <tableColumn id="4" xr3:uid="{8541A14E-3250-4B9C-B315-969FC11BE60A}" name="dir" dataDxfId="17">
       <calculatedColumnFormula>OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{EAD6D5EC-B61E-4A98-B4FD-4932757CFEA3}" name="command" dataDxfId="2">
+    <tableColumn id="6" xr3:uid="{EAD6D5EC-B61E-4A98-B4FD-4932757CFEA3}" name="command" dataDxfId="4">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2459,7 +2460,7 @@
     <tableColumn id="4" xr3:uid="{181C59FC-364D-4421-8E54-98DFF4CA7C05}" name="dir" dataDxfId="33">
       <calculatedColumnFormula>OFFSET(table_4_2[[dir_out]:[dir_out]], table_7_4[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{6D8CC942-572B-44F2-BCA6-4D31A25A4067}" name="command" dataDxfId="1">
+    <tableColumn id="6" xr3:uid="{6D8CC942-572B-44F2-BCA6-4D31A25A4067}" name="command" dataDxfId="3">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_4[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_2[[dir_out]:[dir_out]],table_7_4[[#This Row],[index]] - 1, 0, 1, 1)), ""), " -ext ", var_7_ext_combined)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2475,7 +2476,7 @@
     <tableColumn id="4" xr3:uid="{1222E48F-ED5C-48AA-BA39-1443B841BC9F}" name="dir" dataDxfId="30">
       <calculatedColumnFormula>OFFSET(table_4_3[[dir_out]:[dir_out]], table_7_5[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{89B7E589-2097-43FC-B96B-19D2EF777E97}" name="command_main_data_combined" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{89B7E589-2097-43FC-B96B-19D2EF777E97}" name="command_main_data_combined" dataDxfId="2">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3210,8 +3211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DFB1CC9-23C4-4E30-93CF-6F31CFACE92F}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26538,8 +26539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1375107-D76A-4386-B771-6693BBF75061}">
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView topLeftCell="C37" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39:N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26562,7 +26563,13 @@
         <v>185</v>
       </c>
       <c r="B1" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D1" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -26662,8 +26669,8 @@
         <v>2DSB_R1</v>
       </c>
       <c r="N3" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense -o plots/graphs/individual  --layout_dir layouts/2DSB_R1</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -26719,8 +26726,8 @@
         <v>2DSB_R1</v>
       </c>
       <c r="N4" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_branch -o plots/graphs/individual  --layout_dir layouts/2DSB_R1</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_branch -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -26776,8 +26783,8 @@
         <v>2DSB_R1</v>
       </c>
       <c r="N5" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_cmv -o plots/graphs/individual  --layout_dir layouts/2DSB_R1</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_cmv -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -26833,8 +26840,8 @@
         <v>2DSB_R1</v>
       </c>
       <c r="N6" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense -o plots/graphs/individual  --layout_dir layouts/2DSB_R1</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -26890,8 +26897,8 @@
         <v>2DSB_R1</v>
       </c>
       <c r="N7" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_branch -o plots/graphs/individual  --layout_dir layouts/2DSB_R1</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_branch -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -26947,8 +26954,8 @@
         <v>2DSB_R1</v>
       </c>
       <c r="N8" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_cmv -o plots/graphs/individual  --layout_dir layouts/2DSB_R1</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_cmv -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -27004,8 +27011,8 @@
         <v>2DSB_R2</v>
       </c>
       <c r="N9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense -o plots/graphs/individual  --layout_dir layouts/2DSB_R2</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -27061,8 +27068,8 @@
         <v>2DSB_R2</v>
       </c>
       <c r="N10" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_branch -o plots/graphs/individual  --layout_dir layouts/2DSB_R2</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_branch -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -27118,8 +27125,8 @@
         <v>2DSB_R2</v>
       </c>
       <c r="N11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_cmv -o plots/graphs/individual  --layout_dir layouts/2DSB_R2</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_cmv -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -27175,8 +27182,8 @@
         <v>2DSB_R2</v>
       </c>
       <c r="N12" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense -o plots/graphs/individual  --layout_dir layouts/2DSB_R2</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -27232,8 +27239,8 @@
         <v>2DSB_R2</v>
       </c>
       <c r="N13" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_branch -o plots/graphs/individual  --layout_dir layouts/2DSB_R2</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_branch -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -27289,8 +27296,8 @@
         <v>2DSB_R2</v>
       </c>
       <c r="N14" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_cmv -o plots/graphs/individual  --layout_dir layouts/2DSB_R2</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_cmv -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -27346,8 +27353,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N15" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense -o plots/graphs/individual  --layout_dir layouts/1DSB_R1</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -27403,8 +27410,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N16" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch -o plots/graphs/individual  --layout_dir layouts/1DSB_R1</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -27460,8 +27467,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N17" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv -o plots/graphs/individual  --layout_dir layouts/1DSB_R1</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -27517,8 +27524,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N18" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense -o plots/graphs/individual  --layout_dir layouts/1DSB_R1</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -27574,8 +27581,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N19" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch -o plots/graphs/individual  --layout_dir layouts/1DSB_R1</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -27631,8 +27638,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N20" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv -o plots/graphs/individual  --layout_dir layouts/1DSB_R1</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -27688,8 +27695,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N21" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense -o plots/graphs/individual  --layout_dir layouts/1DSB_R2</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -27745,8 +27752,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N22" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch -o plots/graphs/individual  --layout_dir layouts/1DSB_R2</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -27802,8 +27809,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N23" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv -o plots/graphs/individual  --layout_dir layouts/1DSB_R2</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -27859,8 +27866,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N24" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense -o plots/graphs/individual  --layout_dir layouts/1DSB_R2</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -27916,8 +27923,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N25" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch -o plots/graphs/individual  --layout_dir layouts/1DSB_R2</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -27973,8 +27980,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N26" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv -o plots/graphs/individual  --layout_dir layouts/1DSB_R2</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -28030,8 +28037,8 @@
         <v>1DSB_R1_30bpDown</v>
       </c>
       <c r="N27" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_30bpDown -o plots/graphs/individual  --layout_dir layouts/1DSB_R1_30bpDown</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_30bpDown -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -28087,8 +28094,8 @@
         <v>1DSB_R1_30bpDown</v>
       </c>
       <c r="N28" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch_30bpDown -o plots/graphs/individual  --layout_dir layouts/1DSB_R1_30bpDown</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch_30bpDown -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -28144,8 +28151,8 @@
         <v>1DSB_R1_30bpDown</v>
       </c>
       <c r="N29" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv_30bpDown -o plots/graphs/individual  --layout_dir layouts/1DSB_R1_30bpDown</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv_30bpDown -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -28201,8 +28208,8 @@
         <v>1DSB_R1_30bpDown</v>
       </c>
       <c r="N30" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_30bpDown -o plots/graphs/individual  --layout_dir layouts/1DSB_R1_30bpDown</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_30bpDown -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -28258,8 +28265,8 @@
         <v>1DSB_R1_30bpDown</v>
       </c>
       <c r="N31" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch_30bpDown -o plots/graphs/individual  --layout_dir layouts/1DSB_R1_30bpDown</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch_30bpDown -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -28315,8 +28322,8 @@
         <v>1DSB_R1_30bpDown</v>
       </c>
       <c r="N32" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv_30bpDown -o plots/graphs/individual  --layout_dir layouts/1DSB_R1_30bpDown</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv_30bpDown -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -28372,8 +28379,8 @@
         <v>1DSB_R2_30bpDown</v>
       </c>
       <c r="N33" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_30bpDown -o plots/graphs/individual  --layout_dir layouts/1DSB_R2_30bpDown</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_30bpDown -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -28429,8 +28436,8 @@
         <v>1DSB_R2_30bpDown</v>
       </c>
       <c r="N34" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch_30bpDown -o plots/graphs/individual  --layout_dir layouts/1DSB_R2_30bpDown</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch_30bpDown -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -28486,8 +28493,8 @@
         <v>1DSB_R2_30bpDown</v>
       </c>
       <c r="N35" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv_30bpDown -o plots/graphs/individual  --layout_dir layouts/1DSB_R2_30bpDown</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv_30bpDown -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -28543,8 +28550,8 @@
         <v>1DSB_R2_30bpDown</v>
       </c>
       <c r="N36" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_30bpDown -o plots/graphs/individual  --layout_dir layouts/1DSB_R2_30bpDown</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_30bpDown -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -28600,8 +28607,8 @@
         <v>1DSB_R2_30bpDown</v>
       </c>
       <c r="N37" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch_30bpDown -o plots/graphs/individual  --layout_dir layouts/1DSB_R2_30bpDown</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch_30bpDown -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -28657,8 +28664,8 @@
         <v>1DSB_R2_30bpDown</v>
       </c>
       <c r="N38" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv_30bpDown -o plots/graphs/individual  --layout_dir layouts/1DSB_R2_30bpDown</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv_30bpDown -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -28714,8 +28721,8 @@
         <v>2DSBanti_R1</v>
       </c>
       <c r="N39" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense -o plots/graphs/individual  --layout_dir layouts/2DSBanti_R1</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
@@ -28771,8 +28778,8 @@
         <v>2DSBanti_R1</v>
       </c>
       <c r="N40" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_splicing -o plots/graphs/individual  --layout_dir layouts/2DSBanti_R1</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_splicing -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
@@ -28828,8 +28835,8 @@
         <v>2DSBanti_R2</v>
       </c>
       <c r="N41" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense -o plots/graphs/individual  --layout_dir layouts/2DSBanti_R2</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
@@ -28885,8 +28892,8 @@
         <v>2DSBanti_R2</v>
       </c>
       <c r="N42" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_splicing -o plots/graphs/individual  --layout_dir layouts/2DSBanti_R2</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_splicing -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -28986,8 +28993,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N45" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_nodsb -o plots/graphs/individual  --layout_dir layouts/1DSB_R1</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_nodsb -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
@@ -29043,8 +29050,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N46" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch_nodsb -o plots/graphs/individual  --layout_dir layouts/1DSB_R1</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch_nodsb -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
@@ -29100,8 +29107,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N47" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv_nodsb -o plots/graphs/individual  --layout_dir layouts/1DSB_R1</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv_nodsb -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
@@ -29157,8 +29164,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N48" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_nodsb -o plots/graphs/individual  --layout_dir layouts/1DSB_R1</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_nodsb -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
@@ -29214,8 +29221,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N49" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch_nodsb -o plots/graphs/individual  --layout_dir layouts/1DSB_R1</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch_nodsb -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
@@ -29271,8 +29278,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N50" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv_nodsb -o plots/graphs/individual  --layout_dir layouts/1DSB_R1</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv_nodsb -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
@@ -29328,8 +29335,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N51" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_nodsb -o plots/graphs/individual  --layout_dir layouts/1DSB_R2</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_nodsb -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
@@ -29385,8 +29392,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N52" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch_nodsb -o plots/graphs/individual  --layout_dir layouts/1DSB_R2</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch_nodsb -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
@@ -29442,8 +29449,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N53" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv_nodsb -o plots/graphs/individual  --layout_dir layouts/1DSB_R2</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv_nodsb -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
@@ -29499,8 +29506,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N54" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_nodsb -o plots/graphs/individual  --layout_dir layouts/1DSB_R2</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_nodsb -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
@@ -29556,8 +29563,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N55" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch_nodsb -o plots/graphs/individual  --layout_dir layouts/1DSB_R2</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch_nodsb -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
@@ -29613,8 +29620,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N56" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv_nodsb -o plots/graphs/individual  --layout_dir layouts/1DSB_R2</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv_nodsb -o plots/graphs/individual  -ext html</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tweaks to universal layout to reduce overlap.
</commit_message>
<xml_diff>
--- a/libinfo.xlsx
+++ b/libinfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tchan\Code\SCMB_Project\RNA-mediated_DSB_repair\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE759840-15A4-4825-B197-92F4FE1CA2F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC91ECD-A784-4706-BEDF-E525D5C78536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="5" activeTab="8" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="5" activeTab="9" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
   </bookViews>
   <sheets>
     <sheet name="globals" sheetId="3" r:id="rId1"/>
@@ -42,9 +42,10 @@
     <definedName name="var_7_common_layout_combined">'7_plot_graph_combined'!$B$1</definedName>
     <definedName name="var_7_ext">'7_plot_graph'!$D$1</definedName>
     <definedName name="var_7_ext_combined">'7_plot_graph_combined'!$D$1</definedName>
+    <definedName name="var_7_layout">'7_plot_graph'!$F$1</definedName>
+    <definedName name="var_7_layout_combined">'7_plot_graph_combined'!$F$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -86,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1531" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="192">
   <si>
     <t>yjl217</t>
   </si>
@@ -654,6 +655,15 @@
   <si>
     <t>html</t>
   </si>
+  <si>
+    <t>png</t>
+  </si>
+  <si>
+    <t>layout</t>
+  </si>
+  <si>
+    <t>universal</t>
+  </si>
 </sst>
 </file>
 
@@ -777,6 +787,9 @@
   <dxfs count="202">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -794,7 +807,121 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -899,7 +1026,9 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <b/>
+      </font>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -936,125 +1065,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -2343,44 +2353,44 @@
   <autoFilter ref="A2:N42" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
   <tableColumns count="14">
     <tableColumn id="25" xr3:uid="{C323C376-24D3-4404-9E0F-6E9361862271}" name="index" dataDxfId="39"/>
-    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="29">
+    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="38">
       <calculatedColumnFormula>OFFSET(table_3_1[[dir]:[dir]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="27">
+    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="37">
       <calculatedColumnFormula>OFFSET(table_3_1[[control]:[control]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="28">
+    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="36">
       <calculatedColumnFormula>OFFSET(table_3_1[[ref]:[ref]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="26">
+    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="35">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_pos]:[dsb_pos]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="25">
+    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="34">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_type]:[dsb_type]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="24">
+    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="33">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_type_command]:[dsb_type_command]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="23">
+    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="32">
       <calculatedColumnFormula>OFFSET(table_3_1[[strand]:[strand]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="22">
+    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="31">
       <calculatedColumnFormula>OFFSET(table_3_1[[hguide]:[hguide]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="21">
+    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="30">
       <calculatedColumnFormula>OFFSET(table_3_1[[cell]:[cell]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="20">
+    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="29">
       <calculatedColumnFormula>OFFSET(table_3_1[[treatment]:[treatment]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="19">
+    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="28">
       <calculatedColumnFormula>"without"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="18">
+    <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="27">
       <calculatedColumnFormula>IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="1">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="2">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2391,45 +2401,45 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{B47D9508-D874-40FC-B6F6-C106B48F6A94}" name="table_7_2" displayName="table_7_2" ref="A44:N56" totalsRowShown="0">
   <autoFilter ref="A44:N56" xr:uid="{D74A5276-1A50-4DA1-9131-9669404C8622}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{488C5146-A746-4F74-BCC8-806E4DC740CE}" name="index" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{C2A88DF4-2444-4C4C-A089-6CF9ADE79BD8}" name="dir" dataDxfId="16">
+    <tableColumn id="1" xr3:uid="{488C5146-A746-4F74-BCC8-806E4DC740CE}" name="index" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{C2A88DF4-2444-4C4C-A089-6CF9ADE79BD8}" name="dir" dataDxfId="25">
       <calculatedColumnFormula>OFFSET(table_3_2[[dir]:[dir]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{7698ACE3-2351-400D-B00F-5A70184F8A33}" name="control" dataDxfId="15">
+    <tableColumn id="3" xr3:uid="{7698ACE3-2351-400D-B00F-5A70184F8A33}" name="control" dataDxfId="24">
       <calculatedColumnFormula>OFFSET(table_3_2[[control]:[control]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5E82B04C-FF09-492C-8A23-7E43B5990149}" name="ref" dataDxfId="14">
+    <tableColumn id="4" xr3:uid="{5E82B04C-FF09-492C-8A23-7E43B5990149}" name="ref" dataDxfId="23">
       <calculatedColumnFormula>OFFSET(table_3_2[[ref]:[ref]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{F4D36A0E-549B-4F3A-BCA9-75E151448998}" name="dsb_pos" dataDxfId="13">
+    <tableColumn id="5" xr3:uid="{F4D36A0E-549B-4F3A-BCA9-75E151448998}" name="dsb_pos" dataDxfId="22">
       <calculatedColumnFormula>OFFSET(table_3_2[[dsb_pos]:[dsb_pos]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{AEBBBB88-8CE2-409D-AE19-9C23263250A9}" name="dsb_type" dataDxfId="12">
+    <tableColumn id="6" xr3:uid="{AEBBBB88-8CE2-409D-AE19-9C23263250A9}" name="dsb_type" dataDxfId="21">
       <calculatedColumnFormula>OFFSET(table_3_2[[dsb_type]:[dsb_type]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3E71E7D2-0FA5-4FD5-BDC3-2955A091A9E6}" name="dsb_type_command" dataDxfId="11">
+    <tableColumn id="7" xr3:uid="{3E71E7D2-0FA5-4FD5-BDC3-2955A091A9E6}" name="dsb_type_command" dataDxfId="20">
       <calculatedColumnFormula>OFFSET(table_3_2[[dsb_type_command]:[dsb_type_command]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{EBD35881-E696-4202-9149-75A4EFFFAAD6}" name="strand" dataDxfId="10">
+    <tableColumn id="8" xr3:uid="{EBD35881-E696-4202-9149-75A4EFFFAAD6}" name="strand" dataDxfId="19">
       <calculatedColumnFormula>OFFSET(table_3_2[[strand]:[strand]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{123CA279-0CB6-41C1-9CD8-20D375B9B66D}" name="hguide" dataDxfId="9">
+    <tableColumn id="9" xr3:uid="{123CA279-0CB6-41C1-9CD8-20D375B9B66D}" name="hguide" dataDxfId="18">
       <calculatedColumnFormula>OFFSET(table_3_2[[hguide]:[hguide]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{3DCE3F3A-187D-411E-93FC-8C6C3EE9CAA2}" name="cell" dataDxfId="8">
+    <tableColumn id="10" xr3:uid="{3DCE3F3A-187D-411E-93FC-8C6C3EE9CAA2}" name="cell" dataDxfId="17">
       <calculatedColumnFormula>OFFSET(table_3_2[[cell]:[cell]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{9E585D29-AB3E-4D04-8C1D-24F78339C9A3}" name="treatment" dataDxfId="7">
+    <tableColumn id="11" xr3:uid="{9E585D29-AB3E-4D04-8C1D-24F78339C9A3}" name="treatment" dataDxfId="16">
       <calculatedColumnFormula>OFFSET(table_3_2[[treatment]:[treatment]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{928286B8-23FB-4375-B52B-617DD59D6098}" name="subst_type" dataDxfId="6">
+    <tableColumn id="12" xr3:uid="{928286B8-23FB-4375-B52B-617DD59D6098}" name="subst_type" dataDxfId="15">
       <calculatedColumnFormula>"without"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{E18D2025-56E8-4128-9201-9E0BF8A67AC0}" name="common_layout_dir" dataDxfId="5">
+    <tableColumn id="15" xr3:uid="{E18D2025-56E8-4128-9201-9E0BF8A67AC0}" name="common_layout_dir" dataDxfId="14">
       <calculatedColumnFormula>OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_2[[#This Row],[index]] - 1, 6) + 2, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{0917AB98-1545-4642-9BE8-618AAA1E404A}" name="command" dataDxfId="0">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext)</calculatedColumnFormula>
+    <tableColumn id="13" xr3:uid="{0917AB98-1545-4642-9BE8-618AAA1E404A}" name="command" dataDxfId="1">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2437,15 +2447,15 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{B76EEC45-4FC3-44D5-9B2E-9183DF724F60}" name="table_7_3" displayName="table_7_3" ref="A3:C19" totalsRowShown="0" headerRowDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{B76EEC45-4FC3-44D5-9B2E-9183DF724F60}" name="table_7_3" displayName="table_7_3" ref="A3:C19" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A3:C19" xr:uid="{B76EEC45-4FC3-44D5-9B2E-9183DF724F60}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{FAFADB73-BF3B-401A-8C48-9FCB5D3C4CB6}" name="index" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{8541A14E-3250-4B9C-B315-969FC11BE60A}" name="dir" dataDxfId="17">
+    <tableColumn id="1" xr3:uid="{FAFADB73-BF3B-401A-8C48-9FCB5D3C4CB6}" name="index" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{8541A14E-3250-4B9C-B315-969FC11BE60A}" name="dir" dataDxfId="11">
       <calculatedColumnFormula>OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{EAD6D5EC-B61E-4A98-B4FD-4932757CFEA3}" name="command" dataDxfId="4">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined)</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{EAD6D5EC-B61E-4A98-B4FD-4932757CFEA3}" name="command" dataDxfId="0">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2453,14 +2463,14 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{8B4E853A-A4F1-4022-B857-226C57559A5F}" name="table_7_4" displayName="table_7_4" ref="A21:C23" totalsRowShown="0" headerRowDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{8B4E853A-A4F1-4022-B857-226C57559A5F}" name="table_7_4" displayName="table_7_4" ref="A21:C23" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="A21:C23" xr:uid="{8B4E853A-A4F1-4022-B857-226C57559A5F}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{1ECF32A2-E353-4754-B4C5-11C46AACF6C0}" name="index" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{181C59FC-364D-4421-8E54-98DFF4CA7C05}" name="dir" dataDxfId="33">
+    <tableColumn id="1" xr3:uid="{1ECF32A2-E353-4754-B4C5-11C46AACF6C0}" name="index" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{181C59FC-364D-4421-8E54-98DFF4CA7C05}" name="dir" dataDxfId="8">
       <calculatedColumnFormula>OFFSET(table_4_2[[dir_out]:[dir_out]], table_7_4[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{6D8CC942-572B-44F2-BCA6-4D31A25A4067}" name="command" dataDxfId="3">
+    <tableColumn id="6" xr3:uid="{6D8CC942-572B-44F2-BCA6-4D31A25A4067}" name="command" dataDxfId="7">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_4[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_2[[dir_out]:[dir_out]],table_7_4[[#This Row],[index]] - 1, 0, 1, 1)), ""), " -ext ", var_7_ext_combined)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2469,14 +2479,14 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{58F5EC27-BD76-45AE-8D38-F4E705EF79E9}" name="table_7_5" displayName="table_7_5" ref="A26:C34" totalsRowShown="0" headerRowDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{58F5EC27-BD76-45AE-8D38-F4E705EF79E9}" name="table_7_5" displayName="table_7_5" ref="A26:C34" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A26:C34" xr:uid="{58F5EC27-BD76-45AE-8D38-F4E705EF79E9}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{AAC1476C-44CE-49FD-8254-50BAEAA6929C}" name="index" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{1222E48F-ED5C-48AA-BA39-1443B841BC9F}" name="dir" dataDxfId="30">
+    <tableColumn id="1" xr3:uid="{AAC1476C-44CE-49FD-8254-50BAEAA6929C}" name="index" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{1222E48F-ED5C-48AA-BA39-1443B841BC9F}" name="dir" dataDxfId="4">
       <calculatedColumnFormula>OFFSET(table_4_3[[dir_out]:[dir_out]], table_7_5[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{89B7E589-2097-43FC-B96B-19D2EF777E97}" name="command_main_data_combined" dataDxfId="2">
+    <tableColumn id="6" xr3:uid="{89B7E589-2097-43FC-B96B-19D2EF777E97}" name="command_main_data_combined" dataDxfId="3">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3211,8 +3221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DFB1CC9-23C4-4E30-93CF-6F31CFACE92F}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3230,24 +3240,30 @@
     <col min="11" max="11" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>186</v>
       </c>
       <c r="B1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>187</v>
       </c>
       <c r="D1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>112</v>
       </c>
@@ -3258,7 +3274,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -3267,11 +3283,11 @@
         <v>WT_sgAB_R1_sense_branch</v>
       </c>
       <c r="C4" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_branch -o plots/graphs/combined --layout_dir layouts/2DSB_R1 -ext html</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_branch -o plots/graphs/combinedFALSE -ext png --layout universal</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -3280,11 +3296,11 @@
         <v>WT_sgAB_R1_sense_cmv</v>
       </c>
       <c r="C5" s="2" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_cmv -o plots/graphs/combined --layout_dir layouts/2DSB_R1 -ext html</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_cmv -o plots/graphs/combinedFALSE -ext png --layout universal</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -3293,11 +3309,11 @@
         <v>KO_sgAB_R1_sense_branch</v>
       </c>
       <c r="C6" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_branch -o plots/graphs/combined --layout_dir layouts/2DSB_R1 -ext html</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_branch -o plots/graphs/combinedFALSE -ext png --layout universal</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -3306,11 +3322,11 @@
         <v>KO_sgAB_R1_sense_cmv</v>
       </c>
       <c r="C7" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_cmv -o plots/graphs/combined --layout_dir layouts/2DSB_R1 -ext html</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_cmv -o plots/graphs/combinedFALSE -ext png --layout universal</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -3319,11 +3335,11 @@
         <v>WT_sgAB_R2_sense_branch</v>
       </c>
       <c r="C8" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_branch -o plots/graphs/combined --layout_dir layouts/2DSB_R2 -ext html</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_branch -o plots/graphs/combinedFALSE -ext png --layout universal</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -3332,11 +3348,11 @@
         <v>WT_sgAB_R2_sense_cmv</v>
       </c>
       <c r="C9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_cmv -o plots/graphs/combined --layout_dir layouts/2DSB_R2 -ext html</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_cmv -o plots/graphs/combinedFALSE -ext png --layout universal</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -3345,11 +3361,11 @@
         <v>KO_sgAB_R2_sense_branch</v>
       </c>
       <c r="C10" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_branch -o plots/graphs/combined --layout_dir layouts/2DSB_R2 -ext html</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_branch -o plots/graphs/combinedFALSE -ext png --layout universal</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -3358,11 +3374,11 @@
         <v>KO_sgAB_R2_sense_cmv</v>
       </c>
       <c r="C11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_cmv -o plots/graphs/combined --layout_dir layouts/2DSB_R2 -ext html</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_cmv -o plots/graphs/combinedFALSE -ext png --layout universal</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -3371,11 +3387,11 @@
         <v>WT_sgA_R1_sense_branch</v>
       </c>
       <c r="C12" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_branch -o plots/graphs/combined --layout_dir layouts/1DSB_R1 -ext html</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_branch -o plots/graphs/combinedFALSE -ext png --layout universal</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -3384,11 +3400,11 @@
         <v>WT_sgA_R1_sense_cmv</v>
       </c>
       <c r="C13" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_cmv -o plots/graphs/combined --layout_dir layouts/1DSB_R1 -ext html</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_cmv -o plots/graphs/combinedFALSE -ext png --layout universal</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -3397,11 +3413,11 @@
         <v>KO_sgA_R1_sense_branch</v>
       </c>
       <c r="C14" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_branch -o plots/graphs/combined --layout_dir layouts/1DSB_R1 -ext html</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_branch -o plots/graphs/combinedFALSE -ext png --layout universal</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -3410,11 +3426,11 @@
         <v>KO_sgA_R1_sense_cmv</v>
       </c>
       <c r="C15" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_cmv -o plots/graphs/combined --layout_dir layouts/1DSB_R1 -ext html</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_cmv -o plots/graphs/combinedFALSE -ext png --layout universal</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -3423,8 +3439,8 @@
         <v>WT_sgB_R2_sense_branch</v>
       </c>
       <c r="C16" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_branch -o plots/graphs/combined --layout_dir layouts/1DSB_R2 -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_branch -o plots/graphs/combinedFALSE -ext png --layout universal</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -3436,8 +3452,8 @@
         <v>WT_sgB_R2_sense_cmv</v>
       </c>
       <c r="C17" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_cmv -o plots/graphs/combined --layout_dir layouts/1DSB_R2 -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_cmv -o plots/graphs/combinedFALSE -ext png --layout universal</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -3449,8 +3465,8 @@
         <v>KO_sgB_R2_sense_branch</v>
       </c>
       <c r="C18" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_branch -o plots/graphs/combined --layout_dir layouts/1DSB_R2 -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_branch -o plots/graphs/combinedFALSE -ext png --layout universal</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -3462,8 +3478,8 @@
         <v>KO_sgB_R2_sense_cmv</v>
       </c>
       <c r="C19" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_cmv -o plots/graphs/combined --layout_dir layouts/1DSB_R2 -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_cmv -o plots/graphs/combinedFALSE -ext png --layout universal</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -3487,7 +3503,7 @@
       </c>
       <c r="C22" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_4[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_2[[dir_out]:[dir_out]],table_7_4[[#This Row],[index]] - 1, 0, 1, 1)), ""), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense_splicing -o plots/graphs/combined --layout_dir layouts/2DSBanti_R1 -ext html</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense_splicing -o plots/graphs/combined -ext png</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -3500,7 +3516,7 @@
       </c>
       <c r="C23" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_4[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_2[[dir_out]:[dir_out]],table_7_4[[#This Row],[index]] - 1, 0, 1, 1)), ""), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense_splicing -o plots/graphs/combined --layout_dir layouts/2DSBanti_R2 -ext html</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense_splicing -o plots/graphs/combined -ext png</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -3530,7 +3546,7 @@
       </c>
       <c r="C27" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_branch_nodsb -o plots/graphs/combined --layout_dir layouts/1DSB_R1 -ext html</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_branch_nodsb -o plots/graphs/combined -ext png</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -3543,7 +3559,7 @@
       </c>
       <c r="C28" s="2" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_cmv_nodsb -o plots/graphs/combined --layout_dir layouts/1DSB_R1 -ext html</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_cmv_nodsb -o plots/graphs/combined -ext png</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -3556,7 +3572,7 @@
       </c>
       <c r="C29" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_branch_nodsb -o plots/graphs/combined --layout_dir layouts/1DSB_R1 -ext html</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_branch_nodsb -o plots/graphs/combined -ext png</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -3569,7 +3585,7 @@
       </c>
       <c r="C30" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_cmv_nodsb -o plots/graphs/combined --layout_dir layouts/1DSB_R1 -ext html</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_cmv_nodsb -o plots/graphs/combined -ext png</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -3582,7 +3598,7 @@
       </c>
       <c r="C31" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_branch_nodsb -o plots/graphs/combined --layout_dir layouts/1DSB_R2 -ext html</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_branch_nodsb -o plots/graphs/combined -ext png</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -3595,7 +3611,7 @@
       </c>
       <c r="C32" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_cmv_nodsb -o plots/graphs/combined --layout_dir layouts/1DSB_R2 -ext html</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_cmv_nodsb -o plots/graphs/combined -ext png</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -3608,7 +3624,7 @@
       </c>
       <c r="C33" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_branch_nodsb -o plots/graphs/combined --layout_dir layouts/1DSB_R2 -ext html</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_branch_nodsb -o plots/graphs/combined -ext png</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -3621,15 +3637,16 @@
       </c>
       <c r="C34" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_cmv_nodsb -o plots/graphs/combined --layout_dir layouts/1DSB_R2 -ext html</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_cmv_nodsb -o plots/graphs/combined -ext png</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="3">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
@@ -22912,8 +22929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FCC207B-A9CD-4866-A17E-A3EE763F139F}">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView topLeftCell="C19" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44:L44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26539,8 +26556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1375107-D76A-4386-B771-6693BBF75061}">
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
-      <selection activeCell="N39" sqref="N39:N42"/>
+    <sheetView topLeftCell="C37" workbookViewId="0">
+      <selection activeCell="N46" sqref="N46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26571,6 +26588,12 @@
       <c r="D1" t="s">
         <v>188</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F1" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -26669,8 +26692,8 @@
         <v>2DSB_R1</v>
       </c>
       <c r="N3" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -26726,8 +26749,8 @@
         <v>2DSB_R1</v>
       </c>
       <c r="N4" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_branch -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_branch -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -26783,8 +26806,8 @@
         <v>2DSB_R1</v>
       </c>
       <c r="N5" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_cmv -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_cmv -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -26840,8 +26863,8 @@
         <v>2DSB_R1</v>
       </c>
       <c r="N6" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -26897,8 +26920,8 @@
         <v>2DSB_R1</v>
       </c>
       <c r="N7" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_branch -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_branch -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -26954,8 +26977,8 @@
         <v>2DSB_R1</v>
       </c>
       <c r="N8" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_cmv -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_cmv -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -27011,8 +27034,8 @@
         <v>2DSB_R2</v>
       </c>
       <c r="N9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -27068,8 +27091,8 @@
         <v>2DSB_R2</v>
       </c>
       <c r="N10" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_branch -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_branch -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -27125,8 +27148,8 @@
         <v>2DSB_R2</v>
       </c>
       <c r="N11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_cmv -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_cmv -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -27182,8 +27205,8 @@
         <v>2DSB_R2</v>
       </c>
       <c r="N12" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -27239,8 +27262,8 @@
         <v>2DSB_R2</v>
       </c>
       <c r="N13" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_branch -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_branch -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -27296,8 +27319,8 @@
         <v>2DSB_R2</v>
       </c>
       <c r="N14" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_cmv -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_cmv -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -27353,8 +27376,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N15" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -27410,8 +27433,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N16" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -27467,8 +27490,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N17" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -27524,8 +27547,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N18" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -27581,8 +27604,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N19" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -27638,8 +27661,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N20" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -27695,8 +27718,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N21" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -27752,8 +27775,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N22" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -27809,8 +27832,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N23" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -27866,8 +27889,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N24" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -27923,8 +27946,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N25" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -27980,8 +28003,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N26" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -28037,8 +28060,8 @@
         <v>1DSB_R1_30bpDown</v>
       </c>
       <c r="N27" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_30bpDown -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_30bpDown -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -28094,8 +28117,8 @@
         <v>1DSB_R1_30bpDown</v>
       </c>
       <c r="N28" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch_30bpDown -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch_30bpDown -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -28151,8 +28174,8 @@
         <v>1DSB_R1_30bpDown</v>
       </c>
       <c r="N29" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv_30bpDown -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv_30bpDown -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -28208,8 +28231,8 @@
         <v>1DSB_R1_30bpDown</v>
       </c>
       <c r="N30" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_30bpDown -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_30bpDown -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -28265,8 +28288,8 @@
         <v>1DSB_R1_30bpDown</v>
       </c>
       <c r="N31" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch_30bpDown -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch_30bpDown -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -28322,8 +28345,8 @@
         <v>1DSB_R1_30bpDown</v>
       </c>
       <c r="N32" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv_30bpDown -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv_30bpDown -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -28379,8 +28402,8 @@
         <v>1DSB_R2_30bpDown</v>
       </c>
       <c r="N33" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_30bpDown -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_30bpDown -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -28436,8 +28459,8 @@
         <v>1DSB_R2_30bpDown</v>
       </c>
       <c r="N34" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch_30bpDown -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch_30bpDown -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -28493,8 +28516,8 @@
         <v>1DSB_R2_30bpDown</v>
       </c>
       <c r="N35" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv_30bpDown -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv_30bpDown -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -28550,8 +28573,8 @@
         <v>1DSB_R2_30bpDown</v>
       </c>
       <c r="N36" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_30bpDown -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_30bpDown -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -28607,8 +28630,8 @@
         <v>1DSB_R2_30bpDown</v>
       </c>
       <c r="N37" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch_30bpDown -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch_30bpDown -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -28664,8 +28687,8 @@
         <v>1DSB_R2_30bpDown</v>
       </c>
       <c r="N38" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv_30bpDown -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv_30bpDown -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -28721,8 +28744,8 @@
         <v>2DSBanti_R1</v>
       </c>
       <c r="N39" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
@@ -28778,8 +28801,8 @@
         <v>2DSBanti_R1</v>
       </c>
       <c r="N40" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_splicing -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_splicing -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
@@ -28835,8 +28858,8 @@
         <v>2DSBanti_R2</v>
       </c>
       <c r="N41" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
@@ -28892,8 +28915,8 @@
         <v>2DSBanti_R2</v>
       </c>
       <c r="N42" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_splicing -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_splicing -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -28993,8 +29016,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N45" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_nodsb -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_nodsb -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
@@ -29050,8 +29073,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N46" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch_nodsb -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch_nodsb -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
@@ -29107,8 +29130,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N47" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv_nodsb -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv_nodsb -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
@@ -29164,8 +29187,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N48" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_nodsb -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_nodsb -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
@@ -29221,8 +29244,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N49" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch_nodsb -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch_nodsb -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
@@ -29278,8 +29301,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N50" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv_nodsb -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv_nodsb -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
@@ -29335,8 +29358,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N51" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_nodsb -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_nodsb -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
@@ -29392,8 +29415,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N52" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch_nodsb -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch_nodsb -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
@@ -29449,8 +29472,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N53" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv_nodsb -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv_nodsb -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
@@ -29506,8 +29529,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N54" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_nodsb -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_nodsb -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
@@ -29563,8 +29586,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N55" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch_nodsb -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch_nodsb -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
@@ -29620,8 +29643,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N56" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv_nodsb -o plots/graphs/individual  -ext html</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv_nodsb -o plots/graphs/individual  -ext html --layout universal</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor updates to layout.
</commit_message>
<xml_diff>
--- a/libinfo.xlsx
+++ b/libinfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tchan\Code\SCMB_Project\RNA-mediated_DSB_repair\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC91ECD-A784-4706-BEDF-E525D5C78536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D296A792-47F6-4BBD-A733-3D0B38D568EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="5" activeTab="9" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="4" activeTab="9" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
   </bookViews>
   <sheets>
     <sheet name="globals" sheetId="3" r:id="rId1"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="191">
   <si>
     <t>yjl217</t>
   </si>
@@ -656,9 +656,6 @@
     <t>html</t>
   </si>
   <si>
-    <t>png</t>
-  </si>
-  <si>
     <t>layout</t>
   </si>
   <si>
@@ -766,7 +763,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -779,14 +776,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{FFD19645-61C4-4244-A560-0232B787F38C}"/>
   </cellStyles>
-  <dxfs count="202">
+  <dxfs count="203">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -799,9 +803,51 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -823,27 +869,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2141,7 +2166,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{70502F2F-AE2C-4D63-ADF7-F65702652EBF}" name="table_1_2" displayName="table_1_2" ref="A1:D108" totalsRowShown="0">
   <autoFilter ref="A1:D108" xr:uid="{70502F2F-AE2C-4D63-ADF7-F65702652EBF}"/>
   <tableColumns count="4">
-    <tableColumn id="2" xr3:uid="{BB99DCDA-08D4-474A-ABC3-5229CEAF80CF}" name="id" dataDxfId="201">
+    <tableColumn id="2" xr3:uid="{BB99DCDA-08D4-474A-ABC3-5229CEAF80CF}" name="id" dataDxfId="202">
       <calculatedColumnFormula>INT(MID(table_1_2[[#This Row],[library]], 4, 10))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{5F63B290-093A-48A3-9AFC-EB2FE27DE630}" name="library"/>
@@ -2153,44 +2178,44 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}" name="table_5_1" displayName="table_5_1" ref="A1:M41" totalsRowShown="0" headerRowDxfId="98">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}" name="table_5_1" displayName="table_5_1" ref="A1:M41" totalsRowShown="0" headerRowDxfId="99">
   <autoFilter ref="A1:M41" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
   <tableColumns count="13">
-    <tableColumn id="25" xr3:uid="{43F57146-0E56-46F3-A0E3-717A41010F4A}" name="index" dataDxfId="97"/>
-    <tableColumn id="1" xr3:uid="{B0B3F6B0-7577-49AC-B865-1E873B4DC53C}" name="dir" dataDxfId="96">
+    <tableColumn id="25" xr3:uid="{43F57146-0E56-46F3-A0E3-717A41010F4A}" name="index" dataDxfId="98"/>
+    <tableColumn id="1" xr3:uid="{B0B3F6B0-7577-49AC-B865-1E873B4DC53C}" name="dir" dataDxfId="97">
       <calculatedColumnFormula>table_3_1[[#This Row],[dir]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{D04F356F-9288-416D-ACDA-6BFE128B70D7}" name="control" dataDxfId="95">
+    <tableColumn id="13" xr3:uid="{D04F356F-9288-416D-ACDA-6BFE128B70D7}" name="control" dataDxfId="96">
       <calculatedColumnFormula>table_3_1[[#This Row],[control]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{9C168B22-F534-40D4-947C-918239C33FD9}" name="ref" dataDxfId="94">
+    <tableColumn id="2" xr3:uid="{9C168B22-F534-40D4-947C-918239C33FD9}" name="ref" dataDxfId="95">
       <calculatedColumnFormula>table_3_1[[#This Row],[ref]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{6F64477B-0C66-4251-9156-22307A6D70A0}" name="dsb_pos" dataDxfId="93">
+    <tableColumn id="3" xr3:uid="{6F64477B-0C66-4251-9156-22307A6D70A0}" name="dsb_pos" dataDxfId="94">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_pos]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{D037F4F2-543F-4D7D-AB36-0B253FD61B0D}" name="dsb_type" dataDxfId="92">
+    <tableColumn id="4" xr3:uid="{D037F4F2-543F-4D7D-AB36-0B253FD61B0D}" name="dsb_type" dataDxfId="93">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_type]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{407AC5E6-13CB-409A-8E78-64B8CC121882}" name="dsb_type_command" dataDxfId="91">
+    <tableColumn id="12" xr3:uid="{407AC5E6-13CB-409A-8E78-64B8CC121882}" name="dsb_type_command" dataDxfId="92">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_type_command]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{1A24C844-2A10-4394-818F-0C25A569B414}" name="strand" dataDxfId="90">
+    <tableColumn id="5" xr3:uid="{1A24C844-2A10-4394-818F-0C25A569B414}" name="strand" dataDxfId="91">
       <calculatedColumnFormula>table_3_1[[#This Row],[strand]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{4F0A02F9-5555-489E-BA41-E3CBF81D1114}" name="hguide" dataDxfId="89">
+    <tableColumn id="6" xr3:uid="{4F0A02F9-5555-489E-BA41-E3CBF81D1114}" name="hguide" dataDxfId="90">
       <calculatedColumnFormula>table_3_1[[#This Row],[hguide]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FAE741F2-7C1B-41F2-8875-9F7A2EF40A54}" name="cell" dataDxfId="88">
+    <tableColumn id="7" xr3:uid="{FAE741F2-7C1B-41F2-8875-9F7A2EF40A54}" name="cell" dataDxfId="89">
       <calculatedColumnFormula>table_3_1[[#This Row],[cell]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{FE3ED128-2534-43D1-9244-11AB1FB57650}" name="treatment" dataDxfId="87">
+    <tableColumn id="8" xr3:uid="{FE3ED128-2534-43D1-9244-11AB1FB57650}" name="treatment" dataDxfId="88">
       <calculatedColumnFormula>table_3_1[[#This Row],[treatment]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{65ACBC9C-0EC8-4074-B310-05F4B70BFAD5}" name="subst_type" dataDxfId="86">
+    <tableColumn id="9" xr3:uid="{65ACBC9C-0EC8-4074-B310-05F4B70BFAD5}" name="subst_type" dataDxfId="87">
       <calculatedColumnFormula>"with"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{F80F6FB9-4F35-4819-8285-D77131C6EFCE}" name="command" dataDxfId="85">
+    <tableColumn id="10" xr3:uid="{F80F6FB9-4F35-4819-8285-D77131C6EFCE}" name="command" dataDxfId="86">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2203,40 +2228,40 @@
   <autoFilter ref="A43:M55" xr:uid="{D74A5276-1A50-4DA1-9131-9669404C8622}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{8AC09A63-4226-4C75-8801-68CF93C0F078}" name="index"/>
-    <tableColumn id="2" xr3:uid="{77584C42-D70C-48A4-979A-F4DEA0B31542}" name="dir" dataDxfId="84">
+    <tableColumn id="2" xr3:uid="{77584C42-D70C-48A4-979A-F4DEA0B31542}" name="dir" dataDxfId="85">
       <calculatedColumnFormula>table_3_2[[#This Row],[dir]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{483E3D73-4059-4B65-84EC-5DC4E7008F35}" name="control" dataDxfId="83">
+    <tableColumn id="3" xr3:uid="{483E3D73-4059-4B65-84EC-5DC4E7008F35}" name="control" dataDxfId="84">
       <calculatedColumnFormula>table_3_2[[#This Row],[control]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5859A8DB-4C52-4451-BBB6-C6BEBF497540}" name="ref" dataDxfId="82">
+    <tableColumn id="4" xr3:uid="{5859A8DB-4C52-4451-BBB6-C6BEBF497540}" name="ref" dataDxfId="83">
       <calculatedColumnFormula>table_3_2[[#This Row],[ref]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{06FC4099-C18C-436C-B1E6-9739B71C7F22}" name="dsb_pos" dataDxfId="81">
+    <tableColumn id="5" xr3:uid="{06FC4099-C18C-436C-B1E6-9739B71C7F22}" name="dsb_pos" dataDxfId="82">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_pos]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8F043A8E-C5E7-4596-AE13-3E495C6DB33E}" name="dsb_type" dataDxfId="80">
+    <tableColumn id="6" xr3:uid="{8F043A8E-C5E7-4596-AE13-3E495C6DB33E}" name="dsb_type" dataDxfId="81">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_type]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E2DB136E-6FA9-4095-8B91-F094974333AF}" name="dsb_type_command" dataDxfId="79">
+    <tableColumn id="7" xr3:uid="{E2DB136E-6FA9-4095-8B91-F094974333AF}" name="dsb_type_command" dataDxfId="80">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_type_command]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{55CDC54E-3E43-4365-B1C9-5359F747A157}" name="strand" dataDxfId="78">
+    <tableColumn id="8" xr3:uid="{55CDC54E-3E43-4365-B1C9-5359F747A157}" name="strand" dataDxfId="79">
       <calculatedColumnFormula>table_3_2[[#This Row],[strand]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{056BD8A0-CC40-4C61-9F22-EE7382045F66}" name="hguide" dataDxfId="77">
+    <tableColumn id="9" xr3:uid="{056BD8A0-CC40-4C61-9F22-EE7382045F66}" name="hguide" dataDxfId="78">
       <calculatedColumnFormula>table_3_2[[#This Row],[hguide]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{489E156D-888A-4DDC-BB23-A4721D588249}" name="cell" dataDxfId="76">
+    <tableColumn id="10" xr3:uid="{489E156D-888A-4DDC-BB23-A4721D588249}" name="cell" dataDxfId="77">
       <calculatedColumnFormula>table_3_2[[#This Row],[cell]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{0F1B5F9E-B10D-4258-9052-90BCDC89F0B0}" name="treatment" dataDxfId="75">
+    <tableColumn id="11" xr3:uid="{0F1B5F9E-B10D-4258-9052-90BCDC89F0B0}" name="treatment" dataDxfId="76">
       <calculatedColumnFormula>table_3_2[[#This Row],[treatment]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A2723EF6-80E8-4D8D-A6DC-7556C1996222}" name="subst_type" dataDxfId="74">
+    <tableColumn id="12" xr3:uid="{A2723EF6-80E8-4D8D-A6DC-7556C1996222}" name="subst_type" dataDxfId="75">
       <calculatedColumnFormula>"with"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{02531CCA-6CDE-42BA-80E3-31C0F97A3546}" name="command" dataDxfId="73">
+    <tableColumn id="13" xr3:uid="{02531CCA-6CDE-42BA-80E3-31C0F97A3546}" name="command" dataDxfId="74">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2245,65 +2270,65 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E39D37F2-5006-44FB-A873-CCC98F8BA522}" name="table_6_1" displayName="table_6_1" ref="A1:T7" totalsRowShown="0" headerRowDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E39D37F2-5006-44FB-A873-CCC98F8BA522}" name="table_6_1" displayName="table_6_1" ref="A1:T7" totalsRowShown="0" headerRowDxfId="73">
   <autoFilter ref="A1:T7" xr:uid="{E39D37F2-5006-44FB-A873-CCC98F8BA522}"/>
   <tableColumns count="20">
-    <tableColumn id="25" xr3:uid="{CD5CCC3B-8B5B-4C20-98D1-63A7E1FB075B}" name="index" dataDxfId="71"/>
-    <tableColumn id="18" xr3:uid="{A6E432BE-5846-48EE-948A-BE81A4E2B6F5}" name="dir_1" dataDxfId="70">
+    <tableColumn id="25" xr3:uid="{CD5CCC3B-8B5B-4C20-98D1-63A7E1FB075B}" name="index" dataDxfId="72"/>
+    <tableColumn id="18" xr3:uid="{A6E432BE-5846-48EE-948A-BE81A4E2B6F5}" name="dir_1" dataDxfId="71">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_1]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{A826EC7B-673B-4DCB-8792-35762AD6C5ED}" name="dir_2" dataDxfId="69">
+    <tableColumn id="17" xr3:uid="{A826EC7B-673B-4DCB-8792-35762AD6C5ED}" name="dir_2" dataDxfId="70">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_2]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{F6910118-048E-4746-9072-727F3B1847FE}" name="dir_3" dataDxfId="68">
+    <tableColumn id="16" xr3:uid="{F6910118-048E-4746-9072-727F3B1847FE}" name="dir_3" dataDxfId="69">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_3]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{0BBECB52-3A0A-4374-9C43-DA21C4CA365C}" name="dir_4" dataDxfId="67">
+    <tableColumn id="15" xr3:uid="{0BBECB52-3A0A-4374-9C43-DA21C4CA365C}" name="dir_4" dataDxfId="68">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_4]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{6E2A95BE-29B1-4454-9E5B-BED35BBC5239}" name="dir_5" dataDxfId="66">
+    <tableColumn id="14" xr3:uid="{6E2A95BE-29B1-4454-9E5B-BED35BBC5239}" name="dir_5" dataDxfId="67">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_5]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{4BDBAB17-9D30-4F82-92E5-FBABD10C580E}" name="dir_6" dataDxfId="65">
+    <tableColumn id="1" xr3:uid="{4BDBAB17-9D30-4F82-92E5-FBABD10C580E}" name="dir_6" dataDxfId="66">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_6]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{8377C5E1-81CB-41A4-9754-5BDCCCB5D946}" name="dir_7" dataDxfId="64">
+    <tableColumn id="21" xr3:uid="{8377C5E1-81CB-41A4-9754-5BDCCCB5D946}" name="dir_7" dataDxfId="65">
       <calculatedColumnFormula array="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_7]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{0BBDCF08-0538-454A-A8A3-33839702EB7D}" name="dir_8" dataDxfId="63">
+    <tableColumn id="23" xr3:uid="{0BBDCF08-0538-454A-A8A3-33839702EB7D}" name="dir_8" dataDxfId="64">
       <calculatedColumnFormula array="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_8]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{362AFBD7-D8FE-484B-A796-99C68A4873AF}" name="dir_9" dataDxfId="62">
+    <tableColumn id="24" xr3:uid="{362AFBD7-D8FE-484B-A796-99C68A4873AF}" name="dir_9" dataDxfId="63">
       <calculatedColumnFormula array="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_9]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{F8401415-A0F2-4302-B6F1-2F4769D22B7D}" name="dir_10" dataDxfId="61">
+    <tableColumn id="26" xr3:uid="{F8401415-A0F2-4302-B6F1-2F4769D22B7D}" name="dir_10" dataDxfId="62">
       <calculatedColumnFormula array="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_10]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{EB5FA985-8547-4A83-8A97-6BDBC99AFC75}" name="dir_11" dataDxfId="60">
+    <tableColumn id="27" xr3:uid="{EB5FA985-8547-4A83-8A97-6BDBC99AFC75}" name="dir_11" dataDxfId="61">
       <calculatedColumnFormula array="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_11]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{531860AE-4501-4DFE-ABC6-8AEC03CA2891}" name="dir_12" dataDxfId="59">
+    <tableColumn id="28" xr3:uid="{531860AE-4501-4DFE-ABC6-8AEC03CA2891}" name="dir_12" dataDxfId="60">
       <calculatedColumnFormula array="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_12]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{991CDA96-8100-4EC0-BA2D-509D87E3B77E}" name="control" dataDxfId="58">
+    <tableColumn id="13" xr3:uid="{991CDA96-8100-4EC0-BA2D-509D87E3B77E}" name="control" dataDxfId="59">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 6 * (table_6_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AB636280-F214-4141-A265-B2AC639CF4A7}" name="dsb_type" dataDxfId="57">
+    <tableColumn id="4" xr3:uid="{AB636280-F214-4141-A265-B2AC639CF4A7}" name="dsb_type" dataDxfId="58">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], 6 * (table_6_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{56C39C59-71CD-4F29-9AA2-7C1BE588DDCF}" name="strand" dataDxfId="56">
+    <tableColumn id="5" xr3:uid="{56C39C59-71CD-4F29-9AA2-7C1BE588DDCF}" name="strand" dataDxfId="57">
       <calculatedColumnFormula>OFFSET(table_3_1[strand], 6 * (table_6_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{77B8B06C-E91A-4366-BAAD-4D98914358E6}" name="hguide" dataDxfId="55">
+    <tableColumn id="6" xr3:uid="{77B8B06C-E91A-4366-BAAD-4D98914358E6}" name="hguide" dataDxfId="56">
       <calculatedColumnFormula>OFFSET(table_3_1[hguide], 6 * (table_6_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{64A9E7E6-7F9F-4F61-9A23-E4157ABDCFAC}" name="subst_type" dataDxfId="54">
+    <tableColumn id="9" xr3:uid="{64A9E7E6-7F9F-4F61-9A23-E4157ABDCFAC}" name="subst_type" dataDxfId="55">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{B53E652A-5D37-4D63-8F38-4B8DBDB37226}" name="dir_out" dataDxfId="53">
+    <tableColumn id="19" xr3:uid="{B53E652A-5D37-4D63-8F38-4B8DBDB37226}" name="dir_out" dataDxfId="54">
       <calculatedColumnFormula>_xlfn.CONCAT(table_6_1[[#This Row],[dsb_type]], "_", table_6_1[[#This Row],[strand]], IF(table_6_1[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_1[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{9C3C4C97-49A2-40B9-BCC3-5739C07213CD}" name="command" dataDxfId="52">
+    <tableColumn id="10" xr3:uid="{9C3C4C97-49A2-40B9-BCC3-5739C07213CD}" name="command" dataDxfId="53">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", _xlfn.TEXTJOIN(" ", TRUE, table_6_1[[#This Row],[dir_1]:[dir_12]]), " -o ", layouts, "/", table_6_1[[#This Row],[dir_out]], " --subst_type ", table_6_1[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2312,35 +2337,35 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{5FFA4758-C47A-4F1C-9890-69E7F39BE130}" name="table_6_2" displayName="table_6_2" ref="A10:J12" totalsRowShown="0" headerRowDxfId="51" headerRowBorderDxfId="50" tableBorderDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{5FFA4758-C47A-4F1C-9890-69E7F39BE130}" name="table_6_2" displayName="table_6_2" ref="A10:J12" totalsRowShown="0" headerRowDxfId="52" headerRowBorderDxfId="51" tableBorderDxfId="50">
   <autoFilter ref="A10:J12" xr:uid="{5FFA4758-C47A-4F1C-9890-69E7F39BE130}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{40A0667B-C93C-4531-B41F-A65EDE89F51E}" name="index"/>
-    <tableColumn id="2" xr3:uid="{A54C9A1D-E384-4C87-B6DD-98A7ADBAD240}" name="dir_1" dataDxfId="48">
+    <tableColumn id="2" xr3:uid="{A54C9A1D-E384-4C87-B6DD-98A7ADBAD240}" name="dir_1" dataDxfId="49">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset - 1 + COLUMN() - 2 + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{7CACC7DC-6834-41E4-A17F-74F62473FF4D}" name="dir_2" dataDxfId="47">
+    <tableColumn id="3" xr3:uid="{7CACC7DC-6834-41E4-A17F-74F62473FF4D}" name="dir_2" dataDxfId="48">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset - 1 + COLUMN() - 2 + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{BEB4CA3E-14C3-4D70-BAFF-DBFFE398E04E}" name="control" dataDxfId="46">
+    <tableColumn id="4" xr3:uid="{BEB4CA3E-14C3-4D70-BAFF-DBFFE398E04E}" name="control" dataDxfId="47">
       <calculatedColumnFormula>OFFSET(table_3_1[control], var_6_anti_offset - 1 + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{08F18E8F-5127-4F55-95E0-05877340A45E}" name="dsb_type" dataDxfId="45">
+    <tableColumn id="5" xr3:uid="{08F18E8F-5127-4F55-95E0-05877340A45E}" name="dsb_type" dataDxfId="46">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], var_6_anti_offset - 1 + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B0010190-2798-4D5F-A1DA-8D1F1A867502}" name="strand" dataDxfId="44">
+    <tableColumn id="6" xr3:uid="{B0010190-2798-4D5F-A1DA-8D1F1A867502}" name="strand" dataDxfId="45">
       <calculatedColumnFormula array="1">OFFSET(table_3_1[strand], var_6_anti_offset - 1 + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{689C42CC-8508-4116-808A-19A0641C3F05}" name="hguide" dataDxfId="43">
+    <tableColumn id="7" xr3:uid="{689C42CC-8508-4116-808A-19A0641C3F05}" name="hguide" dataDxfId="44">
       <calculatedColumnFormula>OFFSET(table_3_1[hguide], var_6_anti_offset - 1 + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{48005280-1CD9-4496-941A-723AEDDD9036}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{5F8C6AF1-A602-4306-A909-592B4268C611}" name="dir_out" dataDxfId="42">
+    <tableColumn id="9" xr3:uid="{5F8C6AF1-A602-4306-A909-592B4268C611}" name="dir_out" dataDxfId="43">
       <calculatedColumnFormula>_xlfn.CONCAT(table_6_2[[#This Row],[dsb_type]], "_", table_6_2[[#This Row],[strand]], IF(table_6_2[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_2[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{3AEE0650-E928-4CB1-8CCF-22F967A16636}" name="command" dataDxfId="41">
+    <tableColumn id="10" xr3:uid="{3AEE0650-E928-4CB1-8CCF-22F967A16636}" name="command" dataDxfId="42">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", _xlfn.TEXTJOIN(" ", TRUE, table_6_2[[#This Row],[dir_1]:[dir_2]]), " -o ", layouts, "/", table_6_2[[#This Row],[dir_out]], " --subst_type ", table_6_2[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2349,47 +2374,47 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{86CE8E4A-18BF-427A-81F0-F9655767A016}" name="table_7_1" displayName="table_7_1" ref="A2:N42" totalsRowShown="0" headerRowDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{86CE8E4A-18BF-427A-81F0-F9655767A016}" name="table_7_1" displayName="table_7_1" ref="A2:N42" totalsRowShown="0" headerRowDxfId="41">
   <autoFilter ref="A2:N42" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
   <tableColumns count="14">
-    <tableColumn id="25" xr3:uid="{C323C376-24D3-4404-9E0F-6E9361862271}" name="index" dataDxfId="39"/>
-    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="38">
+    <tableColumn id="25" xr3:uid="{C323C376-24D3-4404-9E0F-6E9361862271}" name="index" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="39">
       <calculatedColumnFormula>OFFSET(table_3_1[[dir]:[dir]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="37">
+    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="38">
       <calculatedColumnFormula>OFFSET(table_3_1[[control]:[control]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="36">
+    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="37">
       <calculatedColumnFormula>OFFSET(table_3_1[[ref]:[ref]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="35">
+    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="36">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_pos]:[dsb_pos]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="34">
+    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="35">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_type]:[dsb_type]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="33">
+    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="34">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_type_command]:[dsb_type_command]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="32">
+    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="33">
       <calculatedColumnFormula>OFFSET(table_3_1[[strand]:[strand]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="31">
+    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="32">
       <calculatedColumnFormula>OFFSET(table_3_1[[hguide]:[hguide]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="30">
+    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="31">
       <calculatedColumnFormula>OFFSET(table_3_1[[cell]:[cell]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="29">
+    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="30">
       <calculatedColumnFormula>OFFSET(table_3_1[[treatment]:[treatment]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="28">
+    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="29">
       <calculatedColumnFormula>"without"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="27">
+    <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="28">
       <calculatedColumnFormula>IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="2">
+    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="7">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2401,44 +2426,44 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{B47D9508-D874-40FC-B6F6-C106B48F6A94}" name="table_7_2" displayName="table_7_2" ref="A44:N56" totalsRowShown="0">
   <autoFilter ref="A44:N56" xr:uid="{D74A5276-1A50-4DA1-9131-9669404C8622}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{488C5146-A746-4F74-BCC8-806E4DC740CE}" name="index" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{C2A88DF4-2444-4C4C-A089-6CF9ADE79BD8}" name="dir" dataDxfId="25">
+    <tableColumn id="1" xr3:uid="{488C5146-A746-4F74-BCC8-806E4DC740CE}" name="index" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{C2A88DF4-2444-4C4C-A089-6CF9ADE79BD8}" name="dir" dataDxfId="26">
       <calculatedColumnFormula>OFFSET(table_3_2[[dir]:[dir]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{7698ACE3-2351-400D-B00F-5A70184F8A33}" name="control" dataDxfId="24">
+    <tableColumn id="3" xr3:uid="{7698ACE3-2351-400D-B00F-5A70184F8A33}" name="control" dataDxfId="25">
       <calculatedColumnFormula>OFFSET(table_3_2[[control]:[control]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5E82B04C-FF09-492C-8A23-7E43B5990149}" name="ref" dataDxfId="23">
+    <tableColumn id="4" xr3:uid="{5E82B04C-FF09-492C-8A23-7E43B5990149}" name="ref" dataDxfId="24">
       <calculatedColumnFormula>OFFSET(table_3_2[[ref]:[ref]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{F4D36A0E-549B-4F3A-BCA9-75E151448998}" name="dsb_pos" dataDxfId="22">
+    <tableColumn id="5" xr3:uid="{F4D36A0E-549B-4F3A-BCA9-75E151448998}" name="dsb_pos" dataDxfId="23">
       <calculatedColumnFormula>OFFSET(table_3_2[[dsb_pos]:[dsb_pos]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{AEBBBB88-8CE2-409D-AE19-9C23263250A9}" name="dsb_type" dataDxfId="21">
+    <tableColumn id="6" xr3:uid="{AEBBBB88-8CE2-409D-AE19-9C23263250A9}" name="dsb_type" dataDxfId="22">
       <calculatedColumnFormula>OFFSET(table_3_2[[dsb_type]:[dsb_type]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3E71E7D2-0FA5-4FD5-BDC3-2955A091A9E6}" name="dsb_type_command" dataDxfId="20">
+    <tableColumn id="7" xr3:uid="{3E71E7D2-0FA5-4FD5-BDC3-2955A091A9E6}" name="dsb_type_command" dataDxfId="21">
       <calculatedColumnFormula>OFFSET(table_3_2[[dsb_type_command]:[dsb_type_command]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{EBD35881-E696-4202-9149-75A4EFFFAAD6}" name="strand" dataDxfId="19">
+    <tableColumn id="8" xr3:uid="{EBD35881-E696-4202-9149-75A4EFFFAAD6}" name="strand" dataDxfId="20">
       <calculatedColumnFormula>OFFSET(table_3_2[[strand]:[strand]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{123CA279-0CB6-41C1-9CD8-20D375B9B66D}" name="hguide" dataDxfId="18">
+    <tableColumn id="9" xr3:uid="{123CA279-0CB6-41C1-9CD8-20D375B9B66D}" name="hguide" dataDxfId="19">
       <calculatedColumnFormula>OFFSET(table_3_2[[hguide]:[hguide]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{3DCE3F3A-187D-411E-93FC-8C6C3EE9CAA2}" name="cell" dataDxfId="17">
+    <tableColumn id="10" xr3:uid="{3DCE3F3A-187D-411E-93FC-8C6C3EE9CAA2}" name="cell" dataDxfId="18">
       <calculatedColumnFormula>OFFSET(table_3_2[[cell]:[cell]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{9E585D29-AB3E-4D04-8C1D-24F78339C9A3}" name="treatment" dataDxfId="16">
+    <tableColumn id="11" xr3:uid="{9E585D29-AB3E-4D04-8C1D-24F78339C9A3}" name="treatment" dataDxfId="17">
       <calculatedColumnFormula>OFFSET(table_3_2[[treatment]:[treatment]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{928286B8-23FB-4375-B52B-617DD59D6098}" name="subst_type" dataDxfId="15">
+    <tableColumn id="12" xr3:uid="{928286B8-23FB-4375-B52B-617DD59D6098}" name="subst_type" dataDxfId="16">
       <calculatedColumnFormula>"without"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{E18D2025-56E8-4128-9201-9E0BF8A67AC0}" name="common_layout_dir" dataDxfId="14">
+    <tableColumn id="15" xr3:uid="{E18D2025-56E8-4128-9201-9E0BF8A67AC0}" name="common_layout_dir" dataDxfId="15">
       <calculatedColumnFormula>OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_2[[#This Row],[index]] - 1, 6) + 2, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{0917AB98-1545-4642-9BE8-618AAA1E404A}" name="command" dataDxfId="1">
+    <tableColumn id="13" xr3:uid="{0917AB98-1545-4642-9BE8-618AAA1E404A}" name="command" dataDxfId="6">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2447,15 +2472,15 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{B76EEC45-4FC3-44D5-9B2E-9183DF724F60}" name="table_7_3" displayName="table_7_3" ref="A3:C19" totalsRowShown="0" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{B76EEC45-4FC3-44D5-9B2E-9183DF724F60}" name="table_7_3" displayName="table_7_3" ref="A3:C19" totalsRowShown="0" headerRowDxfId="14">
   <autoFilter ref="A3:C19" xr:uid="{B76EEC45-4FC3-44D5-9B2E-9183DF724F60}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{FAFADB73-BF3B-401A-8C48-9FCB5D3C4CB6}" name="index" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{8541A14E-3250-4B9C-B315-969FC11BE60A}" name="dir" dataDxfId="11">
+    <tableColumn id="1" xr3:uid="{FAFADB73-BF3B-401A-8C48-9FCB5D3C4CB6}" name="index" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{8541A14E-3250-4B9C-B315-969FC11BE60A}" name="dir" dataDxfId="12">
       <calculatedColumnFormula>OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{EAD6D5EC-B61E-4A98-B4FD-4932757CFEA3}" name="command" dataDxfId="0">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{EAD6D5EC-B61E-4A98-B4FD-4932757CFEA3}" name="command" dataDxfId="4">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2463,15 +2488,15 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{8B4E853A-A4F1-4022-B857-226C57559A5F}" name="table_7_4" displayName="table_7_4" ref="A21:C23" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{8B4E853A-A4F1-4022-B857-226C57559A5F}" name="table_7_4" displayName="table_7_4" ref="A21:C23" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="A21:C23" xr:uid="{8B4E853A-A4F1-4022-B857-226C57559A5F}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{1ECF32A2-E353-4754-B4C5-11C46AACF6C0}" name="index" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{181C59FC-364D-4421-8E54-98DFF4CA7C05}" name="dir" dataDxfId="8">
+    <tableColumn id="1" xr3:uid="{1ECF32A2-E353-4754-B4C5-11C46AACF6C0}" name="index" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{181C59FC-364D-4421-8E54-98DFF4CA7C05}" name="dir" dataDxfId="9">
       <calculatedColumnFormula>OFFSET(table_4_2[[dir_out]:[dir_out]], table_7_4[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{6D8CC942-572B-44F2-BCA6-4D31A25A4067}" name="command" dataDxfId="7">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_4[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_2[[dir_out]:[dir_out]],table_7_4[[#This Row],[index]] - 1, 0, 1, 1)), ""), " -ext ", var_7_ext_combined)</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{6D8CC942-572B-44F2-BCA6-4D31A25A4067}" name="command" dataDxfId="5">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_4[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_2[[dir_out]:[dir_out]],table_7_4[[#This Row],[index]] - 1, 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2479,15 +2504,15 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{58F5EC27-BD76-45AE-8D38-F4E705EF79E9}" name="table_7_5" displayName="table_7_5" ref="A26:C34" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{58F5EC27-BD76-45AE-8D38-F4E705EF79E9}" name="table_7_5" displayName="table_7_5" ref="A26:C34" totalsRowShown="0" headerRowDxfId="8" dataDxfId="0">
   <autoFilter ref="A26:C34" xr:uid="{58F5EC27-BD76-45AE-8D38-F4E705EF79E9}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{AAC1476C-44CE-49FD-8254-50BAEAA6929C}" name="index" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{1222E48F-ED5C-48AA-BA39-1443B841BC9F}" name="dir" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{AAC1476C-44CE-49FD-8254-50BAEAA6929C}" name="index" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{1222E48F-ED5C-48AA-BA39-1443B841BC9F}" name="dir" dataDxfId="2">
       <calculatedColumnFormula>OFFSET(table_4_3[[dir_out]:[dir_out]], table_7_5[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{89B7E589-2097-43FC-B96B-19D2EF777E97}" name="command_main_data_combined" dataDxfId="3">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined)</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{89B7E589-2097-43FC-B96B-19D2EF777E97}" name="command" dataDxfId="1">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2495,10 +2520,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22A90416-B904-4D3D-A6DB-EFCB9FD1EAED}" name="table_1" displayName="table_1" ref="A1:O173" totalsRowShown="0" headerRowDxfId="200">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22A90416-B904-4D3D-A6DB-EFCB9FD1EAED}" name="table_1" displayName="table_1" ref="A1:O173" totalsRowShown="0" headerRowDxfId="201">
   <autoFilter ref="A1:O173" xr:uid="{22A90416-B904-4D3D-A6DB-EFCB9FD1EAED}"/>
   <tableColumns count="15">
-    <tableColumn id="15" xr3:uid="{A06DA701-31D6-44A5-8655-82CAD7E3082B}" name="index" dataDxfId="199"/>
+    <tableColumn id="15" xr3:uid="{A06DA701-31D6-44A5-8655-82CAD7E3082B}" name="index" dataDxfId="200"/>
     <tableColumn id="1" xr3:uid="{5C1CDEE9-AAC7-4E12-B88F-1314CF422335}" name="library"/>
     <tableColumn id="2" xr3:uid="{D4B174CF-F774-4DA7-B75D-573BC94EE10F}" name="cell"/>
     <tableColumn id="3" xr3:uid="{83898EC9-96DA-46D4-B0B8-F68C7607DCF2}" name="control"/>
@@ -2506,25 +2531,25 @@
     <tableColumn id="5" xr3:uid="{81A143FE-8E74-4182-8124-E697DD5A7C62}" name="hguide"/>
     <tableColumn id="6" xr3:uid="{4A316E6A-69F3-4B78-9C01-4675AEB656FA}" name="treatment"/>
     <tableColumn id="7" xr3:uid="{25B8E763-346D-4756-8B58-D3C8CB103545}" name="strand"/>
-    <tableColumn id="8" xr3:uid="{4B708639-BB19-4DC1-A57D-214FA0EFB1EA}" name="dsb_pos" dataDxfId="198">
+    <tableColumn id="8" xr3:uid="{4B708639-BB19-4DC1-A57D-214FA0EFB1EA}" name="dsb_pos" dataDxfId="199">
       <calculatedColumnFormula array="1">IF(E2="2DSB", IF(H2="R1", 67, 46), IF(E2="1DSB", IF(H2="R1", 67, 46), IF(E2="2DSBanti", IF(H2="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{CCF6021C-1B60-4954-A92E-3F2848564215}" name="file_in" dataDxfId="197">
+    <tableColumn id="9" xr3:uid="{CCF6021C-1B60-4954-A92E-3F2848564215}" name="file_in" dataDxfId="198">
       <calculatedColumnFormula>IF(OR(table_1[[#This Row],[control]]="none", table_1[[#This Row],[control]]="30bpDown"), _xlfn.CONCAT(table_1[[#This Row],[library]], IF(table_1[[#This Row],[dsb_type]] = "2DSBanti", "_anti", ""), "_",table_1[[#This Row],[strand]],"_", IF(LEFT(table_1[[#This Row],[dsb_type]], 1)="2","2DSBs", table_1[[#This Row],[hguide]]), ".sam"), _xlfn.CONCAT(table_1[[#This Row],[library]], "_NHEJ_", IF(table_1[[#This Row],[hguide]]="sgA", "hg39", IF(table_1[[#This Row],[hguide]]="sgB", "hg42", "2DSB")), "_", table_1[[#This Row],[strand]], ".sam"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{58220462-2A11-4DAD-A247-C0871AFCFDB4}" name="file_out" dataDxfId="196">
+    <tableColumn id="10" xr3:uid="{58220462-2A11-4DAD-A247-C0871AFCFDB4}" name="file_out" dataDxfId="197">
       <calculatedColumnFormula>_xlfn.CONCAT(table_1[[#This Row],[library]], "_", table_1[[#This Row],[cell]], "_", table_1[[#This Row],[hguide]], "_", table_1[[#This Row],[strand]], "_", table_1[[#This Row],[treatment]], IF(table_1[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_1[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{775EE7A9-3C78-4568-BF98-500DE451177C}" name="ref" dataDxfId="195">
+    <tableColumn id="11" xr3:uid="{775EE7A9-3C78-4568-BF98-500DE451177C}" name="ref" dataDxfId="196">
       <calculatedColumnFormula>_xlfn.CONCAT(table_1[[#This Row],[dsb_type]],"_", table_1[[#This Row],[strand]],"_", table_1[[#This Row],[treatment]], ".fa")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{5B945FB6-D054-40C4-AAEF-BB50B19F8936}" name="total_reads" dataDxfId="194">
+    <tableColumn id="12" xr3:uid="{5B945FB6-D054-40C4-AAEF-BB50B19F8936}" name="total_reads" dataDxfId="195">
       <calculatedColumnFormula>VLOOKUP(INT(MID(table_1[[#This Row],[library]], 4, 10)), table_1_2[#All], IF(table_1[[#This Row],[strand]]="R1", 3, 4))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{66485B06-471E-47D3-BA91-FC751F58FA5A}" name="min_length" dataDxfId="193">
+    <tableColumn id="13" xr3:uid="{66485B06-471E-47D3-BA91-FC751F58FA5A}" name="min_length" dataDxfId="194">
       <calculatedColumnFormula>IF(LEFT(table_1[[#This Row],[dsb_type]], 1) = "2", 50, 130)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{DF3C46EA-690D-4E6A-99CF-BBC2B2F74AFF}" name="command_filter_nhej" dataDxfId="192">
+    <tableColumn id="14" xr3:uid="{DF3C46EA-690D-4E6A-99CF-BBC2B2F74AFF}" name="command_filter_nhej" dataDxfId="193">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", table_1[[#This Row],[file_in]], " -ref ref_seq/", table_1[[#This Row],[ref]], " -o ", libraries_2, "/", table_1[[#This Row],[file_out]], ".tsv", " --min_length ", table_1[[#This Row],[min_length]], " -dsb ", table_1[[#This Row],[dsb_pos]], " --quiet")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2533,38 +2558,38 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}" name="table_2_1" displayName="table_2_1" ref="A1:S41" totalsRowShown="0" headerRowDxfId="191">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}" name="table_2_1" displayName="table_2_1" ref="A1:S41" totalsRowShown="0" headerRowDxfId="192">
   <autoFilter ref="A1:S41" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{C373869E-A92E-4B06-B8E5-C5A873420ED4}" name="index" dataDxfId="190"/>
-    <tableColumn id="2" xr3:uid="{A28AAC50-FA09-494A-B052-8489F07A5A70}" name="ref" dataDxfId="189">
+    <tableColumn id="1" xr3:uid="{C373869E-A92E-4B06-B8E5-C5A873420ED4}" name="index" dataDxfId="191"/>
+    <tableColumn id="2" xr3:uid="{A28AAC50-FA09-494A-B052-8489F07A5A70}" name="ref" dataDxfId="190">
       <calculatedColumnFormula>OFFSET(table_1[ref], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{07D57089-9737-4983-8884-C4ACCDCFF6CB}" name="control" dataDxfId="188">
+    <tableColumn id="18" xr3:uid="{07D57089-9737-4983-8884-C4ACCDCFF6CB}" name="control" dataDxfId="189">
       <calculatedColumnFormula>OFFSET(table_1[control], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{C6423FEA-272F-48D3-BC6A-909FCA937DA9}" name="dsb_type" dataDxfId="187">
+    <tableColumn id="19" xr3:uid="{C6423FEA-272F-48D3-BC6A-909FCA937DA9}" name="dsb_type" dataDxfId="188">
       <calculatedColumnFormula>OFFSET(table_1[dsb_type], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B8F61088-5FFA-4860-BF4E-1BFB301A31D9}" name="dsb_pos" dataDxfId="186">
+    <tableColumn id="3" xr3:uid="{B8F61088-5FFA-4860-BF4E-1BFB301A31D9}" name="dsb_pos" dataDxfId="187">
       <calculatedColumnFormula>OFFSET(table_1[dsb_pos], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{524D5B3D-BB20-420D-B7E9-93A7F77CA728}" name="cell" dataDxfId="185">
+    <tableColumn id="4" xr3:uid="{524D5B3D-BB20-420D-B7E9-93A7F77CA728}" name="cell" dataDxfId="186">
       <calculatedColumnFormula>OFFSET(table_1[cell], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{CC918D20-5D79-4223-9717-2CA0EFFA213F}" name="strand" dataDxfId="184">
+    <tableColumn id="5" xr3:uid="{CC918D20-5D79-4223-9717-2CA0EFFA213F}" name="strand" dataDxfId="185">
       <calculatedColumnFormula>OFFSET(table_1[strand], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B2851465-D533-4787-80C4-E844BB2ABB8C}" name="treatment" dataDxfId="183">
+    <tableColumn id="6" xr3:uid="{B2851465-D533-4787-80C4-E844BB2ABB8C}" name="treatment" dataDxfId="184">
       <calculatedColumnFormula>OFFSET(table_1[treatment], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{849BE448-7739-4815-A2C5-5843F62D83D7}" name="hguide" dataDxfId="182">
+    <tableColumn id="7" xr3:uid="{849BE448-7739-4815-A2C5-5843F62D83D7}" name="hguide" dataDxfId="183">
       <calculatedColumnFormula>OFFSET(table_1[hguide], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{343716D9-C3A9-4F90-A58A-42B1B9C79EBF}" name="output_dir" dataDxfId="181">
+    <tableColumn id="8" xr3:uid="{343716D9-C3A9-4F90-A58A-42B1B9C79EBF}" name="output_dir" dataDxfId="182">
       <calculatedColumnFormula>_xlfn.CONCAT(table_2_1[[#This Row],[cell]], "_", table_2_1[[#This Row],[hguide]], "_", table_2_1[[#This Row],[strand]], "_", table_2_1[[#This Row],[treatment]], IF(table_2_1[[#This Row],[control]]&lt;&gt;"none",_xlfn.CONCAT("_", table_2_1[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D29558AA-D418-4CDD-81AE-A987E7BC501D}" name="input_1" dataDxfId="180">
+    <tableColumn id="9" xr3:uid="{D29558AA-D418-4CDD-81AE-A987E7BC501D}" name="input_1" dataDxfId="181">
       <calculatedColumnFormula array="1">OFFSET(table_1[[file_out]:[file_out]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 11, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="22" xr3:uid="{3F29C0D1-58A3-430E-AAAA-9F679DCA46D6}" name="input_2">
@@ -2576,19 +2601,19 @@
     <tableColumn id="20" xr3:uid="{28521A62-94B3-4C7C-AF90-F4E2F4163D29}" name="input_4">
       <calculatedColumnFormula array="1">OFFSET(table_1[[file_out]:[file_out]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 11, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{E2ABF5A3-B032-47F7-9141-9F269EFD9D49}" name="total_reads_1" dataDxfId="179">
+    <tableColumn id="10" xr3:uid="{E2ABF5A3-B032-47F7-9141-9F269EFD9D49}" name="total_reads_1" dataDxfId="180">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{C7B1BE14-3BD6-413B-8575-DE9712F9761A}" name="total_reads_2" dataDxfId="178">
+    <tableColumn id="12" xr3:uid="{C7B1BE14-3BD6-413B-8575-DE9712F9761A}" name="total_reads_2" dataDxfId="179">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{6A8CE344-45B9-42E3-95D8-8EB6A485D968}" name="total_reads_3" dataDxfId="177">
+    <tableColumn id="14" xr3:uid="{6A8CE344-45B9-42E3-95D8-8EB6A485D968}" name="total_reads_3" dataDxfId="178">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{AC170216-9CAE-43B8-A8E2-8FE1529F6D55}" name="total_reads_4" dataDxfId="176">
+    <tableColumn id="16" xr3:uid="{AC170216-9CAE-43B8-A8E2-8FE1529F6D55}" name="total_reads_4" dataDxfId="177">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{A285A0DD-6F6D-404D-AE2A-0D1FC3DDB459}" name="command" dataDxfId="175">
+    <tableColumn id="17" xr3:uid="{A285A0DD-6F6D-404D-AE2A-0D1FC3DDB459}" name="command" dataDxfId="176">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2600,41 +2625,41 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{7D969AC7-2D2F-45B0-BA99-D174130B0A52}" name="table_2_2" displayName="table_2_2" ref="A44:M56" totalsRowShown="0">
   <autoFilter ref="A44:M56" xr:uid="{7D969AC7-2D2F-45B0-BA99-D174130B0A52}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{D612E3DF-AA8E-4EE0-9306-7903B4821992}" name="index" dataDxfId="174"/>
-    <tableColumn id="2" xr3:uid="{B00239B6-16E0-4472-B8C9-F25D625D21DD}" name="ref" dataDxfId="173">
+    <tableColumn id="1" xr3:uid="{D612E3DF-AA8E-4EE0-9306-7903B4821992}" name="index" dataDxfId="175"/>
+    <tableColumn id="2" xr3:uid="{B00239B6-16E0-4472-B8C9-F25D625D21DD}" name="ref" dataDxfId="174">
       <calculatedColumnFormula>OFFSET(table_1[ref], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{47FE94A7-C208-4138-B063-127D4AE215A0}" name="control" dataDxfId="172">
+    <tableColumn id="3" xr3:uid="{47FE94A7-C208-4138-B063-127D4AE215A0}" name="control" dataDxfId="173">
       <calculatedColumnFormula>OFFSET(table_1[control], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{43B4F550-AB35-4206-AAAB-820BBA723DEA}" name="dsb_type" dataDxfId="171">
+    <tableColumn id="4" xr3:uid="{43B4F550-AB35-4206-AAAB-820BBA723DEA}" name="dsb_type" dataDxfId="172">
       <calculatedColumnFormula>OFFSET(table_1[dsb_type], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7233C674-8249-48C9-814C-599A94DF6097}" name="dsb_pos" dataDxfId="170">
+    <tableColumn id="5" xr3:uid="{7233C674-8249-48C9-814C-599A94DF6097}" name="dsb_pos" dataDxfId="171">
       <calculatedColumnFormula>OFFSET(table_1[dsb_pos], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8FD419DF-3888-4BC8-ACF7-F31E7AB24754}" name="cell" dataDxfId="169">
+    <tableColumn id="6" xr3:uid="{8FD419DF-3888-4BC8-ACF7-F31E7AB24754}" name="cell" dataDxfId="170">
       <calculatedColumnFormula>OFFSET(table_1[cell], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{612FF909-1004-49E1-BC8F-F65A8C97EEFC}" name="strand" dataDxfId="168">
+    <tableColumn id="7" xr3:uid="{612FF909-1004-49E1-BC8F-F65A8C97EEFC}" name="strand" dataDxfId="169">
       <calculatedColumnFormula>OFFSET(table_1[strand], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C57AB4D7-F308-46D6-8F19-069619F8CF1B}" name="treatment" dataDxfId="167">
+    <tableColumn id="8" xr3:uid="{C57AB4D7-F308-46D6-8F19-069619F8CF1B}" name="treatment" dataDxfId="168">
       <calculatedColumnFormula>OFFSET(table_1[treatment], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{27DAC4C9-BDB2-4621-A4F1-0094D063284E}" name="hguide" dataDxfId="166">
+    <tableColumn id="9" xr3:uid="{27DAC4C9-BDB2-4621-A4F1-0094D063284E}" name="hguide" dataDxfId="167">
       <calculatedColumnFormula>OFFSET(table_1[hguide], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{E0E9E8C1-4E85-4EFB-8220-84140FBAAF8E}" name="output_dir" dataDxfId="165">
+    <tableColumn id="10" xr3:uid="{E0E9E8C1-4E85-4EFB-8220-84140FBAAF8E}" name="output_dir" dataDxfId="166">
       <calculatedColumnFormula>_xlfn.CONCAT(table_2_2[[#This Row],[cell]], "_", table_2_2[[#This Row],[hguide]], "_", table_2_2[[#This Row],[strand]], "_", table_2_2[[#This Row],[treatment]], "_nodsb")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{CAC474F1-3930-4766-B491-65C86C5752E8}" name="input" dataDxfId="164">
+    <tableColumn id="11" xr3:uid="{CAC474F1-3930-4766-B491-65C86C5752E8}" name="input" dataDxfId="165">
       <calculatedColumnFormula>OFFSET(table_1[file_out], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{BB84920E-3487-4670-93ED-5671EACD3061}" name="total_reads" dataDxfId="163">
+    <tableColumn id="12" xr3:uid="{BB84920E-3487-4670-93ED-5671EACD3061}" name="total_reads" dataDxfId="164">
       <calculatedColumnFormula>OFFSET(table_1[total_reads], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{0CE6DAF6-0C4C-4EC5-8FE5-9B3840A02412}" name="command" dataDxfId="162">
+    <tableColumn id="13" xr3:uid="{0CE6DAF6-0C4C-4EC5-8FE5-9B3840A02412}" name="command" dataDxfId="163">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_2[[#This Row],[input]], ".tsv ", " --total_reads ", table_2_2[[#This Row],[total_reads]], " -o ", libraries_3, "/", table_2_2[[#This Row],[output_dir]], ".tsv", " --quiet ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2643,47 +2668,47 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}" name="table_3_1" displayName="table_3_1" ref="A1:N41" totalsRowShown="0" headerRowDxfId="161">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}" name="table_3_1" displayName="table_3_1" ref="A1:N41" totalsRowShown="0" headerRowDxfId="162">
   <autoFilter ref="A1:N41" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}"/>
   <tableColumns count="14">
-    <tableColumn id="25" xr3:uid="{93D2F09B-24D5-4FE1-BF34-C037E361889F}" name="index" dataDxfId="160"/>
-    <tableColumn id="1" xr3:uid="{2F28DC66-449D-4F81-AA63-8F24B25F33D1}" name="dir" dataDxfId="159">
+    <tableColumn id="25" xr3:uid="{93D2F09B-24D5-4FE1-BF34-C037E361889F}" name="index" dataDxfId="161"/>
+    <tableColumn id="1" xr3:uid="{2F28DC66-449D-4F81-AA63-8F24B25F33D1}" name="dir" dataDxfId="160">
       <calculatedColumnFormula>OFFSET(table_2_1[output_dir], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{3DF6F698-1F9A-4B05-A310-657CCFCE9F66}" name="control" dataDxfId="158">
+    <tableColumn id="13" xr3:uid="{3DF6F698-1F9A-4B05-A310-657CCFCE9F66}" name="control" dataDxfId="159">
       <calculatedColumnFormula>OFFSET(table_2_1[control], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{362C2395-52F7-4A62-B7BA-2DD97ED5E6FB}" name="ref" dataDxfId="157">
+    <tableColumn id="2" xr3:uid="{362C2395-52F7-4A62-B7BA-2DD97ED5E6FB}" name="ref" dataDxfId="158">
       <calculatedColumnFormula>OFFSET(table_2_1[ref], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5F0895D9-2EF2-4524-8BC7-15A33FE68636}" name="dsb_pos" dataDxfId="156">
+    <tableColumn id="3" xr3:uid="{5F0895D9-2EF2-4524-8BC7-15A33FE68636}" name="dsb_pos" dataDxfId="157">
       <calculatedColumnFormula>OFFSET(table_2_1[dsb_pos], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C6D28829-46E6-4D97-8EA4-0AD12EF6CF10}" name="dsb_type" dataDxfId="155">
+    <tableColumn id="4" xr3:uid="{C6D28829-46E6-4D97-8EA4-0AD12EF6CF10}" name="dsb_type" dataDxfId="156">
       <calculatedColumnFormula>OFFSET(table_2_1[dsb_type], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{E8B2E211-C273-4602-86F0-60EA4259B7A4}" name="dsb_type_command" dataDxfId="154">
+    <tableColumn id="12" xr3:uid="{E8B2E211-C273-4602-86F0-60EA4259B7A4}" name="dsb_type_command" dataDxfId="155">
       <calculatedColumnFormula array="1">IF(table_3_1[[#This Row],[dsb_type]]="2DSB", "2", IF(table_3_1[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(table_3_1[[#This Row],[dsb_type]]="1DSB", "1", NA)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{15578E86-B7BE-4D8E-8FD4-E6C9C4F35C9C}" name="strand" dataDxfId="153">
+    <tableColumn id="5" xr3:uid="{15578E86-B7BE-4D8E-8FD4-E6C9C4F35C9C}" name="strand" dataDxfId="154">
       <calculatedColumnFormula>OFFSET(table_2_1[strand], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3366AC40-6578-4797-B607-19265E7DBF5C}" name="hguide" dataDxfId="152">
+    <tableColumn id="6" xr3:uid="{3366AC40-6578-4797-B607-19265E7DBF5C}" name="hguide" dataDxfId="153">
       <calculatedColumnFormula>MID(OFFSET(table_2_1[hguide], table_3_1[[#This Row],[index]] - 1, 0, 1, 1), 3, 100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{554F4E79-98DE-474B-A5C8-D4B536772E95}" name="cell" dataDxfId="151">
+    <tableColumn id="7" xr3:uid="{554F4E79-98DE-474B-A5C8-D4B536772E95}" name="cell" dataDxfId="152">
       <calculatedColumnFormula>OFFSET(table_2_1[cell], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{32FC5061-DD85-4234-9ED8-FEAF6D9E3BC0}" name="treatment" dataDxfId="150">
+    <tableColumn id="8" xr3:uid="{32FC5061-DD85-4234-9ED8-FEAF6D9E3BC0}" name="treatment" dataDxfId="151">
       <calculatedColumnFormula>OFFSET(table_2_1[treatment], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{DB6998A3-1431-4DDD-8DA0-525B805BF436}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{367B0912-E7A8-4430-962D-4F79EE14E5EA}" name="command_main_data" dataDxfId="149">
+    <tableColumn id="10" xr3:uid="{367B0912-E7A8-4430-962D-4F79EE14E5EA}" name="command_main_data" dataDxfId="150">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_1[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_1[[#This Row],[dir]], " -ref ref_seq/", table_3_1[[#This Row],[ref]], " -dsb ", table_3_1[[#This Row],[dsb_pos]], " --dsb_type ",table_3_1[[#This Row],[dsb_type_command]], " --strand ", table_3_1[[#This Row],[strand]], " --hguide ", table_3_1[[#This Row],[hguide]], " --cell ", table_3_1[[#This Row],[cell]], " --treatment ", table_3_1[[#This Row],[treatment]], " --subst_type ", table_3_1[[#This Row],[subst_type]], " --control ", table_3_1[[#This Row],[control]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{4A65279E-321E-4E3E-8383-26D448C2012F}" name="command_graph_data" dataDxfId="148">
+    <tableColumn id="11" xr3:uid="{4A65279E-321E-4E3E-8383-26D448C2012F}" name="command_graph_data" dataDxfId="149">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_1[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_1[[#This Row],[dir]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2692,47 +2717,47 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}" name="table_3_2" displayName="table_3_2" ref="A43:N55" totalsRowShown="0" headerRowDxfId="147">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}" name="table_3_2" displayName="table_3_2" ref="A43:N55" totalsRowShown="0" headerRowDxfId="148">
   <autoFilter ref="A43:N55" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}"/>
   <tableColumns count="14">
-    <tableColumn id="25" xr3:uid="{B2894846-EBB9-47DC-8DE1-7F1DA571A0B9}" name="index" dataDxfId="146"/>
-    <tableColumn id="1" xr3:uid="{98269DFC-71F0-4066-B063-59597431C1C3}" name="dir" dataDxfId="145">
+    <tableColumn id="25" xr3:uid="{B2894846-EBB9-47DC-8DE1-7F1DA571A0B9}" name="index" dataDxfId="147"/>
+    <tableColumn id="1" xr3:uid="{98269DFC-71F0-4066-B063-59597431C1C3}" name="dir" dataDxfId="146">
       <calculatedColumnFormula>OFFSET(table_2_2[output_dir], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{EB55B964-D8E2-4E0C-B7CF-07043E026664}" name="control" dataDxfId="144">
+    <tableColumn id="13" xr3:uid="{EB55B964-D8E2-4E0C-B7CF-07043E026664}" name="control" dataDxfId="145">
       <calculatedColumnFormula>OFFSET(table_2_2[control], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{7A83EC55-03CE-4608-92D6-6F1C53B539FE}" name="ref" dataDxfId="143">
+    <tableColumn id="2" xr3:uid="{7A83EC55-03CE-4608-92D6-6F1C53B539FE}" name="ref" dataDxfId="144">
       <calculatedColumnFormula>OFFSET(table_2_2[ref], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{13E984FC-9FD2-479F-AB4C-B74DDF5FD234}" name="dsb_pos" dataDxfId="142">
+    <tableColumn id="3" xr3:uid="{13E984FC-9FD2-479F-AB4C-B74DDF5FD234}" name="dsb_pos" dataDxfId="143">
       <calculatedColumnFormula>OFFSET(table_2_2[dsb_pos], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{EF0F2447-2FA1-4517-A5CE-D8DDAAC8D3F2}" name="dsb_type" dataDxfId="141">
+    <tableColumn id="4" xr3:uid="{EF0F2447-2FA1-4517-A5CE-D8DDAAC8D3F2}" name="dsb_type" dataDxfId="142">
       <calculatedColumnFormula>OFFSET(table_2_2[dsb_type], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A1849AE1-952B-42B5-99EE-20BD2E4C5A6A}" name="dsb_type_command" dataDxfId="140">
+    <tableColumn id="12" xr3:uid="{A1849AE1-952B-42B5-99EE-20BD2E4C5A6A}" name="dsb_type_command" dataDxfId="141">
       <calculatedColumnFormula array="1">IF(table_3_2[[#This Row],[dsb_type]]="2DSB", "2", IF(table_3_2[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(table_3_2[[#This Row],[dsb_type]]="1DSB", "1", NA)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{625E12FC-BF17-4E65-99DB-EDD53FEF055D}" name="strand" dataDxfId="139">
+    <tableColumn id="5" xr3:uid="{625E12FC-BF17-4E65-99DB-EDD53FEF055D}" name="strand" dataDxfId="140">
       <calculatedColumnFormula>OFFSET(table_2_2[strand], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0ABF747E-328F-4A80-85AA-4AF871C860C1}" name="hguide" dataDxfId="138">
+    <tableColumn id="6" xr3:uid="{0ABF747E-328F-4A80-85AA-4AF871C860C1}" name="hguide" dataDxfId="139">
       <calculatedColumnFormula>MID(OFFSET(table_2_2[hguide], table_3_2[[#This Row],[index]] - 1, 0, 1, 1), 3, 100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{29D6C48B-05B8-42C6-88A9-0939BC454FE0}" name="cell" dataDxfId="137">
+    <tableColumn id="7" xr3:uid="{29D6C48B-05B8-42C6-88A9-0939BC454FE0}" name="cell" dataDxfId="138">
       <calculatedColumnFormula>OFFSET(table_2_2[cell], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{BD269EBE-94A9-4B57-B984-C7566AC259DE}" name="treatment" dataDxfId="136">
+    <tableColumn id="8" xr3:uid="{BD269EBE-94A9-4B57-B984-C7566AC259DE}" name="treatment" dataDxfId="137">
       <calculatedColumnFormula>OFFSET(table_2_2[treatment], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{142C480D-E258-4979-A008-3940A3FE78E4}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{19804410-83AB-479E-A819-2D7449105C25}" name="command_main_data" dataDxfId="135">
+    <tableColumn id="10" xr3:uid="{19804410-83AB-479E-A819-2D7449105C25}" name="command_main_data" dataDxfId="136">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_2[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_2[[#This Row],[dir]], " -ref ref_seq/", table_3_2[[#This Row],[ref]], " -dsb ", table_3_2[[#This Row],[dsb_pos]], " --dsb_type ",table_3_2[[#This Row],[dsb_type_command]], " --strand ", table_3_2[[#This Row],[strand]], " --hguide ", table_3_2[[#This Row],[hguide]], " --cell ", table_3_2[[#This Row],[cell]], " --treatment ", table_3_2[[#This Row],[treatment]], " --subst_type ", table_3_2[[#This Row],[subst_type]], " --control ", table_3_2[[#This Row],[control]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{212A69BD-0F88-401C-957F-8B6EC8E55AED}" name="command_graph_data" dataDxfId="134">
+    <tableColumn id="11" xr3:uid="{212A69BD-0F88-401C-957F-8B6EC8E55AED}" name="command_graph_data" dataDxfId="135">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_2[[#This Row],[dir]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2741,38 +2766,38 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}" name="table_4_1" displayName="table_4_1" ref="A1:K17" totalsRowShown="0" headerRowDxfId="133">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}" name="table_4_1" displayName="table_4_1" ref="A1:K17" totalsRowShown="0" headerRowDxfId="134">
   <autoFilter ref="A1:K17" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B7EC223D-BA24-48F1-9EE3-DC56DEFDE4C2}" name="index" dataDxfId="132"/>
-    <tableColumn id="7" xr3:uid="{D9F1ADDA-18A2-4F81-862D-6B0F786079FF}" name="control" dataDxfId="131">
+    <tableColumn id="1" xr3:uid="{B7EC223D-BA24-48F1-9EE3-DC56DEFDE4C2}" name="index" dataDxfId="133"/>
+    <tableColumn id="7" xr3:uid="{D9F1ADDA-18A2-4F81-862D-6B0F786079FF}" name="control" dataDxfId="132">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{0EA5A81F-6EA1-4256-9717-03273165F7BF}" name="treatment_1" dataDxfId="130">
+    <tableColumn id="8" xr3:uid="{0EA5A81F-6EA1-4256-9717-03273165F7BF}" name="treatment_1" dataDxfId="131">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5F6D005A-96D8-4801-93E2-101BAE551BA8}" name="dir_1" dataDxfId="129">
+    <tableColumn id="2" xr3:uid="{5F6D005A-96D8-4801-93E2-101BAE551BA8}" name="dir_1" dataDxfId="130">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C21D1AF7-7ABE-4181-AA2A-42227869A8DD}" name="treatment_2" dataDxfId="128">
+    <tableColumn id="9" xr3:uid="{C21D1AF7-7ABE-4181-AA2A-42227869A8DD}" name="treatment_2" dataDxfId="129">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{D66426AC-E0B2-4B07-A4D4-5A74AA033E80}" name="dir_2" dataDxfId="127">
+    <tableColumn id="3" xr3:uid="{D66426AC-E0B2-4B07-A4D4-5A74AA033E80}" name="dir_2" dataDxfId="128">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{0C8146A0-DC77-4DC4-82FF-74F4C74CF33E}" name="treatments_out" dataDxfId="126">
+    <tableColumn id="10" xr3:uid="{0C8146A0-DC77-4DC4-82FF-74F4C74CF33E}" name="treatments_out" dataDxfId="127">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_1[[#This Row],[treatment_1]], "_", table_4_1[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{519A6397-7A3C-4009-B8B9-A71C0B3A591B}" name="dir_out" dataDxfId="125">
+    <tableColumn id="4" xr3:uid="{519A6397-7A3C-4009-B8B9-A71C0B3A591B}" name="dir_out" dataDxfId="126">
       <calculatedColumnFormula>SUBSTITUTE(table_4_1[[#This Row],[dir_1]], table_4_1[[#This Row],[treatment_1]], table_4_1[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E1629355-7D02-4819-98A1-EEB3B5FADE18}" name="subst_type" dataDxfId="124">
+    <tableColumn id="5" xr3:uid="{E1629355-7D02-4819-98A1-EEB3B5FADE18}" name="subst_type" dataDxfId="125">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{BC9117A0-CB6F-4D3C-A0E4-BF8395854D9A}" name="command_main_data_combined" dataDxfId="123">
+    <tableColumn id="6" xr3:uid="{BC9117A0-CB6F-4D3C-A0E4-BF8395854D9A}" name="command_main_data_combined" dataDxfId="124">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_1[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_1[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_1[[#This Row],[dir_out]], " --subst_type ", table_4_1[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{D384013E-9937-4DD8-A36A-43325757359B}" name="command_graph_data" dataDxfId="122">
+    <tableColumn id="11" xr3:uid="{D384013E-9937-4DD8-A36A-43325757359B}" name="command_graph_data" dataDxfId="123">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_1[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_1[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2781,38 +2806,38 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}" name="table_4_2" displayName="table_4_2" ref="A20:K22" totalsRowShown="0" headerRowDxfId="121">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}" name="table_4_2" displayName="table_4_2" ref="A20:K22" totalsRowShown="0" headerRowDxfId="122">
   <autoFilter ref="A20:K22" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{7F5A3A15-751D-407C-A035-61B2605E693F}" name="index" dataDxfId="120"/>
-    <tableColumn id="7" xr3:uid="{45863AB0-FD32-49FE-B4BF-F8EE865F7604}" name="control" dataDxfId="119">
+    <tableColumn id="1" xr3:uid="{7F5A3A15-751D-407C-A035-61B2605E693F}" name="index" dataDxfId="121"/>
+    <tableColumn id="7" xr3:uid="{45863AB0-FD32-49FE-B4BF-F8EE865F7604}" name="control" dataDxfId="120">
       <calculatedColumnFormula>OFFSET(table_3_1[control], var_4_anti_offset + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{CD16648D-267E-410B-A366-3E12367C037C}" name="treatment_1" dataDxfId="118">
+    <tableColumn id="8" xr3:uid="{CD16648D-267E-410B-A366-3E12367C037C}" name="treatment_1" dataDxfId="119">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{10C9F90E-86FD-4BFE-939E-298FD6F69F12}" name="dir_1" dataDxfId="117">
+    <tableColumn id="2" xr3:uid="{10C9F90E-86FD-4BFE-939E-298FD6F69F12}" name="dir_1" dataDxfId="118">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{7AB3E4AB-F43B-4FDE-96D7-FBBB4A8B83BE}" name="treatment_2" dataDxfId="116">
+    <tableColumn id="9" xr3:uid="{7AB3E4AB-F43B-4FDE-96D7-FBBB4A8B83BE}" name="treatment_2" dataDxfId="117">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1) + 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BF948A3E-9649-41BF-A7E7-57BFDE810FE9}" name="dir_2" dataDxfId="115">
+    <tableColumn id="3" xr3:uid="{BF948A3E-9649-41BF-A7E7-57BFDE810FE9}" name="dir_2" dataDxfId="116">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1) + 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{378119E5-F021-4785-A653-4D632F029AA6}" name="treatments_out" dataDxfId="114">
+    <tableColumn id="10" xr3:uid="{378119E5-F021-4785-A653-4D632F029AA6}" name="treatments_out" dataDxfId="115">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_2[[#This Row],[treatment_1]], "_", table_4_2[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AE1A14DC-D0C9-4818-B8CC-09A571E73BC2}" name="dir_out" dataDxfId="113">
+    <tableColumn id="4" xr3:uid="{AE1A14DC-D0C9-4818-B8CC-09A571E73BC2}" name="dir_out" dataDxfId="114">
       <calculatedColumnFormula>SUBSTITUTE(table_4_2[[#This Row],[dir_1]], table_4_2[[#This Row],[treatment_1]], table_4_2[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{F29DAC4E-FEC5-4C1D-AAC1-7CE19E401F25}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{DC4E99F4-97AB-4553-A5FB-D20D3D487947}" name="command_main_data_combined" dataDxfId="112">
+    <tableColumn id="6" xr3:uid="{DC4E99F4-97AB-4553-A5FB-D20D3D487947}" name="command_main_data_combined" dataDxfId="113">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_2[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_2[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_2[[#This Row],[dir_out]], " --subst_type ", table_4_2[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{E19D3001-2E76-4CC2-BF33-D0465C77D538}" name="command_graph_data" dataDxfId="111">
+    <tableColumn id="11" xr3:uid="{E19D3001-2E76-4CC2-BF33-D0465C77D538}" name="command_graph_data" dataDxfId="112">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_2[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2821,38 +2846,38 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}" name="table_4_3" displayName="table_4_3" ref="A25:K33" totalsRowShown="0" headerRowDxfId="110">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}" name="table_4_3" displayName="table_4_3" ref="A25:K33" totalsRowShown="0" headerRowDxfId="111">
   <autoFilter ref="A25:K33" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{33AF3495-7432-4F03-9832-525A370EADEC}" name="index" dataDxfId="109"/>
-    <tableColumn id="7" xr3:uid="{3D66515C-5022-4D48-A834-4320DA4E73F6}" name="control" dataDxfId="108">
+    <tableColumn id="1" xr3:uid="{33AF3495-7432-4F03-9832-525A370EADEC}" name="index" dataDxfId="110"/>
+    <tableColumn id="7" xr3:uid="{3D66515C-5022-4D48-A834-4320DA4E73F6}" name="control" dataDxfId="109">
       <calculatedColumnFormula>OFFSET(table_3_2[control], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{294B17A9-F0F9-42CA-8342-55C00648E3A5}" name="treatment_1" dataDxfId="107">
+    <tableColumn id="8" xr3:uid="{294B17A9-F0F9-42CA-8342-55C00648E3A5}" name="treatment_1" dataDxfId="108">
       <calculatedColumnFormula>OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E13C38CF-C105-4AB5-8602-7D32E688C737}" name="dir_1" dataDxfId="106">
+    <tableColumn id="2" xr3:uid="{E13C38CF-C105-4AB5-8602-7D32E688C737}" name="dir_1" dataDxfId="107">
       <calculatedColumnFormula>OFFSET(table_3_2[dir], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{15B3CC7F-2A3C-4026-8417-A9DD21E4F004}" name="treatment_2" dataDxfId="105">
+    <tableColumn id="9" xr3:uid="{15B3CC7F-2A3C-4026-8417-A9DD21E4F004}" name="treatment_2" dataDxfId="106">
       <calculatedColumnFormula>OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{FF7D9AD3-1A35-4013-88AE-0C00465033CD}" name="dir_2" dataDxfId="104">
+    <tableColumn id="3" xr3:uid="{FF7D9AD3-1A35-4013-88AE-0C00465033CD}" name="dir_2" dataDxfId="105">
       <calculatedColumnFormula>OFFSET(table_3_2[dir], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{9353B2D3-0D23-4FBB-AFEC-EB68549160F4}" name="treatments_out" dataDxfId="103">
+    <tableColumn id="10" xr3:uid="{9353B2D3-0D23-4FBB-AFEC-EB68549160F4}" name="treatments_out" dataDxfId="104">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_3[[#This Row],[treatment_1]], "_", table_4_3[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{77F1D6F0-DE95-4E63-9E7E-D3CA3CF85F37}" name="dir_out" dataDxfId="102">
+    <tableColumn id="4" xr3:uid="{77F1D6F0-DE95-4E63-9E7E-D3CA3CF85F37}" name="dir_out" dataDxfId="103">
       <calculatedColumnFormula>SUBSTITUTE(table_4_3[[#This Row],[dir_1]], table_4_3[[#This Row],[treatment_1]], table_4_3[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{BBF4F840-178E-461E-8C17-36D699EDE038}" name="subst_type" dataDxfId="101">
+    <tableColumn id="5" xr3:uid="{BBF4F840-178E-461E-8C17-36D699EDE038}" name="subst_type" dataDxfId="102">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9434BF8B-81C5-43DF-BCB7-FA7146BF2FE8}" name="command_main_data_combined" dataDxfId="100">
+    <tableColumn id="6" xr3:uid="{9434BF8B-81C5-43DF-BCB7-FA7146BF2FE8}" name="command_main_data_combined" dataDxfId="101">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_3[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_3[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_3[[#This Row],[dir_out]], " --subst_type ", table_4_3[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{1ABF0B7B-4ECE-42BF-A7D8-EA13E98144EE}" name="command_graph_data" dataDxfId="99">
+    <tableColumn id="11" xr3:uid="{1ABF0B7B-4ECE-42BF-A7D8-EA13E98144EE}" name="command_graph_data" dataDxfId="100">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_3[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_3[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3160,7 +3185,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3221,8 +3246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DFB1CC9-23C4-4E30-93CF-6F31CFACE92F}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3251,13 +3276,13 @@
         <v>187</v>
       </c>
       <c r="D1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" t="s">
         <v>190</v>
-      </c>
-      <c r="F1" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3283,8 +3308,8 @@
         <v>WT_sgAB_R1_sense_branch</v>
       </c>
       <c r="C4" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_branch -o plots/graphs/combinedFALSE -ext png --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_branch -o plots/graphs/combined  -ext html --layout universal</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3296,8 +3321,8 @@
         <v>WT_sgAB_R1_sense_cmv</v>
       </c>
       <c r="C5" s="2" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_cmv -o plots/graphs/combinedFALSE -ext png --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_cmv -o plots/graphs/combined  -ext html --layout universal</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3309,8 +3334,8 @@
         <v>KO_sgAB_R1_sense_branch</v>
       </c>
       <c r="C6" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_branch -o plots/graphs/combinedFALSE -ext png --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_branch -o plots/graphs/combined  -ext html --layout universal</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3322,8 +3347,8 @@
         <v>KO_sgAB_R1_sense_cmv</v>
       </c>
       <c r="C7" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_cmv -o plots/graphs/combinedFALSE -ext png --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_cmv -o plots/graphs/combined  -ext html --layout universal</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3335,8 +3360,8 @@
         <v>WT_sgAB_R2_sense_branch</v>
       </c>
       <c r="C8" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_branch -o plots/graphs/combinedFALSE -ext png --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_branch -o plots/graphs/combined  -ext html --layout universal</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3348,8 +3373,8 @@
         <v>WT_sgAB_R2_sense_cmv</v>
       </c>
       <c r="C9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_cmv -o plots/graphs/combinedFALSE -ext png --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_cmv -o plots/graphs/combined  -ext html --layout universal</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3361,8 +3386,8 @@
         <v>KO_sgAB_R2_sense_branch</v>
       </c>
       <c r="C10" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_branch -o plots/graphs/combinedFALSE -ext png --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_branch -o plots/graphs/combined  -ext html --layout universal</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -3374,8 +3399,8 @@
         <v>KO_sgAB_R2_sense_cmv</v>
       </c>
       <c r="C11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_cmv -o plots/graphs/combinedFALSE -ext png --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_cmv -o plots/graphs/combined  -ext html --layout universal</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -3387,8 +3412,8 @@
         <v>WT_sgA_R1_sense_branch</v>
       </c>
       <c r="C12" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_branch -o plots/graphs/combinedFALSE -ext png --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_branch -o plots/graphs/combined  -ext html --layout universal</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3400,8 +3425,8 @@
         <v>WT_sgA_R1_sense_cmv</v>
       </c>
       <c r="C13" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_cmv -o plots/graphs/combinedFALSE -ext png --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_cmv -o plots/graphs/combined  -ext html --layout universal</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -3413,8 +3438,8 @@
         <v>KO_sgA_R1_sense_branch</v>
       </c>
       <c r="C14" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_branch -o plots/graphs/combinedFALSE -ext png --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_branch -o plots/graphs/combined  -ext html --layout universal</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -3426,8 +3451,8 @@
         <v>KO_sgA_R1_sense_cmv</v>
       </c>
       <c r="C15" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_cmv -o plots/graphs/combinedFALSE -ext png --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_cmv -o plots/graphs/combined  -ext html --layout universal</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -3439,8 +3464,8 @@
         <v>WT_sgB_R2_sense_branch</v>
       </c>
       <c r="C16" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_branch -o plots/graphs/combinedFALSE -ext png --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_branch -o plots/graphs/combined  -ext html --layout universal</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -3452,8 +3477,8 @@
         <v>WT_sgB_R2_sense_cmv</v>
       </c>
       <c r="C17" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_cmv -o plots/graphs/combinedFALSE -ext png --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_cmv -o plots/graphs/combined  -ext html --layout universal</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -3465,8 +3490,8 @@
         <v>KO_sgB_R2_sense_branch</v>
       </c>
       <c r="C18" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_branch -o plots/graphs/combinedFALSE -ext png --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_branch -o plots/graphs/combined  -ext html --layout universal</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -3478,8 +3503,8 @@
         <v>KO_sgB_R2_sense_cmv</v>
       </c>
       <c r="C19" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1), "")), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_cmv -o plots/graphs/combinedFALSE -ext png --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_cmv -o plots/graphs/combined  -ext html --layout universal</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -3502,8 +3527,8 @@
         <v>WT_sgCD_R1_antisense_splicing</v>
       </c>
       <c r="C22" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_4[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_2[[dir_out]:[dir_out]],table_7_4[[#This Row],[index]] - 1, 0, 1, 1)), ""), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense_splicing -o plots/graphs/combined -ext png</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_4[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_2[[dir_out]:[dir_out]],table_7_4[[#This Row],[index]] - 1, 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense_splicing -o plots/graphs/combined -ext html --layout universal</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -3515,8 +3540,8 @@
         <v>WT_sgCD_R2_antisense_splicing</v>
       </c>
       <c r="C23" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_4[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_2[[dir_out]:[dir_out]],table_7_4[[#This Row],[index]] - 1, 0, 1, 1)), ""), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense_splicing -o plots/graphs/combined -ext png</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_4[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_2[[dir_out]:[dir_out]],table_7_4[[#This Row],[index]] - 1, 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense_splicing -o plots/graphs/combined -ext html --layout universal</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -3533,111 +3558,111 @@
         <v>87</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>130</v>
+        <v>171</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+      <c r="A27" s="12">
         <v>1</v>
       </c>
-      <c r="B27" t="str">
+      <c r="B27" s="11" t="str">
         <f ca="1">OFFSET(table_4_3[[dir_out]:[dir_out]], table_7_5[[#This Row],[index]] - 1, 0, 1, 1)</f>
         <v>WT_sgA_R1_sense_branch_nodsb</v>
       </c>
-      <c r="C27" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_branch_nodsb -o plots/graphs/combined -ext png</v>
+      <c r="C27" s="11" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_branch_nodsb -o plots/graphs/combined -ext html --layout universal</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="A28" s="12">
         <v>2</v>
       </c>
-      <c r="B28" s="2" t="str">
+      <c r="B28" s="13" t="str">
         <f ca="1">OFFSET(table_4_3[[dir_out]:[dir_out]], table_7_5[[#This Row],[index]] - 1, 0, 1, 1)</f>
         <v>WT_sgA_R1_sense_cmv_nodsb</v>
       </c>
-      <c r="C28" s="2" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_cmv_nodsb -o plots/graphs/combined -ext png</v>
+      <c r="C28" s="13" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_cmv_nodsb -o plots/graphs/combined -ext html --layout universal</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+      <c r="A29" s="12">
         <v>3</v>
       </c>
-      <c r="B29" t="str">
+      <c r="B29" s="11" t="str">
         <f ca="1">OFFSET(table_4_3[[dir_out]:[dir_out]], table_7_5[[#This Row],[index]] - 1, 0, 1, 1)</f>
         <v>KO_sgA_R1_sense_branch_nodsb</v>
       </c>
-      <c r="C29" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_branch_nodsb -o plots/graphs/combined -ext png</v>
+      <c r="C29" s="11" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_branch_nodsb -o plots/graphs/combined -ext html --layout universal</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+      <c r="A30" s="12">
         <v>4</v>
       </c>
-      <c r="B30" t="str">
+      <c r="B30" s="11" t="str">
         <f ca="1">OFFSET(table_4_3[[dir_out]:[dir_out]], table_7_5[[#This Row],[index]] - 1, 0, 1, 1)</f>
         <v>KO_sgA_R1_sense_cmv_nodsb</v>
       </c>
-      <c r="C30" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_cmv_nodsb -o plots/graphs/combined -ext png</v>
+      <c r="C30" s="11" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_cmv_nodsb -o plots/graphs/combined -ext html --layout universal</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+      <c r="A31" s="12">
         <v>5</v>
       </c>
-      <c r="B31" t="str">
+      <c r="B31" s="11" t="str">
         <f ca="1">OFFSET(table_4_3[[dir_out]:[dir_out]], table_7_5[[#This Row],[index]] - 1, 0, 1, 1)</f>
         <v>WT_sgB_R2_sense_branch_nodsb</v>
       </c>
-      <c r="C31" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_branch_nodsb -o plots/graphs/combined -ext png</v>
+      <c r="C31" s="11" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_branch_nodsb -o plots/graphs/combined -ext html --layout universal</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+      <c r="A32" s="12">
         <v>6</v>
       </c>
-      <c r="B32" t="str">
+      <c r="B32" s="11" t="str">
         <f ca="1">OFFSET(table_4_3[[dir_out]:[dir_out]], table_7_5[[#This Row],[index]] - 1, 0, 1, 1)</f>
         <v>WT_sgB_R2_sense_cmv_nodsb</v>
       </c>
-      <c r="C32" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_cmv_nodsb -o plots/graphs/combined -ext png</v>
+      <c r="C32" s="11" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_cmv_nodsb -o plots/graphs/combined -ext html --layout universal</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+      <c r="A33" s="12">
         <v>7</v>
       </c>
-      <c r="B33" t="str">
+      <c r="B33" s="11" t="str">
         <f ca="1">OFFSET(table_4_3[[dir_out]:[dir_out]], table_7_5[[#This Row],[index]] - 1, 0, 1, 1)</f>
         <v>KO_sgB_R2_sense_branch_nodsb</v>
       </c>
-      <c r="C33" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_branch_nodsb -o plots/graphs/combined -ext png</v>
+      <c r="C33" s="11" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_branch_nodsb -o plots/graphs/combined -ext html --layout universal</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+      <c r="A34" s="12">
         <v>8</v>
       </c>
-      <c r="B34" t="str">
+      <c r="B34" s="11" t="str">
         <f ca="1">OFFSET(table_4_3[[dir_out]:[dir_out]], table_7_5[[#This Row],[index]] - 1, 0, 1, 1)</f>
         <v>KO_sgB_R2_sense_cmv_nodsb</v>
       </c>
-      <c r="C34" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_cmv_nodsb -o plots/graphs/combined -ext png</v>
+      <c r="C34" s="11" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_cmv_nodsb -o plots/graphs/combined -ext html --layout universal</v>
       </c>
     </row>
   </sheetData>
@@ -25800,7 +25825,7 @@
   <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+      <selection activeCell="T2" sqref="T2:T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26556,8 +26581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1375107-D76A-4386-B771-6693BBF75061}">
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView topLeftCell="C37" workbookViewId="0">
-      <selection activeCell="N46" sqref="N46"/>
+    <sheetView topLeftCell="C43" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39:N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26589,10 +26614,10 @@
         <v>188</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F1" t="s">
         <v>190</v>
-      </c>
-      <c r="F1" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Analysis comparing old/new NHEJ total reads.
</commit_message>
<xml_diff>
--- a/libinfo.xlsx
+++ b/libinfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tchan\Code\SCMB_Project\RNA-mediated_DSB_repair\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D296A792-47F6-4BBD-A733-3D0B38D568EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8FFD616-62AC-4EFE-BA73-B4EB0CE2ED2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="4" activeTab="9" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
   </bookViews>
   <sheets>
     <sheet name="globals" sheetId="3" r:id="rId1"/>
@@ -3246,8 +3246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DFB1CC9-23C4-4E30-93CF-6F31CFACE92F}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3680,7 +3680,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5334D33C-3E16-4C4F-BA76-1F06B33FAC0B}">
   <dimension ref="A1:D108"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5318,8 +5320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40F1EACD-27DC-4973-8E3A-9162F610D9C4}">
   <dimension ref="A1:O173"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M98" sqref="M98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14689,7 +14691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8D704B5-D01A-4D17-9252-416EA08BC871}">
   <dimension ref="A1:S56"/>
   <sheetViews>
-    <sheetView topLeftCell="H58" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add fractal layout. Put plotting constants in proper file.
</commit_message>
<xml_diff>
--- a/libinfo.xlsx
+++ b/libinfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tchan\Code\SCMB_Project\RNA-mediated_DSB_repair\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8FFD616-62AC-4EFE-BA73-B4EB0CE2ED2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8665DB3-D4C6-4E23-83DC-5FFBD75298F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="4" activeTab="8" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
   </bookViews>
   <sheets>
     <sheet name="globals" sheetId="3" r:id="rId1"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="192">
   <si>
     <t>yjl217</t>
   </si>
@@ -661,6 +661,9 @@
   <si>
     <t>universal</t>
   </si>
+  <si>
+    <t>png</t>
+  </si>
 </sst>
 </file>
 
@@ -785,12 +788,22 @@
   </cellStyles>
   <dxfs count="203">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -835,22 +848,12 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -2414,8 +2417,8 @@
     <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="28">
       <calculatedColumnFormula>IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="7">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="3">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2463,8 +2466,8 @@
     <tableColumn id="15" xr3:uid="{E18D2025-56E8-4128-9201-9E0BF8A67AC0}" name="common_layout_dir" dataDxfId="15">
       <calculatedColumnFormula>OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_2[[#This Row],[index]] - 1, 6) + 2, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{0917AB98-1545-4642-9BE8-618AAA1E404A}" name="command" dataDxfId="6">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</calculatedColumnFormula>
+    <tableColumn id="13" xr3:uid="{0917AB98-1545-4642-9BE8-618AAA1E404A}" name="command" dataDxfId="2">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2479,8 +2482,8 @@
     <tableColumn id="4" xr3:uid="{8541A14E-3250-4B9C-B315-969FC11BE60A}" name="dir" dataDxfId="12">
       <calculatedColumnFormula>OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{EAD6D5EC-B61E-4A98-B4FD-4932757CFEA3}" name="command" dataDxfId="4">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{EAD6D5EC-B61E-4A98-B4FD-4932757CFEA3}" name="command" dataDxfId="1">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2495,8 +2498,8 @@
     <tableColumn id="4" xr3:uid="{181C59FC-364D-4421-8E54-98DFF4CA7C05}" name="dir" dataDxfId="9">
       <calculatedColumnFormula>OFFSET(table_4_2[[dir_out]:[dir_out]], table_7_4[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{6D8CC942-572B-44F2-BCA6-4D31A25A4067}" name="command" dataDxfId="5">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_4[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_2[[dir_out]:[dir_out]],table_7_4[[#This Row],[index]] - 1, 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{6D8CC942-572B-44F2-BCA6-4D31A25A4067}" name="command" dataDxfId="0">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_4[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_2[[dir_out]:[dir_out]],table_7_4[[#This Row],[index]] - 1, 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2504,14 +2507,14 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{58F5EC27-BD76-45AE-8D38-F4E705EF79E9}" name="table_7_5" displayName="table_7_5" ref="A26:C34" totalsRowShown="0" headerRowDxfId="8" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{58F5EC27-BD76-45AE-8D38-F4E705EF79E9}" name="table_7_5" displayName="table_7_5" ref="A26:C34" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A26:C34" xr:uid="{58F5EC27-BD76-45AE-8D38-F4E705EF79E9}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{AAC1476C-44CE-49FD-8254-50BAEAA6929C}" name="index" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{1222E48F-ED5C-48AA-BA39-1443B841BC9F}" name="dir" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{AAC1476C-44CE-49FD-8254-50BAEAA6929C}" name="index" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{1222E48F-ED5C-48AA-BA39-1443B841BC9F}" name="dir" dataDxfId="5">
       <calculatedColumnFormula>OFFSET(table_4_3[[dir_out]:[dir_out]], table_7_5[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{89B7E589-2097-43FC-B96B-19D2EF777E97}" name="command" dataDxfId="1">
+    <tableColumn id="6" xr3:uid="{89B7E589-2097-43FC-B96B-19D2EF777E97}" name="command" dataDxfId="4">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3247,7 +3250,7 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="C22" sqref="C22:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3276,7 +3279,7 @@
         <v>187</v>
       </c>
       <c r="D1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>189</v>
@@ -3308,8 +3311,8 @@
         <v>WT_sgAB_R1_sense_branch</v>
       </c>
       <c r="C4" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_branch -o plots/graphs/combined  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_branch -o plots/graphs/combined/png  -ext png --layout universal</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3321,8 +3324,8 @@
         <v>WT_sgAB_R1_sense_cmv</v>
       </c>
       <c r="C5" s="2" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_cmv -o plots/graphs/combined  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_cmv -o plots/graphs/combined/png  -ext png --layout universal</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3334,8 +3337,8 @@
         <v>KO_sgAB_R1_sense_branch</v>
       </c>
       <c r="C6" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_branch -o plots/graphs/combined  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_branch -o plots/graphs/combined/png  -ext png --layout universal</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3347,8 +3350,8 @@
         <v>KO_sgAB_R1_sense_cmv</v>
       </c>
       <c r="C7" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_cmv -o plots/graphs/combined  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_cmv -o plots/graphs/combined/png  -ext png --layout universal</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3360,8 +3363,8 @@
         <v>WT_sgAB_R2_sense_branch</v>
       </c>
       <c r="C8" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_branch -o plots/graphs/combined  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_branch -o plots/graphs/combined/png  -ext png --layout universal</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3373,8 +3376,8 @@
         <v>WT_sgAB_R2_sense_cmv</v>
       </c>
       <c r="C9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_cmv -o plots/graphs/combined  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_cmv -o plots/graphs/combined/png  -ext png --layout universal</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3386,8 +3389,8 @@
         <v>KO_sgAB_R2_sense_branch</v>
       </c>
       <c r="C10" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_branch -o plots/graphs/combined  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_branch -o plots/graphs/combined/png  -ext png --layout universal</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -3399,8 +3402,8 @@
         <v>KO_sgAB_R2_sense_cmv</v>
       </c>
       <c r="C11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_cmv -o plots/graphs/combined  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_cmv -o plots/graphs/combined/png  -ext png --layout universal</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -3412,8 +3415,8 @@
         <v>WT_sgA_R1_sense_branch</v>
       </c>
       <c r="C12" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_branch -o plots/graphs/combined  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_branch -o plots/graphs/combined/png  -ext png --layout universal</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3425,8 +3428,8 @@
         <v>WT_sgA_R1_sense_cmv</v>
       </c>
       <c r="C13" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_cmv -o plots/graphs/combined  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_cmv -o plots/graphs/combined/png  -ext png --layout universal</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -3438,8 +3441,8 @@
         <v>KO_sgA_R1_sense_branch</v>
       </c>
       <c r="C14" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_branch -o plots/graphs/combined  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_branch -o plots/graphs/combined/png  -ext png --layout universal</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -3451,8 +3454,8 @@
         <v>KO_sgA_R1_sense_cmv</v>
       </c>
       <c r="C15" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_cmv -o plots/graphs/combined  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_cmv -o plots/graphs/combined/png  -ext png --layout universal</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -3464,8 +3467,8 @@
         <v>WT_sgB_R2_sense_branch</v>
       </c>
       <c r="C16" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_branch -o plots/graphs/combined  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_branch -o plots/graphs/combined/png  -ext png --layout universal</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -3477,8 +3480,8 @@
         <v>WT_sgB_R2_sense_cmv</v>
       </c>
       <c r="C17" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_cmv -o plots/graphs/combined  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_cmv -o plots/graphs/combined/png  -ext png --layout universal</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -3490,8 +3493,8 @@
         <v>KO_sgB_R2_sense_branch</v>
       </c>
       <c r="C18" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_branch -o plots/graphs/combined  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_branch -o plots/graphs/combined/png  -ext png --layout universal</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -3503,8 +3506,8 @@
         <v>KO_sgB_R2_sense_cmv</v>
       </c>
       <c r="C19" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_cmv -o plots/graphs/combined  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_cmv -o plots/graphs/combined/png  -ext png --layout universal</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -3527,8 +3530,8 @@
         <v>WT_sgCD_R1_antisense_splicing</v>
       </c>
       <c r="C22" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_4[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_2[[dir_out]:[dir_out]],table_7_4[[#This Row],[index]] - 1, 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense_splicing -o plots/graphs/combined -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_4[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_2[[dir_out]:[dir_out]],table_7_4[[#This Row],[index]] - 1, 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense_splicing -o plots/graphs/combined/png -ext png --layout universal</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -3540,8 +3543,8 @@
         <v>WT_sgCD_R2_antisense_splicing</v>
       </c>
       <c r="C23" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_4[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_2[[dir_out]:[dir_out]],table_7_4[[#This Row],[index]] - 1, 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense_splicing -o plots/graphs/combined -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_4[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_2[[dir_out]:[dir_out]],table_7_4[[#This Row],[index]] - 1, 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense_splicing -o plots/graphs/combined/png -ext png --layout universal</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -3571,7 +3574,7 @@
       </c>
       <c r="C27" s="11" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_branch_nodsb -o plots/graphs/combined -ext html --layout universal</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_branch_nodsb -o plots/graphs/combined -ext png --layout universal</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -3584,7 +3587,7 @@
       </c>
       <c r="C28" s="13" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_cmv_nodsb -o plots/graphs/combined -ext html --layout universal</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_cmv_nodsb -o plots/graphs/combined -ext png --layout universal</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -3597,7 +3600,7 @@
       </c>
       <c r="C29" s="11" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_branch_nodsb -o plots/graphs/combined -ext html --layout universal</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_branch_nodsb -o plots/graphs/combined -ext png --layout universal</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -3610,7 +3613,7 @@
       </c>
       <c r="C30" s="11" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_cmv_nodsb -o plots/graphs/combined -ext html --layout universal</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_cmv_nodsb -o plots/graphs/combined -ext png --layout universal</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -3623,7 +3626,7 @@
       </c>
       <c r="C31" s="11" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_branch_nodsb -o plots/graphs/combined -ext html --layout universal</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_branch_nodsb -o plots/graphs/combined -ext png --layout universal</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -3636,7 +3639,7 @@
       </c>
       <c r="C32" s="11" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_cmv_nodsb -o plots/graphs/combined -ext html --layout universal</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_cmv_nodsb -o plots/graphs/combined -ext png --layout universal</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -3649,7 +3652,7 @@
       </c>
       <c r="C33" s="11" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_branch_nodsb -o plots/graphs/combined -ext html --layout universal</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_branch_nodsb -o plots/graphs/combined -ext png --layout universal</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -3662,7 +3665,7 @@
       </c>
       <c r="C34" s="11" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_cmv_nodsb -o plots/graphs/combined -ext html --layout universal</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_cmv_nodsb -o plots/graphs/combined -ext png --layout universal</v>
       </c>
     </row>
   </sheetData>
@@ -3680,7 +3683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5334D33C-3E16-4C4F-BA76-1F06B33FAC0B}">
   <dimension ref="A1:D108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
@@ -25824,10 +25827,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1417E7-0E2A-4E67-94B4-4030BF5F7C23}">
-  <dimension ref="A1:T19"/>
+  <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2:T7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26563,12 +26566,6 @@
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
     </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F19" cm="1">
-        <f t="array" ref="F19">COLUMN(table_6_1[dir_1])</f>
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -26583,7 +26580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1375107-D76A-4386-B771-6693BBF75061}">
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView topLeftCell="C43" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C43" workbookViewId="0">
       <selection activeCell="N39" sqref="N39:N42"/>
     </sheetView>
   </sheetViews>
@@ -26719,8 +26716,8 @@
         <v>2DSB_R1</v>
       </c>
       <c r="N3" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -26776,8 +26773,8 @@
         <v>2DSB_R1</v>
       </c>
       <c r="N4" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_branch -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_branch -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -26833,8 +26830,8 @@
         <v>2DSB_R1</v>
       </c>
       <c r="N5" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_cmv -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_cmv -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -26890,8 +26887,8 @@
         <v>2DSB_R1</v>
       </c>
       <c r="N6" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -26947,8 +26944,8 @@
         <v>2DSB_R1</v>
       </c>
       <c r="N7" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_branch -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_branch -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -27004,8 +27001,8 @@
         <v>2DSB_R1</v>
       </c>
       <c r="N8" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_cmv -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_cmv -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -27061,8 +27058,8 @@
         <v>2DSB_R2</v>
       </c>
       <c r="N9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -27118,8 +27115,8 @@
         <v>2DSB_R2</v>
       </c>
       <c r="N10" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_branch -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_branch -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -27175,8 +27172,8 @@
         <v>2DSB_R2</v>
       </c>
       <c r="N11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_cmv -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_cmv -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -27232,8 +27229,8 @@
         <v>2DSB_R2</v>
       </c>
       <c r="N12" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -27289,8 +27286,8 @@
         <v>2DSB_R2</v>
       </c>
       <c r="N13" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_branch -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_branch -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -27346,8 +27343,8 @@
         <v>2DSB_R2</v>
       </c>
       <c r="N14" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_cmv -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_cmv -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -27403,8 +27400,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N15" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -27460,8 +27457,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N16" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -27517,8 +27514,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N17" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -27574,8 +27571,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N18" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -27631,8 +27628,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N19" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -27688,8 +27685,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N20" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -27745,8 +27742,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N21" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -27802,8 +27799,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N22" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -27859,8 +27856,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N23" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -27916,8 +27913,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N24" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -27973,8 +27970,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N25" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -28030,8 +28027,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N26" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -28087,8 +28084,8 @@
         <v>1DSB_R1_30bpDown</v>
       </c>
       <c r="N27" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_30bpDown -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_30bpDown -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -28144,8 +28141,8 @@
         <v>1DSB_R1_30bpDown</v>
       </c>
       <c r="N28" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch_30bpDown -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch_30bpDown -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -28201,8 +28198,8 @@
         <v>1DSB_R1_30bpDown</v>
       </c>
       <c r="N29" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv_30bpDown -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv_30bpDown -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -28258,8 +28255,8 @@
         <v>1DSB_R1_30bpDown</v>
       </c>
       <c r="N30" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_30bpDown -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_30bpDown -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -28315,8 +28312,8 @@
         <v>1DSB_R1_30bpDown</v>
       </c>
       <c r="N31" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch_30bpDown -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch_30bpDown -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -28372,8 +28369,8 @@
         <v>1DSB_R1_30bpDown</v>
       </c>
       <c r="N32" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv_30bpDown -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv_30bpDown -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -28429,8 +28426,8 @@
         <v>1DSB_R2_30bpDown</v>
       </c>
       <c r="N33" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_30bpDown -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_30bpDown -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -28486,8 +28483,8 @@
         <v>1DSB_R2_30bpDown</v>
       </c>
       <c r="N34" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch_30bpDown -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch_30bpDown -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -28543,8 +28540,8 @@
         <v>1DSB_R2_30bpDown</v>
       </c>
       <c r="N35" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv_30bpDown -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv_30bpDown -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -28600,8 +28597,8 @@
         <v>1DSB_R2_30bpDown</v>
       </c>
       <c r="N36" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_30bpDown -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_30bpDown -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -28657,8 +28654,8 @@
         <v>1DSB_R2_30bpDown</v>
       </c>
       <c r="N37" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch_30bpDown -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch_30bpDown -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -28714,8 +28711,8 @@
         <v>1DSB_R2_30bpDown</v>
       </c>
       <c r="N38" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv_30bpDown -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv_30bpDown -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -28771,8 +28768,8 @@
         <v>2DSBanti_R1</v>
       </c>
       <c r="N39" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
@@ -28828,8 +28825,8 @@
         <v>2DSBanti_R1</v>
       </c>
       <c r="N40" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_splicing -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_splicing -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
@@ -28885,8 +28882,8 @@
         <v>2DSBanti_R2</v>
       </c>
       <c r="N41" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
@@ -28942,8 +28939,8 @@
         <v>2DSBanti_R2</v>
       </c>
       <c r="N42" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_splicing -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_splicing -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -29043,8 +29040,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N45" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_nodsb -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_nodsb -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
@@ -29100,8 +29097,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N46" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch_nodsb -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch_nodsb -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
@@ -29157,8 +29154,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N47" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv_nodsb -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv_nodsb -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
@@ -29214,8 +29211,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N48" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_nodsb -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_nodsb -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
@@ -29271,8 +29268,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N49" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch_nodsb -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch_nodsb -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
@@ -29328,8 +29325,8 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N50" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv_nodsb -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv_nodsb -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
@@ -29385,8 +29382,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N51" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_nodsb -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_nodsb -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
@@ -29442,8 +29439,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N52" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch_nodsb -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch_nodsb -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
@@ -29499,8 +29496,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N53" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv_nodsb -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv_nodsb -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
@@ -29556,8 +29553,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N54" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_nodsb -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_nodsb -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
@@ -29613,8 +29610,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N55" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch_nodsb -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch_nodsb -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
@@ -29670,8 +29667,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N56" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv_nodsb -o plots/graphs/individual  -ext html --layout universal</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, " ", IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""),  " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv_nodsb -o plots/graphs/individual/html  -ext html --layout universal</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove reverse complement from make_main_data. Reverse complement only in plot_graph.
</commit_message>
<xml_diff>
--- a/libinfo.xlsx
+++ b/libinfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tchan\Code\SCMB_Project\RNA-mediated_DSB_repair\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257CF222-EBE8-4D57-9B06-7C27EED08C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4ADB0C0-203F-4C46-B760-0C2951BFF617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="4" activeTab="7" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="4" activeTab="8" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
   </bookViews>
   <sheets>
     <sheet name="globals" sheetId="3" r:id="rId1"/>
@@ -36,6 +36,7 @@
     <definedName name="subst_type">globals!$B$1</definedName>
     <definedName name="var_2_nodsb_offset">'2_combine'!$A$43</definedName>
     <definedName name="var_4_anti_offset">'4_graph_combined'!$A$19</definedName>
+    <definedName name="var_6_1dsb_offset">'6_common_layout'!$A$18</definedName>
     <definedName name="var_6_anti_offset">'6_common_layout'!$A$10</definedName>
     <definedName name="var_6_anti_ofsfset">'6_common_layout'!$A$10</definedName>
     <definedName name="var_6_layout">'6_common_layout'!$B$1</definedName>
@@ -66,7 +67,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -88,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1555" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1566" uniqueCount="193">
   <si>
     <t>yjl217</t>
   </si>
@@ -800,7 +801,383 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{FFD19645-61C4-4244-A560-0232B787F38C}"/>
   </cellStyles>
-  <dxfs count="225">
+  <dxfs count="235">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -821,10 +1198,399 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor indexed="64"/>
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1189,647 +1955,11 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </right>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </right>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -2543,7 +2673,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{70502F2F-AE2C-4D63-ADF7-F65702652EBF}" name="table_1_2" displayName="table_1_2" ref="A1:D108" totalsRowShown="0">
   <autoFilter ref="A1:D108" xr:uid="{70502F2F-AE2C-4D63-ADF7-F65702652EBF}"/>
   <tableColumns count="4">
-    <tableColumn id="2" xr3:uid="{BB99DCDA-08D4-474A-ABC3-5229CEAF80CF}" name="id" dataDxfId="224">
+    <tableColumn id="2" xr3:uid="{BB99DCDA-08D4-474A-ABC3-5229CEAF80CF}" name="id" dataDxfId="234">
       <calculatedColumnFormula>INT(MID(table_1_2[[#This Row],[library]], 4, 10))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{5F63B290-093A-48A3-9AFC-EB2FE27DE630}" name="library"/>
@@ -2555,44 +2685,44 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}" name="table_5_1" displayName="table_5_1" ref="A1:M41" totalsRowShown="0" headerRowDxfId="121">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}" name="table_5_1" displayName="table_5_1" ref="A1:M41" totalsRowShown="0" headerRowDxfId="131">
   <autoFilter ref="A1:M41" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
   <tableColumns count="13">
-    <tableColumn id="25" xr3:uid="{43F57146-0E56-46F3-A0E3-717A41010F4A}" name="index" dataDxfId="120"/>
-    <tableColumn id="1" xr3:uid="{B0B3F6B0-7577-49AC-B865-1E873B4DC53C}" name="dir" dataDxfId="119">
+    <tableColumn id="25" xr3:uid="{43F57146-0E56-46F3-A0E3-717A41010F4A}" name="index" dataDxfId="130"/>
+    <tableColumn id="1" xr3:uid="{B0B3F6B0-7577-49AC-B865-1E873B4DC53C}" name="dir" dataDxfId="129">
       <calculatedColumnFormula>table_3_1[[#This Row],[dir]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{D04F356F-9288-416D-ACDA-6BFE128B70D7}" name="control" dataDxfId="118">
+    <tableColumn id="13" xr3:uid="{D04F356F-9288-416D-ACDA-6BFE128B70D7}" name="control" dataDxfId="128">
       <calculatedColumnFormula>table_3_1[[#This Row],[control]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{9C168B22-F534-40D4-947C-918239C33FD9}" name="ref" dataDxfId="117">
+    <tableColumn id="2" xr3:uid="{9C168B22-F534-40D4-947C-918239C33FD9}" name="ref" dataDxfId="127">
       <calculatedColumnFormula>table_3_1[[#This Row],[ref]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{6F64477B-0C66-4251-9156-22307A6D70A0}" name="dsb_pos" dataDxfId="116">
+    <tableColumn id="3" xr3:uid="{6F64477B-0C66-4251-9156-22307A6D70A0}" name="dsb_pos" dataDxfId="126">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_pos]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{D037F4F2-543F-4D7D-AB36-0B253FD61B0D}" name="dsb_type" dataDxfId="115">
+    <tableColumn id="4" xr3:uid="{D037F4F2-543F-4D7D-AB36-0B253FD61B0D}" name="dsb_type" dataDxfId="125">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_type]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{407AC5E6-13CB-409A-8E78-64B8CC121882}" name="dsb_type_command" dataDxfId="114">
+    <tableColumn id="12" xr3:uid="{407AC5E6-13CB-409A-8E78-64B8CC121882}" name="dsb_type_command" dataDxfId="124">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_type_command]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{1A24C844-2A10-4394-818F-0C25A569B414}" name="strand" dataDxfId="113">
+    <tableColumn id="5" xr3:uid="{1A24C844-2A10-4394-818F-0C25A569B414}" name="strand" dataDxfId="123">
       <calculatedColumnFormula>table_3_1[[#This Row],[strand]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{4F0A02F9-5555-489E-BA41-E3CBF81D1114}" name="hguide" dataDxfId="112">
+    <tableColumn id="6" xr3:uid="{4F0A02F9-5555-489E-BA41-E3CBF81D1114}" name="hguide" dataDxfId="122">
       <calculatedColumnFormula>table_3_1[[#This Row],[hguide]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FAE741F2-7C1B-41F2-8875-9F7A2EF40A54}" name="cell" dataDxfId="111">
+    <tableColumn id="7" xr3:uid="{FAE741F2-7C1B-41F2-8875-9F7A2EF40A54}" name="cell" dataDxfId="121">
       <calculatedColumnFormula>table_3_1[[#This Row],[cell]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{FE3ED128-2534-43D1-9244-11AB1FB57650}" name="treatment" dataDxfId="110">
+    <tableColumn id="8" xr3:uid="{FE3ED128-2534-43D1-9244-11AB1FB57650}" name="treatment" dataDxfId="120">
       <calculatedColumnFormula>table_3_1[[#This Row],[treatment]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{65ACBC9C-0EC8-4074-B310-05F4B70BFAD5}" name="subst_type" dataDxfId="109">
+    <tableColumn id="9" xr3:uid="{65ACBC9C-0EC8-4074-B310-05F4B70BFAD5}" name="subst_type" dataDxfId="119">
       <calculatedColumnFormula>"with"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{F80F6FB9-4F35-4819-8285-D77131C6EFCE}" name="command" dataDxfId="108">
+    <tableColumn id="10" xr3:uid="{F80F6FB9-4F35-4819-8285-D77131C6EFCE}" name="command" dataDxfId="118">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2605,40 +2735,40 @@
   <autoFilter ref="A43:M55" xr:uid="{D74A5276-1A50-4DA1-9131-9669404C8622}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{8AC09A63-4226-4C75-8801-68CF93C0F078}" name="index"/>
-    <tableColumn id="2" xr3:uid="{77584C42-D70C-48A4-979A-F4DEA0B31542}" name="dir" dataDxfId="107">
+    <tableColumn id="2" xr3:uid="{77584C42-D70C-48A4-979A-F4DEA0B31542}" name="dir" dataDxfId="117">
       <calculatedColumnFormula>table_3_2[[#This Row],[dir]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{483E3D73-4059-4B65-84EC-5DC4E7008F35}" name="control" dataDxfId="106">
+    <tableColumn id="3" xr3:uid="{483E3D73-4059-4B65-84EC-5DC4E7008F35}" name="control" dataDxfId="116">
       <calculatedColumnFormula>table_3_2[[#This Row],[control]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5859A8DB-4C52-4451-BBB6-C6BEBF497540}" name="ref" dataDxfId="105">
+    <tableColumn id="4" xr3:uid="{5859A8DB-4C52-4451-BBB6-C6BEBF497540}" name="ref" dataDxfId="115">
       <calculatedColumnFormula>table_3_2[[#This Row],[ref]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{06FC4099-C18C-436C-B1E6-9739B71C7F22}" name="dsb_pos" dataDxfId="104">
+    <tableColumn id="5" xr3:uid="{06FC4099-C18C-436C-B1E6-9739B71C7F22}" name="dsb_pos" dataDxfId="114">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_pos]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8F043A8E-C5E7-4596-AE13-3E495C6DB33E}" name="dsb_type" dataDxfId="103">
+    <tableColumn id="6" xr3:uid="{8F043A8E-C5E7-4596-AE13-3E495C6DB33E}" name="dsb_type" dataDxfId="113">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_type]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E2DB136E-6FA9-4095-8B91-F094974333AF}" name="dsb_type_command" dataDxfId="102">
+    <tableColumn id="7" xr3:uid="{E2DB136E-6FA9-4095-8B91-F094974333AF}" name="dsb_type_command" dataDxfId="112">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_type_command]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{55CDC54E-3E43-4365-B1C9-5359F747A157}" name="strand" dataDxfId="101">
+    <tableColumn id="8" xr3:uid="{55CDC54E-3E43-4365-B1C9-5359F747A157}" name="strand" dataDxfId="111">
       <calculatedColumnFormula>table_3_2[[#This Row],[strand]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{056BD8A0-CC40-4C61-9F22-EE7382045F66}" name="hguide" dataDxfId="100">
+    <tableColumn id="9" xr3:uid="{056BD8A0-CC40-4C61-9F22-EE7382045F66}" name="hguide" dataDxfId="110">
       <calculatedColumnFormula>table_3_2[[#This Row],[hguide]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{489E156D-888A-4DDC-BB23-A4721D588249}" name="cell" dataDxfId="99">
+    <tableColumn id="10" xr3:uid="{489E156D-888A-4DDC-BB23-A4721D588249}" name="cell" dataDxfId="109">
       <calculatedColumnFormula>table_3_2[[#This Row],[cell]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{0F1B5F9E-B10D-4258-9052-90BCDC89F0B0}" name="treatment" dataDxfId="98">
+    <tableColumn id="11" xr3:uid="{0F1B5F9E-B10D-4258-9052-90BCDC89F0B0}" name="treatment" dataDxfId="108">
       <calculatedColumnFormula>table_3_2[[#This Row],[treatment]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A2723EF6-80E8-4D8D-A6DC-7556C1996222}" name="subst_type" dataDxfId="97">
+    <tableColumn id="12" xr3:uid="{A2723EF6-80E8-4D8D-A6DC-7556C1996222}" name="subst_type" dataDxfId="107">
       <calculatedColumnFormula>"with"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{02531CCA-6CDE-42BA-80E3-31C0F97A3546}" name="command" dataDxfId="96">
+    <tableColumn id="13" xr3:uid="{02531CCA-6CDE-42BA-80E3-31C0F97A3546}" name="command" dataDxfId="106">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2647,65 +2777,65 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E39D37F2-5006-44FB-A873-CCC98F8BA522}" name="table_6_1" displayName="table_6_1" ref="A2:T8" totalsRowShown="0" headerRowDxfId="95" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E39D37F2-5006-44FB-A873-CCC98F8BA522}" name="table_6_1" displayName="table_6_1" ref="A2:T8" totalsRowShown="0" headerRowDxfId="105" dataDxfId="104">
   <autoFilter ref="A2:T8" xr:uid="{E39D37F2-5006-44FB-A873-CCC98F8BA522}"/>
   <tableColumns count="20">
-    <tableColumn id="25" xr3:uid="{CD5CCC3B-8B5B-4C20-98D1-63A7E1FB075B}" name="index" dataDxfId="21"/>
-    <tableColumn id="18" xr3:uid="{A6E432BE-5846-48EE-948A-BE81A4E2B6F5}" name="dir_1" dataDxfId="20">
+    <tableColumn id="25" xr3:uid="{CD5CCC3B-8B5B-4C20-98D1-63A7E1FB075B}" name="index" dataDxfId="103"/>
+    <tableColumn id="18" xr3:uid="{A6E432BE-5846-48EE-948A-BE81A4E2B6F5}" name="dir_1" dataDxfId="102">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_1]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{A826EC7B-673B-4DCB-8792-35762AD6C5ED}" name="dir_2" dataDxfId="19">
+    <tableColumn id="17" xr3:uid="{A826EC7B-673B-4DCB-8792-35762AD6C5ED}" name="dir_2" dataDxfId="101">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_2]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{F6910118-048E-4746-9072-727F3B1847FE}" name="dir_3" dataDxfId="18">
+    <tableColumn id="16" xr3:uid="{F6910118-048E-4746-9072-727F3B1847FE}" name="dir_3" dataDxfId="100">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_3]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{0BBECB52-3A0A-4374-9C43-DA21C4CA365C}" name="dir_4" dataDxfId="17">
+    <tableColumn id="15" xr3:uid="{0BBECB52-3A0A-4374-9C43-DA21C4CA365C}" name="dir_4" dataDxfId="99">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_4]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{6E2A95BE-29B1-4454-9E5B-BED35BBC5239}" name="dir_5" dataDxfId="16">
+    <tableColumn id="14" xr3:uid="{6E2A95BE-29B1-4454-9E5B-BED35BBC5239}" name="dir_5" dataDxfId="98">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_5]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{4BDBAB17-9D30-4F82-92E5-FBABD10C580E}" name="dir_6" dataDxfId="15">
+    <tableColumn id="1" xr3:uid="{4BDBAB17-9D30-4F82-92E5-FBABD10C580E}" name="dir_6" dataDxfId="97">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_6]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{8377C5E1-81CB-41A4-9754-5BDCCCB5D946}" name="dir_7" dataDxfId="14">
+    <tableColumn id="21" xr3:uid="{8377C5E1-81CB-41A4-9754-5BDCCCB5D946}" name="dir_7" dataDxfId="96">
       <calculatedColumnFormula array="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_7]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{0BBDCF08-0538-454A-A8A3-33839702EB7D}" name="dir_8" dataDxfId="13">
+    <tableColumn id="23" xr3:uid="{0BBDCF08-0538-454A-A8A3-33839702EB7D}" name="dir_8" dataDxfId="95">
       <calculatedColumnFormula array="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_8]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{362AFBD7-D8FE-484B-A796-99C68A4873AF}" name="dir_9" dataDxfId="12">
+    <tableColumn id="24" xr3:uid="{362AFBD7-D8FE-484B-A796-99C68A4873AF}" name="dir_9" dataDxfId="94">
       <calculatedColumnFormula array="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_9]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{F8401415-A0F2-4302-B6F1-2F4769D22B7D}" name="dir_10" dataDxfId="11">
+    <tableColumn id="26" xr3:uid="{F8401415-A0F2-4302-B6F1-2F4769D22B7D}" name="dir_10" dataDxfId="93">
       <calculatedColumnFormula array="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_10]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{EB5FA985-8547-4A83-8A97-6BDBC99AFC75}" name="dir_11" dataDxfId="10">
+    <tableColumn id="27" xr3:uid="{EB5FA985-8547-4A83-8A97-6BDBC99AFC75}" name="dir_11" dataDxfId="92">
       <calculatedColumnFormula array="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_11]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{531860AE-4501-4DFE-ABC6-8AEC03CA2891}" name="dir_12" dataDxfId="9">
+    <tableColumn id="28" xr3:uid="{531860AE-4501-4DFE-ABC6-8AEC03CA2891}" name="dir_12" dataDxfId="91">
       <calculatedColumnFormula array="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_12]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{991CDA96-8100-4EC0-BA2D-509D87E3B77E}" name="control" dataDxfId="8">
+    <tableColumn id="13" xr3:uid="{991CDA96-8100-4EC0-BA2D-509D87E3B77E}" name="control" dataDxfId="90">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 6 * (table_6_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AB636280-F214-4141-A265-B2AC639CF4A7}" name="dsb_type" dataDxfId="7">
+    <tableColumn id="4" xr3:uid="{AB636280-F214-4141-A265-B2AC639CF4A7}" name="dsb_type" dataDxfId="89">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], 6 * (table_6_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{56C39C59-71CD-4F29-9AA2-7C1BE588DDCF}" name="strand" dataDxfId="6">
+    <tableColumn id="5" xr3:uid="{56C39C59-71CD-4F29-9AA2-7C1BE588DDCF}" name="strand" dataDxfId="88">
       <calculatedColumnFormula>OFFSET(table_3_1[strand], 6 * (table_6_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{77B8B06C-E91A-4366-BAAD-4D98914358E6}" name="hguide" dataDxfId="5">
+    <tableColumn id="6" xr3:uid="{77B8B06C-E91A-4366-BAAD-4D98914358E6}" name="hguide" dataDxfId="87">
       <calculatedColumnFormula>OFFSET(table_3_1[hguide], 6 * (table_6_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{64A9E7E6-7F9F-4F61-9A23-E4157ABDCFAC}" name="subst_type" dataDxfId="4">
+    <tableColumn id="9" xr3:uid="{64A9E7E6-7F9F-4F61-9A23-E4157ABDCFAC}" name="subst_type" dataDxfId="86">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{B53E652A-5D37-4D63-8F38-4B8DBDB37226}" name="dir_out" dataDxfId="3">
+    <tableColumn id="19" xr3:uid="{B53E652A-5D37-4D63-8F38-4B8DBDB37226}" name="dir_out" dataDxfId="85">
       <calculatedColumnFormula>_xlfn.CONCAT(table_6_1[[#This Row],[dsb_type]], "_", table_6_1[[#This Row],[strand]], IF(table_6_1[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_1[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{9C3C4C97-49A2-40B9-BCC3-5739C07213CD}" name="command" dataDxfId="2">
+    <tableColumn id="10" xr3:uid="{9C3C4C97-49A2-40B9-BCC3-5739C07213CD}" name="command" dataDxfId="84">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", _xlfn.TEXTJOIN(" ", TRUE, table_6_1[[#This Row],[dir_1]:[dir_12]]), " -o ", layouts, "/", table_6_1[[#This Row],[dir_out]], " --subst_type ", table_6_1[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2714,35 +2844,35 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{5FFA4758-C47A-4F1C-9890-69E7F39BE130}" name="table_6_2" displayName="table_6_2" ref="A11:J13" totalsRowShown="0" headerRowDxfId="35" dataDxfId="22" headerRowBorderDxfId="33" tableBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{5FFA4758-C47A-4F1C-9890-69E7F39BE130}" name="table_6_2" displayName="table_6_2" ref="A11:J13" totalsRowShown="0" headerRowDxfId="83" dataDxfId="81" headerRowBorderDxfId="82" tableBorderDxfId="80">
   <autoFilter ref="A11:J13" xr:uid="{5FFA4758-C47A-4F1C-9890-69E7F39BE130}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{40A0667B-C93C-4531-B41F-A65EDE89F51E}" name="index" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{A54C9A1D-E384-4C87-B6DD-98A7ADBAD240}" name="dir_1" dataDxfId="31">
-      <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset - 1 + COLUMN() - 2 + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1))</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{40A0667B-C93C-4531-B41F-A65EDE89F51E}" name="index" dataDxfId="79"/>
+    <tableColumn id="2" xr3:uid="{A54C9A1D-E384-4C87-B6DD-98A7ADBAD240}" name="dir_1" dataDxfId="78">
+      <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset  + COLUMN() - 2 + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{7CACC7DC-6834-41E4-A17F-74F62473FF4D}" name="dir_2" dataDxfId="30">
-      <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset - 1 + COLUMN() - 2 + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1))</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{7CACC7DC-6834-41E4-A17F-74F62473FF4D}" name="dir_2" dataDxfId="77">
+      <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset + COLUMN() - 2 + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{BEB4CA3E-14C3-4D70-BAFF-DBFFE398E04E}" name="control" dataDxfId="29">
-      <calculatedColumnFormula>OFFSET(table_3_1[control], var_6_anti_offset - 1 + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{BEB4CA3E-14C3-4D70-BAFF-DBFFE398E04E}" name="control" dataDxfId="76">
+      <calculatedColumnFormula>OFFSET(table_3_1[control], var_6_anti_offset  + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{08F18E8F-5127-4F55-95E0-05877340A45E}" name="dsb_type" dataDxfId="28">
-      <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], var_6_anti_offset - 1 + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{08F18E8F-5127-4F55-95E0-05877340A45E}" name="dsb_type" dataDxfId="75">
+      <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], var_6_anti_offset  + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B0010190-2798-4D5F-A1DA-8D1F1A867502}" name="strand" dataDxfId="27">
-      <calculatedColumnFormula array="1">OFFSET(table_3_1[strand], var_6_anti_offset - 1 + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{B0010190-2798-4D5F-A1DA-8D1F1A867502}" name="strand" dataDxfId="74">
+      <calculatedColumnFormula array="1">OFFSET(table_3_1[strand], var_6_anti_offset  + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{689C42CC-8508-4116-808A-19A0641C3F05}" name="hguide" dataDxfId="26">
-      <calculatedColumnFormula>OFFSET(table_3_1[hguide], var_6_anti_offset - 1 + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
+    <tableColumn id="7" xr3:uid="{689C42CC-8508-4116-808A-19A0641C3F05}" name="hguide" dataDxfId="73">
+      <calculatedColumnFormula>OFFSET(table_3_1[hguide], var_6_anti_offset + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{48005280-1CD9-4496-941A-723AEDDD9036}" name="subst_type" dataDxfId="25">
+    <tableColumn id="8" xr3:uid="{48005280-1CD9-4496-941A-723AEDDD9036}" name="subst_type" dataDxfId="72">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{5F8C6AF1-A602-4306-A909-592B4268C611}" name="dir_out" dataDxfId="24">
+    <tableColumn id="9" xr3:uid="{5F8C6AF1-A602-4306-A909-592B4268C611}" name="dir_out" dataDxfId="71">
       <calculatedColumnFormula>_xlfn.CONCAT(table_6_2[[#This Row],[dsb_type]], "_", table_6_2[[#This Row],[strand]], IF(table_6_2[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_2[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{3AEE0650-E928-4CB1-8CCF-22F967A16636}" name="command" dataDxfId="23">
+    <tableColumn id="10" xr3:uid="{3AEE0650-E928-4CB1-8CCF-22F967A16636}" name="command" dataDxfId="70">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", _xlfn.TEXTJOIN(" ", TRUE, table_6_2[[#This Row],[dir_1]:[dir_2]]), " -o ", layouts, "/", table_6_2[[#This Row],[dir_out]], " --subst_type ", table_6_2[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2751,30 +2881,33 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}" name="table_6_3" displayName="table_6_3" ref="A15:H17" totalsRowShown="0" headerRowDxfId="52">
-  <autoFilter ref="A15:H17" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}"/>
-  <tableColumns count="8">
-    <tableColumn id="25" xr3:uid="{D7EEB429-5A34-4903-8247-E1BD5C0098AE}" name="index" dataDxfId="51"/>
-    <tableColumn id="18" xr3:uid="{BACD6182-9E09-4A02-A171-8DFCB7543380}" name="dir" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}" name="table_6_3" displayName="table_6_3" ref="A15:I16" totalsRowShown="0" headerRowDxfId="69">
+  <autoFilter ref="A15:I16" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}"/>
+  <tableColumns count="9">
+    <tableColumn id="25" xr3:uid="{D7EEB429-5A34-4903-8247-E1BD5C0098AE}" name="index" dataDxfId="68"/>
+    <tableColumn id="18" xr3:uid="{BACD6182-9E09-4A02-A171-8DFCB7543380}" name="dir" dataDxfId="67">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 12, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{39C35B5A-7D06-4895-BF0F-A803A5F94E2E}" name="strand" dataDxfId="47">
-      <calculatedColumnFormula array="1">_xlfn.TEXTJOIN(" ", TRUE, IF(OFFSET(table_3_1[[strand]:[strand]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_3[dir]) - COLUMN(table_6_3[[dir]:[dir]]), 0, 12, 1) = "R1", "+", "-"))</calculatedColumnFormula>
+    <tableColumn id="2" xr3:uid="{39C35B5A-7D06-4895-BF0F-A803A5F94E2E}" name="strand" dataDxfId="66">
+      <calculatedColumnFormula array="1">_xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[strand]:[strand]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 12, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{F617BC3E-90A8-4E63-B2A4-EAC9DE705FC7}" name="control" dataDxfId="50">
+    <tableColumn id="13" xr3:uid="{F617BC3E-90A8-4E63-B2A4-EAC9DE705FC7}" name="control" dataDxfId="65">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 6 * (table_6_3[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{8E20D9FC-49B1-428A-AC5E-AEDADB1473AC}" name="dsb_type" dataDxfId="46">
+    <tableColumn id="4" xr3:uid="{8E20D9FC-49B1-428A-AC5E-AEDADB1473AC}" name="dsb_type" dataDxfId="64">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], 12 * (table_6_3[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{FB278FFE-A956-4B0C-8CC3-6A0324CBCA11}" name="subst_type" dataDxfId="49">
+    <tableColumn id="33" xr3:uid="{8FF7E83A-9135-4A64-965C-48368A6C0367}" name="hguide">
+      <calculatedColumnFormula array="1">OFFSET(table_3_1[[hguide]:[hguide]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{FB278FFE-A956-4B0C-8CC3-6A0324CBCA11}" name="subst_type" dataDxfId="63">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{E4089767-2E77-4296-9392-7BCD64E1E62D}" name="dir_out" dataDxfId="48">
-      <calculatedColumnFormula>_xlfn.CONCAT(table_6_3[[#This Row],[dsb_type]], IF(table_6_3[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_3[[#This Row],[control]]), ""))</calculatedColumnFormula>
+    <tableColumn id="19" xr3:uid="{E4089767-2E77-4296-9392-7BCD64E1E62D}" name="dir_out" dataDxfId="62">
+      <calculatedColumnFormula>_xlfn.CONCAT(table_6_3[[#This Row],[dsb_type]], "_", table_6_3[[#This Row],[hguide]], IF(table_6_3[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_3[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{8BD09F85-30B0-46CA-A0E3-2CC4F3FB2BD0}" name="command" dataDxfId="45">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_3[[#This Row],[dir]], " -s ", table_6_3[[#This Row],[strand]], " -o ", layouts, "/", table_6_3[[#This Row],[dir_out]], " --subst_type ", table_6_3[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{8BD09F85-30B0-46CA-A0E3-2CC4F3FB2BD0}" name="command" dataDxfId="61">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_3[[#This Row],[dir]], IF(NOT(ISNA(table_6_3[[#This Row],[strand]])), _xlfn.CONCAT(" -s ", table_6_3[[#This Row],[strand]]), ""), " -o ", layouts, "/", table_6_3[[#This Row],[dir_out]], " --subst_type ", table_6_3[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2782,30 +2915,33 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}" name="table_6_4" displayName="table_6_4" ref="A19:H20" totalsRowShown="0" headerRowDxfId="44" headerRowBorderDxfId="42" tableBorderDxfId="43">
-  <autoFilter ref="A19:H20" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{0F421990-E775-4F35-92AF-6BA19E0E8AEE}" name="index"/>
-    <tableColumn id="2" xr3:uid="{81FE7256-F482-4A2C-902D-871C80C1D881}" name="dir_1" dataDxfId="37">
-      <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset - 1 + 4 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 4, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}" name="table_6_4" displayName="table_6_4" ref="A19:I21" totalsRowShown="0" headerRowDxfId="60">
+  <autoFilter ref="A19:I21" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}"/>
+  <tableColumns count="9">
+    <tableColumn id="25" xr3:uid="{4FA5A2E4-C9F7-4673-98E1-BCCE618B100D}" name="index" dataDxfId="59"/>
+    <tableColumn id="18" xr3:uid="{155653FE-38BD-4542-A5AE-2B40B0FD52C7}" name="dir" dataDxfId="58">
+      <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 6, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E9F8E6A0-B4A7-475B-9ED2-9F2A4A9EB628}" name="strand" dataDxfId="36">
-      <calculatedColumnFormula array="1">_xlfn.TEXTJOIN(" ", TRUE, IF(OFFSET(table_3_1[[strand]:[strand]], var_6_anti_offset - 1 + 4 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 4, 1) = "R1", "+", "-"))</calculatedColumnFormula>
+    <tableColumn id="34" xr3:uid="{05E960C2-864E-41C3-A84E-DF767C09AA42}" name="strand" dataDxfId="57">
+      <calculatedColumnFormula>NA()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{84D215B2-E673-4076-824E-08C601909C2B}" name="control" dataDxfId="41">
-      <calculatedColumnFormula>OFFSET(table_3_1[control], var_6_anti_offset - 1 + 4 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
+    <tableColumn id="13" xr3:uid="{9EA58FA8-5496-4600-905A-95909513339B}" name="control" dataDxfId="56">
+      <calculatedColumnFormula>OFFSET(table_3_1[control], 6 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{FA9180EA-3AA0-451A-ACAC-78776C7CB75D}" name="dsb_type" dataDxfId="40">
-      <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], var_6_anti_offset - 1 + 4 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{46390A5F-98AD-4211-85B4-A4DD8E31C40C}" name="dsb_type" dataDxfId="55">
+      <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{E0783723-9246-4BF6-A5DA-E000EA1E5E87}" name="subst_type">
+    <tableColumn id="35" xr3:uid="{5BD83012-469D-4202-9584-AA182CDF11F9}" name="hguide">
+      <calculatedColumnFormula array="1">OFFSET(table_3_1[[hguide]:[hguide]], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{123049FA-F284-452C-8FDD-63F409D9967F}" name="subst_type" dataDxfId="54">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{3D97DBDD-03E9-4A6C-BADA-D01B27A8EE51}" name="dir_out" dataDxfId="39">
-      <calculatedColumnFormula>_xlfn.CONCAT(table_6_4[[#This Row],[dsb_type]], IF(table_6_4[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_4[[#This Row],[control]]), ""))</calculatedColumnFormula>
+    <tableColumn id="19" xr3:uid="{CFCDDB26-095C-4395-82E2-37B45B0CDEAD}" name="dir_out" dataDxfId="53">
+      <calculatedColumnFormula>_xlfn.CONCAT(table_6_4[[#This Row],[dsb_type]], "_", table_6_4[[#This Row],[hguide]], IF(table_6_4[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_4[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5E7626AE-E376-4C60-BA64-B24F95580083}" name="command" dataDxfId="38">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_4[[#This Row],[dir_1]], " - ", table_6_4[[#This Row],[strand]], " -o ", layouts, "/", table_6_4[[#This Row],[dir_out]], " --subst_type ", table_6_4[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{DC6C9CBA-5796-4FFE-878D-BB47DC276187}" name="command" dataDxfId="52">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_4[[#This Row],[dir]], IF(NOT(ISNA(table_6_4[[#This Row],[strand]])), _xlfn.CONCAT(" -s ", table_6_4[[#This Row],[strand]]), ""), " -o ", layouts, "/", table_6_4[[#This Row],[dir_out]], " --subst_type ", table_6_4[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2813,48 +2949,33 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{86CE8E4A-18BF-427A-81F0-F9655767A016}" name="table_7_1" displayName="table_7_1" ref="A2:N42" totalsRowShown="0" headerRowDxfId="94">
-  <autoFilter ref="A2:N42" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
-  <tableColumns count="14">
-    <tableColumn id="25" xr3:uid="{C323C376-24D3-4404-9E0F-6E9361862271}" name="index" dataDxfId="93"/>
-    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="92">
-      <calculatedColumnFormula>OFFSET(table_3_1[[dir]:[dir]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}" name="table_6_5" displayName="table_6_5" ref="A23:I24" totalsRowShown="0" headerRowDxfId="51" headerRowBorderDxfId="50" tableBorderDxfId="49">
+  <autoFilter ref="A23:I24" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{0F421990-E775-4F35-92AF-6BA19E0E8AEE}" name="index"/>
+    <tableColumn id="2" xr3:uid="{81FE7256-F482-4A2C-902D-871C80C1D881}" name="dir" dataDxfId="48">
+      <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]:[index]] - 1), 0, 4, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="91">
-      <calculatedColumnFormula>OFFSET(table_3_1[[control]:[control]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{E9F8E6A0-B4A7-475B-9ED2-9F2A4A9EB628}" name="strand" dataDxfId="47">
+      <calculatedColumnFormula array="1">_xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[strand]:[strand]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]:[index]] - 1), 0, 4, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="90">
-      <calculatedColumnFormula>OFFSET(table_3_1[[ref]:[ref]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{70821CEE-FFC4-44AB-ACF6-DA81A4B053E6}" name="control" dataDxfId="46">
+      <calculatedColumnFormula>OFFSET(table_3_1[control], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="89">
-      <calculatedColumnFormula>OFFSET(table_3_1[[dsb_pos]:[dsb_pos]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{FA9180EA-3AA0-451A-ACAC-78776C7CB75D}" name="dsb_type" dataDxfId="45">
+      <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="88">
-      <calculatedColumnFormula>OFFSET(table_3_1[[dsb_type]:[dsb_type]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
+    <tableColumn id="8" xr3:uid="{E0783723-9246-4BF6-A5DA-E000EA1E5E87}" name="subst_type">
+      <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="87">
-      <calculatedColumnFormula>OFFSET(table_3_1[[dsb_type_command]:[dsb_type_command]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{DE820E4E-FF8B-435B-B07F-D397029AF597}" name="hguide" dataDxfId="44">
+      <calculatedColumnFormula>OFFSET(table_3_1[[hguide]:[hguide]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="86">
-      <calculatedColumnFormula>OFFSET(table_3_1[[strand]:[strand]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
+    <tableColumn id="9" xr3:uid="{3D97DBDD-03E9-4A6C-BADA-D01B27A8EE51}" name="dir_out" dataDxfId="43">
+      <calculatedColumnFormula>_xlfn.CONCAT(table_6_5[[#This Row],[dsb_type]], "_", table_6_5[[#This Row],[hguide]], IF(table_6_5[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_5[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="85">
-      <calculatedColumnFormula>OFFSET(table_3_1[[hguide]:[hguide]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="84">
-      <calculatedColumnFormula>OFFSET(table_3_1[[cell]:[cell]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="83">
-      <calculatedColumnFormula>OFFSET(table_3_1[[treatment]:[treatment]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="82">
-      <calculatedColumnFormula>"without"</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="81">
-      <calculatedColumnFormula>IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="54">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{5E7626AE-E376-4C60-BA64-B24F95580083}" name="command" dataDxfId="42">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_5[[#This Row],[dir]], " -s ", table_6_5[[#This Row],[strand]], " -o ", layouts, "/", table_6_5[[#This Row],[dir_out]], " --subst_type ", table_6_5[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2862,47 +2983,96 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{86CE8E4A-18BF-427A-81F0-F9655767A016}" name="table_7_1" displayName="table_7_1" ref="A2:N42" totalsRowShown="0" headerRowDxfId="41">
+  <autoFilter ref="A2:N42" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
+  <tableColumns count="14">
+    <tableColumn id="25" xr3:uid="{C323C376-24D3-4404-9E0F-6E9361862271}" name="index" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="39">
+      <calculatedColumnFormula>OFFSET(table_3_1[[dir]:[dir]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="38">
+      <calculatedColumnFormula>OFFSET(table_3_1[[control]:[control]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="37">
+      <calculatedColumnFormula>OFFSET(table_3_1[[ref]:[ref]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="36">
+      <calculatedColumnFormula>OFFSET(table_3_1[[dsb_pos]:[dsb_pos]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="35">
+      <calculatedColumnFormula>OFFSET(table_3_1[[dsb_type]:[dsb_type]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="34">
+      <calculatedColumnFormula>OFFSET(table_3_1[[dsb_type_command]:[dsb_type_command]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="33">
+      <calculatedColumnFormula>OFFSET(table_3_1[[strand]:[strand]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="32">
+      <calculatedColumnFormula>OFFSET(table_3_1[[hguide]:[hguide]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="31">
+      <calculatedColumnFormula>OFFSET(table_3_1[[cell]:[cell]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="30">
+      <calculatedColumnFormula>OFFSET(table_3_1[[treatment]:[treatment]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="29">
+      <calculatedColumnFormula>"without"</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="28">
+      <calculatedColumnFormula>IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="0">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{B47D9508-D874-40FC-B6F6-C106B48F6A94}" name="table_7_2" displayName="table_7_2" ref="A44:N56" totalsRowShown="0">
   <autoFilter ref="A44:N56" xr:uid="{D74A5276-1A50-4DA1-9131-9669404C8622}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{488C5146-A746-4F74-BCC8-806E4DC740CE}" name="index" dataDxfId="80"/>
-    <tableColumn id="2" xr3:uid="{C2A88DF4-2444-4C4C-A089-6CF9ADE79BD8}" name="dir" dataDxfId="79">
+    <tableColumn id="1" xr3:uid="{488C5146-A746-4F74-BCC8-806E4DC740CE}" name="index" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{C2A88DF4-2444-4C4C-A089-6CF9ADE79BD8}" name="dir" dataDxfId="26">
       <calculatedColumnFormula>OFFSET(table_3_2[[dir]:[dir]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{7698ACE3-2351-400D-B00F-5A70184F8A33}" name="control" dataDxfId="78">
+    <tableColumn id="3" xr3:uid="{7698ACE3-2351-400D-B00F-5A70184F8A33}" name="control" dataDxfId="25">
       <calculatedColumnFormula>OFFSET(table_3_2[[control]:[control]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5E82B04C-FF09-492C-8A23-7E43B5990149}" name="ref" dataDxfId="77">
+    <tableColumn id="4" xr3:uid="{5E82B04C-FF09-492C-8A23-7E43B5990149}" name="ref" dataDxfId="24">
       <calculatedColumnFormula>OFFSET(table_3_2[[ref]:[ref]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{F4D36A0E-549B-4F3A-BCA9-75E151448998}" name="dsb_pos" dataDxfId="76">
+    <tableColumn id="5" xr3:uid="{F4D36A0E-549B-4F3A-BCA9-75E151448998}" name="dsb_pos" dataDxfId="23">
       <calculatedColumnFormula>OFFSET(table_3_2[[dsb_pos]:[dsb_pos]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{AEBBBB88-8CE2-409D-AE19-9C23263250A9}" name="dsb_type" dataDxfId="75">
+    <tableColumn id="6" xr3:uid="{AEBBBB88-8CE2-409D-AE19-9C23263250A9}" name="dsb_type" dataDxfId="22">
       <calculatedColumnFormula>OFFSET(table_3_2[[dsb_type]:[dsb_type]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3E71E7D2-0FA5-4FD5-BDC3-2955A091A9E6}" name="dsb_type_command" dataDxfId="74">
+    <tableColumn id="7" xr3:uid="{3E71E7D2-0FA5-4FD5-BDC3-2955A091A9E6}" name="dsb_type_command" dataDxfId="21">
       <calculatedColumnFormula>OFFSET(table_3_2[[dsb_type_command]:[dsb_type_command]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{EBD35881-E696-4202-9149-75A4EFFFAAD6}" name="strand" dataDxfId="73">
+    <tableColumn id="8" xr3:uid="{EBD35881-E696-4202-9149-75A4EFFFAAD6}" name="strand" dataDxfId="20">
       <calculatedColumnFormula>OFFSET(table_3_2[[strand]:[strand]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{123CA279-0CB6-41C1-9CD8-20D375B9B66D}" name="hguide" dataDxfId="72">
+    <tableColumn id="9" xr3:uid="{123CA279-0CB6-41C1-9CD8-20D375B9B66D}" name="hguide" dataDxfId="19">
       <calculatedColumnFormula>OFFSET(table_3_2[[hguide]:[hguide]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{3DCE3F3A-187D-411E-93FC-8C6C3EE9CAA2}" name="cell" dataDxfId="71">
+    <tableColumn id="10" xr3:uid="{3DCE3F3A-187D-411E-93FC-8C6C3EE9CAA2}" name="cell" dataDxfId="18">
       <calculatedColumnFormula>OFFSET(table_3_2[[cell]:[cell]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{9E585D29-AB3E-4D04-8C1D-24F78339C9A3}" name="treatment" dataDxfId="70">
+    <tableColumn id="11" xr3:uid="{9E585D29-AB3E-4D04-8C1D-24F78339C9A3}" name="treatment" dataDxfId="17">
       <calculatedColumnFormula>OFFSET(table_3_2[[treatment]:[treatment]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{928286B8-23FB-4375-B52B-617DD59D6098}" name="subst_type" dataDxfId="69">
+    <tableColumn id="12" xr3:uid="{928286B8-23FB-4375-B52B-617DD59D6098}" name="subst_type" dataDxfId="16">
       <calculatedColumnFormula>"without"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{E18D2025-56E8-4128-9201-9E0BF8A67AC0}" name="common_layout_dir" dataDxfId="68">
+    <tableColumn id="15" xr3:uid="{E18D2025-56E8-4128-9201-9E0BF8A67AC0}" name="common_layout_dir" dataDxfId="15">
       <calculatedColumnFormula>OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_2[[#This Row],[index]] - 1, 6) + 2, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{0917AB98-1545-4642-9BE8-618AAA1E404A}" name="command" dataDxfId="53">
+    <tableColumn id="13" xr3:uid="{0917AB98-1545-4642-9BE8-618AAA1E404A}" name="command" dataDxfId="14">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2910,15 +3080,15 @@
 </table>
 </file>
 
-<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{B76EEC45-4FC3-44D5-9B2E-9183DF724F60}" name="table_7_3" displayName="table_7_3" ref="A3:C19" totalsRowShown="0" headerRowDxfId="67">
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{B76EEC45-4FC3-44D5-9B2E-9183DF724F60}" name="table_7_3" displayName="table_7_3" ref="A3:C19" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A3:C19" xr:uid="{B76EEC45-4FC3-44D5-9B2E-9183DF724F60}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{FAFADB73-BF3B-401A-8C48-9FCB5D3C4CB6}" name="index" dataDxfId="66"/>
-    <tableColumn id="4" xr3:uid="{8541A14E-3250-4B9C-B315-969FC11BE60A}" name="dir" dataDxfId="65">
+    <tableColumn id="1" xr3:uid="{FAFADB73-BF3B-401A-8C48-9FCB5D3C4CB6}" name="index" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{8541A14E-3250-4B9C-B315-969FC11BE60A}" name="dir" dataDxfId="11">
       <calculatedColumnFormula>OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{EAD6D5EC-B61E-4A98-B4FD-4932757CFEA3}" name="command" dataDxfId="64">
+    <tableColumn id="6" xr3:uid="{EAD6D5EC-B61E-4A98-B4FD-4932757CFEA3}" name="command" dataDxfId="10">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2926,27 +3096,11 @@
 </table>
 </file>
 
-<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{8B4E853A-A4F1-4022-B857-226C57559A5F}" name="table_7_4" displayName="table_7_4" ref="A21:C23" totalsRowShown="0" headerRowDxfId="63">
-  <autoFilter ref="A21:C23" xr:uid="{8B4E853A-A4F1-4022-B857-226C57559A5F}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{1ECF32A2-E353-4754-B4C5-11C46AACF6C0}" name="index" dataDxfId="62"/>
-    <tableColumn id="4" xr3:uid="{181C59FC-364D-4421-8E54-98DFF4CA7C05}" name="dir" dataDxfId="61">
-      <calculatedColumnFormula>OFFSET(table_4_2[[dir_out]:[dir_out]], table_7_4[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{6D8CC942-572B-44F2-BCA6-4D31A25A4067}" name="command" dataDxfId="60">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_4[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_2[[dir_out]:[dir_out]],table_7_4[[#This Row],[index]] - 1, 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22A90416-B904-4D3D-A6DB-EFCB9FD1EAED}" name="table_1" displayName="table_1" ref="A1:O173" totalsRowShown="0" headerRowDxfId="223">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22A90416-B904-4D3D-A6DB-EFCB9FD1EAED}" name="table_1" displayName="table_1" ref="A1:O173" totalsRowShown="0" headerRowDxfId="233">
   <autoFilter ref="A1:O173" xr:uid="{22A90416-B904-4D3D-A6DB-EFCB9FD1EAED}"/>
   <tableColumns count="15">
-    <tableColumn id="15" xr3:uid="{A06DA701-31D6-44A5-8655-82CAD7E3082B}" name="index" dataDxfId="222"/>
+    <tableColumn id="15" xr3:uid="{A06DA701-31D6-44A5-8655-82CAD7E3082B}" name="index" dataDxfId="232"/>
     <tableColumn id="1" xr3:uid="{5C1CDEE9-AAC7-4E12-B88F-1314CF422335}" name="library"/>
     <tableColumn id="2" xr3:uid="{D4B174CF-F774-4DA7-B75D-573BC94EE10F}" name="cell"/>
     <tableColumn id="3" xr3:uid="{83898EC9-96DA-46D4-B0B8-F68C7607DCF2}" name="control"/>
@@ -2954,25 +3108,25 @@
     <tableColumn id="5" xr3:uid="{81A143FE-8E74-4182-8124-E697DD5A7C62}" name="hguide"/>
     <tableColumn id="6" xr3:uid="{4A316E6A-69F3-4B78-9C01-4675AEB656FA}" name="treatment"/>
     <tableColumn id="7" xr3:uid="{25B8E763-346D-4756-8B58-D3C8CB103545}" name="strand"/>
-    <tableColumn id="8" xr3:uid="{4B708639-BB19-4DC1-A57D-214FA0EFB1EA}" name="dsb_pos" dataDxfId="221">
+    <tableColumn id="8" xr3:uid="{4B708639-BB19-4DC1-A57D-214FA0EFB1EA}" name="dsb_pos" dataDxfId="231">
       <calculatedColumnFormula array="1">IF(E2="2DSB", IF(H2="R1", 67, 46), IF(E2="1DSB", IF(H2="R1", 67, 46), IF(E2="2DSBanti", IF(H2="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{CCF6021C-1B60-4954-A92E-3F2848564215}" name="file_in" dataDxfId="220">
+    <tableColumn id="9" xr3:uid="{CCF6021C-1B60-4954-A92E-3F2848564215}" name="file_in" dataDxfId="230">
       <calculatedColumnFormula>IF(OR(table_1[[#This Row],[control]]="none", table_1[[#This Row],[control]]="30bpDown"), _xlfn.CONCAT(table_1[[#This Row],[library]], IF(table_1[[#This Row],[dsb_type]] = "2DSBanti", "_anti", ""), "_",table_1[[#This Row],[strand]],"_", IF(LEFT(table_1[[#This Row],[dsb_type]], 1)="2","2DSBs", table_1[[#This Row],[hguide]]), ".sam"), _xlfn.CONCAT(table_1[[#This Row],[library]], "_NHEJ_", IF(table_1[[#This Row],[hguide]]="sgA", "hg39", IF(table_1[[#This Row],[hguide]]="sgB", "hg42", "2DSB")), "_", table_1[[#This Row],[strand]], ".sam"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{58220462-2A11-4DAD-A247-C0871AFCFDB4}" name="file_out" dataDxfId="219">
+    <tableColumn id="10" xr3:uid="{58220462-2A11-4DAD-A247-C0871AFCFDB4}" name="file_out" dataDxfId="229">
       <calculatedColumnFormula>_xlfn.CONCAT(table_1[[#This Row],[library]], "_", table_1[[#This Row],[cell]], "_", table_1[[#This Row],[hguide]], "_", table_1[[#This Row],[strand]], "_", table_1[[#This Row],[treatment]], IF(table_1[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_1[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{775EE7A9-3C78-4568-BF98-500DE451177C}" name="ref" dataDxfId="218">
+    <tableColumn id="11" xr3:uid="{775EE7A9-3C78-4568-BF98-500DE451177C}" name="ref" dataDxfId="228">
       <calculatedColumnFormula>_xlfn.CONCAT(table_1[[#This Row],[dsb_type]],"_", table_1[[#This Row],[strand]],"_", table_1[[#This Row],[treatment]], ".fa")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{5B945FB6-D054-40C4-AAEF-BB50B19F8936}" name="total_reads" dataDxfId="217">
+    <tableColumn id="12" xr3:uid="{5B945FB6-D054-40C4-AAEF-BB50B19F8936}" name="total_reads" dataDxfId="227">
       <calculatedColumnFormula>VLOOKUP(INT(MID(table_1[[#This Row],[library]], 4, 10)), table_1_2[#All], IF(table_1[[#This Row],[strand]]="R1", 3, 4))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{66485B06-471E-47D3-BA91-FC751F58FA5A}" name="min_length" dataDxfId="216">
+    <tableColumn id="13" xr3:uid="{66485B06-471E-47D3-BA91-FC751F58FA5A}" name="min_length" dataDxfId="226">
       <calculatedColumnFormula>IF(LEFT(table_1[[#This Row],[dsb_type]], 1) = "2", 50, 130)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{DF3C46EA-690D-4E6A-99CF-BBC2B2F74AFF}" name="command_filter_nhej" dataDxfId="215">
+    <tableColumn id="14" xr3:uid="{DF3C46EA-690D-4E6A-99CF-BBC2B2F74AFF}" name="command_filter_nhej" dataDxfId="225">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", table_1[[#This Row],[file_in]], " -ref ref_seq/", table_1[[#This Row],[ref]], " -o ", libraries_2, "/", table_1[[#This Row],[file_out]], ".tsv", " --min_length ", table_1[[#This Row],[min_length]], " -dsb ", table_1[[#This Row],[dsb_pos]], " --quiet")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2981,14 +3135,30 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{58F5EC27-BD76-45AE-8D38-F4E705EF79E9}" name="table_7_5" displayName="table_7_5" ref="A26:C34" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{8B4E853A-A4F1-4022-B857-226C57559A5F}" name="table_7_4" displayName="table_7_4" ref="A21:C23" totalsRowShown="0" headerRowDxfId="9">
+  <autoFilter ref="A21:C23" xr:uid="{8B4E853A-A4F1-4022-B857-226C57559A5F}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{1ECF32A2-E353-4754-B4C5-11C46AACF6C0}" name="index" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{181C59FC-364D-4421-8E54-98DFF4CA7C05}" name="dir" dataDxfId="7">
+      <calculatedColumnFormula>OFFSET(table_4_2[[dir_out]:[dir_out]], table_7_4[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{6D8CC942-572B-44F2-BCA6-4D31A25A4067}" name="command" dataDxfId="6">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_4[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_2[[dir_out]:[dir_out]],table_7_4[[#This Row],[index]] - 1, 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{58F5EC27-BD76-45AE-8D38-F4E705EF79E9}" name="table_7_5" displayName="table_7_5" ref="A26:C34" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A26:C34" xr:uid="{58F5EC27-BD76-45AE-8D38-F4E705EF79E9}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{AAC1476C-44CE-49FD-8254-50BAEAA6929C}" name="index" dataDxfId="57"/>
-    <tableColumn id="4" xr3:uid="{1222E48F-ED5C-48AA-BA39-1443B841BC9F}" name="dir" dataDxfId="56">
+    <tableColumn id="1" xr3:uid="{AAC1476C-44CE-49FD-8254-50BAEAA6929C}" name="index" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{1222E48F-ED5C-48AA-BA39-1443B841BC9F}" name="dir" dataDxfId="2">
       <calculatedColumnFormula>OFFSET(table_4_3[[dir_out]:[dir_out]], table_7_5[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{89B7E589-2097-43FC-B96B-19D2EF777E97}" name="command" dataDxfId="55">
+    <tableColumn id="6" xr3:uid="{89B7E589-2097-43FC-B96B-19D2EF777E97}" name="command" dataDxfId="1">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2997,38 +3167,38 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}" name="table_2_1" displayName="table_2_1" ref="A1:S41" totalsRowShown="0" headerRowDxfId="214">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}" name="table_2_1" displayName="table_2_1" ref="A1:S41" totalsRowShown="0" headerRowDxfId="224">
   <autoFilter ref="A1:S41" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{C373869E-A92E-4B06-B8E5-C5A873420ED4}" name="index" dataDxfId="213"/>
-    <tableColumn id="2" xr3:uid="{A28AAC50-FA09-494A-B052-8489F07A5A70}" name="ref" dataDxfId="212">
+    <tableColumn id="1" xr3:uid="{C373869E-A92E-4B06-B8E5-C5A873420ED4}" name="index" dataDxfId="223"/>
+    <tableColumn id="2" xr3:uid="{A28AAC50-FA09-494A-B052-8489F07A5A70}" name="ref" dataDxfId="222">
       <calculatedColumnFormula>OFFSET(table_1[ref], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{07D57089-9737-4983-8884-C4ACCDCFF6CB}" name="control" dataDxfId="211">
+    <tableColumn id="18" xr3:uid="{07D57089-9737-4983-8884-C4ACCDCFF6CB}" name="control" dataDxfId="221">
       <calculatedColumnFormula>OFFSET(table_1[control], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{C6423FEA-272F-48D3-BC6A-909FCA937DA9}" name="dsb_type" dataDxfId="210">
+    <tableColumn id="19" xr3:uid="{C6423FEA-272F-48D3-BC6A-909FCA937DA9}" name="dsb_type" dataDxfId="220">
       <calculatedColumnFormula>OFFSET(table_1[dsb_type], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B8F61088-5FFA-4860-BF4E-1BFB301A31D9}" name="dsb_pos" dataDxfId="209">
+    <tableColumn id="3" xr3:uid="{B8F61088-5FFA-4860-BF4E-1BFB301A31D9}" name="dsb_pos" dataDxfId="219">
       <calculatedColumnFormula>OFFSET(table_1[dsb_pos], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{524D5B3D-BB20-420D-B7E9-93A7F77CA728}" name="cell" dataDxfId="208">
+    <tableColumn id="4" xr3:uid="{524D5B3D-BB20-420D-B7E9-93A7F77CA728}" name="cell" dataDxfId="218">
       <calculatedColumnFormula>OFFSET(table_1[cell], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{CC918D20-5D79-4223-9717-2CA0EFFA213F}" name="strand" dataDxfId="207">
+    <tableColumn id="5" xr3:uid="{CC918D20-5D79-4223-9717-2CA0EFFA213F}" name="strand" dataDxfId="217">
       <calculatedColumnFormula>OFFSET(table_1[strand], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B2851465-D533-4787-80C4-E844BB2ABB8C}" name="treatment" dataDxfId="206">
+    <tableColumn id="6" xr3:uid="{B2851465-D533-4787-80C4-E844BB2ABB8C}" name="treatment" dataDxfId="216">
       <calculatedColumnFormula>OFFSET(table_1[treatment], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{849BE448-7739-4815-A2C5-5843F62D83D7}" name="hguide" dataDxfId="205">
+    <tableColumn id="7" xr3:uid="{849BE448-7739-4815-A2C5-5843F62D83D7}" name="hguide" dataDxfId="215">
       <calculatedColumnFormula>OFFSET(table_1[hguide], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{343716D9-C3A9-4F90-A58A-42B1B9C79EBF}" name="output_dir" dataDxfId="204">
+    <tableColumn id="8" xr3:uid="{343716D9-C3A9-4F90-A58A-42B1B9C79EBF}" name="output_dir" dataDxfId="214">
       <calculatedColumnFormula>_xlfn.CONCAT(table_2_1[[#This Row],[cell]], "_", table_2_1[[#This Row],[hguide]], "_", table_2_1[[#This Row],[strand]], "_", table_2_1[[#This Row],[treatment]], IF(table_2_1[[#This Row],[control]]&lt;&gt;"none",_xlfn.CONCAT("_", table_2_1[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D29558AA-D418-4CDD-81AE-A987E7BC501D}" name="input_1" dataDxfId="203">
+    <tableColumn id="9" xr3:uid="{D29558AA-D418-4CDD-81AE-A987E7BC501D}" name="input_1" dataDxfId="213">
       <calculatedColumnFormula array="1">OFFSET(table_1[[file_out]:[file_out]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 11, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="22" xr3:uid="{3F29C0D1-58A3-430E-AAAA-9F679DCA46D6}" name="input_2">
@@ -3040,19 +3210,19 @@
     <tableColumn id="20" xr3:uid="{28521A62-94B3-4C7C-AF90-F4E2F4163D29}" name="input_4">
       <calculatedColumnFormula array="1">OFFSET(table_1[[file_out]:[file_out]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 11, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{E2ABF5A3-B032-47F7-9141-9F269EFD9D49}" name="total_reads_1" dataDxfId="202">
+    <tableColumn id="10" xr3:uid="{E2ABF5A3-B032-47F7-9141-9F269EFD9D49}" name="total_reads_1" dataDxfId="212">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{C7B1BE14-3BD6-413B-8575-DE9712F9761A}" name="total_reads_2" dataDxfId="201">
+    <tableColumn id="12" xr3:uid="{C7B1BE14-3BD6-413B-8575-DE9712F9761A}" name="total_reads_2" dataDxfId="211">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{6A8CE344-45B9-42E3-95D8-8EB6A485D968}" name="total_reads_3" dataDxfId="200">
+    <tableColumn id="14" xr3:uid="{6A8CE344-45B9-42E3-95D8-8EB6A485D968}" name="total_reads_3" dataDxfId="210">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{AC170216-9CAE-43B8-A8E2-8FE1529F6D55}" name="total_reads_4" dataDxfId="199">
+    <tableColumn id="16" xr3:uid="{AC170216-9CAE-43B8-A8E2-8FE1529F6D55}" name="total_reads_4" dataDxfId="209">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{A285A0DD-6F6D-404D-AE2A-0D1FC3DDB459}" name="command" dataDxfId="198">
+    <tableColumn id="17" xr3:uid="{A285A0DD-6F6D-404D-AE2A-0D1FC3DDB459}" name="command" dataDxfId="208">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3064,41 +3234,41 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{7D969AC7-2D2F-45B0-BA99-D174130B0A52}" name="table_2_2" displayName="table_2_2" ref="A44:M56" totalsRowShown="0">
   <autoFilter ref="A44:M56" xr:uid="{7D969AC7-2D2F-45B0-BA99-D174130B0A52}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{D612E3DF-AA8E-4EE0-9306-7903B4821992}" name="index" dataDxfId="197"/>
-    <tableColumn id="2" xr3:uid="{B00239B6-16E0-4472-B8C9-F25D625D21DD}" name="ref" dataDxfId="196">
+    <tableColumn id="1" xr3:uid="{D612E3DF-AA8E-4EE0-9306-7903B4821992}" name="index" dataDxfId="207"/>
+    <tableColumn id="2" xr3:uid="{B00239B6-16E0-4472-B8C9-F25D625D21DD}" name="ref" dataDxfId="206">
       <calculatedColumnFormula>OFFSET(table_1[ref], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{47FE94A7-C208-4138-B063-127D4AE215A0}" name="control" dataDxfId="195">
+    <tableColumn id="3" xr3:uid="{47FE94A7-C208-4138-B063-127D4AE215A0}" name="control" dataDxfId="205">
       <calculatedColumnFormula>OFFSET(table_1[control], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{43B4F550-AB35-4206-AAAB-820BBA723DEA}" name="dsb_type" dataDxfId="194">
+    <tableColumn id="4" xr3:uid="{43B4F550-AB35-4206-AAAB-820BBA723DEA}" name="dsb_type" dataDxfId="204">
       <calculatedColumnFormula>OFFSET(table_1[dsb_type], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7233C674-8249-48C9-814C-599A94DF6097}" name="dsb_pos" dataDxfId="193">
+    <tableColumn id="5" xr3:uid="{7233C674-8249-48C9-814C-599A94DF6097}" name="dsb_pos" dataDxfId="203">
       <calculatedColumnFormula>OFFSET(table_1[dsb_pos], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8FD419DF-3888-4BC8-ACF7-F31E7AB24754}" name="cell" dataDxfId="192">
+    <tableColumn id="6" xr3:uid="{8FD419DF-3888-4BC8-ACF7-F31E7AB24754}" name="cell" dataDxfId="202">
       <calculatedColumnFormula>OFFSET(table_1[cell], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{612FF909-1004-49E1-BC8F-F65A8C97EEFC}" name="strand" dataDxfId="191">
+    <tableColumn id="7" xr3:uid="{612FF909-1004-49E1-BC8F-F65A8C97EEFC}" name="strand" dataDxfId="201">
       <calculatedColumnFormula>OFFSET(table_1[strand], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C57AB4D7-F308-46D6-8F19-069619F8CF1B}" name="treatment" dataDxfId="190">
+    <tableColumn id="8" xr3:uid="{C57AB4D7-F308-46D6-8F19-069619F8CF1B}" name="treatment" dataDxfId="200">
       <calculatedColumnFormula>OFFSET(table_1[treatment], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{27DAC4C9-BDB2-4621-A4F1-0094D063284E}" name="hguide" dataDxfId="189">
+    <tableColumn id="9" xr3:uid="{27DAC4C9-BDB2-4621-A4F1-0094D063284E}" name="hguide" dataDxfId="199">
       <calculatedColumnFormula>OFFSET(table_1[hguide], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{E0E9E8C1-4E85-4EFB-8220-84140FBAAF8E}" name="output_dir" dataDxfId="188">
+    <tableColumn id="10" xr3:uid="{E0E9E8C1-4E85-4EFB-8220-84140FBAAF8E}" name="output_dir" dataDxfId="198">
       <calculatedColumnFormula>_xlfn.CONCAT(table_2_2[[#This Row],[cell]], "_", table_2_2[[#This Row],[hguide]], "_", table_2_2[[#This Row],[strand]], "_", table_2_2[[#This Row],[treatment]], "_nodsb")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{CAC474F1-3930-4766-B491-65C86C5752E8}" name="input" dataDxfId="187">
+    <tableColumn id="11" xr3:uid="{CAC474F1-3930-4766-B491-65C86C5752E8}" name="input" dataDxfId="197">
       <calculatedColumnFormula>OFFSET(table_1[file_out], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{BB84920E-3487-4670-93ED-5671EACD3061}" name="total_reads" dataDxfId="186">
+    <tableColumn id="12" xr3:uid="{BB84920E-3487-4670-93ED-5671EACD3061}" name="total_reads" dataDxfId="196">
       <calculatedColumnFormula>OFFSET(table_1[total_reads], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{0CE6DAF6-0C4C-4EC5-8FE5-9B3840A02412}" name="command" dataDxfId="185">
+    <tableColumn id="13" xr3:uid="{0CE6DAF6-0C4C-4EC5-8FE5-9B3840A02412}" name="command" dataDxfId="195">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_2[[#This Row],[input]], ".tsv ", " --total_reads ", table_2_2[[#This Row],[total_reads]], " -o ", libraries_3, "/", table_2_2[[#This Row],[output_dir]], ".tsv", " --quiet ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3107,47 +3277,47 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}" name="table_3_1" displayName="table_3_1" ref="A1:N41" totalsRowShown="0" headerRowDxfId="184">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}" name="table_3_1" displayName="table_3_1" ref="A1:N41" totalsRowShown="0" headerRowDxfId="194">
   <autoFilter ref="A1:N41" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}"/>
   <tableColumns count="14">
-    <tableColumn id="25" xr3:uid="{93D2F09B-24D5-4FE1-BF34-C037E361889F}" name="index" dataDxfId="183"/>
-    <tableColumn id="1" xr3:uid="{2F28DC66-449D-4F81-AA63-8F24B25F33D1}" name="dir" dataDxfId="182">
+    <tableColumn id="25" xr3:uid="{93D2F09B-24D5-4FE1-BF34-C037E361889F}" name="index" dataDxfId="193"/>
+    <tableColumn id="1" xr3:uid="{2F28DC66-449D-4F81-AA63-8F24B25F33D1}" name="dir" dataDxfId="192">
       <calculatedColumnFormula>OFFSET(table_2_1[output_dir], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{3DF6F698-1F9A-4B05-A310-657CCFCE9F66}" name="control" dataDxfId="181">
+    <tableColumn id="13" xr3:uid="{3DF6F698-1F9A-4B05-A310-657CCFCE9F66}" name="control" dataDxfId="191">
       <calculatedColumnFormula>OFFSET(table_2_1[control], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{362C2395-52F7-4A62-B7BA-2DD97ED5E6FB}" name="ref" dataDxfId="180">
+    <tableColumn id="2" xr3:uid="{362C2395-52F7-4A62-B7BA-2DD97ED5E6FB}" name="ref" dataDxfId="190">
       <calculatedColumnFormula>OFFSET(table_2_1[ref], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5F0895D9-2EF2-4524-8BC7-15A33FE68636}" name="dsb_pos" dataDxfId="179">
+    <tableColumn id="3" xr3:uid="{5F0895D9-2EF2-4524-8BC7-15A33FE68636}" name="dsb_pos" dataDxfId="189">
       <calculatedColumnFormula>OFFSET(table_2_1[dsb_pos], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C6D28829-46E6-4D97-8EA4-0AD12EF6CF10}" name="dsb_type" dataDxfId="178">
+    <tableColumn id="4" xr3:uid="{C6D28829-46E6-4D97-8EA4-0AD12EF6CF10}" name="dsb_type" dataDxfId="188">
       <calculatedColumnFormula>OFFSET(table_2_1[dsb_type], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{E8B2E211-C273-4602-86F0-60EA4259B7A4}" name="dsb_type_command" dataDxfId="177">
+    <tableColumn id="12" xr3:uid="{E8B2E211-C273-4602-86F0-60EA4259B7A4}" name="dsb_type_command" dataDxfId="187">
       <calculatedColumnFormula array="1">IF(table_3_1[[#This Row],[dsb_type]]="2DSB", "2", IF(table_3_1[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(table_3_1[[#This Row],[dsb_type]]="1DSB", "1", NA)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{15578E86-B7BE-4D8E-8FD4-E6C9C4F35C9C}" name="strand" dataDxfId="176">
+    <tableColumn id="5" xr3:uid="{15578E86-B7BE-4D8E-8FD4-E6C9C4F35C9C}" name="strand" dataDxfId="186">
       <calculatedColumnFormula>OFFSET(table_2_1[strand], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3366AC40-6578-4797-B607-19265E7DBF5C}" name="hguide" dataDxfId="175">
+    <tableColumn id="6" xr3:uid="{3366AC40-6578-4797-B607-19265E7DBF5C}" name="hguide" dataDxfId="185">
       <calculatedColumnFormula>MID(OFFSET(table_2_1[hguide], table_3_1[[#This Row],[index]] - 1, 0, 1, 1), 3, 100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{554F4E79-98DE-474B-A5C8-D4B536772E95}" name="cell" dataDxfId="174">
+    <tableColumn id="7" xr3:uid="{554F4E79-98DE-474B-A5C8-D4B536772E95}" name="cell" dataDxfId="184">
       <calculatedColumnFormula>OFFSET(table_2_1[cell], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{32FC5061-DD85-4234-9ED8-FEAF6D9E3BC0}" name="treatment" dataDxfId="173">
+    <tableColumn id="8" xr3:uid="{32FC5061-DD85-4234-9ED8-FEAF6D9E3BC0}" name="treatment" dataDxfId="183">
       <calculatedColumnFormula>OFFSET(table_2_1[treatment], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{DB6998A3-1431-4DDD-8DA0-525B805BF436}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{367B0912-E7A8-4430-962D-4F79EE14E5EA}" name="command_main_data" dataDxfId="172">
+    <tableColumn id="10" xr3:uid="{367B0912-E7A8-4430-962D-4F79EE14E5EA}" name="command_main_data" dataDxfId="182">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_1[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_1[[#This Row],[dir]], " -ref ref_seq/", table_3_1[[#This Row],[ref]], " -dsb ", table_3_1[[#This Row],[dsb_pos]], " --dsb_type ",table_3_1[[#This Row],[dsb_type_command]], " --strand ", table_3_1[[#This Row],[strand]], " --hguide ", table_3_1[[#This Row],[hguide]], " --cell ", table_3_1[[#This Row],[cell]], " --treatment ", table_3_1[[#This Row],[treatment]], " --subst_type ", table_3_1[[#This Row],[subst_type]], " --control ", table_3_1[[#This Row],[control]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{4A65279E-321E-4E3E-8383-26D448C2012F}" name="command_graph_data" dataDxfId="171">
+    <tableColumn id="11" xr3:uid="{4A65279E-321E-4E3E-8383-26D448C2012F}" name="command_graph_data" dataDxfId="181">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_1[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_1[[#This Row],[dir]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3156,47 +3326,47 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}" name="table_3_2" displayName="table_3_2" ref="A43:N55" totalsRowShown="0" headerRowDxfId="170">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}" name="table_3_2" displayName="table_3_2" ref="A43:N55" totalsRowShown="0" headerRowDxfId="180">
   <autoFilter ref="A43:N55" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}"/>
   <tableColumns count="14">
-    <tableColumn id="25" xr3:uid="{B2894846-EBB9-47DC-8DE1-7F1DA571A0B9}" name="index" dataDxfId="169"/>
-    <tableColumn id="1" xr3:uid="{98269DFC-71F0-4066-B063-59597431C1C3}" name="dir" dataDxfId="168">
+    <tableColumn id="25" xr3:uid="{B2894846-EBB9-47DC-8DE1-7F1DA571A0B9}" name="index" dataDxfId="179"/>
+    <tableColumn id="1" xr3:uid="{98269DFC-71F0-4066-B063-59597431C1C3}" name="dir" dataDxfId="178">
       <calculatedColumnFormula>OFFSET(table_2_2[output_dir], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{EB55B964-D8E2-4E0C-B7CF-07043E026664}" name="control" dataDxfId="167">
+    <tableColumn id="13" xr3:uid="{EB55B964-D8E2-4E0C-B7CF-07043E026664}" name="control" dataDxfId="177">
       <calculatedColumnFormula>OFFSET(table_2_2[control], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{7A83EC55-03CE-4608-92D6-6F1C53B539FE}" name="ref" dataDxfId="166">
+    <tableColumn id="2" xr3:uid="{7A83EC55-03CE-4608-92D6-6F1C53B539FE}" name="ref" dataDxfId="176">
       <calculatedColumnFormula>OFFSET(table_2_2[ref], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{13E984FC-9FD2-479F-AB4C-B74DDF5FD234}" name="dsb_pos" dataDxfId="165">
+    <tableColumn id="3" xr3:uid="{13E984FC-9FD2-479F-AB4C-B74DDF5FD234}" name="dsb_pos" dataDxfId="175">
       <calculatedColumnFormula>OFFSET(table_2_2[dsb_pos], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{EF0F2447-2FA1-4517-A5CE-D8DDAAC8D3F2}" name="dsb_type" dataDxfId="164">
+    <tableColumn id="4" xr3:uid="{EF0F2447-2FA1-4517-A5CE-D8DDAAC8D3F2}" name="dsb_type" dataDxfId="174">
       <calculatedColumnFormula>OFFSET(table_2_2[dsb_type], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A1849AE1-952B-42B5-99EE-20BD2E4C5A6A}" name="dsb_type_command" dataDxfId="163">
+    <tableColumn id="12" xr3:uid="{A1849AE1-952B-42B5-99EE-20BD2E4C5A6A}" name="dsb_type_command" dataDxfId="173">
       <calculatedColumnFormula array="1">IF(table_3_2[[#This Row],[dsb_type]]="2DSB", "2", IF(table_3_2[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(table_3_2[[#This Row],[dsb_type]]="1DSB", "1", NA)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{625E12FC-BF17-4E65-99DB-EDD53FEF055D}" name="strand" dataDxfId="162">
+    <tableColumn id="5" xr3:uid="{625E12FC-BF17-4E65-99DB-EDD53FEF055D}" name="strand" dataDxfId="172">
       <calculatedColumnFormula>OFFSET(table_2_2[strand], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0ABF747E-328F-4A80-85AA-4AF871C860C1}" name="hguide" dataDxfId="161">
+    <tableColumn id="6" xr3:uid="{0ABF747E-328F-4A80-85AA-4AF871C860C1}" name="hguide" dataDxfId="171">
       <calculatedColumnFormula>MID(OFFSET(table_2_2[hguide], table_3_2[[#This Row],[index]] - 1, 0, 1, 1), 3, 100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{29D6C48B-05B8-42C6-88A9-0939BC454FE0}" name="cell" dataDxfId="160">
+    <tableColumn id="7" xr3:uid="{29D6C48B-05B8-42C6-88A9-0939BC454FE0}" name="cell" dataDxfId="170">
       <calculatedColumnFormula>OFFSET(table_2_2[cell], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{BD269EBE-94A9-4B57-B984-C7566AC259DE}" name="treatment" dataDxfId="159">
+    <tableColumn id="8" xr3:uid="{BD269EBE-94A9-4B57-B984-C7566AC259DE}" name="treatment" dataDxfId="169">
       <calculatedColumnFormula>OFFSET(table_2_2[treatment], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{142C480D-E258-4979-A008-3940A3FE78E4}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{19804410-83AB-479E-A819-2D7449105C25}" name="command_main_data" dataDxfId="158">
+    <tableColumn id="10" xr3:uid="{19804410-83AB-479E-A819-2D7449105C25}" name="command_main_data" dataDxfId="168">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_2[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_2[[#This Row],[dir]], " -ref ref_seq/", table_3_2[[#This Row],[ref]], " -dsb ", table_3_2[[#This Row],[dsb_pos]], " --dsb_type ",table_3_2[[#This Row],[dsb_type_command]], " --strand ", table_3_2[[#This Row],[strand]], " --hguide ", table_3_2[[#This Row],[hguide]], " --cell ", table_3_2[[#This Row],[cell]], " --treatment ", table_3_2[[#This Row],[treatment]], " --subst_type ", table_3_2[[#This Row],[subst_type]], " --control ", table_3_2[[#This Row],[control]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{212A69BD-0F88-401C-957F-8B6EC8E55AED}" name="command_graph_data" dataDxfId="157">
+    <tableColumn id="11" xr3:uid="{212A69BD-0F88-401C-957F-8B6EC8E55AED}" name="command_graph_data" dataDxfId="167">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_2[[#This Row],[dir]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3205,38 +3375,38 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}" name="table_4_1" displayName="table_4_1" ref="A1:K17" totalsRowShown="0" headerRowDxfId="156">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}" name="table_4_1" displayName="table_4_1" ref="A1:K17" totalsRowShown="0" headerRowDxfId="166">
   <autoFilter ref="A1:K17" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B7EC223D-BA24-48F1-9EE3-DC56DEFDE4C2}" name="index" dataDxfId="155"/>
-    <tableColumn id="7" xr3:uid="{D9F1ADDA-18A2-4F81-862D-6B0F786079FF}" name="control" dataDxfId="154">
+    <tableColumn id="1" xr3:uid="{B7EC223D-BA24-48F1-9EE3-DC56DEFDE4C2}" name="index" dataDxfId="165"/>
+    <tableColumn id="7" xr3:uid="{D9F1ADDA-18A2-4F81-862D-6B0F786079FF}" name="control" dataDxfId="164">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{0EA5A81F-6EA1-4256-9717-03273165F7BF}" name="treatment_1" dataDxfId="153">
+    <tableColumn id="8" xr3:uid="{0EA5A81F-6EA1-4256-9717-03273165F7BF}" name="treatment_1" dataDxfId="163">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5F6D005A-96D8-4801-93E2-101BAE551BA8}" name="dir_1" dataDxfId="152">
+    <tableColumn id="2" xr3:uid="{5F6D005A-96D8-4801-93E2-101BAE551BA8}" name="dir_1" dataDxfId="162">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C21D1AF7-7ABE-4181-AA2A-42227869A8DD}" name="treatment_2" dataDxfId="151">
+    <tableColumn id="9" xr3:uid="{C21D1AF7-7ABE-4181-AA2A-42227869A8DD}" name="treatment_2" dataDxfId="161">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{D66426AC-E0B2-4B07-A4D4-5A74AA033E80}" name="dir_2" dataDxfId="150">
+    <tableColumn id="3" xr3:uid="{D66426AC-E0B2-4B07-A4D4-5A74AA033E80}" name="dir_2" dataDxfId="160">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{0C8146A0-DC77-4DC4-82FF-74F4C74CF33E}" name="treatments_out" dataDxfId="149">
+    <tableColumn id="10" xr3:uid="{0C8146A0-DC77-4DC4-82FF-74F4C74CF33E}" name="treatments_out" dataDxfId="159">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_1[[#This Row],[treatment_1]], "_", table_4_1[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{519A6397-7A3C-4009-B8B9-A71C0B3A591B}" name="dir_out" dataDxfId="148">
+    <tableColumn id="4" xr3:uid="{519A6397-7A3C-4009-B8B9-A71C0B3A591B}" name="dir_out" dataDxfId="158">
       <calculatedColumnFormula>SUBSTITUTE(table_4_1[[#This Row],[dir_1]], table_4_1[[#This Row],[treatment_1]], table_4_1[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E1629355-7D02-4819-98A1-EEB3B5FADE18}" name="subst_type" dataDxfId="147">
+    <tableColumn id="5" xr3:uid="{E1629355-7D02-4819-98A1-EEB3B5FADE18}" name="subst_type" dataDxfId="157">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{BC9117A0-CB6F-4D3C-A0E4-BF8395854D9A}" name="command_main_data_combined" dataDxfId="146">
+    <tableColumn id="6" xr3:uid="{BC9117A0-CB6F-4D3C-A0E4-BF8395854D9A}" name="command_main_data_combined" dataDxfId="156">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_1[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_1[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_1[[#This Row],[dir_out]], " --subst_type ", table_4_1[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{D384013E-9937-4DD8-A36A-43325757359B}" name="command_graph_data" dataDxfId="145">
+    <tableColumn id="11" xr3:uid="{D384013E-9937-4DD8-A36A-43325757359B}" name="command_graph_data" dataDxfId="155">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_1[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_1[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3245,38 +3415,38 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}" name="table_4_2" displayName="table_4_2" ref="A20:K22" totalsRowShown="0" headerRowDxfId="144">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}" name="table_4_2" displayName="table_4_2" ref="A20:K22" totalsRowShown="0" headerRowDxfId="154">
   <autoFilter ref="A20:K22" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{7F5A3A15-751D-407C-A035-61B2605E693F}" name="index" dataDxfId="143"/>
-    <tableColumn id="7" xr3:uid="{45863AB0-FD32-49FE-B4BF-F8EE865F7604}" name="control" dataDxfId="142">
+    <tableColumn id="1" xr3:uid="{7F5A3A15-751D-407C-A035-61B2605E693F}" name="index" dataDxfId="153"/>
+    <tableColumn id="7" xr3:uid="{45863AB0-FD32-49FE-B4BF-F8EE865F7604}" name="control" dataDxfId="152">
       <calculatedColumnFormula>OFFSET(table_3_1[control], var_4_anti_offset + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{CD16648D-267E-410B-A366-3E12367C037C}" name="treatment_1" dataDxfId="141">
+    <tableColumn id="8" xr3:uid="{CD16648D-267E-410B-A366-3E12367C037C}" name="treatment_1" dataDxfId="151">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{10C9F90E-86FD-4BFE-939E-298FD6F69F12}" name="dir_1" dataDxfId="140">
+    <tableColumn id="2" xr3:uid="{10C9F90E-86FD-4BFE-939E-298FD6F69F12}" name="dir_1" dataDxfId="150">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{7AB3E4AB-F43B-4FDE-96D7-FBBB4A8B83BE}" name="treatment_2" dataDxfId="139">
+    <tableColumn id="9" xr3:uid="{7AB3E4AB-F43B-4FDE-96D7-FBBB4A8B83BE}" name="treatment_2" dataDxfId="149">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1) + 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BF948A3E-9649-41BF-A7E7-57BFDE810FE9}" name="dir_2" dataDxfId="138">
+    <tableColumn id="3" xr3:uid="{BF948A3E-9649-41BF-A7E7-57BFDE810FE9}" name="dir_2" dataDxfId="148">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1) + 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{378119E5-F021-4785-A653-4D632F029AA6}" name="treatments_out" dataDxfId="137">
+    <tableColumn id="10" xr3:uid="{378119E5-F021-4785-A653-4D632F029AA6}" name="treatments_out" dataDxfId="147">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_2[[#This Row],[treatment_1]], "_", table_4_2[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AE1A14DC-D0C9-4818-B8CC-09A571E73BC2}" name="dir_out" dataDxfId="136">
+    <tableColumn id="4" xr3:uid="{AE1A14DC-D0C9-4818-B8CC-09A571E73BC2}" name="dir_out" dataDxfId="146">
       <calculatedColumnFormula>SUBSTITUTE(table_4_2[[#This Row],[dir_1]], table_4_2[[#This Row],[treatment_1]], table_4_2[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{F29DAC4E-FEC5-4C1D-AAC1-7CE19E401F25}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{DC4E99F4-97AB-4553-A5FB-D20D3D487947}" name="command_main_data_combined" dataDxfId="135">
+    <tableColumn id="6" xr3:uid="{DC4E99F4-97AB-4553-A5FB-D20D3D487947}" name="command_main_data_combined" dataDxfId="145">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_2[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_2[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_2[[#This Row],[dir_out]], " --subst_type ", table_4_2[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{E19D3001-2E76-4CC2-BF33-D0465C77D538}" name="command_graph_data" dataDxfId="134">
+    <tableColumn id="11" xr3:uid="{E19D3001-2E76-4CC2-BF33-D0465C77D538}" name="command_graph_data" dataDxfId="144">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_2[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3285,38 +3455,38 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}" name="table_4_3" displayName="table_4_3" ref="A25:K33" totalsRowShown="0" headerRowDxfId="133">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}" name="table_4_3" displayName="table_4_3" ref="A25:K33" totalsRowShown="0" headerRowDxfId="143">
   <autoFilter ref="A25:K33" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{33AF3495-7432-4F03-9832-525A370EADEC}" name="index" dataDxfId="132"/>
-    <tableColumn id="7" xr3:uid="{3D66515C-5022-4D48-A834-4320DA4E73F6}" name="control" dataDxfId="131">
+    <tableColumn id="1" xr3:uid="{33AF3495-7432-4F03-9832-525A370EADEC}" name="index" dataDxfId="142"/>
+    <tableColumn id="7" xr3:uid="{3D66515C-5022-4D48-A834-4320DA4E73F6}" name="control" dataDxfId="141">
       <calculatedColumnFormula>OFFSET(table_3_2[control], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{294B17A9-F0F9-42CA-8342-55C00648E3A5}" name="treatment_1" dataDxfId="130">
+    <tableColumn id="8" xr3:uid="{294B17A9-F0F9-42CA-8342-55C00648E3A5}" name="treatment_1" dataDxfId="140">
       <calculatedColumnFormula>OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E13C38CF-C105-4AB5-8602-7D32E688C737}" name="dir_1" dataDxfId="129">
+    <tableColumn id="2" xr3:uid="{E13C38CF-C105-4AB5-8602-7D32E688C737}" name="dir_1" dataDxfId="139">
       <calculatedColumnFormula>OFFSET(table_3_2[dir], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{15B3CC7F-2A3C-4026-8417-A9DD21E4F004}" name="treatment_2" dataDxfId="128">
+    <tableColumn id="9" xr3:uid="{15B3CC7F-2A3C-4026-8417-A9DD21E4F004}" name="treatment_2" dataDxfId="138">
       <calculatedColumnFormula>OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{FF7D9AD3-1A35-4013-88AE-0C00465033CD}" name="dir_2" dataDxfId="127">
+    <tableColumn id="3" xr3:uid="{FF7D9AD3-1A35-4013-88AE-0C00465033CD}" name="dir_2" dataDxfId="137">
       <calculatedColumnFormula>OFFSET(table_3_2[dir], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{9353B2D3-0D23-4FBB-AFEC-EB68549160F4}" name="treatments_out" dataDxfId="126">
+    <tableColumn id="10" xr3:uid="{9353B2D3-0D23-4FBB-AFEC-EB68549160F4}" name="treatments_out" dataDxfId="136">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_3[[#This Row],[treatment_1]], "_", table_4_3[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{77F1D6F0-DE95-4E63-9E7E-D3CA3CF85F37}" name="dir_out" dataDxfId="125">
+    <tableColumn id="4" xr3:uid="{77F1D6F0-DE95-4E63-9E7E-D3CA3CF85F37}" name="dir_out" dataDxfId="135">
       <calculatedColumnFormula>SUBSTITUTE(table_4_3[[#This Row],[dir_1]], table_4_3[[#This Row],[treatment_1]], table_4_3[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{BBF4F840-178E-461E-8C17-36D699EDE038}" name="subst_type" dataDxfId="124">
+    <tableColumn id="5" xr3:uid="{BBF4F840-178E-461E-8C17-36D699EDE038}" name="subst_type" dataDxfId="134">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9434BF8B-81C5-43DF-BCB7-FA7146BF2FE8}" name="command_main_data_combined" dataDxfId="123">
+    <tableColumn id="6" xr3:uid="{9434BF8B-81C5-43DF-BCB7-FA7146BF2FE8}" name="command_main_data_combined" dataDxfId="133">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_3[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_3[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_3[[#This Row],[dir_out]], " --subst_type ", table_4_3[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{1ABF0B7B-4ECE-42BF-A7D8-EA13E98144EE}" name="command_graph_data" dataDxfId="122">
+    <tableColumn id="11" xr3:uid="{1ABF0B7B-4ECE-42BF-A7D8-EA13E98144EE}" name="command_graph_data" dataDxfId="132">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_3[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_3[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -26263,10 +26433,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1417E7-0E2A-4E67-94B4-4030BF5F7C23}">
-  <dimension ref="A1:V24"/>
+  <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26854,7 +27024,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -26900,27 +27070,27 @@
         <v>1</v>
       </c>
       <c r="B12" s="13" t="str" cm="1">
-        <f t="array" aca="1" ref="B12" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset - 1 + COLUMN() - 2 + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1))</f>
+        <f t="array" aca="1" ref="B12" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset  + COLUMN() - 2 + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1))</f>
         <v>libraries_4/WT_sgCD_R1_antisense</v>
       </c>
       <c r="C12" s="13" t="str" cm="1">
-        <f t="array" aca="1" ref="C12" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset - 1 + COLUMN() - 2 + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1))</f>
+        <f t="array" aca="1" ref="C12" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset + COLUMN() - 2 + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1))</f>
         <v>libraries_4/WT_sgCD_R1_splicing</v>
       </c>
       <c r="D12" s="13" t="str">
-        <f ca="1">OFFSET(table_3_1[control], var_6_anti_offset - 1 + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</f>
+        <f ca="1">OFFSET(table_3_1[control], var_6_anti_offset  + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</f>
         <v>none</v>
       </c>
       <c r="E12" s="13" t="str">
-        <f ca="1">OFFSET(table_3_1[dsb_type], var_6_anti_offset - 1 + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</f>
+        <f ca="1">OFFSET(table_3_1[dsb_type], var_6_anti_offset  + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</f>
         <v>2DSBanti</v>
       </c>
       <c r="F12" s="13" t="str" cm="1">
-        <f t="array" aca="1" ref="F12" ca="1">OFFSET(table_3_1[strand], var_6_anti_offset - 1 + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1)</f>
+        <f t="array" aca="1" ref="F12" ca="1">OFFSET(table_3_1[strand], var_6_anti_offset  + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1)</f>
         <v>R1</v>
       </c>
       <c r="G12" s="13" t="str">
-        <f ca="1">OFFSET(table_3_1[hguide], var_6_anti_offset - 1 + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</f>
+        <f ca="1">OFFSET(table_3_1[hguide], var_6_anti_offset + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</f>
         <v>CD</v>
       </c>
       <c r="H12" s="14" t="str">
@@ -26941,27 +27111,27 @@
         <v>2</v>
       </c>
       <c r="B13" s="13" t="str" cm="1">
-        <f t="array" aca="1" ref="B13" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset - 1 + COLUMN() - 2 + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1))</f>
+        <f t="array" aca="1" ref="B13" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset  + COLUMN() - 2 + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1))</f>
         <v>libraries_4/WT_sgCD_R2_antisense</v>
       </c>
       <c r="C13" s="13" t="str" cm="1">
-        <f t="array" aca="1" ref="C13" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset - 1 + COLUMN() - 2 + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1))</f>
+        <f t="array" aca="1" ref="C13" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset + COLUMN() - 2 + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1))</f>
         <v>libraries_4/WT_sgCD_R2_splicing</v>
       </c>
       <c r="D13" s="16" t="str">
-        <f ca="1">OFFSET(table_3_1[control], var_6_anti_offset - 1 + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</f>
+        <f ca="1">OFFSET(table_3_1[control], var_6_anti_offset  + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</f>
         <v>none</v>
       </c>
       <c r="E13" s="16" t="str">
-        <f ca="1">OFFSET(table_3_1[dsb_type], var_6_anti_offset - 1 + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</f>
+        <f ca="1">OFFSET(table_3_1[dsb_type], var_6_anti_offset  + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</f>
         <v>2DSBanti</v>
       </c>
       <c r="F13" s="16" t="str" cm="1">
-        <f t="array" aca="1" ref="F13" ca="1">OFFSET(table_3_1[strand], var_6_anti_offset - 1 + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1)</f>
+        <f t="array" aca="1" ref="F13" ca="1">OFFSET(table_3_1[strand], var_6_anti_offset  + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1)</f>
         <v>R2</v>
       </c>
       <c r="G13" s="16" t="str">
-        <f ca="1">OFFSET(table_3_1[hguide], var_6_anti_offset - 1 + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</f>
+        <f ca="1">OFFSET(table_3_1[hguide], var_6_anti_offset + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</f>
         <v>CD</v>
       </c>
       <c r="H13" s="16" t="str">
@@ -26994,12 +27164,15 @@
         <v>102</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>171</v>
       </c>
     </row>
@@ -27012,8 +27185,8 @@
         <v>libraries_4/WT_sgAB_R1_sense libraries_4/WT_sgAB_R1_branch libraries_4/WT_sgAB_R1_cmv libraries_4/KO_sgAB_R1_sense libraries_4/KO_sgAB_R1_branch libraries_4/KO_sgAB_R1_cmv libraries_4/WT_sgAB_R2_sense libraries_4/WT_sgAB_R2_branch libraries_4/WT_sgAB_R2_cmv libraries_4/KO_sgAB_R2_sense libraries_4/KO_sgAB_R2_branch libraries_4/KO_sgAB_R2_cmv</v>
       </c>
       <c r="C16" s="6" t="str" cm="1">
-        <f t="array" aca="1" ref="C16" ca="1">_xlfn.TEXTJOIN(" ", TRUE, IF(OFFSET(table_3_1[[strand]:[strand]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_3[dir]) - COLUMN(table_6_3[[dir]:[dir]]), 0, 12, 1) = "R1", "+", "-"))</f>
-        <v>+ + + + + + - - - - - -</v>
+        <f t="array" aca="1" ref="C16" ca="1">_xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[strand]:[strand]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 12, 1))</f>
+        <v>R1 R1 R1 R1 R1 R1 R2 R2 R2 R2 R2 R2</v>
       </c>
       <c r="D16" t="str">
         <f ca="1">OFFSET(table_3_1[control], 6 * (table_6_3[[#This Row],[index]] - 1), 0, 1, 1)</f>
@@ -27023,184 +27196,279 @@
         <f ca="1">OFFSET(table_3_1[dsb_type], 12 * (table_6_3[[#This Row],[index]] - 1), 0, 1, 1)</f>
         <v>2DSB</v>
       </c>
-      <c r="F16" t="str">
-        <f t="shared" ref="F16:F17" si="1">subst_type</f>
+      <c r="F16" t="str" cm="1">
+        <f t="array" aca="1" ref="F16" ca="1">OFFSET(table_3_1[[hguide]:[hguide]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 1, 1)</f>
+        <v>AB</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" ref="G16:G21" si="1">subst_type</f>
         <v>without</v>
       </c>
-      <c r="G16" t="str">
-        <f ca="1">_xlfn.CONCAT(table_6_3[[#This Row],[dsb_type]], IF(table_6_3[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_3[[#This Row],[control]]), ""))</f>
-        <v>2DSB</v>
-      </c>
       <c r="H16" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_3[[#This Row],[dir]], " -s ", table_6_3[[#This Row],[strand]], " -o ", layouts, "/", table_6_3[[#This Row],[dir_out]], " --subst_type ", table_6_3[[#This Row],[subst_type]], " --layout ", var_6_layout)</f>
-        <v>python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgAB_R1_sense libraries_4/WT_sgAB_R1_branch libraries_4/WT_sgAB_R1_cmv libraries_4/KO_sgAB_R1_sense libraries_4/KO_sgAB_R1_branch libraries_4/KO_sgAB_R1_cmv libraries_4/WT_sgAB_R2_sense libraries_4/WT_sgAB_R2_branch libraries_4/WT_sgAB_R2_cmv libraries_4/KO_sgAB_R2_sense libraries_4/KO_sgAB_R2_branch libraries_4/KO_sgAB_R2_cmv -s + + + + + + - - - - - - -o layouts/2DSB --subst_type without --layout radial</v>
+        <f ca="1">_xlfn.CONCAT(table_6_3[[#This Row],[dsb_type]], "_", table_6_3[[#This Row],[hguide]], IF(table_6_3[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_3[[#This Row],[control]]), ""))</f>
+        <v>2DSB_AB</v>
+      </c>
+      <c r="I16" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_3[[#This Row],[dir]], IF(NOT(ISNA(table_6_3[[#This Row],[strand]])), _xlfn.CONCAT(" -s ", table_6_3[[#This Row],[strand]]), ""), " -o ", layouts, "/", table_6_3[[#This Row],[dir_out]], " --subst_type ", table_6_3[[#This Row],[subst_type]], " --layout ", var_6_layout)</f>
+        <v>python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgAB_R1_sense libraries_4/WT_sgAB_R1_branch libraries_4/WT_sgAB_R1_cmv libraries_4/KO_sgAB_R1_sense libraries_4/KO_sgAB_R1_branch libraries_4/KO_sgAB_R1_cmv libraries_4/WT_sgAB_R2_sense libraries_4/WT_sgAB_R2_branch libraries_4/WT_sgAB_R2_cmv libraries_4/KO_sgAB_R2_sense libraries_4/KO_sgAB_R2_branch libraries_4/KO_sgAB_R2_cmv -s R1 R1 R1 R1 R1 R1 R2 R2 R2 R2 R2 R2 -o layouts/2DSB_AB --subst_type without --layout radial</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>2</v>
-      </c>
-      <c r="B17" s="6" t="str" cm="1">
-        <f t="array" aca="1" ref="B17" ca="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 12, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</f>
-        <v>libraries_4/WT_sgA_R1_sense libraries_4/WT_sgA_R1_branch libraries_4/WT_sgA_R1_cmv libraries_4/KO_sgA_R1_sense libraries_4/KO_sgA_R1_branch libraries_4/KO_sgA_R1_cmv libraries_4/WT_sgB_R2_sense libraries_4/WT_sgB_R2_branch libraries_4/WT_sgB_R2_cmv libraries_4/KO_sgB_R2_sense libraries_4/KO_sgB_R2_branch libraries_4/KO_sgB_R2_cmv</v>
-      </c>
-      <c r="C17" s="6" t="str" cm="1">
-        <f t="array" aca="1" ref="C17" ca="1">_xlfn.TEXTJOIN(" ", TRUE, IF(OFFSET(table_3_1[[strand]:[strand]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_3[dir]) - COLUMN(table_6_3[[dir]:[dir]]), 0, 12, 1) = "R1", "+", "-"))</f>
-        <v>+ + + + + + - - - - - -</v>
-      </c>
-      <c r="D17" t="str">
-        <f ca="1">OFFSET(table_3_1[control], 6 * (table_6_3[[#This Row],[index]] - 1), 0, 1, 1)</f>
+      <c r="A17" s="3"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>12</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>1</v>
+      </c>
+      <c r="B20" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="B20" ca="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 6, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</f>
+        <v>libraries_4/WT_sgA_R1_sense libraries_4/WT_sgA_R1_branch libraries_4/WT_sgA_R1_cmv libraries_4/KO_sgA_R1_sense libraries_4/KO_sgA_R1_branch libraries_4/KO_sgA_R1_cmv</v>
+      </c>
+      <c r="C20" s="6" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D20" t="str">
+        <f ca="1">OFFSET(table_3_1[control], 6 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</f>
         <v>none</v>
       </c>
-      <c r="E17" t="str">
-        <f ca="1">OFFSET(table_3_1[dsb_type], 12 * (table_6_3[[#This Row],[index]] - 1), 0, 1, 1)</f>
+      <c r="E20" t="str">
+        <f ca="1">OFFSET(table_3_1[dsb_type], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</f>
         <v>1DSB</v>
       </c>
-      <c r="F17" t="str">
+      <c r="F20" t="str" cm="1">
+        <f t="array" aca="1" ref="F20" ca="1">OFFSET(table_3_1[[hguide]:[hguide]], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 1, 1)</f>
+        <v>A</v>
+      </c>
+      <c r="G20" t="str">
         <f t="shared" si="1"/>
         <v>without</v>
       </c>
-      <c r="G17" t="str">
-        <f ca="1">_xlfn.CONCAT(table_6_3[[#This Row],[dsb_type]], IF(table_6_3[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_3[[#This Row],[control]]), ""))</f>
+      <c r="H20" t="str">
+        <f ca="1">_xlfn.CONCAT(table_6_4[[#This Row],[dsb_type]], "_", table_6_4[[#This Row],[hguide]], IF(table_6_4[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_4[[#This Row],[control]]), ""))</f>
+        <v>1DSB_A</v>
+      </c>
+      <c r="I20" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_4[[#This Row],[dir]], IF(NOT(ISNA(table_6_4[[#This Row],[strand]])), _xlfn.CONCAT(" -s ", table_6_4[[#This Row],[strand]]), ""), " -o ", layouts, "/", table_6_4[[#This Row],[dir_out]], " --subst_type ", table_6_4[[#This Row],[subst_type]], " --layout ", var_6_layout)</f>
+        <v>python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgA_R1_sense libraries_4/WT_sgA_R1_branch libraries_4/WT_sgA_R1_cmv libraries_4/KO_sgA_R1_sense libraries_4/KO_sgA_R1_branch libraries_4/KO_sgA_R1_cmv -o layouts/1DSB_A --subst_type without --layout radial</v>
+      </c>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>2</v>
+      </c>
+      <c r="B21" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="B21" ca="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 6, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</f>
+        <v>libraries_4/WT_sgB_R2_sense libraries_4/WT_sgB_R2_branch libraries_4/WT_sgB_R2_cmv libraries_4/KO_sgB_R2_sense libraries_4/KO_sgB_R2_branch libraries_4/KO_sgB_R2_cmv</v>
+      </c>
+      <c r="C21" s="6" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D21" t="str">
+        <f ca="1">OFFSET(table_3_1[control], 6 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</f>
+        <v>none</v>
+      </c>
+      <c r="E21" t="str">
+        <f ca="1">OFFSET(table_3_1[dsb_type], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</f>
         <v>1DSB</v>
       </c>
-      <c r="H17" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_3[[#This Row],[dir]], " -s ", table_6_3[[#This Row],[strand]], " -o ", layouts, "/", table_6_3[[#This Row],[dir_out]], " --subst_type ", table_6_3[[#This Row],[subst_type]], " --layout ", var_6_layout)</f>
-        <v>python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgA_R1_sense libraries_4/WT_sgA_R1_branch libraries_4/WT_sgA_R1_cmv libraries_4/KO_sgA_R1_sense libraries_4/KO_sgA_R1_branch libraries_4/KO_sgA_R1_cmv libraries_4/WT_sgB_R2_sense libraries_4/WT_sgB_R2_branch libraries_4/WT_sgB_R2_cmv libraries_4/KO_sgB_R2_sense libraries_4/KO_sgB_R2_branch libraries_4/KO_sgB_R2_cmv -s + + + + + + - - - - - - -o layouts/1DSB --subst_type without --layout radial</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="F21" t="str" cm="1">
+        <f t="array" aca="1" ref="F21" ca="1">OFFSET(table_3_1[[hguide]:[hguide]], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 1, 1)</f>
+        <v>B</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="1"/>
+        <v>without</v>
+      </c>
+      <c r="H21" t="str">
+        <f ca="1">_xlfn.CONCAT(table_6_4[[#This Row],[dsb_type]], "_", table_6_4[[#This Row],[hguide]], IF(table_6_4[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_4[[#This Row],[control]]), ""))</f>
+        <v>1DSB_B</v>
+      </c>
+      <c r="I21" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_4[[#This Row],[dir]], IF(NOT(ISNA(table_6_4[[#This Row],[strand]])), _xlfn.CONCAT(" -s ", table_6_4[[#This Row],[strand]]), ""), " -o ", layouts, "/", table_6_4[[#This Row],[dir_out]], " --subst_type ", table_6_4[[#This Row],[subst_type]], " --layout ", var_6_layout)</f>
+        <v>python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgB_R2_sense libraries_4/WT_sgB_R2_branch libraries_4/WT_sgB_R2_cmv libraries_4/KO_sgB_R2_sense libraries_4/KO_sgB_R2_branch libraries_4/KO_sgB_R2_cmv -o layouts/1DSB_B --subst_type without --layout radial</v>
+      </c>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="V22" t="str" cm="1">
+        <f t="array" aca="1" ref="V22" ca="1">IF(C16:C16 = "R1", "+", "-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="C19" s="8" t="s">
+      <c r="B23" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D23" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E23" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F23" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G23" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="H23" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="I23" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
         <v>1</v>
       </c>
-      <c r="B20" s="6" t="str" cm="1">
-        <f t="array" aca="1" ref="B20" ca="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset - 1 + 4 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 4, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</f>
+      <c r="B24" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="B24" ca="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]:[index]] - 1), 0, 4, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</f>
         <v>libraries_4/WT_sgCD_R1_antisense libraries_4/WT_sgCD_R1_splicing libraries_4/WT_sgCD_R2_antisense libraries_4/WT_sgCD_R2_splicing</v>
       </c>
-      <c r="C20" s="6" t="str" cm="1">
-        <f t="array" aca="1" ref="C20" ca="1">_xlfn.TEXTJOIN(" ", TRUE, IF(OFFSET(table_3_1[[strand]:[strand]], var_6_anti_offset - 1 + 4 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 4, 1) = "R1", "+", "-"))</f>
-        <v>+ + - -</v>
-      </c>
-      <c r="D20" s="6" t="str">
-        <f ca="1">OFFSET(table_3_1[control], var_6_anti_offset - 1 + 4 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</f>
+      <c r="C24" s="6" t="str" cm="1">
+        <f t="array" aca="1" ref="C24" ca="1">_xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[strand]:[strand]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]:[index]] - 1), 0, 4, 1))</f>
+        <v>R1 R1 R2 R2</v>
+      </c>
+      <c r="D24" s="6" t="str">
+        <f ca="1">OFFSET(table_3_1[control], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</f>
         <v>none</v>
       </c>
-      <c r="E20" s="6" t="str">
-        <f ca="1">OFFSET(table_3_1[dsb_type], var_6_anti_offset - 1 + 4 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</f>
+      <c r="E24" s="6" t="str">
+        <f ca="1">OFFSET(table_3_1[dsb_type], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</f>
         <v>2DSBanti</v>
       </c>
-      <c r="F20" s="4" t="str">
+      <c r="F24" s="4" t="str">
         <f>subst_type</f>
         <v>without</v>
       </c>
-      <c r="G20" s="4" t="str">
-        <f ca="1">_xlfn.CONCAT(table_6_4[[#This Row],[dsb_type]], IF(table_6_4[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_4[[#This Row],[control]]), ""))</f>
-        <v>2DSBanti</v>
-      </c>
-      <c r="H20" s="4" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_4[[#This Row],[dir_1]], " - ", table_6_4[[#This Row],[strand]], " -o ", layouts, "/", table_6_4[[#This Row],[dir_out]], " --subst_type ", table_6_4[[#This Row],[subst_type]], " --layout ", var_6_layout)</f>
-        <v>python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgCD_R1_antisense libraries_4/WT_sgCD_R1_splicing libraries_4/WT_sgCD_R2_antisense libraries_4/WT_sgCD_R2_splicing - + + - - -o layouts/2DSBanti --subst_type without --layout radial</v>
-      </c>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="V21" t="str" cm="1">
-        <f t="array" aca="1" ref="V21" ca="1">IF(C16:C16 = "R1", "+", "-")</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="G24" s="4" t="str">
+        <f ca="1">OFFSET(table_3_1[[hguide]:[hguide]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</f>
+        <v>CD</v>
+      </c>
+      <c r="H24" s="4" t="str">
+        <f ca="1">_xlfn.CONCAT(table_6_5[[#This Row],[dsb_type]], "_", table_6_5[[#This Row],[hguide]], IF(table_6_5[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_5[[#This Row],[control]]), ""))</f>
+        <v>2DSBanti_CD</v>
+      </c>
+      <c r="I24" s="4" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_5[[#This Row],[dir]], " -s ", table_6_5[[#This Row],[strand]], " -o ", layouts, "/", table_6_5[[#This Row],[dir_out]], " --subst_type ", table_6_5[[#This Row],[subst_type]], " --layout ", var_6_layout)</f>
+        <v>python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgCD_R1_antisense libraries_4/WT_sgCD_R1_splicing libraries_4/WT_sgCD_R2_antisense libraries_4/WT_sgCD_R2_splicing -s R1 R1 R2 R2 -o layouts/2DSBanti_CD --subst_type without --layout radial</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="str">
-        <f ca="1">_xlfn.TEXTJOIN(CHAR(10), TRUE, B16:B17,B20)</f>
-        <v>libraries_4/WT_sgAB_R1_sense libraries_4/WT_sgAB_R1_branch libraries_4/WT_sgAB_R1_cmv libraries_4/KO_sgAB_R1_sense libraries_4/KO_sgAB_R1_branch libraries_4/KO_sgAB_R1_cmv libraries_4/WT_sgAB_R2_sense libraries_4/WT_sgAB_R2_branch libraries_4/WT_sgAB_R2_cmv libraries_4/KO_sgAB_R2_sense libraries_4/KO_sgAB_R2_branch libraries_4/KO_sgAB_R2_cmv
-libraries_4/WT_sgA_R1_sense libraries_4/WT_sgA_R1_branch libraries_4/WT_sgA_R1_cmv libraries_4/KO_sgA_R1_sense libraries_4/KO_sgA_R1_branch libraries_4/KO_sgA_R1_cmv libraries_4/WT_sgB_R2_sense libraries_4/WT_sgB_R2_branch libraries_4/WT_sgB_R2_cmv libraries_4/KO_sgB_R2_sense libraries_4/KO_sgB_R2_branch libraries_4/KO_sgB_R2_cmv
-libraries_4/WT_sgCD_R1_antisense libraries_4/WT_sgCD_R1_splicing libraries_4/WT_sgCD_R2_antisense libraries_4/WT_sgCD_R2_splicing</v>
-      </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="str">
+        <f ca="1">_xlfn.TEXTJOIN(CHAR(10), TRUE, table_6_3[command], table_6_4[command], table_6_5[command])</f>
+        <v>python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgAB_R1_sense libraries_4/WT_sgAB_R1_branch libraries_4/WT_sgAB_R1_cmv libraries_4/KO_sgAB_R1_sense libraries_4/KO_sgAB_R1_branch libraries_4/KO_sgAB_R1_cmv libraries_4/WT_sgAB_R2_sense libraries_4/WT_sgAB_R2_branch libraries_4/WT_sgAB_R2_cmv libraries_4/KO_sgAB_R2_sense libraries_4/KO_sgAB_R2_branch libraries_4/KO_sgAB_R2_cmv -s R1 R1 R1 R1 R1 R1 R2 R2 R2 R2 R2 R2 -o layouts/2DSB_AB --subst_type without --layout radial
+python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgA_R1_sense libraries_4/WT_sgA_R1_branch libraries_4/WT_sgA_R1_cmv libraries_4/KO_sgA_R1_sense libraries_4/KO_sgA_R1_branch libraries_4/KO_sgA_R1_cmv -o layouts/1DSB_A --subst_type without --layout radial
+python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgB_R2_sense libraries_4/WT_sgB_R2_branch libraries_4/WT_sgB_R2_cmv libraries_4/KO_sgB_R2_sense libraries_4/KO_sgB_R2_branch libraries_4/KO_sgB_R2_cmv -o layouts/1DSB_B --subst_type without --layout radial
+python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgCD_R1_antisense libraries_4/WT_sgCD_R1_splicing libraries_4/WT_sgCD_R2_antisense libraries_4/WT_sgCD_R2_splicing -s R1 R1 R2 R2 -o layouts/2DSBanti_CD --subst_type without --layout radial</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="4">
+  <tableParts count="5">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
@@ -27209,8 +27477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1375107-D76A-4386-B771-6693BBF75061}">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27346,7 +27614,7 @@
         <v>2DSB_R1</v>
       </c>
       <c r="N3" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_R1 -ext png --layout radial</v>
       </c>
     </row>
@@ -27403,7 +27671,7 @@
         <v>2DSB_R1</v>
       </c>
       <c r="N4" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_R1 -ext png --layout radial</v>
       </c>
     </row>
@@ -27460,7 +27728,7 @@
         <v>2DSB_R1</v>
       </c>
       <c r="N5" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_R1 -ext png --layout radial</v>
       </c>
     </row>
@@ -27517,7 +27785,7 @@
         <v>2DSB_R1</v>
       </c>
       <c r="N6" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_R1 -ext png --layout radial</v>
       </c>
     </row>
@@ -27574,7 +27842,7 @@
         <v>2DSB_R1</v>
       </c>
       <c r="N7" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_R1 -ext png --layout radial</v>
       </c>
     </row>
@@ -27631,7 +27899,7 @@
         <v>2DSB_R1</v>
       </c>
       <c r="N8" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_R1 -ext png --layout radial</v>
       </c>
     </row>
@@ -27688,8 +27956,8 @@
         <v>2DSB_R2</v>
       </c>
       <c r="N9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial --layout_reverse_complement </v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -27745,8 +28013,8 @@
         <v>2DSB_R2</v>
       </c>
       <c r="N10" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial --layout_reverse_complement </v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -27802,8 +28070,8 @@
         <v>2DSB_R2</v>
       </c>
       <c r="N11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial --layout_reverse_complement </v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -27859,8 +28127,8 @@
         <v>2DSB_R2</v>
       </c>
       <c r="N12" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial --layout_reverse_complement </v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -27916,8 +28184,8 @@
         <v>2DSB_R2</v>
       </c>
       <c r="N13" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial --layout_reverse_complement </v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -27973,8 +28241,8 @@
         <v>2DSB_R2</v>
       </c>
       <c r="N14" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial --layout_reverse_complement </v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -28030,7 +28298,7 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N15" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1 -ext png --layout radial</v>
       </c>
     </row>
@@ -28087,7 +28355,7 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N16" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1 -ext png --layout radial</v>
       </c>
     </row>
@@ -28144,7 +28412,7 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N17" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1 -ext png --layout radial</v>
       </c>
     </row>
@@ -28201,7 +28469,7 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N18" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1 -ext png --layout radial</v>
       </c>
     </row>
@@ -28258,7 +28526,7 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N19" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1 -ext png --layout radial</v>
       </c>
     </row>
@@ -28315,7 +28583,7 @@
         <v>1DSB_R1</v>
       </c>
       <c r="N20" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1 -ext png --layout radial</v>
       </c>
     </row>
@@ -28372,8 +28640,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N21" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial --layout_reverse_complement </v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -28429,8 +28697,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N22" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial --layout_reverse_complement </v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -28486,8 +28754,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N23" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial --layout_reverse_complement </v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -28543,8 +28811,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N24" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial --layout_reverse_complement </v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -28600,8 +28868,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N25" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial --layout_reverse_complement </v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -28657,8 +28925,8 @@
         <v>1DSB_R2</v>
       </c>
       <c r="N26" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial --layout_reverse_complement </v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -28714,7 +28982,7 @@
         <v>1DSB_R1_30bpDown</v>
       </c>
       <c r="N27" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1_30bpDown -ext png --layout radial</v>
       </c>
     </row>
@@ -28771,7 +29039,7 @@
         <v>1DSB_R1_30bpDown</v>
       </c>
       <c r="N28" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1_30bpDown -ext png --layout radial</v>
       </c>
     </row>
@@ -28828,7 +29096,7 @@
         <v>1DSB_R1_30bpDown</v>
       </c>
       <c r="N29" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1_30bpDown -ext png --layout radial</v>
       </c>
     </row>
@@ -28885,7 +29153,7 @@
         <v>1DSB_R1_30bpDown</v>
       </c>
       <c r="N30" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1_30bpDown -ext png --layout radial</v>
       </c>
     </row>
@@ -28942,7 +29210,7 @@
         <v>1DSB_R1_30bpDown</v>
       </c>
       <c r="N31" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1_30bpDown -ext png --layout radial</v>
       </c>
     </row>
@@ -28999,7 +29267,7 @@
         <v>1DSB_R1_30bpDown</v>
       </c>
       <c r="N32" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1_30bpDown -ext png --layout radial</v>
       </c>
     </row>
@@ -29056,8 +29324,8 @@
         <v>1DSB_R2_30bpDown</v>
       </c>
       <c r="N33" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2_30bpDown -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2_30bpDown -ext png --layout radial --layout_reverse_complement </v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -29113,8 +29381,8 @@
         <v>1DSB_R2_30bpDown</v>
       </c>
       <c r="N34" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2_30bpDown -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2_30bpDown -ext png --layout radial --layout_reverse_complement </v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -29170,8 +29438,8 @@
         <v>1DSB_R2_30bpDown</v>
       </c>
       <c r="N35" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2_30bpDown -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2_30bpDown -ext png --layout radial --layout_reverse_complement </v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -29227,8 +29495,8 @@
         <v>1DSB_R2_30bpDown</v>
       </c>
       <c r="N36" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2_30bpDown -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2_30bpDown -ext png --layout radial --layout_reverse_complement </v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -29284,8 +29552,8 @@
         <v>1DSB_R2_30bpDown</v>
       </c>
       <c r="N37" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2_30bpDown -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2_30bpDown -ext png --layout radial --layout_reverse_complement </v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -29341,8 +29609,8 @@
         <v>1DSB_R2_30bpDown</v>
       </c>
       <c r="N38" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2_30bpDown -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2_30bpDown -ext png --layout radial --layout_reverse_complement </v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -29398,7 +29666,7 @@
         <v>2DSBanti_R1</v>
       </c>
       <c r="N39" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_R1 -ext png --layout radial</v>
       </c>
     </row>
@@ -29455,7 +29723,7 @@
         <v>2DSBanti_R1</v>
       </c>
       <c r="N40" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_splicing -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_R1 -ext png --layout radial</v>
       </c>
     </row>
@@ -29512,8 +29780,8 @@
         <v>2DSBanti_R2</v>
       </c>
       <c r="N41" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_R2 -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_R2 -ext png --layout radial --layout_reverse_complement </v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
@@ -29569,8 +29837,8 @@
         <v>2DSBanti_R2</v>
       </c>
       <c r="N42" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_splicing -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_R2 -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_splicing -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_R2 -ext png --layout radial --layout_reverse_complement </v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -30309,34 +30577,34 @@
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
         <f ca="1">_xlfn.TEXTJOIN(CHAR(10), TRUE, N3:N26,N39,N40,N41,N42)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_R1 -ext png --layout radial
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_R1 -ext png --layout radial
 python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_R1 -ext png --layout radial
 python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_R1 -ext png --layout radial
 python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_R1 -ext png --layout radial
 python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_R1 -ext png --layout radial
 python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_R1 -ext png --layout radial
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial --layout_reverse_complement 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial --layout_reverse_complement 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial --layout_reverse_complement 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial --layout_reverse_complement 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial --layout_reverse_complement 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial --layout_reverse_complement 
 python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1 -ext png --layout radial
 python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1 -ext png --layout radial
 python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1 -ext png --layout radial
 python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1 -ext png --layout radial
 python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1 -ext png --layout radial
 python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1 -ext png --layout radial
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial --layout_reverse_complement 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial --layout_reverse_complement 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial --layout_reverse_complement 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial --layout_reverse_complement 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial --layout_reverse_complement 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial --layout_reverse_complement 
 python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_R1 -ext png --layout radial
 python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_splicing -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_R1 -ext png --layout radial
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_R2 -ext png --layout radial
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_splicing -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_R2 -ext png --layout radial</v>
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_R2 -ext png --layout radial --layout_reverse_complement 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_splicing -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_R2 -ext png --layout radial --layout_reverse_complement </v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix reverse complementing in common layouts.
</commit_message>
<xml_diff>
--- a/libinfo.xlsx
+++ b/libinfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tchan\Code\SCMB_Project\RNA-mediated_DSB_repair\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4ADB0C0-203F-4C46-B760-0C2951BFF617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB3BE38-39AE-4629-9A4B-CFE1637F4978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="4" activeTab="8" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
   </bookViews>
@@ -38,7 +38,6 @@
     <definedName name="var_4_anti_offset">'4_graph_combined'!$A$19</definedName>
     <definedName name="var_6_1dsb_offset">'6_common_layout'!$A$18</definedName>
     <definedName name="var_6_anti_offset">'6_common_layout'!$A$10</definedName>
-    <definedName name="var_6_anti_ofsfset">'6_common_layout'!$A$10</definedName>
     <definedName name="var_6_layout">'6_common_layout'!$B$1</definedName>
     <definedName name="var_7_common_layout">'7_plot_graph'!$B$1</definedName>
     <definedName name="var_7_common_layout_combined">'7_plot_graph_combined'!$B$1</definedName>
@@ -89,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1566" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1566" uniqueCount="194">
   <si>
     <t>yjl217</t>
   </si>
@@ -669,6 +668,9 @@
   <si>
     <t>radial</t>
   </si>
+  <si>
+    <t>reverse_complement</t>
+  </si>
 </sst>
 </file>
 
@@ -802,6 +804,12 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{FFD19645-61C4-4244-A560-0232B787F38C}"/>
   </cellStyles>
   <dxfs count="235">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1107,9 +1115,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
       </font>
@@ -1278,9 +1283,6 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2888,8 +2890,12 @@
     <tableColumn id="18" xr3:uid="{BACD6182-9E09-4A02-A171-8DFCB7543380}" name="dir" dataDxfId="67">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 12, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{39C35B5A-7D06-4895-BF0F-A803A5F94E2E}" name="strand" dataDxfId="66">
-      <calculatedColumnFormula array="1">_xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[strand]:[strand]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 12, 1))</calculatedColumnFormula>
+    <tableColumn id="2" xr3:uid="{39C35B5A-7D06-4895-BF0F-A803A5F94E2E}" name="reverse_complement" dataDxfId="66">
+      <calculatedColumnFormula array="1">_xlfn.TEXTJOIN(
+  " ",
+  TRUE,
+  IF(OFFSET(table_3_1[[strand]:[strand]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 12, 1) = "R1", 0, 1)
+)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="13" xr3:uid="{F617BC3E-90A8-4E63-B2A4-EAC9DE705FC7}" name="control" dataDxfId="65">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 6 * (table_6_3[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
@@ -2907,7 +2913,7 @@
       <calculatedColumnFormula>_xlfn.CONCAT(table_6_3[[#This Row],[dsb_type]], "_", table_6_3[[#This Row],[hguide]], IF(table_6_3[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_3[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{8BD09F85-30B0-46CA-A0E3-2CC4F3FB2BD0}" name="command" dataDxfId="61">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_3[[#This Row],[dir]], IF(NOT(ISNA(table_6_3[[#This Row],[strand]])), _xlfn.CONCAT(" -s ", table_6_3[[#This Row],[strand]]), ""), " -o ", layouts, "/", table_6_3[[#This Row],[dir_out]], " --subst_type ", table_6_3[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_3[[#This Row],[dir]], IF(NOT(ISNA(table_6_3[[#This Row],[reverse_complement]])), _xlfn.CONCAT(" -rc ", table_6_3[[#This Row],[reverse_complement]]), ""), " -o ", layouts, "/", table_6_3[[#This Row],[dir_out]], " --subst_type ", table_6_3[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2940,8 +2946,8 @@
     <tableColumn id="19" xr3:uid="{CFCDDB26-095C-4395-82E2-37B45B0CDEAD}" name="dir_out" dataDxfId="53">
       <calculatedColumnFormula>_xlfn.CONCAT(table_6_4[[#This Row],[dsb_type]], "_", table_6_4[[#This Row],[hguide]], IF(table_6_4[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_4[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{DC6C9CBA-5796-4FFE-878D-BB47DC276187}" name="command" dataDxfId="52">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_4[[#This Row],[dir]], IF(NOT(ISNA(table_6_4[[#This Row],[strand]])), _xlfn.CONCAT(" -s ", table_6_4[[#This Row],[strand]]), ""), " -o ", layouts, "/", table_6_4[[#This Row],[dir_out]], " --subst_type ", table_6_4[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{DC6C9CBA-5796-4FFE-878D-BB47DC276187}" name="command" dataDxfId="2">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_4[[#This Row],[dir]], IF(NOT(ISNA(table_6_4[[#This Row],[strand]])), _xlfn.CONCAT(" -rc ", table_6_4[[#This Row],[strand]]), ""), " -o ", layouts, "/", table_6_4[[#This Row],[dir_out]], " --subst_type ", table_6_4[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2949,33 +2955,37 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}" name="table_6_5" displayName="table_6_5" ref="A23:I24" totalsRowShown="0" headerRowDxfId="51" headerRowBorderDxfId="50" tableBorderDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}" name="table_6_5" displayName="table_6_5" ref="A23:I24" totalsRowShown="0" headerRowDxfId="52" headerRowBorderDxfId="51" tableBorderDxfId="50">
   <autoFilter ref="A23:I24" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{0F421990-E775-4F35-92AF-6BA19E0E8AEE}" name="index"/>
-    <tableColumn id="2" xr3:uid="{81FE7256-F482-4A2C-902D-871C80C1D881}" name="dir" dataDxfId="48">
+    <tableColumn id="2" xr3:uid="{81FE7256-F482-4A2C-902D-871C80C1D881}" name="dir" dataDxfId="49">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]:[index]] - 1), 0, 4, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E9F8E6A0-B4A7-475B-9ED2-9F2A4A9EB628}" name="strand" dataDxfId="47">
-      <calculatedColumnFormula array="1">_xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[strand]:[strand]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]:[index]] - 1), 0, 4, 1))</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{E9F8E6A0-B4A7-475B-9ED2-9F2A4A9EB628}" name="strand" dataDxfId="48">
+      <calculatedColumnFormula array="1">_xlfn.TEXTJOIN(
+  " ",
+  TRUE,
+  IF(OFFSET(table_3_1[[strand]:[strand]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]:[index]] - 1), 0,4, 1) = "R1", 0, 1)
+)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{70821CEE-FFC4-44AB-ACF6-DA81A4B053E6}" name="control" dataDxfId="46">
+    <tableColumn id="6" xr3:uid="{70821CEE-FFC4-44AB-ACF6-DA81A4B053E6}" name="control" dataDxfId="47">
       <calculatedColumnFormula>OFFSET(table_3_1[control], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{FA9180EA-3AA0-451A-ACAC-78776C7CB75D}" name="dsb_type" dataDxfId="45">
+    <tableColumn id="5" xr3:uid="{FA9180EA-3AA0-451A-ACAC-78776C7CB75D}" name="dsb_type" dataDxfId="46">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{E0783723-9246-4BF6-A5DA-E000EA1E5E87}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DE820E4E-FF8B-435B-B07F-D397029AF597}" name="hguide" dataDxfId="44">
+    <tableColumn id="4" xr3:uid="{DE820E4E-FF8B-435B-B07F-D397029AF597}" name="hguide" dataDxfId="45">
       <calculatedColumnFormula>OFFSET(table_3_1[[hguide]:[hguide]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{3D97DBDD-03E9-4A6C-BADA-D01B27A8EE51}" name="dir_out" dataDxfId="43">
+    <tableColumn id="9" xr3:uid="{3D97DBDD-03E9-4A6C-BADA-D01B27A8EE51}" name="dir_out" dataDxfId="44">
       <calculatedColumnFormula>_xlfn.CONCAT(table_6_5[[#This Row],[dsb_type]], "_", table_6_5[[#This Row],[hguide]], IF(table_6_5[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_5[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5E7626AE-E376-4C60-BA64-B24F95580083}" name="command" dataDxfId="42">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_5[[#This Row],[dir]], " -s ", table_6_5[[#This Row],[strand]], " -o ", layouts, "/", table_6_5[[#This Row],[dir_out]], " --subst_type ", table_6_5[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{5E7626AE-E376-4C60-BA64-B24F95580083}" name="command" dataDxfId="43">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_5[[#This Row],[dir]], " -rc ", table_6_5[[#This Row],[strand]], " -o ", layouts, "/", table_6_5[[#This Row],[dir_out]], " --subst_type ", table_6_5[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2983,48 +2993,57 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{86CE8E4A-18BF-427A-81F0-F9655767A016}" name="table_7_1" displayName="table_7_1" ref="A2:N42" totalsRowShown="0" headerRowDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{86CE8E4A-18BF-427A-81F0-F9655767A016}" name="table_7_1" displayName="table_7_1" ref="A2:N42" totalsRowShown="0" headerRowDxfId="42">
   <autoFilter ref="A2:N42" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
   <tableColumns count="14">
-    <tableColumn id="25" xr3:uid="{C323C376-24D3-4404-9E0F-6E9361862271}" name="index" dataDxfId="40"/>
-    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="39">
+    <tableColumn id="25" xr3:uid="{C323C376-24D3-4404-9E0F-6E9361862271}" name="index" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="40">
       <calculatedColumnFormula>OFFSET(table_3_1[[dir]:[dir]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="38">
+    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="39">
       <calculatedColumnFormula>OFFSET(table_3_1[[control]:[control]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="37">
+    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="38">
       <calculatedColumnFormula>OFFSET(table_3_1[[ref]:[ref]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="36">
+    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="37">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_pos]:[dsb_pos]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="35">
+    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="36">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_type]:[dsb_type]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="34">
+    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="35">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_type_command]:[dsb_type_command]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="33">
+    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="34">
       <calculatedColumnFormula>OFFSET(table_3_1[[strand]:[strand]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="32">
+    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="33">
       <calculatedColumnFormula>OFFSET(table_3_1[[hguide]:[hguide]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="31">
+    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="32">
       <calculatedColumnFormula>OFFSET(table_3_1[[cell]:[cell]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="30">
+    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="31">
       <calculatedColumnFormula>OFFSET(table_3_1[[treatment]:[treatment]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="29">
+    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="30">
       <calculatedColumnFormula>"without"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="28">
-      <calculatedColumnFormula>IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</calculatedColumnFormula>
+    <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="0">
+      <calculatedColumnFormula>IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="0">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="1">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3035,44 +3054,44 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{B47D9508-D874-40FC-B6F6-C106B48F6A94}" name="table_7_2" displayName="table_7_2" ref="A44:N56" totalsRowShown="0">
   <autoFilter ref="A44:N56" xr:uid="{D74A5276-1A50-4DA1-9131-9669404C8622}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{488C5146-A746-4F74-BCC8-806E4DC740CE}" name="index" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{C2A88DF4-2444-4C4C-A089-6CF9ADE79BD8}" name="dir" dataDxfId="26">
+    <tableColumn id="1" xr3:uid="{488C5146-A746-4F74-BCC8-806E4DC740CE}" name="index" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{C2A88DF4-2444-4C4C-A089-6CF9ADE79BD8}" name="dir" dataDxfId="28">
       <calculatedColumnFormula>OFFSET(table_3_2[[dir]:[dir]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{7698ACE3-2351-400D-B00F-5A70184F8A33}" name="control" dataDxfId="25">
+    <tableColumn id="3" xr3:uid="{7698ACE3-2351-400D-B00F-5A70184F8A33}" name="control" dataDxfId="27">
       <calculatedColumnFormula>OFFSET(table_3_2[[control]:[control]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5E82B04C-FF09-492C-8A23-7E43B5990149}" name="ref" dataDxfId="24">
+    <tableColumn id="4" xr3:uid="{5E82B04C-FF09-492C-8A23-7E43B5990149}" name="ref" dataDxfId="26">
       <calculatedColumnFormula>OFFSET(table_3_2[[ref]:[ref]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{F4D36A0E-549B-4F3A-BCA9-75E151448998}" name="dsb_pos" dataDxfId="23">
+    <tableColumn id="5" xr3:uid="{F4D36A0E-549B-4F3A-BCA9-75E151448998}" name="dsb_pos" dataDxfId="25">
       <calculatedColumnFormula>OFFSET(table_3_2[[dsb_pos]:[dsb_pos]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{AEBBBB88-8CE2-409D-AE19-9C23263250A9}" name="dsb_type" dataDxfId="22">
+    <tableColumn id="6" xr3:uid="{AEBBBB88-8CE2-409D-AE19-9C23263250A9}" name="dsb_type" dataDxfId="24">
       <calculatedColumnFormula>OFFSET(table_3_2[[dsb_type]:[dsb_type]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3E71E7D2-0FA5-4FD5-BDC3-2955A091A9E6}" name="dsb_type_command" dataDxfId="21">
+    <tableColumn id="7" xr3:uid="{3E71E7D2-0FA5-4FD5-BDC3-2955A091A9E6}" name="dsb_type_command" dataDxfId="23">
       <calculatedColumnFormula>OFFSET(table_3_2[[dsb_type_command]:[dsb_type_command]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{EBD35881-E696-4202-9149-75A4EFFFAAD6}" name="strand" dataDxfId="20">
+    <tableColumn id="8" xr3:uid="{EBD35881-E696-4202-9149-75A4EFFFAAD6}" name="strand" dataDxfId="22">
       <calculatedColumnFormula>OFFSET(table_3_2[[strand]:[strand]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{123CA279-0CB6-41C1-9CD8-20D375B9B66D}" name="hguide" dataDxfId="19">
+    <tableColumn id="9" xr3:uid="{123CA279-0CB6-41C1-9CD8-20D375B9B66D}" name="hguide" dataDxfId="21">
       <calculatedColumnFormula>OFFSET(table_3_2[[hguide]:[hguide]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{3DCE3F3A-187D-411E-93FC-8C6C3EE9CAA2}" name="cell" dataDxfId="18">
+    <tableColumn id="10" xr3:uid="{3DCE3F3A-187D-411E-93FC-8C6C3EE9CAA2}" name="cell" dataDxfId="20">
       <calculatedColumnFormula>OFFSET(table_3_2[[cell]:[cell]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{9E585D29-AB3E-4D04-8C1D-24F78339C9A3}" name="treatment" dataDxfId="17">
+    <tableColumn id="11" xr3:uid="{9E585D29-AB3E-4D04-8C1D-24F78339C9A3}" name="treatment" dataDxfId="19">
       <calculatedColumnFormula>OFFSET(table_3_2[[treatment]:[treatment]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{928286B8-23FB-4375-B52B-617DD59D6098}" name="subst_type" dataDxfId="16">
+    <tableColumn id="12" xr3:uid="{928286B8-23FB-4375-B52B-617DD59D6098}" name="subst_type" dataDxfId="18">
       <calculatedColumnFormula>"without"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{E18D2025-56E8-4128-9201-9E0BF8A67AC0}" name="common_layout_dir" dataDxfId="15">
+    <tableColumn id="15" xr3:uid="{E18D2025-56E8-4128-9201-9E0BF8A67AC0}" name="common_layout_dir" dataDxfId="17">
       <calculatedColumnFormula>OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_2[[#This Row],[index]] - 1, 6) + 2, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{0917AB98-1545-4642-9BE8-618AAA1E404A}" name="command" dataDxfId="14">
+    <tableColumn id="13" xr3:uid="{0917AB98-1545-4642-9BE8-618AAA1E404A}" name="command" dataDxfId="16">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3081,14 +3100,14 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{B76EEC45-4FC3-44D5-9B2E-9183DF724F60}" name="table_7_3" displayName="table_7_3" ref="A3:C19" totalsRowShown="0" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{B76EEC45-4FC3-44D5-9B2E-9183DF724F60}" name="table_7_3" displayName="table_7_3" ref="A3:C19" totalsRowShown="0" headerRowDxfId="15">
   <autoFilter ref="A3:C19" xr:uid="{B76EEC45-4FC3-44D5-9B2E-9183DF724F60}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{FAFADB73-BF3B-401A-8C48-9FCB5D3C4CB6}" name="index" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{8541A14E-3250-4B9C-B315-969FC11BE60A}" name="dir" dataDxfId="11">
+    <tableColumn id="1" xr3:uid="{FAFADB73-BF3B-401A-8C48-9FCB5D3C4CB6}" name="index" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{8541A14E-3250-4B9C-B315-969FC11BE60A}" name="dir" dataDxfId="13">
       <calculatedColumnFormula>OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{EAD6D5EC-B61E-4A98-B4FD-4932757CFEA3}" name="command" dataDxfId="10">
+    <tableColumn id="6" xr3:uid="{EAD6D5EC-B61E-4A98-B4FD-4932757CFEA3}" name="command" dataDxfId="12">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3135,14 +3154,14 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{8B4E853A-A4F1-4022-B857-226C57559A5F}" name="table_7_4" displayName="table_7_4" ref="A21:C23" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{8B4E853A-A4F1-4022-B857-226C57559A5F}" name="table_7_4" displayName="table_7_4" ref="A21:C23" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="A21:C23" xr:uid="{8B4E853A-A4F1-4022-B857-226C57559A5F}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{1ECF32A2-E353-4754-B4C5-11C46AACF6C0}" name="index" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{181C59FC-364D-4421-8E54-98DFF4CA7C05}" name="dir" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{1ECF32A2-E353-4754-B4C5-11C46AACF6C0}" name="index" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{181C59FC-364D-4421-8E54-98DFF4CA7C05}" name="dir" dataDxfId="9">
       <calculatedColumnFormula>OFFSET(table_4_2[[dir_out]:[dir_out]], table_7_4[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{6D8CC942-572B-44F2-BCA6-4D31A25A4067}" name="command" dataDxfId="6">
+    <tableColumn id="6" xr3:uid="{6D8CC942-572B-44F2-BCA6-4D31A25A4067}" name="command" dataDxfId="8">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_4[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_2[[dir_out]:[dir_out]],table_7_4[[#This Row],[index]] - 1, 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3151,14 +3170,14 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{58F5EC27-BD76-45AE-8D38-F4E705EF79E9}" name="table_7_5" displayName="table_7_5" ref="A26:C34" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{58F5EC27-BD76-45AE-8D38-F4E705EF79E9}" name="table_7_5" displayName="table_7_5" ref="A26:C34" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A26:C34" xr:uid="{58F5EC27-BD76-45AE-8D38-F4E705EF79E9}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{AAC1476C-44CE-49FD-8254-50BAEAA6929C}" name="index" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{1222E48F-ED5C-48AA-BA39-1443B841BC9F}" name="dir" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{AAC1476C-44CE-49FD-8254-50BAEAA6929C}" name="index" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{1222E48F-ED5C-48AA-BA39-1443B841BC9F}" name="dir" dataDxfId="4">
       <calculatedColumnFormula>OFFSET(table_4_3[[dir_out]:[dir_out]], table_7_5[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{89B7E589-2097-43FC-B96B-19D2EF777E97}" name="command" dataDxfId="1">
+    <tableColumn id="6" xr3:uid="{89B7E589-2097-43FC-B96B-19D2EF777E97}" name="command" dataDxfId="3">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -26435,8 +26454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1417E7-0E2A-4E67-94B4-4030BF5F7C23}">
   <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27155,7 +27174,7 @@
         <v>87</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>82</v>
+        <v>193</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>134</v>
@@ -27185,8 +27204,12 @@
         <v>libraries_4/WT_sgAB_R1_sense libraries_4/WT_sgAB_R1_branch libraries_4/WT_sgAB_R1_cmv libraries_4/KO_sgAB_R1_sense libraries_4/KO_sgAB_R1_branch libraries_4/KO_sgAB_R1_cmv libraries_4/WT_sgAB_R2_sense libraries_4/WT_sgAB_R2_branch libraries_4/WT_sgAB_R2_cmv libraries_4/KO_sgAB_R2_sense libraries_4/KO_sgAB_R2_branch libraries_4/KO_sgAB_R2_cmv</v>
       </c>
       <c r="C16" s="6" t="str" cm="1">
-        <f t="array" aca="1" ref="C16" ca="1">_xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[strand]:[strand]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 12, 1))</f>
-        <v>R1 R1 R1 R1 R1 R1 R2 R2 R2 R2 R2 R2</v>
+        <f t="array" aca="1" ref="C16" ca="1">_xlfn.TEXTJOIN(
+  " ",
+  TRUE,
+  IF(OFFSET(table_3_1[[strand]:[strand]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 12, 1) = "R1", 0, 1)
+)</f>
+        <v>0 0 0 0 0 0 1 1 1 1 1 1</v>
       </c>
       <c r="D16" t="str">
         <f ca="1">OFFSET(table_3_1[control], 6 * (table_6_3[[#This Row],[index]] - 1), 0, 1, 1)</f>
@@ -27209,8 +27232,8 @@
         <v>2DSB_AB</v>
       </c>
       <c r="I16" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_3[[#This Row],[dir]], IF(NOT(ISNA(table_6_3[[#This Row],[strand]])), _xlfn.CONCAT(" -s ", table_6_3[[#This Row],[strand]]), ""), " -o ", layouts, "/", table_6_3[[#This Row],[dir_out]], " --subst_type ", table_6_3[[#This Row],[subst_type]], " --layout ", var_6_layout)</f>
-        <v>python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgAB_R1_sense libraries_4/WT_sgAB_R1_branch libraries_4/WT_sgAB_R1_cmv libraries_4/KO_sgAB_R1_sense libraries_4/KO_sgAB_R1_branch libraries_4/KO_sgAB_R1_cmv libraries_4/WT_sgAB_R2_sense libraries_4/WT_sgAB_R2_branch libraries_4/WT_sgAB_R2_cmv libraries_4/KO_sgAB_R2_sense libraries_4/KO_sgAB_R2_branch libraries_4/KO_sgAB_R2_cmv -s R1 R1 R1 R1 R1 R1 R2 R2 R2 R2 R2 R2 -o layouts/2DSB_AB --subst_type without --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_3[[#This Row],[dir]], IF(NOT(ISNA(table_6_3[[#This Row],[reverse_complement]])), _xlfn.CONCAT(" -rc ", table_6_3[[#This Row],[reverse_complement]]), ""), " -o ", layouts, "/", table_6_3[[#This Row],[dir_out]], " --subst_type ", table_6_3[[#This Row],[subst_type]], " --layout ", var_6_layout)</f>
+        <v>python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgAB_R1_sense libraries_4/WT_sgAB_R1_branch libraries_4/WT_sgAB_R1_cmv libraries_4/KO_sgAB_R1_sense libraries_4/KO_sgAB_R1_branch libraries_4/KO_sgAB_R1_cmv libraries_4/WT_sgAB_R2_sense libraries_4/WT_sgAB_R2_branch libraries_4/WT_sgAB_R2_cmv libraries_4/KO_sgAB_R2_sense libraries_4/KO_sgAB_R2_branch libraries_4/KO_sgAB_R2_cmv -rc 0 0 0 0 0 0 1 1 1 1 1 1 -o layouts/2DSB_AB --subst_type without --layout radial</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
@@ -27287,7 +27310,7 @@
         <v>1DSB_A</v>
       </c>
       <c r="I20" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_4[[#This Row],[dir]], IF(NOT(ISNA(table_6_4[[#This Row],[strand]])), _xlfn.CONCAT(" -s ", table_6_4[[#This Row],[strand]]), ""), " -o ", layouts, "/", table_6_4[[#This Row],[dir_out]], " --subst_type ", table_6_4[[#This Row],[subst_type]], " --layout ", var_6_layout)</f>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_4[[#This Row],[dir]], IF(NOT(ISNA(table_6_4[[#This Row],[strand]])), _xlfn.CONCAT(" -rc ", table_6_4[[#This Row],[strand]]), ""), " -o ", layouts, "/", table_6_4[[#This Row],[dir_out]], " --subst_type ", table_6_4[[#This Row],[subst_type]], " --layout ", var_6_layout)</f>
         <v>python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgA_R1_sense libraries_4/WT_sgA_R1_branch libraries_4/WT_sgA_R1_cmv libraries_4/KO_sgA_R1_sense libraries_4/KO_sgA_R1_branch libraries_4/KO_sgA_R1_cmv -o layouts/1DSB_A --subst_type without --layout radial</v>
       </c>
       <c r="J20" s="6"/>
@@ -27327,7 +27350,7 @@
         <v>1DSB_B</v>
       </c>
       <c r="I21" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_4[[#This Row],[dir]], IF(NOT(ISNA(table_6_4[[#This Row],[strand]])), _xlfn.CONCAT(" -s ", table_6_4[[#This Row],[strand]]), ""), " -o ", layouts, "/", table_6_4[[#This Row],[dir_out]], " --subst_type ", table_6_4[[#This Row],[subst_type]], " --layout ", var_6_layout)</f>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_4[[#This Row],[dir]], IF(NOT(ISNA(table_6_4[[#This Row],[strand]])), _xlfn.CONCAT(" -rc ", table_6_4[[#This Row],[strand]]), ""), " -o ", layouts, "/", table_6_4[[#This Row],[dir_out]], " --subst_type ", table_6_4[[#This Row],[subst_type]], " --layout ", var_6_layout)</f>
         <v>python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgB_R2_sense libraries_4/WT_sgB_R2_branch libraries_4/WT_sgB_R2_cmv libraries_4/KO_sgB_R2_sense libraries_4/KO_sgB_R2_branch libraries_4/KO_sgB_R2_cmv -o layouts/1DSB_B --subst_type without --layout radial</v>
       </c>
       <c r="J21" s="1"/>
@@ -27386,8 +27409,12 @@
         <v>libraries_4/WT_sgCD_R1_antisense libraries_4/WT_sgCD_R1_splicing libraries_4/WT_sgCD_R2_antisense libraries_4/WT_sgCD_R2_splicing</v>
       </c>
       <c r="C24" s="6" t="str" cm="1">
-        <f t="array" aca="1" ref="C24" ca="1">_xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[strand]:[strand]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]:[index]] - 1), 0, 4, 1))</f>
-        <v>R1 R1 R2 R2</v>
+        <f t="array" aca="1" ref="C24" ca="1">_xlfn.TEXTJOIN(
+  " ",
+  TRUE,
+  IF(OFFSET(table_3_1[[strand]:[strand]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]:[index]] - 1), 0,4, 1) = "R1", 0, 1)
+)</f>
+        <v>0 0 1 1</v>
       </c>
       <c r="D24" s="6" t="str">
         <f ca="1">OFFSET(table_3_1[control], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</f>
@@ -27410,8 +27437,8 @@
         <v>2DSBanti_CD</v>
       </c>
       <c r="I24" s="4" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_5[[#This Row],[dir]], " -s ", table_6_5[[#This Row],[strand]], " -o ", layouts, "/", table_6_5[[#This Row],[dir_out]], " --subst_type ", table_6_5[[#This Row],[subst_type]], " --layout ", var_6_layout)</f>
-        <v>python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgCD_R1_antisense libraries_4/WT_sgCD_R1_splicing libraries_4/WT_sgCD_R2_antisense libraries_4/WT_sgCD_R2_splicing -s R1 R1 R2 R2 -o layouts/2DSBanti_CD --subst_type without --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_5[[#This Row],[dir]], " -rc ", table_6_5[[#This Row],[strand]], " -o ", layouts, "/", table_6_5[[#This Row],[dir_out]], " --subst_type ", table_6_5[[#This Row],[subst_type]], " --layout ", var_6_layout)</f>
+        <v>python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgCD_R1_antisense libraries_4/WT_sgCD_R1_splicing libraries_4/WT_sgCD_R2_antisense libraries_4/WT_sgCD_R2_splicing -rc 0 0 1 1 -o layouts/2DSBanti_CD --subst_type without --layout radial</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
@@ -27439,10 +27466,10 @@
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="str">
         <f ca="1">_xlfn.TEXTJOIN(CHAR(10), TRUE, table_6_3[command], table_6_4[command], table_6_5[command])</f>
-        <v>python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgAB_R1_sense libraries_4/WT_sgAB_R1_branch libraries_4/WT_sgAB_R1_cmv libraries_4/KO_sgAB_R1_sense libraries_4/KO_sgAB_R1_branch libraries_4/KO_sgAB_R1_cmv libraries_4/WT_sgAB_R2_sense libraries_4/WT_sgAB_R2_branch libraries_4/WT_sgAB_R2_cmv libraries_4/KO_sgAB_R2_sense libraries_4/KO_sgAB_R2_branch libraries_4/KO_sgAB_R2_cmv -s R1 R1 R1 R1 R1 R1 R2 R2 R2 R2 R2 R2 -o layouts/2DSB_AB --subst_type without --layout radial
+        <v>python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgAB_R1_sense libraries_4/WT_sgAB_R1_branch libraries_4/WT_sgAB_R1_cmv libraries_4/KO_sgAB_R1_sense libraries_4/KO_sgAB_R1_branch libraries_4/KO_sgAB_R1_cmv libraries_4/WT_sgAB_R2_sense libraries_4/WT_sgAB_R2_branch libraries_4/WT_sgAB_R2_cmv libraries_4/KO_sgAB_R2_sense libraries_4/KO_sgAB_R2_branch libraries_4/KO_sgAB_R2_cmv -rc 0 0 0 0 0 0 1 1 1 1 1 1 -o layouts/2DSB_AB --subst_type without --layout radial
 python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgA_R1_sense libraries_4/WT_sgA_R1_branch libraries_4/WT_sgA_R1_cmv libraries_4/KO_sgA_R1_sense libraries_4/KO_sgA_R1_branch libraries_4/KO_sgA_R1_cmv -o layouts/1DSB_A --subst_type without --layout radial
 python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgB_R2_sense libraries_4/WT_sgB_R2_branch libraries_4/WT_sgB_R2_cmv libraries_4/KO_sgB_R2_sense libraries_4/KO_sgB_R2_branch libraries_4/KO_sgB_R2_cmv -o layouts/1DSB_B --subst_type without --layout radial
-python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgCD_R1_antisense libraries_4/WT_sgCD_R1_splicing libraries_4/WT_sgCD_R2_antisense libraries_4/WT_sgCD_R2_splicing -s R1 R1 R2 R2 -o layouts/2DSBanti_CD --subst_type without --layout radial</v>
+python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgCD_R1_antisense libraries_4/WT_sgCD_R1_splicing libraries_4/WT_sgCD_R2_antisense libraries_4/WT_sgCD_R2_splicing -rc 0 0 1 1 -o layouts/2DSBanti_CD --subst_type without --layout radial</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -27477,8 +27504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1375107-D76A-4386-B771-6693BBF75061}">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27493,7 +27520,7 @@
     <col min="10" max="10" width="12.140625" customWidth="1"/>
     <col min="11" max="11" width="12.85546875" customWidth="1"/>
     <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" customWidth="1"/>
     <col min="14" max="14" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -27610,12 +27637,21 @@
         <v>without</v>
       </c>
       <c r="M3" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>2DSB_R1</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>2DSB_AB</v>
       </c>
       <c r="N3" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_R1 -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout radial</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -27667,12 +27703,21 @@
         <v>without</v>
       </c>
       <c r="M4" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>2DSB_R1</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>2DSB_AB</v>
       </c>
       <c r="N4" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_R1 -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout radial</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -27724,12 +27769,21 @@
         <v>without</v>
       </c>
       <c r="M5" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>2DSB_R1</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>2DSB_AB</v>
       </c>
       <c r="N5" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_R1 -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout radial</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -27781,12 +27835,21 @@
         <v>without</v>
       </c>
       <c r="M6" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>2DSB_R1</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>2DSB_AB</v>
       </c>
       <c r="N6" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_R1 -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout radial</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -27838,12 +27901,21 @@
         <v>without</v>
       </c>
       <c r="M7" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>2DSB_R1</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>2DSB_AB</v>
       </c>
       <c r="N7" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_R1 -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout radial</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -27895,12 +27967,21 @@
         <v>without</v>
       </c>
       <c r="M8" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>2DSB_R1</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>2DSB_AB</v>
       </c>
       <c r="N8" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_R1 -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout radial</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -27952,12 +28033,21 @@
         <v>without</v>
       </c>
       <c r="M9" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>2DSB_R2</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>2DSB_AB</v>
       </c>
       <c r="N9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial --layout_reverse_complement </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout radial --reverse_complement </v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -28009,12 +28099,21 @@
         <v>without</v>
       </c>
       <c r="M10" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>2DSB_R2</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>2DSB_AB</v>
       </c>
       <c r="N10" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial --layout_reverse_complement </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout radial --reverse_complement </v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -28066,12 +28165,21 @@
         <v>without</v>
       </c>
       <c r="M11" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>2DSB_R2</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>2DSB_AB</v>
       </c>
       <c r="N11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial --layout_reverse_complement </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout radial --reverse_complement </v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -28123,12 +28231,21 @@
         <v>without</v>
       </c>
       <c r="M12" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>2DSB_R2</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>2DSB_AB</v>
       </c>
       <c r="N12" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial --layout_reverse_complement </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout radial --reverse_complement </v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -28180,12 +28297,21 @@
         <v>without</v>
       </c>
       <c r="M13" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>2DSB_R2</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>2DSB_AB</v>
       </c>
       <c r="N13" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial --layout_reverse_complement </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout radial --reverse_complement </v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -28237,12 +28363,21 @@
         <v>without</v>
       </c>
       <c r="M14" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>2DSB_R2</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>2DSB_AB</v>
       </c>
       <c r="N14" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial --layout_reverse_complement </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout radial --reverse_complement </v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -28294,12 +28429,21 @@
         <v>without</v>
       </c>
       <c r="M15" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>1DSB_R1</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>1DSB_A</v>
       </c>
       <c r="N15" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1 -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout radial</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -28351,12 +28495,21 @@
         <v>without</v>
       </c>
       <c r="M16" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>1DSB_R1</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>1DSB_A</v>
       </c>
       <c r="N16" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1 -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout radial</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -28408,12 +28561,21 @@
         <v>without</v>
       </c>
       <c r="M17" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>1DSB_R1</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>1DSB_A</v>
       </c>
       <c r="N17" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1 -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout radial</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -28465,12 +28627,21 @@
         <v>without</v>
       </c>
       <c r="M18" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>1DSB_R1</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>1DSB_A</v>
       </c>
       <c r="N18" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1 -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout radial</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -28522,12 +28693,21 @@
         <v>without</v>
       </c>
       <c r="M19" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>1DSB_R1</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>1DSB_A</v>
       </c>
       <c r="N19" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1 -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout radial</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -28579,12 +28759,21 @@
         <v>without</v>
       </c>
       <c r="M20" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>1DSB_R1</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>1DSB_A</v>
       </c>
       <c r="N20" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1 -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout radial</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -28636,12 +28825,21 @@
         <v>without</v>
       </c>
       <c r="M21" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>1DSB_R2</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>1DSB_B</v>
       </c>
       <c r="N21" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial --layout_reverse_complement </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout radial</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -28693,12 +28891,21 @@
         <v>without</v>
       </c>
       <c r="M22" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>1DSB_R2</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>1DSB_B</v>
       </c>
       <c r="N22" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial --layout_reverse_complement </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout radial</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -28750,12 +28957,21 @@
         <v>without</v>
       </c>
       <c r="M23" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>1DSB_R2</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>1DSB_B</v>
       </c>
       <c r="N23" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial --layout_reverse_complement </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout radial</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -28807,12 +29023,21 @@
         <v>without</v>
       </c>
       <c r="M24" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>1DSB_R2</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>1DSB_B</v>
       </c>
       <c r="N24" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial --layout_reverse_complement </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout radial</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -28864,12 +29089,21 @@
         <v>without</v>
       </c>
       <c r="M25" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>1DSB_R2</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>1DSB_B</v>
       </c>
       <c r="N25" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial --layout_reverse_complement </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout radial</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -28921,12 +29155,21 @@
         <v>without</v>
       </c>
       <c r="M26" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>1DSB_R2</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>1DSB_B</v>
       </c>
       <c r="N26" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial --layout_reverse_complement </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout radial</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -28978,12 +29221,21 @@
         <v>without</v>
       </c>
       <c r="M27" s="9" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>1DSB_R1_30bpDown</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>1DSB_A</v>
       </c>
       <c r="N27" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1_30bpDown -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout radial</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -29035,12 +29287,21 @@
         <v>without</v>
       </c>
       <c r="M28" s="9" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>1DSB_R1_30bpDown</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>1DSB_A</v>
       </c>
       <c r="N28" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1_30bpDown -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout radial</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -29092,12 +29353,21 @@
         <v>without</v>
       </c>
       <c r="M29" s="9" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>1DSB_R1_30bpDown</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>1DSB_A</v>
       </c>
       <c r="N29" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1_30bpDown -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout radial</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -29149,12 +29419,21 @@
         <v>without</v>
       </c>
       <c r="M30" s="9" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>1DSB_R1_30bpDown</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>1DSB_A</v>
       </c>
       <c r="N30" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1_30bpDown -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout radial</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -29206,12 +29485,21 @@
         <v>without</v>
       </c>
       <c r="M31" s="9" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>1DSB_R1_30bpDown</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>1DSB_A</v>
       </c>
       <c r="N31" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1_30bpDown -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout radial</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -29263,12 +29551,21 @@
         <v>without</v>
       </c>
       <c r="M32" s="9" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>1DSB_R1_30bpDown</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>1DSB_A</v>
       </c>
       <c r="N32" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1_30bpDown -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout radial</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -29320,12 +29617,21 @@
         <v>without</v>
       </c>
       <c r="M33" s="9" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>1DSB_R2_30bpDown</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>1DSB_B</v>
       </c>
       <c r="N33" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2_30bpDown -ext png --layout radial --layout_reverse_complement </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout radial</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -29377,12 +29683,21 @@
         <v>without</v>
       </c>
       <c r="M34" s="9" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>1DSB_R2_30bpDown</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>1DSB_B</v>
       </c>
       <c r="N34" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2_30bpDown -ext png --layout radial --layout_reverse_complement </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout radial</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -29434,12 +29749,21 @@
         <v>without</v>
       </c>
       <c r="M35" s="9" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>1DSB_R2_30bpDown</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>1DSB_B</v>
       </c>
       <c r="N35" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2_30bpDown -ext png --layout radial --layout_reverse_complement </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout radial</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -29491,12 +29815,21 @@
         <v>without</v>
       </c>
       <c r="M36" s="9" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>1DSB_R2_30bpDown</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>1DSB_B</v>
       </c>
       <c r="N36" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2_30bpDown -ext png --layout radial --layout_reverse_complement </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout radial</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -29548,12 +29881,21 @@
         <v>without</v>
       </c>
       <c r="M37" s="9" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>1DSB_R2_30bpDown</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>1DSB_B</v>
       </c>
       <c r="N37" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2_30bpDown -ext png --layout radial --layout_reverse_complement </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout radial</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -29605,12 +29947,21 @@
         <v>without</v>
       </c>
       <c r="M38" s="9" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>1DSB_R2_30bpDown</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>1DSB_B</v>
       </c>
       <c r="N38" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2_30bpDown -ext png --layout radial --layout_reverse_complement </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout radial</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -29662,12 +30013,21 @@
         <v>without</v>
       </c>
       <c r="M39" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>2DSBanti_R1</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>2DSBanti_CD</v>
       </c>
       <c r="N39" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_R1 -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_CD -ext png --layout radial</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
@@ -29719,12 +30079,21 @@
         <v>without</v>
       </c>
       <c r="M40" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>2DSBanti_R1</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>2DSBanti_CD</v>
       </c>
       <c r="N40" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_splicing -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_R1 -ext png --layout radial</v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_splicing -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_CD -ext png --layout radial</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
@@ -29776,12 +30145,21 @@
         <v>without</v>
       </c>
       <c r="M41" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>2DSBanti_R2</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>2DSBanti_CD</v>
       </c>
       <c r="N41" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_R2 -ext png --layout radial --layout_reverse_complement </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_CD -ext png --layout radial --reverse_complement </v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
@@ -29833,12 +30211,21 @@
         <v>without</v>
       </c>
       <c r="M42" t="str">
-        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti", OFFSET(table_6_2[[dir_out]:[dir_out]], QUOTIENT( table_7_1[[#This Row],[index]] - 37, 2), 0, 1, 1), OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_1[[#This Row],[index]] - 1, 6), 0, 1, 1))</f>
-        <v>2DSBanti_R2</v>
+        <f ca="1">IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
+      OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
+      IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
+         OFFSET(table_6_3[[dir_out]:[dir_out]], 0, 0, 1, 1),
+         IF(table_7_1[[#This Row],[dsb_type]] = "1DSB",
+              OFFSET(table_6_4[[dir_out]:[dir_out]], IF(table_7_1[[#This Row],[hguide]] = "A", 0, 1), 0, 1, 1),
+              NA()
+         )
+      )
+  )</f>
+        <v>2DSBanti_CD</v>
       </c>
       <c r="N42" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[strand]] = "R2", " --layout_reverse_complement ", ""))</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_splicing -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_R2 -ext png --layout radial --layout_reverse_complement </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_splicing -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_CD -ext png --layout radial --reverse_complement </v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -30577,34 +30964,34 @@
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
         <f ca="1">_xlfn.TEXTJOIN(CHAR(10), TRUE, N3:N26,N39,N40,N41,N42)</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_R1 -ext png --layout radial
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_R1 -ext png --layout radial
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_R1 -ext png --layout radial
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_R1 -ext png --layout radial
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_R1 -ext png --layout radial
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_R1 -ext png --layout radial
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial --layout_reverse_complement 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial --layout_reverse_complement 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial --layout_reverse_complement 
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial --layout_reverse_complement 
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial --layout_reverse_complement 
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_R2 -ext png --layout radial --layout_reverse_complement 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1 -ext png --layout radial
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1 -ext png --layout radial
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1 -ext png --layout radial
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1 -ext png --layout radial
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1 -ext png --layout radial
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_R1 -ext png --layout radial
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial --layout_reverse_complement 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial --layout_reverse_complement 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial --layout_reverse_complement 
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial --layout_reverse_complement 
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial --layout_reverse_complement 
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_R2 -ext png --layout radial --layout_reverse_complement 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_R1 -ext png --layout radial
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_splicing -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_R1 -ext png --layout radial
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_R2 -ext png --layout radial --layout_reverse_complement 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_splicing -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_R2 -ext png --layout radial --layout_reverse_complement </v>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout radial --reverse_complement 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout radial --reverse_complement 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout radial --reverse_complement 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout radial --reverse_complement 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout radial --reverse_complement 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout radial --reverse_complement 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_CD -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_splicing -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_CD -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_CD -ext png --layout radial --reverse_complement 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_splicing -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_CD -ext png --layout radial --reverse_complement </v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update scripts for generating graphs.
</commit_message>
<xml_diff>
--- a/libinfo.xlsx
+++ b/libinfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tchan\Code\SCMB_Project\RNA-mediated_DSB_repair\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB3BE38-39AE-4629-9A4B-CFE1637F4978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC17100-D84A-49C2-B432-7DC16C021BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="4" activeTab="8" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="4" activeTab="9" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
   </bookViews>
   <sheets>
     <sheet name="globals" sheetId="3" r:id="rId1"/>
@@ -40,11 +40,11 @@
     <definedName name="var_6_anti_offset">'6_common_layout'!$A$10</definedName>
     <definedName name="var_6_layout">'6_common_layout'!$B$1</definedName>
     <definedName name="var_7_common_layout">'7_plot_graph'!$B$1</definedName>
-    <definedName name="var_7_common_layout_combined">'7_plot_graph_combined'!$B$1</definedName>
+    <definedName name="var_7_common_layout_combined">'7_plot_graph_combined'!#REF!</definedName>
     <definedName name="var_7_ext">'7_plot_graph'!$D$1</definedName>
-    <definedName name="var_7_ext_combined">'7_plot_graph_combined'!$D$1</definedName>
+    <definedName name="var_7_ext_combined">'7_plot_graph_combined'!#REF!</definedName>
     <definedName name="var_7_layout">'7_plot_graph'!$F$1</definedName>
-    <definedName name="var_7_layout_combined">'7_plot_graph_combined'!$F$1</definedName>
+    <definedName name="var_7_layout_combined">'7_plot_graph_combined'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1566" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1567" uniqueCount="192">
   <si>
     <t>yjl217</t>
   </si>
@@ -648,16 +648,10 @@
     <t>common_layout</t>
   </si>
   <si>
-    <t>common layout</t>
-  </si>
-  <si>
     <t>ext</t>
   </si>
   <si>
     <t>layout</t>
-  </si>
-  <si>
-    <t>universal</t>
   </si>
   <si>
     <t>png</t>
@@ -779,7 +773,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -790,8 +784,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -803,7 +795,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{FFD19645-61C4-4244-A560-0232B787F38C}"/>
   </cellStyles>
-  <dxfs count="235">
+  <dxfs count="238">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -815,71 +807,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -922,6 +849,27 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2675,7 +2623,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{70502F2F-AE2C-4D63-ADF7-F65702652EBF}" name="table_1_2" displayName="table_1_2" ref="A1:D108" totalsRowShown="0">
   <autoFilter ref="A1:D108" xr:uid="{70502F2F-AE2C-4D63-ADF7-F65702652EBF}"/>
   <tableColumns count="4">
-    <tableColumn id="2" xr3:uid="{BB99DCDA-08D4-474A-ABC3-5229CEAF80CF}" name="id" dataDxfId="234">
+    <tableColumn id="2" xr3:uid="{BB99DCDA-08D4-474A-ABC3-5229CEAF80CF}" name="id" dataDxfId="237">
       <calculatedColumnFormula>INT(MID(table_1_2[[#This Row],[library]], 4, 10))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{5F63B290-093A-48A3-9AFC-EB2FE27DE630}" name="library"/>
@@ -2687,44 +2635,44 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}" name="table_5_1" displayName="table_5_1" ref="A1:M41" totalsRowShown="0" headerRowDxfId="131">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}" name="table_5_1" displayName="table_5_1" ref="A1:M41" totalsRowShown="0" headerRowDxfId="134">
   <autoFilter ref="A1:M41" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
   <tableColumns count="13">
-    <tableColumn id="25" xr3:uid="{43F57146-0E56-46F3-A0E3-717A41010F4A}" name="index" dataDxfId="130"/>
-    <tableColumn id="1" xr3:uid="{B0B3F6B0-7577-49AC-B865-1E873B4DC53C}" name="dir" dataDxfId="129">
+    <tableColumn id="25" xr3:uid="{43F57146-0E56-46F3-A0E3-717A41010F4A}" name="index" dataDxfId="133"/>
+    <tableColumn id="1" xr3:uid="{B0B3F6B0-7577-49AC-B865-1E873B4DC53C}" name="dir" dataDxfId="132">
       <calculatedColumnFormula>table_3_1[[#This Row],[dir]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{D04F356F-9288-416D-ACDA-6BFE128B70D7}" name="control" dataDxfId="128">
+    <tableColumn id="13" xr3:uid="{D04F356F-9288-416D-ACDA-6BFE128B70D7}" name="control" dataDxfId="131">
       <calculatedColumnFormula>table_3_1[[#This Row],[control]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{9C168B22-F534-40D4-947C-918239C33FD9}" name="ref" dataDxfId="127">
+    <tableColumn id="2" xr3:uid="{9C168B22-F534-40D4-947C-918239C33FD9}" name="ref" dataDxfId="130">
       <calculatedColumnFormula>table_3_1[[#This Row],[ref]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{6F64477B-0C66-4251-9156-22307A6D70A0}" name="dsb_pos" dataDxfId="126">
+    <tableColumn id="3" xr3:uid="{6F64477B-0C66-4251-9156-22307A6D70A0}" name="dsb_pos" dataDxfId="129">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_pos]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{D037F4F2-543F-4D7D-AB36-0B253FD61B0D}" name="dsb_type" dataDxfId="125">
+    <tableColumn id="4" xr3:uid="{D037F4F2-543F-4D7D-AB36-0B253FD61B0D}" name="dsb_type" dataDxfId="128">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_type]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{407AC5E6-13CB-409A-8E78-64B8CC121882}" name="dsb_type_command" dataDxfId="124">
+    <tableColumn id="12" xr3:uid="{407AC5E6-13CB-409A-8E78-64B8CC121882}" name="dsb_type_command" dataDxfId="127">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_type_command]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{1A24C844-2A10-4394-818F-0C25A569B414}" name="strand" dataDxfId="123">
+    <tableColumn id="5" xr3:uid="{1A24C844-2A10-4394-818F-0C25A569B414}" name="strand" dataDxfId="126">
       <calculatedColumnFormula>table_3_1[[#This Row],[strand]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{4F0A02F9-5555-489E-BA41-E3CBF81D1114}" name="hguide" dataDxfId="122">
+    <tableColumn id="6" xr3:uid="{4F0A02F9-5555-489E-BA41-E3CBF81D1114}" name="hguide" dataDxfId="125">
       <calculatedColumnFormula>table_3_1[[#This Row],[hguide]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FAE741F2-7C1B-41F2-8875-9F7A2EF40A54}" name="cell" dataDxfId="121">
+    <tableColumn id="7" xr3:uid="{FAE741F2-7C1B-41F2-8875-9F7A2EF40A54}" name="cell" dataDxfId="124">
       <calculatedColumnFormula>table_3_1[[#This Row],[cell]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{FE3ED128-2534-43D1-9244-11AB1FB57650}" name="treatment" dataDxfId="120">
+    <tableColumn id="8" xr3:uid="{FE3ED128-2534-43D1-9244-11AB1FB57650}" name="treatment" dataDxfId="123">
       <calculatedColumnFormula>table_3_1[[#This Row],[treatment]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{65ACBC9C-0EC8-4074-B310-05F4B70BFAD5}" name="subst_type" dataDxfId="119">
+    <tableColumn id="9" xr3:uid="{65ACBC9C-0EC8-4074-B310-05F4B70BFAD5}" name="subst_type" dataDxfId="122">
       <calculatedColumnFormula>"with"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{F80F6FB9-4F35-4819-8285-D77131C6EFCE}" name="command" dataDxfId="118">
+    <tableColumn id="10" xr3:uid="{F80F6FB9-4F35-4819-8285-D77131C6EFCE}" name="command" dataDxfId="121">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2737,40 +2685,40 @@
   <autoFilter ref="A43:M55" xr:uid="{D74A5276-1A50-4DA1-9131-9669404C8622}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{8AC09A63-4226-4C75-8801-68CF93C0F078}" name="index"/>
-    <tableColumn id="2" xr3:uid="{77584C42-D70C-48A4-979A-F4DEA0B31542}" name="dir" dataDxfId="117">
+    <tableColumn id="2" xr3:uid="{77584C42-D70C-48A4-979A-F4DEA0B31542}" name="dir" dataDxfId="120">
       <calculatedColumnFormula>table_3_2[[#This Row],[dir]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{483E3D73-4059-4B65-84EC-5DC4E7008F35}" name="control" dataDxfId="116">
+    <tableColumn id="3" xr3:uid="{483E3D73-4059-4B65-84EC-5DC4E7008F35}" name="control" dataDxfId="119">
       <calculatedColumnFormula>table_3_2[[#This Row],[control]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5859A8DB-4C52-4451-BBB6-C6BEBF497540}" name="ref" dataDxfId="115">
+    <tableColumn id="4" xr3:uid="{5859A8DB-4C52-4451-BBB6-C6BEBF497540}" name="ref" dataDxfId="118">
       <calculatedColumnFormula>table_3_2[[#This Row],[ref]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{06FC4099-C18C-436C-B1E6-9739B71C7F22}" name="dsb_pos" dataDxfId="114">
+    <tableColumn id="5" xr3:uid="{06FC4099-C18C-436C-B1E6-9739B71C7F22}" name="dsb_pos" dataDxfId="117">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_pos]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8F043A8E-C5E7-4596-AE13-3E495C6DB33E}" name="dsb_type" dataDxfId="113">
+    <tableColumn id="6" xr3:uid="{8F043A8E-C5E7-4596-AE13-3E495C6DB33E}" name="dsb_type" dataDxfId="116">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_type]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E2DB136E-6FA9-4095-8B91-F094974333AF}" name="dsb_type_command" dataDxfId="112">
+    <tableColumn id="7" xr3:uid="{E2DB136E-6FA9-4095-8B91-F094974333AF}" name="dsb_type_command" dataDxfId="115">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_type_command]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{55CDC54E-3E43-4365-B1C9-5359F747A157}" name="strand" dataDxfId="111">
+    <tableColumn id="8" xr3:uid="{55CDC54E-3E43-4365-B1C9-5359F747A157}" name="strand" dataDxfId="114">
       <calculatedColumnFormula>table_3_2[[#This Row],[strand]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{056BD8A0-CC40-4C61-9F22-EE7382045F66}" name="hguide" dataDxfId="110">
+    <tableColumn id="9" xr3:uid="{056BD8A0-CC40-4C61-9F22-EE7382045F66}" name="hguide" dataDxfId="113">
       <calculatedColumnFormula>table_3_2[[#This Row],[hguide]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{489E156D-888A-4DDC-BB23-A4721D588249}" name="cell" dataDxfId="109">
+    <tableColumn id="10" xr3:uid="{489E156D-888A-4DDC-BB23-A4721D588249}" name="cell" dataDxfId="112">
       <calculatedColumnFormula>table_3_2[[#This Row],[cell]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{0F1B5F9E-B10D-4258-9052-90BCDC89F0B0}" name="treatment" dataDxfId="108">
+    <tableColumn id="11" xr3:uid="{0F1B5F9E-B10D-4258-9052-90BCDC89F0B0}" name="treatment" dataDxfId="111">
       <calculatedColumnFormula>table_3_2[[#This Row],[treatment]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A2723EF6-80E8-4D8D-A6DC-7556C1996222}" name="subst_type" dataDxfId="107">
+    <tableColumn id="12" xr3:uid="{A2723EF6-80E8-4D8D-A6DC-7556C1996222}" name="subst_type" dataDxfId="110">
       <calculatedColumnFormula>"with"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{02531CCA-6CDE-42BA-80E3-31C0F97A3546}" name="command" dataDxfId="106">
+    <tableColumn id="13" xr3:uid="{02531CCA-6CDE-42BA-80E3-31C0F97A3546}" name="command" dataDxfId="109">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2779,65 +2727,65 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E39D37F2-5006-44FB-A873-CCC98F8BA522}" name="table_6_1" displayName="table_6_1" ref="A2:T8" totalsRowShown="0" headerRowDxfId="105" dataDxfId="104">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E39D37F2-5006-44FB-A873-CCC98F8BA522}" name="table_6_1" displayName="table_6_1" ref="A2:T8" totalsRowShown="0" headerRowDxfId="108" dataDxfId="107">
   <autoFilter ref="A2:T8" xr:uid="{E39D37F2-5006-44FB-A873-CCC98F8BA522}"/>
   <tableColumns count="20">
-    <tableColumn id="25" xr3:uid="{CD5CCC3B-8B5B-4C20-98D1-63A7E1FB075B}" name="index" dataDxfId="103"/>
-    <tableColumn id="18" xr3:uid="{A6E432BE-5846-48EE-948A-BE81A4E2B6F5}" name="dir_1" dataDxfId="102">
+    <tableColumn id="25" xr3:uid="{CD5CCC3B-8B5B-4C20-98D1-63A7E1FB075B}" name="index" dataDxfId="106"/>
+    <tableColumn id="18" xr3:uid="{A6E432BE-5846-48EE-948A-BE81A4E2B6F5}" name="dir_1" dataDxfId="105">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_1]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{A826EC7B-673B-4DCB-8792-35762AD6C5ED}" name="dir_2" dataDxfId="101">
+    <tableColumn id="17" xr3:uid="{A826EC7B-673B-4DCB-8792-35762AD6C5ED}" name="dir_2" dataDxfId="104">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_2]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{F6910118-048E-4746-9072-727F3B1847FE}" name="dir_3" dataDxfId="100">
+    <tableColumn id="16" xr3:uid="{F6910118-048E-4746-9072-727F3B1847FE}" name="dir_3" dataDxfId="103">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_3]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{0BBECB52-3A0A-4374-9C43-DA21C4CA365C}" name="dir_4" dataDxfId="99">
+    <tableColumn id="15" xr3:uid="{0BBECB52-3A0A-4374-9C43-DA21C4CA365C}" name="dir_4" dataDxfId="102">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_4]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{6E2A95BE-29B1-4454-9E5B-BED35BBC5239}" name="dir_5" dataDxfId="98">
+    <tableColumn id="14" xr3:uid="{6E2A95BE-29B1-4454-9E5B-BED35BBC5239}" name="dir_5" dataDxfId="101">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_5]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{4BDBAB17-9D30-4F82-92E5-FBABD10C580E}" name="dir_6" dataDxfId="97">
+    <tableColumn id="1" xr3:uid="{4BDBAB17-9D30-4F82-92E5-FBABD10C580E}" name="dir_6" dataDxfId="100">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_6]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{8377C5E1-81CB-41A4-9754-5BDCCCB5D946}" name="dir_7" dataDxfId="96">
+    <tableColumn id="21" xr3:uid="{8377C5E1-81CB-41A4-9754-5BDCCCB5D946}" name="dir_7" dataDxfId="99">
       <calculatedColumnFormula array="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_7]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{0BBDCF08-0538-454A-A8A3-33839702EB7D}" name="dir_8" dataDxfId="95">
+    <tableColumn id="23" xr3:uid="{0BBDCF08-0538-454A-A8A3-33839702EB7D}" name="dir_8" dataDxfId="98">
       <calculatedColumnFormula array="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_8]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{362AFBD7-D8FE-484B-A796-99C68A4873AF}" name="dir_9" dataDxfId="94">
+    <tableColumn id="24" xr3:uid="{362AFBD7-D8FE-484B-A796-99C68A4873AF}" name="dir_9" dataDxfId="97">
       <calculatedColumnFormula array="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_9]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{F8401415-A0F2-4302-B6F1-2F4769D22B7D}" name="dir_10" dataDxfId="93">
+    <tableColumn id="26" xr3:uid="{F8401415-A0F2-4302-B6F1-2F4769D22B7D}" name="dir_10" dataDxfId="96">
       <calculatedColumnFormula array="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_10]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{EB5FA985-8547-4A83-8A97-6BDBC99AFC75}" name="dir_11" dataDxfId="92">
+    <tableColumn id="27" xr3:uid="{EB5FA985-8547-4A83-8A97-6BDBC99AFC75}" name="dir_11" dataDxfId="95">
       <calculatedColumnFormula array="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_11]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{531860AE-4501-4DFE-ABC6-8AEC03CA2891}" name="dir_12" dataDxfId="91">
+    <tableColumn id="28" xr3:uid="{531860AE-4501-4DFE-ABC6-8AEC03CA2891}" name="dir_12" dataDxfId="94">
       <calculatedColumnFormula array="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_12]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{991CDA96-8100-4EC0-BA2D-509D87E3B77E}" name="control" dataDxfId="90">
+    <tableColumn id="13" xr3:uid="{991CDA96-8100-4EC0-BA2D-509D87E3B77E}" name="control" dataDxfId="93">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 6 * (table_6_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AB636280-F214-4141-A265-B2AC639CF4A7}" name="dsb_type" dataDxfId="89">
+    <tableColumn id="4" xr3:uid="{AB636280-F214-4141-A265-B2AC639CF4A7}" name="dsb_type" dataDxfId="92">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], 6 * (table_6_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{56C39C59-71CD-4F29-9AA2-7C1BE588DDCF}" name="strand" dataDxfId="88">
+    <tableColumn id="5" xr3:uid="{56C39C59-71CD-4F29-9AA2-7C1BE588DDCF}" name="strand" dataDxfId="91">
       <calculatedColumnFormula>OFFSET(table_3_1[strand], 6 * (table_6_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{77B8B06C-E91A-4366-BAAD-4D98914358E6}" name="hguide" dataDxfId="87">
+    <tableColumn id="6" xr3:uid="{77B8B06C-E91A-4366-BAAD-4D98914358E6}" name="hguide" dataDxfId="90">
       <calculatedColumnFormula>OFFSET(table_3_1[hguide], 6 * (table_6_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{64A9E7E6-7F9F-4F61-9A23-E4157ABDCFAC}" name="subst_type" dataDxfId="86">
+    <tableColumn id="9" xr3:uid="{64A9E7E6-7F9F-4F61-9A23-E4157ABDCFAC}" name="subst_type" dataDxfId="89">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{B53E652A-5D37-4D63-8F38-4B8DBDB37226}" name="dir_out" dataDxfId="85">
+    <tableColumn id="19" xr3:uid="{B53E652A-5D37-4D63-8F38-4B8DBDB37226}" name="dir_out" dataDxfId="88">
       <calculatedColumnFormula>_xlfn.CONCAT(table_6_1[[#This Row],[dsb_type]], "_", table_6_1[[#This Row],[strand]], IF(table_6_1[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_1[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{9C3C4C97-49A2-40B9-BCC3-5739C07213CD}" name="command" dataDxfId="84">
+    <tableColumn id="10" xr3:uid="{9C3C4C97-49A2-40B9-BCC3-5739C07213CD}" name="command" dataDxfId="87">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", _xlfn.TEXTJOIN(" ", TRUE, table_6_1[[#This Row],[dir_1]:[dir_12]]), " -o ", layouts, "/", table_6_1[[#This Row],[dir_out]], " --subst_type ", table_6_1[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2846,35 +2794,35 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{5FFA4758-C47A-4F1C-9890-69E7F39BE130}" name="table_6_2" displayName="table_6_2" ref="A11:J13" totalsRowShown="0" headerRowDxfId="83" dataDxfId="81" headerRowBorderDxfId="82" tableBorderDxfId="80">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{5FFA4758-C47A-4F1C-9890-69E7F39BE130}" name="table_6_2" displayName="table_6_2" ref="A11:J13" totalsRowShown="0" headerRowDxfId="86" dataDxfId="84" headerRowBorderDxfId="85" tableBorderDxfId="83">
   <autoFilter ref="A11:J13" xr:uid="{5FFA4758-C47A-4F1C-9890-69E7F39BE130}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{40A0667B-C93C-4531-B41F-A65EDE89F51E}" name="index" dataDxfId="79"/>
-    <tableColumn id="2" xr3:uid="{A54C9A1D-E384-4C87-B6DD-98A7ADBAD240}" name="dir_1" dataDxfId="78">
+    <tableColumn id="1" xr3:uid="{40A0667B-C93C-4531-B41F-A65EDE89F51E}" name="index" dataDxfId="82"/>
+    <tableColumn id="2" xr3:uid="{A54C9A1D-E384-4C87-B6DD-98A7ADBAD240}" name="dir_1" dataDxfId="81">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset  + COLUMN() - 2 + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{7CACC7DC-6834-41E4-A17F-74F62473FF4D}" name="dir_2" dataDxfId="77">
+    <tableColumn id="3" xr3:uid="{7CACC7DC-6834-41E4-A17F-74F62473FF4D}" name="dir_2" dataDxfId="80">
       <calculatedColumnFormula array="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset + COLUMN() - 2 + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{BEB4CA3E-14C3-4D70-BAFF-DBFFE398E04E}" name="control" dataDxfId="76">
+    <tableColumn id="4" xr3:uid="{BEB4CA3E-14C3-4D70-BAFF-DBFFE398E04E}" name="control" dataDxfId="79">
       <calculatedColumnFormula>OFFSET(table_3_1[control], var_6_anti_offset  + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{08F18E8F-5127-4F55-95E0-05877340A45E}" name="dsb_type" dataDxfId="75">
+    <tableColumn id="5" xr3:uid="{08F18E8F-5127-4F55-95E0-05877340A45E}" name="dsb_type" dataDxfId="78">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], var_6_anti_offset  + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B0010190-2798-4D5F-A1DA-8D1F1A867502}" name="strand" dataDxfId="74">
+    <tableColumn id="6" xr3:uid="{B0010190-2798-4D5F-A1DA-8D1F1A867502}" name="strand" dataDxfId="77">
       <calculatedColumnFormula array="1">OFFSET(table_3_1[strand], var_6_anti_offset  + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{689C42CC-8508-4116-808A-19A0641C3F05}" name="hguide" dataDxfId="73">
+    <tableColumn id="7" xr3:uid="{689C42CC-8508-4116-808A-19A0641C3F05}" name="hguide" dataDxfId="76">
       <calculatedColumnFormula>OFFSET(table_3_1[hguide], var_6_anti_offset + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{48005280-1CD9-4496-941A-723AEDDD9036}" name="subst_type" dataDxfId="72">
+    <tableColumn id="8" xr3:uid="{48005280-1CD9-4496-941A-723AEDDD9036}" name="subst_type" dataDxfId="75">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{5F8C6AF1-A602-4306-A909-592B4268C611}" name="dir_out" dataDxfId="71">
+    <tableColumn id="9" xr3:uid="{5F8C6AF1-A602-4306-A909-592B4268C611}" name="dir_out" dataDxfId="74">
       <calculatedColumnFormula>_xlfn.CONCAT(table_6_2[[#This Row],[dsb_type]], "_", table_6_2[[#This Row],[strand]], IF(table_6_2[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_2[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{3AEE0650-E928-4CB1-8CCF-22F967A16636}" name="command" dataDxfId="70">
+    <tableColumn id="10" xr3:uid="{3AEE0650-E928-4CB1-8CCF-22F967A16636}" name="command" dataDxfId="73">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", _xlfn.TEXTJOIN(" ", TRUE, table_6_2[[#This Row],[dir_1]:[dir_2]]), " -o ", layouts, "/", table_6_2[[#This Row],[dir_out]], " --subst_type ", table_6_2[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2883,36 +2831,36 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}" name="table_6_3" displayName="table_6_3" ref="A15:I16" totalsRowShown="0" headerRowDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}" name="table_6_3" displayName="table_6_3" ref="A15:I16" totalsRowShown="0" headerRowDxfId="72">
   <autoFilter ref="A15:I16" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}"/>
   <tableColumns count="9">
-    <tableColumn id="25" xr3:uid="{D7EEB429-5A34-4903-8247-E1BD5C0098AE}" name="index" dataDxfId="68"/>
-    <tableColumn id="18" xr3:uid="{BACD6182-9E09-4A02-A171-8DFCB7543380}" name="dir" dataDxfId="67">
+    <tableColumn id="25" xr3:uid="{D7EEB429-5A34-4903-8247-E1BD5C0098AE}" name="index" dataDxfId="71"/>
+    <tableColumn id="18" xr3:uid="{BACD6182-9E09-4A02-A171-8DFCB7543380}" name="dir" dataDxfId="70">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 12, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{39C35B5A-7D06-4895-BF0F-A803A5F94E2E}" name="reverse_complement" dataDxfId="66">
+    <tableColumn id="2" xr3:uid="{39C35B5A-7D06-4895-BF0F-A803A5F94E2E}" name="reverse_complement" dataDxfId="69">
       <calculatedColumnFormula array="1">_xlfn.TEXTJOIN(
   " ",
   TRUE,
   IF(OFFSET(table_3_1[[strand]:[strand]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 12, 1) = "R1", 0, 1)
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{F617BC3E-90A8-4E63-B2A4-EAC9DE705FC7}" name="control" dataDxfId="65">
+    <tableColumn id="13" xr3:uid="{F617BC3E-90A8-4E63-B2A4-EAC9DE705FC7}" name="control" dataDxfId="68">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 6 * (table_6_3[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{8E20D9FC-49B1-428A-AC5E-AEDADB1473AC}" name="dsb_type" dataDxfId="64">
+    <tableColumn id="4" xr3:uid="{8E20D9FC-49B1-428A-AC5E-AEDADB1473AC}" name="dsb_type" dataDxfId="67">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], 12 * (table_6_3[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="33" xr3:uid="{8FF7E83A-9135-4A64-965C-48368A6C0367}" name="hguide">
       <calculatedColumnFormula array="1">OFFSET(table_3_1[[hguide]:[hguide]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{FB278FFE-A956-4B0C-8CC3-6A0324CBCA11}" name="subst_type" dataDxfId="63">
+    <tableColumn id="9" xr3:uid="{FB278FFE-A956-4B0C-8CC3-6A0324CBCA11}" name="subst_type" dataDxfId="66">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{E4089767-2E77-4296-9392-7BCD64E1E62D}" name="dir_out" dataDxfId="62">
+    <tableColumn id="19" xr3:uid="{E4089767-2E77-4296-9392-7BCD64E1E62D}" name="dir_out" dataDxfId="65">
       <calculatedColumnFormula>_xlfn.CONCAT(table_6_3[[#This Row],[dsb_type]], "_", table_6_3[[#This Row],[hguide]], IF(table_6_3[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_3[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{8BD09F85-30B0-46CA-A0E3-2CC4F3FB2BD0}" name="command" dataDxfId="61">
+    <tableColumn id="10" xr3:uid="{8BD09F85-30B0-46CA-A0E3-2CC4F3FB2BD0}" name="command" dataDxfId="64">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_3[[#This Row],[dir]], IF(NOT(ISNA(table_6_3[[#This Row],[reverse_complement]])), _xlfn.CONCAT(" -rc ", table_6_3[[#This Row],[reverse_complement]]), ""), " -o ", layouts, "/", table_6_3[[#This Row],[dir_out]], " --subst_type ", table_6_3[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2921,32 +2869,32 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}" name="table_6_4" displayName="table_6_4" ref="A19:I21" totalsRowShown="0" headerRowDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}" name="table_6_4" displayName="table_6_4" ref="A19:I21" totalsRowShown="0" headerRowDxfId="63">
   <autoFilter ref="A19:I21" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}"/>
   <tableColumns count="9">
-    <tableColumn id="25" xr3:uid="{4FA5A2E4-C9F7-4673-98E1-BCCE618B100D}" name="index" dataDxfId="59"/>
-    <tableColumn id="18" xr3:uid="{155653FE-38BD-4542-A5AE-2B40B0FD52C7}" name="dir" dataDxfId="58">
+    <tableColumn id="25" xr3:uid="{4FA5A2E4-C9F7-4673-98E1-BCCE618B100D}" name="index" dataDxfId="62"/>
+    <tableColumn id="18" xr3:uid="{155653FE-38BD-4542-A5AE-2B40B0FD52C7}" name="dir" dataDxfId="61">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 6, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{05E960C2-864E-41C3-A84E-DF767C09AA42}" name="strand" dataDxfId="57">
+    <tableColumn id="34" xr3:uid="{05E960C2-864E-41C3-A84E-DF767C09AA42}" name="strand" dataDxfId="60">
       <calculatedColumnFormula>NA()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{9EA58FA8-5496-4600-905A-95909513339B}" name="control" dataDxfId="56">
+    <tableColumn id="13" xr3:uid="{9EA58FA8-5496-4600-905A-95909513339B}" name="control" dataDxfId="59">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 6 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{46390A5F-98AD-4211-85B4-A4DD8E31C40C}" name="dsb_type" dataDxfId="55">
+    <tableColumn id="4" xr3:uid="{46390A5F-98AD-4211-85B4-A4DD8E31C40C}" name="dsb_type" dataDxfId="58">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="35" xr3:uid="{5BD83012-469D-4202-9584-AA182CDF11F9}" name="hguide">
       <calculatedColumnFormula array="1">OFFSET(table_3_1[[hguide]:[hguide]], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{123049FA-F284-452C-8FDD-63F409D9967F}" name="subst_type" dataDxfId="54">
+    <tableColumn id="9" xr3:uid="{123049FA-F284-452C-8FDD-63F409D9967F}" name="subst_type" dataDxfId="57">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{CFCDDB26-095C-4395-82E2-37B45B0CDEAD}" name="dir_out" dataDxfId="53">
+    <tableColumn id="19" xr3:uid="{CFCDDB26-095C-4395-82E2-37B45B0CDEAD}" name="dir_out" dataDxfId="56">
       <calculatedColumnFormula>_xlfn.CONCAT(table_6_4[[#This Row],[dsb_type]], "_", table_6_4[[#This Row],[hguide]], IF(table_6_4[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_4[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{DC6C9CBA-5796-4FFE-878D-BB47DC276187}" name="command" dataDxfId="2">
+    <tableColumn id="10" xr3:uid="{DC6C9CBA-5796-4FFE-878D-BB47DC276187}" name="command" dataDxfId="15">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_4[[#This Row],[dir]], IF(NOT(ISNA(table_6_4[[#This Row],[strand]])), _xlfn.CONCAT(" -rc ", table_6_4[[#This Row],[strand]]), ""), " -o ", layouts, "/", table_6_4[[#This Row],[dir_out]], " --subst_type ", table_6_4[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2955,36 +2903,36 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}" name="table_6_5" displayName="table_6_5" ref="A23:I24" totalsRowShown="0" headerRowDxfId="52" headerRowBorderDxfId="51" tableBorderDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}" name="table_6_5" displayName="table_6_5" ref="A23:I24" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53">
   <autoFilter ref="A23:I24" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{0F421990-E775-4F35-92AF-6BA19E0E8AEE}" name="index"/>
-    <tableColumn id="2" xr3:uid="{81FE7256-F482-4A2C-902D-871C80C1D881}" name="dir" dataDxfId="49">
+    <tableColumn id="2" xr3:uid="{81FE7256-F482-4A2C-902D-871C80C1D881}" name="dir" dataDxfId="52">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]:[index]] - 1), 0, 4, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E9F8E6A0-B4A7-475B-9ED2-9F2A4A9EB628}" name="strand" dataDxfId="48">
+    <tableColumn id="3" xr3:uid="{E9F8E6A0-B4A7-475B-9ED2-9F2A4A9EB628}" name="strand" dataDxfId="51">
       <calculatedColumnFormula array="1">_xlfn.TEXTJOIN(
   " ",
   TRUE,
   IF(OFFSET(table_3_1[[strand]:[strand]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]:[index]] - 1), 0,4, 1) = "R1", 0, 1)
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{70821CEE-FFC4-44AB-ACF6-DA81A4B053E6}" name="control" dataDxfId="47">
+    <tableColumn id="6" xr3:uid="{70821CEE-FFC4-44AB-ACF6-DA81A4B053E6}" name="control" dataDxfId="50">
       <calculatedColumnFormula>OFFSET(table_3_1[control], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{FA9180EA-3AA0-451A-ACAC-78776C7CB75D}" name="dsb_type" dataDxfId="46">
+    <tableColumn id="5" xr3:uid="{FA9180EA-3AA0-451A-ACAC-78776C7CB75D}" name="dsb_type" dataDxfId="49">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{E0783723-9246-4BF6-A5DA-E000EA1E5E87}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DE820E4E-FF8B-435B-B07F-D397029AF597}" name="hguide" dataDxfId="45">
+    <tableColumn id="4" xr3:uid="{DE820E4E-FF8B-435B-B07F-D397029AF597}" name="hguide" dataDxfId="48">
       <calculatedColumnFormula>OFFSET(table_3_1[[hguide]:[hguide]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{3D97DBDD-03E9-4A6C-BADA-D01B27A8EE51}" name="dir_out" dataDxfId="44">
+    <tableColumn id="9" xr3:uid="{3D97DBDD-03E9-4A6C-BADA-D01B27A8EE51}" name="dir_out" dataDxfId="47">
       <calculatedColumnFormula>_xlfn.CONCAT(table_6_5[[#This Row],[dsb_type]], "_", table_6_5[[#This Row],[hguide]], IF(table_6_5[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_5[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5E7626AE-E376-4C60-BA64-B24F95580083}" name="command" dataDxfId="43">
+    <tableColumn id="10" xr3:uid="{5E7626AE-E376-4C60-BA64-B24F95580083}" name="command" dataDxfId="46">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_5[[#This Row],[dir]], " -rc ", table_6_5[[#This Row],[strand]], " -o ", layouts, "/", table_6_5[[#This Row],[dir_out]], " --subst_type ", table_6_5[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2993,44 +2941,44 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{86CE8E4A-18BF-427A-81F0-F9655767A016}" name="table_7_1" displayName="table_7_1" ref="A2:N42" totalsRowShown="0" headerRowDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{86CE8E4A-18BF-427A-81F0-F9655767A016}" name="table_7_1" displayName="table_7_1" ref="A2:N42" totalsRowShown="0" headerRowDxfId="45">
   <autoFilter ref="A2:N42" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
   <tableColumns count="14">
-    <tableColumn id="25" xr3:uid="{C323C376-24D3-4404-9E0F-6E9361862271}" name="index" dataDxfId="41"/>
-    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="40">
+    <tableColumn id="25" xr3:uid="{C323C376-24D3-4404-9E0F-6E9361862271}" name="index" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="43">
       <calculatedColumnFormula>OFFSET(table_3_1[[dir]:[dir]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="39">
+    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="42">
       <calculatedColumnFormula>OFFSET(table_3_1[[control]:[control]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="38">
+    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="41">
       <calculatedColumnFormula>OFFSET(table_3_1[[ref]:[ref]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="37">
+    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="40">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_pos]:[dsb_pos]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="36">
+    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="39">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_type]:[dsb_type]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="35">
+    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="38">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_type_command]:[dsb_type_command]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="34">
+    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="37">
       <calculatedColumnFormula>OFFSET(table_3_1[[strand]:[strand]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="33">
+    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="36">
       <calculatedColumnFormula>OFFSET(table_3_1[[hguide]:[hguide]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="32">
+    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="35">
       <calculatedColumnFormula>OFFSET(table_3_1[[cell]:[cell]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="31">
+    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="34">
       <calculatedColumnFormula>OFFSET(table_3_1[[treatment]:[treatment]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="30">
+    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="33">
       <calculatedColumnFormula>"without"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="0">
+    <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="13">
       <calculatedColumnFormula>IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
       OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
       IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
@@ -3042,7 +2990,7 @@
       )
   )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="1">
+    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="14">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_1[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3054,44 +3002,44 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{B47D9508-D874-40FC-B6F6-C106B48F6A94}" name="table_7_2" displayName="table_7_2" ref="A44:N56" totalsRowShown="0">
   <autoFilter ref="A44:N56" xr:uid="{D74A5276-1A50-4DA1-9131-9669404C8622}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{488C5146-A746-4F74-BCC8-806E4DC740CE}" name="index" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{C2A88DF4-2444-4C4C-A089-6CF9ADE79BD8}" name="dir" dataDxfId="28">
+    <tableColumn id="1" xr3:uid="{488C5146-A746-4F74-BCC8-806E4DC740CE}" name="index" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{C2A88DF4-2444-4C4C-A089-6CF9ADE79BD8}" name="dir" dataDxfId="31">
       <calculatedColumnFormula>OFFSET(table_3_2[[dir]:[dir]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{7698ACE3-2351-400D-B00F-5A70184F8A33}" name="control" dataDxfId="27">
+    <tableColumn id="3" xr3:uid="{7698ACE3-2351-400D-B00F-5A70184F8A33}" name="control" dataDxfId="30">
       <calculatedColumnFormula>OFFSET(table_3_2[[control]:[control]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5E82B04C-FF09-492C-8A23-7E43B5990149}" name="ref" dataDxfId="26">
+    <tableColumn id="4" xr3:uid="{5E82B04C-FF09-492C-8A23-7E43B5990149}" name="ref" dataDxfId="29">
       <calculatedColumnFormula>OFFSET(table_3_2[[ref]:[ref]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{F4D36A0E-549B-4F3A-BCA9-75E151448998}" name="dsb_pos" dataDxfId="25">
+    <tableColumn id="5" xr3:uid="{F4D36A0E-549B-4F3A-BCA9-75E151448998}" name="dsb_pos" dataDxfId="28">
       <calculatedColumnFormula>OFFSET(table_3_2[[dsb_pos]:[dsb_pos]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{AEBBBB88-8CE2-409D-AE19-9C23263250A9}" name="dsb_type" dataDxfId="24">
+    <tableColumn id="6" xr3:uid="{AEBBBB88-8CE2-409D-AE19-9C23263250A9}" name="dsb_type" dataDxfId="27">
       <calculatedColumnFormula>OFFSET(table_3_2[[dsb_type]:[dsb_type]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3E71E7D2-0FA5-4FD5-BDC3-2955A091A9E6}" name="dsb_type_command" dataDxfId="23">
+    <tableColumn id="7" xr3:uid="{3E71E7D2-0FA5-4FD5-BDC3-2955A091A9E6}" name="dsb_type_command" dataDxfId="26">
       <calculatedColumnFormula>OFFSET(table_3_2[[dsb_type_command]:[dsb_type_command]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{EBD35881-E696-4202-9149-75A4EFFFAAD6}" name="strand" dataDxfId="22">
+    <tableColumn id="8" xr3:uid="{EBD35881-E696-4202-9149-75A4EFFFAAD6}" name="strand" dataDxfId="25">
       <calculatedColumnFormula>OFFSET(table_3_2[[strand]:[strand]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{123CA279-0CB6-41C1-9CD8-20D375B9B66D}" name="hguide" dataDxfId="21">
+    <tableColumn id="9" xr3:uid="{123CA279-0CB6-41C1-9CD8-20D375B9B66D}" name="hguide" dataDxfId="24">
       <calculatedColumnFormula>OFFSET(table_3_2[[hguide]:[hguide]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{3DCE3F3A-187D-411E-93FC-8C6C3EE9CAA2}" name="cell" dataDxfId="20">
+    <tableColumn id="10" xr3:uid="{3DCE3F3A-187D-411E-93FC-8C6C3EE9CAA2}" name="cell" dataDxfId="23">
       <calculatedColumnFormula>OFFSET(table_3_2[[cell]:[cell]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{9E585D29-AB3E-4D04-8C1D-24F78339C9A3}" name="treatment" dataDxfId="19">
+    <tableColumn id="11" xr3:uid="{9E585D29-AB3E-4D04-8C1D-24F78339C9A3}" name="treatment" dataDxfId="22">
       <calculatedColumnFormula>OFFSET(table_3_2[[treatment]:[treatment]], table_7_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{928286B8-23FB-4375-B52B-617DD59D6098}" name="subst_type" dataDxfId="18">
+    <tableColumn id="12" xr3:uid="{928286B8-23FB-4375-B52B-617DD59D6098}" name="subst_type" dataDxfId="21">
       <calculatedColumnFormula>"without"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{E18D2025-56E8-4128-9201-9E0BF8A67AC0}" name="common_layout_dir" dataDxfId="17">
+    <tableColumn id="15" xr3:uid="{E18D2025-56E8-4128-9201-9E0BF8A67AC0}" name="common_layout_dir" dataDxfId="20">
       <calculatedColumnFormula>OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_2[[#This Row],[index]] - 1, 6) + 2, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{0917AB98-1545-4642-9BE8-618AAA1E404A}" name="command" dataDxfId="16">
+    <tableColumn id="13" xr3:uid="{0917AB98-1545-4642-9BE8-618AAA1E404A}" name="command" dataDxfId="19">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3100,15 +3048,27 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{B76EEC45-4FC3-44D5-9B2E-9183DF724F60}" name="table_7_3" displayName="table_7_3" ref="A3:C19" totalsRowShown="0" headerRowDxfId="15">
-  <autoFilter ref="A3:C19" xr:uid="{B76EEC45-4FC3-44D5-9B2E-9183DF724F60}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{FAFADB73-BF3B-401A-8C48-9FCB5D3C4CB6}" name="index" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{8541A14E-3250-4B9C-B315-969FC11BE60A}" name="dir" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{B76EEC45-4FC3-44D5-9B2E-9183DF724F60}" name="table_7_3" displayName="table_7_3" ref="A1:G17" totalsRowShown="0" headerRowDxfId="18">
+  <autoFilter ref="A1:G17" xr:uid="{B76EEC45-4FC3-44D5-9B2E-9183DF724F60}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{FAFADB73-BF3B-401A-8C48-9FCB5D3C4CB6}" name="index" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{8541A14E-3250-4B9C-B315-969FC11BE60A}" name="dir" dataDxfId="16">
       <calculatedColumnFormula>OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{EAD6D5EC-B61E-4A98-B4FD-4932757CFEA3}" name="command" dataDxfId="12">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{627FA44D-7936-4906-80A6-6ABAA9A96C24}" name="strand" dataDxfId="11">
+      <calculatedColumnFormula>OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{D23E086E-5C74-4A74-98A1-113456947567}" name="hguide" dataDxfId="10">
+      <calculatedColumnFormula>OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{9CE51D1A-4478-4FC1-B156-568596E4C385}" name="dsb_type" dataDxfId="9">
+      <calculatedColumnFormula>OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{E2BCDA0F-EDF0-4576-A173-675A35AE49D2}" name="common_layout_dir" dataDxfId="12">
+      <calculatedColumnFormula>OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{EAD6D5EC-B61E-4A98-B4FD-4932757CFEA3}" name="command" dataDxfId="8">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_3[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_3[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3116,10 +3076,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22A90416-B904-4D3D-A6DB-EFCB9FD1EAED}" name="table_1" displayName="table_1" ref="A1:O173" totalsRowShown="0" headerRowDxfId="233">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22A90416-B904-4D3D-A6DB-EFCB9FD1EAED}" name="table_1" displayName="table_1" ref="A1:O173" totalsRowShown="0" headerRowDxfId="236">
   <autoFilter ref="A1:O173" xr:uid="{22A90416-B904-4D3D-A6DB-EFCB9FD1EAED}"/>
   <tableColumns count="15">
-    <tableColumn id="15" xr3:uid="{A06DA701-31D6-44A5-8655-82CAD7E3082B}" name="index" dataDxfId="232"/>
+    <tableColumn id="15" xr3:uid="{A06DA701-31D6-44A5-8655-82CAD7E3082B}" name="index" dataDxfId="235"/>
     <tableColumn id="1" xr3:uid="{5C1CDEE9-AAC7-4E12-B88F-1314CF422335}" name="library"/>
     <tableColumn id="2" xr3:uid="{D4B174CF-F774-4DA7-B75D-573BC94EE10F}" name="cell"/>
     <tableColumn id="3" xr3:uid="{83898EC9-96DA-46D4-B0B8-F68C7607DCF2}" name="control"/>
@@ -3127,25 +3087,25 @@
     <tableColumn id="5" xr3:uid="{81A143FE-8E74-4182-8124-E697DD5A7C62}" name="hguide"/>
     <tableColumn id="6" xr3:uid="{4A316E6A-69F3-4B78-9C01-4675AEB656FA}" name="treatment"/>
     <tableColumn id="7" xr3:uid="{25B8E763-346D-4756-8B58-D3C8CB103545}" name="strand"/>
-    <tableColumn id="8" xr3:uid="{4B708639-BB19-4DC1-A57D-214FA0EFB1EA}" name="dsb_pos" dataDxfId="231">
+    <tableColumn id="8" xr3:uid="{4B708639-BB19-4DC1-A57D-214FA0EFB1EA}" name="dsb_pos" dataDxfId="234">
       <calculatedColumnFormula array="1">IF(E2="2DSB", IF(H2="R1", 67, 46), IF(E2="1DSB", IF(H2="R1", 67, 46), IF(E2="2DSBanti", IF(H2="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{CCF6021C-1B60-4954-A92E-3F2848564215}" name="file_in" dataDxfId="230">
+    <tableColumn id="9" xr3:uid="{CCF6021C-1B60-4954-A92E-3F2848564215}" name="file_in" dataDxfId="233">
       <calculatedColumnFormula>IF(OR(table_1[[#This Row],[control]]="none", table_1[[#This Row],[control]]="30bpDown"), _xlfn.CONCAT(table_1[[#This Row],[library]], IF(table_1[[#This Row],[dsb_type]] = "2DSBanti", "_anti", ""), "_",table_1[[#This Row],[strand]],"_", IF(LEFT(table_1[[#This Row],[dsb_type]], 1)="2","2DSBs", table_1[[#This Row],[hguide]]), ".sam"), _xlfn.CONCAT(table_1[[#This Row],[library]], "_NHEJ_", IF(table_1[[#This Row],[hguide]]="sgA", "hg39", IF(table_1[[#This Row],[hguide]]="sgB", "hg42", "2DSB")), "_", table_1[[#This Row],[strand]], ".sam"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{58220462-2A11-4DAD-A247-C0871AFCFDB4}" name="file_out" dataDxfId="229">
+    <tableColumn id="10" xr3:uid="{58220462-2A11-4DAD-A247-C0871AFCFDB4}" name="file_out" dataDxfId="232">
       <calculatedColumnFormula>_xlfn.CONCAT(table_1[[#This Row],[library]], "_", table_1[[#This Row],[cell]], "_", table_1[[#This Row],[hguide]], "_", table_1[[#This Row],[strand]], "_", table_1[[#This Row],[treatment]], IF(table_1[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_1[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{775EE7A9-3C78-4568-BF98-500DE451177C}" name="ref" dataDxfId="228">
+    <tableColumn id="11" xr3:uid="{775EE7A9-3C78-4568-BF98-500DE451177C}" name="ref" dataDxfId="231">
       <calculatedColumnFormula>_xlfn.CONCAT(table_1[[#This Row],[dsb_type]],"_", table_1[[#This Row],[strand]],"_", table_1[[#This Row],[treatment]], ".fa")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{5B945FB6-D054-40C4-AAEF-BB50B19F8936}" name="total_reads" dataDxfId="227">
+    <tableColumn id="12" xr3:uid="{5B945FB6-D054-40C4-AAEF-BB50B19F8936}" name="total_reads" dataDxfId="230">
       <calculatedColumnFormula>VLOOKUP(INT(MID(table_1[[#This Row],[library]], 4, 10)), table_1_2[#All], IF(table_1[[#This Row],[strand]]="R1", 3, 4))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{66485B06-471E-47D3-BA91-FC751F58FA5A}" name="min_length" dataDxfId="226">
+    <tableColumn id="13" xr3:uid="{66485B06-471E-47D3-BA91-FC751F58FA5A}" name="min_length" dataDxfId="229">
       <calculatedColumnFormula>IF(LEFT(table_1[[#This Row],[dsb_type]], 1) = "2", 50, 130)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{DF3C46EA-690D-4E6A-99CF-BBC2B2F74AFF}" name="command_filter_nhej" dataDxfId="225">
+    <tableColumn id="14" xr3:uid="{DF3C46EA-690D-4E6A-99CF-BBC2B2F74AFF}" name="command_filter_nhej" dataDxfId="228">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", table_1[[#This Row],[file_in]], " -ref ref_seq/", table_1[[#This Row],[ref]], " -o ", libraries_2, "/", table_1[[#This Row],[file_out]], ".tsv", " --min_length ", table_1[[#This Row],[min_length]], " -dsb ", table_1[[#This Row],[dsb_pos]], " --quiet")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3154,31 +3114,27 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{8B4E853A-A4F1-4022-B857-226C57559A5F}" name="table_7_4" displayName="table_7_4" ref="A21:C23" totalsRowShown="0" headerRowDxfId="11">
-  <autoFilter ref="A21:C23" xr:uid="{8B4E853A-A4F1-4022-B857-226C57559A5F}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{1ECF32A2-E353-4754-B4C5-11C46AACF6C0}" name="index" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{181C59FC-364D-4421-8E54-98DFF4CA7C05}" name="dir" dataDxfId="9">
-      <calculatedColumnFormula>OFFSET(table_4_2[[dir_out]:[dir_out]], table_7_4[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{1EF3A7F2-091F-42AE-91CA-D18AA0FD8430}" name="table_7_39" displayName="table_7_39" ref="A19:G21" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A19:G21" xr:uid="{1EF3A7F2-091F-42AE-91CA-D18AA0FD8430}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{D25401DE-9587-4D52-A7E4-1182AFAAC5F6}" name="index" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{D669EE3E-402E-4224-BA98-DE9E0722137B}" name="dir" dataDxfId="4">
+      <calculatedColumnFormula>OFFSET(table_4_2[], table_7_39[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{6D8CC942-572B-44F2-BCA6-4D31A25A4067}" name="command" dataDxfId="8">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_4[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_2[[dir_out]:[dir_out]],table_7_4[[#This Row],[index]] - 1, 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{2B75E3A0-0699-4170-8EC2-74B07D76FA5F}" name="strand" dataDxfId="3">
+      <calculatedColumnFormula>OFFSET(table_7_1[[strand]:[strand]], 37 + 2 * QUOTIENT(table_7_39[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{58F5EC27-BD76-45AE-8D38-F4E705EF79E9}" name="table_7_5" displayName="table_7_5" ref="A26:C34" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A26:C34" xr:uid="{58F5EC27-BD76-45AE-8D38-F4E705EF79E9}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{AAC1476C-44CE-49FD-8254-50BAEAA6929C}" name="index" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{1222E48F-ED5C-48AA-BA39-1443B841BC9F}" name="dir" dataDxfId="4">
-      <calculatedColumnFormula>OFFSET(table_4_3[[dir_out]:[dir_out]], table_7_5[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{E4B22932-5A45-4536-9287-472A2DAB716B}" name="hguide" dataDxfId="2">
+      <calculatedColumnFormula>OFFSET(table_7_1[[hguide]:[hguide]], 37 + 2 * QUOTIENT(table_7_39[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{89B7E589-2097-43FC-B96B-19D2EF777E97}" name="command" dataDxfId="3">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</calculatedColumnFormula>
+    <tableColumn id="7" xr3:uid="{B62FF923-C030-49D9-971F-232E1B61FD42}" name="dsb_type" dataDxfId="1">
+      <calculatedColumnFormula>OFFSET(table_7_1[[dsb_type]:[dsb_type]], 37 + 2 * QUOTIENT(table_7_39[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{F6CF1684-EFBE-4FE3-B11C-E53417FDF011}" name="common_layout_dir" dataDxfId="0">
+      <calculatedColumnFormula>OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 37 + 2 * QUOTIENT(table_7_39[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{7C0FCF3E-3C81-4367-967B-F1ACE83A43C9}" name="command" dataDxfId="5">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_39[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_39[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_39[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_39[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3186,38 +3142,38 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}" name="table_2_1" displayName="table_2_1" ref="A1:S41" totalsRowShown="0" headerRowDxfId="224">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}" name="table_2_1" displayName="table_2_1" ref="A1:S41" totalsRowShown="0" headerRowDxfId="227">
   <autoFilter ref="A1:S41" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{C373869E-A92E-4B06-B8E5-C5A873420ED4}" name="index" dataDxfId="223"/>
-    <tableColumn id="2" xr3:uid="{A28AAC50-FA09-494A-B052-8489F07A5A70}" name="ref" dataDxfId="222">
+    <tableColumn id="1" xr3:uid="{C373869E-A92E-4B06-B8E5-C5A873420ED4}" name="index" dataDxfId="226"/>
+    <tableColumn id="2" xr3:uid="{A28AAC50-FA09-494A-B052-8489F07A5A70}" name="ref" dataDxfId="225">
       <calculatedColumnFormula>OFFSET(table_1[ref], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{07D57089-9737-4983-8884-C4ACCDCFF6CB}" name="control" dataDxfId="221">
+    <tableColumn id="18" xr3:uid="{07D57089-9737-4983-8884-C4ACCDCFF6CB}" name="control" dataDxfId="224">
       <calculatedColumnFormula>OFFSET(table_1[control], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{C6423FEA-272F-48D3-BC6A-909FCA937DA9}" name="dsb_type" dataDxfId="220">
+    <tableColumn id="19" xr3:uid="{C6423FEA-272F-48D3-BC6A-909FCA937DA9}" name="dsb_type" dataDxfId="223">
       <calculatedColumnFormula>OFFSET(table_1[dsb_type], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B8F61088-5FFA-4860-BF4E-1BFB301A31D9}" name="dsb_pos" dataDxfId="219">
+    <tableColumn id="3" xr3:uid="{B8F61088-5FFA-4860-BF4E-1BFB301A31D9}" name="dsb_pos" dataDxfId="222">
       <calculatedColumnFormula>OFFSET(table_1[dsb_pos], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{524D5B3D-BB20-420D-B7E9-93A7F77CA728}" name="cell" dataDxfId="218">
+    <tableColumn id="4" xr3:uid="{524D5B3D-BB20-420D-B7E9-93A7F77CA728}" name="cell" dataDxfId="221">
       <calculatedColumnFormula>OFFSET(table_1[cell], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{CC918D20-5D79-4223-9717-2CA0EFFA213F}" name="strand" dataDxfId="217">
+    <tableColumn id="5" xr3:uid="{CC918D20-5D79-4223-9717-2CA0EFFA213F}" name="strand" dataDxfId="220">
       <calculatedColumnFormula>OFFSET(table_1[strand], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B2851465-D533-4787-80C4-E844BB2ABB8C}" name="treatment" dataDxfId="216">
+    <tableColumn id="6" xr3:uid="{B2851465-D533-4787-80C4-E844BB2ABB8C}" name="treatment" dataDxfId="219">
       <calculatedColumnFormula>OFFSET(table_1[treatment], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{849BE448-7739-4815-A2C5-5843F62D83D7}" name="hguide" dataDxfId="215">
+    <tableColumn id="7" xr3:uid="{849BE448-7739-4815-A2C5-5843F62D83D7}" name="hguide" dataDxfId="218">
       <calculatedColumnFormula>OFFSET(table_1[hguide], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{343716D9-C3A9-4F90-A58A-42B1B9C79EBF}" name="output_dir" dataDxfId="214">
+    <tableColumn id="8" xr3:uid="{343716D9-C3A9-4F90-A58A-42B1B9C79EBF}" name="output_dir" dataDxfId="217">
       <calculatedColumnFormula>_xlfn.CONCAT(table_2_1[[#This Row],[cell]], "_", table_2_1[[#This Row],[hguide]], "_", table_2_1[[#This Row],[strand]], "_", table_2_1[[#This Row],[treatment]], IF(table_2_1[[#This Row],[control]]&lt;&gt;"none",_xlfn.CONCAT("_", table_2_1[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D29558AA-D418-4CDD-81AE-A987E7BC501D}" name="input_1" dataDxfId="213">
+    <tableColumn id="9" xr3:uid="{D29558AA-D418-4CDD-81AE-A987E7BC501D}" name="input_1" dataDxfId="216">
       <calculatedColumnFormula array="1">OFFSET(table_1[[file_out]:[file_out]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 11, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="22" xr3:uid="{3F29C0D1-58A3-430E-AAAA-9F679DCA46D6}" name="input_2">
@@ -3229,19 +3185,19 @@
     <tableColumn id="20" xr3:uid="{28521A62-94B3-4C7C-AF90-F4E2F4163D29}" name="input_4">
       <calculatedColumnFormula array="1">OFFSET(table_1[[file_out]:[file_out]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 11, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{E2ABF5A3-B032-47F7-9141-9F269EFD9D49}" name="total_reads_1" dataDxfId="212">
+    <tableColumn id="10" xr3:uid="{E2ABF5A3-B032-47F7-9141-9F269EFD9D49}" name="total_reads_1" dataDxfId="215">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{C7B1BE14-3BD6-413B-8575-DE9712F9761A}" name="total_reads_2" dataDxfId="211">
+    <tableColumn id="12" xr3:uid="{C7B1BE14-3BD6-413B-8575-DE9712F9761A}" name="total_reads_2" dataDxfId="214">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{6A8CE344-45B9-42E3-95D8-8EB6A485D968}" name="total_reads_3" dataDxfId="210">
+    <tableColumn id="14" xr3:uid="{6A8CE344-45B9-42E3-95D8-8EB6A485D968}" name="total_reads_3" dataDxfId="213">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{AC170216-9CAE-43B8-A8E2-8FE1529F6D55}" name="total_reads_4" dataDxfId="209">
+    <tableColumn id="16" xr3:uid="{AC170216-9CAE-43B8-A8E2-8FE1529F6D55}" name="total_reads_4" dataDxfId="212">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{A285A0DD-6F6D-404D-AE2A-0D1FC3DDB459}" name="command" dataDxfId="208">
+    <tableColumn id="17" xr3:uid="{A285A0DD-6F6D-404D-AE2A-0D1FC3DDB459}" name="command" dataDxfId="211">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3253,41 +3209,41 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{7D969AC7-2D2F-45B0-BA99-D174130B0A52}" name="table_2_2" displayName="table_2_2" ref="A44:M56" totalsRowShown="0">
   <autoFilter ref="A44:M56" xr:uid="{7D969AC7-2D2F-45B0-BA99-D174130B0A52}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{D612E3DF-AA8E-4EE0-9306-7903B4821992}" name="index" dataDxfId="207"/>
-    <tableColumn id="2" xr3:uid="{B00239B6-16E0-4472-B8C9-F25D625D21DD}" name="ref" dataDxfId="206">
+    <tableColumn id="1" xr3:uid="{D612E3DF-AA8E-4EE0-9306-7903B4821992}" name="index" dataDxfId="210"/>
+    <tableColumn id="2" xr3:uid="{B00239B6-16E0-4472-B8C9-F25D625D21DD}" name="ref" dataDxfId="209">
       <calculatedColumnFormula>OFFSET(table_1[ref], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{47FE94A7-C208-4138-B063-127D4AE215A0}" name="control" dataDxfId="205">
+    <tableColumn id="3" xr3:uid="{47FE94A7-C208-4138-B063-127D4AE215A0}" name="control" dataDxfId="208">
       <calculatedColumnFormula>OFFSET(table_1[control], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{43B4F550-AB35-4206-AAAB-820BBA723DEA}" name="dsb_type" dataDxfId="204">
+    <tableColumn id="4" xr3:uid="{43B4F550-AB35-4206-AAAB-820BBA723DEA}" name="dsb_type" dataDxfId="207">
       <calculatedColumnFormula>OFFSET(table_1[dsb_type], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7233C674-8249-48C9-814C-599A94DF6097}" name="dsb_pos" dataDxfId="203">
+    <tableColumn id="5" xr3:uid="{7233C674-8249-48C9-814C-599A94DF6097}" name="dsb_pos" dataDxfId="206">
       <calculatedColumnFormula>OFFSET(table_1[dsb_pos], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8FD419DF-3888-4BC8-ACF7-F31E7AB24754}" name="cell" dataDxfId="202">
+    <tableColumn id="6" xr3:uid="{8FD419DF-3888-4BC8-ACF7-F31E7AB24754}" name="cell" dataDxfId="205">
       <calculatedColumnFormula>OFFSET(table_1[cell], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{612FF909-1004-49E1-BC8F-F65A8C97EEFC}" name="strand" dataDxfId="201">
+    <tableColumn id="7" xr3:uid="{612FF909-1004-49E1-BC8F-F65A8C97EEFC}" name="strand" dataDxfId="204">
       <calculatedColumnFormula>OFFSET(table_1[strand], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C57AB4D7-F308-46D6-8F19-069619F8CF1B}" name="treatment" dataDxfId="200">
+    <tableColumn id="8" xr3:uid="{C57AB4D7-F308-46D6-8F19-069619F8CF1B}" name="treatment" dataDxfId="203">
       <calculatedColumnFormula>OFFSET(table_1[treatment], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{27DAC4C9-BDB2-4621-A4F1-0094D063284E}" name="hguide" dataDxfId="199">
+    <tableColumn id="9" xr3:uid="{27DAC4C9-BDB2-4621-A4F1-0094D063284E}" name="hguide" dataDxfId="202">
       <calculatedColumnFormula>OFFSET(table_1[hguide], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{E0E9E8C1-4E85-4EFB-8220-84140FBAAF8E}" name="output_dir" dataDxfId="198">
+    <tableColumn id="10" xr3:uid="{E0E9E8C1-4E85-4EFB-8220-84140FBAAF8E}" name="output_dir" dataDxfId="201">
       <calculatedColumnFormula>_xlfn.CONCAT(table_2_2[[#This Row],[cell]], "_", table_2_2[[#This Row],[hguide]], "_", table_2_2[[#This Row],[strand]], "_", table_2_2[[#This Row],[treatment]], "_nodsb")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{CAC474F1-3930-4766-B491-65C86C5752E8}" name="input" dataDxfId="197">
+    <tableColumn id="11" xr3:uid="{CAC474F1-3930-4766-B491-65C86C5752E8}" name="input" dataDxfId="200">
       <calculatedColumnFormula>OFFSET(table_1[file_out], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{BB84920E-3487-4670-93ED-5671EACD3061}" name="total_reads" dataDxfId="196">
+    <tableColumn id="12" xr3:uid="{BB84920E-3487-4670-93ED-5671EACD3061}" name="total_reads" dataDxfId="199">
       <calculatedColumnFormula>OFFSET(table_1[total_reads], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{0CE6DAF6-0C4C-4EC5-8FE5-9B3840A02412}" name="command" dataDxfId="195">
+    <tableColumn id="13" xr3:uid="{0CE6DAF6-0C4C-4EC5-8FE5-9B3840A02412}" name="command" dataDxfId="198">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_2[[#This Row],[input]], ".tsv ", " --total_reads ", table_2_2[[#This Row],[total_reads]], " -o ", libraries_3, "/", table_2_2[[#This Row],[output_dir]], ".tsv", " --quiet ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3296,47 +3252,47 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}" name="table_3_1" displayName="table_3_1" ref="A1:N41" totalsRowShown="0" headerRowDxfId="194">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}" name="table_3_1" displayName="table_3_1" ref="A1:N41" totalsRowShown="0" headerRowDxfId="197">
   <autoFilter ref="A1:N41" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}"/>
   <tableColumns count="14">
-    <tableColumn id="25" xr3:uid="{93D2F09B-24D5-4FE1-BF34-C037E361889F}" name="index" dataDxfId="193"/>
-    <tableColumn id="1" xr3:uid="{2F28DC66-449D-4F81-AA63-8F24B25F33D1}" name="dir" dataDxfId="192">
+    <tableColumn id="25" xr3:uid="{93D2F09B-24D5-4FE1-BF34-C037E361889F}" name="index" dataDxfId="196"/>
+    <tableColumn id="1" xr3:uid="{2F28DC66-449D-4F81-AA63-8F24B25F33D1}" name="dir" dataDxfId="195">
       <calculatedColumnFormula>OFFSET(table_2_1[output_dir], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{3DF6F698-1F9A-4B05-A310-657CCFCE9F66}" name="control" dataDxfId="191">
+    <tableColumn id="13" xr3:uid="{3DF6F698-1F9A-4B05-A310-657CCFCE9F66}" name="control" dataDxfId="194">
       <calculatedColumnFormula>OFFSET(table_2_1[control], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{362C2395-52F7-4A62-B7BA-2DD97ED5E6FB}" name="ref" dataDxfId="190">
+    <tableColumn id="2" xr3:uid="{362C2395-52F7-4A62-B7BA-2DD97ED5E6FB}" name="ref" dataDxfId="193">
       <calculatedColumnFormula>OFFSET(table_2_1[ref], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5F0895D9-2EF2-4524-8BC7-15A33FE68636}" name="dsb_pos" dataDxfId="189">
+    <tableColumn id="3" xr3:uid="{5F0895D9-2EF2-4524-8BC7-15A33FE68636}" name="dsb_pos" dataDxfId="192">
       <calculatedColumnFormula>OFFSET(table_2_1[dsb_pos], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C6D28829-46E6-4D97-8EA4-0AD12EF6CF10}" name="dsb_type" dataDxfId="188">
+    <tableColumn id="4" xr3:uid="{C6D28829-46E6-4D97-8EA4-0AD12EF6CF10}" name="dsb_type" dataDxfId="191">
       <calculatedColumnFormula>OFFSET(table_2_1[dsb_type], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{E8B2E211-C273-4602-86F0-60EA4259B7A4}" name="dsb_type_command" dataDxfId="187">
+    <tableColumn id="12" xr3:uid="{E8B2E211-C273-4602-86F0-60EA4259B7A4}" name="dsb_type_command" dataDxfId="190">
       <calculatedColumnFormula array="1">IF(table_3_1[[#This Row],[dsb_type]]="2DSB", "2", IF(table_3_1[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(table_3_1[[#This Row],[dsb_type]]="1DSB", "1", NA)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{15578E86-B7BE-4D8E-8FD4-E6C9C4F35C9C}" name="strand" dataDxfId="186">
+    <tableColumn id="5" xr3:uid="{15578E86-B7BE-4D8E-8FD4-E6C9C4F35C9C}" name="strand" dataDxfId="189">
       <calculatedColumnFormula>OFFSET(table_2_1[strand], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3366AC40-6578-4797-B607-19265E7DBF5C}" name="hguide" dataDxfId="185">
+    <tableColumn id="6" xr3:uid="{3366AC40-6578-4797-B607-19265E7DBF5C}" name="hguide" dataDxfId="188">
       <calculatedColumnFormula>MID(OFFSET(table_2_1[hguide], table_3_1[[#This Row],[index]] - 1, 0, 1, 1), 3, 100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{554F4E79-98DE-474B-A5C8-D4B536772E95}" name="cell" dataDxfId="184">
+    <tableColumn id="7" xr3:uid="{554F4E79-98DE-474B-A5C8-D4B536772E95}" name="cell" dataDxfId="187">
       <calculatedColumnFormula>OFFSET(table_2_1[cell], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{32FC5061-DD85-4234-9ED8-FEAF6D9E3BC0}" name="treatment" dataDxfId="183">
+    <tableColumn id="8" xr3:uid="{32FC5061-DD85-4234-9ED8-FEAF6D9E3BC0}" name="treatment" dataDxfId="186">
       <calculatedColumnFormula>OFFSET(table_2_1[treatment], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{DB6998A3-1431-4DDD-8DA0-525B805BF436}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{367B0912-E7A8-4430-962D-4F79EE14E5EA}" name="command_main_data" dataDxfId="182">
+    <tableColumn id="10" xr3:uid="{367B0912-E7A8-4430-962D-4F79EE14E5EA}" name="command_main_data" dataDxfId="185">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_1[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_1[[#This Row],[dir]], " -ref ref_seq/", table_3_1[[#This Row],[ref]], " -dsb ", table_3_1[[#This Row],[dsb_pos]], " --dsb_type ",table_3_1[[#This Row],[dsb_type_command]], " --strand ", table_3_1[[#This Row],[strand]], " --hguide ", table_3_1[[#This Row],[hguide]], " --cell ", table_3_1[[#This Row],[cell]], " --treatment ", table_3_1[[#This Row],[treatment]], " --subst_type ", table_3_1[[#This Row],[subst_type]], " --control ", table_3_1[[#This Row],[control]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{4A65279E-321E-4E3E-8383-26D448C2012F}" name="command_graph_data" dataDxfId="181">
+    <tableColumn id="11" xr3:uid="{4A65279E-321E-4E3E-8383-26D448C2012F}" name="command_graph_data" dataDxfId="184">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_1[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_1[[#This Row],[dir]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3345,47 +3301,47 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}" name="table_3_2" displayName="table_3_2" ref="A43:N55" totalsRowShown="0" headerRowDxfId="180">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}" name="table_3_2" displayName="table_3_2" ref="A43:N55" totalsRowShown="0" headerRowDxfId="183">
   <autoFilter ref="A43:N55" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}"/>
   <tableColumns count="14">
-    <tableColumn id="25" xr3:uid="{B2894846-EBB9-47DC-8DE1-7F1DA571A0B9}" name="index" dataDxfId="179"/>
-    <tableColumn id="1" xr3:uid="{98269DFC-71F0-4066-B063-59597431C1C3}" name="dir" dataDxfId="178">
+    <tableColumn id="25" xr3:uid="{B2894846-EBB9-47DC-8DE1-7F1DA571A0B9}" name="index" dataDxfId="182"/>
+    <tableColumn id="1" xr3:uid="{98269DFC-71F0-4066-B063-59597431C1C3}" name="dir" dataDxfId="181">
       <calculatedColumnFormula>OFFSET(table_2_2[output_dir], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{EB55B964-D8E2-4E0C-B7CF-07043E026664}" name="control" dataDxfId="177">
+    <tableColumn id="13" xr3:uid="{EB55B964-D8E2-4E0C-B7CF-07043E026664}" name="control" dataDxfId="180">
       <calculatedColumnFormula>OFFSET(table_2_2[control], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{7A83EC55-03CE-4608-92D6-6F1C53B539FE}" name="ref" dataDxfId="176">
+    <tableColumn id="2" xr3:uid="{7A83EC55-03CE-4608-92D6-6F1C53B539FE}" name="ref" dataDxfId="179">
       <calculatedColumnFormula>OFFSET(table_2_2[ref], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{13E984FC-9FD2-479F-AB4C-B74DDF5FD234}" name="dsb_pos" dataDxfId="175">
+    <tableColumn id="3" xr3:uid="{13E984FC-9FD2-479F-AB4C-B74DDF5FD234}" name="dsb_pos" dataDxfId="178">
       <calculatedColumnFormula>OFFSET(table_2_2[dsb_pos], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{EF0F2447-2FA1-4517-A5CE-D8DDAAC8D3F2}" name="dsb_type" dataDxfId="174">
+    <tableColumn id="4" xr3:uid="{EF0F2447-2FA1-4517-A5CE-D8DDAAC8D3F2}" name="dsb_type" dataDxfId="177">
       <calculatedColumnFormula>OFFSET(table_2_2[dsb_type], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A1849AE1-952B-42B5-99EE-20BD2E4C5A6A}" name="dsb_type_command" dataDxfId="173">
+    <tableColumn id="12" xr3:uid="{A1849AE1-952B-42B5-99EE-20BD2E4C5A6A}" name="dsb_type_command" dataDxfId="176">
       <calculatedColumnFormula array="1">IF(table_3_2[[#This Row],[dsb_type]]="2DSB", "2", IF(table_3_2[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(table_3_2[[#This Row],[dsb_type]]="1DSB", "1", NA)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{625E12FC-BF17-4E65-99DB-EDD53FEF055D}" name="strand" dataDxfId="172">
+    <tableColumn id="5" xr3:uid="{625E12FC-BF17-4E65-99DB-EDD53FEF055D}" name="strand" dataDxfId="175">
       <calculatedColumnFormula>OFFSET(table_2_2[strand], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0ABF747E-328F-4A80-85AA-4AF871C860C1}" name="hguide" dataDxfId="171">
+    <tableColumn id="6" xr3:uid="{0ABF747E-328F-4A80-85AA-4AF871C860C1}" name="hguide" dataDxfId="174">
       <calculatedColumnFormula>MID(OFFSET(table_2_2[hguide], table_3_2[[#This Row],[index]] - 1, 0, 1, 1), 3, 100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{29D6C48B-05B8-42C6-88A9-0939BC454FE0}" name="cell" dataDxfId="170">
+    <tableColumn id="7" xr3:uid="{29D6C48B-05B8-42C6-88A9-0939BC454FE0}" name="cell" dataDxfId="173">
       <calculatedColumnFormula>OFFSET(table_2_2[cell], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{BD269EBE-94A9-4B57-B984-C7566AC259DE}" name="treatment" dataDxfId="169">
+    <tableColumn id="8" xr3:uid="{BD269EBE-94A9-4B57-B984-C7566AC259DE}" name="treatment" dataDxfId="172">
       <calculatedColumnFormula>OFFSET(table_2_2[treatment], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{142C480D-E258-4979-A008-3940A3FE78E4}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{19804410-83AB-479E-A819-2D7449105C25}" name="command_main_data" dataDxfId="168">
+    <tableColumn id="10" xr3:uid="{19804410-83AB-479E-A819-2D7449105C25}" name="command_main_data" dataDxfId="171">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_2[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_2[[#This Row],[dir]], " -ref ref_seq/", table_3_2[[#This Row],[ref]], " -dsb ", table_3_2[[#This Row],[dsb_pos]], " --dsb_type ",table_3_2[[#This Row],[dsb_type_command]], " --strand ", table_3_2[[#This Row],[strand]], " --hguide ", table_3_2[[#This Row],[hguide]], " --cell ", table_3_2[[#This Row],[cell]], " --treatment ", table_3_2[[#This Row],[treatment]], " --subst_type ", table_3_2[[#This Row],[subst_type]], " --control ", table_3_2[[#This Row],[control]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{212A69BD-0F88-401C-957F-8B6EC8E55AED}" name="command_graph_data" dataDxfId="167">
+    <tableColumn id="11" xr3:uid="{212A69BD-0F88-401C-957F-8B6EC8E55AED}" name="command_graph_data" dataDxfId="170">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_2[[#This Row],[dir]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3394,38 +3350,38 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}" name="table_4_1" displayName="table_4_1" ref="A1:K17" totalsRowShown="0" headerRowDxfId="166">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}" name="table_4_1" displayName="table_4_1" ref="A1:K17" totalsRowShown="0" headerRowDxfId="169">
   <autoFilter ref="A1:K17" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B7EC223D-BA24-48F1-9EE3-DC56DEFDE4C2}" name="index" dataDxfId="165"/>
-    <tableColumn id="7" xr3:uid="{D9F1ADDA-18A2-4F81-862D-6B0F786079FF}" name="control" dataDxfId="164">
+    <tableColumn id="1" xr3:uid="{B7EC223D-BA24-48F1-9EE3-DC56DEFDE4C2}" name="index" dataDxfId="168"/>
+    <tableColumn id="7" xr3:uid="{D9F1ADDA-18A2-4F81-862D-6B0F786079FF}" name="control" dataDxfId="167">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{0EA5A81F-6EA1-4256-9717-03273165F7BF}" name="treatment_1" dataDxfId="163">
+    <tableColumn id="8" xr3:uid="{0EA5A81F-6EA1-4256-9717-03273165F7BF}" name="treatment_1" dataDxfId="166">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5F6D005A-96D8-4801-93E2-101BAE551BA8}" name="dir_1" dataDxfId="162">
+    <tableColumn id="2" xr3:uid="{5F6D005A-96D8-4801-93E2-101BAE551BA8}" name="dir_1" dataDxfId="165">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C21D1AF7-7ABE-4181-AA2A-42227869A8DD}" name="treatment_2" dataDxfId="161">
+    <tableColumn id="9" xr3:uid="{C21D1AF7-7ABE-4181-AA2A-42227869A8DD}" name="treatment_2" dataDxfId="164">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{D66426AC-E0B2-4B07-A4D4-5A74AA033E80}" name="dir_2" dataDxfId="160">
+    <tableColumn id="3" xr3:uid="{D66426AC-E0B2-4B07-A4D4-5A74AA033E80}" name="dir_2" dataDxfId="163">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{0C8146A0-DC77-4DC4-82FF-74F4C74CF33E}" name="treatments_out" dataDxfId="159">
+    <tableColumn id="10" xr3:uid="{0C8146A0-DC77-4DC4-82FF-74F4C74CF33E}" name="treatments_out" dataDxfId="162">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_1[[#This Row],[treatment_1]], "_", table_4_1[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{519A6397-7A3C-4009-B8B9-A71C0B3A591B}" name="dir_out" dataDxfId="158">
+    <tableColumn id="4" xr3:uid="{519A6397-7A3C-4009-B8B9-A71C0B3A591B}" name="dir_out" dataDxfId="161">
       <calculatedColumnFormula>SUBSTITUTE(table_4_1[[#This Row],[dir_1]], table_4_1[[#This Row],[treatment_1]], table_4_1[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E1629355-7D02-4819-98A1-EEB3B5FADE18}" name="subst_type" dataDxfId="157">
+    <tableColumn id="5" xr3:uid="{E1629355-7D02-4819-98A1-EEB3B5FADE18}" name="subst_type" dataDxfId="160">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{BC9117A0-CB6F-4D3C-A0E4-BF8395854D9A}" name="command_main_data_combined" dataDxfId="156">
+    <tableColumn id="6" xr3:uid="{BC9117A0-CB6F-4D3C-A0E4-BF8395854D9A}" name="command_main_data_combined" dataDxfId="159">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_1[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_1[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_1[[#This Row],[dir_out]], " --subst_type ", table_4_1[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{D384013E-9937-4DD8-A36A-43325757359B}" name="command_graph_data" dataDxfId="155">
+    <tableColumn id="11" xr3:uid="{D384013E-9937-4DD8-A36A-43325757359B}" name="command_graph_data" dataDxfId="158">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_1[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_1[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3434,38 +3390,38 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}" name="table_4_2" displayName="table_4_2" ref="A20:K22" totalsRowShown="0" headerRowDxfId="154">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}" name="table_4_2" displayName="table_4_2" ref="A20:K22" totalsRowShown="0" headerRowDxfId="157">
   <autoFilter ref="A20:K22" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{7F5A3A15-751D-407C-A035-61B2605E693F}" name="index" dataDxfId="153"/>
-    <tableColumn id="7" xr3:uid="{45863AB0-FD32-49FE-B4BF-F8EE865F7604}" name="control" dataDxfId="152">
+    <tableColumn id="1" xr3:uid="{7F5A3A15-751D-407C-A035-61B2605E693F}" name="index" dataDxfId="156"/>
+    <tableColumn id="7" xr3:uid="{45863AB0-FD32-49FE-B4BF-F8EE865F7604}" name="control" dataDxfId="155">
       <calculatedColumnFormula>OFFSET(table_3_1[control], var_4_anti_offset + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{CD16648D-267E-410B-A366-3E12367C037C}" name="treatment_1" dataDxfId="151">
+    <tableColumn id="8" xr3:uid="{CD16648D-267E-410B-A366-3E12367C037C}" name="treatment_1" dataDxfId="154">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{10C9F90E-86FD-4BFE-939E-298FD6F69F12}" name="dir_1" dataDxfId="150">
+    <tableColumn id="2" xr3:uid="{10C9F90E-86FD-4BFE-939E-298FD6F69F12}" name="dir_1" dataDxfId="153">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{7AB3E4AB-F43B-4FDE-96D7-FBBB4A8B83BE}" name="treatment_2" dataDxfId="149">
+    <tableColumn id="9" xr3:uid="{7AB3E4AB-F43B-4FDE-96D7-FBBB4A8B83BE}" name="treatment_2" dataDxfId="152">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1) + 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BF948A3E-9649-41BF-A7E7-57BFDE810FE9}" name="dir_2" dataDxfId="148">
+    <tableColumn id="3" xr3:uid="{BF948A3E-9649-41BF-A7E7-57BFDE810FE9}" name="dir_2" dataDxfId="151">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1) + 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{378119E5-F021-4785-A653-4D632F029AA6}" name="treatments_out" dataDxfId="147">
+    <tableColumn id="10" xr3:uid="{378119E5-F021-4785-A653-4D632F029AA6}" name="treatments_out" dataDxfId="150">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_2[[#This Row],[treatment_1]], "_", table_4_2[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AE1A14DC-D0C9-4818-B8CC-09A571E73BC2}" name="dir_out" dataDxfId="146">
+    <tableColumn id="4" xr3:uid="{AE1A14DC-D0C9-4818-B8CC-09A571E73BC2}" name="dir_out" dataDxfId="149">
       <calculatedColumnFormula>SUBSTITUTE(table_4_2[[#This Row],[dir_1]], table_4_2[[#This Row],[treatment_1]], table_4_2[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{F29DAC4E-FEC5-4C1D-AAC1-7CE19E401F25}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{DC4E99F4-97AB-4553-A5FB-D20D3D487947}" name="command_main_data_combined" dataDxfId="145">
+    <tableColumn id="6" xr3:uid="{DC4E99F4-97AB-4553-A5FB-D20D3D487947}" name="command_main_data_combined" dataDxfId="148">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_2[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_2[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_2[[#This Row],[dir_out]], " --subst_type ", table_4_2[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{E19D3001-2E76-4CC2-BF33-D0465C77D538}" name="command_graph_data" dataDxfId="144">
+    <tableColumn id="11" xr3:uid="{E19D3001-2E76-4CC2-BF33-D0465C77D538}" name="command_graph_data" dataDxfId="147">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_2[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3474,38 +3430,38 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}" name="table_4_3" displayName="table_4_3" ref="A25:K33" totalsRowShown="0" headerRowDxfId="143">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}" name="table_4_3" displayName="table_4_3" ref="A25:K33" totalsRowShown="0" headerRowDxfId="146">
   <autoFilter ref="A25:K33" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{33AF3495-7432-4F03-9832-525A370EADEC}" name="index" dataDxfId="142"/>
-    <tableColumn id="7" xr3:uid="{3D66515C-5022-4D48-A834-4320DA4E73F6}" name="control" dataDxfId="141">
+    <tableColumn id="1" xr3:uid="{33AF3495-7432-4F03-9832-525A370EADEC}" name="index" dataDxfId="145"/>
+    <tableColumn id="7" xr3:uid="{3D66515C-5022-4D48-A834-4320DA4E73F6}" name="control" dataDxfId="144">
       <calculatedColumnFormula>OFFSET(table_3_2[control], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{294B17A9-F0F9-42CA-8342-55C00648E3A5}" name="treatment_1" dataDxfId="140">
+    <tableColumn id="8" xr3:uid="{294B17A9-F0F9-42CA-8342-55C00648E3A5}" name="treatment_1" dataDxfId="143">
       <calculatedColumnFormula>OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E13C38CF-C105-4AB5-8602-7D32E688C737}" name="dir_1" dataDxfId="139">
+    <tableColumn id="2" xr3:uid="{E13C38CF-C105-4AB5-8602-7D32E688C737}" name="dir_1" dataDxfId="142">
       <calculatedColumnFormula>OFFSET(table_3_2[dir], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{15B3CC7F-2A3C-4026-8417-A9DD21E4F004}" name="treatment_2" dataDxfId="138">
+    <tableColumn id="9" xr3:uid="{15B3CC7F-2A3C-4026-8417-A9DD21E4F004}" name="treatment_2" dataDxfId="141">
       <calculatedColumnFormula>OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{FF7D9AD3-1A35-4013-88AE-0C00465033CD}" name="dir_2" dataDxfId="137">
+    <tableColumn id="3" xr3:uid="{FF7D9AD3-1A35-4013-88AE-0C00465033CD}" name="dir_2" dataDxfId="140">
       <calculatedColumnFormula>OFFSET(table_3_2[dir], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{9353B2D3-0D23-4FBB-AFEC-EB68549160F4}" name="treatments_out" dataDxfId="136">
+    <tableColumn id="10" xr3:uid="{9353B2D3-0D23-4FBB-AFEC-EB68549160F4}" name="treatments_out" dataDxfId="139">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_3[[#This Row],[treatment_1]], "_", table_4_3[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{77F1D6F0-DE95-4E63-9E7E-D3CA3CF85F37}" name="dir_out" dataDxfId="135">
+    <tableColumn id="4" xr3:uid="{77F1D6F0-DE95-4E63-9E7E-D3CA3CF85F37}" name="dir_out" dataDxfId="138">
       <calculatedColumnFormula>SUBSTITUTE(table_4_3[[#This Row],[dir_1]], table_4_3[[#This Row],[treatment_1]], table_4_3[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{BBF4F840-178E-461E-8C17-36D699EDE038}" name="subst_type" dataDxfId="134">
+    <tableColumn id="5" xr3:uid="{BBF4F840-178E-461E-8C17-36D699EDE038}" name="subst_type" dataDxfId="137">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9434BF8B-81C5-43DF-BCB7-FA7146BF2FE8}" name="command_main_data_combined" dataDxfId="133">
+    <tableColumn id="6" xr3:uid="{9434BF8B-81C5-43DF-BCB7-FA7146BF2FE8}" name="command_main_data_combined" dataDxfId="136">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_3[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_3[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_3[[#This Row],[dir_out]], " --subst_type ", table_4_3[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{1ABF0B7B-4ECE-42BF-A7D8-EA13E98144EE}" name="command_graph_data" dataDxfId="132">
+    <tableColumn id="11" xr3:uid="{1ABF0B7B-4ECE-42BF-A7D8-EA13E98144EE}" name="command_graph_data" dataDxfId="135">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_3[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_3[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3872,10 +3828,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DFB1CC9-23C4-4E30-93CF-6F31CFACE92F}">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:C23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3893,413 +3849,606 @@
     <col min="11" max="11" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B1" t="b">
-        <v>0</v>
+        <v>112</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D1" t="s">
-        <v>190</v>
+        <v>82</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>103</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="F1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="str">
+      <c r="B2" s="2" t="str">
         <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
         <v>WT_sgAB_R1_sense_branch</v>
       </c>
-      <c r="C4" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_branch -o plots/graphs/combined/png  -ext png --layout universal</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="C2" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R1</v>
+      </c>
+      <c r="D2" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>AB</v>
+      </c>
+      <c r="E2" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>2DSB</v>
+      </c>
+      <c r="F2" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>2DSB_AB</v>
+      </c>
+      <c r="G2" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_3[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_3[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_branch -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout radial</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="2" t="str">
+      <c r="B3" s="2" t="str">
         <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
         <v>WT_sgAB_R1_sense_cmv</v>
       </c>
-      <c r="C5" s="2" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_cmv -o plots/graphs/combined/png  -ext png --layout universal</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R1</v>
+      </c>
+      <c r="D3" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>AB</v>
+      </c>
+      <c r="E3" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>2DSB</v>
+      </c>
+      <c r="F3" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>2DSB_AB</v>
+      </c>
+      <c r="G3" s="2" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_3[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_3[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout radial</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
+        <v>KO_sgAB_R1_sense_branch</v>
+      </c>
+      <c r="C4" t="str">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R1</v>
+      </c>
+      <c r="D4" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>AB</v>
+      </c>
+      <c r="E4" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>2DSB</v>
+      </c>
+      <c r="F4" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>2DSB_AB</v>
+      </c>
+      <c r="G4" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_3[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_3[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_branch -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout radial</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
+        <v>KO_sgAB_R1_sense_cmv</v>
+      </c>
+      <c r="C5" t="str">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R1</v>
+      </c>
+      <c r="D5" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>AB</v>
+      </c>
+      <c r="E5" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>2DSB</v>
+      </c>
+      <c r="F5" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>2DSB_AB</v>
+      </c>
+      <c r="G5" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_3[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_3[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout radial</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B6" t="str">
         <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>KO_sgAB_R1_sense_branch</v>
+        <v>WT_sgAB_R2_sense_branch</v>
       </c>
       <c r="C6" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_branch -o plots/graphs/combined/png  -ext png --layout universal</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R2</v>
+      </c>
+      <c r="D6" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>AB</v>
+      </c>
+      <c r="E6" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>2DSB</v>
+      </c>
+      <c r="F6" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>2DSB_AB</v>
+      </c>
+      <c r="G6" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_3[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_3[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_branch -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout radial --reverse_complement </v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" t="str">
         <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>KO_sgAB_R1_sense_cmv</v>
+        <v>WT_sgAB_R2_sense_cmv</v>
       </c>
       <c r="C7" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_cmv -o plots/graphs/combined/png  -ext png --layout universal</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R2</v>
+      </c>
+      <c r="D7" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>AB</v>
+      </c>
+      <c r="E7" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>2DSB</v>
+      </c>
+      <c r="F7" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>2DSB_AB</v>
+      </c>
+      <c r="G7" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_3[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_3[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout radial --reverse_complement </v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B8" t="str">
         <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>WT_sgAB_R2_sense_branch</v>
+        <v>KO_sgAB_R2_sense_branch</v>
       </c>
       <c r="C8" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_branch -o plots/graphs/combined/png  -ext png --layout universal</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R2</v>
+      </c>
+      <c r="D8" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>AB</v>
+      </c>
+      <c r="E8" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>2DSB</v>
+      </c>
+      <c r="F8" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>2DSB_AB</v>
+      </c>
+      <c r="G8" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_3[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_3[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_branch -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout radial --reverse_complement </v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B9" t="str">
         <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>WT_sgAB_R2_sense_cmv</v>
+        <v>KO_sgAB_R2_sense_cmv</v>
       </c>
       <c r="C9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_cmv -o plots/graphs/combined/png  -ext png --layout universal</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R2</v>
+      </c>
+      <c r="D9" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>AB</v>
+      </c>
+      <c r="E9" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>2DSB</v>
+      </c>
+      <c r="F9" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>2DSB_AB</v>
+      </c>
+      <c r="G9" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_3[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_3[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout radial --reverse_complement </v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B10" t="str">
         <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>KO_sgAB_R2_sense_branch</v>
+        <v>WT_sgA_R1_sense_branch</v>
       </c>
       <c r="C10" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_branch -o plots/graphs/combined/png  -ext png --layout universal</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R1</v>
+      </c>
+      <c r="D10" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>A</v>
+      </c>
+      <c r="E10" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1DSB</v>
+      </c>
+      <c r="F10" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1DSB_A</v>
+      </c>
+      <c r="G10" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_3[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_3[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_branch -o plots/graphs/combined/png --layout_dir layouts/1DSB_A -ext png --layout radial</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B11" t="str">
         <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>KO_sgAB_R2_sense_cmv</v>
+        <v>WT_sgA_R1_sense_cmv</v>
       </c>
       <c r="C11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_cmv -o plots/graphs/combined/png  -ext png --layout universal</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R1</v>
+      </c>
+      <c r="D11" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>A</v>
+      </c>
+      <c r="E11" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1DSB</v>
+      </c>
+      <c r="F11" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1DSB_A</v>
+      </c>
+      <c r="G11" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_3[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_3[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/1DSB_A -ext png --layout radial</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B12" t="str">
         <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>WT_sgA_R1_sense_branch</v>
+        <v>KO_sgA_R1_sense_branch</v>
       </c>
       <c r="C12" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_branch -o plots/graphs/combined/png  -ext png --layout universal</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R1</v>
+      </c>
+      <c r="D12" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>A</v>
+      </c>
+      <c r="E12" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1DSB</v>
+      </c>
+      <c r="F12" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1DSB_A</v>
+      </c>
+      <c r="G12" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_3[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_3[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_branch -o plots/graphs/combined/png --layout_dir layouts/1DSB_A -ext png --layout radial</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B13" t="str">
         <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>WT_sgA_R1_sense_cmv</v>
+        <v>KO_sgA_R1_sense_cmv</v>
       </c>
       <c r="C13" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_cmv -o plots/graphs/combined/png  -ext png --layout universal</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R1</v>
+      </c>
+      <c r="D13" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>A</v>
+      </c>
+      <c r="E13" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1DSB</v>
+      </c>
+      <c r="F13" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1DSB_A</v>
+      </c>
+      <c r="G13" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_3[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_3[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/1DSB_A -ext png --layout radial</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B14" t="str">
         <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>KO_sgA_R1_sense_branch</v>
+        <v>WT_sgB_R2_sense_branch</v>
       </c>
       <c r="C14" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_branch -o plots/graphs/combined/png  -ext png --layout universal</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R2</v>
+      </c>
+      <c r="D14" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>B</v>
+      </c>
+      <c r="E14" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1DSB</v>
+      </c>
+      <c r="F14" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1DSB_B</v>
+      </c>
+      <c r="G14" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_3[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_3[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_branch -o plots/graphs/combined/png --layout_dir layouts/1DSB_B -ext png --layout radial</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B15" t="str">
         <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>KO_sgA_R1_sense_cmv</v>
+        <v>WT_sgB_R2_sense_cmv</v>
       </c>
       <c r="C15" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_cmv -o plots/graphs/combined/png  -ext png --layout universal</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R2</v>
+      </c>
+      <c r="D15" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>B</v>
+      </c>
+      <c r="E15" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1DSB</v>
+      </c>
+      <c r="F15" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1DSB_B</v>
+      </c>
+      <c r="G15" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_3[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_3[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/1DSB_B -ext png --layout radial</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B16" t="str">
         <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>WT_sgB_R2_sense_branch</v>
+        <v>KO_sgB_R2_sense_branch</v>
       </c>
       <c r="C16" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_branch -o plots/graphs/combined/png  -ext png --layout universal</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R2</v>
+      </c>
+      <c r="D16" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>B</v>
+      </c>
+      <c r="E16" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1DSB</v>
+      </c>
+      <c r="F16" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1DSB_B</v>
+      </c>
+      <c r="G16" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_3[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_3[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_branch -o plots/graphs/combined/png --layout_dir layouts/1DSB_B -ext png --layout radial</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B17" t="str">
         <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>WT_sgB_R2_sense_cmv</v>
+        <v>KO_sgB_R2_sense_cmv</v>
       </c>
       <c r="C17" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_cmv -o plots/graphs/combined/png  -ext png --layout universal</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>15</v>
-      </c>
-      <c r="B18" t="str">
-        <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>KO_sgB_R2_sense_branch</v>
-      </c>
-      <c r="C18" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_branch -o plots/graphs/combined/png  -ext png --layout universal</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>16</v>
-      </c>
-      <c r="B19" t="str">
-        <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>KO_sgB_R2_sense_cmv</v>
-      </c>
-      <c r="C19" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], QUOTIENT(table_7_3[[#This Row],[index]] - 1, 4), 0, 1, 1)), " "), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_cmv -o plots/graphs/combined/png  -ext png --layout universal</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R2</v>
+      </c>
+      <c r="D17" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>B</v>
+      </c>
+      <c r="E17" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1DSB</v>
+      </c>
+      <c r="F17" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1DSB_B</v>
+      </c>
+      <c r="G17" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_3[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_3[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/1DSB_B -ext png --layout radial</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>1</v>
       </c>
-      <c r="B22" t="str">
-        <f ca="1">OFFSET(table_4_2[[dir_out]:[dir_out]], table_7_4[[#This Row],[index]] - 1, 0, 1, 1)</f>
+      <c r="B20" s="2" t="str">
+        <f ca="1">OFFSET(table_4_2[], table_7_39[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
         <v>WT_sgCD_R1_antisense_splicing</v>
       </c>
-      <c r="C22" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_4[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_2[[dir_out]:[dir_out]],table_7_4[[#This Row],[index]] - 1, 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense_splicing -o plots/graphs/combined/png -ext png --layout universal</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="C20" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 37 + 2 * QUOTIENT(table_7_39[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
+        <v>R1</v>
+      </c>
+      <c r="D20" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 37 + 2 * QUOTIENT(table_7_39[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
+        <v>CD</v>
+      </c>
+      <c r="E20" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 37 + 2 * QUOTIENT(table_7_39[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
+        <v>2DSBanti</v>
+      </c>
+      <c r="F20" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 37 + 2 * QUOTIENT(table_7_39[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
+        <v>2DSBanti_CD</v>
+      </c>
+      <c r="G20" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_39[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_39[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_39[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_39[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense_splicing -o plots/graphs/combined/png --layout_dir layouts/2DSBanti_CD -ext png --layout radial</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
         <v>2</v>
       </c>
+      <c r="B21" s="2" t="str">
+        <f ca="1">OFFSET(table_4_2[], table_7_39[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
+        <v>WT_sgCD_R2_antisense_splicing</v>
+      </c>
+      <c r="C21" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 37 + 2 * QUOTIENT(table_7_39[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
+        <v>R2</v>
+      </c>
+      <c r="D21" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 37 + 2 * QUOTIENT(table_7_39[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
+        <v>CD</v>
+      </c>
+      <c r="E21" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 37 + 2 * QUOTIENT(table_7_39[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
+        <v>2DSBanti</v>
+      </c>
+      <c r="F21" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 37 + 2 * QUOTIENT(table_7_39[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
+        <v>2DSBanti_CD</v>
+      </c>
+      <c r="G21" s="2" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_39[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_39[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(OR(var_7_layout = "universal", var_7_layout = "fractal", AND(table_7_39[[#This Row],[dsb_type]] &lt;&gt; "1DSB", table_7_39[[#This Row],[strand]] = "R2")), " --reverse_complement ", ""))</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense_splicing -o plots/graphs/combined/png --layout_dir layouts/2DSBanti_CD -ext png --layout radial --reverse_complement </v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>189</v>
+      </c>
       <c r="B23" t="str">
-        <f ca="1">OFFSET(table_4_2[[dir_out]:[dir_out]], table_7_4[[#This Row],[index]] - 1, 0, 1, 1)</f>
-        <v>WT_sgCD_R2_antisense_splicing</v>
-      </c>
-      <c r="C23" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_4[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_2[[dir_out]:[dir_out]],table_7_4[[#This Row],[index]] - 1, 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense_splicing -o plots/graphs/combined/png -ext png --layout universal</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="K24" s="2"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="10">
-        <v>1</v>
-      </c>
-      <c r="B27" s="9" t="str">
-        <f ca="1">OFFSET(table_4_3[[dir_out]:[dir_out]], table_7_5[[#This Row],[index]] - 1, 0, 1, 1)</f>
-        <v>WT_sgA_R1_sense_branch_nodsb</v>
-      </c>
-      <c r="C27" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_branch_nodsb -o plots/graphs/combined -ext png --layout universal</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="10">
-        <v>2</v>
-      </c>
-      <c r="B28" s="11" t="str">
-        <f ca="1">OFFSET(table_4_3[[dir_out]:[dir_out]], table_7_5[[#This Row],[index]] - 1, 0, 1, 1)</f>
-        <v>WT_sgA_R1_sense_cmv_nodsb</v>
-      </c>
-      <c r="C28" s="11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_cmv_nodsb -o plots/graphs/combined -ext png --layout universal</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="10">
-        <v>3</v>
-      </c>
-      <c r="B29" s="9" t="str">
-        <f ca="1">OFFSET(table_4_3[[dir_out]:[dir_out]], table_7_5[[#This Row],[index]] - 1, 0, 1, 1)</f>
-        <v>KO_sgA_R1_sense_branch_nodsb</v>
-      </c>
-      <c r="C29" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_branch_nodsb -o plots/graphs/combined -ext png --layout universal</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="10">
-        <v>4</v>
-      </c>
-      <c r="B30" s="9" t="str">
-        <f ca="1">OFFSET(table_4_3[[dir_out]:[dir_out]], table_7_5[[#This Row],[index]] - 1, 0, 1, 1)</f>
-        <v>KO_sgA_R1_sense_cmv_nodsb</v>
-      </c>
-      <c r="C30" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_cmv_nodsb -o plots/graphs/combined -ext png --layout universal</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="10">
-        <v>5</v>
-      </c>
-      <c r="B31" s="9" t="str">
-        <f ca="1">OFFSET(table_4_3[[dir_out]:[dir_out]], table_7_5[[#This Row],[index]] - 1, 0, 1, 1)</f>
-        <v>WT_sgB_R2_sense_branch_nodsb</v>
-      </c>
-      <c r="C31" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_branch_nodsb -o plots/graphs/combined -ext png --layout universal</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="10">
-        <v>6</v>
-      </c>
-      <c r="B32" s="9" t="str">
-        <f ca="1">OFFSET(table_4_3[[dir_out]:[dir_out]], table_7_5[[#This Row],[index]] - 1, 0, 1, 1)</f>
-        <v>WT_sgB_R2_sense_cmv_nodsb</v>
-      </c>
-      <c r="C32" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_cmv_nodsb -o plots/graphs/combined -ext png --layout universal</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="10">
-        <v>7</v>
-      </c>
-      <c r="B33" s="9" t="str">
-        <f ca="1">OFFSET(table_4_3[[dir_out]:[dir_out]], table_7_5[[#This Row],[index]] - 1, 0, 1, 1)</f>
-        <v>KO_sgB_R2_sense_branch_nodsb</v>
-      </c>
-      <c r="C33" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_branch_nodsb -o plots/graphs/combined -ext png --layout universal</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="10">
-        <v>8</v>
-      </c>
-      <c r="B34" s="9" t="str">
-        <f ca="1">OFFSET(table_4_3[[dir_out]:[dir_out]], table_7_5[[#This Row],[index]] - 1, 0, 1, 1)</f>
-        <v>KO_sgB_R2_sense_cmv_nodsb</v>
-      </c>
-      <c r="C34" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_5[[#This Row],[dir]], " -o ", graphs_combined, IF(var_7_common_layout_combined, _xlfn.CONCAT(" --layout_dir ", layouts, "/", OFFSET(table_6_1[[dir_out]:[dir_out]], 2 + QUOTIENT(table_7_5[[#This Row],[index]] - 1, 4), 0, 1, 1)), ""), " -ext ", var_7_ext_combined, " --layout ", var_7_layout_combined)</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_cmv_nodsb -o plots/graphs/combined -ext png --layout universal</v>
+        <f ca="1">_xlfn.TEXTJOIN(CHAR(10), TRUE, G2:G17, G20:G21)</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_branch -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_branch -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_branch -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout radial --reverse_complement 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout radial --reverse_complement 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_branch -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout radial --reverse_complement 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout radial --reverse_complement 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_branch -o plots/graphs/combined/png --layout_dir layouts/1DSB_A -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/1DSB_A -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_branch -o plots/graphs/combined/png --layout_dir layouts/1DSB_A -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/1DSB_A -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_branch -o plots/graphs/combined/png --layout_dir layouts/1DSB_B -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/1DSB_B -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_branch -o plots/graphs/combined/png --layout_dir layouts/1DSB_B -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/1DSB_B -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense_splicing -o plots/graphs/combined/png --layout_dir layouts/2DSBanti_CD -ext png --layout radial
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense_splicing -o plots/graphs/combined/png --layout_dir layouts/2DSBanti_CD -ext png --layout radial --reverse_complement </v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="3">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
@@ -22264,7 +22413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AFDA2BA-58B9-4C12-83E9-7C389A51814A}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="K33" sqref="K26:K33"/>
     </sheetView>
   </sheetViews>
@@ -26478,10 +26627,10 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -26547,54 +26696,54 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="17">
+      <c r="A3" s="15">
         <v>1</v>
       </c>
-      <c r="B3" s="13" t="str" cm="1">
+      <c r="B3" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_1]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/WT_sgAB_R1_sense</v>
       </c>
-      <c r="C3" s="13" t="str" cm="1">
+      <c r="C3" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="C3" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_2]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/WT_sgAB_R1_branch</v>
       </c>
-      <c r="D3" s="13" t="str" cm="1">
+      <c r="D3" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="D3" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_3]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/WT_sgAB_R1_cmv</v>
       </c>
-      <c r="E3" s="13" t="str" cm="1">
+      <c r="E3" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="E3" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_4]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/KO_sgAB_R1_sense</v>
       </c>
-      <c r="F3" s="13" t="str" cm="1">
+      <c r="F3" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="F3" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_5]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/KO_sgAB_R1_branch</v>
       </c>
-      <c r="G3" s="13" t="str" cm="1">
+      <c r="G3" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="G3" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_6]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/KO_sgAB_R1_cmv</v>
       </c>
-      <c r="H3" s="13" t="str" cm="1">
+      <c r="H3" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="H3" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_7]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v/>
       </c>
-      <c r="I3" s="13" t="str" cm="1">
+      <c r="I3" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="I3" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_8]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v/>
       </c>
-      <c r="J3" s="13" t="str" cm="1">
+      <c r="J3" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="J3" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_9]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v/>
       </c>
-      <c r="K3" s="13" t="str" cm="1">
+      <c r="K3" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="K3" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_10]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v/>
       </c>
-      <c r="L3" s="13" t="str" cm="1">
+      <c r="L3" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="L3" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_11]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v/>
       </c>
-      <c r="M3" s="13" t="str" cm="1">
+      <c r="M3" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="M3" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_12]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v/>
       </c>
@@ -26628,54 +26777,54 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
+      <c r="A4" s="15">
         <v>2</v>
       </c>
-      <c r="B4" s="13" t="str" cm="1">
+      <c r="B4" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="B4" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_1]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/WT_sgAB_R2_sense</v>
       </c>
-      <c r="C4" s="13" t="str" cm="1">
+      <c r="C4" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="C4" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_2]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/WT_sgAB_R2_branch</v>
       </c>
-      <c r="D4" s="13" t="str" cm="1">
+      <c r="D4" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="D4" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_3]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/WT_sgAB_R2_cmv</v>
       </c>
-      <c r="E4" s="13" t="str" cm="1">
+      <c r="E4" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="E4" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_4]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/KO_sgAB_R2_sense</v>
       </c>
-      <c r="F4" s="13" t="str" cm="1">
+      <c r="F4" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="F4" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_5]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/KO_sgAB_R2_branch</v>
       </c>
-      <c r="G4" s="13" t="str" cm="1">
+      <c r="G4" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="G4" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_6]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/KO_sgAB_R2_cmv</v>
       </c>
-      <c r="H4" s="13" t="str" cm="1">
+      <c r="H4" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="H4" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_7]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v/>
       </c>
-      <c r="I4" s="13" t="str" cm="1">
+      <c r="I4" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="I4" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_8]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v/>
       </c>
-      <c r="J4" s="13" t="str" cm="1">
+      <c r="J4" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="J4" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_9]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v/>
       </c>
-      <c r="K4" s="13" t="str" cm="1">
+      <c r="K4" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="K4" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_10]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v/>
       </c>
-      <c r="L4" s="13" t="str" cm="1">
+      <c r="L4" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="L4" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_11]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v/>
       </c>
-      <c r="M4" s="13" t="str" cm="1">
+      <c r="M4" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="M4" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_12]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v/>
       </c>
@@ -26709,54 +26858,54 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
+      <c r="A5" s="15">
         <v>3</v>
       </c>
-      <c r="B5" s="13" t="str" cm="1">
+      <c r="B5" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="B5" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_1]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/WT_sgA_R1_sense</v>
       </c>
-      <c r="C5" s="13" t="str" cm="1">
+      <c r="C5" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="C5" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_2]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/WT_sgA_R1_branch</v>
       </c>
-      <c r="D5" s="13" t="str" cm="1">
+      <c r="D5" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="D5" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_3]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/WT_sgA_R1_cmv</v>
       </c>
-      <c r="E5" s="13" t="str" cm="1">
+      <c r="E5" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="E5" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_4]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/KO_sgA_R1_sense</v>
       </c>
-      <c r="F5" s="13" t="str" cm="1">
+      <c r="F5" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="F5" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_5]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/KO_sgA_R1_branch</v>
       </c>
-      <c r="G5" s="13" t="str" cm="1">
+      <c r="G5" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="G5" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_6]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/KO_sgA_R1_cmv</v>
       </c>
-      <c r="H5" s="13" t="str" cm="1">
+      <c r="H5" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="H5" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_7]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v>libraries_4/WT_sgA_R1_sense_nodsb</v>
       </c>
-      <c r="I5" s="13" t="str" cm="1">
+      <c r="I5" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="I5" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_8]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v>libraries_4/WT_sgA_R1_branch_nodsb</v>
       </c>
-      <c r="J5" s="13" t="str" cm="1">
+      <c r="J5" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="J5" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_9]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v>libraries_4/WT_sgA_R1_cmv_nodsb</v>
       </c>
-      <c r="K5" s="13" t="str" cm="1">
+      <c r="K5" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="K5" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_10]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v>libraries_4/KO_sgA_R1_sense_nodsb</v>
       </c>
-      <c r="L5" s="13" t="str" cm="1">
+      <c r="L5" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="L5" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_11]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v>libraries_4/KO_sgA_R1_branch_nodsb</v>
       </c>
-      <c r="M5" s="13" t="str" cm="1">
+      <c r="M5" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="M5" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_12]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v>libraries_4/KO_sgA_R1_cmv_nodsb</v>
       </c>
@@ -26790,54 +26939,54 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
+      <c r="A6" s="15">
         <v>4</v>
       </c>
-      <c r="B6" s="13" t="str" cm="1">
+      <c r="B6" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="B6" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_1]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/WT_sgB_R2_sense</v>
       </c>
-      <c r="C6" s="13" t="str" cm="1">
+      <c r="C6" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_2]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/WT_sgB_R2_branch</v>
       </c>
-      <c r="D6" s="13" t="str" cm="1">
+      <c r="D6" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="D6" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_3]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/WT_sgB_R2_cmv</v>
       </c>
-      <c r="E6" s="13" t="str" cm="1">
+      <c r="E6" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="E6" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_4]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/KO_sgB_R2_sense</v>
       </c>
-      <c r="F6" s="13" t="str" cm="1">
+      <c r="F6" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="F6" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_5]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/KO_sgB_R2_branch</v>
       </c>
-      <c r="G6" s="13" t="str" cm="1">
+      <c r="G6" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="G6" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_6]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/KO_sgB_R2_cmv</v>
       </c>
-      <c r="H6" s="13" t="str" cm="1">
+      <c r="H6" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="H6" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_7]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v>libraries_4/WT_sgB_R2_sense_nodsb</v>
       </c>
-      <c r="I6" s="13" t="str" cm="1">
+      <c r="I6" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="I6" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_8]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v>libraries_4/WT_sgB_R2_branch_nodsb</v>
       </c>
-      <c r="J6" s="13" t="str" cm="1">
+      <c r="J6" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="J6" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_9]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v>libraries_4/WT_sgB_R2_cmv_nodsb</v>
       </c>
-      <c r="K6" s="13" t="str" cm="1">
+      <c r="K6" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="K6" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_10]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v>libraries_4/KO_sgB_R2_sense_nodsb</v>
       </c>
-      <c r="L6" s="13" t="str" cm="1">
+      <c r="L6" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="L6" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_11]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v>libraries_4/KO_sgB_R2_branch_nodsb</v>
       </c>
-      <c r="M6" s="13" t="str" cm="1">
+      <c r="M6" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="M6" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_12]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v>libraries_4/KO_sgB_R2_cmv_nodsb</v>
       </c>
@@ -26871,54 +27020,54 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
+      <c r="A7" s="15">
         <v>5</v>
       </c>
-      <c r="B7" s="13" t="str" cm="1">
+      <c r="B7" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="B7" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_1]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/WT_sgA_R1_sense_30bpDown</v>
       </c>
-      <c r="C7" s="13" t="str" cm="1">
+      <c r="C7" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="C7" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_2]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/WT_sgA_R1_branch_30bpDown</v>
       </c>
-      <c r="D7" s="13" t="str" cm="1">
+      <c r="D7" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="D7" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_3]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/WT_sgA_R1_cmv_30bpDown</v>
       </c>
-      <c r="E7" s="13" t="str" cm="1">
+      <c r="E7" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="E7" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_4]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/KO_sgA_R1_sense_30bpDown</v>
       </c>
-      <c r="F7" s="13" t="str" cm="1">
+      <c r="F7" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="F7" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_5]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/KO_sgA_R1_branch_30bpDown</v>
       </c>
-      <c r="G7" s="13" t="str" cm="1">
+      <c r="G7" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="G7" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_6]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/KO_sgA_R1_cmv_30bpDown</v>
       </c>
-      <c r="H7" s="13" t="str" cm="1">
+      <c r="H7" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="H7" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_7]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v/>
       </c>
-      <c r="I7" s="13" t="str" cm="1">
+      <c r="I7" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="I7" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_8]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v/>
       </c>
-      <c r="J7" s="13" t="str" cm="1">
+      <c r="J7" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="J7" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_9]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v/>
       </c>
-      <c r="K7" s="13" t="str" cm="1">
+      <c r="K7" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="K7" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_10]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v/>
       </c>
-      <c r="L7" s="13" t="str" cm="1">
+      <c r="L7" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="L7" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_11]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v/>
       </c>
-      <c r="M7" s="13" t="str" cm="1">
+      <c r="M7" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="M7" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_12]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v/>
       </c>
@@ -26952,54 +27101,54 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
+      <c r="A8" s="15">
         <v>6</v>
       </c>
-      <c r="B8" s="13" t="str" cm="1">
+      <c r="B8" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="B8" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_1]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/WT_sgB_R2_sense_30bpDown</v>
       </c>
-      <c r="C8" s="13" t="str" cm="1">
+      <c r="C8" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="C8" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_2]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/WT_sgB_R2_branch_30bpDown</v>
       </c>
-      <c r="D8" s="13" t="str" cm="1">
+      <c r="D8" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="D8" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_3]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/WT_sgB_R2_cmv_30bpDown</v>
       </c>
-      <c r="E8" s="13" t="str" cm="1">
+      <c r="E8" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="E8" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_4]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/KO_sgB_R2_sense_30bpDown</v>
       </c>
-      <c r="F8" s="13" t="str" cm="1">
+      <c r="F8" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="F8" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_5]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/KO_sgB_R2_branch_30bpDown</v>
       </c>
-      <c r="G8" s="13" t="str" cm="1">
+      <c r="G8" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="G8" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 1) + COLUMN(table_6_1[dir_6]) - COLUMN(table_6_1[[dir_1]:[dir_1]]), 0, 1, 1))</f>
         <v>libraries_4/KO_sgB_R2_cmv_30bpDown</v>
       </c>
-      <c r="H8" s="13" t="str" cm="1">
+      <c r="H8" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="H8" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_7]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v/>
       </c>
-      <c r="I8" s="13" t="str" cm="1">
+      <c r="I8" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="I8" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_8]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v/>
       </c>
-      <c r="J8" s="13" t="str" cm="1">
+      <c r="J8" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="J8" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_9]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v/>
       </c>
-      <c r="K8" s="13" t="str" cm="1">
+      <c r="K8" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="K8" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_10]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v/>
       </c>
-      <c r="L8" s="13" t="str" cm="1">
+      <c r="L8" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="L8" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_11]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v/>
       </c>
-      <c r="M8" s="13" t="str" cm="1">
+      <c r="M8" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="M8" ca="1">IF(AND(table_6_1[[#This Row],[dsb_type]:[dsb_type]]="1DSB", table_6_1[[#This Row],[control]:[control]]="none"), _xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_2[[dir]:[dir]], 6 * (table_6_1[[#This Row],[index]:[index]] - 3) + COLUMN(table_6_1[[#This Row],[dir_12]]) -COLUMN(table_6_1[[#This Row],[dir_7]:[dir_7]]), 0, 1, 1)), "")</f>
         <v/>
       </c>
@@ -27085,83 +27234,83 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
+      <c r="A12" s="10">
         <v>1</v>
       </c>
-      <c r="B12" s="13" t="str" cm="1">
+      <c r="B12" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="B12" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset  + COLUMN() - 2 + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1))</f>
         <v>libraries_4/WT_sgCD_R1_antisense</v>
       </c>
-      <c r="C12" s="13" t="str" cm="1">
+      <c r="C12" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="C12" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset + COLUMN() - 2 + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1))</f>
         <v>libraries_4/WT_sgCD_R1_splicing</v>
       </c>
-      <c r="D12" s="13" t="str">
+      <c r="D12" s="11" t="str">
         <f ca="1">OFFSET(table_3_1[control], var_6_anti_offset  + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</f>
         <v>none</v>
       </c>
-      <c r="E12" s="13" t="str">
+      <c r="E12" s="11" t="str">
         <f ca="1">OFFSET(table_3_1[dsb_type], var_6_anti_offset  + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</f>
         <v>2DSBanti</v>
       </c>
-      <c r="F12" s="13" t="str" cm="1">
+      <c r="F12" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="F12" ca="1">OFFSET(table_3_1[strand], var_6_anti_offset  + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1)</f>
         <v>R1</v>
       </c>
-      <c r="G12" s="13" t="str">
+      <c r="G12" s="11" t="str">
         <f ca="1">OFFSET(table_3_1[hguide], var_6_anti_offset + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</f>
         <v>CD</v>
       </c>
-      <c r="H12" s="14" t="str">
+      <c r="H12" s="12" t="str">
         <f>subst_type</f>
         <v>without</v>
       </c>
-      <c r="I12" s="14" t="str">
+      <c r="I12" s="12" t="str">
         <f ca="1">_xlfn.CONCAT(table_6_2[[#This Row],[dsb_type]], "_", table_6_2[[#This Row],[strand]], IF(table_6_2[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_2[[#This Row],[control]]), ""))</f>
         <v>2DSBanti_R1</v>
       </c>
-      <c r="J12" s="14" t="str">
+      <c r="J12" s="12" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", _xlfn.TEXTJOIN(" ", TRUE, table_6_2[[#This Row],[dir_1]:[dir_2]]), " -o ", layouts, "/", table_6_2[[#This Row],[dir_out]], " --subst_type ", table_6_2[[#This Row],[subst_type]], " --layout ", var_6_layout)</f>
         <v>python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgCD_R1_antisense libraries_4/WT_sgCD_R1_splicing -o layouts/2DSBanti_R1 --subst_type without --layout radial</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="15">
+      <c r="A13" s="13">
         <v>2</v>
       </c>
-      <c r="B13" s="13" t="str" cm="1">
+      <c r="B13" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="B13" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset  + COLUMN() - 2 + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1))</f>
         <v>libraries_4/WT_sgCD_R2_antisense</v>
       </c>
-      <c r="C13" s="13" t="str" cm="1">
+      <c r="C13" s="11" t="str" cm="1">
         <f t="array" aca="1" ref="C13" ca="1">_xlfn.CONCAT(libraries_4, "/", OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset + COLUMN() - 2 + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1))</f>
         <v>libraries_4/WT_sgCD_R2_splicing</v>
       </c>
-      <c r="D13" s="16" t="str">
+      <c r="D13" s="14" t="str">
         <f ca="1">OFFSET(table_3_1[control], var_6_anti_offset  + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</f>
         <v>none</v>
       </c>
-      <c r="E13" s="16" t="str">
+      <c r="E13" s="14" t="str">
         <f ca="1">OFFSET(table_3_1[dsb_type], var_6_anti_offset  + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</f>
         <v>2DSBanti</v>
       </c>
-      <c r="F13" s="16" t="str" cm="1">
+      <c r="F13" s="14" t="str" cm="1">
         <f t="array" aca="1" ref="F13" ca="1">OFFSET(table_3_1[strand], var_6_anti_offset  + 2 * (table_6_2[[#This Row],[index]:[index]] - 1), 0, 1, 1)</f>
         <v>R2</v>
       </c>
-      <c r="G13" s="16" t="str">
+      <c r="G13" s="14" t="str">
         <f ca="1">OFFSET(table_3_1[hguide], var_6_anti_offset + 2 * (table_6_2[[#This Row],[index]] - 1), 0, 1, 1)</f>
         <v>CD</v>
       </c>
-      <c r="H13" s="16" t="str">
+      <c r="H13" s="14" t="str">
         <f>subst_type</f>
         <v>without</v>
       </c>
-      <c r="I13" s="16" t="str">
+      <c r="I13" s="14" t="str">
         <f ca="1">_xlfn.CONCAT(table_6_2[[#This Row],[dsb_type]], "_", table_6_2[[#This Row],[strand]], IF(table_6_2[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_2[[#This Row],[control]]), ""))</f>
         <v>2DSBanti_R2</v>
       </c>
-      <c r="J13" s="16" t="str">
+      <c r="J13" s="14" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", _xlfn.TEXTJOIN(" ", TRUE, table_6_2[[#This Row],[dir_1]:[dir_2]]), " -o ", layouts, "/", table_6_2[[#This Row],[dir_out]], " --subst_type ", table_6_2[[#This Row],[subst_type]], " --layout ", var_6_layout)</f>
         <v>python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgCD_R2_antisense libraries_4/WT_sgCD_R2_splicing -o layouts/2DSBanti_R2 --subst_type without --layout radial</v>
       </c>
@@ -27174,7 +27323,7 @@
         <v>87</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>134</v>
@@ -27453,7 +27602,7 @@
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -27504,8 +27653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1375107-D76A-4386-B771-6693BBF75061}">
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView topLeftCell="B25" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27532,16 +27681,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>190</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="F1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -30958,7 +31107,7 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update colors of vertices.
</commit_message>
<xml_diff>
--- a/libinfo.xlsx
+++ b/libinfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tchan\Code\SCMB_Project\RNA-mediated_DSB_repair\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB0BB2A-C564-4A7B-BBDF-7D3D0E08C676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5F43E8-14D5-4850-B9C8-4D53EC01201B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="4" activeTab="9" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="4" activeTab="8" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
   </bookViews>
   <sheets>
     <sheet name="globals" sheetId="3" r:id="rId1"/>
@@ -22,9 +22,9 @@
     <sheet name="5_histogram_3d" sheetId="11" r:id="rId7"/>
     <sheet name="6_common_layout" sheetId="14" r:id="rId8"/>
     <sheet name="7_plot_graph" sheetId="13" r:id="rId9"/>
-    <sheet name="7_plot_graph_combined" sheetId="15" r:id="rId10"/>
   </sheets>
   <definedNames>
+    <definedName name="graphs">globals!$A$9</definedName>
     <definedName name="graphs_combined">globals!$A$7</definedName>
     <definedName name="graphs_individual">globals!$A$6</definedName>
     <definedName name="histogram_3d">globals!$A$5</definedName>
@@ -40,12 +40,12 @@
     <definedName name="var_6_anti_offset">'6_common_layout'!$A$11</definedName>
     <definedName name="var_6_layout">'6_common_layout'!$B$1</definedName>
     <definedName name="var_7_common_layout">'7_plot_graph'!$B$1</definedName>
-    <definedName name="var_7_common_layout_combined">'7_plot_graph_combined'!#REF!</definedName>
+    <definedName name="var_7_common_layout_combined">#REF!</definedName>
     <definedName name="var_7_ext">'7_plot_graph'!$D$1</definedName>
-    <definedName name="var_7_ext_combined">'7_plot_graph_combined'!#REF!</definedName>
+    <definedName name="var_7_ext_combined">#REF!</definedName>
     <definedName name="var_7_height">'7_plot_graph'!$J$1</definedName>
     <definedName name="var_7_layout">'7_plot_graph'!$F$1</definedName>
-    <definedName name="var_7_layout_combined">'7_plot_graph_combined'!#REF!</definedName>
+    <definedName name="var_7_layout_combined">#REF!</definedName>
     <definedName name="var_7_width">'7_plot_graph'!$H$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1531" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1530" uniqueCount="186">
   <si>
     <t>yjl217</t>
   </si>
@@ -646,6 +646,9 @@
   <si>
     <t>range_args</t>
   </si>
+  <si>
+    <t>plots/graphs</t>
+  </si>
 </sst>
 </file>
 
@@ -784,8 +787,20 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -800,7 +815,24 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -867,51 +899,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1132,6 +1119,22 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -2079,7 +2082,7 @@
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="19" xr3:uid="{E4089767-2E77-4296-9392-7BCD64E1E62D}" name="dir_out" dataDxfId="57">
-      <calculatedColumnFormula>_xlfn.CONCAT(table_6_3[[#This Row],[dsb_type]], "_", table_6_3[[#This Row],[hguide]], IF(table_6_3[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_3[[#This Row],[control]]), ""))</calculatedColumnFormula>
+      <calculatedColumnFormula>_xlfn.CONCAT(var_6_layout, "/", table_6_3[[#This Row],[dsb_type]], "_", table_6_3[[#This Row],[hguide]], IF(table_6_3[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_3[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{8BD09F85-30B0-46CA-A0E3-2CC4F3FB2BD0}" name="command" dataDxfId="56">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_3[[#This Row],[dir]], IF(NOT(ISNA(table_6_3[[#This Row],[reverse_complement]])), _xlfn.CONCAT(" -rc ", table_6_3[[#This Row],[reverse_complement]]), ""), " -o ", layouts, "/", table_6_3[[#This Row],[dir_out]], " --subst_type ", table_6_3[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
@@ -2097,23 +2100,23 @@
     <tableColumn id="18" xr3:uid="{155653FE-38BD-4542-A5AE-2B40B0FD52C7}" name="dir" dataDxfId="53">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 6, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{05E960C2-864E-41C3-A84E-DF767C09AA42}" name="reverse_complement" dataDxfId="6">
+    <tableColumn id="34" xr3:uid="{05E960C2-864E-41C3-A84E-DF767C09AA42}" name="reverse_complement" dataDxfId="52">
       <calculatedColumnFormula>IF(table_6_4[[#This Row],[hguide]]="A",NA(), IF(var_6_layout = "universal", "1 1 1 1 1 1", NA()))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{9EA58FA8-5496-4600-905A-95909513339B}" name="control" dataDxfId="52">
+    <tableColumn id="13" xr3:uid="{9EA58FA8-5496-4600-905A-95909513339B}" name="control" dataDxfId="51">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 6 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{46390A5F-98AD-4211-85B4-A4DD8E31C40C}" name="dsb_type" dataDxfId="51">
+    <tableColumn id="4" xr3:uid="{46390A5F-98AD-4211-85B4-A4DD8E31C40C}" name="dsb_type" dataDxfId="50">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="35" xr3:uid="{5BD83012-469D-4202-9584-AA182CDF11F9}" name="hguide">
       <calculatedColumnFormula array="1">OFFSET(table_3_1[[hguide]:[hguide]], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{123049FA-F284-452C-8FDD-63F409D9967F}" name="subst_type" dataDxfId="50">
+    <tableColumn id="9" xr3:uid="{123049FA-F284-452C-8FDD-63F409D9967F}" name="subst_type" dataDxfId="49">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{CFCDDB26-095C-4395-82E2-37B45B0CDEAD}" name="dir_out" dataDxfId="49">
-      <calculatedColumnFormula>_xlfn.CONCAT(table_6_4[[#This Row],[dsb_type]], "_", table_6_4[[#This Row],[hguide]], IF(table_6_4[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_4[[#This Row],[control]]), ""))</calculatedColumnFormula>
+    <tableColumn id="19" xr3:uid="{CFCDDB26-095C-4395-82E2-37B45B0CDEAD}" name="dir_out" dataDxfId="22">
+      <calculatedColumnFormula>_xlfn.CONCAT(var_6_layout, "/", table_6_4[[#This Row],[dsb_type]], "_", table_6_4[[#This Row],[hguide]], IF(table_6_4[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_4[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{DC6C9CBA-5796-4FFE-878D-BB47DC276187}" name="command" dataDxfId="48">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_4[[#This Row],[dir]], IF(NOT(ISNA(table_6_4[[#This Row],[reverse_complement]])), _xlfn.CONCAT(" -rc ", table_6_4[[#This Row],[reverse_complement]]), ""), " -o ", layouts, "/", table_6_4[[#This Row],[dir_out]], " --subst_type ", table_6_4[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
@@ -2151,7 +2154,7 @@
       <calculatedColumnFormula>OFFSET(table_3_1[[hguide]:[hguide]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{3D97DBDD-03E9-4A6C-BADA-D01B27A8EE51}" name="dir_out" dataDxfId="39">
-      <calculatedColumnFormula>_xlfn.CONCAT(table_6_5[[#This Row],[dsb_type]], "_", table_6_5[[#This Row],[hguide]], IF(table_6_5[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_5[[#This Row],[control]]), ""))</calculatedColumnFormula>
+      <calculatedColumnFormula>_xlfn.CONCAT(var_6_layout, "/", table_6_5[[#This Row],[dsb_type]], "_", table_6_5[[#This Row],[hguide]], IF(table_6_5[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_5[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{5E7626AE-E376-4C60-BA64-B24F95580083}" name="command" dataDxfId="38">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_5[[#This Row],[dir]], " -rc ", table_6_5[[#This Row],[strand]], " -o ", layouts, "/", table_6_5[[#This Row],[dir_out]], " --subst_type ", table_6_5[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
@@ -2211,14 +2214,14 @@
       )
   )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{7AF47D8C-A10C-454A-8FE8-6D4A4FFD2B60}" name="reverse_complement" dataDxfId="7">
+    <tableColumn id="11" xr3:uid="{7AF47D8C-A10C-454A-8FE8-6D4A4FFD2B60}" name="reverse_complement" dataDxfId="23">
       <calculatedColumnFormula>AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="15" xr3:uid="{0D90823C-DABB-4D5B-952B-ECA267C2D98A}" name="range_args" dataDxfId="1">
-      <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="5">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="21">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2226,33 +2229,33 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{B76EEC45-4FC3-44D5-9B2E-9183DF724F60}" name="table_7_3" displayName="table_7_3" ref="A1:I17" totalsRowShown="0" headerRowDxfId="23">
-  <autoFilter ref="A1:I17" xr:uid="{B76EEC45-4FC3-44D5-9B2E-9183DF724F60}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}" name="table_7_2" displayName="table_7_2" ref="A44:I60" totalsRowShown="0" headerRowDxfId="20">
+  <autoFilter ref="A44:I60" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{FAFADB73-BF3B-401A-8C48-9FCB5D3C4CB6}" name="index" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{8541A14E-3250-4B9C-B315-969FC11BE60A}" name="dir" dataDxfId="21">
-      <calculatedColumnFormula>OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{B2B7DB73-4221-4AF0-A850-325F3752E3E0}" name="index" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{7CBFD0EC-49AE-431E-A905-A56D19FE8F5B}" name="dir" dataDxfId="18">
+      <calculatedColumnFormula>OFFSET(table_4_1[], table_7_2[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{627FA44D-7936-4906-80A6-6ABAA9A96C24}" name="strand" dataDxfId="20">
-      <calculatedColumnFormula>OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{8B726DB7-A763-4D99-9E71-D69E0FA3D7BF}" name="strand" dataDxfId="17">
+      <calculatedColumnFormula>OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{D23E086E-5C74-4A74-98A1-113456947567}" name="hguide" dataDxfId="19">
-      <calculatedColumnFormula>OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{E7E8C40B-8285-4EE4-A61D-1F147432D708}" name="hguide" dataDxfId="16">
+      <calculatedColumnFormula>OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{9CE51D1A-4478-4FC1-B156-568596E4C385}" name="dsb_type" dataDxfId="18">
-      <calculatedColumnFormula>OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
+    <tableColumn id="7" xr3:uid="{64B9691C-2BDA-4EE7-B149-7349BFA40A22}" name="dsb_type" dataDxfId="15">
+      <calculatedColumnFormula>OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E2BCDA0F-EDF0-4576-A173-675A35AE49D2}" name="common_layout_dir" dataDxfId="17">
-      <calculatedColumnFormula>OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
+    <tableColumn id="2" xr3:uid="{46F7ABEC-3D59-449F-B3B9-3B53D4C4E17C}" name="common_layout_dir" dataDxfId="14">
+      <calculatedColumnFormula>OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B12F1B26-6634-4A2F-872E-5DF17842CC54}" name="reverse_complement" dataDxfId="16">
-      <calculatedColumnFormula>OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
+    <tableColumn id="8" xr3:uid="{BFEA7E87-08AD-4F58-8B7D-A592368549F0}" name="reverse_complement" dataDxfId="13">
+      <calculatedColumnFormula>OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{78ADDC76-1E4A-49DA-9DC4-5BDB64D8FA9A}" name="range_args" dataDxfId="4">
-      <calculatedColumnFormula>OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
+    <tableColumn id="9" xr3:uid="{928832B4-7BAB-42E7-88BC-BB633DA53A2E}" name="range_args" dataDxfId="12">
+      <calculatedColumnFormula>OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{EAD6D5EC-B61E-4A98-B4FD-4932757CFEA3}" name="command" dataDxfId="0">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height,  " ",  table_7_3[[#This Row],[range_args]])</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{FEA012AC-7DC4-4D11-9B59-A05887E08F6E}" name="command" dataDxfId="0">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/combined/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2260,33 +2263,33 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{1EF3A7F2-091F-42AE-91CA-D18AA0FD8430}" name="table_7_39" displayName="table_7_39" ref="A19:I21" totalsRowShown="0" headerRowDxfId="15">
-  <autoFilter ref="A19:I21" xr:uid="{1EF3A7F2-091F-42AE-91CA-D18AA0FD8430}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}" name="table_7_3" displayName="table_7_3" ref="A62:I64" totalsRowShown="0" headerRowDxfId="11">
+  <autoFilter ref="A62:I64" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{D25401DE-9587-4D52-A7E4-1182AFAAC5F6}" name="index" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{D669EE3E-402E-4224-BA98-DE9E0722137B}" name="dir" dataDxfId="13">
-      <calculatedColumnFormula>OFFSET(table_4_2[], table_7_39[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{E718984E-FC22-4321-9162-791892D20032}" name="index" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{A71ABC91-B291-4CD9-A2A1-F6CA41CEE59E}" name="dir" dataDxfId="9">
+      <calculatedColumnFormula>OFFSET(table_4_2[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{2B75E3A0-0699-4170-8EC2-74B07D76FA5F}" name="strand" dataDxfId="12">
-      <calculatedColumnFormula>OFFSET(table_7_1[[strand]:[strand]], 37 + 2 * QUOTIENT(table_7_39[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{8D7F2EAB-990D-439F-AE1F-6FB6AFC6C4B1}" name="strand" dataDxfId="8">
+      <calculatedColumnFormula>OFFSET(table_7_1[[strand]:[strand]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E4B22932-5A45-4536-9287-472A2DAB716B}" name="hguide" dataDxfId="11">
-      <calculatedColumnFormula>OFFSET(table_7_1[[hguide]:[hguide]], 37 + 2 * QUOTIENT(table_7_39[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{B8ABFFB9-C4F5-4866-8F37-B49F31C44F20}" name="hguide" dataDxfId="7">
+      <calculatedColumnFormula>OFFSET(table_7_1[[hguide]:[hguide]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{B62FF923-C030-49D9-971F-232E1B61FD42}" name="dsb_type" dataDxfId="10">
-      <calculatedColumnFormula>OFFSET(table_7_1[[dsb_type]:[dsb_type]], 37 + 2 * QUOTIENT(table_7_39[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
+    <tableColumn id="7" xr3:uid="{3835BF64-C6A9-440B-96F5-A2332AB91438}" name="dsb_type" dataDxfId="6">
+      <calculatedColumnFormula>OFFSET(table_7_1[[dsb_type]:[dsb_type]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{F6CF1684-EFBE-4FE3-B11C-E53417FDF011}" name="common_layout_dir" dataDxfId="9">
-      <calculatedColumnFormula>OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 37 + 2 * QUOTIENT(table_7_39[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
+    <tableColumn id="2" xr3:uid="{C07D080E-B5A2-43FC-84BA-BCBD008F3B26}" name="common_layout_dir" dataDxfId="5">
+      <calculatedColumnFormula>OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{EC825B3A-7D72-47DB-8D6B-7A1BCF23C6EA}" name="reverse_complement" dataDxfId="8">
-      <calculatedColumnFormula>OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 37 + 2 * QUOTIENT(table_7_39[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
+    <tableColumn id="8" xr3:uid="{6E360CD4-3BFD-4CC3-A93F-137C46B62651}" name="reverse_complement" dataDxfId="4">
+      <calculatedColumnFormula>OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{9409AE53-C004-46B2-8125-5DF9F3A53090}" name="range_args" dataDxfId="3">
-      <calculatedColumnFormula>OFFSET(table_7_1[[range_args]:[range_args]], 37 + 2 * QUOTIENT(table_7_39[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
+    <tableColumn id="9" xr3:uid="{A1862EF0-F072-4796-964D-7EDA8C8787B0}" name="range_args" dataDxfId="3">
+      <calculatedColumnFormula>OFFSET(table_7_1[[range_args]:[range_args]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{7C0FCF3E-3C81-4367-967B-F1ACE83A43C9}" name="command" dataDxfId="2">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_39[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_39[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_39[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height,  " ",  table_7_39[[#This Row],[range_args]])</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{D5ADEB9F-0405-4E9D-BDA9-7ECD31E23490}" name="command" dataDxfId="2">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/combined/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_3[[#This Row],[range_args]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2956,10 +2959,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86129707-88BE-44BB-B759-1CA0FE147BD8}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3011,793 +3014,13 @@
         <v>171</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>185</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DFB1CC9-23C4-4E30-93CF-6F31CFACE92F}">
-  <dimension ref="A1:I24"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
-    <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" customWidth="1"/>
-    <col min="9" max="9" width="50.7109375" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="str">
-        <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>WT_sgAB_R1_sense_branch</v>
-      </c>
-      <c r="C2" s="2" t="str">
-        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>R1</v>
-      </c>
-      <c r="D2" s="2" t="str">
-        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>AB</v>
-      </c>
-      <c r="E2" s="2" t="str">
-        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>2DSB</v>
-      </c>
-      <c r="F2" s="2" t="str">
-        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>2DSB_AB</v>
-      </c>
-      <c r="G2" s="2" t="b">
-        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>0</v>
-      </c>
-      <c r="H2" s="2" t="str">
-        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
-      </c>
-      <c r="I2" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height,  " ",  table_7_3[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_branch -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 </v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="str">
-        <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>WT_sgAB_R1_sense_cmv</v>
-      </c>
-      <c r="C3" s="2" t="str">
-        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>R1</v>
-      </c>
-      <c r="D3" s="2" t="str">
-        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>AB</v>
-      </c>
-      <c r="E3" s="2" t="str">
-        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>2DSB</v>
-      </c>
-      <c r="F3" s="2" t="str">
-        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>2DSB_AB</v>
-      </c>
-      <c r="G3" s="2" t="b">
-        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>0</v>
-      </c>
-      <c r="H3" s="2" t="str">
-        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
-      </c>
-      <c r="I3" s="2" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height,  " ",  table_7_3[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 </v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" t="str">
-        <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>KO_sgAB_R1_sense_branch</v>
-      </c>
-      <c r="C4" t="str">
-        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>R1</v>
-      </c>
-      <c r="D4" t="str">
-        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>AB</v>
-      </c>
-      <c r="E4" t="str">
-        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>2DSB</v>
-      </c>
-      <c r="F4" t="str">
-        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>2DSB_AB</v>
-      </c>
-      <c r="G4" t="b">
-        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>0</v>
-      </c>
-      <c r="H4" t="str">
-        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
-      </c>
-      <c r="I4" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height,  " ",  table_7_3[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_branch -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 </v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" t="str">
-        <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>KO_sgAB_R1_sense_cmv</v>
-      </c>
-      <c r="C5" t="str">
-        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>R1</v>
-      </c>
-      <c r="D5" t="str">
-        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>AB</v>
-      </c>
-      <c r="E5" t="str">
-        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>2DSB</v>
-      </c>
-      <c r="F5" t="str">
-        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>2DSB_AB</v>
-      </c>
-      <c r="G5" t="b">
-        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>0</v>
-      </c>
-      <c r="H5" t="str">
-        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
-      </c>
-      <c r="I5" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height,  " ",  table_7_3[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 </v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" t="str">
-        <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>WT_sgAB_R2_sense_branch</v>
-      </c>
-      <c r="C6" t="str">
-        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>R2</v>
-      </c>
-      <c r="D6" t="str">
-        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>AB</v>
-      </c>
-      <c r="E6" t="str">
-        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>2DSB</v>
-      </c>
-      <c r="F6" t="str">
-        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>2DSB_AB</v>
-      </c>
-      <c r="G6" t="b">
-        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="H6" t="str">
-        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
-      </c>
-      <c r="I6" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height,  " ",  table_7_3[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_branch -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 </v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" t="str">
-        <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>WT_sgAB_R2_sense_cmv</v>
-      </c>
-      <c r="C7" t="str">
-        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>R2</v>
-      </c>
-      <c r="D7" t="str">
-        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>AB</v>
-      </c>
-      <c r="E7" t="str">
-        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>2DSB</v>
-      </c>
-      <c r="F7" t="str">
-        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>2DSB_AB</v>
-      </c>
-      <c r="G7" t="b">
-        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="H7" t="str">
-        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
-      </c>
-      <c r="I7" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height,  " ",  table_7_3[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 </v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" t="str">
-        <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>KO_sgAB_R2_sense_branch</v>
-      </c>
-      <c r="C8" t="str">
-        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>R2</v>
-      </c>
-      <c r="D8" t="str">
-        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>AB</v>
-      </c>
-      <c r="E8" t="str">
-        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>2DSB</v>
-      </c>
-      <c r="F8" t="str">
-        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>2DSB_AB</v>
-      </c>
-      <c r="G8" t="b">
-        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="H8" t="str">
-        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
-      </c>
-      <c r="I8" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height,  " ",  table_7_3[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_branch -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 </v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" t="str">
-        <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>KO_sgAB_R2_sense_cmv</v>
-      </c>
-      <c r="C9" t="str">
-        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>R2</v>
-      </c>
-      <c r="D9" t="str">
-        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>AB</v>
-      </c>
-      <c r="E9" t="str">
-        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>2DSB</v>
-      </c>
-      <c r="F9" t="str">
-        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>2DSB_AB</v>
-      </c>
-      <c r="G9" t="b">
-        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="H9" t="str">
-        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
-      </c>
-      <c r="I9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height,  " ",  table_7_3[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 </v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" t="str">
-        <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>WT_sgA_R1_sense_branch</v>
-      </c>
-      <c r="C10" t="str">
-        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>R1</v>
-      </c>
-      <c r="D10" t="str">
-        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>A</v>
-      </c>
-      <c r="E10" t="str">
-        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>1DSB</v>
-      </c>
-      <c r="F10" t="str">
-        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>1DSB_A</v>
-      </c>
-      <c r="G10" t="b">
-        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>0</v>
-      </c>
-      <c r="H10" t="str">
-        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v xml:space="preserve"> --range_x -12 12 --range_y -22 18 </v>
-      </c>
-      <c r="I10" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height,  " ",  table_7_3[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_branch -o plots/graphs/combined/png --layout_dir layouts/1DSB_A -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 18 </v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" t="str">
-        <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>WT_sgA_R1_sense_cmv</v>
-      </c>
-      <c r="C11" t="str">
-        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>R1</v>
-      </c>
-      <c r="D11" t="str">
-        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>A</v>
-      </c>
-      <c r="E11" t="str">
-        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>1DSB</v>
-      </c>
-      <c r="F11" t="str">
-        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>1DSB_A</v>
-      </c>
-      <c r="G11" t="b">
-        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>0</v>
-      </c>
-      <c r="H11" t="str">
-        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v xml:space="preserve"> --range_x -12 12 --range_y -22 18 </v>
-      </c>
-      <c r="I11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height,  " ",  table_7_3[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/1DSB_A -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 18 </v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" t="str">
-        <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>KO_sgA_R1_sense_branch</v>
-      </c>
-      <c r="C12" t="str">
-        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>R1</v>
-      </c>
-      <c r="D12" t="str">
-        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>A</v>
-      </c>
-      <c r="E12" t="str">
-        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>1DSB</v>
-      </c>
-      <c r="F12" t="str">
-        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>1DSB_A</v>
-      </c>
-      <c r="G12" t="b">
-        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>0</v>
-      </c>
-      <c r="H12" t="str">
-        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v xml:space="preserve"> --range_x -12 12 --range_y -22 18 </v>
-      </c>
-      <c r="I12" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height,  " ",  table_7_3[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_branch -o plots/graphs/combined/png --layout_dir layouts/1DSB_A -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 18 </v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" t="str">
-        <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>KO_sgA_R1_sense_cmv</v>
-      </c>
-      <c r="C13" t="str">
-        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>R1</v>
-      </c>
-      <c r="D13" t="str">
-        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>A</v>
-      </c>
-      <c r="E13" t="str">
-        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>1DSB</v>
-      </c>
-      <c r="F13" t="str">
-        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>1DSB_A</v>
-      </c>
-      <c r="G13" t="b">
-        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>0</v>
-      </c>
-      <c r="H13" t="str">
-        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v xml:space="preserve"> --range_x -12 12 --range_y -22 18 </v>
-      </c>
-      <c r="I13" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height,  " ",  table_7_3[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/1DSB_A -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 18 </v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" t="str">
-        <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>WT_sgB_R2_sense_branch</v>
-      </c>
-      <c r="C14" t="str">
-        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>R2</v>
-      </c>
-      <c r="D14" t="str">
-        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>B</v>
-      </c>
-      <c r="E14" t="str">
-        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>1DSB</v>
-      </c>
-      <c r="F14" t="str">
-        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>1DSB_B</v>
-      </c>
-      <c r="G14" t="b">
-        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="H14" t="str">
-        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v xml:space="preserve"> --range_x -12 12 --range_y -20 10 </v>
-      </c>
-      <c r="I14" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height,  " ",  table_7_3[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_branch -o plots/graphs/combined/png --layout_dir layouts/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -20 10 </v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" t="str">
-        <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>WT_sgB_R2_sense_cmv</v>
-      </c>
-      <c r="C15" t="str">
-        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>R2</v>
-      </c>
-      <c r="D15" t="str">
-        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>B</v>
-      </c>
-      <c r="E15" t="str">
-        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>1DSB</v>
-      </c>
-      <c r="F15" t="str">
-        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>1DSB_B</v>
-      </c>
-      <c r="G15" t="b">
-        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="H15" t="str">
-        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v xml:space="preserve"> --range_x -12 12 --range_y -20 10 </v>
-      </c>
-      <c r="I15" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height,  " ",  table_7_3[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -20 10 </v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" t="str">
-        <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>KO_sgB_R2_sense_branch</v>
-      </c>
-      <c r="C16" t="str">
-        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>R2</v>
-      </c>
-      <c r="D16" t="str">
-        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>B</v>
-      </c>
-      <c r="E16" t="str">
-        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>1DSB</v>
-      </c>
-      <c r="F16" t="str">
-        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>1DSB_B</v>
-      </c>
-      <c r="G16" t="b">
-        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="H16" t="str">
-        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v xml:space="preserve"> --range_x -12 12 --range_y -20 10 </v>
-      </c>
-      <c r="I16" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height,  " ",  table_7_3[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_branch -o plots/graphs/combined/png --layout_dir layouts/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -20 10 </v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" t="str">
-        <f ca="1">OFFSET(table_4_1[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>KO_sgB_R2_sense_cmv</v>
-      </c>
-      <c r="C17" t="str">
-        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>R2</v>
-      </c>
-      <c r="D17" t="str">
-        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>B</v>
-      </c>
-      <c r="E17" t="str">
-        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>1DSB</v>
-      </c>
-      <c r="F17" t="str">
-        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>1DSB_B</v>
-      </c>
-      <c r="G17" t="b">
-        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="H17" t="str">
-        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v xml:space="preserve"> --range_x -12 12 --range_y -20 10 </v>
-      </c>
-      <c r="I17" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height,  " ",  table_7_3[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -20 10 </v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>1</v>
-      </c>
-      <c r="B20" s="2" t="str">
-        <f ca="1">OFFSET(table_4_2[], table_7_39[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>WT_sgCD_R1_antisense_splicing</v>
-      </c>
-      <c r="C20" s="2" t="str">
-        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 37 + 2 * QUOTIENT(table_7_39[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
-        <v>R1</v>
-      </c>
-      <c r="D20" s="2" t="str">
-        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 37 + 2 * QUOTIENT(table_7_39[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
-        <v>CD</v>
-      </c>
-      <c r="E20" s="2" t="str">
-        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 37 + 2 * QUOTIENT(table_7_39[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
-        <v>2DSBanti</v>
-      </c>
-      <c r="F20" s="2" t="str">
-        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 37 + 2 * QUOTIENT(table_7_39[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
-        <v>2DSBanti_CD</v>
-      </c>
-      <c r="G20" s="2" t="b">
-        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 37 + 2 * QUOTIENT(table_7_39[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
-        <v>0</v>
-      </c>
-      <c r="H20" s="2" t="str">
-        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 37 + 2 * QUOTIENT(table_7_39[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
-        <v xml:space="preserve"> --range_x -12 12 --range_y -18 24 </v>
-      </c>
-      <c r="I20" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_39[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_39[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_39[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height,  " ",  table_7_39[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense_splicing -o plots/graphs/combined/png --layout_dir layouts/2DSBanti_CD -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -18 24 </v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>2</v>
-      </c>
-      <c r="B21" s="2" t="str">
-        <f ca="1">OFFSET(table_4_2[], table_7_39[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
-        <v>WT_sgCD_R2_antisense_splicing</v>
-      </c>
-      <c r="C21" s="2" t="str">
-        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 37 + 2 * QUOTIENT(table_7_39[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
-        <v>R2</v>
-      </c>
-      <c r="D21" s="2" t="str">
-        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 37 + 2 * QUOTIENT(table_7_39[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
-        <v>CD</v>
-      </c>
-      <c r="E21" s="2" t="str">
-        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 37 + 2 * QUOTIENT(table_7_39[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
-        <v>2DSBanti</v>
-      </c>
-      <c r="F21" s="2" t="str">
-        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 37 + 2 * QUOTIENT(table_7_39[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
-        <v>2DSBanti_CD</v>
-      </c>
-      <c r="G21" s="2" t="b">
-        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 37 + 2 * QUOTIENT(table_7_39[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
-        <v>1</v>
-      </c>
-      <c r="H21" s="2" t="str">
-        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 37 + 2 * QUOTIENT(table_7_39[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
-        <v xml:space="preserve"> --range_x -12 12 --range_y -18 24 </v>
-      </c>
-      <c r="I21" s="2" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_39[[#This Row],[dir]], " -o ", graphs_combined, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_39[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_39[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height,  " ",  table_7_39[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense_splicing -o plots/graphs/combined/png --layout_dir layouts/2DSBanti_CD -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -18 24 </v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="str">
-        <f ca="1">_xlfn.TEXTJOIN(CHAR(10), TRUE, I2:I17, I20:I21)</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_branch -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_branch -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_branch -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_branch -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_branch -o plots/graphs/combined/png --layout_dir layouts/1DSB_A -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 18 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/1DSB_A -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 18 
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_branch -o plots/graphs/combined/png --layout_dir layouts/1DSB_A -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 18 
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/1DSB_A -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 18 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_branch -o plots/graphs/combined/png --layout_dir layouts/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -20 10 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -20 10 
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_branch -o plots/graphs/combined/png --layout_dir layouts/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -20 10 
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_cmv -o plots/graphs/combined/png --layout_dir layouts/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -20 10 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense_splicing -o plots/graphs/combined/png --layout_dir layouts/2DSBanti_CD -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -18 24 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense_splicing -o plots/graphs/combined/png --layout_dir layouts/2DSBanti_CD -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -18 24 </v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="2">
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
-  </tableParts>
 </worksheet>
 </file>
 
@@ -25952,7 +25175,7 @@
   <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26043,12 +25266,12 @@
         <v>without</v>
       </c>
       <c r="H4" t="str">
-        <f ca="1">_xlfn.CONCAT(table_6_3[[#This Row],[dsb_type]], "_", table_6_3[[#This Row],[hguide]], IF(table_6_3[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_3[[#This Row],[control]]), ""))</f>
-        <v>2DSB_AB</v>
+        <f ca="1">_xlfn.CONCAT(var_6_layout, "/", table_6_3[[#This Row],[dsb_type]], "_", table_6_3[[#This Row],[hguide]], IF(table_6_3[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_3[[#This Row],[control]]), ""))</f>
+        <v>universal/2DSB_AB</v>
       </c>
       <c r="I4" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_3[[#This Row],[dir]], IF(NOT(ISNA(table_6_3[[#This Row],[reverse_complement]])), _xlfn.CONCAT(" -rc ", table_6_3[[#This Row],[reverse_complement]]), ""), " -o ", layouts, "/", table_6_3[[#This Row],[dir_out]], " --subst_type ", table_6_3[[#This Row],[subst_type]], " --layout ", var_6_layout)</f>
-        <v>python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgAB_R1_sense libraries_4/WT_sgAB_R1_branch libraries_4/WT_sgAB_R1_cmv libraries_4/KO_sgAB_R1_sense libraries_4/KO_sgAB_R1_branch libraries_4/KO_sgAB_R1_cmv libraries_4/WT_sgAB_R2_sense libraries_4/WT_sgAB_R2_branch libraries_4/WT_sgAB_R2_cmv libraries_4/KO_sgAB_R2_sense libraries_4/KO_sgAB_R2_branch libraries_4/KO_sgAB_R2_cmv -rc 0 0 0 0 0 0 1 1 1 1 1 1 -o layouts/2DSB_AB --subst_type without --layout universal</v>
+        <v>python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgAB_R1_sense libraries_4/WT_sgAB_R1_branch libraries_4/WT_sgAB_R1_cmv libraries_4/KO_sgAB_R1_sense libraries_4/KO_sgAB_R1_branch libraries_4/KO_sgAB_R1_cmv libraries_4/WT_sgAB_R2_sense libraries_4/WT_sgAB_R2_branch libraries_4/WT_sgAB_R2_cmv libraries_4/KO_sgAB_R2_sense libraries_4/KO_sgAB_R2_branch libraries_4/KO_sgAB_R2_cmv -rc 0 0 0 0 0 0 1 1 1 1 1 1 -o layouts/universal/2DSB_AB --subst_type without --layout universal</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -26121,12 +25344,12 @@
         <v>without</v>
       </c>
       <c r="H8" t="str">
-        <f ca="1">_xlfn.CONCAT(table_6_4[[#This Row],[dsb_type]], "_", table_6_4[[#This Row],[hguide]], IF(table_6_4[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_4[[#This Row],[control]]), ""))</f>
-        <v>1DSB_A</v>
+        <f ca="1">_xlfn.CONCAT(var_6_layout, "/", table_6_4[[#This Row],[dsb_type]], "_", table_6_4[[#This Row],[hguide]], IF(table_6_4[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_4[[#This Row],[control]]), ""))</f>
+        <v>universal/1DSB_A</v>
       </c>
       <c r="I8" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_4[[#This Row],[dir]], IF(NOT(ISNA(table_6_4[[#This Row],[reverse_complement]])), _xlfn.CONCAT(" -rc ", table_6_4[[#This Row],[reverse_complement]]), ""), " -o ", layouts, "/", table_6_4[[#This Row],[dir_out]], " --subst_type ", table_6_4[[#This Row],[subst_type]], " --layout ", var_6_layout)</f>
-        <v>python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgA_R1_sense libraries_4/WT_sgA_R1_branch libraries_4/WT_sgA_R1_cmv libraries_4/KO_sgA_R1_sense libraries_4/KO_sgA_R1_branch libraries_4/KO_sgA_R1_cmv -o layouts/1DSB_A --subst_type without --layout universal</v>
+        <v>python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgA_R1_sense libraries_4/WT_sgA_R1_branch libraries_4/WT_sgA_R1_cmv libraries_4/KO_sgA_R1_sense libraries_4/KO_sgA_R1_branch libraries_4/KO_sgA_R1_cmv -o layouts/universal/1DSB_A --subst_type without --layout universal</v>
       </c>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
@@ -26161,12 +25384,12 @@
         <v>without</v>
       </c>
       <c r="H9" t="str">
-        <f ca="1">_xlfn.CONCAT(table_6_4[[#This Row],[dsb_type]], "_", table_6_4[[#This Row],[hguide]], IF(table_6_4[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_4[[#This Row],[control]]), ""))</f>
-        <v>1DSB_B</v>
+        <f ca="1">_xlfn.CONCAT(var_6_layout, "/", table_6_4[[#This Row],[dsb_type]], "_", table_6_4[[#This Row],[hguide]], IF(table_6_4[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_4[[#This Row],[control]]), ""))</f>
+        <v>universal/1DSB_B</v>
       </c>
       <c r="I9" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_4[[#This Row],[dir]], IF(NOT(ISNA(table_6_4[[#This Row],[reverse_complement]])), _xlfn.CONCAT(" -rc ", table_6_4[[#This Row],[reverse_complement]]), ""), " -o ", layouts, "/", table_6_4[[#This Row],[dir_out]], " --subst_type ", table_6_4[[#This Row],[subst_type]], " --layout ", var_6_layout)</f>
-        <v>python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgB_R2_sense libraries_4/WT_sgB_R2_branch libraries_4/WT_sgB_R2_cmv libraries_4/KO_sgB_R2_sense libraries_4/KO_sgB_R2_branch libraries_4/KO_sgB_R2_cmv -rc 1 1 1 1 1 1 -o layouts/1DSB_B --subst_type without --layout universal</v>
+        <v>python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgB_R2_sense libraries_4/WT_sgB_R2_branch libraries_4/WT_sgB_R2_cmv libraries_4/KO_sgB_R2_sense libraries_4/KO_sgB_R2_branch libraries_4/KO_sgB_R2_cmv -rc 1 1 1 1 1 1 -o layouts/universal/1DSB_B --subst_type without --layout universal</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -26259,12 +25482,12 @@
         <v>CD</v>
       </c>
       <c r="H13" s="4" t="str">
-        <f ca="1">_xlfn.CONCAT(table_6_5[[#This Row],[dsb_type]], "_", table_6_5[[#This Row],[hguide]], IF(table_6_5[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_5[[#This Row],[control]]), ""))</f>
-        <v>2DSBanti_CD</v>
+        <f ca="1">_xlfn.CONCAT(var_6_layout, "/", table_6_5[[#This Row],[dsb_type]], "_", table_6_5[[#This Row],[hguide]], IF(table_6_5[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_5[[#This Row],[control]]), ""))</f>
+        <v>universal/2DSBanti_CD</v>
       </c>
       <c r="I13" s="4" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_5[[#This Row],[dir]], " -rc ", table_6_5[[#This Row],[strand]], " -o ", layouts, "/", table_6_5[[#This Row],[dir_out]], " --subst_type ", table_6_5[[#This Row],[subst_type]], " --layout ", var_6_layout)</f>
-        <v>python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgCD_R1_antisense libraries_4/WT_sgCD_R1_splicing libraries_4/WT_sgCD_R2_antisense libraries_4/WT_sgCD_R2_splicing -rc 0 0 1 1 -o layouts/2DSBanti_CD --subst_type without --layout universal</v>
+        <v>python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgCD_R1_antisense libraries_4/WT_sgCD_R1_splicing libraries_4/WT_sgCD_R2_antisense libraries_4/WT_sgCD_R2_splicing -rc 0 0 1 1 -o layouts/universal/2DSBanti_CD --subst_type without --layout universal</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -26292,10 +25515,10 @@
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="str">
         <f ca="1">_xlfn.TEXTJOIN(CHAR(10), TRUE, table_6_3[command], table_6_4[command], table_6_5[command])</f>
-        <v>python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgAB_R1_sense libraries_4/WT_sgAB_R1_branch libraries_4/WT_sgAB_R1_cmv libraries_4/KO_sgAB_R1_sense libraries_4/KO_sgAB_R1_branch libraries_4/KO_sgAB_R1_cmv libraries_4/WT_sgAB_R2_sense libraries_4/WT_sgAB_R2_branch libraries_4/WT_sgAB_R2_cmv libraries_4/KO_sgAB_R2_sense libraries_4/KO_sgAB_R2_branch libraries_4/KO_sgAB_R2_cmv -rc 0 0 0 0 0 0 1 1 1 1 1 1 -o layouts/2DSB_AB --subst_type without --layout universal
-python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgA_R1_sense libraries_4/WT_sgA_R1_branch libraries_4/WT_sgA_R1_cmv libraries_4/KO_sgA_R1_sense libraries_4/KO_sgA_R1_branch libraries_4/KO_sgA_R1_cmv -o layouts/1DSB_A --subst_type without --layout universal
-python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgB_R2_sense libraries_4/WT_sgB_R2_branch libraries_4/WT_sgB_R2_cmv libraries_4/KO_sgB_R2_sense libraries_4/KO_sgB_R2_branch libraries_4/KO_sgB_R2_cmv -rc 1 1 1 1 1 1 -o layouts/1DSB_B --subst_type without --layout universal
-python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgCD_R1_antisense libraries_4/WT_sgCD_R1_splicing libraries_4/WT_sgCD_R2_antisense libraries_4/WT_sgCD_R2_splicing -rc 0 0 1 1 -o layouts/2DSBanti_CD --subst_type without --layout universal</v>
+        <v>python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgAB_R1_sense libraries_4/WT_sgAB_R1_branch libraries_4/WT_sgAB_R1_cmv libraries_4/KO_sgAB_R1_sense libraries_4/KO_sgAB_R1_branch libraries_4/KO_sgAB_R1_cmv libraries_4/WT_sgAB_R2_sense libraries_4/WT_sgAB_R2_branch libraries_4/WT_sgAB_R2_cmv libraries_4/KO_sgAB_R2_sense libraries_4/KO_sgAB_R2_branch libraries_4/KO_sgAB_R2_cmv -rc 0 0 0 0 0 0 1 1 1 1 1 1 -o layouts/universal/2DSB_AB --subst_type without --layout universal
+python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgA_R1_sense libraries_4/WT_sgA_R1_branch libraries_4/WT_sgA_R1_cmv libraries_4/KO_sgA_R1_sense libraries_4/KO_sgA_R1_branch libraries_4/KO_sgA_R1_cmv -o layouts/universal/1DSB_A --subst_type without --layout universal
+python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgB_R2_sense libraries_4/WT_sgB_R2_branch libraries_4/WT_sgB_R2_cmv libraries_4/KO_sgB_R2_sense libraries_4/KO_sgB_R2_branch libraries_4/KO_sgB_R2_cmv -rc 1 1 1 1 1 1 -o layouts/universal/1DSB_B --subst_type without --layout universal
+python 2_graph_processing/make_common_layout.py -i libraries_4/WT_sgCD_R1_antisense libraries_4/WT_sgCD_R1_splicing libraries_4/WT_sgCD_R2_antisense libraries_4/WT_sgCD_R2_splicing -rc 0 0 1 1 -o layouts/universal/2DSBanti_CD --subst_type without --layout universal</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -26326,10 +25549,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1375107-D76A-4386-B771-6693BBF75061}">
-  <dimension ref="A1:P45"/>
+  <dimension ref="A1:P67"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26364,8 +25587,9 @@
       <c r="E1" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="F1" t="s">
-        <v>183</v>
+      <c r="F1" t="str">
+        <f>IF(var_7_common_layout, var_6_layout, "universal")</f>
+        <v>universal</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>181</v>
@@ -26377,7 +25601,7 @@
         <v>182</v>
       </c>
       <c r="J1">
-        <v>1863</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -26489,19 +25713,19 @@
          )
       )
   )</f>
-        <v>2DSB_AB</v>
+        <v>universal/2DSB_AB</v>
       </c>
       <c r="N3" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>0</v>
       </c>
       <c r="O3" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
       </c>
       <c r="P3" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 </v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -26563,19 +25787,19 @@
          )
       )
   )</f>
-        <v>2DSB_AB</v>
+        <v>universal/2DSB_AB</v>
       </c>
       <c r="N4" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>0</v>
       </c>
       <c r="O4" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
       </c>
       <c r="P4" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 </v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -26637,19 +25861,19 @@
          )
       )
   )</f>
-        <v>2DSB_AB</v>
+        <v>universal/2DSB_AB</v>
       </c>
       <c r="N5" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>0</v>
       </c>
       <c r="O5" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
       </c>
       <c r="P5" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 </v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -26711,19 +25935,19 @@
          )
       )
   )</f>
-        <v>2DSB_AB</v>
+        <v>universal/2DSB_AB</v>
       </c>
       <c r="N6" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>0</v>
       </c>
       <c r="O6" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
       </c>
       <c r="P6" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 </v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -26785,19 +26009,19 @@
          )
       )
   )</f>
-        <v>2DSB_AB</v>
+        <v>universal/2DSB_AB</v>
       </c>
       <c r="N7" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>0</v>
       </c>
       <c r="O7" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
       </c>
       <c r="P7" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 </v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -26859,19 +26083,19 @@
          )
       )
   )</f>
-        <v>2DSB_AB</v>
+        <v>universal/2DSB_AB</v>
       </c>
       <c r="N8" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>0</v>
       </c>
       <c r="O8" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
       </c>
       <c r="P8" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 </v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -26933,19 +26157,19 @@
          )
       )
   )</f>
-        <v>2DSB_AB</v>
+        <v>universal/2DSB_AB</v>
       </c>
       <c r="N9" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>1</v>
       </c>
       <c r="O9" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
       </c>
       <c r="P9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 </v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -27007,19 +26231,19 @@
          )
       )
   )</f>
-        <v>2DSB_AB</v>
+        <v>universal/2DSB_AB</v>
       </c>
       <c r="N10" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>1</v>
       </c>
       <c r="O10" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
       </c>
       <c r="P10" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 </v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -27081,19 +26305,19 @@
          )
       )
   )</f>
-        <v>2DSB_AB</v>
+        <v>universal/2DSB_AB</v>
       </c>
       <c r="N11" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>1</v>
       </c>
       <c r="O11" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
       </c>
       <c r="P11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 </v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -27155,19 +26379,19 @@
          )
       )
   )</f>
-        <v>2DSB_AB</v>
+        <v>universal/2DSB_AB</v>
       </c>
       <c r="N12" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>1</v>
       </c>
       <c r="O12" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
       </c>
       <c r="P12" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 </v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -27229,19 +26453,19 @@
          )
       )
   )</f>
-        <v>2DSB_AB</v>
+        <v>universal/2DSB_AB</v>
       </c>
       <c r="N13" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>1</v>
       </c>
       <c r="O13" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
       </c>
       <c r="P13" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 </v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -27303,19 +26527,19 @@
          )
       )
   )</f>
-        <v>2DSB_AB</v>
+        <v>universal/2DSB_AB</v>
       </c>
       <c r="N14" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>1</v>
       </c>
       <c r="O14" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
       </c>
       <c r="P14" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 </v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -27377,19 +26601,19 @@
          )
       )
   )</f>
-        <v>1DSB_A</v>
+        <v>universal/1DSB_A</v>
       </c>
       <c r="N15" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>0</v>
       </c>
       <c r="O15" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -22 18 </v>
       </c>
       <c r="P15" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 18 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 18 </v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -27451,19 +26675,19 @@
          )
       )
   )</f>
-        <v>1DSB_A</v>
+        <v>universal/1DSB_A</v>
       </c>
       <c r="N16" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>0</v>
       </c>
       <c r="O16" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -22 18 </v>
       </c>
       <c r="P16" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 18 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 18 </v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -27525,19 +26749,19 @@
          )
       )
   )</f>
-        <v>1DSB_A</v>
+        <v>universal/1DSB_A</v>
       </c>
       <c r="N17" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>0</v>
       </c>
       <c r="O17" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -22 18 </v>
       </c>
       <c r="P17" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 18 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 18 </v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -27599,19 +26823,19 @@
          )
       )
   )</f>
-        <v>1DSB_A</v>
+        <v>universal/1DSB_A</v>
       </c>
       <c r="N18" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>0</v>
       </c>
       <c r="O18" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -22 18 </v>
       </c>
       <c r="P18" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 18 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 18 </v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -27673,19 +26897,19 @@
          )
       )
   )</f>
-        <v>1DSB_A</v>
+        <v>universal/1DSB_A</v>
       </c>
       <c r="N19" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>0</v>
       </c>
       <c r="O19" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -22 18 </v>
       </c>
       <c r="P19" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 18 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 18 </v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -27747,19 +26971,19 @@
          )
       )
   )</f>
-        <v>1DSB_A</v>
+        <v>universal/1DSB_A</v>
       </c>
       <c r="N20" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>0</v>
       </c>
       <c r="O20" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -22 18 </v>
       </c>
       <c r="P20" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 18 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 18 </v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -27821,19 +27045,19 @@
          )
       )
   )</f>
-        <v>1DSB_B</v>
+        <v>universal/1DSB_B</v>
       </c>
       <c r="N21" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>1</v>
       </c>
       <c r="O21" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -20 10 </v>
       </c>
       <c r="P21" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -20 10 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -20 10 </v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -27895,19 +27119,19 @@
          )
       )
   )</f>
-        <v>1DSB_B</v>
+        <v>universal/1DSB_B</v>
       </c>
       <c r="N22" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>1</v>
       </c>
       <c r="O22" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -20 10 </v>
       </c>
       <c r="P22" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -20 10 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -20 10 </v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -27969,19 +27193,19 @@
          )
       )
   )</f>
-        <v>1DSB_B</v>
+        <v>universal/1DSB_B</v>
       </c>
       <c r="N23" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>1</v>
       </c>
       <c r="O23" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -20 10 </v>
       </c>
       <c r="P23" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -20 10 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -20 10 </v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -28043,19 +27267,19 @@
          )
       )
   )</f>
-        <v>1DSB_B</v>
+        <v>universal/1DSB_B</v>
       </c>
       <c r="N24" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>1</v>
       </c>
       <c r="O24" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -20 10 </v>
       </c>
       <c r="P24" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -20 10 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -20 10 </v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -28117,19 +27341,19 @@
          )
       )
   )</f>
-        <v>1DSB_B</v>
+        <v>universal/1DSB_B</v>
       </c>
       <c r="N25" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>1</v>
       </c>
       <c r="O25" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -20 10 </v>
       </c>
       <c r="P25" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -20 10 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -20 10 </v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -28191,19 +27415,19 @@
          )
       )
   )</f>
-        <v>1DSB_B</v>
+        <v>universal/1DSB_B</v>
       </c>
       <c r="N26" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>1</v>
       </c>
       <c r="O26" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -20 10 </v>
       </c>
       <c r="P26" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -20 10 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -20 10 </v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -28265,19 +27489,19 @@
          )
       )
   )</f>
-        <v>1DSB_A</v>
+        <v>universal/1DSB_A</v>
       </c>
       <c r="N27" s="9" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>0</v>
       </c>
       <c r="O27" s="9" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -22 18 </v>
       </c>
       <c r="P27" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 18 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 18 </v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -28339,19 +27563,19 @@
          )
       )
   )</f>
-        <v>1DSB_A</v>
+        <v>universal/1DSB_A</v>
       </c>
       <c r="N28" s="9" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>0</v>
       </c>
       <c r="O28" s="9" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -22 18 </v>
       </c>
       <c r="P28" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 18 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 18 </v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -28413,19 +27637,19 @@
          )
       )
   )</f>
-        <v>1DSB_A</v>
+        <v>universal/1DSB_A</v>
       </c>
       <c r="N29" s="9" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>0</v>
       </c>
       <c r="O29" s="9" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -22 18 </v>
       </c>
       <c r="P29" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 18 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 18 </v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
@@ -28487,19 +27711,19 @@
          )
       )
   )</f>
-        <v>1DSB_A</v>
+        <v>universal/1DSB_A</v>
       </c>
       <c r="N30" s="9" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>0</v>
       </c>
       <c r="O30" s="9" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -22 18 </v>
       </c>
       <c r="P30" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 18 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 18 </v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -28561,19 +27785,19 @@
          )
       )
   )</f>
-        <v>1DSB_A</v>
+        <v>universal/1DSB_A</v>
       </c>
       <c r="N31" s="9" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>0</v>
       </c>
       <c r="O31" s="9" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -22 18 </v>
       </c>
       <c r="P31" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 18 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 18 </v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -28635,19 +27859,19 @@
          )
       )
   )</f>
-        <v>1DSB_A</v>
+        <v>universal/1DSB_A</v>
       </c>
       <c r="N32" s="9" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>0</v>
       </c>
       <c r="O32" s="9" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -22 18 </v>
       </c>
       <c r="P32" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 18 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 18 </v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -28709,19 +27933,19 @@
          )
       )
   )</f>
-        <v>1DSB_B</v>
+        <v>universal/1DSB_B</v>
       </c>
       <c r="N33" s="9" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>1</v>
       </c>
       <c r="O33" s="9" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -20 10 </v>
       </c>
       <c r="P33" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -20 10 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -20 10 </v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -28783,19 +28007,19 @@
          )
       )
   )</f>
-        <v>1DSB_B</v>
+        <v>universal/1DSB_B</v>
       </c>
       <c r="N34" s="9" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>1</v>
       </c>
       <c r="O34" s="9" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -20 10 </v>
       </c>
       <c r="P34" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -20 10 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -20 10 </v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -28857,19 +28081,19 @@
          )
       )
   )</f>
-        <v>1DSB_B</v>
+        <v>universal/1DSB_B</v>
       </c>
       <c r="N35" s="9" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>1</v>
       </c>
       <c r="O35" s="9" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -20 10 </v>
       </c>
       <c r="P35" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -20 10 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -20 10 </v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -28931,19 +28155,19 @@
          )
       )
   )</f>
-        <v>1DSB_B</v>
+        <v>universal/1DSB_B</v>
       </c>
       <c r="N36" s="9" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>1</v>
       </c>
       <c r="O36" s="9" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -20 10 </v>
       </c>
       <c r="P36" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -20 10 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -20 10 </v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
@@ -29005,19 +28229,19 @@
          )
       )
   )</f>
-        <v>1DSB_B</v>
+        <v>universal/1DSB_B</v>
       </c>
       <c r="N37" s="9" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>1</v>
       </c>
       <c r="O37" s="9" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -20 10 </v>
       </c>
       <c r="P37" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -20 10 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -20 10 </v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
@@ -29079,19 +28303,19 @@
          )
       )
   )</f>
-        <v>1DSB_B</v>
+        <v>universal/1DSB_B</v>
       </c>
       <c r="N38" s="9" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>1</v>
       </c>
       <c r="O38" s="9" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -20 10 </v>
       </c>
       <c r="P38" s="9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv_30bpDown -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -20 10 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -20 10 </v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -29153,19 +28377,19 @@
          )
       )
   )</f>
-        <v>2DSBanti_CD</v>
+        <v>universal/2DSBanti_CD</v>
       </c>
       <c r="N39" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>0</v>
       </c>
       <c r="O39" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -18 24 </v>
       </c>
       <c r="P39" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_CD -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -18 24 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSBanti_CD -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -18 24 </v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
@@ -29227,19 +28451,19 @@
          )
       )
   )</f>
-        <v>2DSBanti_CD</v>
+        <v>universal/2DSBanti_CD</v>
       </c>
       <c r="N40" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>0</v>
       </c>
       <c r="O40" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -18 24 </v>
       </c>
       <c r="P40" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_splicing -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_CD -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -18 24 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_splicing -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSBanti_CD -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -18 24 </v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
@@ -29301,19 +28525,19 @@
          )
       )
   )</f>
-        <v>2DSBanti_CD</v>
+        <v>universal/2DSBanti_CD</v>
       </c>
       <c r="N41" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>1</v>
       </c>
       <c r="O41" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -18 24 </v>
       </c>
       <c r="P41" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_CD -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -18 24 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSBanti_CD -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -18 24 </v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
@@ -29375,64 +28599,808 @@
          )
       )
   )</f>
-        <v>2DSBanti_CD</v>
+        <v>universal/2DSBanti_CD</v>
       </c>
       <c r="N42" t="b">
         <f ca="1">AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</f>
         <v>1</v>
       </c>
       <c r="O42" t="str">
-        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))))</f>
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -18 24 </v>
       </c>
       <c r="P42" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs_individual, "/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_splicing -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_CD -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -18 24 </v>
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_splicing -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSBanti_CD -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -18 24 </v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>1</v>
+      </c>
+      <c r="B45" s="2" t="str">
+        <f ca="1">OFFSET(table_4_1[], table_7_2[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
+        <v>WT_sgAB_R1_sense_branch</v>
+      </c>
+      <c r="C45" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R1</v>
+      </c>
+      <c r="D45" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>AB</v>
+      </c>
+      <c r="E45" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>2DSB</v>
+      </c>
+      <c r="F45" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>universal/2DSB_AB</v>
+      </c>
+      <c r="G45" s="2" t="b">
+        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="H45" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
+      </c>
+      <c r="I45" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/combined/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 </v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>2</v>
+      </c>
+      <c r="B46" s="2" t="str">
+        <f ca="1">OFFSET(table_4_1[], table_7_2[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
+        <v>WT_sgAB_R1_sense_cmv</v>
+      </c>
+      <c r="C46" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R1</v>
+      </c>
+      <c r="D46" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>AB</v>
+      </c>
+      <c r="E46" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>2DSB</v>
+      </c>
+      <c r="F46" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>universal/2DSB_AB</v>
+      </c>
+      <c r="G46" s="2" t="b">
+        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="H46" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
+      </c>
+      <c r="I46" s="2" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/combined/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 </v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>3</v>
+      </c>
+      <c r="B47" t="str">
+        <f ca="1">OFFSET(table_4_1[], table_7_2[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
+        <v>KO_sgAB_R1_sense_branch</v>
+      </c>
+      <c r="C47" t="str">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R1</v>
+      </c>
+      <c r="D47" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>AB</v>
+      </c>
+      <c r="E47" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>2DSB</v>
+      </c>
+      <c r="F47" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>universal/2DSB_AB</v>
+      </c>
+      <c r="G47" t="b">
+        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="H47" t="str">
+        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
+      </c>
+      <c r="I47" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/combined/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 </v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>4</v>
+      </c>
+      <c r="B48" t="str">
+        <f ca="1">OFFSET(table_4_1[], table_7_2[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
+        <v>KO_sgAB_R1_sense_cmv</v>
+      </c>
+      <c r="C48" t="str">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R1</v>
+      </c>
+      <c r="D48" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>AB</v>
+      </c>
+      <c r="E48" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>2DSB</v>
+      </c>
+      <c r="F48" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>universal/2DSB_AB</v>
+      </c>
+      <c r="G48" t="b">
+        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="H48" t="str">
+        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
+      </c>
+      <c r="I48" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/combined/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 </v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>5</v>
+      </c>
+      <c r="B49" t="str">
+        <f ca="1">OFFSET(table_4_1[], table_7_2[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
+        <v>WT_sgAB_R2_sense_branch</v>
+      </c>
+      <c r="C49" t="str">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R2</v>
+      </c>
+      <c r="D49" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>AB</v>
+      </c>
+      <c r="E49" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>2DSB</v>
+      </c>
+      <c r="F49" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>universal/2DSB_AB</v>
+      </c>
+      <c r="G49" t="b">
+        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H49" t="str">
+        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
+      </c>
+      <c r="I49" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/combined/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 </v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>6</v>
+      </c>
+      <c r="B50" t="str">
+        <f ca="1">OFFSET(table_4_1[], table_7_2[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
+        <v>WT_sgAB_R2_sense_cmv</v>
+      </c>
+      <c r="C50" t="str">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R2</v>
+      </c>
+      <c r="D50" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>AB</v>
+      </c>
+      <c r="E50" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>2DSB</v>
+      </c>
+      <c r="F50" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>universal/2DSB_AB</v>
+      </c>
+      <c r="G50" t="b">
+        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H50" t="str">
+        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
+      </c>
+      <c r="I50" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/combined/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 </v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>7</v>
+      </c>
+      <c r="B51" t="str">
+        <f ca="1">OFFSET(table_4_1[], table_7_2[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
+        <v>KO_sgAB_R2_sense_branch</v>
+      </c>
+      <c r="C51" t="str">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R2</v>
+      </c>
+      <c r="D51" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>AB</v>
+      </c>
+      <c r="E51" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>2DSB</v>
+      </c>
+      <c r="F51" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>universal/2DSB_AB</v>
+      </c>
+      <c r="G51" t="b">
+        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H51" t="str">
+        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
+      </c>
+      <c r="I51" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/combined/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 </v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>8</v>
+      </c>
+      <c r="B52" t="str">
+        <f ca="1">OFFSET(table_4_1[], table_7_2[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
+        <v>KO_sgAB_R2_sense_cmv</v>
+      </c>
+      <c r="C52" t="str">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R2</v>
+      </c>
+      <c r="D52" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>AB</v>
+      </c>
+      <c r="E52" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>2DSB</v>
+      </c>
+      <c r="F52" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>universal/2DSB_AB</v>
+      </c>
+      <c r="G52" t="b">
+        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H52" t="str">
+        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
+      </c>
+      <c r="I52" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/combined/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 </v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>9</v>
+      </c>
+      <c r="B53" t="str">
+        <f ca="1">OFFSET(table_4_1[], table_7_2[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
+        <v>WT_sgA_R1_sense_branch</v>
+      </c>
+      <c r="C53" t="str">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R1</v>
+      </c>
+      <c r="D53" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>A</v>
+      </c>
+      <c r="E53" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1DSB</v>
+      </c>
+      <c r="F53" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>universal/1DSB_A</v>
+      </c>
+      <c r="G53" t="b">
+        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="H53" t="str">
+        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v xml:space="preserve"> --range_x -12 12 --range_y -22 18 </v>
+      </c>
+      <c r="I53" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/combined/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 18 </v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>10</v>
+      </c>
+      <c r="B54" t="str">
+        <f ca="1">OFFSET(table_4_1[], table_7_2[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
+        <v>WT_sgA_R1_sense_cmv</v>
+      </c>
+      <c r="C54" t="str">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R1</v>
+      </c>
+      <c r="D54" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>A</v>
+      </c>
+      <c r="E54" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1DSB</v>
+      </c>
+      <c r="F54" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>universal/1DSB_A</v>
+      </c>
+      <c r="G54" t="b">
+        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="H54" t="str">
+        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v xml:space="preserve"> --range_x -12 12 --range_y -22 18 </v>
+      </c>
+      <c r="I54" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/combined/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 18 </v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>11</v>
+      </c>
+      <c r="B55" t="str">
+        <f ca="1">OFFSET(table_4_1[], table_7_2[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
+        <v>KO_sgA_R1_sense_branch</v>
+      </c>
+      <c r="C55" t="str">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R1</v>
+      </c>
+      <c r="D55" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>A</v>
+      </c>
+      <c r="E55" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1DSB</v>
+      </c>
+      <c r="F55" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>universal/1DSB_A</v>
+      </c>
+      <c r="G55" t="b">
+        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="H55" t="str">
+        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v xml:space="preserve"> --range_x -12 12 --range_y -22 18 </v>
+      </c>
+      <c r="I55" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/combined/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 18 </v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>12</v>
+      </c>
+      <c r="B56" t="str">
+        <f ca="1">OFFSET(table_4_1[], table_7_2[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
+        <v>KO_sgA_R1_sense_cmv</v>
+      </c>
+      <c r="C56" t="str">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R1</v>
+      </c>
+      <c r="D56" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>A</v>
+      </c>
+      <c r="E56" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1DSB</v>
+      </c>
+      <c r="F56" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>universal/1DSB_A</v>
+      </c>
+      <c r="G56" t="b">
+        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="H56" t="str">
+        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v xml:space="preserve"> --range_x -12 12 --range_y -22 18 </v>
+      </c>
+      <c r="I56" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/combined/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 18 </v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>13</v>
+      </c>
+      <c r="B57" t="str">
+        <f ca="1">OFFSET(table_4_1[], table_7_2[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
+        <v>WT_sgB_R2_sense_branch</v>
+      </c>
+      <c r="C57" t="str">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R2</v>
+      </c>
+      <c r="D57" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>B</v>
+      </c>
+      <c r="E57" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1DSB</v>
+      </c>
+      <c r="F57" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>universal/1DSB_B</v>
+      </c>
+      <c r="G57" t="b">
+        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H57" t="str">
+        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v xml:space="preserve"> --range_x -12 12 --range_y -20 10 </v>
+      </c>
+      <c r="I57" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/combined/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -20 10 </v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>14</v>
+      </c>
+      <c r="B58" t="str">
+        <f ca="1">OFFSET(table_4_1[], table_7_2[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
+        <v>WT_sgB_R2_sense_cmv</v>
+      </c>
+      <c r="C58" t="str">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R2</v>
+      </c>
+      <c r="D58" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>B</v>
+      </c>
+      <c r="E58" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1DSB</v>
+      </c>
+      <c r="F58" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>universal/1DSB_B</v>
+      </c>
+      <c r="G58" t="b">
+        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H58" t="str">
+        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v xml:space="preserve"> --range_x -12 12 --range_y -20 10 </v>
+      </c>
+      <c r="I58" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/combined/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -20 10 </v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>15</v>
+      </c>
+      <c r="B59" t="str">
+        <f ca="1">OFFSET(table_4_1[], table_7_2[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
+        <v>KO_sgB_R2_sense_branch</v>
+      </c>
+      <c r="C59" t="str">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R2</v>
+      </c>
+      <c r="D59" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>B</v>
+      </c>
+      <c r="E59" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1DSB</v>
+      </c>
+      <c r="F59" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>universal/1DSB_B</v>
+      </c>
+      <c r="G59" t="b">
+        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H59" t="str">
+        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v xml:space="preserve"> --range_x -12 12 --range_y -20 10 </v>
+      </c>
+      <c r="I59" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/combined/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -20 10 </v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>16</v>
+      </c>
+      <c r="B60" t="str">
+        <f ca="1">OFFSET(table_4_1[], table_7_2[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
+        <v>KO_sgB_R2_sense_cmv</v>
+      </c>
+      <c r="C60" t="str">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>R2</v>
+      </c>
+      <c r="D60" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>B</v>
+      </c>
+      <c r="E60" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1DSB</v>
+      </c>
+      <c r="F60" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>universal/1DSB_B</v>
+      </c>
+      <c r="G60" t="b">
+        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H60" t="str">
+        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
+        <v xml:space="preserve"> --range_x -12 12 --range_y -20 10 </v>
+      </c>
+      <c r="I60" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/combined/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -20 10 </v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>1</v>
+      </c>
+      <c r="B63" s="2" t="str">
+        <f ca="1">OFFSET(table_4_2[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
+        <v>WT_sgCD_R1_antisense_splicing</v>
+      </c>
+      <c r="C63" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
+        <v>R1</v>
+      </c>
+      <c r="D63" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
+        <v>CD</v>
+      </c>
+      <c r="E63" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
+        <v>2DSBanti</v>
+      </c>
+      <c r="F63" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
+        <v>universal/2DSBanti_CD</v>
+      </c>
+      <c r="G63" s="2" t="b">
+        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="H63" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
+        <v xml:space="preserve"> --range_x -12 12 --range_y -18 24 </v>
+      </c>
+      <c r="I63" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/combined/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_3[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense_splicing -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSBanti_CD -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -18 24 </v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>2</v>
+      </c>
+      <c r="B64" s="2" t="str">
+        <f ca="1">OFFSET(table_4_2[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</f>
+        <v>WT_sgCD_R2_antisense_splicing</v>
+      </c>
+      <c r="C64" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[strand]:[strand]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
+        <v>R2</v>
+      </c>
+      <c r="D64" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[hguide]:[hguide]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
+        <v>CD</v>
+      </c>
+      <c r="E64" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[dsb_type]:[dsb_type]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
+        <v>2DSBanti</v>
+      </c>
+      <c r="F64" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
+        <v>universal/2DSBanti_CD</v>
+      </c>
+      <c r="G64" s="2" t="b">
+        <f ca="1">OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="H64" s="2" t="str">
+        <f ca="1">OFFSET(table_7_1[[range_args]:[range_args]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</f>
+        <v xml:space="preserve"> --range_x -12 12 --range_y -18 24 </v>
+      </c>
+      <c r="I64" s="2" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/combined/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_3[[#This Row],[range_args]])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense_splicing -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSBanti_CD -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -18 24 </v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" t="str">
-        <f ca="1">_xlfn.TEXTJOIN(CHAR(10), TRUE, P3:P26,P39,P40,P41,P42)</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -22 20 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 18 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 18 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 18 
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 18 
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 18 
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_A -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -22 18 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -20 10 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -20 10 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -20 10 
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -20 10 
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -20 10 
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv -o plots/graphs/individual/png --layout_dir layouts/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -20 10 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_CD -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -18 24 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_splicing -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_CD -ext png --layout universal --width 2400 --height 1863  --range_x -12 12 --range_y -18 24 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_CD -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -18 24 
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_splicing -o plots/graphs/individual/png --layout_dir layouts/2DSBanti_CD -ext png --layout universal --reverse_complement  --width 2400 --height 1863  --range_x -12 12 --range_y -18 24 </v>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="str">
+        <f ca="1">_xlfn.TEXTJOIN(CHAR(10), TRUE, P3:P26,P39:P42, table_7_2[command], table_7_3[command])</f>
+        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 18 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 18 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 18 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 18 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 18 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 18 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -20 10 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -20 10 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -20 10 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -20 10 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -20 10 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -20 10 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSBanti_CD -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -18 24 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_splicing -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSBanti_CD -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -18 24 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSBanti_CD -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -18 24 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_splicing -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSBanti_CD -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -18 24 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 18 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 18 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 18 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 18 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -20 10 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -20 10 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -20 10 
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -20 10 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense_splicing -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSBanti_CD -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -18 24 
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense_splicing -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSBanti_CD -ext png --layout universal --reverse_complement  --width 2400 --height 1800  --range_x -12 12 --range_y -18 24 </v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="3">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add position of universal layout legend to plot graphs args.
</commit_message>
<xml_diff>
--- a/libinfo.xlsx
+++ b/libinfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tchan\Code\SCMB_Project\RNA-mediated_DSB_repair\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5F43E8-14D5-4850-B9C8-4D53EC01201B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55DBCC6A-174B-44F1-B396-F14F6D7BEE2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="4" activeTab="8" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
   </bookViews>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1530" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1537" uniqueCount="187">
   <si>
     <t>yjl217</t>
   </si>
@@ -649,6 +649,9 @@
   <si>
     <t>plots/graphs</t>
   </si>
+  <si>
+    <t>universal_layout_legend_pos_x</t>
+  </si>
 </sst>
 </file>
 
@@ -767,7 +770,25 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{FFD19645-61C4-4244-A560-0232B787F38C}"/>
   </cellStyles>
-  <dxfs count="194">
+  <dxfs count="200">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -890,9 +911,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1105,6 +1123,9 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1951,7 +1972,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{70502F2F-AE2C-4D63-ADF7-F65702652EBF}" name="table_1_2" displayName="table_1_2" ref="A1:D108" totalsRowShown="0">
   <autoFilter ref="A1:D108" xr:uid="{70502F2F-AE2C-4D63-ADF7-F65702652EBF}"/>
   <tableColumns count="4">
-    <tableColumn id="2" xr3:uid="{BB99DCDA-08D4-474A-ABC3-5229CEAF80CF}" name="id" dataDxfId="193">
+    <tableColumn id="2" xr3:uid="{BB99DCDA-08D4-474A-ABC3-5229CEAF80CF}" name="id" dataDxfId="199">
       <calculatedColumnFormula>INT(MID(table_1_2[[#This Row],[library]], 4, 10))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{5F63B290-093A-48A3-9AFC-EB2FE27DE630}" name="library"/>
@@ -1963,44 +1984,44 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}" name="table_5_1" displayName="table_5_1" ref="A1:M41" totalsRowShown="0" headerRowDxfId="90">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}" name="table_5_1" displayName="table_5_1" ref="A1:M41" totalsRowShown="0" headerRowDxfId="96">
   <autoFilter ref="A1:M41" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
   <tableColumns count="13">
-    <tableColumn id="25" xr3:uid="{43F57146-0E56-46F3-A0E3-717A41010F4A}" name="index" dataDxfId="89"/>
-    <tableColumn id="1" xr3:uid="{B0B3F6B0-7577-49AC-B865-1E873B4DC53C}" name="dir" dataDxfId="88">
+    <tableColumn id="25" xr3:uid="{43F57146-0E56-46F3-A0E3-717A41010F4A}" name="index" dataDxfId="95"/>
+    <tableColumn id="1" xr3:uid="{B0B3F6B0-7577-49AC-B865-1E873B4DC53C}" name="dir" dataDxfId="94">
       <calculatedColumnFormula>table_3_1[[#This Row],[dir]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{D04F356F-9288-416D-ACDA-6BFE128B70D7}" name="control" dataDxfId="87">
+    <tableColumn id="13" xr3:uid="{D04F356F-9288-416D-ACDA-6BFE128B70D7}" name="control" dataDxfId="93">
       <calculatedColumnFormula>table_3_1[[#This Row],[control]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{9C168B22-F534-40D4-947C-918239C33FD9}" name="ref" dataDxfId="86">
+    <tableColumn id="2" xr3:uid="{9C168B22-F534-40D4-947C-918239C33FD9}" name="ref" dataDxfId="92">
       <calculatedColumnFormula>table_3_1[[#This Row],[ref]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{6F64477B-0C66-4251-9156-22307A6D70A0}" name="dsb_pos" dataDxfId="85">
+    <tableColumn id="3" xr3:uid="{6F64477B-0C66-4251-9156-22307A6D70A0}" name="dsb_pos" dataDxfId="91">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_pos]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{D037F4F2-543F-4D7D-AB36-0B253FD61B0D}" name="dsb_type" dataDxfId="84">
+    <tableColumn id="4" xr3:uid="{D037F4F2-543F-4D7D-AB36-0B253FD61B0D}" name="dsb_type" dataDxfId="90">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_type]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{407AC5E6-13CB-409A-8E78-64B8CC121882}" name="dsb_type_command" dataDxfId="83">
+    <tableColumn id="12" xr3:uid="{407AC5E6-13CB-409A-8E78-64B8CC121882}" name="dsb_type_command" dataDxfId="89">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_type_command]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{1A24C844-2A10-4394-818F-0C25A569B414}" name="strand" dataDxfId="82">
+    <tableColumn id="5" xr3:uid="{1A24C844-2A10-4394-818F-0C25A569B414}" name="strand" dataDxfId="88">
       <calculatedColumnFormula>table_3_1[[#This Row],[strand]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{4F0A02F9-5555-489E-BA41-E3CBF81D1114}" name="hguide" dataDxfId="81">
+    <tableColumn id="6" xr3:uid="{4F0A02F9-5555-489E-BA41-E3CBF81D1114}" name="hguide" dataDxfId="87">
       <calculatedColumnFormula>table_3_1[[#This Row],[hguide]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FAE741F2-7C1B-41F2-8875-9F7A2EF40A54}" name="cell" dataDxfId="80">
+    <tableColumn id="7" xr3:uid="{FAE741F2-7C1B-41F2-8875-9F7A2EF40A54}" name="cell" dataDxfId="86">
       <calculatedColumnFormula>table_3_1[[#This Row],[cell]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{FE3ED128-2534-43D1-9244-11AB1FB57650}" name="treatment" dataDxfId="79">
+    <tableColumn id="8" xr3:uid="{FE3ED128-2534-43D1-9244-11AB1FB57650}" name="treatment" dataDxfId="85">
       <calculatedColumnFormula>table_3_1[[#This Row],[treatment]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{65ACBC9C-0EC8-4074-B310-05F4B70BFAD5}" name="subst_type" dataDxfId="78">
+    <tableColumn id="9" xr3:uid="{65ACBC9C-0EC8-4074-B310-05F4B70BFAD5}" name="subst_type" dataDxfId="84">
       <calculatedColumnFormula>"with"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{F80F6FB9-4F35-4819-8285-D77131C6EFCE}" name="command" dataDxfId="77">
+    <tableColumn id="10" xr3:uid="{F80F6FB9-4F35-4819-8285-D77131C6EFCE}" name="command" dataDxfId="83">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2013,40 +2034,40 @@
   <autoFilter ref="A43:M55" xr:uid="{D74A5276-1A50-4DA1-9131-9669404C8622}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{8AC09A63-4226-4C75-8801-68CF93C0F078}" name="index"/>
-    <tableColumn id="2" xr3:uid="{77584C42-D70C-48A4-979A-F4DEA0B31542}" name="dir" dataDxfId="76">
+    <tableColumn id="2" xr3:uid="{77584C42-D70C-48A4-979A-F4DEA0B31542}" name="dir" dataDxfId="82">
       <calculatedColumnFormula>table_3_2[[#This Row],[dir]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{483E3D73-4059-4B65-84EC-5DC4E7008F35}" name="control" dataDxfId="75">
+    <tableColumn id="3" xr3:uid="{483E3D73-4059-4B65-84EC-5DC4E7008F35}" name="control" dataDxfId="81">
       <calculatedColumnFormula>table_3_2[[#This Row],[control]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5859A8DB-4C52-4451-BBB6-C6BEBF497540}" name="ref" dataDxfId="74">
+    <tableColumn id="4" xr3:uid="{5859A8DB-4C52-4451-BBB6-C6BEBF497540}" name="ref" dataDxfId="80">
       <calculatedColumnFormula>table_3_2[[#This Row],[ref]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{06FC4099-C18C-436C-B1E6-9739B71C7F22}" name="dsb_pos" dataDxfId="73">
+    <tableColumn id="5" xr3:uid="{06FC4099-C18C-436C-B1E6-9739B71C7F22}" name="dsb_pos" dataDxfId="79">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_pos]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8F043A8E-C5E7-4596-AE13-3E495C6DB33E}" name="dsb_type" dataDxfId="72">
+    <tableColumn id="6" xr3:uid="{8F043A8E-C5E7-4596-AE13-3E495C6DB33E}" name="dsb_type" dataDxfId="78">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_type]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E2DB136E-6FA9-4095-8B91-F094974333AF}" name="dsb_type_command" dataDxfId="71">
+    <tableColumn id="7" xr3:uid="{E2DB136E-6FA9-4095-8B91-F094974333AF}" name="dsb_type_command" dataDxfId="77">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_type_command]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{55CDC54E-3E43-4365-B1C9-5359F747A157}" name="strand" dataDxfId="70">
+    <tableColumn id="8" xr3:uid="{55CDC54E-3E43-4365-B1C9-5359F747A157}" name="strand" dataDxfId="76">
       <calculatedColumnFormula>table_3_2[[#This Row],[strand]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{056BD8A0-CC40-4C61-9F22-EE7382045F66}" name="hguide" dataDxfId="69">
+    <tableColumn id="9" xr3:uid="{056BD8A0-CC40-4C61-9F22-EE7382045F66}" name="hguide" dataDxfId="75">
       <calculatedColumnFormula>table_3_2[[#This Row],[hguide]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{489E156D-888A-4DDC-BB23-A4721D588249}" name="cell" dataDxfId="68">
+    <tableColumn id="10" xr3:uid="{489E156D-888A-4DDC-BB23-A4721D588249}" name="cell" dataDxfId="74">
       <calculatedColumnFormula>table_3_2[[#This Row],[cell]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{0F1B5F9E-B10D-4258-9052-90BCDC89F0B0}" name="treatment" dataDxfId="67">
+    <tableColumn id="11" xr3:uid="{0F1B5F9E-B10D-4258-9052-90BCDC89F0B0}" name="treatment" dataDxfId="73">
       <calculatedColumnFormula>table_3_2[[#This Row],[treatment]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A2723EF6-80E8-4D8D-A6DC-7556C1996222}" name="subst_type" dataDxfId="66">
+    <tableColumn id="12" xr3:uid="{A2723EF6-80E8-4D8D-A6DC-7556C1996222}" name="subst_type" dataDxfId="72">
       <calculatedColumnFormula>"with"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{02531CCA-6CDE-42BA-80E3-31C0F97A3546}" name="command" dataDxfId="65">
+    <tableColumn id="13" xr3:uid="{02531CCA-6CDE-42BA-80E3-31C0F97A3546}" name="command" dataDxfId="71">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2055,36 +2076,36 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}" name="table_6_3" displayName="table_6_3" ref="A3:I4" totalsRowShown="0" headerRowDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}" name="table_6_3" displayName="table_6_3" ref="A3:I4" totalsRowShown="0" headerRowDxfId="70">
   <autoFilter ref="A3:I4" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}"/>
   <tableColumns count="9">
-    <tableColumn id="25" xr3:uid="{D7EEB429-5A34-4903-8247-E1BD5C0098AE}" name="index" dataDxfId="63"/>
-    <tableColumn id="18" xr3:uid="{BACD6182-9E09-4A02-A171-8DFCB7543380}" name="dir" dataDxfId="62">
+    <tableColumn id="25" xr3:uid="{D7EEB429-5A34-4903-8247-E1BD5C0098AE}" name="index" dataDxfId="69"/>
+    <tableColumn id="18" xr3:uid="{BACD6182-9E09-4A02-A171-8DFCB7543380}" name="dir" dataDxfId="68">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 12, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{39C35B5A-7D06-4895-BF0F-A803A5F94E2E}" name="reverse_complement" dataDxfId="61">
+    <tableColumn id="2" xr3:uid="{39C35B5A-7D06-4895-BF0F-A803A5F94E2E}" name="reverse_complement" dataDxfId="67">
       <calculatedColumnFormula array="1">_xlfn.TEXTJOIN(
   " ",
   TRUE,
   IF(OFFSET(table_3_1[[strand]:[strand]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 12, 1) = "R1", 0, 1)
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{F617BC3E-90A8-4E63-B2A4-EAC9DE705FC7}" name="control" dataDxfId="60">
+    <tableColumn id="13" xr3:uid="{F617BC3E-90A8-4E63-B2A4-EAC9DE705FC7}" name="control" dataDxfId="66">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 6 * (table_6_3[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{8E20D9FC-49B1-428A-AC5E-AEDADB1473AC}" name="dsb_type" dataDxfId="59">
+    <tableColumn id="4" xr3:uid="{8E20D9FC-49B1-428A-AC5E-AEDADB1473AC}" name="dsb_type" dataDxfId="65">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], 12 * (table_6_3[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="33" xr3:uid="{8FF7E83A-9135-4A64-965C-48368A6C0367}" name="hguide">
       <calculatedColumnFormula array="1">OFFSET(table_3_1[[hguide]:[hguide]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{FB278FFE-A956-4B0C-8CC3-6A0324CBCA11}" name="subst_type" dataDxfId="58">
+    <tableColumn id="9" xr3:uid="{FB278FFE-A956-4B0C-8CC3-6A0324CBCA11}" name="subst_type" dataDxfId="64">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{E4089767-2E77-4296-9392-7BCD64E1E62D}" name="dir_out" dataDxfId="57">
+    <tableColumn id="19" xr3:uid="{E4089767-2E77-4296-9392-7BCD64E1E62D}" name="dir_out" dataDxfId="63">
       <calculatedColumnFormula>_xlfn.CONCAT(var_6_layout, "/", table_6_3[[#This Row],[dsb_type]], "_", table_6_3[[#This Row],[hguide]], IF(table_6_3[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_3[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{8BD09F85-30B0-46CA-A0E3-2CC4F3FB2BD0}" name="command" dataDxfId="56">
+    <tableColumn id="10" xr3:uid="{8BD09F85-30B0-46CA-A0E3-2CC4F3FB2BD0}" name="command" dataDxfId="62">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_3[[#This Row],[dir]], IF(NOT(ISNA(table_6_3[[#This Row],[reverse_complement]])), _xlfn.CONCAT(" -rc ", table_6_3[[#This Row],[reverse_complement]]), ""), " -o ", layouts, "/", table_6_3[[#This Row],[dir_out]], " --subst_type ", table_6_3[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2093,32 +2114,32 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}" name="table_6_4" displayName="table_6_4" ref="A7:I9" totalsRowShown="0" headerRowDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}" name="table_6_4" displayName="table_6_4" ref="A7:I9" totalsRowShown="0" headerRowDxfId="61">
   <autoFilter ref="A7:I9" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}"/>
   <tableColumns count="9">
-    <tableColumn id="25" xr3:uid="{4FA5A2E4-C9F7-4673-98E1-BCCE618B100D}" name="index" dataDxfId="54"/>
-    <tableColumn id="18" xr3:uid="{155653FE-38BD-4542-A5AE-2B40B0FD52C7}" name="dir" dataDxfId="53">
+    <tableColumn id="25" xr3:uid="{4FA5A2E4-C9F7-4673-98E1-BCCE618B100D}" name="index" dataDxfId="60"/>
+    <tableColumn id="18" xr3:uid="{155653FE-38BD-4542-A5AE-2B40B0FD52C7}" name="dir" dataDxfId="59">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 6, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{05E960C2-864E-41C3-A84E-DF767C09AA42}" name="reverse_complement" dataDxfId="52">
+    <tableColumn id="34" xr3:uid="{05E960C2-864E-41C3-A84E-DF767C09AA42}" name="reverse_complement" dataDxfId="58">
       <calculatedColumnFormula>IF(table_6_4[[#This Row],[hguide]]="A",NA(), IF(var_6_layout = "universal", "1 1 1 1 1 1", NA()))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{9EA58FA8-5496-4600-905A-95909513339B}" name="control" dataDxfId="51">
+    <tableColumn id="13" xr3:uid="{9EA58FA8-5496-4600-905A-95909513339B}" name="control" dataDxfId="57">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 6 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{46390A5F-98AD-4211-85B4-A4DD8E31C40C}" name="dsb_type" dataDxfId="50">
+    <tableColumn id="4" xr3:uid="{46390A5F-98AD-4211-85B4-A4DD8E31C40C}" name="dsb_type" dataDxfId="56">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="35" xr3:uid="{5BD83012-469D-4202-9584-AA182CDF11F9}" name="hguide">
       <calculatedColumnFormula array="1">OFFSET(table_3_1[[hguide]:[hguide]], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{123049FA-F284-452C-8FDD-63F409D9967F}" name="subst_type" dataDxfId="49">
+    <tableColumn id="9" xr3:uid="{123049FA-F284-452C-8FDD-63F409D9967F}" name="subst_type" dataDxfId="55">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{CFCDDB26-095C-4395-82E2-37B45B0CDEAD}" name="dir_out" dataDxfId="22">
+    <tableColumn id="19" xr3:uid="{CFCDDB26-095C-4395-82E2-37B45B0CDEAD}" name="dir_out" dataDxfId="54">
       <calculatedColumnFormula>_xlfn.CONCAT(var_6_layout, "/", table_6_4[[#This Row],[dsb_type]], "_", table_6_4[[#This Row],[hguide]], IF(table_6_4[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_4[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{DC6C9CBA-5796-4FFE-878D-BB47DC276187}" name="command" dataDxfId="48">
+    <tableColumn id="10" xr3:uid="{DC6C9CBA-5796-4FFE-878D-BB47DC276187}" name="command" dataDxfId="53">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_4[[#This Row],[dir]], IF(NOT(ISNA(table_6_4[[#This Row],[reverse_complement]])), _xlfn.CONCAT(" -rc ", table_6_4[[#This Row],[reverse_complement]]), ""), " -o ", layouts, "/", table_6_4[[#This Row],[dir_out]], " --subst_type ", table_6_4[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2127,36 +2148,36 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}" name="table_6_5" displayName="table_6_5" ref="A12:I13" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}" name="table_6_5" displayName="table_6_5" ref="A12:I13" totalsRowShown="0" headerRowDxfId="52" headerRowBorderDxfId="51" tableBorderDxfId="50">
   <autoFilter ref="A12:I13" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{0F421990-E775-4F35-92AF-6BA19E0E8AEE}" name="index"/>
-    <tableColumn id="2" xr3:uid="{81FE7256-F482-4A2C-902D-871C80C1D881}" name="dir" dataDxfId="44">
+    <tableColumn id="2" xr3:uid="{81FE7256-F482-4A2C-902D-871C80C1D881}" name="dir" dataDxfId="49">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]:[index]] - 1), 0, 4, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E9F8E6A0-B4A7-475B-9ED2-9F2A4A9EB628}" name="strand" dataDxfId="43">
+    <tableColumn id="3" xr3:uid="{E9F8E6A0-B4A7-475B-9ED2-9F2A4A9EB628}" name="strand" dataDxfId="48">
       <calculatedColumnFormula array="1">_xlfn.TEXTJOIN(
   " ",
   TRUE,
   IF(OFFSET(table_3_1[[strand]:[strand]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]:[index]] - 1), 0,4, 1) = "R1", 0, 1)
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{70821CEE-FFC4-44AB-ACF6-DA81A4B053E6}" name="control" dataDxfId="42">
+    <tableColumn id="6" xr3:uid="{70821CEE-FFC4-44AB-ACF6-DA81A4B053E6}" name="control" dataDxfId="47">
       <calculatedColumnFormula>OFFSET(table_3_1[control], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{FA9180EA-3AA0-451A-ACAC-78776C7CB75D}" name="dsb_type" dataDxfId="41">
+    <tableColumn id="5" xr3:uid="{FA9180EA-3AA0-451A-ACAC-78776C7CB75D}" name="dsb_type" dataDxfId="46">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{E0783723-9246-4BF6-A5DA-E000EA1E5E87}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DE820E4E-FF8B-435B-B07F-D397029AF597}" name="hguide" dataDxfId="40">
+    <tableColumn id="4" xr3:uid="{DE820E4E-FF8B-435B-B07F-D397029AF597}" name="hguide" dataDxfId="45">
       <calculatedColumnFormula>OFFSET(table_3_1[[hguide]:[hguide]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{3D97DBDD-03E9-4A6C-BADA-D01B27A8EE51}" name="dir_out" dataDxfId="39">
+    <tableColumn id="9" xr3:uid="{3D97DBDD-03E9-4A6C-BADA-D01B27A8EE51}" name="dir_out" dataDxfId="44">
       <calculatedColumnFormula>_xlfn.CONCAT(var_6_layout, "/", table_6_5[[#This Row],[dsb_type]], "_", table_6_5[[#This Row],[hguide]], IF(table_6_5[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_5[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5E7626AE-E376-4C60-BA64-B24F95580083}" name="command" dataDxfId="38">
+    <tableColumn id="10" xr3:uid="{5E7626AE-E376-4C60-BA64-B24F95580083}" name="command" dataDxfId="43">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_5[[#This Row],[dir]], " -rc ", table_6_5[[#This Row],[strand]], " -o ", layouts, "/", table_6_5[[#This Row],[dir_out]], " --subst_type ", table_6_5[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2165,44 +2186,44 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{86CE8E4A-18BF-427A-81F0-F9655767A016}" name="table_7_1" displayName="table_7_1" ref="A2:P42" totalsRowShown="0" headerRowDxfId="37">
-  <autoFilter ref="A2:P42" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
-  <tableColumns count="16">
-    <tableColumn id="25" xr3:uid="{C323C376-24D3-4404-9E0F-6E9361862271}" name="index" dataDxfId="36"/>
-    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{86CE8E4A-18BF-427A-81F0-F9655767A016}" name="table_7_1" displayName="table_7_1" ref="A2:R42" totalsRowShown="0" headerRowDxfId="42">
+  <autoFilter ref="A2:R42" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
+  <tableColumns count="18">
+    <tableColumn id="25" xr3:uid="{C323C376-24D3-4404-9E0F-6E9361862271}" name="index" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="40">
       <calculatedColumnFormula>OFFSET(table_3_1[[dir]:[dir]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="34">
+    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="39">
       <calculatedColumnFormula>OFFSET(table_3_1[[control]:[control]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="33">
+    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="38">
       <calculatedColumnFormula>OFFSET(table_3_1[[ref]:[ref]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="32">
+    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="37">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_pos]:[dsb_pos]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="31">
+    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="36">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_type]:[dsb_type]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="30">
+    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="35">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_type_command]:[dsb_type_command]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="29">
+    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="34">
       <calculatedColumnFormula>OFFSET(table_3_1[[strand]:[strand]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="28">
+    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="33">
       <calculatedColumnFormula>OFFSET(table_3_1[[hguide]:[hguide]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="27">
+    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="32">
       <calculatedColumnFormula>OFFSET(table_3_1[[cell]:[cell]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="26">
+    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="31">
       <calculatedColumnFormula>OFFSET(table_3_1[[treatment]:[treatment]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="25">
+    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="30">
       <calculatedColumnFormula>"without"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="24">
+    <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="29">
       <calculatedColumnFormula>IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
       OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
       IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
@@ -2214,14 +2235,20 @@
       )
   )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{7AF47D8C-A10C-454A-8FE8-6D4A4FFD2B60}" name="reverse_complement" dataDxfId="23">
+    <tableColumn id="11" xr3:uid="{7AF47D8C-A10C-454A-8FE8-6D4A4FFD2B60}" name="reverse_complement" dataDxfId="28">
       <calculatedColumnFormula>AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{0D90823C-DABB-4D5B-952B-ECA267C2D98A}" name="range_args" dataDxfId="1">
+    <tableColumn id="15" xr3:uid="{0D90823C-DABB-4D5B-952B-ECA267C2D98A}" name="range_args" dataDxfId="27">
       <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="21">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</calculatedColumnFormula>
+    <tableColumn id="17" xr3:uid="{891739FF-B093-4EE5-A0A2-20948C58CB96}" name="universal_layout_legend_pos_x" dataDxfId="3">
+      <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 10, IF(table_7_1[[#This Row],[hguide]]="A", 10, IF(table_7_1[[#This Row],[hguide]]="B", 10, IF(table_7_1[[#This Row],[hguide]]="CD", 10, NA())))), NA())</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="16" xr3:uid="{680D5200-6ABF-4323-82E5-C6AF5DA257FD}" name="output_dir" dataDxfId="5">
+      <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/individual/", var_7_ext)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="4">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], IF(NOT(ISNA(table_7_1[[#This Row],[universal_layout_legend_pos_x]])), _xlfn.CONCAT(" --universal_layout_legend_pos_x ", table_7_1[[#This Row],[universal_layout_legend_pos_x]], "")))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2229,33 +2256,39 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}" name="table_7_2" displayName="table_7_2" ref="A44:I60" totalsRowShown="0" headerRowDxfId="20">
-  <autoFilter ref="A44:I60" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{B2B7DB73-4221-4AF0-A850-325F3752E3E0}" name="index" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{7CBFD0EC-49AE-431E-A905-A56D19FE8F5B}" name="dir" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}" name="table_7_2" displayName="table_7_2" ref="A44:K60" totalsRowShown="0" headerRowDxfId="26">
+  <autoFilter ref="A44:K60" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{B2B7DB73-4221-4AF0-A850-325F3752E3E0}" name="index" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{7CBFD0EC-49AE-431E-A905-A56D19FE8F5B}" name="dir" dataDxfId="24">
       <calculatedColumnFormula>OFFSET(table_4_1[], table_7_2[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8B726DB7-A763-4D99-9E71-D69E0FA3D7BF}" name="strand" dataDxfId="17">
+    <tableColumn id="3" xr3:uid="{8B726DB7-A763-4D99-9E71-D69E0FA3D7BF}" name="strand" dataDxfId="23">
       <calculatedColumnFormula>OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E7E8C40B-8285-4EE4-A61D-1F147432D708}" name="hguide" dataDxfId="16">
+    <tableColumn id="5" xr3:uid="{E7E8C40B-8285-4EE4-A61D-1F147432D708}" name="hguide" dataDxfId="22">
       <calculatedColumnFormula>OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{64B9691C-2BDA-4EE7-B149-7349BFA40A22}" name="dsb_type" dataDxfId="15">
+    <tableColumn id="7" xr3:uid="{64B9691C-2BDA-4EE7-B149-7349BFA40A22}" name="dsb_type" dataDxfId="21">
       <calculatedColumnFormula>OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{46F7ABEC-3D59-449F-B3B9-3B53D4C4E17C}" name="common_layout_dir" dataDxfId="14">
+    <tableColumn id="2" xr3:uid="{46F7ABEC-3D59-449F-B3B9-3B53D4C4E17C}" name="common_layout_dir" dataDxfId="20">
       <calculatedColumnFormula>OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{BFEA7E87-08AD-4F58-8B7D-A592368549F0}" name="reverse_complement" dataDxfId="13">
+    <tableColumn id="8" xr3:uid="{BFEA7E87-08AD-4F58-8B7D-A592368549F0}" name="reverse_complement" dataDxfId="19">
       <calculatedColumnFormula>OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{928832B4-7BAB-42E7-88BC-BB633DA53A2E}" name="range_args" dataDxfId="12">
+    <tableColumn id="9" xr3:uid="{928832B4-7BAB-42E7-88BC-BB633DA53A2E}" name="range_args" dataDxfId="18">
       <calculatedColumnFormula>OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{FEA012AC-7DC4-4D11-9B59-A05887E08F6E}" name="command" dataDxfId="0">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/combined/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]])</calculatedColumnFormula>
+    <tableColumn id="11" xr3:uid="{E157268B-09A6-4B13-AD6D-24B6BD4C0B56}" name="universal_layout_legend_pos_x" dataDxfId="2">
+      <calculatedColumnFormula>OFFSET(table_7_1[[universal_layout_legend_pos_x]:[universal_layout_legend_pos_x]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{28F0CC58-CEE1-4245-A4B6-361813C46856}" name="output_dir" dataDxfId="6">
+      <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/combined/", var_7_ext)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{FEA012AC-7DC4-4D11-9B59-A05887E08F6E}" name="command" dataDxfId="7">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2263,32 +2296,38 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}" name="table_7_3" displayName="table_7_3" ref="A62:I64" totalsRowShown="0" headerRowDxfId="11">
-  <autoFilter ref="A62:I64" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{E718984E-FC22-4321-9162-791892D20032}" name="index" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{A71ABC91-B291-4CD9-A2A1-F6CA41CEE59E}" name="dir" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}" name="table_7_3" displayName="table_7_3" ref="A62:K64" totalsRowShown="0" headerRowDxfId="17">
+  <autoFilter ref="A62:K64" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{E718984E-FC22-4321-9162-791892D20032}" name="index" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{A71ABC91-B291-4CD9-A2A1-F6CA41CEE59E}" name="dir" dataDxfId="15">
       <calculatedColumnFormula>OFFSET(table_4_2[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8D7F2EAB-990D-439F-AE1F-6FB6AFC6C4B1}" name="strand" dataDxfId="8">
+    <tableColumn id="3" xr3:uid="{8D7F2EAB-990D-439F-AE1F-6FB6AFC6C4B1}" name="strand" dataDxfId="14">
       <calculatedColumnFormula>OFFSET(table_7_1[[strand]:[strand]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B8ABFFB9-C4F5-4866-8F37-B49F31C44F20}" name="hguide" dataDxfId="7">
+    <tableColumn id="5" xr3:uid="{B8ABFFB9-C4F5-4866-8F37-B49F31C44F20}" name="hguide" dataDxfId="13">
       <calculatedColumnFormula>OFFSET(table_7_1[[hguide]:[hguide]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3835BF64-C6A9-440B-96F5-A2332AB91438}" name="dsb_type" dataDxfId="6">
+    <tableColumn id="7" xr3:uid="{3835BF64-C6A9-440B-96F5-A2332AB91438}" name="dsb_type" dataDxfId="12">
       <calculatedColumnFormula>OFFSET(table_7_1[[dsb_type]:[dsb_type]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{C07D080E-B5A2-43FC-84BA-BCBD008F3B26}" name="common_layout_dir" dataDxfId="5">
+    <tableColumn id="2" xr3:uid="{C07D080E-B5A2-43FC-84BA-BCBD008F3B26}" name="common_layout_dir" dataDxfId="11">
       <calculatedColumnFormula>OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{6E360CD4-3BFD-4CC3-A93F-137C46B62651}" name="reverse_complement" dataDxfId="4">
+    <tableColumn id="8" xr3:uid="{6E360CD4-3BFD-4CC3-A93F-137C46B62651}" name="reverse_complement" dataDxfId="10">
       <calculatedColumnFormula>OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{A1862EF0-F072-4796-964D-7EDA8C8787B0}" name="range_args" dataDxfId="3">
+    <tableColumn id="9" xr3:uid="{A1862EF0-F072-4796-964D-7EDA8C8787B0}" name="range_args" dataDxfId="9">
       <calculatedColumnFormula>OFFSET(table_7_1[[range_args]:[range_args]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{D5ADEB9F-0405-4E9D-BDA9-7ECD31E23490}" name="command" dataDxfId="2">
+    <tableColumn id="11" xr3:uid="{312C98E0-05A4-4DD6-86F6-6BFBF9058DC2}" name="universal_layout_legend_pos_x" dataDxfId="0">
+      <calculatedColumnFormula>OFFSET(table_7_1[[universal_layout_legend_pos_x]:[universal_layout_legend_pos_x]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{28284CC2-E402-4A85-83F5-4FC36722329E}" name="output_dir" dataDxfId="1">
+      <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/combined/", var_7_ext)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{D5ADEB9F-0405-4E9D-BDA9-7ECD31E23490}" name="command" dataDxfId="8">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/combined/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_3[[#This Row],[range_args]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2297,10 +2336,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22A90416-B904-4D3D-A6DB-EFCB9FD1EAED}" name="table_1" displayName="table_1" ref="A1:O173" totalsRowShown="0" headerRowDxfId="192">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22A90416-B904-4D3D-A6DB-EFCB9FD1EAED}" name="table_1" displayName="table_1" ref="A1:O173" totalsRowShown="0" headerRowDxfId="198">
   <autoFilter ref="A1:O173" xr:uid="{22A90416-B904-4D3D-A6DB-EFCB9FD1EAED}"/>
   <tableColumns count="15">
-    <tableColumn id="15" xr3:uid="{A06DA701-31D6-44A5-8655-82CAD7E3082B}" name="index" dataDxfId="191"/>
+    <tableColumn id="15" xr3:uid="{A06DA701-31D6-44A5-8655-82CAD7E3082B}" name="index" dataDxfId="197"/>
     <tableColumn id="1" xr3:uid="{5C1CDEE9-AAC7-4E12-B88F-1314CF422335}" name="library"/>
     <tableColumn id="2" xr3:uid="{D4B174CF-F774-4DA7-B75D-573BC94EE10F}" name="cell"/>
     <tableColumn id="3" xr3:uid="{83898EC9-96DA-46D4-B0B8-F68C7607DCF2}" name="control"/>
@@ -2308,25 +2347,25 @@
     <tableColumn id="5" xr3:uid="{81A143FE-8E74-4182-8124-E697DD5A7C62}" name="hguide"/>
     <tableColumn id="6" xr3:uid="{4A316E6A-69F3-4B78-9C01-4675AEB656FA}" name="treatment"/>
     <tableColumn id="7" xr3:uid="{25B8E763-346D-4756-8B58-D3C8CB103545}" name="strand"/>
-    <tableColumn id="8" xr3:uid="{4B708639-BB19-4DC1-A57D-214FA0EFB1EA}" name="dsb_pos" dataDxfId="190">
+    <tableColumn id="8" xr3:uid="{4B708639-BB19-4DC1-A57D-214FA0EFB1EA}" name="dsb_pos" dataDxfId="196">
       <calculatedColumnFormula array="1">IF(E2="2DSB", IF(H2="R1", 67, 46), IF(E2="1DSB", IF(H2="R1", 67, 46), IF(E2="2DSBanti", IF(H2="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{CCF6021C-1B60-4954-A92E-3F2848564215}" name="file_in" dataDxfId="189">
+    <tableColumn id="9" xr3:uid="{CCF6021C-1B60-4954-A92E-3F2848564215}" name="file_in" dataDxfId="195">
       <calculatedColumnFormula>IF(OR(table_1[[#This Row],[control]]="none", table_1[[#This Row],[control]]="30bpDown"), _xlfn.CONCAT(table_1[[#This Row],[library]], IF(table_1[[#This Row],[dsb_type]] = "2DSBanti", "_anti", ""), "_",table_1[[#This Row],[strand]],"_", IF(LEFT(table_1[[#This Row],[dsb_type]], 1)="2","2DSBs", table_1[[#This Row],[hguide]]), ".sam"), _xlfn.CONCAT(table_1[[#This Row],[library]], "_NHEJ_", IF(table_1[[#This Row],[hguide]]="sgA", "hg39", IF(table_1[[#This Row],[hguide]]="sgB", "hg42", "2DSB")), "_", table_1[[#This Row],[strand]], ".sam"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{58220462-2A11-4DAD-A247-C0871AFCFDB4}" name="file_out" dataDxfId="188">
+    <tableColumn id="10" xr3:uid="{58220462-2A11-4DAD-A247-C0871AFCFDB4}" name="file_out" dataDxfId="194">
       <calculatedColumnFormula>_xlfn.CONCAT(table_1[[#This Row],[library]], "_", table_1[[#This Row],[cell]], "_", table_1[[#This Row],[hguide]], "_", table_1[[#This Row],[strand]], "_", table_1[[#This Row],[treatment]], IF(table_1[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_1[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{775EE7A9-3C78-4568-BF98-500DE451177C}" name="ref" dataDxfId="187">
+    <tableColumn id="11" xr3:uid="{775EE7A9-3C78-4568-BF98-500DE451177C}" name="ref" dataDxfId="193">
       <calculatedColumnFormula>_xlfn.CONCAT(table_1[[#This Row],[dsb_type]],"_", table_1[[#This Row],[strand]],"_", table_1[[#This Row],[treatment]], ".fa")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{5B945FB6-D054-40C4-AAEF-BB50B19F8936}" name="total_reads" dataDxfId="186">
+    <tableColumn id="12" xr3:uid="{5B945FB6-D054-40C4-AAEF-BB50B19F8936}" name="total_reads" dataDxfId="192">
       <calculatedColumnFormula>VLOOKUP(INT(MID(table_1[[#This Row],[library]], 4, 10)), table_1_2[#All], IF(table_1[[#This Row],[strand]]="R1", 3, 4))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{66485B06-471E-47D3-BA91-FC751F58FA5A}" name="min_length" dataDxfId="185">
+    <tableColumn id="13" xr3:uid="{66485B06-471E-47D3-BA91-FC751F58FA5A}" name="min_length" dataDxfId="191">
       <calculatedColumnFormula>IF(LEFT(table_1[[#This Row],[dsb_type]], 1) = "2", 50, 130)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{DF3C46EA-690D-4E6A-99CF-BBC2B2F74AFF}" name="command_filter_nhej" dataDxfId="184">
+    <tableColumn id="14" xr3:uid="{DF3C46EA-690D-4E6A-99CF-BBC2B2F74AFF}" name="command_filter_nhej" dataDxfId="190">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", table_1[[#This Row],[file_in]], " -ref ref_seq/", table_1[[#This Row],[ref]], " -o ", libraries_2, "/", table_1[[#This Row],[file_out]], ".tsv", " --min_length ", table_1[[#This Row],[min_length]], " -dsb ", table_1[[#This Row],[dsb_pos]], " --quiet")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2335,38 +2374,38 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}" name="table_2_1" displayName="table_2_1" ref="A1:S41" totalsRowShown="0" headerRowDxfId="183">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}" name="table_2_1" displayName="table_2_1" ref="A1:S41" totalsRowShown="0" headerRowDxfId="189">
   <autoFilter ref="A1:S41" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{C373869E-A92E-4B06-B8E5-C5A873420ED4}" name="index" dataDxfId="182"/>
-    <tableColumn id="2" xr3:uid="{A28AAC50-FA09-494A-B052-8489F07A5A70}" name="ref" dataDxfId="181">
+    <tableColumn id="1" xr3:uid="{C373869E-A92E-4B06-B8E5-C5A873420ED4}" name="index" dataDxfId="188"/>
+    <tableColumn id="2" xr3:uid="{A28AAC50-FA09-494A-B052-8489F07A5A70}" name="ref" dataDxfId="187">
       <calculatedColumnFormula>OFFSET(table_1[ref], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{07D57089-9737-4983-8884-C4ACCDCFF6CB}" name="control" dataDxfId="180">
+    <tableColumn id="18" xr3:uid="{07D57089-9737-4983-8884-C4ACCDCFF6CB}" name="control" dataDxfId="186">
       <calculatedColumnFormula>OFFSET(table_1[control], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{C6423FEA-272F-48D3-BC6A-909FCA937DA9}" name="dsb_type" dataDxfId="179">
+    <tableColumn id="19" xr3:uid="{C6423FEA-272F-48D3-BC6A-909FCA937DA9}" name="dsb_type" dataDxfId="185">
       <calculatedColumnFormula>OFFSET(table_1[dsb_type], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B8F61088-5FFA-4860-BF4E-1BFB301A31D9}" name="dsb_pos" dataDxfId="178">
+    <tableColumn id="3" xr3:uid="{B8F61088-5FFA-4860-BF4E-1BFB301A31D9}" name="dsb_pos" dataDxfId="184">
       <calculatedColumnFormula>OFFSET(table_1[dsb_pos], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{524D5B3D-BB20-420D-B7E9-93A7F77CA728}" name="cell" dataDxfId="177">
+    <tableColumn id="4" xr3:uid="{524D5B3D-BB20-420D-B7E9-93A7F77CA728}" name="cell" dataDxfId="183">
       <calculatedColumnFormula>OFFSET(table_1[cell], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{CC918D20-5D79-4223-9717-2CA0EFFA213F}" name="strand" dataDxfId="176">
+    <tableColumn id="5" xr3:uid="{CC918D20-5D79-4223-9717-2CA0EFFA213F}" name="strand" dataDxfId="182">
       <calculatedColumnFormula>OFFSET(table_1[strand], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B2851465-D533-4787-80C4-E844BB2ABB8C}" name="treatment" dataDxfId="175">
+    <tableColumn id="6" xr3:uid="{B2851465-D533-4787-80C4-E844BB2ABB8C}" name="treatment" dataDxfId="181">
       <calculatedColumnFormula>OFFSET(table_1[treatment], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{849BE448-7739-4815-A2C5-5843F62D83D7}" name="hguide" dataDxfId="174">
+    <tableColumn id="7" xr3:uid="{849BE448-7739-4815-A2C5-5843F62D83D7}" name="hguide" dataDxfId="180">
       <calculatedColumnFormula>OFFSET(table_1[hguide], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{343716D9-C3A9-4F90-A58A-42B1B9C79EBF}" name="output_dir" dataDxfId="173">
+    <tableColumn id="8" xr3:uid="{343716D9-C3A9-4F90-A58A-42B1B9C79EBF}" name="output_dir" dataDxfId="179">
       <calculatedColumnFormula>_xlfn.CONCAT(table_2_1[[#This Row],[cell]], "_", table_2_1[[#This Row],[hguide]], "_", table_2_1[[#This Row],[strand]], "_", table_2_1[[#This Row],[treatment]], IF(table_2_1[[#This Row],[control]]&lt;&gt;"none",_xlfn.CONCAT("_", table_2_1[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D29558AA-D418-4CDD-81AE-A987E7BC501D}" name="input_1" dataDxfId="172">
+    <tableColumn id="9" xr3:uid="{D29558AA-D418-4CDD-81AE-A987E7BC501D}" name="input_1" dataDxfId="178">
       <calculatedColumnFormula array="1">OFFSET(table_1[[file_out]:[file_out]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 11, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="22" xr3:uid="{3F29C0D1-58A3-430E-AAAA-9F679DCA46D6}" name="input_2">
@@ -2378,19 +2417,19 @@
     <tableColumn id="20" xr3:uid="{28521A62-94B3-4C7C-AF90-F4E2F4163D29}" name="input_4">
       <calculatedColumnFormula array="1">OFFSET(table_1[[file_out]:[file_out]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 11, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{E2ABF5A3-B032-47F7-9141-9F269EFD9D49}" name="total_reads_1" dataDxfId="171">
+    <tableColumn id="10" xr3:uid="{E2ABF5A3-B032-47F7-9141-9F269EFD9D49}" name="total_reads_1" dataDxfId="177">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{C7B1BE14-3BD6-413B-8575-DE9712F9761A}" name="total_reads_2" dataDxfId="170">
+    <tableColumn id="12" xr3:uid="{C7B1BE14-3BD6-413B-8575-DE9712F9761A}" name="total_reads_2" dataDxfId="176">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{6A8CE344-45B9-42E3-95D8-8EB6A485D968}" name="total_reads_3" dataDxfId="169">
+    <tableColumn id="14" xr3:uid="{6A8CE344-45B9-42E3-95D8-8EB6A485D968}" name="total_reads_3" dataDxfId="175">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{AC170216-9CAE-43B8-A8E2-8FE1529F6D55}" name="total_reads_4" dataDxfId="168">
+    <tableColumn id="16" xr3:uid="{AC170216-9CAE-43B8-A8E2-8FE1529F6D55}" name="total_reads_4" dataDxfId="174">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{A285A0DD-6F6D-404D-AE2A-0D1FC3DDB459}" name="command" dataDxfId="167">
+    <tableColumn id="17" xr3:uid="{A285A0DD-6F6D-404D-AE2A-0D1FC3DDB459}" name="command" dataDxfId="173">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2402,41 +2441,41 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{7D969AC7-2D2F-45B0-BA99-D174130B0A52}" name="table_2_2" displayName="table_2_2" ref="A44:M56" totalsRowShown="0">
   <autoFilter ref="A44:M56" xr:uid="{7D969AC7-2D2F-45B0-BA99-D174130B0A52}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{D612E3DF-AA8E-4EE0-9306-7903B4821992}" name="index" dataDxfId="166"/>
-    <tableColumn id="2" xr3:uid="{B00239B6-16E0-4472-B8C9-F25D625D21DD}" name="ref" dataDxfId="165">
+    <tableColumn id="1" xr3:uid="{D612E3DF-AA8E-4EE0-9306-7903B4821992}" name="index" dataDxfId="172"/>
+    <tableColumn id="2" xr3:uid="{B00239B6-16E0-4472-B8C9-F25D625D21DD}" name="ref" dataDxfId="171">
       <calculatedColumnFormula>OFFSET(table_1[ref], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{47FE94A7-C208-4138-B063-127D4AE215A0}" name="control" dataDxfId="164">
+    <tableColumn id="3" xr3:uid="{47FE94A7-C208-4138-B063-127D4AE215A0}" name="control" dataDxfId="170">
       <calculatedColumnFormula>OFFSET(table_1[control], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{43B4F550-AB35-4206-AAAB-820BBA723DEA}" name="dsb_type" dataDxfId="163">
+    <tableColumn id="4" xr3:uid="{43B4F550-AB35-4206-AAAB-820BBA723DEA}" name="dsb_type" dataDxfId="169">
       <calculatedColumnFormula>OFFSET(table_1[dsb_type], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7233C674-8249-48C9-814C-599A94DF6097}" name="dsb_pos" dataDxfId="162">
+    <tableColumn id="5" xr3:uid="{7233C674-8249-48C9-814C-599A94DF6097}" name="dsb_pos" dataDxfId="168">
       <calculatedColumnFormula>OFFSET(table_1[dsb_pos], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8FD419DF-3888-4BC8-ACF7-F31E7AB24754}" name="cell" dataDxfId="161">
+    <tableColumn id="6" xr3:uid="{8FD419DF-3888-4BC8-ACF7-F31E7AB24754}" name="cell" dataDxfId="167">
       <calculatedColumnFormula>OFFSET(table_1[cell], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{612FF909-1004-49E1-BC8F-F65A8C97EEFC}" name="strand" dataDxfId="160">
+    <tableColumn id="7" xr3:uid="{612FF909-1004-49E1-BC8F-F65A8C97EEFC}" name="strand" dataDxfId="166">
       <calculatedColumnFormula>OFFSET(table_1[strand], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C57AB4D7-F308-46D6-8F19-069619F8CF1B}" name="treatment" dataDxfId="159">
+    <tableColumn id="8" xr3:uid="{C57AB4D7-F308-46D6-8F19-069619F8CF1B}" name="treatment" dataDxfId="165">
       <calculatedColumnFormula>OFFSET(table_1[treatment], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{27DAC4C9-BDB2-4621-A4F1-0094D063284E}" name="hguide" dataDxfId="158">
+    <tableColumn id="9" xr3:uid="{27DAC4C9-BDB2-4621-A4F1-0094D063284E}" name="hguide" dataDxfId="164">
       <calculatedColumnFormula>OFFSET(table_1[hguide], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{E0E9E8C1-4E85-4EFB-8220-84140FBAAF8E}" name="output_dir" dataDxfId="157">
+    <tableColumn id="10" xr3:uid="{E0E9E8C1-4E85-4EFB-8220-84140FBAAF8E}" name="output_dir" dataDxfId="163">
       <calculatedColumnFormula>_xlfn.CONCAT(table_2_2[[#This Row],[cell]], "_", table_2_2[[#This Row],[hguide]], "_", table_2_2[[#This Row],[strand]], "_", table_2_2[[#This Row],[treatment]], "_nodsb")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{CAC474F1-3930-4766-B491-65C86C5752E8}" name="input" dataDxfId="156">
+    <tableColumn id="11" xr3:uid="{CAC474F1-3930-4766-B491-65C86C5752E8}" name="input" dataDxfId="162">
       <calculatedColumnFormula>OFFSET(table_1[file_out], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{BB84920E-3487-4670-93ED-5671EACD3061}" name="total_reads" dataDxfId="155">
+    <tableColumn id="12" xr3:uid="{BB84920E-3487-4670-93ED-5671EACD3061}" name="total_reads" dataDxfId="161">
       <calculatedColumnFormula>OFFSET(table_1[total_reads], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{0CE6DAF6-0C4C-4EC5-8FE5-9B3840A02412}" name="command" dataDxfId="154">
+    <tableColumn id="13" xr3:uid="{0CE6DAF6-0C4C-4EC5-8FE5-9B3840A02412}" name="command" dataDxfId="160">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_2[[#This Row],[input]], ".tsv ", " --total_reads ", table_2_2[[#This Row],[total_reads]], " -o ", libraries_3, "/", table_2_2[[#This Row],[output_dir]], ".tsv", " --quiet ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2445,47 +2484,47 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}" name="table_3_1" displayName="table_3_1" ref="A1:N41" totalsRowShown="0" headerRowDxfId="153">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}" name="table_3_1" displayName="table_3_1" ref="A1:N41" totalsRowShown="0" headerRowDxfId="159">
   <autoFilter ref="A1:N41" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}"/>
   <tableColumns count="14">
-    <tableColumn id="25" xr3:uid="{93D2F09B-24D5-4FE1-BF34-C037E361889F}" name="index" dataDxfId="152"/>
-    <tableColumn id="1" xr3:uid="{2F28DC66-449D-4F81-AA63-8F24B25F33D1}" name="dir" dataDxfId="151">
+    <tableColumn id="25" xr3:uid="{93D2F09B-24D5-4FE1-BF34-C037E361889F}" name="index" dataDxfId="158"/>
+    <tableColumn id="1" xr3:uid="{2F28DC66-449D-4F81-AA63-8F24B25F33D1}" name="dir" dataDxfId="157">
       <calculatedColumnFormula>OFFSET(table_2_1[output_dir], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{3DF6F698-1F9A-4B05-A310-657CCFCE9F66}" name="control" dataDxfId="150">
+    <tableColumn id="13" xr3:uid="{3DF6F698-1F9A-4B05-A310-657CCFCE9F66}" name="control" dataDxfId="156">
       <calculatedColumnFormula>OFFSET(table_2_1[control], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{362C2395-52F7-4A62-B7BA-2DD97ED5E6FB}" name="ref" dataDxfId="149">
+    <tableColumn id="2" xr3:uid="{362C2395-52F7-4A62-B7BA-2DD97ED5E6FB}" name="ref" dataDxfId="155">
       <calculatedColumnFormula>OFFSET(table_2_1[ref], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5F0895D9-2EF2-4524-8BC7-15A33FE68636}" name="dsb_pos" dataDxfId="148">
+    <tableColumn id="3" xr3:uid="{5F0895D9-2EF2-4524-8BC7-15A33FE68636}" name="dsb_pos" dataDxfId="154">
       <calculatedColumnFormula>OFFSET(table_2_1[dsb_pos], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C6D28829-46E6-4D97-8EA4-0AD12EF6CF10}" name="dsb_type" dataDxfId="147">
+    <tableColumn id="4" xr3:uid="{C6D28829-46E6-4D97-8EA4-0AD12EF6CF10}" name="dsb_type" dataDxfId="153">
       <calculatedColumnFormula>OFFSET(table_2_1[dsb_type], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{E8B2E211-C273-4602-86F0-60EA4259B7A4}" name="dsb_type_command" dataDxfId="146">
+    <tableColumn id="12" xr3:uid="{E8B2E211-C273-4602-86F0-60EA4259B7A4}" name="dsb_type_command" dataDxfId="152">
       <calculatedColumnFormula array="1">IF(table_3_1[[#This Row],[dsb_type]]="2DSB", "2", IF(table_3_1[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(table_3_1[[#This Row],[dsb_type]]="1DSB", "1", NA)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{15578E86-B7BE-4D8E-8FD4-E6C9C4F35C9C}" name="strand" dataDxfId="145">
+    <tableColumn id="5" xr3:uid="{15578E86-B7BE-4D8E-8FD4-E6C9C4F35C9C}" name="strand" dataDxfId="151">
       <calculatedColumnFormula>OFFSET(table_2_1[strand], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3366AC40-6578-4797-B607-19265E7DBF5C}" name="hguide" dataDxfId="144">
+    <tableColumn id="6" xr3:uid="{3366AC40-6578-4797-B607-19265E7DBF5C}" name="hguide" dataDxfId="150">
       <calculatedColumnFormula>MID(OFFSET(table_2_1[hguide], table_3_1[[#This Row],[index]] - 1, 0, 1, 1), 3, 100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{554F4E79-98DE-474B-A5C8-D4B536772E95}" name="cell" dataDxfId="143">
+    <tableColumn id="7" xr3:uid="{554F4E79-98DE-474B-A5C8-D4B536772E95}" name="cell" dataDxfId="149">
       <calculatedColumnFormula>OFFSET(table_2_1[cell], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{32FC5061-DD85-4234-9ED8-FEAF6D9E3BC0}" name="treatment" dataDxfId="142">
+    <tableColumn id="8" xr3:uid="{32FC5061-DD85-4234-9ED8-FEAF6D9E3BC0}" name="treatment" dataDxfId="148">
       <calculatedColumnFormula>OFFSET(table_2_1[treatment], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{DB6998A3-1431-4DDD-8DA0-525B805BF436}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{367B0912-E7A8-4430-962D-4F79EE14E5EA}" name="command_main_data" dataDxfId="141">
+    <tableColumn id="10" xr3:uid="{367B0912-E7A8-4430-962D-4F79EE14E5EA}" name="command_main_data" dataDxfId="147">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_1[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_1[[#This Row],[dir]], " -ref ref_seq/", table_3_1[[#This Row],[ref]], " -dsb ", table_3_1[[#This Row],[dsb_pos]], " --dsb_type ",table_3_1[[#This Row],[dsb_type_command]], " --strand ", table_3_1[[#This Row],[strand]], " --hguide ", table_3_1[[#This Row],[hguide]], " --cell ", table_3_1[[#This Row],[cell]], " --treatment ", table_3_1[[#This Row],[treatment]], " --subst_type ", table_3_1[[#This Row],[subst_type]], " --control ", table_3_1[[#This Row],[control]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{4A65279E-321E-4E3E-8383-26D448C2012F}" name="command_graph_data" dataDxfId="140">
+    <tableColumn id="11" xr3:uid="{4A65279E-321E-4E3E-8383-26D448C2012F}" name="command_graph_data" dataDxfId="146">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_1[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_1[[#This Row],[dir]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2494,47 +2533,47 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}" name="table_3_2" displayName="table_3_2" ref="A43:N55" totalsRowShown="0" headerRowDxfId="139">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}" name="table_3_2" displayName="table_3_2" ref="A43:N55" totalsRowShown="0" headerRowDxfId="145">
   <autoFilter ref="A43:N55" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}"/>
   <tableColumns count="14">
-    <tableColumn id="25" xr3:uid="{B2894846-EBB9-47DC-8DE1-7F1DA571A0B9}" name="index" dataDxfId="138"/>
-    <tableColumn id="1" xr3:uid="{98269DFC-71F0-4066-B063-59597431C1C3}" name="dir" dataDxfId="137">
+    <tableColumn id="25" xr3:uid="{B2894846-EBB9-47DC-8DE1-7F1DA571A0B9}" name="index" dataDxfId="144"/>
+    <tableColumn id="1" xr3:uid="{98269DFC-71F0-4066-B063-59597431C1C3}" name="dir" dataDxfId="143">
       <calculatedColumnFormula>OFFSET(table_2_2[output_dir], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{EB55B964-D8E2-4E0C-B7CF-07043E026664}" name="control" dataDxfId="136">
+    <tableColumn id="13" xr3:uid="{EB55B964-D8E2-4E0C-B7CF-07043E026664}" name="control" dataDxfId="142">
       <calculatedColumnFormula>OFFSET(table_2_2[control], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{7A83EC55-03CE-4608-92D6-6F1C53B539FE}" name="ref" dataDxfId="135">
+    <tableColumn id="2" xr3:uid="{7A83EC55-03CE-4608-92D6-6F1C53B539FE}" name="ref" dataDxfId="141">
       <calculatedColumnFormula>OFFSET(table_2_2[ref], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{13E984FC-9FD2-479F-AB4C-B74DDF5FD234}" name="dsb_pos" dataDxfId="134">
+    <tableColumn id="3" xr3:uid="{13E984FC-9FD2-479F-AB4C-B74DDF5FD234}" name="dsb_pos" dataDxfId="140">
       <calculatedColumnFormula>OFFSET(table_2_2[dsb_pos], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{EF0F2447-2FA1-4517-A5CE-D8DDAAC8D3F2}" name="dsb_type" dataDxfId="133">
+    <tableColumn id="4" xr3:uid="{EF0F2447-2FA1-4517-A5CE-D8DDAAC8D3F2}" name="dsb_type" dataDxfId="139">
       <calculatedColumnFormula>OFFSET(table_2_2[dsb_type], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A1849AE1-952B-42B5-99EE-20BD2E4C5A6A}" name="dsb_type_command" dataDxfId="132">
+    <tableColumn id="12" xr3:uid="{A1849AE1-952B-42B5-99EE-20BD2E4C5A6A}" name="dsb_type_command" dataDxfId="138">
       <calculatedColumnFormula array="1">IF(table_3_2[[#This Row],[dsb_type]]="2DSB", "2", IF(table_3_2[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(table_3_2[[#This Row],[dsb_type]]="1DSB", "1", NA)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{625E12FC-BF17-4E65-99DB-EDD53FEF055D}" name="strand" dataDxfId="131">
+    <tableColumn id="5" xr3:uid="{625E12FC-BF17-4E65-99DB-EDD53FEF055D}" name="strand" dataDxfId="137">
       <calculatedColumnFormula>OFFSET(table_2_2[strand], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0ABF747E-328F-4A80-85AA-4AF871C860C1}" name="hguide" dataDxfId="130">
+    <tableColumn id="6" xr3:uid="{0ABF747E-328F-4A80-85AA-4AF871C860C1}" name="hguide" dataDxfId="136">
       <calculatedColumnFormula>MID(OFFSET(table_2_2[hguide], table_3_2[[#This Row],[index]] - 1, 0, 1, 1), 3, 100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{29D6C48B-05B8-42C6-88A9-0939BC454FE0}" name="cell" dataDxfId="129">
+    <tableColumn id="7" xr3:uid="{29D6C48B-05B8-42C6-88A9-0939BC454FE0}" name="cell" dataDxfId="135">
       <calculatedColumnFormula>OFFSET(table_2_2[cell], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{BD269EBE-94A9-4B57-B984-C7566AC259DE}" name="treatment" dataDxfId="128">
+    <tableColumn id="8" xr3:uid="{BD269EBE-94A9-4B57-B984-C7566AC259DE}" name="treatment" dataDxfId="134">
       <calculatedColumnFormula>OFFSET(table_2_2[treatment], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{142C480D-E258-4979-A008-3940A3FE78E4}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{19804410-83AB-479E-A819-2D7449105C25}" name="command_main_data" dataDxfId="127">
+    <tableColumn id="10" xr3:uid="{19804410-83AB-479E-A819-2D7449105C25}" name="command_main_data" dataDxfId="133">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_2[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_2[[#This Row],[dir]], " -ref ref_seq/", table_3_2[[#This Row],[ref]], " -dsb ", table_3_2[[#This Row],[dsb_pos]], " --dsb_type ",table_3_2[[#This Row],[dsb_type_command]], " --strand ", table_3_2[[#This Row],[strand]], " --hguide ", table_3_2[[#This Row],[hguide]], " --cell ", table_3_2[[#This Row],[cell]], " --treatment ", table_3_2[[#This Row],[treatment]], " --subst_type ", table_3_2[[#This Row],[subst_type]], " --control ", table_3_2[[#This Row],[control]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{212A69BD-0F88-401C-957F-8B6EC8E55AED}" name="command_graph_data" dataDxfId="126">
+    <tableColumn id="11" xr3:uid="{212A69BD-0F88-401C-957F-8B6EC8E55AED}" name="command_graph_data" dataDxfId="132">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_2[[#This Row],[dir]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2543,38 +2582,38 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}" name="table_4_1" displayName="table_4_1" ref="A1:K17" totalsRowShown="0" headerRowDxfId="125">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}" name="table_4_1" displayName="table_4_1" ref="A1:K17" totalsRowShown="0" headerRowDxfId="131">
   <autoFilter ref="A1:K17" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B7EC223D-BA24-48F1-9EE3-DC56DEFDE4C2}" name="index" dataDxfId="124"/>
-    <tableColumn id="7" xr3:uid="{D9F1ADDA-18A2-4F81-862D-6B0F786079FF}" name="control" dataDxfId="123">
+    <tableColumn id="1" xr3:uid="{B7EC223D-BA24-48F1-9EE3-DC56DEFDE4C2}" name="index" dataDxfId="130"/>
+    <tableColumn id="7" xr3:uid="{D9F1ADDA-18A2-4F81-862D-6B0F786079FF}" name="control" dataDxfId="129">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{0EA5A81F-6EA1-4256-9717-03273165F7BF}" name="treatment_1" dataDxfId="122">
+    <tableColumn id="8" xr3:uid="{0EA5A81F-6EA1-4256-9717-03273165F7BF}" name="treatment_1" dataDxfId="128">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5F6D005A-96D8-4801-93E2-101BAE551BA8}" name="dir_1" dataDxfId="121">
+    <tableColumn id="2" xr3:uid="{5F6D005A-96D8-4801-93E2-101BAE551BA8}" name="dir_1" dataDxfId="127">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C21D1AF7-7ABE-4181-AA2A-42227869A8DD}" name="treatment_2" dataDxfId="120">
+    <tableColumn id="9" xr3:uid="{C21D1AF7-7ABE-4181-AA2A-42227869A8DD}" name="treatment_2" dataDxfId="126">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{D66426AC-E0B2-4B07-A4D4-5A74AA033E80}" name="dir_2" dataDxfId="119">
+    <tableColumn id="3" xr3:uid="{D66426AC-E0B2-4B07-A4D4-5A74AA033E80}" name="dir_2" dataDxfId="125">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{0C8146A0-DC77-4DC4-82FF-74F4C74CF33E}" name="treatments_out" dataDxfId="118">
+    <tableColumn id="10" xr3:uid="{0C8146A0-DC77-4DC4-82FF-74F4C74CF33E}" name="treatments_out" dataDxfId="124">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_1[[#This Row],[treatment_1]], "_", table_4_1[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{519A6397-7A3C-4009-B8B9-A71C0B3A591B}" name="dir_out" dataDxfId="117">
+    <tableColumn id="4" xr3:uid="{519A6397-7A3C-4009-B8B9-A71C0B3A591B}" name="dir_out" dataDxfId="123">
       <calculatedColumnFormula>SUBSTITUTE(table_4_1[[#This Row],[dir_1]], table_4_1[[#This Row],[treatment_1]], table_4_1[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E1629355-7D02-4819-98A1-EEB3B5FADE18}" name="subst_type" dataDxfId="116">
+    <tableColumn id="5" xr3:uid="{E1629355-7D02-4819-98A1-EEB3B5FADE18}" name="subst_type" dataDxfId="122">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{BC9117A0-CB6F-4D3C-A0E4-BF8395854D9A}" name="command_main_data_combined" dataDxfId="115">
+    <tableColumn id="6" xr3:uid="{BC9117A0-CB6F-4D3C-A0E4-BF8395854D9A}" name="command_main_data_combined" dataDxfId="121">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_1[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_1[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_1[[#This Row],[dir_out]], " --subst_type ", table_4_1[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{D384013E-9937-4DD8-A36A-43325757359B}" name="command_graph_data" dataDxfId="114">
+    <tableColumn id="11" xr3:uid="{D384013E-9937-4DD8-A36A-43325757359B}" name="command_graph_data" dataDxfId="120">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_1[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_1[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2583,38 +2622,38 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}" name="table_4_2" displayName="table_4_2" ref="A20:K22" totalsRowShown="0" headerRowDxfId="113">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}" name="table_4_2" displayName="table_4_2" ref="A20:K22" totalsRowShown="0" headerRowDxfId="119">
   <autoFilter ref="A20:K22" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{7F5A3A15-751D-407C-A035-61B2605E693F}" name="index" dataDxfId="112"/>
-    <tableColumn id="7" xr3:uid="{45863AB0-FD32-49FE-B4BF-F8EE865F7604}" name="control" dataDxfId="111">
+    <tableColumn id="1" xr3:uid="{7F5A3A15-751D-407C-A035-61B2605E693F}" name="index" dataDxfId="118"/>
+    <tableColumn id="7" xr3:uid="{45863AB0-FD32-49FE-B4BF-F8EE865F7604}" name="control" dataDxfId="117">
       <calculatedColumnFormula>OFFSET(table_3_1[control], var_4_anti_offset + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{CD16648D-267E-410B-A366-3E12367C037C}" name="treatment_1" dataDxfId="110">
+    <tableColumn id="8" xr3:uid="{CD16648D-267E-410B-A366-3E12367C037C}" name="treatment_1" dataDxfId="116">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{10C9F90E-86FD-4BFE-939E-298FD6F69F12}" name="dir_1" dataDxfId="109">
+    <tableColumn id="2" xr3:uid="{10C9F90E-86FD-4BFE-939E-298FD6F69F12}" name="dir_1" dataDxfId="115">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{7AB3E4AB-F43B-4FDE-96D7-FBBB4A8B83BE}" name="treatment_2" dataDxfId="108">
+    <tableColumn id="9" xr3:uid="{7AB3E4AB-F43B-4FDE-96D7-FBBB4A8B83BE}" name="treatment_2" dataDxfId="114">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1) + 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BF948A3E-9649-41BF-A7E7-57BFDE810FE9}" name="dir_2" dataDxfId="107">
+    <tableColumn id="3" xr3:uid="{BF948A3E-9649-41BF-A7E7-57BFDE810FE9}" name="dir_2" dataDxfId="113">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1) + 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{378119E5-F021-4785-A653-4D632F029AA6}" name="treatments_out" dataDxfId="106">
+    <tableColumn id="10" xr3:uid="{378119E5-F021-4785-A653-4D632F029AA6}" name="treatments_out" dataDxfId="112">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_2[[#This Row],[treatment_1]], "_", table_4_2[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AE1A14DC-D0C9-4818-B8CC-09A571E73BC2}" name="dir_out" dataDxfId="105">
+    <tableColumn id="4" xr3:uid="{AE1A14DC-D0C9-4818-B8CC-09A571E73BC2}" name="dir_out" dataDxfId="111">
       <calculatedColumnFormula>SUBSTITUTE(table_4_2[[#This Row],[dir_1]], table_4_2[[#This Row],[treatment_1]], table_4_2[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{F29DAC4E-FEC5-4C1D-AAC1-7CE19E401F25}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{DC4E99F4-97AB-4553-A5FB-D20D3D487947}" name="command_main_data_combined" dataDxfId="104">
+    <tableColumn id="6" xr3:uid="{DC4E99F4-97AB-4553-A5FB-D20D3D487947}" name="command_main_data_combined" dataDxfId="110">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_2[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_2[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_2[[#This Row],[dir_out]], " --subst_type ", table_4_2[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{E19D3001-2E76-4CC2-BF33-D0465C77D538}" name="command_graph_data" dataDxfId="103">
+    <tableColumn id="11" xr3:uid="{E19D3001-2E76-4CC2-BF33-D0465C77D538}" name="command_graph_data" dataDxfId="109">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_2[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2623,38 +2662,38 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}" name="table_4_3" displayName="table_4_3" ref="A25:K33" totalsRowShown="0" headerRowDxfId="102">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}" name="table_4_3" displayName="table_4_3" ref="A25:K33" totalsRowShown="0" headerRowDxfId="108">
   <autoFilter ref="A25:K33" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{33AF3495-7432-4F03-9832-525A370EADEC}" name="index" dataDxfId="101"/>
-    <tableColumn id="7" xr3:uid="{3D66515C-5022-4D48-A834-4320DA4E73F6}" name="control" dataDxfId="100">
+    <tableColumn id="1" xr3:uid="{33AF3495-7432-4F03-9832-525A370EADEC}" name="index" dataDxfId="107"/>
+    <tableColumn id="7" xr3:uid="{3D66515C-5022-4D48-A834-4320DA4E73F6}" name="control" dataDxfId="106">
       <calculatedColumnFormula>OFFSET(table_3_2[control], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{294B17A9-F0F9-42CA-8342-55C00648E3A5}" name="treatment_1" dataDxfId="99">
+    <tableColumn id="8" xr3:uid="{294B17A9-F0F9-42CA-8342-55C00648E3A5}" name="treatment_1" dataDxfId="105">
       <calculatedColumnFormula>OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E13C38CF-C105-4AB5-8602-7D32E688C737}" name="dir_1" dataDxfId="98">
+    <tableColumn id="2" xr3:uid="{E13C38CF-C105-4AB5-8602-7D32E688C737}" name="dir_1" dataDxfId="104">
       <calculatedColumnFormula>OFFSET(table_3_2[dir], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{15B3CC7F-2A3C-4026-8417-A9DD21E4F004}" name="treatment_2" dataDxfId="97">
+    <tableColumn id="9" xr3:uid="{15B3CC7F-2A3C-4026-8417-A9DD21E4F004}" name="treatment_2" dataDxfId="103">
       <calculatedColumnFormula>OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{FF7D9AD3-1A35-4013-88AE-0C00465033CD}" name="dir_2" dataDxfId="96">
+    <tableColumn id="3" xr3:uid="{FF7D9AD3-1A35-4013-88AE-0C00465033CD}" name="dir_2" dataDxfId="102">
       <calculatedColumnFormula>OFFSET(table_3_2[dir], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{9353B2D3-0D23-4FBB-AFEC-EB68549160F4}" name="treatments_out" dataDxfId="95">
+    <tableColumn id="10" xr3:uid="{9353B2D3-0D23-4FBB-AFEC-EB68549160F4}" name="treatments_out" dataDxfId="101">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_3[[#This Row],[treatment_1]], "_", table_4_3[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{77F1D6F0-DE95-4E63-9E7E-D3CA3CF85F37}" name="dir_out" dataDxfId="94">
+    <tableColumn id="4" xr3:uid="{77F1D6F0-DE95-4E63-9E7E-D3CA3CF85F37}" name="dir_out" dataDxfId="100">
       <calculatedColumnFormula>SUBSTITUTE(table_4_3[[#This Row],[dir_1]], table_4_3[[#This Row],[treatment_1]], table_4_3[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{BBF4F840-178E-461E-8C17-36D699EDE038}" name="subst_type" dataDxfId="93">
+    <tableColumn id="5" xr3:uid="{BBF4F840-178E-461E-8C17-36D699EDE038}" name="subst_type" dataDxfId="99">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9434BF8B-81C5-43DF-BCB7-FA7146BF2FE8}" name="command_main_data_combined" dataDxfId="92">
+    <tableColumn id="6" xr3:uid="{9434BF8B-81C5-43DF-BCB7-FA7146BF2FE8}" name="command_main_data_combined" dataDxfId="98">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_3[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_3[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_3[[#This Row],[dir_out]], " --subst_type ", table_4_3[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{1ABF0B7B-4ECE-42BF-A7D8-EA13E98144EE}" name="command_graph_data" dataDxfId="91">
+    <tableColumn id="11" xr3:uid="{1ABF0B7B-4ECE-42BF-A7D8-EA13E98144EE}" name="command_graph_data" dataDxfId="97">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_3[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_3[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -22302,10 +22341,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FCC207B-A9CD-4866-A17E-A3EE763F139F}">
-  <dimension ref="A1:M55"/>
+  <dimension ref="A1:M58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B41"/>
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25161,11 +25200,74 @@
         <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_cmv_nodsb -o plots/histogram_3d/</v>
       </c>
     </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" t="str">
+        <f ca="1">_xlfn.TEXTJOIN(CHAR(10), TRUE, M2:M41,M44:M55)</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgAB_R1_sense -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgAB_R1_branch -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgAB_R1_cmv -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgAB_R1_sense -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgAB_R1_branch -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgAB_R1_cmv -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgAB_R2_sense -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgAB_R2_branch -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgAB_R2_cmv -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgAB_R2_sense -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgAB_R2_branch -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgAB_R2_cmv -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_sense -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_branch -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_cmv -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_sense -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_branch -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_cmv -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_sense -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_branch -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_cmv -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_sense -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_branch -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_cmv -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_sense_30bpDown -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_branch_30bpDown -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_cmv_30bpDown -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_sense_30bpDown -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_branch_30bpDown -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_cmv_30bpDown -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_sense_30bpDown -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_branch_30bpDown -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_cmv_30bpDown -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_sense_30bpDown -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_branch_30bpDown -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_cmv_30bpDown -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgCD_R1_antisense -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgCD_R1_splicing -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgCD_R2_antisense -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgCD_R2_splicing -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_sense_nodsb -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_branch_nodsb -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_cmv_nodsb -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_sense_nodsb -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_branch_nodsb -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_cmv_nodsb -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_sense_nodsb -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_branch_nodsb -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_cmv_nodsb -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_sense_nodsb -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_branch_nodsb -o plots/histogram_3d/
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_cmv_nodsb -o plots/histogram_3d/</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -25174,8 +25276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1417E7-0E2A-4E67-94B4-4030BF5F7C23}">
   <dimension ref="A1:V17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25549,10 +25651,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1375107-D76A-4386-B771-6693BBF75061}">
-  <dimension ref="A1:P67"/>
+  <dimension ref="A1:R67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" topLeftCell="C49" workbookViewId="0">
+      <selection activeCell="K66" sqref="K66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25571,7 +25673,7 @@
     <col min="14" max="14" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>175</v>
       </c>
@@ -25604,7 +25706,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>112</v>
       </c>
@@ -25651,10 +25753,16 @@
         <v>184</v>
       </c>
       <c r="P2" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -25723,12 +25831,20 @@
         <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
       </c>
-      <c r="P3" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 </v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P3">
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 10, IF(table_7_1[[#This Row],[hguide]]="A", 10, IF(table_7_1[[#This Row],[hguide]]="B", 10, IF(table_7_1[[#This Row],[hguide]]="CD", 10, NA())))), NA())</f>
+        <v>10</v>
+      </c>
+      <c r="Q3" t="str">
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/individual/", var_7_ext)</f>
+        <v>plots/graphs/universal/individual/png</v>
+      </c>
+      <c r="R3" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], IF(NOT(ISNA(table_7_1[[#This Row],[universal_layout_legend_pos_x]])), _xlfn.CONCAT(" --universal_layout_legend_pos_x ", table_7_1[[#This Row],[universal_layout_legend_pos_x]], "")))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 20  --universal_layout_legend_pos_x 10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -25797,12 +25913,20 @@
         <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
       </c>
-      <c r="P4" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 </v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P4">
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 10, IF(table_7_1[[#This Row],[hguide]]="A", 10, IF(table_7_1[[#This Row],[hguide]]="B", 10, IF(table_7_1[[#This Row],[hguide]]="CD", 10, NA())))), NA())</f>
+        <v>10</v>
+      </c>
+      <c r="Q4" t="str">
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/individual/", var_7_ext)</f>
+        <v>plots/graphs/universal/individual/png</v>
+      </c>
+      <c r="R4" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], IF(NOT(ISNA(table_7_1[[#This Row],[universal_layout_legend_pos_x]])), _xlfn.CONCAT(" --universal_layout_legend_pos_x ", table_7_1[[#This Row],[universal_layout_legend_pos_x]], "")))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 20  --universal_layout_legend_pos_x 10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -25871,12 +25995,20 @@
         <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 12 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 12 --range_y -18 24 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 12 --range_y -22 18 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 12 --range_y -20 10 ", NA())))), "")</f>
         <v xml:space="preserve"> --range_x -12 12 --range_y -22 20 </v>
       </c>
-      <c r="P5" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", graphs, "/", var_7_layout, "/individual/", var_7_ext, IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]])</f>
-        <v xml:space="preserve">python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range_y -22 20 </v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P5">
+        <f ca="1">IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 10, IF(table_7_1[[#This Row],[hguide]]="A", 10, IF(table_7_1[[#This Row],[hguide]]="B", 10, IF(table_7_1[[#This Row],[hguide]]="CD", 10, NA())))), NA())</f>
+        <v>10</v>
+      </c>
+      <c r="Q5" t="str">
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/individual/", var_7_ext)</f>
+        <v>plots/graphs/universal/individual/png</v>
+      </c>
+      <c r="R5" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], IF(NOT(ISNA(table_7_1[[#This Row],[universal_layout_legend_pos_x]])), _xlfn.CONCAT(" --universal_layout_legend_pos_x ", table_7_1[[#This Row],[universal_layout_legend_pos_x]], "")))</f>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800  --range_x -12 12 --range